<commit_message>
add new content tags to quick start
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23198CBE-5B5A-F144-B019-3FDB8FA8D031}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D4A99B-544D-214A-B59C-630238B89E98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-71680" yWindow="-12140" windowWidth="47680" windowHeight="17540" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-71680" yWindow="-12140" windowWidth="47680" windowHeight="17540" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2605,11 +2605,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AB98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C35" sqref="C35"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7893,10 +7893,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q88"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7949,7 +7950,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -7974,7 +7975,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -7999,7 +8000,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -8024,7 +8025,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -8049,7 +8050,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -8080,7 +8081,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -8105,7 +8106,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -8130,7 +8131,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -8156,7 +8157,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -8183,7 +8184,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -8209,7 +8210,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -8234,7 +8235,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -8265,7 +8266,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -8290,7 +8291,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -8315,7 +8316,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -8346,7 +8347,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -8372,7 +8373,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -8403,7 +8404,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -8430,7 +8431,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>21</v>
       </c>
@@ -8456,7 +8457,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>22</v>
       </c>
@@ -8481,7 +8482,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>23</v>
       </c>
@@ -8507,7 +8508,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>24</v>
       </c>
@@ -8534,7 +8535,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>25</v>
       </c>
@@ -8561,7 +8562,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>26</v>
       </c>
@@ -8588,7 +8589,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>27</v>
       </c>
@@ -8613,7 +8614,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>28</v>
       </c>
@@ -8638,7 +8639,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>29</v>
       </c>
@@ -8663,7 +8664,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>30</v>
       </c>
@@ -8694,7 +8695,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>31</v>
       </c>
@@ -8725,7 +8726,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>32</v>
       </c>
@@ -8756,7 +8757,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>33</v>
       </c>
@@ -8787,7 +8788,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>36</v>
       </c>
@@ -8864,6 +8865,9 @@
       <c r="D35" s="1" t="s">
         <v>580</v>
       </c>
+      <c r="E35" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="F35" s="1" t="s">
         <v>70</v>
       </c>
@@ -8954,6 +8958,9 @@
       <c r="D38" s="1" t="s">
         <v>577</v>
       </c>
+      <c r="E38" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="F38" s="1" t="s">
         <v>70</v>
       </c>
@@ -8984,6 +8991,9 @@
       <c r="D39" s="1" t="s">
         <v>578</v>
       </c>
+      <c r="E39" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="F39" s="1" t="s">
         <v>70</v>
       </c>
@@ -9014,6 +9024,9 @@
       <c r="D40" s="1" t="s">
         <v>579</v>
       </c>
+      <c r="E40" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="F40" s="1" t="s">
         <v>70</v>
       </c>
@@ -9030,7 +9043,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>42</v>
       </c>
@@ -9060,7 +9073,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>45</v>
       </c>
@@ -9091,7 +9104,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>46</v>
       </c>
@@ -9122,7 +9135,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>49</v>
       </c>
@@ -9152,7 +9165,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>50</v>
       </c>
@@ -9185,7 +9198,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>51</v>
       </c>
@@ -9215,7 +9228,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>52</v>
       </c>
@@ -9248,7 +9261,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>53</v>
       </c>
@@ -9278,7 +9291,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>56</v>
       </c>
@@ -9308,7 +9321,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>57</v>
       </c>
@@ -9338,7 +9351,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>58</v>
       </c>
@@ -9368,7 +9381,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>59</v>
       </c>
@@ -9398,7 +9411,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>60</v>
       </c>
@@ -9428,7 +9441,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>63</v>
       </c>
@@ -9459,7 +9472,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>64</v>
       </c>
@@ -9490,7 +9503,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>67</v>
       </c>
@@ -9523,7 +9536,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>68</v>
       </c>
@@ -9556,7 +9569,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>69</v>
       </c>
@@ -9589,7 +9602,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>70</v>
       </c>
@@ -9622,7 +9635,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>73</v>
       </c>
@@ -9653,7 +9666,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <f>SUBTOTAL(9,M101)</f>
         <v>0</v>
@@ -9684,7 +9697,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>75</v>
       </c>
@@ -9715,7 +9728,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>76</v>
       </c>
@@ -9746,7 +9759,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>77</v>
       </c>
@@ -9777,7 +9790,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>80</v>
       </c>
@@ -9809,7 +9822,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>81</v>
       </c>
@@ -9842,7 +9855,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>82</v>
       </c>
@@ -9872,7 +9885,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>83</v>
       </c>
@@ -9905,7 +9918,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>84</v>
       </c>
@@ -9935,7 +9948,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>85</v>
       </c>
@@ -9965,7 +9978,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>88</v>
       </c>
@@ -9998,7 +10011,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>89</v>
       </c>
@@ -10030,7 +10043,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>90</v>
       </c>
@@ -10062,7 +10075,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>91</v>
       </c>
@@ -10094,7 +10107,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>94</v>
       </c>
@@ -10127,7 +10140,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>97</v>
       </c>
@@ -10160,7 +10173,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code.</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>100</v>
       </c>
@@ -10193,7 +10206,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>101</v>
       </c>
@@ -10226,7 +10239,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>102</v>
       </c>
@@ -10259,7 +10272,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>103</v>
       </c>
@@ -10292,7 +10305,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="81" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>104</v>
       </c>
@@ -10328,7 +10341,7 @@
       <c r="P81" s="1"/>
       <c r="Q81" s="1"/>
     </row>
-    <row r="82" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>107</v>
       </c>
@@ -10359,7 +10372,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="83" spans="1:17" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>108</v>
       </c>
@@ -10388,7 +10401,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="84" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>109</v>
       </c>
@@ -10421,7 +10434,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="85" spans="1:17" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>110</v>
       </c>
@@ -10454,7 +10467,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="86" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>111</v>
       </c>
@@ -10484,7 +10497,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="87" spans="1:17" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>112</v>
       </c>
@@ -10515,7 +10528,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="88" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>115</v>
       </c>
@@ -10545,7 +10558,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K88" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
+  <autoFilter ref="A1:K88" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Condition"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K132">
     <sortCondition ref="A1"/>
   </sortState>

</xml_diff>

<commit_message>
update careteam intro and notes
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BF2F87B-DBD8-6743-B15B-4009D232C53B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9270C36B-8547-8F45-9F36-229AA4FC89FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-66900" yWindow="-1720" windowWidth="55960" windowHeight="14700" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2210" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2209" uniqueCount="602">
   <si>
     <t>Element</t>
   </si>
@@ -2000,12 +2000,6 @@
     <t>GET [base]/Encounter?patient=example1&amp;discharge-disposition=01</t>
   </si>
   <si>
-    <t>support fetching a CareTeam</t>
-  </si>
-  <si>
-    <t>CareTeam:participant:Practitioner,CareTeam:participant:Patient,CareTeam:participant:RelatedPerson,</t>
-  </si>
-  <si>
     <t>role</t>
   </si>
   <si>
@@ -2015,18 +2009,9 @@
     <t>DOES THIS DO ANYTHING?</t>
   </si>
   <si>
-    <t>!CareTeam</t>
-  </si>
-  <si>
     <t>support searching for all current care team members for a patient. DOES THIS DO ANYTHING?</t>
   </si>
   <si>
-    <t>GET [base]/CareTeam?patient=1137192&amp;status=active~GET [base]/CareTeam?patient=1137192&amp;status=active&amp;_include=CareTeam:participant:Practitioner&amp;_include=CareTeam:participant:Patient&amp;_include=CareTeam:participant:RelatedPerson</t>
-  </si>
-  <si>
-    <t>Fetches a bundle of all CareTeam resources for the specified patient and status =`active` and may include CareTeam Patient, RelatedPerson and Practitioner participants</t>
-  </si>
-  <si>
     <t>patient,role</t>
   </si>
   <si>
@@ -2037,6 +2022,18 @@
   </si>
   <si>
     <t>Fetches a bundle of all CareTeam resources for the specified patient and participant role</t>
+  </si>
+  <si>
+    <t>CareTeam:participant:PractitionerRole,CareTeam:participant:Practitioner,CareTeam:participant:Patient,CareTeam:participant:RelatedPerson</t>
+  </si>
+  <si>
+    <t>GET [base]/CareTeam?patient=1137192&amp;status=active~GET [base]/CareTeam?patient=1137192&amp;status=active&amp;_include=CareTeam:participant:RelatedPerson&amp;_include=CareTeam:participant:Patient&amp;_include=CareTeam:participant:Practitioner&amp;_include=CareTeam:participant:PractitionerRole</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all CareTeam resources for the specified patient and status =`active` and may include CareTeam Patient, RelatedPerson and Practitioner and PractitionerRole participants.  
+To get Pactiitioner name and identifier using PractitionerRole:  
+1) Search for the careteam PractiitionerRole: GET [base]/CareTeam?patient=[id]&amp;status=active&amp;_include=CareTeam:participant:RelatedPerson  
+2) using the FHIR _id from the PractitionerRole.practitioner element resource,  fetch the Practitioner resources using  GET [base]/Practitioner?_id=[id]</t>
   </si>
 </sst>
 </file>
@@ -2660,10 +2657,10 @@
   <dimension ref="A1:AB102"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="O23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="R23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z86" sqref="Z86"/>
+      <selection pane="bottomRight" activeCell="X83" sqref="X83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2678,7 +2675,8 @@
     <col min="9" max="9" width="8.83203125" style="1"/>
     <col min="10" max="10" width="14.33203125" customWidth="1"/>
     <col min="12" max="12" width="31.1640625" style="1" customWidth="1"/>
-    <col min="13" max="25" width="13.33203125" style="1" customWidth="1"/>
+    <col min="13" max="24" width="13.33203125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="27.83203125" style="1" customWidth="1"/>
     <col min="26" max="26" width="90.6640625" style="1" customWidth="1"/>
     <col min="27" max="27" width="83.5" style="2" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="38.1640625" customWidth="1"/>
@@ -7078,7 +7076,7 @@
         <v>56</v>
       </c>
       <c r="X83" s="1" t="s">
-        <v>592</v>
+        <v>599</v>
       </c>
       <c r="Y83" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B83)&amp;"s for a patient"</f>
@@ -7102,7 +7100,7 @@
         <v>20</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>596</v>
+        <v>268</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>55</v>
@@ -7115,7 +7113,7 @@
       </c>
       <c r="G84" s="1" t="str">
         <f t="shared" si="40"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!careteam</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>56</v>
@@ -7131,7 +7129,7 @@
       </c>
       <c r="L84" s="1" t="str">
         <f t="shared" ref="L84:L85" si="46">B84&amp;"."&amp;C84</f>
-        <v>!CareTeam._id</v>
+        <v>Practitioner._id</v>
       </c>
       <c r="M84" s="1" t="s">
         <v>56</v>
@@ -7139,20 +7137,20 @@
       <c r="O84" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="X84" s="1" t="s">
-        <v>592</v>
-      </c>
-      <c r="Y84" s="5" t="s">
-        <v>591</v>
+      <c r="Y84" s="5" t="str">
+        <f>"support fetching a "&amp;B84</f>
+        <v>support fetching a Practitioner</v>
       </c>
       <c r="Z84" s="5" t="str">
-        <f>"GET [base]/"&amp;B84&amp;"?name=Smith"</f>
-        <v>GET [base]/!CareTeam?name=Smith</v>
-      </c>
-      <c r="AA84" s="2"/>
+        <f>"GET [base]/"&amp;B84&amp;"/practitioner-1~GET [base]/"&amp;B84&amp;"?_id=practitioner-1"</f>
+        <v>GET [base]/Practitioner/practitioner-1~GET [base]/Practitioner?_id=practitioner-1</v>
+      </c>
+      <c r="AA84" s="12" t="s">
+        <v>593</v>
+      </c>
       <c r="AB84" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B84)&amp;"-"&amp;SUBSTITUTE(C84,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-!careteam-id.html</v>
+        <v>SearchParameter-us-core-practitioner-id.html</v>
       </c>
     </row>
     <row r="85" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -7216,7 +7214,7 @@
         <v>249</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>70</v>
@@ -7257,14 +7255,14 @@
         <v>56</v>
       </c>
       <c r="Y86" s="5" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="Z86" s="5" t="str">
         <f>"GET [base]/"&amp;B86&amp;"?"&amp;C86&amp;"=http://snomed.info/sct\|17561000"</f>
         <v>GET [base]/CareTeam?role=http://snomed.info/sct\|17561000</v>
       </c>
       <c r="AA86" s="12" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="AB86" s="1" t="str">
         <f t="shared" ref="AB86" si="50">"SearchParameter-us-core-"&amp;LOWER((B86)&amp;"-"&amp;C86&amp;".html")</f>
@@ -8192,7 +8190,7 @@
   <dimension ref="A1:Q91"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="I1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="J95" sqref="J95"/>
+      <selection activeCell="K77" sqref="K77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10470,7 +10468,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" s="1" customFormat="1" ht="137" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>94</v>
       </c>
@@ -10497,13 +10495,13 @@
         <v>312</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>598</v>
-      </c>
-      <c r="K77" s="5" t="s">
-        <v>599</v>
+        <v>600</v>
+      </c>
+      <c r="K77" s="12" t="s">
+        <v>601</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
@@ -10935,7 +10933,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="E91" s="1" t="b">
         <v>1</v>
@@ -10947,13 +10945,13 @@
         <v>106</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add obs for clinical tests and imaging
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6B6509-38B0-0148-AB1B-AFE5EBA0A7A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55663B1B-0FAE-5447-A88D-B36CC0F5E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <sheet name="sp_combos" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$90</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$91</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$102</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
@@ -2662,11 +2662,11 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:AB102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="F84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F84" sqref="F84"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8192,8 +8192,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q91"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="K104" sqref="K104"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9499,7 +9499,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>49</v>
       </c>
@@ -9529,7 +9529,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>50</v>
       </c>
@@ -9562,7 +9562,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>51</v>
       </c>
@@ -9592,7 +9592,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>52</v>
       </c>
@@ -9625,7 +9625,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>53</v>
       </c>
@@ -9655,7 +9655,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>56</v>
       </c>
@@ -9685,7 +9685,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>57</v>
       </c>
@@ -9715,7 +9715,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>58</v>
       </c>
@@ -9745,7 +9745,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>59</v>
       </c>
@@ -9775,7 +9775,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>60</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>63</v>
       </c>
@@ -9836,7 +9836,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>64</v>
       </c>
@@ -9867,7 +9867,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>67</v>
       </c>
@@ -9900,7 +9900,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>68</v>
       </c>
@@ -9933,7 +9933,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>69</v>
       </c>
@@ -9966,7 +9966,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>70</v>
       </c>
@@ -9999,7 +9999,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>73</v>
       </c>
@@ -10030,7 +10030,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <f>SUBTOTAL(9,M103)</f>
         <v>0</v>
@@ -10061,7 +10061,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>75</v>
       </c>
@@ -10092,7 +10092,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>76</v>
       </c>
@@ -10123,7 +10123,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>77</v>
       </c>
@@ -10154,7 +10154,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>80</v>
       </c>
@@ -10186,7 +10186,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>81</v>
       </c>
@@ -10219,7 +10219,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>82</v>
       </c>
@@ -10249,7 +10249,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>83</v>
       </c>
@@ -10282,7 +10282,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>84</v>
       </c>
@@ -10312,7 +10312,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>85</v>
       </c>
@@ -10342,7 +10342,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>88</v>
       </c>
@@ -10375,7 +10375,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>89</v>
       </c>
@@ -10407,7 +10407,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>90</v>
       </c>
@@ -10439,7 +10439,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>91</v>
       </c>
@@ -10471,7 +10471,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="1" customFormat="1" ht="137" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" s="1" customFormat="1" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>94</v>
       </c>
@@ -10924,7 +10924,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="91" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>94</v>
       </c>
@@ -10958,10 +10958,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K90" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
+  <autoFilter ref="A1:K91" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
     <filterColumn colId="1">
       <filters>
-        <filter val="CareTeam"/>
+        <filter val="DiagnosticReport"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
add clinical test report
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55663B1B-0FAE-5447-A88D-B36CC0F5E6FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3B9816-B0C5-3147-BDF9-3939366A6772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -116,11 +116,22 @@
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
+    <author>tc={64123793-88FC-AA4D-9FF9-21C390EA52F3}</author>
     <author>tc={4C3DF362-0F09-CC4A-8C76-08E5FFBB7F41}</author>
     <author>tc={55554AA4-06E7-B947-A224-22F62EAAB8DA}</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{4C3DF362-0F09-CC4A-8C76-08E5FFBB7F41}">
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{64123793-88FC-AA4D-9FF9-21C390EA52F3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    add column for include file
+Reply:
+    make this a comma separate list of profiles</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{4C3DF362-0F09-CC4A-8C76-08E5FFBB7F41}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -128,7 +139,7 @@
     does this do anything if not delete row</t>
       </text>
     </comment>
-    <comment ref="I39" authorId="1" shapeId="0" xr:uid="{55554AA4-06E7-B947-A224-22F62EAAB8DA}">
+    <comment ref="I39" authorId="2" shapeId="0" xr:uid="{55554AA4-06E7-B947-A224-22F62EAAB8DA}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2046,7 +2057,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2141,6 +2152,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2555,6 +2572,12 @@
 
 <file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C1" dT="2021-11-10T17:47:31.83" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{64123793-88FC-AA4D-9FF9-21C390EA52F3}">
+    <text>add column for include file</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2021-11-10T17:48:52.85" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{0B433B21-67D8-2942-8EC7-C5BF55E34A64}" parentId="{64123793-88FC-AA4D-9FF9-21C390EA52F3}">
+    <text>make this a comma separate list of profiles</text>
+  </threadedComment>
   <threadedComment ref="I1" dT="2021-11-08T19:54:50.37" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{4C3DF362-0F09-CC4A-8C76-08E5FFBB7F41}">
     <text>does this do anything if not delete row</text>
   </threadedComment>
@@ -2663,10 +2686,10 @@
   <dimension ref="A1:AB102"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F84" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="G77" sqref="G77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6504,7 +6527,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>69</v>
       </c>
@@ -6557,7 +6580,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>70</v>
       </c>
@@ -6607,7 +6630,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>71</v>
       </c>
@@ -6660,7 +6683,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -6714,7 +6737,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>73</v>
       </c>
@@ -7101,7 +7124,7 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>20</v>
       </c>
@@ -7932,7 +7955,7 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="99" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>93</v>
       </c>
@@ -7987,7 +8010,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="100" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>94</v>
       </c>
@@ -8174,7 +8197,7 @@
   <autoFilter ref="A1:AB102" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Practitioner"/>
+        <filter val="Observation"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8193,7 +8216,7 @@
   <dimension ref="A1:Q91"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B98" sqref="B98"/>
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9499,7 +9522,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>49</v>
       </c>
@@ -9529,7 +9552,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>50</v>
       </c>
@@ -9562,7 +9585,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>51</v>
       </c>
@@ -9592,7 +9615,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>52</v>
       </c>
@@ -9625,7 +9648,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>53</v>
       </c>
@@ -9655,7 +9678,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>56</v>
       </c>
@@ -9685,7 +9708,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>57</v>
       </c>
@@ -9715,7 +9738,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>58</v>
       </c>
@@ -9745,7 +9768,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>59</v>
       </c>
@@ -9775,7 +9798,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>60</v>
       </c>
@@ -9805,7 +9828,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>63</v>
       </c>
@@ -9836,7 +9859,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>64</v>
       </c>
@@ -9867,7 +9890,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>67</v>
       </c>
@@ -9900,7 +9923,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>68</v>
       </c>
@@ -9933,7 +9956,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>69</v>
       </c>
@@ -9966,7 +9989,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>70</v>
       </c>
@@ -9999,7 +10022,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>73</v>
       </c>
@@ -10030,7 +10053,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <f>SUBTOTAL(9,M103)</f>
         <v>0</v>
@@ -10061,7 +10084,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>75</v>
       </c>
@@ -10092,7 +10115,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>76</v>
       </c>
@@ -10123,7 +10146,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>77</v>
       </c>
@@ -10154,7 +10177,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>80</v>
       </c>
@@ -10186,7 +10209,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>81</v>
       </c>
@@ -10219,7 +10242,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>82</v>
       </c>
@@ -10249,7 +10272,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>83</v>
       </c>
@@ -10282,7 +10305,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>84</v>
       </c>
@@ -10507,7 +10530,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>97</v>
       </c>
@@ -10540,7 +10563,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code.</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>100</v>
       </c>
@@ -10573,7 +10596,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>101</v>
       </c>
@@ -10606,7 +10629,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="81" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>102</v>
       </c>
@@ -10639,7 +10662,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="82" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>103</v>
       </c>
@@ -10672,7 +10695,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>104</v>
       </c>
@@ -10961,7 +10984,7 @@
   <autoFilter ref="A1:K91" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
     <filterColumn colId="1">
       <filters>
-        <filter val="DiagnosticReport"/>
+        <filter val="Observation"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
add sr sps and notes
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FF0F96-4720-E045-8B8B-254F201CBDD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAD592F-5DF0-274C-A162-2AA740C5E904}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$91</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$107</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="604">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="617">
   <si>
     <t>Element</t>
   </si>
@@ -2051,6 +2051,45 @@
 To get Practitioner name and identifier using PractitionerRole:  
 1) Search for the careteam PractitionerRole: GET [base]/CareTeam?patient=[id]&amp;status=active&amp;_include=CareTeam:participant:PractitionerRole  
 2) using the FHIR _id from the PractitionerRole.practitioner element resource,  fetch the Practitioner resources using  GET [base]/Practitioner?_id=[id]</t>
+  </si>
+  <si>
+    <t>ServiceRequest</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest-note</t>
+  </si>
+  <si>
+    <t>support searching for reports by code and date DOES THIS DO ANYTHING!!!!</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=1137192&amp;status=completed</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=f201&amp;category=http://loinc.org\|LG41762-2&amp;date=ge2010-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=f201&amp;category=http://loinc.org\|LG41762-2</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=1032702&amp;code=http://snomed.info/sct|35637008</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=f201&amp;code=http://snomed.info/sct|35637008&amp;date=ge2019-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>support fetching a ServiceRequest</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest/1032702~GET [base]/ServiceRequest?_id=1032702</t>
+  </si>
+  <si>
+    <t>authored</t>
+  </si>
+  <si>
+    <t>patient,category,authored</t>
+  </si>
+  <si>
+    <t>patient,code,authored</t>
   </si>
 </sst>
 </file>
@@ -2683,13 +2722,13 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB102"/>
+  <dimension ref="A1:AB108"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G77" sqref="G77"/>
+      <selection pane="bottomRight" activeCell="C109" sqref="C109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3904,7 +3943,7 @@
         <v>SearchParameter-us-core-encounter-discharge-disposition.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -3954,7 +3993,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -4002,7 +4041,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -4049,7 +4088,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -4098,7 +4137,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -4142,7 +4181,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -4199,7 +4238,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -6527,7 +6566,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>69</v>
       </c>
@@ -6547,7 +6586,7 @@
         <v>525</v>
       </c>
       <c r="G73" s="1" t="str">
-        <f t="shared" ref="G73:G102" si="40">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B73)</f>
+        <f t="shared" ref="G73:G103" si="40">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B73)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H73" s="1" t="s">
@@ -6580,7 +6619,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>70</v>
       </c>
@@ -6630,7 +6669,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>71</v>
       </c>
@@ -6683,7 +6722,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -6737,7 +6776,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>73</v>
       </c>
@@ -7331,7 +7370,7 @@
         <v>91</v>
       </c>
       <c r="L87" s="1" t="str">
-        <f t="shared" ref="L87:L102" si="51">B87&amp;"."&amp;C87</f>
+        <f t="shared" ref="L87:L108" si="51">B87&amp;"."&amp;C87</f>
         <v>Device.patient</v>
       </c>
       <c r="M87" s="1" t="s">
@@ -8193,11 +8232,350 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
+    <row r="103" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>49</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C103" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E103" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F103" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="G103" s="1" t="str">
+        <f t="shared" si="40"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I103" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J103" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L103" s="1" t="str">
+        <f t="shared" si="51"/>
+        <v>ServiceRequest.status</v>
+      </c>
+      <c r="M103" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N103" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O103" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y103" s="5"/>
+      <c r="Z103" s="5"/>
+      <c r="AA103" s="12"/>
+      <c r="AB103" s="1" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B103)&amp;"-"&amp;C103&amp;".html")</f>
+        <v>SearchParameter-us-core-servicerequest-status.html</v>
+      </c>
+    </row>
+    <row r="104" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>50</v>
+      </c>
+      <c r="B104" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C104" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D104" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E104" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F104" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="G104" s="1" t="str">
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B104)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I104" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L104" s="1" t="str">
+        <f t="shared" si="51"/>
+        <v>ServiceRequest.patient</v>
+      </c>
+      <c r="M104" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O104" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y104" s="1" t="str">
+        <f>"support searching for all "&amp;LOWER(B104)&amp;"s for a patient"</f>
+        <v>support searching for all servicerequests for a patient</v>
+      </c>
+      <c r="Z104" s="5" t="str">
+        <f>"GET [base]/"&amp;B104&amp;"?patient=1137192"</f>
+        <v>GET [base]/ServiceRequest?patient=1137192</v>
+      </c>
+      <c r="AA104" s="12" t="str">
+        <f>"Fetches a bundle of all "&amp;B104&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient</v>
+      </c>
+      <c r="AB104" s="1" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B104)&amp;"-"&amp;C104&amp;".html")</f>
+        <v>SearchParameter-us-core-servicerequest-patient.html</v>
+      </c>
+    </row>
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>51</v>
+      </c>
+      <c r="B105" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C105" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D105" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E105" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F105" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="G105" s="1" t="str">
+        <f t="shared" ref="G105:G108" si="56">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I105" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J105" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L105" s="1" t="str">
+        <f t="shared" si="51"/>
+        <v>ServiceRequest.category</v>
+      </c>
+      <c r="M105" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O105" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y105" s="5"/>
+      <c r="Z105" s="5"/>
+      <c r="AA105" s="12"/>
+      <c r="AB105" s="1" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B105)&amp;"-"&amp;C105&amp;".html")</f>
+        <v>SearchParameter-us-core-servicerequest-category.html</v>
+      </c>
+    </row>
+    <row r="106" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>52</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E106" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F106" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="G106" s="1" t="str">
+        <f t="shared" si="56"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I106" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L106" s="1" t="str">
+        <f t="shared" si="51"/>
+        <v>ServiceRequest.code</v>
+      </c>
+      <c r="M106" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="N106" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O106" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y106" s="5"/>
+      <c r="Z106" s="5"/>
+      <c r="AA106" s="12"/>
+      <c r="AB106" s="1" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B106)&amp;"-"&amp;C106&amp;".html")</f>
+        <v>SearchParameter-us-core-servicerequest-code.html</v>
+      </c>
+    </row>
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>53</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E107" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F107" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="G107" s="1" t="str">
+        <f t="shared" si="56"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I107" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="L107" s="1" t="str">
+        <f t="shared" si="51"/>
+        <v>ServiceRequest.authored</v>
+      </c>
+      <c r="M107" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O107" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="P107" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="S107" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA107" s="12"/>
+      <c r="AB107" s="1" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B107)&amp;"-"&amp;C107&amp;".html")</f>
+        <v>SearchParameter-us-core-servicerequest-authored.html</v>
+      </c>
+    </row>
+    <row r="108" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A108" s="1">
+        <v>20</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E108" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G108" s="1" t="str">
+        <f t="shared" si="56"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I108" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L108" s="1" t="str">
+        <f t="shared" si="51"/>
+        <v>ServiceRequest._id</v>
+      </c>
+      <c r="M108" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O108" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y108" s="5" t="s">
+        <v>612</v>
+      </c>
+      <c r="Z108" s="5" t="s">
+        <v>613</v>
+      </c>
+      <c r="AA108" s="2"/>
+      <c r="AB108" s="1" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B108)&amp;"-"&amp;SUBSTITUTE(C108,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-servicerequest-id.html</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AB102" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
+  <autoFilter ref="A1:AB107" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Observation"/>
+        <filter val="Patient"/>
+        <filter val="ServiceRequest"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8213,10 +8591,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:Q91"/>
+  <dimension ref="A1:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9522,7 +9900,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>49</v>
       </c>
@@ -9552,7 +9930,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>50</v>
       </c>
@@ -9585,7 +9963,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>51</v>
       </c>
@@ -9615,7 +9993,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>52</v>
       </c>
@@ -9648,7 +10026,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>53</v>
       </c>
@@ -9678,7 +10056,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>56</v>
       </c>
@@ -9708,7 +10086,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>57</v>
       </c>
@@ -9738,7 +10116,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>58</v>
       </c>
@@ -9768,7 +10146,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>59</v>
       </c>
@@ -9798,7 +10176,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>60</v>
       </c>
@@ -9828,7 +10206,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>63</v>
       </c>
@@ -9859,7 +10237,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>64</v>
       </c>
@@ -9890,7 +10268,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>67</v>
       </c>
@@ -9923,7 +10301,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>68</v>
       </c>
@@ -9956,7 +10334,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>69</v>
       </c>
@@ -9989,7 +10367,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>70</v>
       </c>
@@ -10022,7 +10400,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>73</v>
       </c>
@@ -10053,7 +10431,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <f>SUBTOTAL(9,M103)</f>
         <v>0</v>
@@ -10084,7 +10462,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>75</v>
       </c>
@@ -10115,7 +10493,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>76</v>
       </c>
@@ -10146,7 +10524,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>77</v>
       </c>
@@ -10177,7 +10555,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>80</v>
       </c>
@@ -10209,7 +10587,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>81</v>
       </c>
@@ -10242,7 +10620,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>82</v>
       </c>
@@ -10272,7 +10650,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>83</v>
       </c>
@@ -10305,7 +10683,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>84</v>
       </c>
@@ -10530,7 +10908,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>97</v>
       </c>
@@ -10563,7 +10941,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code.</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>100</v>
       </c>
@@ -10596,7 +10974,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>101</v>
       </c>
@@ -10629,7 +11007,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="81" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>102</v>
       </c>
@@ -10662,7 +11040,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="82" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>103</v>
       </c>
@@ -10695,7 +11073,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>104</v>
       </c>
@@ -10980,11 +11358,176 @@
         <v>598</v>
       </c>
     </row>
+    <row r="92" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>56</v>
+      </c>
+      <c r="B92" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C92" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="E92" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F92" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I92" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="J92" s="5" t="s">
+        <v>607</v>
+      </c>
+      <c r="K92" s="5" t="str">
+        <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="93" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>57</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C93" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E93" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I93" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="J93" s="5" t="s">
+        <v>609</v>
+      </c>
+      <c r="K93" s="5" t="str">
+        <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient and  a category code"</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
+      </c>
+    </row>
+    <row r="94" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>58</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C94" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E94" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G94" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I94" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="J94" s="5" t="s">
+        <v>610</v>
+      </c>
+      <c r="K94" s="5" t="str">
+        <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
+    <row r="95" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>59</v>
+      </c>
+      <c r="B95" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C95" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="E95" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F95" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G95" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I95" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="J95" s="5" t="s">
+        <v>608</v>
+      </c>
+      <c r="K95" s="5" t="str">
+        <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date and a category code"</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
+      </c>
+    </row>
+    <row r="96" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="1">
+        <v>60</v>
+      </c>
+      <c r="B96" s="1" t="s">
+        <v>604</v>
+      </c>
+      <c r="C96" s="11" t="s">
+        <v>605</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="E96" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G96" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="I96" s="5" t="s">
+        <v>606</v>
+      </c>
+      <c r="J96" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="K96" s="5" t="str">
+        <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K91" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Observation"/>
+        <filter val="DiagnosticReport"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
fix prov white list formatting
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41A323F7-6BB6-FD44-93AE-E8B674140E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F1AC66-1FCD-D44E-8D58-B5630EA13F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2068,12 +2068,6 @@
     <t>GET [base]/ServiceRequest?patient=f201&amp;category=http://loinc.org\|LG41762-2</t>
   </si>
   <si>
-    <t>GET [base]/ServiceRequest?patient=1032702&amp;code=http://snomed.info/sct|35637008</t>
-  </si>
-  <si>
-    <t>GET [base]/ServiceRequest?patient=f201&amp;code=http://snomed.info/sct|35637008&amp;date=ge2019-01-14T00:00:00Z</t>
-  </si>
-  <si>
     <t>support fetching a ServiceRequest</t>
   </si>
   <si>
@@ -2090,6 +2084,12 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=f201&amp;code=http://snomed.info/sct\|35637008&amp;date=ge2019-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=1032702&amp;code=http://snomed.info/sct\|35637008</t>
   </si>
 </sst>
 </file>
@@ -8467,7 +8467,7 @@
         <v>604</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>30</v>
@@ -8559,10 +8559,10 @@
         <v>56</v>
       </c>
       <c r="Y108" s="5" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="Z108" s="5" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="AA108" s="2"/>
       <c r="AB108" s="1" t="str">
@@ -8593,8 +8593,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q96"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J99" sqref="J99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11366,7 +11366,7 @@
         <v>604</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>116</v>
@@ -11399,7 +11399,7 @@
         <v>604</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>145</v>
@@ -11432,7 +11432,7 @@
         <v>604</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>147</v>
@@ -11450,7 +11450,7 @@
         <v>200</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>609</v>
+        <v>616</v>
       </c>
       <c r="K94" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11465,10 +11465,10 @@
         <v>604</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="E95" s="1" t="b">
         <v>1</v>
@@ -11498,10 +11498,10 @@
         <v>604</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="E96" s="1" t="b">
         <v>1</v>
@@ -11516,7 +11516,7 @@
         <v>605</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>610</v>
+        <v>615</v>
       </c>
       <c r="K96" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>

</xml_diff>

<commit_message>
add goal description sp
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25F1AC66-1FCD-D44E-8D58-B5630EA13F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFDF557-D469-F648-9A20-DB77D19FDF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,8 +26,8 @@
     <sheet name="sp_combos" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$91</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$108</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2307" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="620">
   <si>
     <t>Element</t>
   </si>
@@ -2091,12 +2091,21 @@
   <si>
     <t>GET [base]/ServiceRequest?patient=1032702&amp;code=http://snomed.info/sct\|35637008</t>
   </si>
+  <si>
+    <t>patient,description</t>
+  </si>
+  <si>
+    <t>support searching for all goals for a patient by date DOES THIS DO ANYTHING!!!</t>
+  </si>
+  <si>
+    <t>GET [base]/Goal?patient=1137192&amp;description=http://snomed.info/sct\|1078229009</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2191,12 +2200,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2722,13 +2725,13 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB108"/>
+  <dimension ref="A1:AB109"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C58" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C109" sqref="C109"/>
+      <selection pane="bottomRight" activeCell="D114" sqref="D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3943,7 +3946,7 @@
         <v>SearchParameter-us-core-encounter-discharge-disposition.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -3993,7 +3996,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -4041,7 +4044,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -4088,7 +4091,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -4137,7 +4140,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -4181,7 +4184,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -4238,7 +4241,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -5758,7 +5761,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -5808,7 +5811,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -5867,7 +5870,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -7370,7 +7373,7 @@
         <v>91</v>
       </c>
       <c r="L87" s="1" t="str">
-        <f t="shared" ref="L87:L108" si="51">B87&amp;"."&amp;C87</f>
+        <f t="shared" ref="L87:L109" si="51">B87&amp;"."&amp;C87</f>
         <v>Device.patient</v>
       </c>
       <c r="M87" s="1" t="s">
@@ -8232,7 +8235,7 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="103" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>49</v>
       </c>
@@ -8288,7 +8291,7 @@
         <v>SearchParameter-us-core-servicerequest-status.html</v>
       </c>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>50</v>
       </c>
@@ -8350,7 +8353,7 @@
         <v>SearchParameter-us-core-servicerequest-patient.html</v>
       </c>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>51</v>
       </c>
@@ -8370,7 +8373,7 @@
         <v>525</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f t="shared" ref="G105:G108" si="56">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
+        <f t="shared" ref="G105:G109" si="56">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H105" s="1" t="s">
@@ -8403,7 +8406,7 @@
         <v>SearchParameter-us-core-servicerequest-category.html</v>
       </c>
     </row>
-    <row r="106" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>52</v>
       </c>
@@ -8459,7 +8462,7 @@
         <v>SearchParameter-us-core-servicerequest-code.html</v>
       </c>
     </row>
-    <row r="107" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>53</v>
       </c>
@@ -8516,7 +8519,7 @@
         <v>SearchParameter-us-core-servicerequest-authored.html</v>
       </c>
     </row>
-    <row r="108" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>20</v>
       </c>
@@ -8570,12 +8573,60 @@
         <v>SearchParameter-us-core-servicerequest-id.html</v>
       </c>
     </row>
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>56</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E109" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="F109" s="2"/>
+      <c r="G109" s="1" t="str">
+        <f t="shared" si="56"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I109" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L109" s="1" t="str">
+        <f t="shared" si="51"/>
+        <v>Goal.description</v>
+      </c>
+      <c r="M109" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O109" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="AA109" s="12"/>
+      <c r="AB109" s="1" t="str">
+        <f t="shared" ref="AB109" si="57">"SearchParameter-us-core-"&amp;LOWER((B109)&amp;"-"&amp;C109&amp;".html")</f>
+        <v>SearchParameter-us-core-goal-description.html</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AB107" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
+  <autoFilter ref="A1:AB108" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Patient"/>
-        <filter val="ServiceRequest"/>
+        <filter val="Goal"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8591,10 +8642,10 @@
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:Q96"/>
+  <dimension ref="A1:Q97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J99" sqref="J99"/>
+      <selection activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9900,7 +9951,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>49</v>
       </c>
@@ -9930,7 +9981,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>50</v>
       </c>
@@ -9963,7 +10014,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>51</v>
       </c>
@@ -9993,7 +10044,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>52</v>
       </c>
@@ -10026,7 +10077,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>53</v>
       </c>
@@ -10056,7 +10107,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>56</v>
       </c>
@@ -10086,7 +10137,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>57</v>
       </c>
@@ -10116,7 +10167,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>58</v>
       </c>
@@ -10146,7 +10197,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>59</v>
       </c>
@@ -10176,7 +10227,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>60</v>
       </c>
@@ -10206,7 +10257,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>63</v>
       </c>
@@ -10237,7 +10288,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="57" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>64</v>
       </c>
@@ -11358,7 +11409,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="92" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>56</v>
       </c>
@@ -11391,7 +11442,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="93" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>57</v>
       </c>
@@ -11424,7 +11475,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
       </c>
     </row>
-    <row r="94" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>58</v>
       </c>
@@ -11457,7 +11508,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="95" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>59</v>
       </c>
@@ -11490,7 +11541,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
       </c>
     </row>
-    <row r="96" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>60</v>
       </c>
@@ -11523,11 +11574,45 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
+    <row r="97" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>64</v>
+      </c>
+      <c r="B97" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C97" s="1" t="str">
+        <f t="shared" ref="C97" si="10">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B97)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="E97" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="I97" s="5" t="s">
+        <v>618</v>
+      </c>
+      <c r="J97" s="5" t="s">
+        <v>619</v>
+      </c>
+      <c r="K97" s="5" t="str">
+        <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified "&amp;SUBSTITUTE(D97,","," and ")</f>
+        <v>Fetches a bundle of all Goal resources for the specified patient and description</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K91" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
+  <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
     <filterColumn colId="1">
       <filters>
-        <filter val="DiagnosticReport"/>
+        <filter val="Goal"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
add related relatedperson search, update capabiltystatement, FHIR-33069
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFDF557-D469-F648-9A20-DB77D19FDF2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C26BC1-3582-1F41-B01F-BA5263019F51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-22340" yWindow="-21140" windowWidth="45560" windowHeight="21140" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -27,7 +27,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$96</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$108</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$111</definedName>
   </definedNames>
   <calcPr calcId="191029" refMode="R1C1"/>
   <extLst>
@@ -152,7 +152,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2398" uniqueCount="638">
   <si>
     <t>Element</t>
   </si>
@@ -1409,10 +1409,6 @@
   </si>
   <si>
     <t>The DocumentReference.type binding SHALL support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set</t>
-  </si>
-  <si>
-    <t>1. See the [General Security Considerations](security.html) section for requirements and recommendations.
-1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` unauthorized response code.</t>
   </si>
   <si>
     <t>US Core Laboratory Result Observation Profile</t>
@@ -1566,9 +1562,6 @@
     <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order,plan` and authoredon date</t>
   </si>
   <si>
-    <t>3.1.1</t>
-  </si>
-  <si>
     <t>4.0.1</t>
   </si>
   <si>
@@ -1600,9 +1593,6 @@
   </si>
   <si>
     <t>publishervalue</t>
-  </si>
-  <si>
-    <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ONC 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and and the ONC [U.S. Core Data for Interoperability (USCDI)](https://www.healthit.gov/isa/sites/isa/files/2020-03/USCDI-Version1-2020-Final-Standard.pdf).  US Core Clients have the option of choosing from this list to access necessary data based on their local use cases and other contextual requirements.</t>
   </si>
   <si>
     <t>!http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationstatement</t>
@@ -1710,10 +1700,6 @@
   </si>
   <si>
     <t>* The US Core Location  and PractitionerRole Profiles are not explicitly referenced in any US Core Profile. However they **SHOULD** be used as the default profile if referenced by another US Core profile.</t>
-  </si>
-  <si>
-    <t>* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent laboratory tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
-* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it.</t>
   </si>
   <si>
     <t xml:space="preserve">* For ONC's USCDI requirements, each Patient must support the following additional elements. These elements are included in the formal definition of the profile. The patient examples include all of these elements.
@@ -1933,9 +1919,6 @@
     - distinct identifier</t>
   </si>
   <si>
-    <t>http://fhir-registry.smarthealthit.org</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/uv/bulkdata/ImplementationGuide/hl7.fhir.uv.bulkdata</t>
   </si>
   <si>
@@ -2099,6 +2082,86 @@
   </si>
   <si>
     <t>GET [base]/Goal?patient=1137192&amp;description=http://snomed.info/sct\|1078229009</t>
+  </si>
+  <si>
+    <t>1. See the [General Security Considerations](security.html) section for requirements and recommendations.
+1. A server **SHALL** reject any unauthorized requests by returning an `HTTP 401` "Unauthorized", `HTTP 403` "Forbidden", or `HTTP 404` "Not Found"</t>
+  </si>
+  <si>
+    <t>5.0.0</t>
+  </si>
+  <si>
+    <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ONC 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and the ONC [U.S. Core Data for Interoperability (USCDI) Version 2 July 2021](https://www.healthit.gov/isa/sites/isa/files/2021-07/USCDI-Version-2-July-2021-Final.pdf).  US Core Clients have the option of choosing from this list to access necessary data based on their local use cases and other contextual requirements.</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/smart-app-launch/ImplementationGuide/hl7.fhir.uv.smart-app-launch</t>
+  </si>
+  <si>
+    <t>US Core Clinical Test Result Observation Profile</t>
+  </si>
+  <si>
+    <t>US Core RelatedPerson Profile</t>
+  </si>
+  <si>
+    <t>US Core Screening Response Observation Profile</t>
+  </si>
+  <si>
+    <t>US Core ServiceRequest Profile</t>
+  </si>
+  <si>
+    <t>US Core Social History Assessment Observation Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</t>
+  </si>
+  <si>
+    <t>US Core Diagnostic Imaging Result Observation Profile</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-clinical-test</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-social-history-assessment</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-screening-response</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-imaging</t>
+  </si>
+  <si>
+    <t>RelatedPerson</t>
+  </si>
+  <si>
+    <t>In order to access care team member's names, identifiers, locations, and contact information, the CareTeam profile supports several types of care team participants. They are represented as references to other profiles and include the following four profiles which are marked as must support:
+  1. US Core Practitioner Profile
+  1. US Core PractitionerRole Profile
+  1. US Core Patient Profile
+  1. US Core RelatedPerson Profile
+  * Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references (and `_include` search parameters), but **SHALL** support *at least* one of them.
+  * The client application **SHALL** support all four profile references.
+  * Bacause the US Core PractitionerRole Profile supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the US Core Practitioner Profile. An example of how to access the practitioner name and identifier is shown in the quick start section below.
+  * Servers that supports only US Core Practitioner Profile **SHALL** provide implementation specific guidance how to access a provider's location and contact information using only the Practitioner resource.</t>
+  </si>
+  <si>
+    <t>* Systems **SHOULD** support `Observation.effectivePeriod` to accurately represent tests that are collected over a period of time (for example, a 24-Hour Urine Collection test).
+* An Observation without a value, **SHALL** include a reason why the data is absent unless there are component observations, or references to other Observations that are grouped within it
+    * Systems that never provide an observation without a value are not required to support `Observation.dataAbsentReason`</t>
+  </si>
+  <si>
+    <t>SHOULD,SHOULD,SHOULD,SHOULD</t>
+  </si>
+  <si>
+    <t>conf_RelatedPerson</t>
+  </si>
+  <si>
+    <t>conf_ServiceRequest</t>
+  </si>
+  <si>
+    <t>support fetching a RelatedPerson</t>
+  </si>
+  <si>
+    <t>GET [base]/RelatedPerson/shaw-niece~GET [base]/RelatedPerson?_id=shaw-niece</t>
   </si>
 </sst>
 </file>
@@ -2652,34 +2715,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B2" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="B3" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="B4" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
       <c r="B5" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2687,12 +2750,12 @@
         <v>68</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
@@ -2700,15 +2763,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="B8" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -2725,13 +2788,13 @@
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:AB109"/>
+  <dimension ref="A1:AB111"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C58" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="U23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D114" sqref="D114"/>
+      <selection pane="bottomRight" activeCell="Z113" sqref="Z113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2779,7 +2842,7 @@
         <v>41</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>32</v>
@@ -3001,7 +3064,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3209,7 +3272,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3258,7 +3321,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3320,7 +3383,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3371,7 +3434,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3419,7 +3482,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3530,7 +3593,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3580,7 +3643,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3634,7 +3697,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3691,7 +3754,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3740,7 +3803,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>585</v>
+        <v>580</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>30</v>
@@ -3749,7 +3812,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G19" s="1" t="str">
         <f t="shared" ref="G19" si="8">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B19)</f>
@@ -3810,7 +3873,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3860,7 +3923,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G21" s="1" t="str">
         <f t="shared" ref="G21" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
@@ -3901,7 +3964,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>586</v>
+        <v>581</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>30</v>
@@ -3910,7 +3973,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3946,7 +4009,7 @@
         <v>SearchParameter-us-core-encounter-discharge-disposition.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -3996,7 +4059,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -4013,7 +4076,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="G24" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4044,7 +4107,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -4061,7 +4124,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="G25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4091,7 +4154,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -4108,7 +4171,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G26" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4140,7 +4203,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -4184,7 +4247,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -4201,7 +4264,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4241,7 +4304,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -4282,7 +4345,7 @@
       </c>
       <c r="S29"/>
       <c r="Y29" s="5" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="Z29" s="1" t="s">
         <v>173</v>
@@ -4638,7 +4701,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4683,7 +4746,7 @@
         <v>138</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>570</v>
+        <v>565</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>30</v>
@@ -4692,7 +4755,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G38" s="1" t="str">
         <f t="shared" ref="G38:G40" si="16">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B38)</f>
@@ -4740,7 +4803,7 @@
         <v>138</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>571</v>
+        <v>566</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>30</v>
@@ -4749,7 +4812,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G39" s="1" t="str">
         <f t="shared" si="16"/>
@@ -4797,7 +4860,7 @@
         <v>138</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>572</v>
+        <v>567</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>30</v>
@@ -4806,7 +4869,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G40" s="1" t="str">
         <f t="shared" si="16"/>
@@ -4863,7 +4926,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G41" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4904,7 +4967,7 @@
         <v>138</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>30</v>
@@ -4913,7 +4976,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G42" s="1" t="str">
         <f t="shared" ref="G42" si="19">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B42)</f>
@@ -4942,7 +5005,7 @@
         <v>56</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>573</v>
+        <v>568</v>
       </c>
       <c r="Z42" s="5" t="str">
         <f>"GET [base]/"&amp;B42&amp;"?patient=1137192"</f>
@@ -4974,7 +5037,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G43" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5033,7 +5096,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G44" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5083,7 +5146,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G45" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5190,7 +5253,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G47" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5243,7 +5306,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G48" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5302,7 +5365,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G49" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5352,7 +5415,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G50" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5402,7 +5465,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G51" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5456,7 +5519,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G52" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5509,7 +5572,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G53" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5562,7 +5625,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G54" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B54)</f>
@@ -5621,7 +5684,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G55" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5671,7 +5734,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G56" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5724,7 +5787,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G57" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5761,7 +5824,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -5778,7 +5841,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G58" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5811,7 +5874,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -5828,7 +5891,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G59" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5870,7 +5933,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -5887,7 +5950,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="G60" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5941,7 +6004,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G61" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5985,7 +6048,7 @@
         <v>181</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>30</v>
@@ -5994,7 +6057,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G62" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6047,7 +6110,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G63" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6089,7 +6152,7 @@
         <v>181</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>30</v>
@@ -6098,7 +6161,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G64" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6149,7 +6212,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G65" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6191,7 +6254,7 @@
         <v>62</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>62</v>
@@ -6203,7 +6266,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G66" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6244,7 +6307,7 @@
         <v>63</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>90</v>
@@ -6256,7 +6319,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G67" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6302,7 +6365,7 @@
         <v>64</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>229</v>
@@ -6314,7 +6377,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G68" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6368,7 +6431,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G69" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6421,7 +6484,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G70" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6479,7 +6542,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G71" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6533,7 +6596,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G72" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6586,7 +6649,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G73" s="1" t="str">
         <f t="shared" ref="G73:G103" si="40">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B73)</f>
@@ -6639,7 +6702,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G74" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6689,7 +6752,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G75" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6742,7 +6805,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G76" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6796,7 +6859,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G77" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6855,7 +6918,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G78" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6905,7 +6968,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G79" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6955,7 +7018,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G80" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7009,7 +7072,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G81" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7068,7 +7131,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G82" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7104,7 +7167,7 @@
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>79</v>
       </c>
@@ -7121,7 +7184,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G83" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7147,7 +7210,7 @@
         <v>56</v>
       </c>
       <c r="X83" s="1" t="s">
-        <v>599</v>
+        <v>594</v>
       </c>
       <c r="Y83" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B83)&amp;"s for a patient"</f>
@@ -7217,14 +7280,14 @@
         <v>GET [base]/Practitioner/practitioner-1~GET [base]/Practitioner?_id=practitioner-1</v>
       </c>
       <c r="AA84" s="12" t="s">
-        <v>593</v>
+        <v>588</v>
       </c>
       <c r="AB84" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B84)&amp;"-"&amp;SUBSTITUTE(C84,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-practitioner-id.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>80</v>
       </c>
@@ -7241,7 +7304,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G85" s="1" t="str">
         <f t="shared" ref="G85" si="47">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B85)</f>
@@ -7277,7 +7340,7 @@
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>80</v>
       </c>
@@ -7285,7 +7348,7 @@
         <v>249</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>591</v>
+        <v>586</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>70</v>
@@ -7294,7 +7357,7 @@
         <v>0</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G86" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7326,15 +7389,13 @@
         <v>56</v>
       </c>
       <c r="Y86" s="5" t="s">
-        <v>592</v>
+        <v>587</v>
       </c>
       <c r="Z86" s="5" t="str">
         <f>"GET [base]/"&amp;B86&amp;"?"&amp;C86&amp;"=http://snomed.info/sct\|17561000"</f>
         <v>GET [base]/CareTeam?role=http://snomed.info/sct\|17561000</v>
       </c>
-      <c r="AA86" s="12" t="s">
-        <v>593</v>
-      </c>
+      <c r="AA86" s="12"/>
       <c r="AB86" s="1" t="str">
         <f t="shared" ref="AB86" si="50">"SearchParameter-us-core-"&amp;LOWER((B86)&amp;"-"&amp;C86&amp;".html")</f>
         <v>SearchParameter-us-core-careteam-role.html</v>
@@ -7357,7 +7418,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G87" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B87)</f>
@@ -7373,7 +7434,7 @@
         <v>91</v>
       </c>
       <c r="L87" s="1" t="str">
-        <f t="shared" ref="L87:L109" si="51">B87&amp;"."&amp;C87</f>
+        <f t="shared" ref="L87:L110" si="51">B87&amp;"."&amp;C87</f>
         <v>Device.patient</v>
       </c>
       <c r="M87" s="1" t="s">
@@ -7416,7 +7477,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G88" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B88)</f>
@@ -8069,7 +8130,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G100" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8127,7 +8188,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G101" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8188,7 +8249,7 @@
         <v>1</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G102" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8240,7 +8301,7 @@
         <v>49</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>62</v>
@@ -8252,7 +8313,7 @@
         <v>0</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G103" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8296,7 +8357,7 @@
         <v>50</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>90</v>
@@ -8308,7 +8369,7 @@
         <v>1</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="G104" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B104)</f>
@@ -8358,7 +8419,7 @@
         <v>51</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>140</v>
@@ -8370,10 +8431,10 @@
         <v>0</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G105" s="1" t="str">
-        <f t="shared" ref="G105:G109" si="56">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
+        <f t="shared" ref="G105:G111" si="56">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H105" s="1" t="s">
@@ -8411,7 +8472,7 @@
         <v>52</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>26</v>
@@ -8423,7 +8484,7 @@
         <v>0</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="G106" s="1" t="str">
         <f t="shared" si="56"/>
@@ -8467,10 +8528,10 @@
         <v>53</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>30</v>
@@ -8479,7 +8540,7 @@
         <v>0</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="G107" s="1" t="str">
         <f t="shared" si="56"/>
@@ -8524,7 +8585,7 @@
         <v>20</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>55</v>
@@ -8562,10 +8623,10 @@
         <v>56</v>
       </c>
       <c r="Y108" s="5" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
       <c r="Z108" s="5" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
       <c r="AA108" s="2"/>
       <c r="AB108" s="1" t="str">
@@ -8573,7 +8634,7 @@
         <v>SearchParameter-us-core-servicerequest-id.html</v>
       </c>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>56</v>
       </c>
@@ -8622,11 +8683,129 @@
         <v>SearchParameter-us-core-goal-description.html</v>
       </c>
     </row>
+    <row r="110" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>20</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E110" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="G110" s="1" t="str">
+        <f t="shared" si="56"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I110" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="L110" s="1" t="str">
+        <f t="shared" si="51"/>
+        <v>RelatedPerson._id</v>
+      </c>
+      <c r="M110" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O110" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y110" s="5" t="s">
+        <v>636</v>
+      </c>
+      <c r="Z110" s="5" t="s">
+        <v>637</v>
+      </c>
+      <c r="AA110" s="12"/>
+      <c r="AB110" s="1" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B110)&amp;"-"&amp;SUBSTITUTE(C110,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-relatedperson-id.html</v>
+      </c>
+    </row>
+    <row r="111" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>79</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E111" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="F111" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="G111" s="1" t="str">
+        <f t="shared" si="56"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I111" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="K111" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="L111" s="1" t="str">
+        <f>B111&amp;"."&amp;C111</f>
+        <v>RelatedPerson.patient</v>
+      </c>
+      <c r="M111" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y111" s="1" t="str">
+        <f>"support searching for all "&amp;LOWER(B111)&amp;"s for a patient"</f>
+        <v>support searching for all relatedpersons for a patient</v>
+      </c>
+      <c r="Z111" s="5" t="str">
+        <f>"GET [base]/"&amp;B111&amp;"?patient=1032702"</f>
+        <v>GET [base]/RelatedPerson?patient=1032702</v>
+      </c>
+      <c r="AA111" s="12" t="str">
+        <f>"Fetches a bundle of all "&amp;B111&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all RelatedPerson resources for the specified patient</v>
+      </c>
+      <c r="AB111" s="1" t="str">
+        <f>"SearchParameter-us-core-"&amp;LOWER((B111)&amp;"-"&amp;C111&amp;".html")</f>
+        <v>SearchParameter-us-core-relatedperson-patient.html</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AB108" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
+  <autoFilter ref="A1:AB111" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Goal"/>
+        <filter val="CareTeam"/>
+        <filter val="Patient"/>
+        <filter val="RelatedPerson"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -8644,8 +8823,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="J102" sqref="J102"/>
+    <sheetView topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J102" sqref="A1:Q97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8677,7 +8856,7 @@
         <v>96</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>584</v>
+        <v>579</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>97</v>
@@ -9007,7 +9186,7 @@
         <v>305</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="K13" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9107,7 +9286,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>587</v>
+        <v>582</v>
       </c>
       <c r="E17" s="1" t="b">
         <v>1</v>
@@ -9122,7 +9301,7 @@
         <v>306</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>588</v>
+        <v>583</v>
       </c>
       <c r="K17" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9198,7 +9377,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>589</v>
+        <v>584</v>
       </c>
       <c r="E20" s="1" t="b">
         <v>1</v>
@@ -9213,7 +9392,7 @@
         <v>311</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>590</v>
+        <v>585</v>
       </c>
       <c r="K20" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9661,7 +9840,7 @@
         <v>150</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>146</v>
@@ -9679,7 +9858,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>577</v>
+        <v>572</v>
       </c>
       <c r="E37" s="1" t="b">
         <v>1</v>
@@ -9694,10 +9873,10 @@
         <v>150</v>
       </c>
       <c r="J37" s="5" t="s">
-        <v>582</v>
+        <v>577</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>583</v>
+        <v>578</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -9754,7 +9933,7 @@
         <v>153</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>578</v>
+        <v>573</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>156</v>
@@ -9772,7 +9951,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>574</v>
+        <v>569</v>
       </c>
       <c r="E40" s="1" t="b">
         <v>1</v>
@@ -9787,7 +9966,7 @@
         <v>153</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>579</v>
+        <v>574</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>156</v>
@@ -9805,7 +9984,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>575</v>
+        <v>570</v>
       </c>
       <c r="E41" s="1" t="b">
         <v>1</v>
@@ -9820,7 +9999,7 @@
         <v>153</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>580</v>
+        <v>575</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>156</v>
@@ -9838,7 +10017,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>576</v>
+        <v>571</v>
       </c>
       <c r="E42" s="1" t="b">
         <v>1</v>
@@ -9853,7 +10032,7 @@
         <v>153</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>581</v>
+        <v>576</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>156</v>
@@ -9886,7 +10065,7 @@
         <v>326</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -9913,7 +10092,7 @@
         <v>167</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="K44" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B44&amp;" resources for the specified "&amp;SUBSTITUTE(D44,","," and ")</f>
@@ -10070,7 +10249,7 @@
         <v>196</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="K49" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -10100,7 +10279,7 @@
         <v>227</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="K50" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10220,7 +10399,7 @@
         <v>202</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="K54" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -10250,7 +10429,7 @@
         <v>221</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="K55" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B55&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10331,7 +10510,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>12</v>
@@ -10340,16 +10519,16 @@
         <v>106</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>435</v>
+      </c>
+      <c r="J58" s="5" t="s">
         <v>462</v>
       </c>
-      <c r="I58" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>463</v>
-      </c>
       <c r="K58" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10364,7 +10543,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>12</v>
@@ -10373,16 +10552,16 @@
         <v>106</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>186</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10397,7 +10576,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>70</v>
@@ -10406,16 +10585,16 @@
         <v>106</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>186</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10430,7 +10609,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>70</v>
@@ -10439,16 +10618,16 @@
         <v>219</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>231</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -10456,7 +10635,7 @@
         <v>73</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C62" s="1" t="str">
         <f t="shared" si="8"/>
@@ -10488,7 +10667,7 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C63" s="1" t="str">
         <f t="shared" si="8"/>
@@ -10599,7 +10778,7 @@
         <v>228</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="K66" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -10614,7 +10793,7 @@
         <v>183</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>238</v>
@@ -10626,13 +10805,13 @@
         <v>106</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>281</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>322</v>
@@ -10646,7 +10825,7 @@
         <v>183</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>145</v>
@@ -10658,13 +10837,13 @@
         <v>106</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>222</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="K68" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -10679,7 +10858,7 @@
         <v>183</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>147</v>
@@ -10709,7 +10888,7 @@
         <v>183</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>195</v>
@@ -10721,13 +10900,13 @@
         <v>219</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>226</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="K70" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -10742,7 +10921,7 @@
         <v>183</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>220</v>
@@ -10757,7 +10936,7 @@
         <v>224</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="K71" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10772,7 +10951,7 @@
         <v>321</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>116</v>
@@ -10853,7 +11032,7 @@
         <v>242</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="K74" s="5" t="s">
         <v>246</v>
@@ -10917,7 +11096,7 @@
         <v>241</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>535</v>
+        <v>531</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>248</v>
@@ -10950,13 +11129,13 @@
         <v>312</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>594</v>
+        <v>589</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>600</v>
+        <v>595</v>
       </c>
       <c r="K77" s="12" t="s">
-        <v>603</v>
+        <v>598</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
@@ -11000,7 +11179,7 @@
         <v>183</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>238</v>
@@ -11012,13 +11191,13 @@
         <v>106</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>280</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K79" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B79&amp;" resources for the specified "&amp;SUBSTITUTE(D79,","," and ")</f>
@@ -11033,7 +11212,7 @@
         <v>183</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>145</v>
@@ -11045,13 +11224,13 @@
         <v>106</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>279</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="K80" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B80&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -11066,7 +11245,7 @@
         <v>183</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>147</v>
@@ -11078,7 +11257,7 @@
         <v>106</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>282</v>
@@ -11099,7 +11278,7 @@
         <v>183</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>195</v>
@@ -11111,13 +11290,13 @@
         <v>219</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>284</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="K82" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B82&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -11132,7 +11311,7 @@
         <v>183</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>220</v>
@@ -11147,7 +11326,7 @@
         <v>285</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>538</v>
+        <v>534</v>
       </c>
       <c r="K83" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes."</f>
@@ -11280,7 +11459,7 @@
         <v>297</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="K87" s="5" t="s">
         <v>299</v>
@@ -11340,7 +11519,7 @@
         <v>302</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>540</v>
+        <v>536</v>
       </c>
       <c r="K89" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -11355,7 +11534,7 @@
         <v>250</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>118</v>
@@ -11388,7 +11567,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>595</v>
+        <v>590</v>
       </c>
       <c r="E91" s="1" t="b">
         <v>1</v>
@@ -11400,13 +11579,13 @@
         <v>106</v>
       </c>
       <c r="I91" s="5" t="s">
-        <v>596</v>
+        <v>591</v>
       </c>
       <c r="J91" s="5" t="s">
-        <v>597</v>
+        <v>592</v>
       </c>
       <c r="K91" s="5" t="s">
-        <v>598</v>
+        <v>593</v>
       </c>
     </row>
     <row r="92" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
@@ -11414,10 +11593,10 @@
         <v>56</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>116</v>
@@ -11435,7 +11614,7 @@
         <v>304</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>606</v>
+        <v>601</v>
       </c>
       <c r="K92" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -11447,10 +11626,10 @@
         <v>57</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>145</v>
@@ -11468,7 +11647,7 @@
         <v>199</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>608</v>
+        <v>603</v>
       </c>
       <c r="K93" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient and  a category code"</f>
@@ -11480,10 +11659,10 @@
         <v>58</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>147</v>
@@ -11501,7 +11680,7 @@
         <v>200</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>616</v>
+        <v>611</v>
       </c>
       <c r="K94" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11513,13 +11692,13 @@
         <v>59</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
       <c r="E95" s="1" t="b">
         <v>1</v>
@@ -11534,7 +11713,7 @@
         <v>202</v>
       </c>
       <c r="J95" s="5" t="s">
-        <v>607</v>
+        <v>602</v>
       </c>
       <c r="K95" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date and a category code"</f>
@@ -11546,13 +11725,13 @@
         <v>60</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>604</v>
+        <v>599</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>614</v>
+        <v>609</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
       <c r="E96" s="1" t="b">
         <v>1</v>
@@ -11564,10 +11743,10 @@
         <v>219</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>605</v>
+        <v>600</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
       <c r="K96" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -11586,7 +11765,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>617</v>
+        <v>612</v>
       </c>
       <c r="E97" s="1" t="b">
         <v>1</v>
@@ -11598,10 +11777,10 @@
         <v>106</v>
       </c>
       <c r="I97" s="5" t="s">
-        <v>618</v>
+        <v>613</v>
       </c>
       <c r="J97" s="5" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="K97" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified "&amp;SUBSTITUTE(D97,","," and ")</f>
@@ -11629,8 +11808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD12"/>
+    <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11660,15 +11839,15 @@
         <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>470</v>
+        <v>616</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -11676,7 +11855,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>482</v>
+        <v>617</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -11692,7 +11871,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -11700,36 +11879,36 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>419</v>
+        <v>615</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>541</v>
+        <v>537</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>554</v>
+        <v>550</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>70</v>
@@ -11745,13 +11924,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="61.5" customWidth="1"/>
-    <col min="2" max="2" width="35.83203125" customWidth="1"/>
+    <col min="2" max="2" width="71" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -11760,7 +11939,7 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
@@ -11771,13 +11950,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>565</v>
+        <v>618</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>567</v>
+        <v>562</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -11785,13 +11964,13 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>566</v>
+        <v>561</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>70</v>
@@ -11828,16 +12007,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>552</v>
+        <v>548</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>60</v>
@@ -11851,13 +12030,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>569</v>
+        <v>564</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
@@ -11870,9 +12049,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -11962,10 +12143,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -12112,7 +12293,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>341</v>
@@ -12127,10 +12308,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>12</v>
@@ -12142,10 +12323,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>12</v>
@@ -12157,10 +12338,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>12</v>
@@ -12172,10 +12353,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
@@ -12187,10 +12368,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>12</v>
@@ -12202,10 +12383,10 @@
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>12</v>
@@ -12216,10 +12397,10 @@
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>12</v>
@@ -12230,10 +12411,10 @@
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>12</v>
@@ -12244,10 +12425,10 @@
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>12</v>
@@ -12258,10 +12439,10 @@
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>12</v>
@@ -12272,10 +12453,10 @@
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>12</v>
@@ -12286,10 +12467,10 @@
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>12</v>
@@ -12300,10 +12481,10 @@
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>12</v>
@@ -12314,10 +12495,10 @@
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>12</v>
@@ -12328,10 +12509,10 @@
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
-        <v>601</v>
+        <v>596</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>602</v>
+        <v>597</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>12</v>
@@ -12430,16 +12611,100 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>445</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>447</v>
-      </c>
       <c r="D38" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" s="11" t="s">
+        <v>626</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>619</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>620</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>628</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>621</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>622</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" s="11" t="s">
+        <v>627</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>623</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" s="11" t="s">
+        <v>629</v>
+      </c>
+      <c r="B44" s="11" t="s">
+        <v>625</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -12455,13 +12720,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Y59"/>
+  <dimension ref="A1:Y61"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomRight" activeCell="V4" sqref="V4:W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12494,7 +12759,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
@@ -12545,16 +12810,16 @@
         <v>412</v>
       </c>
       <c r="V1" s="4" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="W1" s="4" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="X1" s="4" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="Y1" s="4" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -12576,13 +12841,13 @@
         <v>70</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y2" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="163" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>235</v>
       </c>
@@ -12590,7 +12855,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>19</v>
@@ -12599,27 +12864,36 @@
         <v>70</v>
       </c>
       <c r="X3" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y3" s="17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="279" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>249</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C4" s="2" t="s">
+        <v>631</v>
+      </c>
       <c r="T4" s="1" t="s">
         <v>19</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>70</v>
       </c>
+      <c r="V4" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>594</v>
+      </c>
       <c r="X4" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y4" s="17" t="s">
         <v>12</v>
@@ -12639,7 +12913,7 @@
         <v>70</v>
       </c>
       <c r="X5" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y5" s="17" t="s">
         <v>12</v>
@@ -12653,7 +12927,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>19</v>
@@ -12662,7 +12936,7 @@
         <v>70</v>
       </c>
       <c r="X6" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y6" s="17" t="s">
         <v>12</v>
@@ -12682,7 +12956,7 @@
         <v>70</v>
       </c>
       <c r="X7" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y7" s="17" t="s">
         <v>12</v>
@@ -12705,7 +12979,7 @@
         <v>70</v>
       </c>
       <c r="X8" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y8" s="17" t="s">
         <v>12</v>
@@ -12719,7 +12993,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>19</v>
@@ -12728,7 +13002,7 @@
         <v>70</v>
       </c>
       <c r="X9" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y9" s="17" t="s">
         <v>12</v>
@@ -12748,7 +13022,7 @@
         <v>70</v>
       </c>
       <c r="X10" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y10" s="17" t="s">
         <v>12</v>
@@ -12762,7 +13036,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>19</v>
@@ -12771,7 +13045,7 @@
         <v>70</v>
       </c>
       <c r="X11" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y11" s="17" t="s">
         <v>12</v>
@@ -12785,7 +13059,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>19</v>
@@ -12804,7 +13078,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>19</v>
@@ -12823,7 +13097,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>19</v>
@@ -12838,7 +13112,7 @@
         <v>209</v>
       </c>
       <c r="X14" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y14" s="17" t="s">
         <v>12</v>
@@ -12846,13 +13120,13 @@
     </row>
     <row r="15" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>19</v>
@@ -12867,7 +13141,7 @@
         <v>401</v>
       </c>
       <c r="X15" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y15" s="17" t="s">
         <v>12</v>
@@ -12881,7 +13155,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>512</v>
+        <v>632</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>19</v>
@@ -12890,7 +13164,7 @@
         <v>70</v>
       </c>
       <c r="X16" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y16" s="17" t="s">
         <v>12</v>
@@ -12920,7 +13194,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="T18" s="1" t="s">
         <v>19</v>
@@ -12929,7 +13203,7 @@
         <v>70</v>
       </c>
       <c r="X18" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y18" s="17" t="s">
         <v>12</v>
@@ -12959,7 +13233,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="T20" s="1" t="s">
         <v>19</v>
@@ -12968,7 +13242,7 @@
         <v>70</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>274</v>
@@ -12984,7 +13258,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="T21" s="1" t="s">
         <v>19</v>
@@ -12993,7 +13267,7 @@
         <v>70</v>
       </c>
       <c r="X21" s="17" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="Y21" s="17" t="s">
         <v>12</v>
@@ -13001,13 +13275,13 @@
     </row>
     <row r="22" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>19</v>
@@ -13016,27 +13290,73 @@
         <v>70</v>
       </c>
     </row>
-    <row r="23" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>455</v>
+    <row r="23" spans="1:25" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>630</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24"/>
+        <v>12</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="T23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X23" s="17" t="s">
+        <v>457</v>
+      </c>
+      <c r="Y23" s="17" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="T24" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X24" s="17" t="s">
+        <v>457</v>
+      </c>
+      <c r="Y24" s="17" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="25" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25"/>
-    </row>
-    <row r="56" spans="22:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V56" s="7"/>
-      <c r="X56" s="7"/>
-      <c r="Y56" s="7"/>
-    </row>
-    <row r="59" spans="22:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y59" s="7"/>
+      <c r="A25" t="s">
+        <v>454</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26"/>
+    </row>
+    <row r="27" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27"/>
+    </row>
+    <row r="58" spans="22:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V58" s="7"/>
+      <c r="X58" s="7"/>
+      <c r="Y58" s="7"/>
+    </row>
+    <row r="61" spans="22:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y61" s="7"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A21">
@@ -13094,24 +13414,24 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>452</v>
+      </c>
+      <c r="B3" t="s">
         <v>453</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>454</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>455</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -13124,13 +13444,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W1" sqref="W1"/>
+      <selection pane="bottomRight" activeCell="T27" sqref="T27:T28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13144,10 +13464,13 @@
     <col min="14" max="14" width="17.33203125" customWidth="1"/>
     <col min="17" max="17" width="31.33203125" customWidth="1"/>
     <col min="18" max="18" width="31.33203125" style="1" customWidth="1"/>
-    <col min="24" max="24" width="20.1640625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="22.6640625" customWidth="1"/>
+    <col min="22" max="22" width="38.33203125" customWidth="1"/>
+    <col min="23" max="23" width="23" customWidth="1"/>
+    <col min="24" max="26" width="36.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:27" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -13167,7 +13490,7 @@
         <v>378</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>379</v>
@@ -13200,7 +13523,7 @@
         <v>388</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>389</v>
@@ -13218,13 +13541,19 @@
         <v>393</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="64" x14ac:dyDescent="0.2">
+        <v>634</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -13244,7 +13573,7 @@
         <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -13294,8 +13623,14 @@
       <c r="X2" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -13363,8 +13698,14 @@
       <c r="X3" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -13431,8 +13772,14 @@
       <c r="X4" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -13499,8 +13846,14 @@
       <c r="X5" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -13567,8 +13920,14 @@
       <c r="X6" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -13635,8 +13994,14 @@
       <c r="X7" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -13703,8 +14068,14 @@
       <c r="X8" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -13771,8 +14142,14 @@
       <c r="X9" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="Y9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z9" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -13837,6 +14214,12 @@
         <v>30</v>
       </c>
       <c r="X10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z10" s="1" t="s">
         <v>30</v>
       </c>
     </row>
@@ -13850,7 +14233,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13866,12 +14249,12 @@
         <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
@@ -13880,7 +14263,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
@@ -13889,7 +14272,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>30</v>
@@ -13898,7 +14281,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
update capabilitystatements for client and server
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{142091DD-0C7D-4144-9A88-23205F9C4C42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F1BCF8-F8F6-4541-B249-0A04F80B1A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-500" yWindow="-21140" windowWidth="18920" windowHeight="21140" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20520" yWindow="-21140" windowWidth="21640" windowHeight="21140" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -55,7 +55,7 @@
           <rPr>
             <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -64,7 +64,7 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -2233,19 +2233,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color rgb="FF333333"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -2280,6 +2267,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -2351,14 +2351,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -2804,14 +2804,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AB111"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="U23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Z113" sqref="Z113"/>
+      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2919,7 +2918,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="2" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2966,7 +2965,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3013,7 +3012,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3064,7 +3063,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3123,7 +3122,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3170,7 +3169,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3221,7 +3220,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3272,7 +3271,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3321,7 +3320,7 @@
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3383,7 +3382,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3434,7 +3433,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -3482,7 +3481,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -3540,7 +3539,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -3593,7 +3592,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -3643,7 +3642,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -3697,7 +3696,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -3754,7 +3753,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -3812,7 +3811,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -3873,7 +3872,7 @@
         <v>SearchParameter-us-core-encounter-location.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -3923,7 +3922,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -3973,7 +3972,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -4026,7 +4025,7 @@
         <v>SearchParameter-us-core-encounter-discharge-disposition.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -4376,7 +4375,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -4419,7 +4418,7 @@
         <v>SearchParameter-us-core-!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -4463,7 +4462,7 @@
         <v>SearchParameter-us-core-!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -4510,7 +4509,7 @@
         <v>SearchParameter-us-core-!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>30</v>
       </c>
@@ -4554,7 +4553,7 @@
         <v>SearchParameter-us-core-!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>31</v>
       </c>
@@ -4611,7 +4610,7 @@
         <v>SearchParameter-us-core-!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>32</v>
       </c>
@@ -4656,7 +4655,7 @@
         <v>SearchParameter-us-core-!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>33</v>
       </c>
@@ -4701,7 +4700,7 @@
         <v>SearchParameter-us-core-!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>34</v>
       </c>
@@ -4755,7 +4754,7 @@
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>35</v>
       </c>
@@ -4812,7 +4811,7 @@
         <v>SearchParameter-us-core-condition-asserted-date.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>36</v>
       </c>
@@ -4869,7 +4868,7 @@
         <v>SearchParameter-us-core-condition-recorded-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>37</v>
       </c>
@@ -4926,7 +4925,7 @@
         <v>SearchParameter-us-core-condition-abatement-date.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>38</v>
       </c>
@@ -4976,7 +4975,7 @@
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>12</v>
       </c>
@@ -5037,7 +5036,7 @@
         <v>SearchParameter-us-core-condition-encounter.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>39</v>
       </c>
@@ -5096,7 +5095,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>40</v>
       </c>
@@ -5146,7 +5145,7 @@
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>41</v>
       </c>
@@ -5200,7 +5199,7 @@
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>42</v>
       </c>
@@ -5253,7 +5252,7 @@
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43</v>
       </c>
@@ -5306,7 +5305,7 @@
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>44</v>
       </c>
@@ -5365,7 +5364,7 @@
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>45</v>
       </c>
@@ -5415,7 +5414,7 @@
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>46</v>
       </c>
@@ -5465,7 +5464,7 @@
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>47</v>
       </c>
@@ -5519,7 +5518,7 @@
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>48</v>
       </c>
@@ -5572,7 +5571,7 @@
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>49</v>
       </c>
@@ -5625,7 +5624,7 @@
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>50</v>
       </c>
@@ -5684,7 +5683,7 @@
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>51</v>
       </c>
@@ -5734,7 +5733,7 @@
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>52</v>
       </c>
@@ -5787,7 +5786,7 @@
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>53</v>
       </c>
@@ -5841,7 +5840,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -5891,7 +5890,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -5950,7 +5949,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -6004,7 +6003,7 @@
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>57</v>
       </c>
@@ -6057,7 +6056,7 @@
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>58</v>
       </c>
@@ -6110,7 +6109,7 @@
         <v>SearchParameter-us-core-medicationrequest-intent.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -6161,7 +6160,7 @@
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -6212,7 +6211,7 @@
         <v>SearchParameter-us-core-medicationrequest-encounter.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>61</v>
       </c>
@@ -6266,7 +6265,7 @@
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>62</v>
       </c>
@@ -6319,7 +6318,7 @@
         <v>SearchParameter-us-core-!medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>63</v>
       </c>
@@ -6377,7 +6376,7 @@
         <v>SearchParameter-us-core-!medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>64</v>
       </c>
@@ -6431,7 +6430,7 @@
         <v>SearchParameter-us-core-!medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>65</v>
       </c>
@@ -6484,7 +6483,7 @@
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>66</v>
       </c>
@@ -6542,7 +6541,7 @@
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>67</v>
       </c>
@@ -6596,7 +6595,7 @@
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>68</v>
       </c>
@@ -6649,7 +6648,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>69</v>
       </c>
@@ -6702,7 +6701,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>70</v>
       </c>
@@ -6752,7 +6751,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>71</v>
       </c>
@@ -6805,7 +6804,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -6859,7 +6858,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>73</v>
       </c>
@@ -6918,7 +6917,7 @@
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>74</v>
       </c>
@@ -6968,7 +6967,7 @@
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="79" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>75</v>
       </c>
@@ -7018,7 +7017,7 @@
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>76</v>
       </c>
@@ -7072,7 +7071,7 @@
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>77</v>
       </c>
@@ -7131,7 +7130,7 @@
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>78</v>
       </c>
@@ -7246,7 +7245,7 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>20</v>
       </c>
@@ -7418,7 +7417,7 @@
         <v>SearchParameter-us-core-careteam-role.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>81</v>
       </c>
@@ -7477,7 +7476,7 @@
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>82</v>
       </c>
@@ -7526,7 +7525,7 @@
         <v>SearchParameter-us-core-device-type.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>83</v>
       </c>
@@ -7581,7 +7580,7 @@
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>84</v>
       </c>
@@ -7636,7 +7635,7 @@
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>85</v>
       </c>
@@ -7691,7 +7690,7 @@
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>86</v>
       </c>
@@ -7745,7 +7744,7 @@
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>87</v>
       </c>
@@ -7800,7 +7799,7 @@
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="94" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>88</v>
       </c>
@@ -7855,7 +7854,7 @@
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="95" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>89</v>
       </c>
@@ -7910,7 +7909,7 @@
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="96" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>90</v>
       </c>
@@ -7965,7 +7964,7 @@
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="97" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>91</v>
       </c>
@@ -8020,7 +8019,7 @@
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="98" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>92</v>
       </c>
@@ -8075,7 +8074,7 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="99" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>93</v>
       </c>
@@ -8130,7 +8129,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="100" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>94</v>
       </c>
@@ -8188,7 +8187,7 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="101" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>95</v>
       </c>
@@ -8249,7 +8248,7 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>96</v>
       </c>
@@ -8313,7 +8312,7 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="103" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>49</v>
       </c>
@@ -8369,7 +8368,7 @@
         <v>SearchParameter-us-core-servicerequest-status.html</v>
       </c>
     </row>
-    <row r="104" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>50</v>
       </c>
@@ -8431,7 +8430,7 @@
         <v>SearchParameter-us-core-servicerequest-patient.html</v>
       </c>
     </row>
-    <row r="105" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>51</v>
       </c>
@@ -8484,7 +8483,7 @@
         <v>SearchParameter-us-core-servicerequest-category.html</v>
       </c>
     </row>
-    <row r="106" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>52</v>
       </c>
@@ -8540,7 +8539,7 @@
         <v>SearchParameter-us-core-servicerequest-code.html</v>
       </c>
     </row>
-    <row r="107" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>53</v>
       </c>
@@ -8597,7 +8596,7 @@
         <v>SearchParameter-us-core-servicerequest-authored.html</v>
       </c>
     </row>
-    <row r="108" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>20</v>
       </c>
@@ -8651,7 +8650,7 @@
         <v>SearchParameter-us-core-servicerequest-id.html</v>
       </c>
     </row>
-    <row r="109" spans="1:28" s="1" customFormat="1" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:28" s="1" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>56</v>
       </c>
@@ -8817,15 +8816,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB111" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="CareTeam"/>
-        <filter val="Patient"/>
-        <filter val="RelatedPerson"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AB111" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA36">
     <sortCondition ref="B1"/>
   </sortState>
@@ -8837,11 +8828,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection sqref="A1:Q97"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8894,7 +8884,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -8919,7 +8909,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -8944,7 +8934,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -8969,7 +8959,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -8994,7 +8984,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -9025,7 +9015,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -9050,7 +9040,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -9075,7 +9065,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -9101,7 +9091,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -9128,7 +9118,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -9154,7 +9144,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -9179,7 +9169,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -9210,7 +9200,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -9235,7 +9225,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -9260,7 +9250,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -9291,7 +9281,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -9325,7 +9315,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and location</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -9351,7 +9341,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -9382,7 +9372,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -9416,7 +9406,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and discharge-disposition</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -9443,7 +9433,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -9469,7 +9459,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -9494,7 +9484,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -9520,7 +9510,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -9547,7 +9537,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -9574,7 +9564,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -9601,7 +9591,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="28" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -9626,7 +9616,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -9651,7 +9641,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -9676,7 +9666,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -9707,7 +9697,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -9738,7 +9728,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -9769,7 +9759,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="34" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -9800,7 +9790,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="35" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>36</v>
       </c>
@@ -9833,7 +9823,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="36" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>37</v>
       </c>
@@ -9863,7 +9853,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="37" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>37</v>
       </c>
@@ -9896,7 +9886,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>38</v>
       </c>
@@ -9926,7 +9916,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>39</v>
       </c>
@@ -9956,7 +9946,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="40" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -9989,7 +9979,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="41" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -10022,7 +10012,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="42" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>39</v>
       </c>
@@ -10055,7 +10045,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -10085,7 +10075,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="44" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>45</v>
       </c>
@@ -10116,7 +10106,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="45" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>46</v>
       </c>
@@ -10147,7 +10137,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="46" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>49</v>
       </c>
@@ -10177,7 +10167,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>50</v>
       </c>
@@ -10210,7 +10200,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="48" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>51</v>
       </c>
@@ -10240,7 +10230,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="1" customFormat="1" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>52</v>
       </c>
@@ -10273,7 +10263,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>53</v>
       </c>
@@ -10303,7 +10293,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="51" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>56</v>
       </c>
@@ -10333,7 +10323,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="52" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>57</v>
       </c>
@@ -10363,7 +10353,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="53" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>58</v>
       </c>
@@ -10393,7 +10383,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="54" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>59</v>
       </c>
@@ -10423,7 +10413,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="55" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>60</v>
       </c>
@@ -10453,7 +10443,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="56" spans="1:11" s="1" customFormat="1" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>63</v>
       </c>
@@ -10515,7 +10505,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>67</v>
       </c>
@@ -10548,7 +10538,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="59" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>68</v>
       </c>
@@ -10581,7 +10571,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="60" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>69</v>
       </c>
@@ -10614,7 +10604,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="61" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>70</v>
       </c>
@@ -10647,7 +10637,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="62" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>73</v>
       </c>
@@ -10678,7 +10668,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="63" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <f>SUBTOTAL(9,M103)</f>
         <v>0</v>
@@ -10709,7 +10699,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="64" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>75</v>
       </c>
@@ -10740,7 +10730,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>76</v>
       </c>
@@ -10771,7 +10761,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>77</v>
       </c>
@@ -10802,7 +10792,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>80</v>
       </c>
@@ -10834,7 +10824,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="68" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>81</v>
       </c>
@@ -10867,7 +10857,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="69" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>82</v>
       </c>
@@ -10897,7 +10887,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="70" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>83</v>
       </c>
@@ -10930,7 +10920,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>84</v>
       </c>
@@ -10960,7 +10950,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>85</v>
       </c>
@@ -10990,7 +10980,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="73" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>88</v>
       </c>
@@ -11023,7 +11013,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="74" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>89</v>
       </c>
@@ -11055,7 +11045,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>90</v>
       </c>
@@ -11087,7 +11077,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="76" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>91</v>
       </c>
@@ -11119,7 +11109,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="77" spans="1:11" s="1" customFormat="1" ht="136" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" s="1" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>94</v>
       </c>
@@ -11155,7 +11145,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="78" spans="1:11" s="1" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>97</v>
       </c>
@@ -11188,7 +11178,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code.</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>100</v>
       </c>
@@ -11221,7 +11211,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>101</v>
       </c>
@@ -11254,7 +11244,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="81" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>102</v>
       </c>
@@ -11287,7 +11277,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="82" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>103</v>
       </c>
@@ -11320,7 +11310,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="83" spans="1:17" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>104</v>
       </c>
@@ -11356,7 +11346,7 @@
       <c r="P83" s="1"/>
       <c r="Q83" s="1"/>
     </row>
-    <row r="84" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>107</v>
       </c>
@@ -11387,7 +11377,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="85" spans="1:17" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:17" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>108</v>
       </c>
@@ -11416,7 +11406,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="86" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>109</v>
       </c>
@@ -11449,7 +11439,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="87" spans="1:17" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:17" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>110</v>
       </c>
@@ -11482,7 +11472,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="88" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>111</v>
       </c>
@@ -11512,7 +11502,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="89" spans="1:17" s="1" customFormat="1" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:17" s="1" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>112</v>
       </c>
@@ -11543,7 +11533,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="90" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>115</v>
       </c>
@@ -11572,7 +11562,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="91" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>94</v>
       </c>
@@ -11605,7 +11595,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="92" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>56</v>
       </c>
@@ -11638,7 +11628,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="93" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>57</v>
       </c>
@@ -11671,7 +11661,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
       </c>
     </row>
-    <row r="94" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>58</v>
       </c>
@@ -11704,7 +11694,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="95" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>59</v>
       </c>
@@ -11737,7 +11727,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
       </c>
     </row>
-    <row r="96" spans="1:17" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>60</v>
       </c>
@@ -11805,13 +11795,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="Goal"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K134">
     <sortCondition ref="A1"/>
   </sortState>
@@ -11825,8 +11809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11940,8 +11924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A70CC787-78D8-4AA0-BE43-37746049F77C}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="88" zoomScaleNormal="88" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12068,8 +12052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G44"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
+      <selection sqref="A1:E45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12739,11 +12723,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="V2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="W4" sqref="W4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13470,10 +13454,10 @@
   <dimension ref="A1:AA10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="U2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T27" sqref="T27:T28"/>
+      <selection pane="bottomRight" activeCell="Y1" sqref="Y1:Z1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14256,7 +14240,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Clarify Condition.clinicalStatus FHIR-33518, FHIR-34468
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core-R4/input/resources_spreadsheets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2F1BCF8-F8F6-4541-B249-0A04F80B1A75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B77B5C-20F1-E945-A1B9-432D345A8F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20520" yWindow="-21140" windowWidth="21640" windowHeight="21140" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -29,7 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$96</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$111</definedName>
   </definedNames>
-  <calcPr calcId="191029" refMode="R1C1"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1123,9 +1123,6 @@
     <t>Fetches a bundle of all Observation resources for the specified patient and category = `laboratory` and status</t>
   </si>
   <si>
-    <t>Fetches a bundle of all Condition resources for the specified patient and all "active" statuses (active,relapse,remission). This will not return any "entered in error" resources because of the conditional presence of the clinicalStatus element.</t>
-  </si>
-  <si>
     <t>support searching a practitioner by an identifier such as an NPI</t>
   </si>
   <si>
@@ -2179,6 +2176,9 @@
   * Although both are marked as must support, the server systems are not required to support both `Encounter.location.location` and `Encounter.serviceProvider`, but they **SHALL** support *at least one* of these elements.
   * The client application **SHALL** support both elements.
   * if using `Encounter.locatison.location` it **SHOULD** conform to US Core Location.  However, as a result of implementation feedback, it **MAY**  reference the base FHIR Location resource.  See this guidance on Referencing US Core Profiles</t>
+  </si>
+  <si>
+    <t>Implementation Notes: Fetches a bundle of all Condition resources for the specified patient and all "active" statuses (active,relapse,remission). This will *exclude* diagnoses and health concerns without a clinicalStatus specified.</t>
   </si>
 </sst>
 </file>
@@ -2732,34 +2732,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B3" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>469</v>
+      </c>
+      <c r="B4" t="s">
         <v>470</v>
-      </c>
-      <c r="B4" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>471</v>
+      </c>
+      <c r="B5" t="s">
         <v>472</v>
-      </c>
-      <c r="B5" t="s">
-        <v>473</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2767,12 +2767,12 @@
         <v>68</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
@@ -2780,15 +2780,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B8" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -2858,7 +2858,7 @@
         <v>41</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>32</v>
@@ -3080,7 +3080,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3288,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3337,7 +3337,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3399,7 +3399,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3450,7 +3450,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3498,7 +3498,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3582,7 +3582,7 @@
         <v>212</v>
       </c>
       <c r="Z14" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="AA14" s="2" t="s">
         <v>171</v>
@@ -3609,7 +3609,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3659,7 +3659,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3713,7 +3713,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3770,7 +3770,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3819,7 +3819,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>30</v>
@@ -3828,7 +3828,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G19" s="1" t="str">
         <f t="shared" ref="G19" si="8">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B19)</f>
@@ -3889,7 +3889,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3939,7 +3939,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G21" s="1" t="str">
         <f t="shared" ref="G21" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
@@ -3980,7 +3980,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>30</v>
@@ -3989,7 +3989,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4068,7 +4068,7 @@
         <v>76</v>
       </c>
       <c r="Z23" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="AB23" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B23)&amp;"-"&amp;SUBSTITUTE(C23,"_","")&amp;".html")</f>
@@ -4092,7 +4092,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G24" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4140,7 +4140,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4187,7 +4187,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G26" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4280,7 +4280,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4361,7 +4361,7 @@
       </c>
       <c r="S29"/>
       <c r="Y29" s="5" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="Z29" s="1" t="s">
         <v>173</v>
@@ -4717,7 +4717,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4762,7 +4762,7 @@
         <v>138</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>30</v>
@@ -4771,7 +4771,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G38" s="1" t="str">
         <f t="shared" ref="G38:G40" si="16">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B38)</f>
@@ -4819,7 +4819,7 @@
         <v>138</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>30</v>
@@ -4828,7 +4828,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G39" s="1" t="str">
         <f t="shared" si="16"/>
@@ -4876,7 +4876,7 @@
         <v>138</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>30</v>
@@ -4885,7 +4885,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G40" s="1" t="str">
         <f t="shared" si="16"/>
@@ -4942,7 +4942,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G41" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4983,7 +4983,7 @@
         <v>138</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>30</v>
@@ -4992,7 +4992,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G42" s="1" t="str">
         <f t="shared" ref="G42" si="19">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B42)</f>
@@ -5021,7 +5021,7 @@
         <v>56</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="Z42" s="5" t="str">
         <f>"GET [base]/"&amp;B42&amp;"?patient=1137192"</f>
@@ -5053,7 +5053,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G43" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5112,7 +5112,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G44" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5162,7 +5162,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G45" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5242,7 +5242,7 @@
         <v>287</v>
       </c>
       <c r="Z46" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AA46" s="2" t="s">
         <v>288</v>
@@ -5269,7 +5269,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G47" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5322,7 +5322,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G48" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5381,7 +5381,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G49" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5431,7 +5431,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G50" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5481,7 +5481,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G51" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5535,7 +5535,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G52" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5588,7 +5588,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G53" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5641,7 +5641,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G54" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B54)</f>
@@ -5700,7 +5700,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G55" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5750,7 +5750,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G56" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5803,7 +5803,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G57" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5857,7 +5857,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G58" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5907,7 +5907,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G59" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5957,7 +5957,7 @@
         <v>180</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>30</v>
@@ -5966,7 +5966,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G60" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6020,7 +6020,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G61" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6064,7 +6064,7 @@
         <v>181</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>30</v>
@@ -6073,7 +6073,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G62" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6126,7 +6126,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G63" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6168,7 +6168,7 @@
         <v>181</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>30</v>
@@ -6177,7 +6177,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G64" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6228,7 +6228,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G65" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6270,7 +6270,7 @@
         <v>62</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>62</v>
@@ -6282,7 +6282,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G66" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6323,7 +6323,7 @@
         <v>63</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>90</v>
@@ -6335,7 +6335,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G67" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6365,7 +6365,7 @@
         <v>215</v>
       </c>
       <c r="Z67" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AA67" s="12" t="str">
         <f>"Fetches a bundle of all "&amp;B67&amp; " resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
@@ -6381,7 +6381,7 @@
         <v>64</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>229</v>
@@ -6393,7 +6393,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G68" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6447,7 +6447,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G69" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6500,7 +6500,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G70" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6558,7 +6558,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G71" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6612,7 +6612,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G72" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6665,7 +6665,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G73" s="1" t="str">
         <f t="shared" ref="G73:G103" si="40">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B73)</f>
@@ -6718,7 +6718,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G74" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6768,7 +6768,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G75" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6821,7 +6821,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G76" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6875,7 +6875,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G77" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6934,7 +6934,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G78" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6984,7 +6984,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G79" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7034,7 +7034,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G80" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7088,7 +7088,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G81" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7147,7 +7147,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G82" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7200,7 +7200,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G83" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7226,7 +7226,7 @@
         <v>56</v>
       </c>
       <c r="X83" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="Y83" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B83)&amp;"s for a patient"</f>
@@ -7296,7 +7296,7 @@
         <v>GET [base]/Practitioner/practitioner-1~GET [base]/Practitioner?_id=practitioner-1</v>
       </c>
       <c r="AA84" s="12" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="AB84" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B84)&amp;"-"&amp;SUBSTITUTE(C84,"_","")&amp;".html")</f>
@@ -7320,7 +7320,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G85" s="1" t="str">
         <f t="shared" ref="G85" si="47">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B85)</f>
@@ -7364,7 +7364,7 @@
         <v>249</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>70</v>
@@ -7373,7 +7373,7 @@
         <v>0</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G86" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7405,7 +7405,7 @@
         <v>56</v>
       </c>
       <c r="Y86" s="5" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="Z86" s="5" t="str">
         <f>"GET [base]/"&amp;B86&amp;"?"&amp;C86&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -7434,7 +7434,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G87" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B87)</f>
@@ -7493,7 +7493,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G88" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B88)</f>
@@ -8146,7 +8146,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G100" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8172,7 +8172,7 @@
         <v>56</v>
       </c>
       <c r="Y100" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="Z100" s="5" t="str">
         <f>"GET [base]/"&amp;B100&amp;"?dentifier=http://hl7.org/fhir/sid/us-npi\|97860456"</f>
@@ -8204,7 +8204,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G101" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8233,7 +8233,7 @@
         <v>274</v>
       </c>
       <c r="Y101" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="Z101" s="5" t="str">
         <f>"GET [base]/"&amp;B101&amp;"?specialty=http://nucc.org/provider-taxonomy\|208D0000X"</f>
@@ -8265,7 +8265,7 @@
         <v>1</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G102" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8317,7 +8317,7 @@
         <v>49</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>62</v>
@@ -8329,7 +8329,7 @@
         <v>0</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G103" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8373,7 +8373,7 @@
         <v>50</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>90</v>
@@ -8385,7 +8385,7 @@
         <v>1</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G104" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B104)</f>
@@ -8435,7 +8435,7 @@
         <v>51</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>140</v>
@@ -8447,7 +8447,7 @@
         <v>0</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G105" s="1" t="str">
         <f t="shared" ref="G105:G111" si="56">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
@@ -8488,7 +8488,7 @@
         <v>52</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>26</v>
@@ -8500,7 +8500,7 @@
         <v>0</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="G106" s="1" t="str">
         <f t="shared" si="56"/>
@@ -8544,10 +8544,10 @@
         <v>53</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>30</v>
@@ -8556,7 +8556,7 @@
         <v>0</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="G107" s="1" t="str">
         <f t="shared" si="56"/>
@@ -8601,7 +8601,7 @@
         <v>20</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>55</v>
@@ -8639,10 +8639,10 @@
         <v>56</v>
       </c>
       <c r="Y108" s="5" t="s">
+        <v>602</v>
+      </c>
+      <c r="Z108" s="5" t="s">
         <v>603</v>
-      </c>
-      <c r="Z108" s="5" t="s">
-        <v>604</v>
       </c>
       <c r="AA108" s="2"/>
       <c r="AB108" s="1" t="str">
@@ -8704,7 +8704,7 @@
         <v>20</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>55</v>
@@ -8742,10 +8742,10 @@
         <v>56</v>
       </c>
       <c r="Y110" s="5" t="s">
+        <v>633</v>
+      </c>
+      <c r="Z110" s="5" t="s">
         <v>634</v>
-      </c>
-      <c r="Z110" s="5" t="s">
-        <v>635</v>
       </c>
       <c r="AA110" s="12"/>
       <c r="AB110" s="1" t="str">
@@ -8758,7 +8758,7 @@
         <v>79</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>90</v>
@@ -8770,7 +8770,7 @@
         <v>1</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G111" s="1" t="str">
         <f t="shared" si="56"/>
@@ -8830,8 +8830,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8863,7 +8863,7 @@
         <v>96</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>97</v>
@@ -9193,7 +9193,7 @@
         <v>305</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K13" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9293,10 +9293,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>581</v>
-      </c>
-      <c r="E17" s="1" t="b">
-        <v>1</v>
+        <v>580</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>70</v>
@@ -9308,7 +9305,7 @@
         <v>306</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="K17" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9384,10 +9381,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>583</v>
-      </c>
-      <c r="E20" s="1" t="b">
-        <v>1</v>
+        <v>582</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>70</v>
@@ -9399,7 +9393,7 @@
         <v>311</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="K20" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9804,6 +9798,9 @@
       <c r="D35" s="1" t="s">
         <v>144</v>
       </c>
+      <c r="E35" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="F35" s="1" t="s">
         <v>70</v>
       </c>
@@ -9811,16 +9808,16 @@
         <v>106</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>155</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>323</v>
+        <v>639</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9847,7 +9844,7 @@
         <v>150</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>146</v>
@@ -9865,10 +9862,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>571</v>
-      </c>
-      <c r="E37" s="1" t="b">
-        <v>1</v>
+        <v>570</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>70</v>
@@ -9880,10 +9874,10 @@
         <v>150</v>
       </c>
       <c r="J37" s="5" t="s">
+        <v>575</v>
+      </c>
+      <c r="K37" s="5" t="s">
         <v>576</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -9910,7 +9904,7 @@
         <v>151</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="K38" s="5" t="s">
         <v>152</v>
@@ -9940,7 +9934,7 @@
         <v>153</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>156</v>
@@ -9958,10 +9952,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>568</v>
-      </c>
-      <c r="E40" s="1" t="b">
-        <v>1</v>
+        <v>567</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>70</v>
@@ -9973,7 +9964,7 @@
         <v>153</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>156</v>
@@ -9991,10 +9982,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>569</v>
-      </c>
-      <c r="E41" s="1" t="b">
-        <v>1</v>
+        <v>568</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>70</v>
@@ -10006,7 +9994,7 @@
         <v>153</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>156</v>
@@ -10024,10 +10012,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>570</v>
-      </c>
-      <c r="E42" s="1" t="b">
-        <v>1</v>
+        <v>569</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>70</v>
@@ -10039,7 +10024,7 @@
         <v>153</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>156</v>
@@ -10069,10 +10054,10 @@
         <v>162</v>
       </c>
       <c r="J43" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10099,7 +10084,7 @@
         <v>167</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K44" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B44&amp;" resources for the specified "&amp;SUBSTITUTE(D44,","," and ")</f>
@@ -10187,7 +10172,7 @@
         <v>106</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>194</v>
@@ -10250,13 +10235,13 @@
         <v>219</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I49" s="5" t="s">
         <v>196</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K49" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -10286,7 +10271,7 @@
         <v>227</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K50" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10406,7 +10391,7 @@
         <v>202</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K54" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -10436,7 +10421,7 @@
         <v>221</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K55" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B55&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10486,7 +10471,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>70</v>
@@ -10498,7 +10483,7 @@
         <v>208</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K57" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B57&amp;" resources for the specified "&amp;SUBSTITUTE(D57,","," and ")</f>
@@ -10517,7 +10502,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>12</v>
@@ -10526,16 +10511,16 @@
         <v>106</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>434</v>
+      </c>
+      <c r="J58" s="5" t="s">
         <v>461</v>
       </c>
-      <c r="I58" s="5" t="s">
-        <v>435</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>462</v>
-      </c>
       <c r="K58" s="5" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10550,7 +10535,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>12</v>
@@ -10559,16 +10544,16 @@
         <v>106</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>186</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10583,7 +10568,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>70</v>
@@ -10592,16 +10577,16 @@
         <v>106</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>186</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10616,7 +10601,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>70</v>
@@ -10625,16 +10610,16 @@
         <v>219</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>231</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10642,7 +10627,7 @@
         <v>73</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C62" s="1" t="str">
         <f t="shared" si="8"/>
@@ -10661,7 +10646,7 @@
         <v>188</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="K62" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified "&amp;SUBSTITUTE(D62,","," and ")</f>
@@ -10674,7 +10659,7 @@
         <v>0</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C63" s="1" t="str">
         <f t="shared" si="8"/>
@@ -10693,7 +10678,7 @@
         <v>232</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="K63" s="5" t="s">
         <v>234</v>
@@ -10785,7 +10770,7 @@
         <v>228</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="K66" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -10800,7 +10785,7 @@
         <v>183</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>238</v>
@@ -10812,13 +10797,13 @@
         <v>106</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>281</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>322</v>
@@ -10832,7 +10817,7 @@
         <v>183</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>145</v>
@@ -10844,13 +10829,13 @@
         <v>106</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>222</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="K68" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -10865,7 +10850,7 @@
         <v>183</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>147</v>
@@ -10880,7 +10865,7 @@
         <v>225</v>
       </c>
       <c r="J69" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="K69" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -10895,7 +10880,7 @@
         <v>183</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>195</v>
@@ -10907,13 +10892,13 @@
         <v>219</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>226</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="K70" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -10928,7 +10913,7 @@
         <v>183</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>220</v>
@@ -10943,7 +10928,7 @@
         <v>224</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K71" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10958,7 +10943,7 @@
         <v>321</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>116</v>
@@ -11000,7 +10985,7 @@
         <v>106</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I73" s="5" t="s">
         <v>243</v>
@@ -11033,13 +11018,13 @@
         <v>219</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I74" s="5" t="s">
         <v>242</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="K74" s="5" t="s">
         <v>246</v>
@@ -11065,7 +11050,7 @@
         <v>106</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I75" s="5" t="s">
         <v>240</v>
@@ -11097,13 +11082,13 @@
         <v>219</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I76" s="5" t="s">
         <v>241</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>248</v>
@@ -11123,9 +11108,6 @@
       <c r="D77" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E77" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="F77" s="1" t="s">
         <v>12</v>
       </c>
@@ -11136,13 +11118,13 @@
         <v>312</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="K77" s="12" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -11165,7 +11147,7 @@
         <v>106</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="I78" s="5" t="s">
         <v>278</v>
@@ -11186,7 +11168,7 @@
         <v>183</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>238</v>
@@ -11198,13 +11180,13 @@
         <v>106</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>280</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="K79" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B79&amp;" resources for the specified "&amp;SUBSTITUTE(D79,","," and ")</f>
@@ -11219,7 +11201,7 @@
         <v>183</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>145</v>
@@ -11231,13 +11213,13 @@
         <v>106</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>279</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="K80" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B80&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -11252,7 +11234,7 @@
         <v>183</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>147</v>
@@ -11264,7 +11246,7 @@
         <v>106</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>282</v>
@@ -11285,7 +11267,7 @@
         <v>183</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>195</v>
@@ -11297,13 +11279,13 @@
         <v>219</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>284</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="K82" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B82&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -11318,7 +11300,7 @@
         <v>183</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>220</v>
@@ -11333,7 +11315,7 @@
         <v>285</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="K83" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes."</f>
@@ -11427,7 +11409,7 @@
         <v>106</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I86" s="5" t="s">
         <v>296</v>
@@ -11460,13 +11442,13 @@
         <v>219</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I87" s="5" t="s">
         <v>297</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="K87" s="5" t="s">
         <v>299</v>
@@ -11496,7 +11478,7 @@
         <v>301</v>
       </c>
       <c r="J88" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K88" s="5" t="s">
         <v>298</v>
@@ -11526,7 +11508,7 @@
         <v>302</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="K89" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -11541,7 +11523,7 @@
         <v>250</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>118</v>
@@ -11553,13 +11535,13 @@
         <v>106</v>
       </c>
       <c r="I90" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="J90" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="K90" s="5" t="s">
         <v>397</v>
-      </c>
-      <c r="K90" s="5" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="91" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -11574,10 +11556,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>589</v>
-      </c>
-      <c r="E91" s="1" t="b">
-        <v>1</v>
+        <v>588</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>70</v>
@@ -11586,13 +11565,13 @@
         <v>106</v>
       </c>
       <c r="I91" s="5" t="s">
+        <v>589</v>
+      </c>
+      <c r="J91" s="5" t="s">
         <v>590</v>
       </c>
-      <c r="J91" s="5" t="s">
+      <c r="K91" s="5" t="s">
         <v>591</v>
-      </c>
-      <c r="K91" s="5" t="s">
-        <v>592</v>
       </c>
     </row>
     <row r="92" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -11600,17 +11579,14 @@
         <v>56</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E92" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="F92" s="1" t="s">
         <v>70</v>
       </c>
@@ -11621,7 +11597,7 @@
         <v>304</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="K92" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -11633,17 +11609,14 @@
         <v>57</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E93" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="F93" s="1" t="s">
         <v>12</v>
       </c>
@@ -11654,7 +11627,7 @@
         <v>199</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="K93" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient and  a category code"</f>
@@ -11666,17 +11639,14 @@
         <v>58</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E94" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="F94" s="1" t="s">
         <v>12</v>
       </c>
@@ -11687,7 +11657,7 @@
         <v>200</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="K94" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11699,16 +11669,13 @@
         <v>59</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>606</v>
-      </c>
-      <c r="E95" s="1" t="b">
-        <v>1</v>
+        <v>605</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>12</v>
@@ -11720,7 +11687,7 @@
         <v>202</v>
       </c>
       <c r="J95" s="5" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="K95" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date and a category code"</f>
@@ -11732,16 +11699,13 @@
         <v>60</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>607</v>
-      </c>
-      <c r="E96" s="1" t="b">
-        <v>1</v>
+        <v>606</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>70</v>
@@ -11750,10 +11714,10 @@
         <v>219</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="K96" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -11772,10 +11736,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>611</v>
-      </c>
-      <c r="E97" s="1" t="b">
-        <v>1</v>
+        <v>610</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>12</v>
@@ -11784,10 +11745,10 @@
         <v>106</v>
       </c>
       <c r="I97" s="5" t="s">
+        <v>611</v>
+      </c>
+      <c r="J97" s="5" t="s">
         <v>612</v>
-      </c>
-      <c r="J97" s="5" t="s">
-        <v>613</v>
       </c>
       <c r="K97" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified "&amp;SUBSTITUTE(D97,","," and ")</f>
@@ -11832,7 +11793,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="3" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -11840,15 +11801,15 @@
         <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -11856,7 +11817,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -11872,7 +11833,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -11880,36 +11841,36 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>70</v>
@@ -11940,7 +11901,7 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
@@ -11951,13 +11912,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -11965,13 +11926,13 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>70</v>
@@ -12008,16 +11969,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>539</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>540</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>541</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>60</v>
@@ -12031,13 +11992,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
@@ -12087,7 +12048,7 @@
         <v>73</v>
       </c>
       <c r="B2" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -12102,7 +12063,7 @@
         <v>237</v>
       </c>
       <c r="B3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="D3" t="s">
         <v>12</v>
@@ -12114,10 +12075,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>12</v>
@@ -12129,10 +12090,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
@@ -12144,10 +12105,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -12162,7 +12123,7 @@
         <v>189</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
@@ -12177,7 +12138,7 @@
         <v>190</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>12</v>
@@ -12189,10 +12150,10 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>347</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>348</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
@@ -12204,10 +12165,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
@@ -12219,10 +12180,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>365</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>366</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
@@ -12234,10 +12195,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>344</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>345</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
@@ -12249,10 +12210,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
@@ -12264,25 +12225,25 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>358</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="D14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>359</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>360</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>349</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>350</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
@@ -12294,10 +12255,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>12</v>
@@ -12309,10 +12270,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>12</v>
@@ -12324,10 +12285,10 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>12</v>
@@ -12339,10 +12300,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>12</v>
@@ -12354,10 +12315,10 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>12</v>
@@ -12369,10 +12330,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>12</v>
@@ -12384,10 +12345,10 @@
     </row>
     <row r="22" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>12</v>
@@ -12398,10 +12359,10 @@
     </row>
     <row r="23" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>12</v>
@@ -12412,10 +12373,10 @@
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>12</v>
@@ -12426,10 +12387,10 @@
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>12</v>
@@ -12440,10 +12401,10 @@
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>12</v>
@@ -12454,10 +12415,10 @@
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>12</v>
@@ -12468,10 +12429,10 @@
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>12</v>
@@ -12482,10 +12443,10 @@
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>12</v>
@@ -12496,10 +12457,10 @@
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>12</v>
@@ -12510,10 +12471,10 @@
     </row>
     <row r="31" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
+        <v>594</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>595</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>596</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>12</v>
@@ -12527,7 +12488,7 @@
         <v>276</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>12</v>
@@ -12539,10 +12500,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>354</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>355</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>12</v>
@@ -12557,7 +12518,7 @@
         <v>75</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>12</v>
@@ -12568,10 +12529,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>343</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>12</v>
@@ -12583,10 +12544,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>362</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>363</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
@@ -12598,10 +12559,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>356</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>357</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>12</v>
@@ -12612,24 +12573,24 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
+        <v>444</v>
+      </c>
+      <c r="B38" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>446</v>
-      </c>
       <c r="D38" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>12</v>
@@ -12640,24 +12601,24 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>12</v>
@@ -12668,24 +12629,24 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>12</v>
@@ -12696,10 +12657,10 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>12</v>
@@ -12760,67 +12721,67 @@
         <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="H1" t="s">
         <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="J1" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>407</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>399</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>408</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>409</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>402</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>410</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>411</v>
       </c>
       <c r="T1" t="s">
         <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="V1" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>543</v>
       </c>
-      <c r="W1" s="4" t="s">
-        <v>542</v>
-      </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>544</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>545</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -12842,7 +12803,7 @@
         <v>70</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y2" s="17" t="s">
         <v>12</v>
@@ -12856,7 +12817,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>19</v>
@@ -12865,7 +12826,7 @@
         <v>70</v>
       </c>
       <c r="X3" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y3" s="17" t="s">
         <v>12</v>
@@ -12879,7 +12840,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>19</v>
@@ -12888,13 +12849,13 @@
         <v>70</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="X4" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y4" s="17" t="s">
         <v>12</v>
@@ -12908,7 +12869,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>19</v>
@@ -12917,7 +12878,7 @@
         <v>70</v>
       </c>
       <c r="X5" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y5" s="17" t="s">
         <v>12</v>
@@ -12931,7 +12892,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>19</v>
@@ -12940,7 +12901,7 @@
         <v>70</v>
       </c>
       <c r="X6" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y6" s="17" t="s">
         <v>12</v>
@@ -12954,7 +12915,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>19</v>
@@ -12963,7 +12924,7 @@
         <v>70</v>
       </c>
       <c r="X7" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y7" s="17" t="s">
         <v>12</v>
@@ -12977,7 +12938,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="T8" s="1" t="s">
         <v>19</v>
@@ -12986,7 +12947,7 @@
         <v>70</v>
       </c>
       <c r="X8" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y8" s="17" t="s">
         <v>12</v>
@@ -13000,7 +12961,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>19</v>
@@ -13009,7 +12970,7 @@
         <v>70</v>
       </c>
       <c r="X9" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y9" s="17" t="s">
         <v>12</v>
@@ -13029,7 +12990,7 @@
         <v>70</v>
       </c>
       <c r="X10" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y10" s="17" t="s">
         <v>12</v>
@@ -13043,7 +13004,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>19</v>
@@ -13052,7 +13013,7 @@
         <v>70</v>
       </c>
       <c r="X11" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y11" s="17" t="s">
         <v>12</v>
@@ -13066,7 +13027,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>19</v>
@@ -13079,13 +13040,13 @@
     </row>
     <row r="13" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>19</v>
@@ -13104,7 +13065,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>19</v>
@@ -13119,7 +13080,7 @@
         <v>209</v>
       </c>
       <c r="X14" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y14" s="17" t="s">
         <v>12</v>
@@ -13127,13 +13088,13 @@
     </row>
     <row r="15" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>19</v>
@@ -13145,10 +13106,10 @@
         <v>70</v>
       </c>
       <c r="W15" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="X15" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y15" s="17" t="s">
         <v>12</v>
@@ -13162,7 +13123,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>19</v>
@@ -13171,7 +13132,7 @@
         <v>70</v>
       </c>
       <c r="X16" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y16" s="17" t="s">
         <v>12</v>
@@ -13201,7 +13162,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="T18" s="1" t="s">
         <v>19</v>
@@ -13210,7 +13171,7 @@
         <v>70</v>
       </c>
       <c r="X18" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y18" s="17" t="s">
         <v>12</v>
@@ -13240,7 +13201,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="T20" s="1" t="s">
         <v>19</v>
@@ -13249,7 +13210,7 @@
         <v>70</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>274</v>
@@ -13265,7 +13226,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="T21" s="1" t="s">
         <v>19</v>
@@ -13274,7 +13235,7 @@
         <v>70</v>
       </c>
       <c r="X21" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y21" s="17" t="s">
         <v>12</v>
@@ -13282,13 +13243,13 @@
     </row>
     <row r="22" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>19</v>
@@ -13299,7 +13260,7 @@
     </row>
     <row r="23" spans="1:25" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>12</v>
@@ -13314,7 +13275,7 @@
         <v>70</v>
       </c>
       <c r="X23" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y23" s="17" t="s">
         <v>12</v>
@@ -13322,7 +13283,7 @@
     </row>
     <row r="24" spans="1:25" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>12</v>
@@ -13337,7 +13298,7 @@
         <v>70</v>
       </c>
       <c r="X24" s="17" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="Y24" s="17" t="s">
         <v>12</v>
@@ -13345,7 +13306,7 @@
     </row>
     <row r="25" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>70</v>
@@ -13409,10 +13370,10 @@
     </row>
     <row r="2" spans="1:5" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B2" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C2" s="16" t="s">
         <v>178</v>
@@ -13421,24 +13382,24 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>451</v>
+      </c>
+      <c r="B3" t="s">
         <v>452</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>453</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>454</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -13482,82 +13443,82 @@
         <v>26</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>375</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>378</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>385</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="R1" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>390</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" t="s">
         <v>392</v>
       </c>
-      <c r="W1" t="s">
-        <v>393</v>
-      </c>
       <c r="X1" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>631</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>632</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>633</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
     </row>
     <row r="2" spans="1:27" ht="64" x14ac:dyDescent="0.2">
@@ -13580,7 +13541,7 @@
         <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -14256,12 +14217,12 @@
         <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
@@ -14270,7 +14231,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
@@ -14279,7 +14240,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>30</v>
@@ -14288,7 +14249,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Change Goal.description search requirement from SHALL to SHOULD [FHIR-34546]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B77B5C-20F1-E945-A1B9-432D345A8F16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC42E3A-1ED4-3F44-8EF0-F7C8C403992B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2807,10 +2807,10 @@
   <dimension ref="A1:AB111"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="U23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" sqref="A1:XFD1048576"/>
+      <selection pane="bottomRight" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3837,9 +3837,6 @@
       <c r="H19" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I19" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J19" s="1" t="s">
         <v>56</v>
       </c>
@@ -3998,9 +3995,6 @@
       <c r="H22" t="s">
         <v>56</v>
       </c>
-      <c r="I22" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J22" t="s">
         <v>56</v>
       </c>
@@ -4780,9 +4774,6 @@
       <c r="H38" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I38" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J38" s="1" t="s">
         <v>56</v>
       </c>
@@ -4837,9 +4828,6 @@
       <c r="H39" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I39" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J39" s="1" t="s">
         <v>56</v>
       </c>
@@ -4893,9 +4881,6 @@
       </c>
       <c r="H40" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="I40" s="1" t="b">
-        <v>1</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>56</v>
@@ -5000,9 +4985,6 @@
       </c>
       <c r="H42" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="I42" s="1" t="b">
-        <v>1</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>56</v>
@@ -7268,9 +7250,6 @@
       <c r="H84" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I84" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J84" s="1" t="s">
         <v>56</v>
       </c>
@@ -7382,9 +7361,6 @@
       <c r="H86" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I86" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J86" s="1" t="s">
         <v>56</v>
       </c>
@@ -8337,9 +8313,6 @@
       </c>
       <c r="H103" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="I103" s="1" t="b">
-        <v>1</v>
       </c>
       <c r="J103" s="1" t="s">
         <v>56</v>
@@ -8394,9 +8367,6 @@
       <c r="H104" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I104" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J104" s="1" t="s">
         <v>56</v>
       </c>
@@ -8455,9 +8425,6 @@
       </c>
       <c r="H105" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="I105" s="1" t="b">
-        <v>1</v>
       </c>
       <c r="J105" s="1" t="s">
         <v>56</v>
@@ -8509,9 +8476,6 @@
       <c r="H106" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I106" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J106" s="1" t="s">
         <v>56</v>
       </c>
@@ -8565,9 +8529,6 @@
       <c r="H107" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I107" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J107" s="1" t="s">
         <v>56</v>
       </c>
@@ -8619,9 +8580,6 @@
       <c r="H108" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I108" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J108" s="1" t="s">
         <v>56</v>
       </c>
@@ -8674,9 +8632,6 @@
       <c r="H109" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I109" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J109" s="1" t="s">
         <v>56</v>
       </c>
@@ -8722,9 +8677,6 @@
       <c r="H110" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I110" s="1" t="b">
-        <v>1</v>
-      </c>
       <c r="J110" s="1" t="s">
         <v>56</v>
       </c>
@@ -8778,9 +8730,6 @@
       </c>
       <c r="H111" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="I111" s="1" t="b">
-        <v>1</v>
       </c>
       <c r="J111" s="1" t="s">
         <v>56</v>
@@ -8830,8 +8779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A54" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E97" sqref="E97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11738,8 +11687,11 @@
       <c r="D97" s="1" t="s">
         <v>610</v>
       </c>
+      <c r="E97" s="1" t="b">
+        <v>1</v>
+      </c>
       <c r="F97" s="1" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="G97" s="1" t="s">
         <v>106</v>

</xml_diff>

<commit_message>
Clarify $docref operation expectations [FHIR-35380](https://jira.hl7.org/browse/FHIR-35380)
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10313"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{795DB637-6588-F44B-85A5-02C1EC67C7F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8545C8-969F-244D-A48E-0DD0E8CF4164}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2420" yWindow="500" windowWidth="57440" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2420" yWindow="500" windowWidth="57440" windowHeight="28300" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1365,10 +1365,6 @@
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-lab</t>
   </si>
   <si>
-    <t>A server **SHALL** be capable of responding to a $docref operation and  capable of returning at least a reference to a generated CCD document, if available. **MAY** provide references to other 'on-demand' and 'stable' documents (or 'delayed/deferred assembly') that meet the query parameters as well. If a context date range is supplied the server ** SHOULD**  provide references to any document that falls within the date range If no date range is supplied, then the server **SHALL** provide references to last or current encounter.  **SHOULD** document what resources, if any, are returned as included resources
-`GET [base]/DocumentReference/$docref?patient=[id]`</t>
-  </si>
-  <si>
     <t>category=http://terminology.hl7.org/CodeSystem/observation-category|laboratory</t>
   </si>
   <si>
@@ -2265,6 +2261,10 @@
   </si>
   <si>
     <t>Documents/FHIR/US-Core/input/</t>
+  </si>
+  <si>
+    <t>A server **SHALL** be capable of responding to a $docref operation and  capable of returning at least a reference to a generated CCD document, if available. **MAY** provide references to other 'on-demand' and 'stable' documents (or 'delayed/deferred assembly') that meet the query parameters as well. If a context date range is supplied the server ** SHOULD**  provide references to any document that falls within the date range.  If no date range is supplied, then the server **SHALL** provide references to last or current document(s).  **SHOULD** document what resources, if any, are returned as included resources
+`GET [base]/DocumentReference/$docref?patient=[id]`</t>
   </si>
 </sst>
 </file>
@@ -2813,34 +2813,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B2" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>463</v>
+      </c>
+      <c r="B4" t="s">
         <v>464</v>
-      </c>
-      <c r="B4" t="s">
-        <v>465</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>465</v>
+      </c>
+      <c r="B5" t="s">
         <v>466</v>
-      </c>
-      <c r="B5" t="s">
-        <v>467</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -2848,12 +2848,12 @@
         <v>68</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B7" t="s">
         <v>60</v>
@@ -2861,15 +2861,15 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -2887,7 +2887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C112" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -2939,7 +2939,7 @@
         <v>41</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>32</v>
@@ -3161,7 +3161,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G5" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3369,7 +3369,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G9" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3418,7 +3418,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G10" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3480,7 +3480,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G11" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3531,7 +3531,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G12" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3579,7 +3579,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G13" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3690,7 +3690,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G15" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3740,7 +3740,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G16" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3794,7 +3794,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G17" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3851,7 +3851,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G18" s="1" t="str">
         <f t="shared" si="1"/>
@@ -3900,7 +3900,7 @@
         <v>22</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>30</v>
@@ -3909,7 +3909,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G19" s="1" t="str">
         <f t="shared" ref="G19" si="8">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B19)</f>
@@ -3967,7 +3967,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G20" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4017,7 +4017,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G21" s="1" t="str">
         <f t="shared" ref="G21" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
@@ -4058,7 +4058,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>30</v>
@@ -4067,7 +4067,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G22" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4167,7 +4167,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G24" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4215,7 +4215,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="G25" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4262,7 +4262,7 @@
         <v>0</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G26" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4355,7 +4355,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G28" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4436,7 +4436,7 @@
       </c>
       <c r="S29"/>
       <c r="Y29" s="5" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="Z29" s="1" t="s">
         <v>173</v>
@@ -4792,7 +4792,7 @@
         <v>0</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G37" s="1" t="str">
         <f t="shared" si="1"/>
@@ -4837,7 +4837,7 @@
         <v>138</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>30</v>
@@ -4846,7 +4846,7 @@
         <v>0</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G38" s="1" t="str">
         <f t="shared" ref="G38:G40" si="16">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B38)</f>
@@ -4891,7 +4891,7 @@
         <v>138</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>30</v>
@@ -4900,7 +4900,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G39" s="1" t="str">
         <f t="shared" si="16"/>
@@ -4945,7 +4945,7 @@
         <v>138</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>30</v>
@@ -4954,7 +4954,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G40" s="1" t="str">
         <f t="shared" si="16"/>
@@ -5008,7 +5008,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G41" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5049,7 +5049,7 @@
         <v>138</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>30</v>
@@ -5058,7 +5058,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G42" s="1" t="str">
         <f t="shared" ref="G42" si="19">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B42)</f>
@@ -5084,7 +5084,7 @@
         <v>56</v>
       </c>
       <c r="Y42" s="1" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="Z42" s="5" t="str">
         <f>"GET [base]/"&amp;B42&amp;"?patient=1137192"</f>
@@ -5116,7 +5116,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G43" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5175,7 +5175,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G44" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5225,7 +5225,7 @@
         <v>0</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G45" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5332,7 +5332,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G47" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5385,7 +5385,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G48" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5444,7 +5444,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G49" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5494,7 +5494,7 @@
         <v>0</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G50" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5544,7 +5544,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G51" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5598,7 +5598,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G52" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5651,7 +5651,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G53" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5704,7 +5704,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G54" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B54)</f>
@@ -5763,7 +5763,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G55" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5813,7 +5813,7 @@
         <v>0</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G56" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5866,7 +5866,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G57" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5920,7 +5920,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G58" s="1" t="str">
         <f t="shared" si="1"/>
@@ -5970,7 +5970,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G59" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6029,7 +6029,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G60" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6083,7 +6083,7 @@
         <v>0</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G61" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6127,7 +6127,7 @@
         <v>181</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>30</v>
@@ -6136,7 +6136,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G62" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6189,7 +6189,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G63" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6231,7 +6231,7 @@
         <v>181</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>30</v>
@@ -6240,7 +6240,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G64" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6291,7 +6291,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G65" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6333,7 +6333,7 @@
         <v>62</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>62</v>
@@ -6345,7 +6345,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G66" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6386,7 +6386,7 @@
         <v>63</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>90</v>
@@ -6398,7 +6398,7 @@
         <v>1</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G67" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6444,7 +6444,7 @@
         <v>64</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C68" s="1" t="s">
         <v>228</v>
@@ -6456,7 +6456,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G68" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6510,7 +6510,7 @@
         <v>0</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G69" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6563,7 +6563,7 @@
         <v>1</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G70" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6621,7 +6621,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G71" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6675,7 +6675,7 @@
         <v>0</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G72" s="1" t="str">
         <f t="shared" si="1"/>
@@ -6728,7 +6728,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G73" s="1" t="str">
         <f t="shared" ref="G73:G103" si="40">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B73)</f>
@@ -6781,7 +6781,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G74" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6831,7 +6831,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G75" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6884,7 +6884,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G76" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6938,7 +6938,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G77" s="1" t="str">
         <f t="shared" si="40"/>
@@ -6997,7 +6997,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G78" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7047,7 +7047,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G79" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7097,7 +7097,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G80" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7151,7 +7151,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G81" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7210,7 +7210,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G82" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7263,7 +7263,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G83" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7289,7 +7289,7 @@
         <v>56</v>
       </c>
       <c r="X83" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="Y83" s="1" t="str">
         <f>"support searching for all "&amp;LOWER(B83)&amp;"s for a patient"</f>
@@ -7356,7 +7356,7 @@
         <v>GET [base]/Practitioner/practitioner-1~GET [base]/Practitioner?_id=practitioner-1</v>
       </c>
       <c r="AA84" s="12" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="AB84" s="1" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B84)&amp;"-"&amp;SUBSTITUTE(C84,"_","")&amp;".html")</f>
@@ -7380,7 +7380,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G85" s="1" t="str">
         <f t="shared" ref="G85" si="47">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B85)</f>
@@ -7424,7 +7424,7 @@
         <v>248</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="D86" s="1" t="s">
         <v>70</v>
@@ -7433,7 +7433,7 @@
         <v>0</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G86" s="1" t="str">
         <f t="shared" si="40"/>
@@ -7462,7 +7462,7 @@
         <v>56</v>
       </c>
       <c r="Y86" s="5" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="Z86" s="5" t="str">
         <f>"GET [base]/"&amp;B86&amp;"?"&amp;C86&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -7491,7 +7491,7 @@
         <v>1</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G87" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B87)</f>
@@ -7550,7 +7550,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G88" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B88)</f>
@@ -8203,7 +8203,7 @@
         <v>1</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G100" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8261,7 +8261,7 @@
         <v>1</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G101" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8322,7 +8322,7 @@
         <v>1</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G102" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8374,7 +8374,7 @@
         <v>49</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C103" s="1" t="s">
         <v>62</v>
@@ -8386,7 +8386,7 @@
         <v>0</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G103" s="1" t="str">
         <f t="shared" si="40"/>
@@ -8427,7 +8427,7 @@
         <v>50</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>90</v>
@@ -8439,7 +8439,7 @@
         <v>1</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G104" s="1" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B104)</f>
@@ -8486,7 +8486,7 @@
         <v>51</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>140</v>
@@ -8498,7 +8498,7 @@
         <v>0</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G105" s="1" t="str">
         <f t="shared" ref="G105:G117" si="56">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
@@ -8536,7 +8536,7 @@
         <v>52</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>26</v>
@@ -8548,7 +8548,7 @@
         <v>0</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G106" s="1" t="str">
         <f t="shared" si="56"/>
@@ -8589,10 +8589,10 @@
         <v>53</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>30</v>
@@ -8601,7 +8601,7 @@
         <v>0</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G107" s="1" t="str">
         <f t="shared" si="56"/>
@@ -8643,7 +8643,7 @@
         <v>20</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>55</v>
@@ -8678,10 +8678,10 @@
         <v>56</v>
       </c>
       <c r="Y108" s="5" t="s">
+        <v>591</v>
+      </c>
+      <c r="Z108" s="5" t="s">
         <v>592</v>
-      </c>
-      <c r="Z108" s="5" t="s">
-        <v>593</v>
       </c>
       <c r="AA108" s="2"/>
       <c r="AB108" s="1" t="str">
@@ -8740,7 +8740,7 @@
         <v>20</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C110" s="1" t="s">
         <v>55</v>
@@ -8775,10 +8775,10 @@
         <v>56</v>
       </c>
       <c r="Y110" s="5" t="s">
+        <v>616</v>
+      </c>
+      <c r="Z110" s="5" t="s">
         <v>617</v>
-      </c>
-      <c r="Z110" s="5" t="s">
-        <v>618</v>
       </c>
       <c r="AA110" s="12"/>
       <c r="AB110" s="1" t="str">
@@ -8791,7 +8791,7 @@
         <v>79</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>90</v>
@@ -8803,7 +8803,7 @@
         <v>1</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G111" s="1" t="str">
         <f t="shared" si="56"/>
@@ -8850,7 +8850,7 @@
         <v>80</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>55</v>
@@ -8889,7 +8889,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z112" s="5" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="AB112" s="1" t="str">
         <f t="shared" ref="AB112:AB117" si="59">"SearchParameter-us-core-"&amp;LOWER((B112)&amp;"-"&amp;SUBSTITUTE(C112,"_","")&amp;".html")</f>
@@ -8901,7 +8901,7 @@
         <v>81</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>90</v>
@@ -8913,7 +8913,7 @@
         <v>1</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G113" s="1" t="str">
         <f t="shared" si="56"/>
@@ -8960,7 +8960,7 @@
         <v>82</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C114" s="1" t="s">
         <v>62</v>
@@ -8972,7 +8972,7 @@
         <v>0</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G114" s="1" t="str">
         <f t="shared" si="56"/>
@@ -9001,7 +9001,7 @@
         <v>56</v>
       </c>
       <c r="Y114" s="22" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="AB114" s="1" t="str">
         <f t="shared" si="59"/>
@@ -9013,10 +9013,10 @@
         <v>83</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="D115" s="1" t="s">
         <v>30</v>
@@ -9025,7 +9025,7 @@
         <v>0</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="G115" s="1" t="str">
         <f t="shared" si="56"/>
@@ -9041,16 +9041,16 @@
         <v>57</v>
       </c>
       <c r="L115" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="M115" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y115" s="22" t="s">
         <v>660</v>
-      </c>
-      <c r="M115" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="O115" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y115" s="22" t="s">
-        <v>661</v>
       </c>
       <c r="AB115" s="1" t="str">
         <f t="shared" si="59"/>
@@ -9062,10 +9062,10 @@
         <v>84</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D116" s="1" t="s">
         <v>30</v>
@@ -9074,7 +9074,7 @@
         <v>0</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G116" s="1" t="str">
         <f t="shared" si="56"/>
@@ -9106,7 +9106,7 @@
         <v>93</v>
       </c>
       <c r="Y116" s="22" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="AB116" s="1" t="str">
         <f t="shared" si="59"/>
@@ -9118,10 +9118,10 @@
         <v>85</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D117" s="1" t="s">
         <v>30</v>
@@ -9130,7 +9130,7 @@
         <v>0</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G117" s="1" t="str">
         <f t="shared" si="56"/>
@@ -9156,7 +9156,7 @@
         <v>56</v>
       </c>
       <c r="Y117" s="22" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="AB117" s="1" t="str">
         <f t="shared" si="59"/>
@@ -9214,7 +9214,7 @@
         <v>96</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>97</v>
@@ -9544,7 +9544,7 @@
         <v>304</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K13" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9644,7 +9644,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>70</v>
@@ -9656,7 +9656,7 @@
         <v>305</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K17" s="5" t="str">
         <f t="shared" si="1"/>
@@ -9732,7 +9732,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>70</v>
@@ -9744,7 +9744,7 @@
         <v>310</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="K20" s="5" t="str">
         <f t="shared" si="1"/>
@@ -10168,7 +10168,7 @@
         <v>330</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10195,7 +10195,7 @@
         <v>150</v>
       </c>
       <c r="J36" s="5" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="K36" s="5" t="s">
         <v>146</v>
@@ -10213,7 +10213,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>70</v>
@@ -10225,10 +10225,10 @@
         <v>150</v>
       </c>
       <c r="J37" s="5" t="s">
+        <v>565</v>
+      </c>
+      <c r="K37" s="5" t="s">
         <v>566</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>567</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10285,7 +10285,7 @@
         <v>153</v>
       </c>
       <c r="J39" s="5" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="K39" s="5" t="s">
         <v>156</v>
@@ -10303,7 +10303,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>70</v>
@@ -10315,7 +10315,7 @@
         <v>153</v>
       </c>
       <c r="J40" s="5" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K40" s="5" t="s">
         <v>156</v>
@@ -10333,7 +10333,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>70</v>
@@ -10345,7 +10345,7 @@
         <v>153</v>
       </c>
       <c r="J41" s="5" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="K41" s="5" t="s">
         <v>156</v>
@@ -10363,7 +10363,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>70</v>
@@ -10375,7 +10375,7 @@
         <v>153</v>
       </c>
       <c r="J42" s="5" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="K42" s="5" t="s">
         <v>156</v>
@@ -10408,7 +10408,7 @@
         <v>324</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10435,7 +10435,7 @@
         <v>167</v>
       </c>
       <c r="J44" s="5" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K44" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B44&amp;" resources for the specified "&amp;SUBSTITUTE(D44,","," and ")</f>
@@ -10592,7 +10592,7 @@
         <v>195</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K49" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -10622,7 +10622,7 @@
         <v>226</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K50" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10742,7 +10742,7 @@
         <v>201</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K54" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -10772,7 +10772,7 @@
         <v>220</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K55" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B55&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -10853,7 +10853,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>12</v>
@@ -10862,16 +10862,16 @@
         <v>106</v>
       </c>
       <c r="H58" s="1" t="s">
+        <v>454</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>428</v>
+      </c>
+      <c r="J58" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="I58" s="5" t="s">
-        <v>429</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>456</v>
-      </c>
       <c r="K58" s="5" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="59" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10886,7 +10886,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>12</v>
@@ -10895,16 +10895,16 @@
         <v>106</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I59" s="5" t="s">
         <v>185</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
     </row>
     <row r="60" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10919,7 +10919,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>70</v>
@@ -10928,16 +10928,16 @@
         <v>106</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I60" s="5" t="s">
         <v>185</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="K60" s="5" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
     </row>
     <row r="61" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10952,7 +10952,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>70</v>
@@ -10961,16 +10961,16 @@
         <v>218</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>230</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="K61" s="5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="62" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -10978,7 +10978,7 @@
         <v>73</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C62" s="1" t="str">
         <f t="shared" si="8"/>
@@ -11010,7 +11010,7 @@
         <v>#REF!</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C63" s="1" t="str">
         <f t="shared" si="8"/>
@@ -11121,7 +11121,7 @@
         <v>227</v>
       </c>
       <c r="J66" s="5" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K66" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -11148,13 +11148,13 @@
         <v>106</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I67" s="5" t="s">
         <v>280</v>
       </c>
       <c r="J67" s="5" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="K67" s="5" t="s">
         <v>321</v>
@@ -11180,13 +11180,13 @@
         <v>106</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I68" s="5" t="s">
         <v>221</v>
       </c>
       <c r="J68" s="5" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="K68" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -11243,13 +11243,13 @@
         <v>218</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I70" s="5" t="s">
         <v>225</v>
       </c>
       <c r="J70" s="5" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="K70" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -11279,7 +11279,7 @@
         <v>223</v>
       </c>
       <c r="J71" s="5" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K71" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11375,7 +11375,7 @@
         <v>241</v>
       </c>
       <c r="J74" s="5" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="K74" s="5" t="s">
         <v>245</v>
@@ -11439,7 +11439,7 @@
         <v>240</v>
       </c>
       <c r="J76" s="5" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="K76" s="5" t="s">
         <v>247</v>
@@ -11447,7 +11447,7 @@
     </row>
     <row r="77" spans="1:11" s="1" customFormat="1" ht="136" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>248</v>
@@ -11469,13 +11469,13 @@
         <v>311</v>
       </c>
       <c r="I77" s="5" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="J77" s="5" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="K77" s="12" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="78" spans="1:11" s="1" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -11519,7 +11519,7 @@
         <v>183</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>237</v>
@@ -11531,13 +11531,13 @@
         <v>106</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I79" s="5" t="s">
         <v>279</v>
       </c>
       <c r="J79" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="K79" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B79&amp;" resources for the specified "&amp;SUBSTITUTE(D79,","," and ")</f>
@@ -11552,7 +11552,7 @@
         <v>183</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D80" s="1" t="s">
         <v>145</v>
@@ -11564,13 +11564,13 @@
         <v>106</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I80" s="5" t="s">
         <v>278</v>
       </c>
       <c r="J80" s="5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="K80" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B80&amp;" resources for the specified patient and a category code = `vital-signs`"</f>
@@ -11585,7 +11585,7 @@
         <v>183</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>147</v>
@@ -11597,7 +11597,7 @@
         <v>106</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I81" s="5" t="s">
         <v>281</v>
@@ -11618,7 +11618,7 @@
         <v>183</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>194</v>
@@ -11630,13 +11630,13 @@
         <v>218</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="I82" s="5" t="s">
         <v>283</v>
       </c>
       <c r="J82" s="5" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="K82" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B82&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -11651,7 +11651,7 @@
         <v>183</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D83" s="1" t="s">
         <v>219</v>
@@ -11666,7 +11666,7 @@
         <v>284</v>
       </c>
       <c r="J83" s="5" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="K83" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes."</f>
@@ -11799,7 +11799,7 @@
         <v>296</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K87" s="5" t="s">
         <v>298</v>
@@ -11859,7 +11859,7 @@
         <v>301</v>
       </c>
       <c r="J89" s="5" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="K89" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -11874,7 +11874,7 @@
         <v>249</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>118</v>
@@ -11907,7 +11907,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>70</v>
@@ -11916,13 +11916,13 @@
         <v>106</v>
       </c>
       <c r="I91" s="5" t="s">
+        <v>579</v>
+      </c>
+      <c r="J91" s="5" t="s">
         <v>580</v>
       </c>
-      <c r="J91" s="5" t="s">
+      <c r="K91" s="5" t="s">
         <v>581</v>
-      </c>
-      <c r="K91" s="5" t="s">
-        <v>582</v>
       </c>
     </row>
     <row r="92" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -11930,10 +11930,10 @@
         <v>56</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>116</v>
@@ -11948,7 +11948,7 @@
         <v>303</v>
       </c>
       <c r="J92" s="5" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K92" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -11960,10 +11960,10 @@
         <v>57</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>145</v>
@@ -11978,7 +11978,7 @@
         <v>198</v>
       </c>
       <c r="J93" s="5" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
       <c r="K93" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient and  a category code"</f>
@@ -11990,10 +11990,10 @@
         <v>58</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>147</v>
@@ -12008,7 +12008,7 @@
         <v>199</v>
       </c>
       <c r="J94" s="5" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="K94" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12020,13 +12020,13 @@
         <v>59</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>12</v>
@@ -12038,7 +12038,7 @@
         <v>201</v>
       </c>
       <c r="J95" s="5" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="K95" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date and a category code"</f>
@@ -12050,13 +12050,13 @@
         <v>60</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>70</v>
@@ -12065,10 +12065,10 @@
         <v>218</v>
       </c>
       <c r="I96" s="5" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="J96" s="5" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="K96" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -12087,7 +12087,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="E97" s="1" t="b">
         <v>1</v>
@@ -12099,10 +12099,10 @@
         <v>106</v>
       </c>
       <c r="I97" s="5" t="s">
+        <v>600</v>
+      </c>
+      <c r="J97" s="5" t="s">
         <v>601</v>
-      </c>
-      <c r="J97" s="5" t="s">
-        <v>602</v>
       </c>
       <c r="K97" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified "&amp;SUBSTITUTE(D97,","," and ")</f>
@@ -12114,10 +12114,10 @@
         <v>65</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C98" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>116</v>
@@ -12129,10 +12129,10 @@
         <v>106</v>
       </c>
       <c r="I98" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="J98" s="5" t="s">
         <v>672</v>
-      </c>
-      <c r="J98" s="5" t="s">
-        <v>673</v>
       </c>
       <c r="K98" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified "&amp;SUBSTITUTE(D98,","," and ")</f>
@@ -12144,13 +12144,13 @@
         <v>66</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>70</v>
@@ -12159,13 +12159,13 @@
         <v>106</v>
       </c>
       <c r="H99" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="I99" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="I99" s="1" t="s">
-        <v>672</v>
-      </c>
       <c r="J99" s="5" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="K99" s="1" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified "&amp;SUBSTITUTE(D99,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12177,13 +12177,13 @@
         <v>67</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C100" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>70</v>
@@ -12192,10 +12192,10 @@
         <v>149</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J100" s="5" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="K100" s="5" t="str">
         <f>"Fetches a bundle of all "&amp;B100&amp;" resources for the specified patient and date"</f>
@@ -12207,13 +12207,13 @@
         <v>68</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C101" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D101" s="20" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>70</v>
@@ -12222,13 +12222,13 @@
         <v>218</v>
       </c>
       <c r="H101" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="I101" s="1" t="s">
         <v>671</v>
       </c>
-      <c r="I101" s="1" t="s">
-        <v>672</v>
-      </c>
       <c r="J101" s="5" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K101" s="1" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12240,13 +12240,13 @@
         <v>69</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="C102" s="21" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D102" s="20" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="F102" s="1" t="s">
         <v>70</v>
@@ -12255,10 +12255,10 @@
         <v>91</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J102" s="5" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="K102" s="1" t="str">
         <f>"Fetches a bundle of all "&amp;B102&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12311,15 +12311,15 @@
         <v>67</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="4" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="139.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12327,7 +12327,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -12343,7 +12343,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12351,36 +12351,36 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>70</v>
@@ -12411,7 +12411,7 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
@@ -12422,13 +12422,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -12436,13 +12436,13 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="11" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>70</v>
@@ -12479,16 +12479,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>531</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>532</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>60</v>
@@ -12502,13 +12502,13 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="E2" s="19" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>12</v>
@@ -12600,10 +12600,10 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="21" t="s">
+        <v>632</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>633</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>634</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
@@ -12615,10 +12615,10 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
+        <v>639</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>640</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>641</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>12</v>
@@ -12630,10 +12630,10 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
@@ -12690,7 +12690,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>365</v>
@@ -12705,91 +12705,91 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>626</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>627</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>628</v>
       </c>
       <c r="G12" s="1"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G13" s="1"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G15" s="1"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="21" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="G17" s="1"/>
     </row>
@@ -12883,10 +12883,10 @@
     </row>
     <row r="24" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="21" t="s">
+        <v>628</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>629</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>630</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>12</v>
@@ -12897,10 +12897,10 @@
     </row>
     <row r="25" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A25" s="21" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>12</v>
@@ -12911,10 +12911,10 @@
     </row>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="21" t="s">
+        <v>630</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>631</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>632</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>12</v>
@@ -12925,10 +12925,10 @@
     </row>
     <row r="27" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A27" s="21" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>12</v>
@@ -12939,10 +12939,10 @@
     </row>
     <row r="28" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="21" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>12</v>
@@ -12953,10 +12953,10 @@
     </row>
     <row r="29" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="21" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>12</v>
@@ -12967,10 +12967,10 @@
     </row>
     <row r="30" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="21" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>12</v>
@@ -12995,10 +12995,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" s="21" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>12</v>
@@ -13010,10 +13010,10 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" s="21" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>12</v>
@@ -13025,10 +13025,10 @@
     </row>
     <row r="34" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="21" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>12</v>
@@ -13039,10 +13039,10 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" s="21" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>12</v>
@@ -13054,10 +13054,10 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" s="21" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>12</v>
@@ -13069,10 +13069,10 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" s="21" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>12</v>
@@ -13083,10 +13083,10 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" s="21" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>12</v>
@@ -13097,10 +13097,10 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" s="21" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>12</v>
@@ -13111,10 +13111,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" s="21" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>12</v>
@@ -13125,10 +13125,10 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" s="21" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>12</v>
@@ -13139,10 +13139,10 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="21" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>12</v>
@@ -13153,10 +13153,10 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" s="21" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>12</v>
@@ -13237,58 +13237,58 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="21" t="s">
+        <v>438</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>440</v>
-      </c>
       <c r="D49" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="21" t="s">
+        <v>644</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>645</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="D50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>646</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="21" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="21" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
   </sheetData>
@@ -13306,10 +13306,10 @@
   <dimension ref="A1:Y62"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Q5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B23" sqref="B23"/>
+      <selection pane="bottomRight" activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13342,7 +13342,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
@@ -13393,16 +13393,16 @@
         <v>406</v>
       </c>
       <c r="V1" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="W1" s="4" t="s">
+        <v>532</v>
+      </c>
+      <c r="X1" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="W1" s="4" t="s">
-        <v>533</v>
-      </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>535</v>
-      </c>
-      <c r="Y1" s="4" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -13424,7 +13424,7 @@
         <v>70</v>
       </c>
       <c r="X2" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y2" s="17" t="s">
         <v>12</v>
@@ -13438,7 +13438,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="T3" s="1" t="s">
         <v>19</v>
@@ -13447,7 +13447,7 @@
         <v>70</v>
       </c>
       <c r="X3" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y3" s="17" t="s">
         <v>12</v>
@@ -13461,7 +13461,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="T4" s="1" t="s">
         <v>19</v>
@@ -13470,13 +13470,13 @@
         <v>70</v>
       </c>
       <c r="V4" s="1" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="W4" s="1" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="X4" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y4" s="17" t="s">
         <v>12</v>
@@ -13490,7 +13490,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="T5" s="1" t="s">
         <v>19</v>
@@ -13499,7 +13499,7 @@
         <v>70</v>
       </c>
       <c r="X5" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y5" s="17" t="s">
         <v>12</v>
@@ -13513,7 +13513,7 @@
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="T6" s="1" t="s">
         <v>19</v>
@@ -13522,7 +13522,7 @@
         <v>70</v>
       </c>
       <c r="X6" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y6" s="17" t="s">
         <v>12</v>
@@ -13536,7 +13536,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="T7" s="1" t="s">
         <v>19</v>
@@ -13545,7 +13545,7 @@
         <v>70</v>
       </c>
       <c r="X7" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y7" s="17" t="s">
         <v>12</v>
@@ -13568,7 +13568,7 @@
         <v>70</v>
       </c>
       <c r="X8" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y8" s="17" t="s">
         <v>12</v>
@@ -13582,7 +13582,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="T9" s="1" t="s">
         <v>19</v>
@@ -13591,7 +13591,7 @@
         <v>70</v>
       </c>
       <c r="X9" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y9" s="17" t="s">
         <v>12</v>
@@ -13611,7 +13611,7 @@
         <v>70</v>
       </c>
       <c r="X10" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y10" s="17" t="s">
         <v>12</v>
@@ -13625,7 +13625,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="T11" s="1" t="s">
         <v>19</v>
@@ -13634,7 +13634,7 @@
         <v>70</v>
       </c>
       <c r="X11" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y11" s="17" t="s">
         <v>12</v>
@@ -13648,7 +13648,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="T12" s="1" t="s">
         <v>19</v>
@@ -13667,7 +13667,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="T13" s="1" t="s">
         <v>19</v>
@@ -13686,7 +13686,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="T14" s="1" t="s">
         <v>19</v>
@@ -13701,7 +13701,7 @@
         <v>208</v>
       </c>
       <c r="X14" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y14" s="17" t="s">
         <v>12</v>
@@ -13709,13 +13709,13 @@
     </row>
     <row r="15" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T15" s="1" t="s">
         <v>19</v>
@@ -13730,7 +13730,7 @@
         <v>395</v>
       </c>
       <c r="X15" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y15" s="17" t="s">
         <v>12</v>
@@ -13744,7 +13744,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="T16" s="1" t="s">
         <v>19</v>
@@ -13753,7 +13753,7 @@
         <v>70</v>
       </c>
       <c r="X16" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y16" s="17" t="s">
         <v>12</v>
@@ -13783,7 +13783,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="T18" s="1" t="s">
         <v>19</v>
@@ -13792,7 +13792,7 @@
         <v>70</v>
       </c>
       <c r="X18" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y18" s="17" t="s">
         <v>12</v>
@@ -13822,7 +13822,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="T20" s="1" t="s">
         <v>19</v>
@@ -13831,7 +13831,7 @@
         <v>70</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="W20" s="1" t="s">
         <v>273</v>
@@ -13847,7 +13847,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="T21" s="1" t="s">
         <v>19</v>
@@ -13856,7 +13856,7 @@
         <v>70</v>
       </c>
       <c r="X21" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y21" s="17" t="s">
         <v>12</v>
@@ -13864,13 +13864,13 @@
     </row>
     <row r="22" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="T22" s="1" t="s">
         <v>19</v>
@@ -13881,13 +13881,13 @@
     </row>
     <row r="23" spans="1:25" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>70</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -13898,7 +13898,7 @@
         <v>70</v>
       </c>
       <c r="X23" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y23" s="17" t="s">
         <v>12</v>
@@ -13906,7 +13906,7 @@
     </row>
     <row r="24" spans="1:25" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>12</v>
@@ -13921,7 +13921,7 @@
         <v>70</v>
       </c>
       <c r="X24" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y24" s="17" t="s">
         <v>12</v>
@@ -13929,7 +13929,7 @@
     </row>
     <row r="25" spans="1:25" s="1" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>12</v>
@@ -13944,7 +13944,7 @@
         <v>70</v>
       </c>
       <c r="X25" s="17" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="Y25" s="17" t="s">
         <v>12</v>
@@ -13952,7 +13952,7 @@
     </row>
     <row r="26" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>70</v>
@@ -13985,8 +13985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14028,24 +14028,24 @@
         <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>415</v>
+        <v>678</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B3" t="s">
         <v>446</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>447</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>448</v>
-      </c>
-      <c r="D3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -14106,7 +14106,7 @@
         <v>372</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>373</v>
@@ -14139,7 +14139,7 @@
         <v>382</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>383</v>
@@ -14157,19 +14157,19 @@
         <v>387</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="Z1" s="1" t="s">
+        <v>614</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="AA1" s="1" t="s">
-        <v>616</v>
-      </c>
       <c r="AB1" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
     </row>
     <row r="2" spans="1:28" ht="64" x14ac:dyDescent="0.2">
@@ -14192,7 +14192,7 @@
         <v>30</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -14895,12 +14895,12 @@
         <v>25</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>30</v>
@@ -14909,7 +14909,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>30</v>
@@ -14918,7 +14918,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>30</v>
@@ -14927,7 +14927,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
FHIR-35297  add medicationdispense ( still need to complete the quick start)
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F68D08-9397-5A40-9C86-F48937169D22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804ED81B-1314-054D-B746-F6FAA5EDA11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9820" yWindow="-28300" windowWidth="34120" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="140" yWindow="500" windowWidth="36720" windowHeight="28080" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2592" uniqueCount="690">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="708">
   <si>
     <t>Element</t>
   </si>
@@ -2325,6 +2325,64 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-occupation</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-specimen</t>
+  </si>
+  <si>
+    <t>US Core Specimen Profile</t>
+  </si>
+  <si>
+    <t>Specimen</t>
+  </si>
+  <si>
+    <t>conf_Specimen</t>
+  </si>
+  <si>
+    <t>conf_SpecimenRequest</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</t>
+  </si>
+  <si>
+    <t>US Core MedicationDispense Profile</t>
+  </si>
+  <si>
+    <t>MedicationDispense</t>
+  </si>
+  <si>
+    <t>MedicationDispense:medication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* The MedicationDispense resources can represent a medication using either a code or refer to the Medication resource. When referencing Medication, the resource may be [contained](http://hl7.org/fhir/R4/references.html#contained) or an external resource. The server application **MAY** choose any one way or more than one method, but if an external reference to Medication is used, the server **SHALL** support the _include` parameter for searching this element. The client application must support all methods.
+ For example, A server **SHALL** be capable of returning dispense records for all medications for a patient using one of or both:
+ `GET /MedicationDispense?patient=[id]`
+ `GET /MedicationDispense?patient=[id]&amp;_include=MedicationDispense:medication`
+</t>
+  </si>
+  <si>
+    <t>conf_MedicationDispense</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on there dispensed status and dispense type.</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>patient,whenhandedover</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on when it was dispensed to the patient.</t>
+  </si>
+  <si>
+    <t>!MedicationDispense</t>
+  </si>
+  <si>
+    <t>whenHandedOver</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on there dispensed status</t>
   </si>
 </sst>
 </file>
@@ -2941,13 +2999,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AB118"/>
+  <dimension ref="A1:AB122"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I101" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C84" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L128" sqref="L128"/>
+      <selection pane="bottomRight" activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8543,7 +8601,7 @@
         <v>505</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" ref="G105:G118" si="56">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
+        <f t="shared" ref="G105:G122" si="56">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H105" t="s">
@@ -8916,7 +8974,7 @@
         <v>57</v>
       </c>
       <c r="L112" t="str">
-        <f t="shared" ref="L112:L118" si="58">B112&amp;"."&amp;C112</f>
+        <f t="shared" ref="L112:L122" si="58">B112&amp;"."&amp;C112</f>
         <v>QuestionnaireResponse._id</v>
       </c>
       <c r="M112" t="s">
@@ -9263,6 +9321,229 @@
       <c r="AB118" t="str">
         <f t="shared" si="59"/>
         <v>SearchParameter-us-core-coverage-patient.html</v>
+      </c>
+    </row>
+    <row r="119" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A119">
+        <v>87</v>
+      </c>
+      <c r="B119" t="s">
+        <v>697</v>
+      </c>
+      <c r="C119" t="s">
+        <v>62</v>
+      </c>
+      <c r="D119" t="s">
+        <v>30</v>
+      </c>
+      <c r="E119" t="b">
+        <v>0</v>
+      </c>
+      <c r="F119" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="G119" t="str">
+        <f t="shared" si="56"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+      </c>
+      <c r="H119" t="s">
+        <v>56</v>
+      </c>
+      <c r="I119" t="s">
+        <v>56</v>
+      </c>
+      <c r="J119" t="s">
+        <v>56</v>
+      </c>
+      <c r="K119" t="s">
+        <v>57</v>
+      </c>
+      <c r="L119" t="str">
+        <f t="shared" si="58"/>
+        <v>MedicationDispense.status</v>
+      </c>
+      <c r="M119" t="s">
+        <v>56</v>
+      </c>
+      <c r="N119" t="s">
+        <v>12</v>
+      </c>
+      <c r="O119" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y119" s="4"/>
+      <c r="Z119" s="4"/>
+      <c r="AA119" s="10"/>
+      <c r="AB119" t="str">
+        <f t="shared" ref="AB119:AB122" si="60">"SearchParameter-us-core-"&amp;LOWER((B119)&amp;"-"&amp;C119&amp;".html")</f>
+        <v>SearchParameter-us-core-medicationdispense-status.html</v>
+      </c>
+    </row>
+    <row r="120" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120">
+        <v>88</v>
+      </c>
+      <c r="B120" t="s">
+        <v>697</v>
+      </c>
+      <c r="C120" t="s">
+        <v>13</v>
+      </c>
+      <c r="D120" t="s">
+        <v>30</v>
+      </c>
+      <c r="E120" t="b">
+        <v>0</v>
+      </c>
+      <c r="F120" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="G120" t="str">
+        <f t="shared" si="56"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+      </c>
+      <c r="H120" t="s">
+        <v>56</v>
+      </c>
+      <c r="I120" t="s">
+        <v>56</v>
+      </c>
+      <c r="J120" t="s">
+        <v>56</v>
+      </c>
+      <c r="K120" t="s">
+        <v>57</v>
+      </c>
+      <c r="L120" t="str">
+        <f t="shared" si="58"/>
+        <v>MedicationDispense.type</v>
+      </c>
+      <c r="M120" t="s">
+        <v>56</v>
+      </c>
+      <c r="N120" t="s">
+        <v>12</v>
+      </c>
+      <c r="O120" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y120" s="4"/>
+      <c r="Z120" s="4"/>
+      <c r="AA120" s="10"/>
+      <c r="AB120" t="str">
+        <f t="shared" si="60"/>
+        <v>SearchParameter-us-core-medicationdispense-type.html</v>
+      </c>
+    </row>
+    <row r="121" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A121">
+        <v>89</v>
+      </c>
+      <c r="B121" t="s">
+        <v>697</v>
+      </c>
+      <c r="C121" t="s">
+        <v>90</v>
+      </c>
+      <c r="D121" t="s">
+        <v>12</v>
+      </c>
+      <c r="E121" t="b">
+        <v>1</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="G121" t="str">
+        <f t="shared" si="56"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+      </c>
+      <c r="H121" t="s">
+        <v>56</v>
+      </c>
+      <c r="I121" t="s">
+        <v>56</v>
+      </c>
+      <c r="J121" t="s">
+        <v>56</v>
+      </c>
+      <c r="K121" t="s">
+        <v>91</v>
+      </c>
+      <c r="L121" t="str">
+        <f t="shared" si="58"/>
+        <v>MedicationDispense.patient</v>
+      </c>
+      <c r="M121" t="s">
+        <v>56</v>
+      </c>
+      <c r="O121" t="s">
+        <v>56</v>
+      </c>
+      <c r="W121" s="6"/>
+      <c r="X121" s="6"/>
+      <c r="Z121" s="10"/>
+      <c r="AA121" s="10"/>
+      <c r="AB121" t="str">
+        <f t="shared" si="60"/>
+        <v>SearchParameter-us-core-medicationdispense-patient.html</v>
+      </c>
+    </row>
+    <row r="122" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A122">
+        <v>61</v>
+      </c>
+      <c r="B122" t="s">
+        <v>705</v>
+      </c>
+      <c r="C122" t="s">
+        <v>706</v>
+      </c>
+      <c r="D122" t="s">
+        <v>30</v>
+      </c>
+      <c r="E122" t="b">
+        <v>0</v>
+      </c>
+      <c r="F122" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="G122" t="str">
+        <f t="shared" si="56"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
+      </c>
+      <c r="H122" t="s">
+        <v>56</v>
+      </c>
+      <c r="I122" t="s">
+        <v>56</v>
+      </c>
+      <c r="J122" t="s">
+        <v>56</v>
+      </c>
+      <c r="K122" t="s">
+        <v>79</v>
+      </c>
+      <c r="L122" t="str">
+        <f t="shared" si="58"/>
+        <v>!MedicationDispense.whenHandedOver</v>
+      </c>
+      <c r="M122" t="s">
+        <v>56</v>
+      </c>
+      <c r="O122" t="s">
+        <v>56</v>
+      </c>
+      <c r="P122" t="s">
+        <v>70</v>
+      </c>
+      <c r="S122" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA122" s="10"/>
+      <c r="AB122" t="str">
+        <f t="shared" si="60"/>
+        <v>SearchParameter-us-core-!medicationdispense-whenhandedover.html</v>
       </c>
     </row>
   </sheetData>
@@ -9278,13 +9559,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K102"/>
+  <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C77" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C77" sqref="C77"/>
+      <selection pane="bottomRight" activeCell="C110" sqref="C110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -11989,7 +12270,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>94</v>
+        <v>116</v>
       </c>
       <c r="B91" t="s">
         <v>248</v>
@@ -12019,7 +12300,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>56</v>
+        <v>117</v>
       </c>
       <c r="B92" t="s">
         <v>579</v>
@@ -12049,7 +12330,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>57</v>
+        <v>118</v>
       </c>
       <c r="B93" t="s">
         <v>579</v>
@@ -12079,7 +12360,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>58</v>
+        <v>119</v>
       </c>
       <c r="B94" t="s">
         <v>579</v>
@@ -12109,7 +12390,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>59</v>
+        <v>120</v>
       </c>
       <c r="B95" t="s">
         <v>579</v>
@@ -12139,7 +12420,7 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>60</v>
+        <v>121</v>
       </c>
       <c r="B96" t="s">
         <v>579</v>
@@ -12169,7 +12450,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="B97" t="s">
         <v>180</v>
@@ -12200,7 +12481,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>65</v>
+        <v>123</v>
       </c>
       <c r="B98" t="s">
         <v>630</v>
@@ -12230,7 +12511,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>66</v>
+        <v>124</v>
       </c>
       <c r="B99" t="s">
         <v>630</v>
@@ -12263,7 +12544,7 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>67</v>
+        <v>125</v>
       </c>
       <c r="B100" t="s">
         <v>630</v>
@@ -12293,7 +12574,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>68</v>
+        <v>126</v>
       </c>
       <c r="B101" t="s">
         <v>630</v>
@@ -12326,7 +12607,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>69</v>
+        <v>127</v>
       </c>
       <c r="B102" t="s">
         <v>630</v>
@@ -12352,6 +12633,108 @@
       <c r="K102" t="str">
         <f>"Fetches a bundle of all "&amp;B102&amp;" resources for the specified patient that have been completed against a specified form."</f>
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A103">
+        <v>129</v>
+      </c>
+      <c r="B103" s="18" t="s">
+        <v>697</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="D103" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="E103" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F103" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G103" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="H103" s="18"/>
+      <c r="I103" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="J103" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="K103" t="str">
+        <f>"Fetches a bundle of all "&amp;B103&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed)).</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A104">
+        <v>129</v>
+      </c>
+      <c r="B104" s="18" t="s">
+        <v>697</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="D104" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E104" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F104" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G104" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="H104" s="18"/>
+      <c r="I104" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="J104" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="K104" t="str">
+        <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed).</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A105">
+        <v>130</v>
+      </c>
+      <c r="B105" s="18" t="s">
+        <v>705</v>
+      </c>
+      <c r="C105" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="D105" s="18" t="s">
+        <v>703</v>
+      </c>
+      <c r="E105" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F105" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G105" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="H105" s="18"/>
+      <c r="I105" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="J105" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="K105" t="str">
+        <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient for a given dispense and date or range"</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient for a given dispense and date or range</v>
       </c>
     </row>
   </sheetData>
@@ -12603,10 +12986,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="B12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12706,7 +13089,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" t="s">
         <v>679</v>
       </c>
       <c r="B7" t="s">
@@ -12888,7 +13271,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="21" t="s">
+      <c r="A20" t="s">
         <v>341</v>
       </c>
       <c r="B20" t="s">
@@ -12944,25 +13327,25 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="21" t="s">
+        <v>695</v>
+      </c>
+      <c r="B24" t="s">
+        <v>696</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="19" t="s">
         <v>413</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>412</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="21" t="s">
-        <v>688</v>
-      </c>
-      <c r="B25" t="s">
-        <v>684</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
@@ -12972,11 +13355,11 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="21" t="s">
-        <v>687</v>
+      <c r="A26" t="s">
+        <v>688</v>
       </c>
       <c r="B26" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -12986,11 +13369,11 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="21" t="s">
-        <v>689</v>
+      <c r="A27" t="s">
+        <v>687</v>
       </c>
       <c r="B27" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -13000,11 +13383,11 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="19" t="s">
-        <v>614</v>
+      <c r="A28" t="s">
+        <v>689</v>
       </c>
       <c r="B28" t="s">
-        <v>615</v>
+        <v>686</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -13015,10 +13398,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>492</v>
+        <v>614</v>
       </c>
       <c r="B29" t="s">
-        <v>483</v>
+        <v>615</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -13029,10 +13412,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>616</v>
+        <v>492</v>
       </c>
       <c r="B30" t="s">
-        <v>617</v>
+        <v>483</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -13043,10 +13426,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
-        <v>491</v>
+        <v>616</v>
       </c>
       <c r="B31" t="s">
-        <v>482</v>
+        <v>617</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -13057,10 +13440,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B32" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -13071,10 +13454,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
-        <v>501</v>
+        <v>490</v>
       </c>
       <c r="B33" t="s">
-        <v>500</v>
+        <v>481</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -13085,10 +13468,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
-        <v>441</v>
+        <v>501</v>
       </c>
       <c r="B34" t="s">
-        <v>440</v>
+        <v>500</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
@@ -13099,10 +13482,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="19" t="s">
-        <v>275</v>
+        <v>441</v>
       </c>
       <c r="B35" t="s">
-        <v>343</v>
+        <v>440</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -13113,10 +13496,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="19" t="s">
-        <v>577</v>
+        <v>275</v>
       </c>
       <c r="B36" t="s">
-        <v>619</v>
+        <v>343</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
@@ -13127,10 +13510,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
-        <v>487</v>
+        <v>577</v>
       </c>
       <c r="B37" t="s">
-        <v>478</v>
+        <v>619</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -13141,10 +13524,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B38" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -13155,10 +13538,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="B39" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -13169,10 +13552,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
-        <v>622</v>
+        <v>486</v>
       </c>
       <c r="B40" t="s">
-        <v>611</v>
+        <v>477</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -13183,10 +13566,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>485</v>
+        <v>622</v>
       </c>
       <c r="B41" t="s">
-        <v>476</v>
+        <v>611</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -13197,10 +13580,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>601</v>
+        <v>485</v>
       </c>
       <c r="B42" t="s">
-        <v>626</v>
+        <v>476</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -13211,10 +13594,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="B43" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -13225,10 +13608,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>498</v>
+        <v>600</v>
       </c>
       <c r="B44" t="s">
-        <v>497</v>
+        <v>627</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -13239,10 +13622,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B45" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -13253,10 +13636,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="B46" t="s">
-        <v>480</v>
+        <v>499</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -13267,10 +13650,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
-        <v>484</v>
+        <v>489</v>
       </c>
       <c r="B47" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -13281,134 +13664,162 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
-        <v>348</v>
+        <v>484</v>
       </c>
       <c r="B48" t="s">
-        <v>349</v>
+        <v>475</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
       </c>
       <c r="E48" t="s">
-        <v>260</v>
+        <v>183</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="19" t="s">
-        <v>75</v>
+        <v>348</v>
       </c>
       <c r="B49" t="s">
-        <v>364</v>
+        <v>349</v>
       </c>
       <c r="D49" t="s">
         <v>12</v>
       </c>
       <c r="E49" t="s">
-        <v>21</v>
+        <v>260</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="19" t="s">
-        <v>339</v>
+        <v>75</v>
       </c>
       <c r="B50" t="s">
-        <v>340</v>
+        <v>364</v>
       </c>
       <c r="D50" t="s">
         <v>12</v>
       </c>
       <c r="E50" t="s">
-        <v>267</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="19" t="s">
-        <v>356</v>
+        <v>339</v>
       </c>
       <c r="B51" t="s">
-        <v>357</v>
+        <v>340</v>
       </c>
       <c r="D51" t="s">
         <v>12</v>
       </c>
       <c r="E51" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="19" t="s">
-        <v>350</v>
+        <v>356</v>
       </c>
       <c r="B52" t="s">
-        <v>351</v>
+        <v>357</v>
       </c>
       <c r="D52" t="s">
         <v>12</v>
       </c>
       <c r="E52" t="s">
-        <v>182</v>
+        <v>269</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="19" t="s">
-        <v>437</v>
+        <v>350</v>
       </c>
       <c r="B53" t="s">
-        <v>438</v>
+        <v>351</v>
       </c>
       <c r="D53" t="s">
         <v>12</v>
       </c>
       <c r="E53" t="s">
-        <v>436</v>
+        <v>182</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="19" t="s">
-        <v>628</v>
+        <v>437</v>
       </c>
       <c r="B54" t="s">
-        <v>629</v>
+        <v>438</v>
       </c>
       <c r="D54" t="s">
         <v>12</v>
       </c>
       <c r="E54" t="s">
-        <v>630</v>
+        <v>436</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
-        <v>599</v>
+        <v>628</v>
       </c>
       <c r="B55" t="s">
-        <v>597</v>
+        <v>629</v>
       </c>
       <c r="D55" t="s">
         <v>12</v>
       </c>
       <c r="E55" t="s">
-        <v>602</v>
+        <v>630</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
+        <v>599</v>
+      </c>
+      <c r="B56" t="s">
+        <v>597</v>
+      </c>
+      <c r="D56" t="s">
+        <v>12</v>
+      </c>
+      <c r="E56" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="19" t="s">
         <v>589</v>
       </c>
-      <c r="B56" t="s">
+      <c r="B57" t="s">
         <v>598</v>
       </c>
-      <c r="D56" t="s">
-        <v>12</v>
-      </c>
-      <c r="E56" t="s">
+      <c r="D57" t="s">
+        <v>12</v>
+      </c>
+      <c r="E57" t="s">
         <v>579</v>
       </c>
     </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58" s="19" t="s">
+        <v>690</v>
+      </c>
+      <c r="B58" t="s">
+        <v>691</v>
+      </c>
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
+        <v>692</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E42">
-    <sortCondition ref="E2:E42"/>
-    <sortCondition ref="B2:B42"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E43">
+    <sortCondition ref="E2:E43"/>
+    <sortCondition ref="B2:B43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -13417,13 +13828,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:Y63"/>
+  <dimension ref="A1:Y65"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="S6" sqref="S6"/>
+      <selection pane="bottomRight" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13839,13 +14250,13 @@
     </row>
     <row r="16" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>435</v>
+        <v>697</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>473</v>
+        <v>699</v>
       </c>
       <c r="T16" t="s">
         <v>19</v>
@@ -13857,7 +14268,7 @@
         <v>70</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>395</v>
+        <v>698</v>
       </c>
       <c r="X16" s="15" t="s">
         <v>449</v>
@@ -13868,13 +14279,13 @@
     </row>
     <row r="17" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>183</v>
+        <v>435</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>668</v>
+        <v>473</v>
       </c>
       <c r="T17" t="s">
         <v>19</v>
@@ -13882,6 +14293,12 @@
       <c r="U17" t="s">
         <v>70</v>
       </c>
+      <c r="V17" t="s">
+        <v>70</v>
+      </c>
+      <c r="W17" s="6" t="s">
+        <v>395</v>
+      </c>
       <c r="X17" s="15" t="s">
         <v>449</v>
       </c>
@@ -13891,13 +14308,13 @@
     </row>
     <row r="18" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>260</v>
+        <v>183</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="T18" t="s">
         <v>19</v>
@@ -13905,18 +14322,22 @@
       <c r="U18" t="s">
         <v>70</v>
       </c>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
+      <c r="X18" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y18" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="19" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>260</v>
       </c>
       <c r="B19" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="T19" t="s">
         <v>19</v>
@@ -13924,19 +14345,18 @@
       <c r="U19" t="s">
         <v>70</v>
       </c>
-      <c r="X19" s="15" t="s">
-        <v>449</v>
-      </c>
-      <c r="Y19" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
     </row>
     <row r="20" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>267</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
         <v>12</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>666</v>
       </c>
       <c r="T20" t="s">
         <v>19</v>
@@ -13944,18 +14364,19 @@
       <c r="U20" t="s">
         <v>70</v>
       </c>
-      <c r="X20" s="15"/>
-      <c r="Y20" s="15"/>
+      <c r="X20" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y20" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="21" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="B21" t="s">
         <v>12</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>495</v>
       </c>
       <c r="T21" t="s">
         <v>19</v>
@@ -13963,24 +14384,18 @@
       <c r="U21" t="s">
         <v>70</v>
       </c>
-      <c r="V21" t="s">
-        <v>531</v>
-      </c>
-      <c r="W21" t="s">
-        <v>273</v>
-      </c>
       <c r="X21" s="15"/>
       <c r="Y21" s="15"/>
     </row>
     <row r="22" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>182</v>
+        <v>269</v>
       </c>
       <c r="B22" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>665</v>
+        <v>495</v>
       </c>
       <c r="T22" t="s">
         <v>19</v>
@@ -13988,22 +14403,24 @@
       <c r="U22" t="s">
         <v>70</v>
       </c>
-      <c r="X22" s="15" t="s">
-        <v>449</v>
-      </c>
-      <c r="Y22" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V22" t="s">
+        <v>531</v>
+      </c>
+      <c r="W22" t="s">
+        <v>273</v>
+      </c>
+      <c r="X22" s="15"/>
+      <c r="Y22" s="15"/>
+    </row>
+    <row r="23" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>436</v>
+        <v>182</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="T23" t="s">
         <v>19</v>
@@ -14011,16 +14428,22 @@
       <c r="U23" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X23" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y23" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>630</v>
+        <v>436</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>639</v>
+        <v>664</v>
       </c>
       <c r="T24" t="s">
         <v>19</v>
@@ -14028,19 +14451,16 @@
       <c r="U24" t="s">
         <v>70</v>
       </c>
-      <c r="X24" s="15" t="s">
-        <v>449</v>
-      </c>
-      <c r="Y24" s="15" t="s">
-        <v>12</v>
-      </c>
     </row>
     <row r="25" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>602</v>
+        <v>630</v>
       </c>
       <c r="B25" t="s">
-        <v>12</v>
+        <v>70</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>639</v>
       </c>
       <c r="T25" t="s">
         <v>19</v>
@@ -14057,7 +14477,7 @@
     </row>
     <row r="26" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>579</v>
+        <v>602</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
@@ -14075,25 +14495,61 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>579</v>
+      </c>
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="T27" t="s">
+        <v>19</v>
+      </c>
+      <c r="U27" t="s">
+        <v>70</v>
+      </c>
+      <c r="X27" s="15" t="s">
+        <v>449</v>
+      </c>
+      <c r="Y27" s="15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>692</v>
+      </c>
+      <c r="B28" t="s">
+        <v>12</v>
+      </c>
+      <c r="T28" t="s">
+        <v>19</v>
+      </c>
+      <c r="U28" t="s">
+        <v>70</v>
+      </c>
+      <c r="X28" s="15"/>
+      <c r="Y28" s="15"/>
+    </row>
+    <row r="29" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>446</v>
       </c>
-      <c r="B27" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="60" spans="22:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V60" s="6"/>
-      <c r="X60" s="6"/>
-      <c r="Y60" s="6"/>
-    </row>
-    <row r="63" spans="22:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="Y63" s="6"/>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="62" spans="22:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V62" s="6"/>
+      <c r="X62" s="6"/>
+      <c r="Y62" s="6"/>
+    </row>
+    <row r="65" spans="25:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="Y65" s="6"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A22">
-    <sortCondition ref="A2:A22"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:A23">
+    <sortCondition ref="A2:A23"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -14177,13 +14633,13 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AF10"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomRight" activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14196,16 +14652,19 @@
     <col min="8" max="8" width="58.33203125" style="1" customWidth="1"/>
     <col min="9" max="9" width="28.1640625" customWidth="1"/>
     <col min="15" max="15" width="17.33203125" customWidth="1"/>
-    <col min="18" max="19" width="31.33203125" customWidth="1"/>
-    <col min="22" max="22" width="22.6640625" customWidth="1"/>
-    <col min="23" max="23" width="38.33203125" customWidth="1"/>
-    <col min="24" max="24" width="23" customWidth="1"/>
-    <col min="25" max="26" width="36.5" customWidth="1"/>
-    <col min="27" max="27" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="31.33203125" customWidth="1"/>
+    <col min="23" max="23" width="22.6640625" customWidth="1"/>
+    <col min="24" max="24" width="38.33203125" customWidth="1"/>
+    <col min="25" max="25" width="23" customWidth="1"/>
+    <col min="26" max="27" width="36.5" customWidth="1"/>
+    <col min="28" max="28" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -14252,49 +14711,58 @@
         <v>379</v>
       </c>
       <c r="P1" t="s">
+        <v>700</v>
+      </c>
+      <c r="Q1" t="s">
         <v>380</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>381</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>382</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>450</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>383</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>384</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>385</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>386</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>387</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>439</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>640</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>604</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>605</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
+        <v>693</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>694</v>
+      </c>
+      <c r="AF1" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="2" spans="1:29" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:32" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -14349,7 +14817,7 @@
       <c r="R2" t="s">
         <v>30</v>
       </c>
-      <c r="T2" t="s">
+      <c r="S2" t="s">
         <v>30</v>
       </c>
       <c r="U2" t="s">
@@ -14376,8 +14844,17 @@
       <c r="AB2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AC2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -14429,10 +14906,10 @@
       <c r="R3" t="s">
         <v>12</v>
       </c>
-      <c r="S3" s="1"/>
-      <c r="T3" t="s">
-        <v>12</v>
-      </c>
+      <c r="S3" t="s">
+        <v>12</v>
+      </c>
+      <c r="T3" s="1"/>
       <c r="U3" t="s">
         <v>12</v>
       </c>
@@ -14446,19 +14923,28 @@
         <v>12</v>
       </c>
       <c r="Y3" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="Z3" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="AA3" t="s">
         <v>12</v>
       </c>
       <c r="AB3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+        <v>12</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -14510,7 +14996,7 @@
       <c r="R4" t="s">
         <v>12</v>
       </c>
-      <c r="T4" t="s">
+      <c r="S4" t="s">
         <v>12</v>
       </c>
       <c r="U4" t="s">
@@ -14537,8 +15023,17 @@
       <c r="AB4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AC4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>12</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -14590,7 +15085,7 @@
       <c r="R5" t="s">
         <v>70</v>
       </c>
-      <c r="T5" t="s">
+      <c r="S5" t="s">
         <v>70</v>
       </c>
       <c r="U5" t="s">
@@ -14617,8 +15112,17 @@
       <c r="AB5" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AC5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -14670,7 +15174,7 @@
       <c r="R6" t="s">
         <v>30</v>
       </c>
-      <c r="T6" t="s">
+      <c r="S6" t="s">
         <v>30</v>
       </c>
       <c r="U6" t="s">
@@ -14697,8 +15201,17 @@
       <c r="AB6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AC6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -14750,7 +15263,7 @@
       <c r="R7" t="s">
         <v>30</v>
       </c>
-      <c r="T7" t="s">
+      <c r="S7" t="s">
         <v>30</v>
       </c>
       <c r="U7" t="s">
@@ -14777,8 +15290,17 @@
       <c r="AB7" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AC7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -14830,7 +15352,7 @@
       <c r="R8" t="s">
         <v>30</v>
       </c>
-      <c r="T8" t="s">
+      <c r="S8" t="s">
         <v>30</v>
       </c>
       <c r="U8" t="s">
@@ -14857,8 +15379,17 @@
       <c r="AB8" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AC8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -14910,7 +15441,7 @@
       <c r="R9" t="s">
         <v>70</v>
       </c>
-      <c r="T9" t="s">
+      <c r="S9" t="s">
         <v>70</v>
       </c>
       <c r="U9" t="s">
@@ -14937,8 +15468,17 @@
       <c r="AB9" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="AC9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -14990,7 +15530,7 @@
       <c r="R10" t="s">
         <v>30</v>
       </c>
-      <c r="T10" t="s">
+      <c r="S10" t="s">
         <v>30</v>
       </c>
       <c r="U10" t="s">
@@ -15015,6 +15555,15 @@
         <v>30</v>
       </c>
       <c r="AB10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE10" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
FHIR-38702 complete medicationdispense update change-log intro
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{804ED81B-1314-054D-B746-F6FAA5EDA11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCEFB36F-C963-2A45-BB25-4E4286329C21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="140" yWindow="500" windowWidth="36720" windowHeight="28080" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2711" uniqueCount="708">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2701" uniqueCount="711">
   <si>
     <t>Element</t>
   </si>
@@ -2364,9 +2364,6 @@
     <t>conf_MedicationDispense</t>
   </si>
   <si>
-    <t>support searching for prescriptions for a patient based on there dispensed status and dispense type.</t>
-  </si>
-  <si>
     <t>foo</t>
   </si>
   <si>
@@ -2382,7 +2379,19 @@
     <t>whenHandedOver</t>
   </si>
   <si>
-    <t>support searching for prescriptions for a patient based on there dispensed status</t>
+    <t>GET [base]/MedicationDispense?patient=14676~GET [base]/MedicationStatement?patient=14676&amp;_include=MedicationDispense:medication</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationDispense?patient=1137192&amp;status=completed~GET [base]/MedicationDispense?patient=1137192&amp;status=completed&amp;_include=MedicationDispense:medication</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on their dispensed status</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on their dispensed status and dispense type.</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationDispense?patient=1137192&amp;status=&amp;type=~GET [base]/MedicationDispense?patient=1137192&amp;status=&amp;type=FFP&amp;_include=MedicationDispense:medication</t>
   </si>
 </sst>
 </file>
@@ -3001,11 +3010,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AB122"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C84" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="N28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B121" sqref="B121"/>
+      <selection pane="bottomRight" activeCell="W64" sqref="W64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3018,7 +3027,7 @@
     <col min="7" max="7" width="60" customWidth="1"/>
     <col min="10" max="10" width="14.33203125" customWidth="1"/>
     <col min="12" max="12" width="31.1640625" customWidth="1"/>
-    <col min="13" max="24" width="13.33203125" hidden="1" customWidth="1"/>
+    <col min="13" max="24" width="13.33203125" customWidth="1"/>
     <col min="25" max="25" width="85.33203125" customWidth="1"/>
     <col min="26" max="26" width="90.6640625" customWidth="1"/>
     <col min="27" max="27" width="83.5" style="1" bestFit="1" customWidth="1"/>
@@ -6315,7 +6324,9 @@
         <v>56</v>
       </c>
       <c r="W63" s="6"/>
-      <c r="X63" s="6"/>
+      <c r="X63" s="6" t="s">
+        <v>208</v>
+      </c>
       <c r="Z63" s="10"/>
       <c r="AA63" s="10"/>
       <c r="AB63" t="str">
@@ -6531,8 +6542,8 @@
         <v>336</v>
       </c>
       <c r="AA67" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B67&amp; " resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
-        <v>Fetches a bundle of all !MedicationStatement resources for the specified patient. Mandatory for client to support the _include parameter. Optional for server to support the _include parameter.</v>
+        <f>"Fetches a bundle of all "&amp;B67&amp; " resources for the specified patient.W63+X63 Mandatory for client to support the _include parameter. Optional for server to support the _include parameter."</f>
+        <v>Fetches a bundle of all !MedicationStatement resources for the specified patient.W63+X63 Mandatory for client to support the _include parameter. Optional for server to support the _include parameter.</v>
       </c>
       <c r="AB67" t="str">
         <f t="shared" ref="AB67:AB68" si="36">"SearchParameter-us-core-"&amp;LOWER((B67)&amp;"-"&amp;C67&amp;".html")</f>
@@ -9435,7 +9446,7 @@
         <v>SearchParameter-us-core-medicationdispense-type.html</v>
       </c>
     </row>
-    <row r="121" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>89</v>
       </c>
@@ -9480,10 +9491,16 @@
       <c r="O121" t="s">
         <v>56</v>
       </c>
-      <c r="W121" s="6"/>
-      <c r="X121" s="6"/>
-      <c r="Z121" s="10"/>
-      <c r="AA121" s="10"/>
+      <c r="X121" s="6" t="s">
+        <v>698</v>
+      </c>
+      <c r="Z121" s="10" t="s">
+        <v>706</v>
+      </c>
+      <c r="AA121" s="10" t="str">
+        <f>"Fetches a bundle of all "&amp;B121&amp; " resources for the specified patient."</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient.</v>
+      </c>
       <c r="AB121" t="str">
         <f t="shared" si="60"/>
         <v>SearchParameter-us-core-medicationdispense-patient.html</v>
@@ -9494,10 +9511,10 @@
         <v>61</v>
       </c>
       <c r="B122" t="s">
+        <v>704</v>
+      </c>
+      <c r="C122" t="s">
         <v>705</v>
-      </c>
-      <c r="C122" t="s">
-        <v>706</v>
       </c>
       <c r="D122" t="s">
         <v>30</v>
@@ -9561,11 +9578,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:K105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C86" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C75" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C110" sqref="C110"/>
+      <selection pane="bottomRight" activeCell="A103" sqref="A103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12305,8 +12322,9 @@
       <c r="B92" t="s">
         <v>579</v>
       </c>
-      <c r="C92" t="s">
-        <v>589</v>
+      <c r="C92" t="str">
+        <f t="shared" ref="C92:C105" si="10">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B92)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D92" t="s">
         <v>116</v>
@@ -12335,8 +12353,9 @@
       <c r="B93" t="s">
         <v>579</v>
       </c>
-      <c r="C93" t="s">
-        <v>589</v>
+      <c r="C93" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D93" t="s">
         <v>145</v>
@@ -12365,8 +12384,9 @@
       <c r="B94" t="s">
         <v>579</v>
       </c>
-      <c r="C94" t="s">
-        <v>589</v>
+      <c r="C94" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D94" t="s">
         <v>147</v>
@@ -12395,8 +12415,9 @@
       <c r="B95" t="s">
         <v>579</v>
       </c>
-      <c r="C95" t="s">
-        <v>589</v>
+      <c r="C95" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D95" t="s">
         <v>587</v>
@@ -12425,8 +12446,9 @@
       <c r="B96" t="s">
         <v>579</v>
       </c>
-      <c r="C96" t="s">
-        <v>589</v>
+      <c r="C96" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D96" t="s">
         <v>588</v>
@@ -12456,7 +12478,7 @@
         <v>180</v>
       </c>
       <c r="C97" t="str">
-        <f t="shared" ref="C97" si="10">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B97)</f>
+        <f t="shared" si="10"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D97" t="s">
@@ -12486,8 +12508,9 @@
       <c r="B98" t="s">
         <v>630</v>
       </c>
-      <c r="C98" s="19" t="s">
-        <v>628</v>
+      <c r="C98" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D98" t="s">
         <v>116</v>
@@ -12516,8 +12539,9 @@
       <c r="B99" t="s">
         <v>630</v>
       </c>
-      <c r="C99" s="19" t="s">
-        <v>628</v>
+      <c r="C99" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D99" t="s">
         <v>650</v>
@@ -12549,8 +12573,9 @@
       <c r="B100" t="s">
         <v>630</v>
       </c>
-      <c r="C100" s="19" t="s">
-        <v>628</v>
+      <c r="C100" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D100" t="s">
         <v>651</v>
@@ -12579,8 +12604,9 @@
       <c r="B101" t="s">
         <v>630</v>
       </c>
-      <c r="C101" s="19" t="s">
-        <v>628</v>
+      <c r="C101" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D101" s="18" t="s">
         <v>652</v>
@@ -12612,8 +12638,9 @@
       <c r="B102" t="s">
         <v>630</v>
       </c>
-      <c r="C102" s="19" t="s">
-        <v>628</v>
+      <c r="C102" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D102" s="18" t="s">
         <v>653</v>
@@ -12635,15 +12662,16 @@
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>129</v>
       </c>
       <c r="B103" s="18" t="s">
         <v>697</v>
       </c>
-      <c r="C103" s="18" t="s">
-        <v>346</v>
+      <c r="C103" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D103" s="18" t="s">
         <v>116</v>
@@ -12659,10 +12687,10 @@
       </c>
       <c r="H103" s="18"/>
       <c r="I103" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="J103" s="4" t="s">
         <v>707</v>
-      </c>
-      <c r="J103" s="4" t="s">
-        <v>702</v>
       </c>
       <c r="K103" t="str">
         <f>"Fetches a bundle of all "&amp;B103&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12676,8 +12704,9 @@
       <c r="B104" s="18" t="s">
         <v>697</v>
       </c>
-      <c r="C104" s="18" t="s">
-        <v>346</v>
+      <c r="C104" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D104" s="18" t="s">
         <v>117</v>
@@ -12693,10 +12722,10 @@
       </c>
       <c r="H104" s="18"/>
       <c r="I104" s="4" t="s">
-        <v>701</v>
+        <v>709</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>702</v>
+        <v>710</v>
       </c>
       <c r="K104" t="str">
         <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12708,13 +12737,14 @@
         <v>130</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>705</v>
-      </c>
-      <c r="C105" s="18" t="s">
-        <v>346</v>
+        <v>704</v>
+      </c>
+      <c r="C105" t="str">
+        <f t="shared" si="10"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E105" s="18" t="s">
         <v>56</v>
@@ -12727,10 +12757,10 @@
       </c>
       <c r="H105" s="18"/>
       <c r="I105" s="4" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="J105" s="4" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="K105" t="str">
         <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient for a given dispense and date or range"</f>

</xml_diff>

<commit_message>
FHIR- 34724 : update to lab and procedures
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CE0D29-3559-B744-B993-55FE499DCF9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A621A5-FB13-FE46-873F-F15B03A4B5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43740" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$97</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$119</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$120</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2729" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2739" uniqueCount="719">
   <si>
     <t>Element</t>
   </si>
@@ -2394,18 +2394,9 @@
     <t>GET [base]/MedicationDispense?patient=1137192&amp;status=&amp;type=~GET [base]/MedicationDispense?patient=1137192&amp;status=&amp;type=FFP&amp;_include=MedicationDispense:medication</t>
   </si>
   <si>
-    <t>deceased</t>
-  </si>
-  <si>
-    <t>deceased,family</t>
-  </si>
-  <si>
     <t>support searching for a patient by date of death and family name</t>
   </si>
   <si>
-    <t>GET [base]/Patient?family=Shaw&amp;deceased=2022-07-22</t>
-  </si>
-  <si>
     <t>tribal-affiliation</t>
   </si>
   <si>
@@ -2416,6 +2407,15 @@
   </si>
   <si>
     <t>GET [base]/Patient?tribal-affiliiation=Shaw</t>
+  </si>
+  <si>
+    <t>death-date</t>
+  </si>
+  <si>
+    <t>death-date,family</t>
+  </si>
+  <si>
+    <t>GET [base]/Patient?family=Shaw&amp;death-date=2022-07-22</t>
   </si>
 </sst>
 </file>
@@ -3031,13 +3031,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AB124"/>
+  <dimension ref="A1:AB125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="P80" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="T84" sqref="T84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4344,7 +4344,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>711</v>
+        <v>716</v>
       </c>
       <c r="D25" t="s">
         <v>30</v>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="L25" t="str">
         <f t="shared" ref="L25" si="15">B25&amp;"."&amp;C25</f>
-        <v>Patient.deceased</v>
+        <v>Patient.death-date</v>
       </c>
       <c r="M25" t="s">
         <v>56</v>
@@ -4383,7 +4383,7 @@
       </c>
       <c r="AB25" t="str">
         <f t="shared" ref="AB25" si="16">"SearchParameter-us-core-"&amp;LOWER((B25)&amp;"-"&amp;C25&amp;".html")</f>
-        <v>SearchParameter-us-core-patient-deceased.html</v>
+        <v>SearchParameter-us-core-patient-death-date.html</v>
       </c>
     </row>
     <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -4643,7 +4643,7 @@
         <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -4668,7 +4668,7 @@
         <v>57</v>
       </c>
       <c r="L31" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="M31" t="s">
         <v>56</v>
@@ -4677,10 +4677,10 @@
         <v>56</v>
       </c>
       <c r="Y31" s="4" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="Z31" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="AA31" s="10" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -8741,7 +8741,7 @@
         <v>505</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" ref="G107:G124" si="61">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B107)</f>
+        <f t="shared" ref="G107:G125" si="61">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B107)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H107" t="s">
@@ -9072,7 +9072,7 @@
         <v>support searching for all relatedpersons for a patient</v>
       </c>
       <c r="Z113" s="4" t="str">
-        <f>"GET [base]/"&amp;B113&amp;"?patient=1032702"</f>
+        <f>"GET [base]/"&amp;B113&amp;"?"&amp;C113&amp;"=1032702"</f>
         <v>GET [base]/RelatedPerson?patient=1032702</v>
       </c>
       <c r="AA113" s="10" t="str">
@@ -9086,36 +9086,39 @@
     </row>
     <row r="114" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="B114" t="s">
-        <v>630</v>
+        <v>602</v>
       </c>
       <c r="C114" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="D114" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="E114" t="b">
         <v>1</v>
       </c>
       <c r="G114" t="str">
         <f t="shared" si="61"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
       </c>
       <c r="H114" t="s">
         <v>56</v>
       </c>
+      <c r="I114" t="s">
+        <v>56</v>
+      </c>
       <c r="J114" t="s">
         <v>56</v>
       </c>
       <c r="K114" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="L114" t="str">
-        <f t="shared" ref="L114:L124" si="63">B114&amp;"."&amp;C114</f>
-        <v>QuestionnaireResponse._id</v>
+        <f>B114&amp;"."&amp;C114</f>
+        <v>RelatedPerson.name</v>
       </c>
       <c r="M114" t="s">
         <v>56</v>
@@ -9123,36 +9126,37 @@
       <c r="O114" t="s">
         <v>56</v>
       </c>
-      <c r="Y114" s="4" t="str">
-        <f>"support fetching a "&amp;B114</f>
-        <v>support fetching a QuestionnaireResponse</v>
-      </c>
-      <c r="Z114" s="4" t="s">
-        <v>648</v>
+      <c r="Y114" s="4" t="s">
+        <v>470</v>
+      </c>
+      <c r="Z114" s="4" t="str">
+        <f>"GET [base]/"&amp;B114&amp;"?"&amp;C114&amp;"=Mary Shaw"</f>
+        <v>GET [base]/RelatedPerson?name=Mary Shaw</v>
+      </c>
+      <c r="AA114" s="10" t="str">
+        <f>"Fetches a bundle of all "&amp;B114&amp;" resources matching the name"</f>
+        <v>Fetches a bundle of all RelatedPerson resources matching the name</v>
       </c>
       <c r="AB114" t="str">
-        <f t="shared" ref="AB114:AB120" si="64">"SearchParameter-us-core-"&amp;LOWER((B114)&amp;"-"&amp;SUBSTITUTE(C114,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-questionnaireresponse-id.html</v>
+        <f t="shared" ref="AB114" si="63">"SearchParameter-us-core-"&amp;LOWER((B114)&amp;"-"&amp;SUBSTITUTE(C114,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-relatedperson-name.html</v>
       </c>
     </row>
     <row r="115" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B115" t="s">
         <v>630</v>
       </c>
       <c r="C115" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="D115" t="s">
         <v>12</v>
       </c>
       <c r="E115" t="b">
         <v>1</v>
-      </c>
-      <c r="F115" s="1" t="s">
-        <v>502</v>
       </c>
       <c r="G115" t="str">
         <f t="shared" si="61"/>
@@ -9165,11 +9169,11 @@
         <v>56</v>
       </c>
       <c r="K115" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="L115" t="str">
-        <f t="shared" si="63"/>
-        <v>QuestionnaireResponse.patient</v>
+        <f t="shared" ref="L115:L125" si="64">B115&amp;"."&amp;C115</f>
+        <v>QuestionnaireResponse._id</v>
       </c>
       <c r="M115" t="s">
         <v>56</v>
@@ -9177,41 +9181,36 @@
       <c r="O115" t="s">
         <v>56</v>
       </c>
-      <c r="Y115" t="str">
-        <f>"support searching for all "&amp;LOWER(B115)&amp;"s for a patient"</f>
-        <v>support searching for all questionnaireresponses for a patient</v>
-      </c>
-      <c r="Z115" s="4" t="str">
-        <f>"GET [base]/"&amp;B115&amp;"?patient=1032702"</f>
-        <v>GET [base]/QuestionnaireResponse?patient=1032702</v>
-      </c>
-      <c r="AA115" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B115&amp; " resources for the specified patient"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient</v>
+      <c r="Y115" s="4" t="str">
+        <f>"support fetching a "&amp;B115</f>
+        <v>support fetching a QuestionnaireResponse</v>
+      </c>
+      <c r="Z115" s="4" t="s">
+        <v>648</v>
       </c>
       <c r="AB115" t="str">
-        <f t="shared" si="64"/>
-        <v>SearchParameter-us-core-questionnaireresponse-patient.html</v>
+        <f t="shared" ref="AB115:AB121" si="65">"SearchParameter-us-core-"&amp;LOWER((B115)&amp;"-"&amp;SUBSTITUTE(C115,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-questionnaireresponse-id.html</v>
       </c>
     </row>
     <row r="116" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B116" t="s">
         <v>630</v>
       </c>
       <c r="C116" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="D116" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E116" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="G116" t="str">
         <f t="shared" si="61"/>
@@ -9224,38 +9223,44 @@
         <v>56</v>
       </c>
       <c r="K116" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="L116" t="str">
-        <f t="shared" si="63"/>
-        <v>QuestionnaireResponse.status</v>
+        <f t="shared" si="64"/>
+        <v>QuestionnaireResponse.patient</v>
       </c>
       <c r="M116" t="s">
         <v>56</v>
       </c>
-      <c r="N116" t="s">
-        <v>12</v>
-      </c>
       <c r="O116" t="s">
         <v>56</v>
       </c>
-      <c r="Y116" s="20" t="s">
-        <v>645</v>
+      <c r="Y116" t="str">
+        <f>"support searching for all "&amp;LOWER(B116)&amp;"s for a patient"</f>
+        <v>support searching for all questionnaireresponses for a patient</v>
+      </c>
+      <c r="Z116" s="4" t="str">
+        <f>"GET [base]/"&amp;B116&amp;"?patient=1032702"</f>
+        <v>GET [base]/QuestionnaireResponse?patient=1032702</v>
+      </c>
+      <c r="AA116" s="10" t="str">
+        <f>"Fetches a bundle of all "&amp;B116&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient</v>
       </c>
       <c r="AB116" t="str">
-        <f t="shared" si="64"/>
-        <v>SearchParameter-us-core-questionnaireresponse-status.html</v>
+        <f t="shared" si="65"/>
+        <v>SearchParameter-us-core-questionnaireresponse-patient.html</v>
       </c>
     </row>
     <row r="117" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B117" t="s">
         <v>630</v>
       </c>
       <c r="C117" t="s">
-        <v>641</v>
+        <v>62</v>
       </c>
       <c r="D117" t="s">
         <v>30</v>
@@ -9279,32 +9284,36 @@
       <c r="K117" t="s">
         <v>57</v>
       </c>
-      <c r="L117" t="s">
-        <v>643</v>
+      <c r="L117" t="str">
+        <f t="shared" si="64"/>
+        <v>QuestionnaireResponse.status</v>
       </c>
       <c r="M117" t="s">
         <v>56</v>
       </c>
+      <c r="N117" t="s">
+        <v>12</v>
+      </c>
       <c r="O117" t="s">
         <v>56</v>
       </c>
       <c r="Y117" s="20" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="AB117" t="str">
-        <f t="shared" si="64"/>
-        <v>SearchParameter-us-core-questionnaireresponse-tag.html</v>
+        <f t="shared" si="65"/>
+        <v>SearchParameter-us-core-questionnaireresponse-status.html</v>
       </c>
     </row>
     <row r="118" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
         <v>630</v>
       </c>
       <c r="C118" t="s">
-        <v>586</v>
+        <v>641</v>
       </c>
       <c r="D118" t="s">
         <v>30</v>
@@ -9313,7 +9322,7 @@
         <v>0</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="G118" t="str">
         <f t="shared" si="61"/>
@@ -9326,11 +9335,10 @@
         <v>56</v>
       </c>
       <c r="K118" t="s">
-        <v>79</v>
-      </c>
-      <c r="L118" t="str">
-        <f t="shared" si="63"/>
-        <v>QuestionnaireResponse.authored</v>
+        <v>57</v>
+      </c>
+      <c r="L118" t="s">
+        <v>643</v>
       </c>
       <c r="M118" t="s">
         <v>56</v>
@@ -9338,29 +9346,23 @@
       <c r="O118" t="s">
         <v>56</v>
       </c>
-      <c r="P118" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="S118" t="s">
-        <v>93</v>
-      </c>
       <c r="Y118" s="20" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="AB118" t="str">
-        <f t="shared" si="64"/>
-        <v>SearchParameter-us-core-questionnaireresponse-authored.html</v>
+        <f t="shared" si="65"/>
+        <v>SearchParameter-us-core-questionnaireresponse-tag.html</v>
       </c>
     </row>
     <row r="119" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B119" t="s">
         <v>630</v>
       </c>
       <c r="C119" t="s">
-        <v>642</v>
+        <v>586</v>
       </c>
       <c r="D119" t="s">
         <v>30</v>
@@ -9369,7 +9371,7 @@
         <v>0</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="G119" t="str">
         <f t="shared" si="61"/>
@@ -9382,11 +9384,11 @@
         <v>56</v>
       </c>
       <c r="K119" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="L119" t="str">
-        <f t="shared" si="63"/>
-        <v>QuestionnaireResponse.questionnaire</v>
+        <f t="shared" si="64"/>
+        <v>QuestionnaireResponse.authored</v>
       </c>
       <c r="M119" t="s">
         <v>56</v>
@@ -9394,41 +9396,44 @@
       <c r="O119" t="s">
         <v>56</v>
       </c>
+      <c r="P119" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="S119" t="s">
+        <v>93</v>
+      </c>
       <c r="Y119" s="20" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="AB119" t="str">
-        <f t="shared" si="64"/>
-        <v>SearchParameter-us-core-questionnaireresponse-questionnaire.html</v>
+        <f t="shared" si="65"/>
+        <v>SearchParameter-us-core-questionnaireresponse-authored.html</v>
       </c>
     </row>
     <row r="120" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B120" t="s">
-        <v>681</v>
+        <v>630</v>
       </c>
       <c r="C120" t="s">
-        <v>90</v>
+        <v>642</v>
       </c>
       <c r="D120" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E120" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F120" s="1" t="s">
         <v>502</v>
       </c>
       <c r="G120" t="str">
         <f t="shared" si="61"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-coverage</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H120" t="s">
-        <v>56</v>
-      </c>
-      <c r="I120" t="s">
         <v>56</v>
       </c>
       <c r="J120" t="s">
@@ -9438,8 +9443,8 @@
         <v>91</v>
       </c>
       <c r="L120" t="str">
-        <f t="shared" si="63"/>
-        <v>Coverage.patient</v>
+        <f t="shared" si="64"/>
+        <v>QuestionnaireResponse.questionnaire</v>
       </c>
       <c r="M120" t="s">
         <v>56</v>
@@ -9447,44 +9452,36 @@
       <c r="O120" t="s">
         <v>56</v>
       </c>
-      <c r="Y120" t="s">
-        <v>683</v>
-      </c>
-      <c r="Z120" s="4" t="str">
-        <f>"GET [base]/"&amp;B120&amp;"?patient=1137192"</f>
-        <v>GET [base]/Coverage?patient=1137192</v>
-      </c>
-      <c r="AA120" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B120&amp; " resources for the specified patient"</f>
-        <v>Fetches a bundle of all Coverage resources for the specified patient</v>
+      <c r="Y120" s="20" t="s">
+        <v>647</v>
       </c>
       <c r="AB120" t="str">
-        <f t="shared" si="64"/>
-        <v>SearchParameter-us-core-coverage-patient.html</v>
+        <f t="shared" si="65"/>
+        <v>SearchParameter-us-core-questionnaireresponse-questionnaire.html</v>
       </c>
     </row>
     <row r="121" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B121" t="s">
-        <v>697</v>
+        <v>681</v>
       </c>
       <c r="C121" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="D121" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E121" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="G121" t="str">
         <f t="shared" si="61"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-coverage</v>
       </c>
       <c r="H121" t="s">
         <v>56</v>
@@ -9496,38 +9493,43 @@
         <v>56</v>
       </c>
       <c r="K121" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="L121" t="str">
-        <f t="shared" si="63"/>
-        <v>MedicationDispense.status</v>
+        <f t="shared" si="64"/>
+        <v>Coverage.patient</v>
       </c>
       <c r="M121" t="s">
         <v>56</v>
       </c>
-      <c r="N121" t="s">
-        <v>12</v>
-      </c>
       <c r="O121" t="s">
         <v>56</v>
       </c>
-      <c r="Y121" s="4"/>
-      <c r="Z121" s="4"/>
-      <c r="AA121" s="10"/>
+      <c r="Y121" t="s">
+        <v>683</v>
+      </c>
+      <c r="Z121" s="4" t="str">
+        <f>"GET [base]/"&amp;B121&amp;"?patient=1137192"</f>
+        <v>GET [base]/Coverage?patient=1137192</v>
+      </c>
+      <c r="AA121" s="10" t="str">
+        <f>"Fetches a bundle of all "&amp;B121&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all Coverage resources for the specified patient</v>
+      </c>
       <c r="AB121" t="str">
-        <f t="shared" ref="AB121:AB124" si="65">"SearchParameter-us-core-"&amp;LOWER((B121)&amp;"-"&amp;C121&amp;".html")</f>
-        <v>SearchParameter-us-core-medicationdispense-status.html</v>
+        <f t="shared" si="65"/>
+        <v>SearchParameter-us-core-coverage-patient.html</v>
       </c>
     </row>
     <row r="122" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B122" t="s">
         <v>697</v>
       </c>
       <c r="C122" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="D122" t="s">
         <v>30</v>
@@ -9555,8 +9557,8 @@
         <v>57</v>
       </c>
       <c r="L122" t="str">
-        <f t="shared" si="63"/>
-        <v>MedicationDispense.type</v>
+        <f t="shared" si="64"/>
+        <v>MedicationDispense.status</v>
       </c>
       <c r="M122" t="s">
         <v>56</v>
@@ -9571,28 +9573,28 @@
       <c r="Z122" s="4"/>
       <c r="AA122" s="10"/>
       <c r="AB122" t="str">
-        <f t="shared" si="65"/>
-        <v>SearchParameter-us-core-medicationdispense-type.html</v>
-      </c>
-    </row>
-    <row r="123" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" ref="AB122:AB125" si="66">"SearchParameter-us-core-"&amp;LOWER((B122)&amp;"-"&amp;C122&amp;".html")</f>
+        <v>SearchParameter-us-core-medicationdispense-status.html</v>
+      </c>
+    </row>
+    <row r="123" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B123" t="s">
         <v>697</v>
       </c>
       <c r="C123" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="D123" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E123" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="G123" t="str">
         <f t="shared" si="61"/>
@@ -9608,92 +9610,148 @@
         <v>56</v>
       </c>
       <c r="K123" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="L123" t="str">
-        <f t="shared" si="63"/>
-        <v>MedicationDispense.patient</v>
+        <f t="shared" si="64"/>
+        <v>MedicationDispense.type</v>
       </c>
       <c r="M123" t="s">
         <v>56</v>
       </c>
+      <c r="N123" t="s">
+        <v>12</v>
+      </c>
       <c r="O123" t="s">
         <v>56</v>
       </c>
-      <c r="X123" s="6" t="s">
-        <v>698</v>
-      </c>
-      <c r="Z123" s="10" t="s">
-        <v>706</v>
-      </c>
-      <c r="AA123" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B123&amp; " resources for the specified patient."</f>
-        <v>Fetches a bundle of all MedicationDispense resources for the specified patient.</v>
-      </c>
+      <c r="Y123" s="4"/>
+      <c r="Z123" s="4"/>
+      <c r="AA123" s="10"/>
       <c r="AB123" t="str">
-        <f t="shared" si="65"/>
-        <v>SearchParameter-us-core-medicationdispense-patient.html</v>
-      </c>
-    </row>
-    <row r="124" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="66"/>
+        <v>SearchParameter-us-core-medicationdispense-type.html</v>
+      </c>
+    </row>
+    <row r="124" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124">
-        <v>61</v>
+        <v>89</v>
       </c>
       <c r="B124" t="s">
-        <v>704</v>
+        <v>697</v>
       </c>
       <c r="C124" t="s">
-        <v>705</v>
+        <v>90</v>
       </c>
       <c r="D124" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E124" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G124" t="str">
         <f t="shared" si="61"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+      </c>
+      <c r="H124" t="s">
+        <v>56</v>
+      </c>
+      <c r="I124" t="s">
+        <v>56</v>
+      </c>
+      <c r="J124" t="s">
+        <v>56</v>
+      </c>
+      <c r="K124" t="s">
+        <v>91</v>
+      </c>
+      <c r="L124" t="str">
+        <f t="shared" si="64"/>
+        <v>MedicationDispense.patient</v>
+      </c>
+      <c r="M124" t="s">
+        <v>56</v>
+      </c>
+      <c r="O124" t="s">
+        <v>56</v>
+      </c>
+      <c r="X124" s="6" t="s">
+        <v>698</v>
+      </c>
+      <c r="Z124" s="10" t="s">
+        <v>706</v>
+      </c>
+      <c r="AA124" s="10" t="str">
+        <f>"Fetches a bundle of all "&amp;B124&amp; " resources for the specified patient."</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient.</v>
+      </c>
+      <c r="AB124" t="str">
+        <f t="shared" si="66"/>
+        <v>SearchParameter-us-core-medicationdispense-patient.html</v>
+      </c>
+    </row>
+    <row r="125" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>61</v>
+      </c>
+      <c r="B125" t="s">
+        <v>704</v>
+      </c>
+      <c r="C125" t="s">
+        <v>705</v>
+      </c>
+      <c r="D125" t="s">
+        <v>30</v>
+      </c>
+      <c r="E125" t="b">
+        <v>0</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="G125" t="str">
+        <f t="shared" si="61"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
-      <c r="H124" t="s">
-        <v>56</v>
-      </c>
-      <c r="I124" t="s">
-        <v>56</v>
-      </c>
-      <c r="J124" t="s">
-        <v>56</v>
-      </c>
-      <c r="K124" t="s">
+      <c r="H125" t="s">
+        <v>56</v>
+      </c>
+      <c r="I125" t="s">
+        <v>56</v>
+      </c>
+      <c r="J125" t="s">
+        <v>56</v>
+      </c>
+      <c r="K125" t="s">
         <v>79</v>
       </c>
-      <c r="L124" t="str">
-        <f t="shared" si="63"/>
+      <c r="L125" t="str">
+        <f t="shared" si="64"/>
         <v>!MedicationDispense.whenHandedOver</v>
       </c>
-      <c r="M124" t="s">
-        <v>56</v>
-      </c>
-      <c r="O124" t="s">
-        <v>56</v>
-      </c>
-      <c r="P124" t="s">
-        <v>70</v>
-      </c>
-      <c r="S124" t="s">
+      <c r="M125" t="s">
+        <v>56</v>
+      </c>
+      <c r="O125" t="s">
+        <v>56</v>
+      </c>
+      <c r="P125" t="s">
+        <v>70</v>
+      </c>
+      <c r="S125" t="s">
         <v>93</v>
       </c>
-      <c r="AA124" s="10"/>
-      <c r="AB124" t="str">
-        <f t="shared" si="65"/>
+      <c r="AA125" s="10"/>
+      <c r="AB125" t="str">
+        <f t="shared" si="66"/>
         <v>SearchParameter-us-core-!medicationdispense-whenhandedover.html</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB119" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
+  <autoFilter ref="A1:AB120" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA38">
     <sortCondition ref="B1"/>
   </sortState>
@@ -9711,7 +9769,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
+      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10582,7 +10640,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>712</v>
+        <v>717</v>
       </c>
       <c r="F32" t="s">
         <v>70</v>
@@ -10591,14 +10649,14 @@
         <v>134</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>714</v>
+        <v>718</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" ref="K32" si="7">"Fetches a bundle of all "&amp;B32&amp;" resources matching the specified "&amp;SUBSTITUTE(D32,","," and ")</f>
-        <v>Fetches a bundle of all Patient resources matching the specified deceased and family</v>
+        <v>Fetches a bundle of all Patient resources matching the specified death-date and family</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update package-list to publication-request/embed fragments in ig template
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A621A5-FB13-FE46-873F-F15B03A4B5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D27633D-F214-7744-BDA1-02F318F3B322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="43740" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="17060" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1533,9 +1533,6 @@
     <t>publishervalue</t>
   </si>
   <si>
-    <t>support searching for a patient by a server defined search that matches any of the string fields in the HumanName, including family, give, prefix, suffix, suffix, and/or text</t>
-  </si>
-  <si>
     <t>profile_conf</t>
   </si>
   <si>
@@ -1812,9 +1809,6 @@
   </si>
   <si>
     <t>GET [base]Condition?patient=555580&amp;abatement-date=ge2018-01-14</t>
-  </si>
-  <si>
-    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis?encounter=1036</t>
   </si>
   <si>
     <t>Fetches a bundle of all Condition resources for the specified patient and category and encounter. When category = "encounter-diagnosis" will return the encounter diagnosis for the encounter.</t>
@@ -2416,6 +2410,12 @@
   </si>
   <si>
     <t>GET [base]/Patient?family=Shaw&amp;death-date=2022-07-22</t>
+  </si>
+  <si>
+    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis&amp;encounter=1036</t>
+  </si>
+  <si>
+    <t>support searching for a patient by a server defined search that matches any of the string fields in the HumanName, including family, given, prefix, suffix, suffix, and/or text</t>
   </si>
 </sst>
 </file>
@@ -2965,7 +2965,7 @@
         <v>466</v>
       </c>
       <c r="B2" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2973,7 +2973,7 @@
         <v>467</v>
       </c>
       <c r="B3" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -2997,7 +2997,7 @@
         <v>68</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3013,12 +3013,12 @@
         <v>469</v>
       </c>
       <c r="B8" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -3034,10 +3034,10 @@
   <dimension ref="A1:AB125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="P80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="N92" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T84" sqref="T84"/>
+      <selection pane="bottomRight" activeCell="W113" sqref="W113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3083,7 +3083,7 @@
         <v>41</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>32</v>
@@ -3305,7 +3305,7 @@
         <v>0</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G5" t="str">
         <f t="shared" si="1"/>
@@ -3513,7 +3513,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G9" t="str">
         <f t="shared" si="1"/>
@@ -3562,7 +3562,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G10" t="str">
         <f t="shared" si="1"/>
@@ -3620,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G11" t="str">
         <f t="shared" si="1"/>
@@ -3670,7 +3670,7 @@
         <v>0</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G12" t="str">
         <f t="shared" si="1"/>
@@ -3718,7 +3718,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G13" t="str">
         <f t="shared" si="1"/>
@@ -3829,7 +3829,7 @@
         <v>0</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G15" t="str">
         <f t="shared" si="1"/>
@@ -3879,7 +3879,7 @@
         <v>0</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G16" t="str">
         <f t="shared" si="1"/>
@@ -3933,7 +3933,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G17" t="str">
         <f t="shared" si="1"/>
@@ -3990,7 +3990,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G18" t="str">
         <f t="shared" si="1"/>
@@ -4039,7 +4039,7 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="D19" t="s">
         <v>30</v>
@@ -4048,7 +4048,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G19" t="str">
         <f t="shared" ref="G19" si="8">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B19)</f>
@@ -4106,7 +4106,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G20" t="str">
         <f t="shared" si="1"/>
@@ -4156,7 +4156,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G21" t="str">
         <f t="shared" ref="G21" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
@@ -4197,7 +4197,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="D22" t="s">
         <v>30</v>
@@ -4206,7 +4206,7 @@
         <v>0</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G22" t="str">
         <f t="shared" si="1"/>
@@ -4306,7 +4306,7 @@
         <v>0</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G24" t="str">
         <f t="shared" si="1"/>
@@ -4344,7 +4344,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="D25" t="s">
         <v>30</v>
@@ -4353,7 +4353,7 @@
         <v>0</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G25" t="str">
         <f t="shared" ref="G25" si="14">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B25)</f>
@@ -4403,7 +4403,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
@@ -4449,7 +4449,7 @@
         <v>0</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G27" t="str">
         <f t="shared" si="1"/>
@@ -4541,7 +4541,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G29" t="str">
         <f t="shared" si="1"/>
@@ -4621,7 +4621,7 @@
         <v>56</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>470</v>
+        <v>718</v>
       </c>
       <c r="Z30" t="s">
         <v>173</v>
@@ -4643,7 +4643,7 @@
         <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -4668,19 +4668,19 @@
         <v>57</v>
       </c>
       <c r="L31" t="s">
+        <v>711</v>
+      </c>
+      <c r="M31" t="s">
+        <v>56</v>
+      </c>
+      <c r="O31" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y31" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="Z31" t="s">
         <v>713</v>
-      </c>
-      <c r="M31" t="s">
-        <v>56</v>
-      </c>
-      <c r="O31" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y31" s="4" t="s">
-        <v>714</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>715</v>
       </c>
       <c r="AA31" s="10" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -5030,7 +5030,7 @@
         <v>0</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G39" t="str">
         <f t="shared" si="1"/>
@@ -5075,7 +5075,7 @@
         <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D40" t="s">
         <v>30</v>
@@ -5084,7 +5084,7 @@
         <v>0</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G40" t="str">
         <f t="shared" ref="G40:G42" si="21">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B40)</f>
@@ -5129,7 +5129,7 @@
         <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="D41" t="s">
         <v>30</v>
@@ -5138,7 +5138,7 @@
         <v>0</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G41" t="str">
         <f t="shared" si="21"/>
@@ -5183,7 +5183,7 @@
         <v>138</v>
       </c>
       <c r="C42" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="D42" t="s">
         <v>30</v>
@@ -5192,7 +5192,7 @@
         <v>0</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G42" t="str">
         <f t="shared" si="21"/>
@@ -5246,7 +5246,7 @@
         <v>0</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G43" t="str">
         <f t="shared" si="1"/>
@@ -5296,7 +5296,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" ref="G44" si="24">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B44)</f>
@@ -5322,7 +5322,7 @@
         <v>56</v>
       </c>
       <c r="Y44" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="Z44" s="4" t="str">
         <f>"GET [base]/"&amp;B44&amp;"?patient=1137192"</f>
@@ -5354,7 +5354,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G45" t="str">
         <f t="shared" si="1"/>
@@ -5413,7 +5413,7 @@
         <v>0</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G46" t="str">
         <f t="shared" si="1"/>
@@ -5463,7 +5463,7 @@
         <v>0</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G47" t="str">
         <f t="shared" si="1"/>
@@ -5570,7 +5570,7 @@
         <v>0</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G49" t="str">
         <f t="shared" si="1"/>
@@ -5623,7 +5623,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G50" t="str">
         <f t="shared" si="1"/>
@@ -5682,7 +5682,7 @@
         <v>0</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G51" t="str">
         <f t="shared" si="1"/>
@@ -5732,7 +5732,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="1"/>
@@ -5782,7 +5782,7 @@
         <v>0</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G53" t="str">
         <f t="shared" si="1"/>
@@ -5836,7 +5836,7 @@
         <v>0</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G54" t="str">
         <f t="shared" si="1"/>
@@ -5889,7 +5889,7 @@
         <v>0</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G55" t="str">
         <f t="shared" si="1"/>
@@ -5942,7 +5942,7 @@
         <v>1</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G56" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B56)</f>
@@ -6001,7 +6001,7 @@
         <v>0</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G57" t="str">
         <f t="shared" si="1"/>
@@ -6051,7 +6051,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G58" t="str">
         <f t="shared" si="1"/>
@@ -6104,7 +6104,7 @@
         <v>0</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G59" t="str">
         <f t="shared" si="1"/>
@@ -6158,7 +6158,7 @@
         <v>0</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G60" t="str">
         <f t="shared" si="1"/>
@@ -6208,7 +6208,7 @@
         <v>1</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G61" t="str">
         <f t="shared" si="1"/>
@@ -6267,7 +6267,7 @@
         <v>0</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="G62" t="str">
         <f t="shared" si="1"/>
@@ -6321,7 +6321,7 @@
         <v>0</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G63" t="str">
         <f t="shared" si="1"/>
@@ -6374,7 +6374,7 @@
         <v>0</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G64" t="str">
         <f t="shared" si="1"/>
@@ -6427,7 +6427,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="1"/>
@@ -6480,7 +6480,7 @@
         <v>0</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G66" t="str">
         <f t="shared" si="1"/>
@@ -6531,7 +6531,7 @@
         <v>0</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G67" t="str">
         <f t="shared" si="1"/>
@@ -6585,7 +6585,7 @@
         <v>0</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G68" t="str">
         <f t="shared" si="1"/>
@@ -6638,7 +6638,7 @@
         <v>1</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G69" t="str">
         <f t="shared" si="1"/>
@@ -6696,7 +6696,7 @@
         <v>0</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G70" t="str">
         <f t="shared" si="1"/>
@@ -6750,7 +6750,7 @@
         <v>0</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G71" t="str">
         <f t="shared" si="1"/>
@@ -6803,7 +6803,7 @@
         <v>1</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G72" t="str">
         <f t="shared" si="1"/>
@@ -6861,7 +6861,7 @@
         <v>0</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G73" t="str">
         <f t="shared" si="1"/>
@@ -6915,7 +6915,7 @@
         <v>0</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G74" t="str">
         <f t="shared" si="1"/>
@@ -6968,7 +6968,7 @@
         <v>0</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G75" t="str">
         <f t="shared" ref="G75:G105" si="45">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B75)</f>
@@ -7021,7 +7021,7 @@
         <v>0</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G76" t="str">
         <f t="shared" si="45"/>
@@ -7071,7 +7071,7 @@
         <v>0</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G77" t="str">
         <f t="shared" si="45"/>
@@ -7124,7 +7124,7 @@
         <v>0</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G78" t="str">
         <f t="shared" si="45"/>
@@ -7178,7 +7178,7 @@
         <v>0</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G79" t="str">
         <f t="shared" si="45"/>
@@ -7237,7 +7237,7 @@
         <v>0</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G80" t="str">
         <f t="shared" si="45"/>
@@ -7287,7 +7287,7 @@
         <v>0</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G81" t="str">
         <f t="shared" si="45"/>
@@ -7337,7 +7337,7 @@
         <v>0</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G82" t="str">
         <f t="shared" si="45"/>
@@ -7391,7 +7391,7 @@
         <v>0</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G83" t="str">
         <f t="shared" si="45"/>
@@ -7450,7 +7450,7 @@
         <v>0</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G84" t="str">
         <f t="shared" si="45"/>
@@ -7503,7 +7503,7 @@
         <v>0</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G85" t="str">
         <f t="shared" si="45"/>
@@ -7529,7 +7529,7 @@
         <v>56</v>
       </c>
       <c r="X85" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="Y85" t="str">
         <f>"support searching for all "&amp;LOWER(B85)&amp;"s for a patient"</f>
@@ -7596,7 +7596,7 @@
         <v>GET [base]/Practitioner/practitioner-1~GET [base]/Practitioner?_id=practitioner-1</v>
       </c>
       <c r="AA86" s="10" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="AB86" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B86)&amp;"-"&amp;SUBSTITUTE(C86,"_","")&amp;".html")</f>
@@ -7620,7 +7620,7 @@
         <v>0</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G87" t="str">
         <f t="shared" ref="G87" si="52">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B87)</f>
@@ -7664,7 +7664,7 @@
         <v>248</v>
       </c>
       <c r="C88" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="D88" t="s">
         <v>70</v>
@@ -7673,7 +7673,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G88" t="str">
         <f t="shared" si="45"/>
@@ -7702,7 +7702,7 @@
         <v>56</v>
       </c>
       <c r="Y88" s="4" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="Z88" s="4" t="str">
         <f>"GET [base]/"&amp;B88&amp;"?"&amp;C88&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -7731,7 +7731,7 @@
         <v>1</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G89" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B89)</f>
@@ -7790,7 +7790,7 @@
         <v>0</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G90" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B90)</f>
@@ -8443,7 +8443,7 @@
         <v>1</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G102" t="str">
         <f t="shared" si="45"/>
@@ -8501,7 +8501,7 @@
         <v>1</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G103" t="str">
         <f t="shared" si="45"/>
@@ -8562,7 +8562,7 @@
         <v>1</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="45"/>
@@ -8614,7 +8614,7 @@
         <v>49</v>
       </c>
       <c r="B105" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C105" t="s">
         <v>62</v>
@@ -8626,7 +8626,7 @@
         <v>0</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="45"/>
@@ -8667,7 +8667,7 @@
         <v>50</v>
       </c>
       <c r="B106" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C106" t="s">
         <v>90</v>
@@ -8679,7 +8679,7 @@
         <v>1</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G106" t="str">
         <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B106)</f>
@@ -8726,7 +8726,7 @@
         <v>51</v>
       </c>
       <c r="B107" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C107" t="s">
         <v>140</v>
@@ -8738,7 +8738,7 @@
         <v>0</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G107" t="str">
         <f t="shared" ref="G107:G125" si="61">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B107)</f>
@@ -8776,7 +8776,7 @@
         <v>52</v>
       </c>
       <c r="B108" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C108" t="s">
         <v>26</v>
@@ -8788,7 +8788,7 @@
         <v>0</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G108" t="str">
         <f t="shared" si="61"/>
@@ -8829,10 +8829,10 @@
         <v>53</v>
       </c>
       <c r="B109" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C109" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D109" t="s">
         <v>30</v>
@@ -8841,7 +8841,7 @@
         <v>0</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G109" t="str">
         <f t="shared" si="61"/>
@@ -8883,7 +8883,7 @@
         <v>20</v>
       </c>
       <c r="B110" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C110" t="s">
         <v>55</v>
@@ -8918,10 +8918,10 @@
         <v>56</v>
       </c>
       <c r="Y110" s="4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="Z110" s="4" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="AB110" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B110)&amp;"-"&amp;SUBSTITUTE(C110,"_","")&amp;".html")</f>
@@ -8979,7 +8979,7 @@
         <v>20</v>
       </c>
       <c r="B112" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C112" t="s">
         <v>55</v>
@@ -9014,10 +9014,10 @@
         <v>56</v>
       </c>
       <c r="Y112" s="4" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="Z112" s="4" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="AA112" s="10"/>
       <c r="AB112" t="str">
@@ -9030,7 +9030,7 @@
         <v>79</v>
       </c>
       <c r="B113" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C113" t="s">
         <v>90</v>
@@ -9042,7 +9042,7 @@
         <v>1</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G113" t="str">
         <f t="shared" si="61"/>
@@ -9089,7 +9089,7 @@
         <v>26</v>
       </c>
       <c r="B114" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C114" t="s">
         <v>23</v>
@@ -9127,7 +9127,7 @@
         <v>56</v>
       </c>
       <c r="Y114" s="4" t="s">
-        <v>470</v>
+        <v>718</v>
       </c>
       <c r="Z114" s="4" t="str">
         <f>"GET [base]/"&amp;B114&amp;"?"&amp;C114&amp;"=Mary Shaw"</f>
@@ -9147,7 +9147,7 @@
         <v>80</v>
       </c>
       <c r="B115" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C115" t="s">
         <v>55</v>
@@ -9186,7 +9186,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z115" s="4" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="AB115" t="str">
         <f t="shared" ref="AB115:AB121" si="65">"SearchParameter-us-core-"&amp;LOWER((B115)&amp;"-"&amp;SUBSTITUTE(C115,"_","")&amp;".html")</f>
@@ -9198,7 +9198,7 @@
         <v>81</v>
       </c>
       <c r="B116" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C116" t="s">
         <v>90</v>
@@ -9210,7 +9210,7 @@
         <v>1</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G116" t="str">
         <f t="shared" si="61"/>
@@ -9257,7 +9257,7 @@
         <v>82</v>
       </c>
       <c r="B117" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C117" t="s">
         <v>62</v>
@@ -9269,7 +9269,7 @@
         <v>0</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G117" t="str">
         <f t="shared" si="61"/>
@@ -9298,7 +9298,7 @@
         <v>56</v>
       </c>
       <c r="Y117" s="20" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="AB117" t="str">
         <f t="shared" si="65"/>
@@ -9310,10 +9310,10 @@
         <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C118" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="D118" t="s">
         <v>30</v>
@@ -9322,7 +9322,7 @@
         <v>0</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G118" t="str">
         <f t="shared" si="61"/>
@@ -9338,7 +9338,7 @@
         <v>57</v>
       </c>
       <c r="L118" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="M118" t="s">
         <v>56</v>
@@ -9347,7 +9347,7 @@
         <v>56</v>
       </c>
       <c r="Y118" s="20" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="65"/>
@@ -9359,10 +9359,10 @@
         <v>84</v>
       </c>
       <c r="B119" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C119" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="D119" t="s">
         <v>30</v>
@@ -9371,7 +9371,7 @@
         <v>0</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G119" t="str">
         <f t="shared" si="61"/>
@@ -9403,7 +9403,7 @@
         <v>93</v>
       </c>
       <c r="Y119" s="20" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="65"/>
@@ -9415,10 +9415,10 @@
         <v>85</v>
       </c>
       <c r="B120" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C120" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="D120" t="s">
         <v>30</v>
@@ -9427,7 +9427,7 @@
         <v>0</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G120" t="str">
         <f t="shared" si="61"/>
@@ -9453,7 +9453,7 @@
         <v>56</v>
       </c>
       <c r="Y120" s="20" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="65"/>
@@ -9465,7 +9465,7 @@
         <v>86</v>
       </c>
       <c r="B121" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="C121" t="s">
         <v>90</v>
@@ -9477,7 +9477,7 @@
         <v>1</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G121" t="str">
         <f t="shared" si="61"/>
@@ -9506,7 +9506,7 @@
         <v>56</v>
       </c>
       <c r="Y121" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="Z121" s="4" t="str">
         <f>"GET [base]/"&amp;B121&amp;"?patient=1137192"</f>
@@ -9526,7 +9526,7 @@
         <v>87</v>
       </c>
       <c r="B122" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C122" t="s">
         <v>62</v>
@@ -9538,7 +9538,7 @@
         <v>0</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G122" t="str">
         <f t="shared" si="61"/>
@@ -9582,7 +9582,7 @@
         <v>88</v>
       </c>
       <c r="B123" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C123" t="s">
         <v>13</v>
@@ -9594,7 +9594,7 @@
         <v>0</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G123" t="str">
         <f t="shared" si="61"/>
@@ -9638,7 +9638,7 @@
         <v>89</v>
       </c>
       <c r="B124" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C124" t="s">
         <v>90</v>
@@ -9650,7 +9650,7 @@
         <v>1</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="G124" t="str">
         <f t="shared" si="61"/>
@@ -9679,10 +9679,10 @@
         <v>56</v>
       </c>
       <c r="X124" s="6" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="Z124" s="10" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="AA124" s="10" t="str">
         <f>"Fetches a bundle of all "&amp;B124&amp; " resources for the specified patient."</f>
@@ -9698,10 +9698,10 @@
         <v>61</v>
       </c>
       <c r="B125" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C125" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="D125" t="s">
         <v>30</v>
@@ -9710,7 +9710,7 @@
         <v>0</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="G125" t="str">
         <f t="shared" si="61"/>
@@ -9769,7 +9769,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomRight" activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9782,7 +9782,7 @@
     <col min="7" max="7" width="21.5" customWidth="1"/>
     <col min="8" max="8" width="121.6640625" customWidth="1"/>
     <col min="9" max="9" width="88.83203125" customWidth="1"/>
-    <col min="10" max="10" width="120" customWidth="1"/>
+    <col min="10" max="10" width="255.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="83.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9800,7 +9800,7 @@
         <v>96</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>97</v>
@@ -10130,7 +10130,7 @@
         <v>304</v>
       </c>
       <c r="J13" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="K13" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10230,7 +10230,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="F17" t="s">
         <v>70</v>
@@ -10242,7 +10242,7 @@
         <v>305</v>
       </c>
       <c r="J17" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10318,7 +10318,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="F20" t="s">
         <v>70</v>
@@ -10330,7 +10330,7 @@
         <v>310</v>
       </c>
       <c r="J20" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10640,7 +10640,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="F32" t="s">
         <v>70</v>
@@ -10649,10 +10649,10 @@
         <v>134</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" ref="K32" si="7">"Fetches a bundle of all "&amp;B32&amp;" resources matching the specified "&amp;SUBSTITUTE(D32,","," and ")</f>
@@ -10782,7 +10782,7 @@
         <v>330</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -10827,7 +10827,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="F38" t="s">
         <v>70</v>
@@ -10839,10 +10839,10 @@
         <v>150</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>558</v>
+        <v>717</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -10899,7 +10899,7 @@
         <v>153</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>156</v>
@@ -10917,7 +10917,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F41" t="s">
         <v>70</v>
@@ -10929,7 +10929,7 @@
         <v>153</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>156</v>
@@ -10947,7 +10947,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F42" t="s">
         <v>70</v>
@@ -10959,7 +10959,7 @@
         <v>153</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>156</v>
@@ -10977,7 +10977,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F43" t="s">
         <v>70</v>
@@ -10989,7 +10989,7 @@
         <v>153</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>156</v>
@@ -11049,7 +11049,7 @@
         <v>167</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="K45" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B45&amp;" resources for the specified "&amp;SUBSTITUTE(D45,","," and ")</f>
@@ -11206,7 +11206,7 @@
         <v>195</v>
       </c>
       <c r="J50" s="8" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K50" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -11236,7 +11236,7 @@
         <v>226</v>
       </c>
       <c r="J51" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K51" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B51&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11356,7 +11356,7 @@
         <v>201</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K55" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B55&amp;" resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes"</f>
@@ -11386,7 +11386,7 @@
         <v>220</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="K56" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11581,7 +11581,7 @@
         <v>230</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="K62" s="4" t="s">
         <v>460</v>
@@ -11735,7 +11735,7 @@
         <v>227</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="K67" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B67&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -11863,7 +11863,7 @@
         <v>225</v>
       </c>
       <c r="J71" s="4" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K71" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -11893,7 +11893,7 @@
         <v>223</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11989,7 +11989,7 @@
         <v>241</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="K75" s="4" t="s">
         <v>245</v>
@@ -12053,7 +12053,7 @@
         <v>240</v>
       </c>
       <c r="J77" s="4" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="K77" s="4" t="s">
         <v>247</v>
@@ -12061,7 +12061,7 @@
     </row>
     <row r="78" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="B78" t="s">
         <v>248</v>
@@ -12083,13 +12083,13 @@
         <v>311</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="J78" s="4" t="s">
+        <v>574</v>
+      </c>
+      <c r="K78" s="10" t="s">
         <v>576</v>
-      </c>
-      <c r="K78" s="10" t="s">
-        <v>578</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -12133,7 +12133,7 @@
         <v>183</v>
       </c>
       <c r="C80" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D80" t="s">
         <v>237</v>
@@ -12166,7 +12166,7 @@
         <v>183</v>
       </c>
       <c r="C81" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D81" t="s">
         <v>145</v>
@@ -12199,7 +12199,7 @@
         <v>183</v>
       </c>
       <c r="C82" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D82" t="s">
         <v>147</v>
@@ -12232,7 +12232,7 @@
         <v>183</v>
       </c>
       <c r="C83" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D83" t="s">
         <v>194</v>
@@ -12250,7 +12250,7 @@
         <v>283</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="K83" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified patient and date and a category code = `vital-signs`"</f>
@@ -12265,7 +12265,7 @@
         <v>183</v>
       </c>
       <c r="C84" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="D84" t="s">
         <v>219</v>
@@ -12280,7 +12280,7 @@
         <v>284</v>
       </c>
       <c r="J84" s="4" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="K84" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B84&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes."</f>
@@ -12407,7 +12407,7 @@
         <v>296</v>
       </c>
       <c r="J88" s="8" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="K88" s="4" t="s">
         <v>298</v>
@@ -12467,7 +12467,7 @@
         <v>301</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="K90" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -12515,7 +12515,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D92" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F92" t="s">
         <v>70</v>
@@ -12524,13 +12524,13 @@
         <v>106</v>
       </c>
       <c r="I92" s="4" t="s">
+        <v>570</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="K92" s="4" t="s">
         <v>572</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>573</v>
-      </c>
-      <c r="K92" s="4" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -12538,7 +12538,7 @@
         <v>117</v>
       </c>
       <c r="B93" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" ref="C93:C106" si="12">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B93)</f>
@@ -12557,7 +12557,7 @@
         <v>303</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="K93" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
@@ -12569,7 +12569,7 @@
         <v>118</v>
       </c>
       <c r="B94" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="12"/>
@@ -12588,7 +12588,7 @@
         <v>198</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="K94" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient and  a category code"</f>
@@ -12600,7 +12600,7 @@
         <v>119</v>
       </c>
       <c r="B95" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="12"/>
@@ -12619,7 +12619,7 @@
         <v>199</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K95" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12631,14 +12631,14 @@
         <v>120</v>
       </c>
       <c r="B96" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D96" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="F96" t="s">
         <v>12</v>
@@ -12650,7 +12650,7 @@
         <v>201</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="K96" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and date and a category code"</f>
@@ -12662,14 +12662,14 @@
         <v>121</v>
       </c>
       <c r="B97" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D97" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="F97" t="s">
         <v>70</v>
@@ -12678,10 +12678,10 @@
         <v>218</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="K97" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -12700,7 +12700,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D98" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="F98" t="s">
         <v>70</v>
@@ -12709,10 +12709,10 @@
         <v>106</v>
       </c>
       <c r="I98" s="4" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="K98" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified "&amp;SUBSTITUTE(D98,","," and ")</f>
@@ -12724,7 +12724,7 @@
         <v>123</v>
       </c>
       <c r="B99" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="12"/>
@@ -12740,10 +12740,10 @@
         <v>106</v>
       </c>
       <c r="I99" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="K99" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified "&amp;SUBSTITUTE(D99,","," and ")</f>
@@ -12755,14 +12755,14 @@
         <v>124</v>
       </c>
       <c r="B100" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D100" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="F100" t="s">
         <v>70</v>
@@ -12771,13 +12771,13 @@
         <v>106</v>
       </c>
       <c r="H100" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="I100" t="s">
+        <v>653</v>
+      </c>
+      <c r="J100" s="4" t="s">
         <v>655</v>
-      </c>
-      <c r="J100" s="4" t="s">
-        <v>657</v>
       </c>
       <c r="K100" t="str">
         <f>"Fetches a bundle of all "&amp;B100&amp;" resources for the specified "&amp;SUBSTITUTE(D100,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12789,14 +12789,14 @@
         <v>125</v>
       </c>
       <c r="B101" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D101" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="F101" t="s">
         <v>70</v>
@@ -12805,10 +12805,10 @@
         <v>149</v>
       </c>
       <c r="I101" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="K101" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient and date"</f>
@@ -12820,14 +12820,14 @@
         <v>126</v>
       </c>
       <c r="B102" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="F102" t="s">
         <v>70</v>
@@ -12836,13 +12836,13 @@
         <v>218</v>
       </c>
       <c r="H102" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="I102" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J102" s="4" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="K102" t="str">
         <f>"Fetches a bundle of all "&amp;B102&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12854,14 +12854,14 @@
         <v>127</v>
       </c>
       <c r="B103" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="F103" t="s">
         <v>70</v>
@@ -12870,10 +12870,10 @@
         <v>91</v>
       </c>
       <c r="I103" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="J103" s="4" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="K103" t="str">
         <f>"Fetches a bundle of all "&amp;B103&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12885,7 +12885,7 @@
         <v>129</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="12"/>
@@ -12905,10 +12905,10 @@
       </c>
       <c r="H104" s="18"/>
       <c r="I104" s="4" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="K104" t="str">
         <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12920,7 +12920,7 @@
         <v>129</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="12"/>
@@ -12940,10 +12940,10 @@
       </c>
       <c r="H105" s="18"/>
       <c r="I105" s="4" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="J105" s="4" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="K105" t="str">
         <f>"Fetches a bundle of all "&amp;B105&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12955,14 +12955,14 @@
         <v>130</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="E106" s="18" t="s">
         <v>56</v>
@@ -12975,10 +12975,10 @@
       </c>
       <c r="H106" s="18"/>
       <c r="I106" s="4" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="J106" s="4" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="K106" t="str">
         <f>"Fetches a bundle of all "&amp;B105&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -13031,7 +13031,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13047,7 +13047,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -13063,7 +13063,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13071,36 +13071,36 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B9" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B10" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="B12" t="s">
         <v>70</v>
@@ -13131,7 +13131,7 @@
         <v>23</v>
       </c>
       <c r="B1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="C1" t="s">
         <v>60</v>
@@ -13142,13 +13142,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="B2" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="C2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="D2" t="s">
         <v>70</v>
@@ -13156,13 +13156,13 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D3" t="s">
         <v>70</v>
@@ -13192,16 +13192,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>524</v>
+      </c>
+      <c r="B1" t="s">
         <v>525</v>
-      </c>
-      <c r="B1" t="s">
-        <v>526</v>
       </c>
       <c r="C1" t="s">
         <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="E1" t="s">
         <v>60</v>
@@ -13215,13 +13215,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -13310,10 +13310,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="B5" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -13324,10 +13324,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="B6" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -13338,16 +13338,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>677</v>
+      </c>
+      <c r="B7" t="s">
+        <v>678</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>679</v>
-      </c>
-      <c r="B7" t="s">
-        <v>680</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>681</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13408,7 +13408,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="B12" t="s">
         <v>365</v>
@@ -13422,86 +13422,86 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="B13" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
       </c>
       <c r="E13" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
       <c r="B14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="B15" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="B16" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B17" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
       <c r="B18" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -13576,16 +13576,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>693</v>
+      </c>
+      <c r="B24" t="s">
+        <v>694</v>
+      </c>
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
         <v>695</v>
-      </c>
-      <c r="B24" t="s">
-        <v>696</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>697</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13604,10 +13604,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="B26" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -13618,10 +13618,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="B27" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -13632,10 +13632,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="B28" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -13646,10 +13646,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="B29" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -13660,10 +13660,10 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="19" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B30" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="D30" t="s">
         <v>12</v>
@@ -13674,10 +13674,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
       <c r="B31" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -13688,10 +13688,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="19" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B32" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -13702,10 +13702,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="19" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B33" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -13716,10 +13716,10 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="19" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B34" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D34" t="s">
         <v>12</v>
@@ -13758,10 +13758,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="B37" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -13772,10 +13772,10 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="19" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B38" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="D38" t="s">
         <v>12</v>
@@ -13786,10 +13786,10 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="19" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B39" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D39" t="s">
         <v>12</v>
@@ -13800,10 +13800,10 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="19" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B40" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="D40" t="s">
         <v>12</v>
@@ -13814,10 +13814,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B41" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -13828,10 +13828,10 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="19" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B42" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D42" t="s">
         <v>12</v>
@@ -13842,10 +13842,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="B43" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -13856,10 +13856,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="B44" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -13870,10 +13870,10 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="19" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B45" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D45" t="s">
         <v>12</v>
@@ -13884,10 +13884,10 @@
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="19" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B46" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -13898,10 +13898,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="19" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B47" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -13912,10 +13912,10 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="19" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B48" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D48" t="s">
         <v>12</v>
@@ -14010,58 +14010,58 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
+        <v>626</v>
+      </c>
+      <c r="B55" t="s">
+        <v>627</v>
+      </c>
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" t="s">
         <v>628</v>
-      </c>
-      <c r="B55" t="s">
-        <v>629</v>
-      </c>
-      <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
       <c r="B56" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
       </c>
       <c r="E56" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="B57" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="B58" t="s">
+        <v>689</v>
+      </c>
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
         <v>690</v>
-      </c>
-      <c r="B58" t="s">
-        <v>691</v>
-      </c>
-      <c r="D58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" t="s">
-        <v>692</v>
       </c>
     </row>
   </sheetData>
@@ -14115,7 +14115,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F1" t="s">
         <v>15</v>
@@ -14166,16 +14166,16 @@
         <v>406</v>
       </c>
       <c r="V1" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="X1" s="3" t="s">
         <v>528</v>
       </c>
-      <c r="W1" s="3" t="s">
-        <v>527</v>
-      </c>
-      <c r="X1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>529</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>530</v>
       </c>
     </row>
     <row r="2" spans="1:25" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -14209,7 +14209,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="T3" t="s">
         <v>19</v>
@@ -14232,7 +14232,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="T4" t="s">
         <v>19</v>
@@ -14241,10 +14241,10 @@
         <v>70</v>
       </c>
       <c r="V4" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="W4" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="X4" s="15" t="s">
         <v>449</v>
@@ -14261,7 +14261,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="T5" t="s">
         <v>19</v>
@@ -14278,7 +14278,7 @@
     </row>
     <row r="6" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -14304,7 +14304,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="T7" t="s">
         <v>19</v>
@@ -14348,7 +14348,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14371,7 +14371,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="T10" t="s">
         <v>19</v>
@@ -14414,7 +14414,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="T12" t="s">
         <v>19</v>
@@ -14437,7 +14437,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T13" t="s">
         <v>19</v>
@@ -14456,7 +14456,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="T14" t="s">
         <v>19</v>
@@ -14475,7 +14475,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="T15" t="s">
         <v>19</v>
@@ -14498,13 +14498,13 @@
     </row>
     <row r="16" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>695</v>
+      </c>
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>697</v>
-      </c>
-      <c r="B16" t="s">
-        <v>12</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>699</v>
       </c>
       <c r="T16" t="s">
         <v>19</v>
@@ -14516,7 +14516,7 @@
         <v>70</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="X16" s="15" t="s">
         <v>449</v>
@@ -14533,7 +14533,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="T17" t="s">
         <v>19</v>
@@ -14562,7 +14562,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="T18" t="s">
         <v>19</v>
@@ -14585,7 +14585,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="T19" t="s">
         <v>19</v>
@@ -14604,7 +14604,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="T20" t="s">
         <v>19</v>
@@ -14643,7 +14643,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="T22" t="s">
         <v>19</v>
@@ -14652,7 +14652,7 @@
         <v>70</v>
       </c>
       <c r="V22" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="W22" t="s">
         <v>273</v>
@@ -14668,7 +14668,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="T23" t="s">
         <v>19</v>
@@ -14691,7 +14691,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="T24" t="s">
         <v>19</v>
@@ -14702,13 +14702,13 @@
     </row>
     <row r="25" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="B25" t="s">
         <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="T25" t="s">
         <v>19</v>
@@ -14725,7 +14725,7 @@
     </row>
     <row r="26" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
@@ -14745,7 +14745,7 @@
     </row>
     <row r="27" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
@@ -14765,7 +14765,7 @@
     </row>
     <row r="28" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -14851,7 +14851,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -14929,7 +14929,7 @@
         <v>371</v>
       </c>
       <c r="F1" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="G1" t="s">
         <v>372</v>
@@ -14959,7 +14959,7 @@
         <v>379</v>
       </c>
       <c r="P1" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="Q1" t="s">
         <v>380</v>
@@ -14992,19 +14992,19 @@
         <v>439</v>
       </c>
       <c r="AA1" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="AB1" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="AC1" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="AD1" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="AE1" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="AF1" t="s">
         <v>448</v>

</xml_diff>

<commit_message>
Fix Quick Start Rendering FHIR-39367
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D27633D-F214-7744-BDA1-02F318F3B322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7153F003-53E9-8540-83FD-D3B4D58399E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="17060" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2739" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2738" uniqueCount="718">
   <si>
     <t>Element</t>
   </si>
@@ -1839,9 +1839,6 @@
   </si>
   <si>
     <t>support searching a careteam by participant role</t>
-  </si>
-  <si>
-    <t>DOES THIS DO ANYTHING?</t>
   </si>
   <si>
     <t>support searching for all current care team members for a patient. DOES THIS DO ANYTHING?</t>
@@ -2965,7 +2962,7 @@
         <v>466</v>
       </c>
       <c r="B2" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2997,7 +2994,7 @@
         <v>68</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3013,7 +3010,7 @@
         <v>469</v>
       </c>
       <c r="B8" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -3034,10 +3031,10 @@
   <dimension ref="A1:AB125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="N92" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="W54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W113" sqref="W113"/>
+      <selection pane="bottomRight" activeCell="Y63" sqref="Y63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4344,7 +4341,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D25" t="s">
         <v>30</v>
@@ -4621,7 +4618,7 @@
         <v>56</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="Z30" t="s">
         <v>173</v>
@@ -4643,7 +4640,7 @@
         <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -4668,19 +4665,19 @@
         <v>57</v>
       </c>
       <c r="L31" t="s">
+        <v>710</v>
+      </c>
+      <c r="M31" t="s">
+        <v>56</v>
+      </c>
+      <c r="O31" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>711</v>
       </c>
-      <c r="M31" t="s">
-        <v>56</v>
-      </c>
-      <c r="O31" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>712</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>713</v>
       </c>
       <c r="AA31" s="10" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -7529,7 +7526,7 @@
         <v>56</v>
       </c>
       <c r="X85" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="Y85" t="str">
         <f>"support searching for all "&amp;LOWER(B85)&amp;"s for a patient"</f>
@@ -7595,9 +7592,7 @@
         <f>"GET [base]/"&amp;B86&amp;"/practitioner-1~GET [base]/"&amp;B86&amp;"?_id=practitioner-1"</f>
         <v>GET [base]/Practitioner/practitioner-1~GET [base]/Practitioner?_id=practitioner-1</v>
       </c>
-      <c r="AA86" s="10" t="s">
-        <v>567</v>
-      </c>
+      <c r="AA86" s="10"/>
       <c r="AB86" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B86)&amp;"-"&amp;SUBSTITUTE(C86,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-practitioner-id.html</v>
@@ -8614,7 +8609,7 @@
         <v>49</v>
       </c>
       <c r="B105" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C105" t="s">
         <v>62</v>
@@ -8667,7 +8662,7 @@
         <v>50</v>
       </c>
       <c r="B106" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C106" t="s">
         <v>90</v>
@@ -8726,7 +8721,7 @@
         <v>51</v>
       </c>
       <c r="B107" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C107" t="s">
         <v>140</v>
@@ -8776,7 +8771,7 @@
         <v>52</v>
       </c>
       <c r="B108" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C108" t="s">
         <v>26</v>
@@ -8829,10 +8824,10 @@
         <v>53</v>
       </c>
       <c r="B109" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C109" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D109" t="s">
         <v>30</v>
@@ -8883,7 +8878,7 @@
         <v>20</v>
       </c>
       <c r="B110" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C110" t="s">
         <v>55</v>
@@ -8918,10 +8913,10 @@
         <v>56</v>
       </c>
       <c r="Y110" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="Z110" s="4" t="s">
         <v>582</v>
-      </c>
-      <c r="Z110" s="4" t="s">
-        <v>583</v>
       </c>
       <c r="AB110" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B110)&amp;"-"&amp;SUBSTITUTE(C110,"_","")&amp;".html")</f>
@@ -8979,7 +8974,7 @@
         <v>20</v>
       </c>
       <c r="B112" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C112" t="s">
         <v>55</v>
@@ -9014,10 +9009,10 @@
         <v>56</v>
       </c>
       <c r="Y112" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="Z112" s="4" t="s">
         <v>604</v>
-      </c>
-      <c r="Z112" s="4" t="s">
-        <v>605</v>
       </c>
       <c r="AA112" s="10"/>
       <c r="AB112" t="str">
@@ -9030,7 +9025,7 @@
         <v>79</v>
       </c>
       <c r="B113" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C113" t="s">
         <v>90</v>
@@ -9089,7 +9084,7 @@
         <v>26</v>
       </c>
       <c r="B114" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C114" t="s">
         <v>23</v>
@@ -9127,7 +9122,7 @@
         <v>56</v>
       </c>
       <c r="Y114" s="4" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="Z114" s="4" t="str">
         <f>"GET [base]/"&amp;B114&amp;"?"&amp;C114&amp;"=Mary Shaw"</f>
@@ -9147,7 +9142,7 @@
         <v>80</v>
       </c>
       <c r="B115" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C115" t="s">
         <v>55</v>
@@ -9186,7 +9181,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z115" s="4" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="AB115" t="str">
         <f t="shared" ref="AB115:AB121" si="65">"SearchParameter-us-core-"&amp;LOWER((B115)&amp;"-"&amp;SUBSTITUTE(C115,"_","")&amp;".html")</f>
@@ -9198,7 +9193,7 @@
         <v>81</v>
       </c>
       <c r="B116" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C116" t="s">
         <v>90</v>
@@ -9257,7 +9252,7 @@
         <v>82</v>
       </c>
       <c r="B117" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C117" t="s">
         <v>62</v>
@@ -9298,7 +9293,7 @@
         <v>56</v>
       </c>
       <c r="Y117" s="20" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AB117" t="str">
         <f t="shared" si="65"/>
@@ -9310,10 +9305,10 @@
         <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C118" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
       <c r="D118" t="s">
         <v>30</v>
@@ -9338,16 +9333,16 @@
         <v>57</v>
       </c>
       <c r="L118" t="s">
+        <v>640</v>
+      </c>
+      <c r="M118" t="s">
+        <v>56</v>
+      </c>
+      <c r="O118" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y118" s="20" t="s">
         <v>641</v>
-      </c>
-      <c r="M118" t="s">
-        <v>56</v>
-      </c>
-      <c r="O118" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y118" s="20" t="s">
-        <v>642</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="65"/>
@@ -9359,10 +9354,10 @@
         <v>84</v>
       </c>
       <c r="B119" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C119" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="D119" t="s">
         <v>30</v>
@@ -9403,7 +9398,7 @@
         <v>93</v>
       </c>
       <c r="Y119" s="20" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="65"/>
@@ -9415,10 +9410,10 @@
         <v>85</v>
       </c>
       <c r="B120" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C120" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="D120" t="s">
         <v>30</v>
@@ -9453,7 +9448,7 @@
         <v>56</v>
       </c>
       <c r="Y120" s="20" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="65"/>
@@ -9465,7 +9460,7 @@
         <v>86</v>
       </c>
       <c r="B121" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C121" t="s">
         <v>90</v>
@@ -9506,7 +9501,7 @@
         <v>56</v>
       </c>
       <c r="Y121" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="Z121" s="4" t="str">
         <f>"GET [base]/"&amp;B121&amp;"?patient=1137192"</f>
@@ -9526,7 +9521,7 @@
         <v>87</v>
       </c>
       <c r="B122" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C122" t="s">
         <v>62</v>
@@ -9582,7 +9577,7 @@
         <v>88</v>
       </c>
       <c r="B123" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C123" t="s">
         <v>13</v>
@@ -9638,7 +9633,7 @@
         <v>89</v>
       </c>
       <c r="B124" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C124" t="s">
         <v>90</v>
@@ -9679,10 +9674,10 @@
         <v>56</v>
       </c>
       <c r="X124" s="6" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="Z124" s="10" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="AA124" s="10" t="str">
         <f>"Fetches a bundle of all "&amp;B124&amp; " resources for the specified patient."</f>
@@ -9698,10 +9693,10 @@
         <v>61</v>
       </c>
       <c r="B125" t="s">
+        <v>701</v>
+      </c>
+      <c r="C125" t="s">
         <v>702</v>
-      </c>
-      <c r="C125" t="s">
-        <v>703</v>
       </c>
       <c r="D125" t="s">
         <v>30</v>
@@ -10640,7 +10635,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="F32" t="s">
         <v>70</v>
@@ -10649,10 +10644,10 @@
         <v>134</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" ref="K32" si="7">"Fetches a bundle of all "&amp;B32&amp;" resources matching the specified "&amp;SUBSTITUTE(D32,","," and ")</f>
@@ -10782,7 +10777,7 @@
         <v>330</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -10839,7 +10834,7 @@
         <v>150</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>557</v>
@@ -12061,7 +12056,7 @@
     </row>
     <row r="78" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="B78" t="s">
         <v>248</v>
@@ -12083,13 +12078,13 @@
         <v>311</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="K78" s="10" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -12515,7 +12510,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D92" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F92" t="s">
         <v>70</v>
@@ -12524,13 +12519,13 @@
         <v>106</v>
       </c>
       <c r="I92" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="J92" s="4" t="s">
         <v>570</v>
       </c>
-      <c r="J92" s="4" t="s">
+      <c r="K92" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="K92" s="4" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
@@ -12538,7 +12533,7 @@
         <v>117</v>
       </c>
       <c r="B93" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" ref="C93:C106" si="12">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B93)</f>
@@ -12557,7 +12552,7 @@
         <v>303</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K93" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
@@ -12569,7 +12564,7 @@
         <v>118</v>
       </c>
       <c r="B94" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="12"/>
@@ -12588,7 +12583,7 @@
         <v>198</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K94" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient and  a category code"</f>
@@ -12600,7 +12595,7 @@
         <v>119</v>
       </c>
       <c r="B95" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="12"/>
@@ -12619,7 +12614,7 @@
         <v>199</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
       <c r="K95" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12631,14 +12626,14 @@
         <v>120</v>
       </c>
       <c r="B96" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D96" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F96" t="s">
         <v>12</v>
@@ -12650,7 +12645,7 @@
         <v>201</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="K96" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and date and a category code"</f>
@@ -12662,14 +12657,14 @@
         <v>121</v>
       </c>
       <c r="B97" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D97" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="F97" t="s">
         <v>70</v>
@@ -12678,10 +12673,10 @@
         <v>218</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="K97" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -12700,7 +12695,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D98" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="F98" t="s">
         <v>70</v>
@@ -12709,10 +12704,10 @@
         <v>106</v>
       </c>
       <c r="I98" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>591</v>
-      </c>
-      <c r="J98" s="4" t="s">
-        <v>592</v>
       </c>
       <c r="K98" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified "&amp;SUBSTITUTE(D98,","," and ")</f>
@@ -12724,7 +12719,7 @@
         <v>123</v>
       </c>
       <c r="B99" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="12"/>
@@ -12740,10 +12735,10 @@
         <v>106</v>
       </c>
       <c r="I99" t="s">
+        <v>652</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>653</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>654</v>
       </c>
       <c r="K99" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified "&amp;SUBSTITUTE(D99,","," and ")</f>
@@ -12755,14 +12750,14 @@
         <v>124</v>
       </c>
       <c r="B100" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D100" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="F100" t="s">
         <v>70</v>
@@ -12771,13 +12766,13 @@
         <v>106</v>
       </c>
       <c r="H100" t="s">
+        <v>651</v>
+      </c>
+      <c r="I100" t="s">
         <v>652</v>
       </c>
-      <c r="I100" t="s">
-        <v>653</v>
-      </c>
       <c r="J100" s="4" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
       <c r="K100" t="str">
         <f>"Fetches a bundle of all "&amp;B100&amp;" resources for the specified "&amp;SUBSTITUTE(D100,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12789,14 +12784,14 @@
         <v>125</v>
       </c>
       <c r="B101" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D101" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="F101" t="s">
         <v>70</v>
@@ -12805,10 +12800,10 @@
         <v>149</v>
       </c>
       <c r="I101" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="K101" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient and date"</f>
@@ -12820,14 +12815,14 @@
         <v>126</v>
       </c>
       <c r="B102" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D102" s="18" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="F102" t="s">
         <v>70</v>
@@ -12836,13 +12831,13 @@
         <v>218</v>
       </c>
       <c r="H102" t="s">
+        <v>651</v>
+      </c>
+      <c r="I102" t="s">
         <v>652</v>
       </c>
-      <c r="I102" t="s">
-        <v>653</v>
-      </c>
       <c r="J102" s="4" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="K102" t="str">
         <f>"Fetches a bundle of all "&amp;B102&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12854,14 +12849,14 @@
         <v>127</v>
       </c>
       <c r="B103" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="F103" t="s">
         <v>70</v>
@@ -12870,10 +12865,10 @@
         <v>91</v>
       </c>
       <c r="I103" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="J103" s="4" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="K103" t="str">
         <f>"Fetches a bundle of all "&amp;B103&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12885,7 +12880,7 @@
         <v>129</v>
       </c>
       <c r="B104" s="18" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="12"/>
@@ -12905,10 +12900,10 @@
       </c>
       <c r="H104" s="18"/>
       <c r="I104" s="4" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K104" t="str">
         <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12920,7 +12915,7 @@
         <v>129</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="12"/>
@@ -12940,10 +12935,10 @@
       </c>
       <c r="H105" s="18"/>
       <c r="I105" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="J105" s="4" t="s">
         <v>707</v>
-      </c>
-      <c r="J105" s="4" t="s">
-        <v>708</v>
       </c>
       <c r="K105" t="str">
         <f>"Fetches a bundle of all "&amp;B105&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12955,14 +12950,14 @@
         <v>130</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E106" s="18" t="s">
         <v>56</v>
@@ -12975,10 +12970,10 @@
       </c>
       <c r="H106" s="18"/>
       <c r="I106" s="4" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="J106" s="4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="K106" t="str">
         <f>"Fetches a bundle of all "&amp;B105&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -13031,7 +13026,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13047,7 +13042,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -13063,7 +13058,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13071,7 +13066,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -13145,7 +13140,7 @@
         <v>536</v>
       </c>
       <c r="B2" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="C2" t="s">
         <v>542</v>
@@ -13310,10 +13305,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="B5" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -13324,10 +13319,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B6" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -13338,16 +13333,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>676</v>
+      </c>
+      <c r="B7" t="s">
         <v>677</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>678</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>679</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13408,7 +13403,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="19" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="B12" t="s">
         <v>365</v>
@@ -13422,86 +13417,86 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B13" t="s">
+        <v>609</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
         <v>610</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>611</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="19" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="B14" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
       </c>
       <c r="E14" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="19" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="B15" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="D15" t="s">
         <v>12</v>
       </c>
       <c r="E15" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="19" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="B16" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
       </c>
       <c r="E16" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="19" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="B17" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
       </c>
       <c r="E17" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="19" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B18" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -13576,16 +13571,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>692</v>
+      </c>
+      <c r="B24" t="s">
         <v>693</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
         <v>694</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>695</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13604,10 +13599,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B26" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -13618,10 +13613,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B27" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -13632,10 +13627,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="B28" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -13646,10 +13641,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
+        <v>611</v>
+      </c>
+      <c r="B29" t="s">
         <v>612</v>
-      </c>
-      <c r="B29" t="s">
-        <v>613</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -13674,10 +13669,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
+        <v>613</v>
+      </c>
+      <c r="B31" t="s">
         <v>614</v>
-      </c>
-      <c r="B31" t="s">
-        <v>615</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -13758,10 +13753,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B37" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -13814,10 +13809,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B41" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -13842,10 +13837,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="B43" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -13856,10 +13851,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B44" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -14010,58 +14005,58 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
+        <v>625</v>
+      </c>
+      <c r="B55" t="s">
         <v>626</v>
       </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" t="s">
         <v>627</v>
-      </c>
-      <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B56" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
       </c>
       <c r="E56" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B57" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
+        <v>687</v>
+      </c>
+      <c r="B58" t="s">
         <v>688</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
         <v>689</v>
-      </c>
-      <c r="D58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" t="s">
-        <v>690</v>
       </c>
     </row>
   </sheetData>
@@ -14232,7 +14227,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="T4" t="s">
         <v>19</v>
@@ -14241,10 +14236,10 @@
         <v>70</v>
       </c>
       <c r="V4" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="W4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="X4" s="15" t="s">
         <v>449</v>
@@ -14261,7 +14256,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="T5" t="s">
         <v>19</v>
@@ -14278,7 +14273,7 @@
     </row>
     <row r="6" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -14304,7 +14299,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="T7" t="s">
         <v>19</v>
@@ -14348,7 +14343,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14371,7 +14366,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="T10" t="s">
         <v>19</v>
@@ -14414,7 +14409,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="T12" t="s">
         <v>19</v>
@@ -14498,13 +14493,13 @@
     </row>
     <row r="16" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="T16" t="s">
         <v>19</v>
@@ -14516,7 +14511,7 @@
         <v>70</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="X16" s="15" t="s">
         <v>449</v>
@@ -14562,7 +14557,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="T18" t="s">
         <v>19</v>
@@ -14585,7 +14580,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="T19" t="s">
         <v>19</v>
@@ -14604,7 +14599,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="T20" t="s">
         <v>19</v>
@@ -14668,7 +14663,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="T23" t="s">
         <v>19</v>
@@ -14691,7 +14686,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="T24" t="s">
         <v>19</v>
@@ -14702,13 +14697,13 @@
     </row>
     <row r="25" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="B25" t="s">
         <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="T25" t="s">
         <v>19</v>
@@ -14725,7 +14720,7 @@
     </row>
     <row r="26" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
@@ -14745,7 +14740,7 @@
     </row>
     <row r="27" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
@@ -14765,7 +14760,7 @@
     </row>
     <row r="28" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -14851,7 +14846,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -14929,7 +14924,7 @@
         <v>371</v>
       </c>
       <c r="F1" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="G1" t="s">
         <v>372</v>
@@ -14959,7 +14954,7 @@
         <v>379</v>
       </c>
       <c r="P1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="Q1" t="s">
         <v>380</v>
@@ -14992,19 +14987,19 @@
         <v>439</v>
       </c>
       <c r="AA1" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="AB1" t="s">
+        <v>601</v>
+      </c>
+      <c r="AC1" t="s">
         <v>602</v>
       </c>
-      <c r="AC1" t="s">
-        <v>603</v>
-      </c>
       <c r="AD1" t="s">
+        <v>690</v>
+      </c>
+      <c r="AE1" t="s">
         <v>691</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>692</v>
       </c>
       <c r="AF1" t="s">
         <v>448</v>

</xml_diff>

<commit_message>
Remove extra instance or the word ""resource"" in Lab observation narrative profile FHIR-37507
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFD3CD0D-06C0-B045-B492-983203D8D523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460B0808-56A6-0347-B271-B7DC64CDDE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3025,10 +3025,10 @@
   <dimension ref="A1:AB125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q100" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q16" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Y114" sqref="Y114"/>
+      <selection pane="bottomRight" activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Add recommended search combination of patient + status FHIR-19803
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{460B0808-56A6-0347-B271-B7DC64CDDE98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51879F10-E165-C642-B5D0-6A95D3AD4594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34200" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -26,8 +26,8 @@
     <sheet name="sp_combos" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$97</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$120</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$126</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2738" uniqueCount="718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2755" uniqueCount="720">
   <si>
     <t>Element</t>
   </si>
@@ -2077,9 +2077,6 @@
   </si>
   <si>
     <t>GET [base]/QuestionnaireResponse/AHC-HRSN-screening-example~GET [base]/QuestionnaireResponse/?_id=AHC-HRSN-screening-example</t>
-  </si>
-  <si>
-    <t></t>
   </si>
   <si>
     <t>patient,_tag</t>
@@ -2391,6 +2388,15 @@
   </si>
   <si>
     <t>support searching for a patient by a server defined search that matches any of the string fields in the HumanName, including family, given, prefix, suffix, and/or text</t>
+  </si>
+  <si>
+    <t>support searching for all devices with a given status for a patient (for example all active devices)</t>
+  </si>
+  <si>
+    <t>GET [base]/Device?patient=1316024&amp;status=active</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Device resources for the specified patient and status</t>
   </si>
 </sst>
 </file>
@@ -2956,7 +2962,7 @@
         <v>466</v>
       </c>
       <c r="B2" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -3022,13 +3028,13 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:AB125"/>
+  <dimension ref="A1:AB126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="Q16" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X26" sqref="X26"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4024,7 +4030,7 @@
     </row>
     <row r="19" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
@@ -4082,7 +4088,7 @@
     </row>
     <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
@@ -4132,7 +4138,7 @@
     </row>
     <row r="21" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>22</v>
@@ -4182,7 +4188,7 @@
     </row>
     <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -4232,7 +4238,7 @@
     </row>
     <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B23" t="s">
         <v>21</v>
@@ -4282,7 +4288,7 @@
     </row>
     <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
         <v>21</v>
@@ -4329,13 +4335,13 @@
     </row>
     <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="D25" t="s">
         <v>30</v>
@@ -4379,7 +4385,7 @@
     </row>
     <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B26" t="s">
         <v>21</v>
@@ -4425,7 +4431,7 @@
     </row>
     <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B27" t="s">
         <v>21</v>
@@ -4473,7 +4479,7 @@
     </row>
     <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B28" t="s">
         <v>21</v>
@@ -4517,7 +4523,7 @@
     </row>
     <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B29" t="s">
         <v>21</v>
@@ -4574,7 +4580,7 @@
     </row>
     <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B30" t="s">
         <v>21</v>
@@ -4612,7 +4618,7 @@
         <v>56</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="Z30" t="s">
         <v>173</v>
@@ -4628,13 +4634,13 @@
     </row>
     <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
         <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -4659,19 +4665,19 @@
         <v>57</v>
       </c>
       <c r="L31" t="s">
+        <v>706</v>
+      </c>
+      <c r="M31" t="s">
+        <v>56</v>
+      </c>
+      <c r="O31" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="M31" t="s">
-        <v>56</v>
-      </c>
-      <c r="O31" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>708</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>709</v>
       </c>
       <c r="AA31" s="10" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4684,7 +4690,7 @@
     </row>
     <row r="32" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>158</v>
@@ -4727,7 +4733,7 @@
     </row>
     <row r="33" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>158</v>
@@ -4771,7 +4777,7 @@
     </row>
     <row r="34" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>158</v>
@@ -4818,7 +4824,7 @@
     </row>
     <row r="35" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>158</v>
@@ -4862,7 +4868,7 @@
     </row>
     <row r="36" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>158</v>
@@ -4918,7 +4924,7 @@
     </row>
     <row r="37" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>158</v>
@@ -4962,7 +4968,7 @@
     </row>
     <row r="38" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
         <v>158</v>
@@ -5006,7 +5012,7 @@
     </row>
     <row r="39" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>138</v>
@@ -5060,7 +5066,7 @@
     </row>
     <row r="40" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>138</v>
@@ -5114,7 +5120,7 @@
     </row>
     <row r="41" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>138</v>
@@ -5168,7 +5174,7 @@
     </row>
     <row r="42" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>138</v>
@@ -5222,7 +5228,7 @@
     </row>
     <row r="43" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>138</v>
@@ -5272,7 +5278,7 @@
     </row>
     <row r="44" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>12</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>138</v>
@@ -5330,7 +5336,7 @@
     </row>
     <row r="45" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>161</v>
@@ -5389,7 +5395,7 @@
     </row>
     <row r="46" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>161</v>
@@ -5439,7 +5445,7 @@
     </row>
     <row r="47" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>161</v>
@@ -5493,7 +5499,7 @@
     </row>
     <row r="48" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>178</v>
@@ -5546,7 +5552,7 @@
     </row>
     <row r="49" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>178</v>
@@ -5599,7 +5605,7 @@
     </row>
     <row r="50" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>178</v>
@@ -5658,7 +5664,7 @@
     </row>
     <row r="51" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>178</v>
@@ -5708,7 +5714,7 @@
     </row>
     <row r="52" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>178</v>
@@ -5758,7 +5764,7 @@
     </row>
     <row r="53" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>178</v>
@@ -5812,7 +5818,7 @@
     </row>
     <row r="54" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>178</v>
@@ -5865,7 +5871,7 @@
     </row>
     <row r="55" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>179</v>
@@ -5918,7 +5924,7 @@
     </row>
     <row r="56" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>179</v>
@@ -5977,7 +5983,7 @@
     </row>
     <row r="57" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>179</v>
@@ -6027,7 +6033,7 @@
     </row>
     <row r="58" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>179</v>
@@ -6080,7 +6086,7 @@
     </row>
     <row r="59" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>179</v>
@@ -6134,7 +6140,7 @@
     </row>
     <row r="60" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>180</v>
@@ -6184,7 +6190,7 @@
     </row>
     <row r="61" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>180</v>
@@ -6243,7 +6249,7 @@
     </row>
     <row r="62" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>180</v>
@@ -6297,7 +6303,7 @@
     </row>
     <row r="63" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>181</v>
@@ -6350,7 +6356,7 @@
     </row>
     <row r="64" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>181</v>
@@ -6403,7 +6409,7 @@
     </row>
     <row r="65" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>181</v>
@@ -6456,7 +6462,7 @@
     </row>
     <row r="66" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>181</v>
@@ -6507,7 +6513,7 @@
     </row>
     <row r="67" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>181</v>
@@ -6561,7 +6567,7 @@
     </row>
     <row r="68" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>435</v>
@@ -6614,7 +6620,7 @@
     </row>
     <row r="69" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>435</v>
@@ -6672,7 +6678,7 @@
     </row>
     <row r="70" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>435</v>
@@ -6726,7 +6732,7 @@
     </row>
     <row r="71" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>182</v>
@@ -6779,7 +6785,7 @@
     </row>
     <row r="72" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>182</v>
@@ -6837,7 +6843,7 @@
     </row>
     <row r="73" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>182</v>
@@ -6891,7 +6897,7 @@
     </row>
     <row r="74" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>182</v>
@@ -6944,7 +6950,7 @@
     </row>
     <row r="75" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>183</v>
@@ -6962,7 +6968,7 @@
         <v>503</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" ref="G75:G105" si="45">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B75)</f>
+        <f t="shared" ref="G75:G106" si="45">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B75)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H75" t="s">
@@ -6997,7 +7003,7 @@
     </row>
     <row r="76" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>183</v>
@@ -7047,7 +7053,7 @@
     </row>
     <row r="77" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>183</v>
@@ -7100,7 +7106,7 @@
     </row>
     <row r="78" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>183</v>
@@ -7154,7 +7160,7 @@
     </row>
     <row r="79" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>183</v>
@@ -7213,7 +7219,7 @@
     </row>
     <row r="80" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>234</v>
@@ -7263,7 +7269,7 @@
     </row>
     <row r="81" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>314</v>
@@ -7313,7 +7319,7 @@
     </row>
     <row r="82" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>234</v>
@@ -7367,7 +7373,7 @@
     </row>
     <row r="83" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>234</v>
@@ -7426,7 +7432,7 @@
     </row>
     <row r="84" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>234</v>
@@ -7479,7 +7485,7 @@
     </row>
     <row r="85" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>248</v>
@@ -7541,7 +7547,7 @@
     </row>
     <row r="86" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>20</v>
+        <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>267</v>
@@ -7594,7 +7600,7 @@
     </row>
     <row r="87" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>248</v>
@@ -7647,7 +7653,7 @@
     </row>
     <row r="88" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>248</v>
@@ -7705,7 +7711,7 @@
     </row>
     <row r="89" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>249</v>
@@ -7736,7 +7742,7 @@
         <v>91</v>
       </c>
       <c r="L89" t="str">
-        <f t="shared" ref="L89:L112" si="56">B89&amp;"."&amp;C89</f>
+        <f t="shared" ref="L89:L113" si="56">B89&amp;"."&amp;C89</f>
         <v>Device.patient</v>
       </c>
       <c r="M89" t="s">
@@ -7758,13 +7764,13 @@
         <v>Fetches a bundle of all Device resources for the specified patient</v>
       </c>
       <c r="AB89" t="str">
-        <f t="shared" ref="AB89:AB100" si="57">"SearchParameter-us-core-"&amp;LOWER((B89)&amp;"-"&amp;C89&amp;".html")</f>
+        <f t="shared" ref="AB89:AB101" si="57">"SearchParameter-us-core-"&amp;LOWER((B89)&amp;"-"&amp;C89&amp;".html")</f>
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
     <row r="90" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s">
         <v>249</v>
@@ -7813,23 +7819,26 @@
     </row>
     <row r="91" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>83</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C91" t="s">
-        <v>23</v>
+        <v>62</v>
       </c>
       <c r="D91" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E91" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>503</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="45"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-"&amp;LOWER(B91)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable-device</v>
       </c>
       <c r="H91" t="s">
         <v>56</v>
@@ -7838,43 +7847,37 @@
         <v>56</v>
       </c>
       <c r="K91" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="L91" t="str">
-        <f t="shared" si="56"/>
-        <v>Location.name</v>
+        <f t="shared" ref="L91" si="59">B91&amp;"."&amp;C91</f>
+        <v>Device.status</v>
       </c>
       <c r="M91" t="s">
         <v>56</v>
       </c>
+      <c r="N91" t="s">
+        <v>12</v>
+      </c>
       <c r="O91" t="s">
         <v>56</v>
       </c>
-      <c r="Y91" t="s">
-        <v>254</v>
-      </c>
-      <c r="Z91" s="4" t="str">
-        <f>"GET [base]/"&amp;B91&amp;"?name=Health"</f>
-        <v>GET [base]/Location?name=Health</v>
-      </c>
-      <c r="AA91" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B91&amp; " resources that match the name"</f>
-        <v>Fetches a bundle of all Location resources that match the name</v>
-      </c>
+      <c r="Z91" s="4"/>
+      <c r="AA91" s="10"/>
       <c r="AB91" t="str">
-        <f t="shared" si="57"/>
-        <v>SearchParameter-us-core-location-name.html</v>
+        <f t="shared" ref="AB91" si="60">"SearchParameter-us-core-"&amp;LOWER((B91)&amp;"-"&amp;C91&amp;".html")</f>
+        <v>SearchParameter-us-core-device-status.html</v>
       </c>
     </row>
     <row r="92" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="B92" t="s">
         <v>250</v>
       </c>
       <c r="C92" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="D92" t="s">
         <v>12</v>
@@ -7897,7 +7900,7 @@
       </c>
       <c r="L92" t="str">
         <f t="shared" si="56"/>
-        <v>Location.address</v>
+        <v>Location.name</v>
       </c>
       <c r="M92" t="s">
         <v>56</v>
@@ -7906,33 +7909,33 @@
         <v>56</v>
       </c>
       <c r="Y92" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="Z92" s="4" t="str">
-        <f>"GET [base]/"&amp;B92&amp;"?address=Arbor"</f>
-        <v>GET [base]/Location?address=Arbor</v>
+        <f>"GET [base]/"&amp;B92&amp;"?name=Health"</f>
+        <v>GET [base]/Location?name=Health</v>
       </c>
       <c r="AA92" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B92&amp; " resources that match the address string"</f>
-        <v>Fetches a bundle of all Location resources that match the address string</v>
+        <f>"Fetches a bundle of all "&amp;B92&amp; " resources that match the name"</f>
+        <v>Fetches a bundle of all Location resources that match the name</v>
       </c>
       <c r="AB92" t="str">
         <f t="shared" si="57"/>
-        <v>SearchParameter-us-core-location-address.html</v>
+        <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
     <row r="93" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
         <v>250</v>
       </c>
       <c r="C93" t="s">
-        <v>251</v>
+        <v>86</v>
       </c>
       <c r="D93" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="E93" t="b">
         <v>1</v>
@@ -7952,7 +7955,7 @@
       </c>
       <c r="L93" t="str">
         <f t="shared" si="56"/>
-        <v>Location.address-city</v>
+        <v>Location.address</v>
       </c>
       <c r="M93" t="s">
         <v>56</v>
@@ -7961,30 +7964,30 @@
         <v>56</v>
       </c>
       <c r="Y93" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="Z93" s="4" t="str">
-        <f>"GET [base]/"&amp;B93&amp;"?address-city=Ann Arbor"</f>
-        <v>GET [base]/Location?address-city=Ann Arbor</v>
+        <f>"GET [base]/"&amp;B93&amp;"?address=Arbor"</f>
+        <v>GET [base]/Location?address=Arbor</v>
       </c>
       <c r="AA93" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B93&amp; " resources for the city"</f>
-        <v>Fetches a bundle of all Location resources for the city</v>
+        <f>"Fetches a bundle of all "&amp;B93&amp; " resources that match the address string"</f>
+        <v>Fetches a bundle of all Location resources that match the address string</v>
       </c>
       <c r="AB93" t="str">
         <f t="shared" si="57"/>
-        <v>SearchParameter-us-core-location-address-city.html</v>
+        <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
     <row r="94" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>250</v>
       </c>
       <c r="C94" t="s">
-        <v>315</v>
+        <v>251</v>
       </c>
       <c r="D94" t="s">
         <v>70</v>
@@ -8007,7 +8010,7 @@
       </c>
       <c r="L94" t="str">
         <f t="shared" si="56"/>
-        <v>Location.address-state</v>
+        <v>Location.address-city</v>
       </c>
       <c r="M94" t="s">
         <v>56</v>
@@ -8016,29 +8019,30 @@
         <v>56</v>
       </c>
       <c r="Y94" t="s">
-        <v>257</v>
-      </c>
-      <c r="Z94" s="4" t="s">
-        <v>259</v>
+        <v>256</v>
+      </c>
+      <c r="Z94" s="4" t="str">
+        <f>"GET [base]/"&amp;B94&amp;"?address-city=Ann Arbor"</f>
+        <v>GET [base]/Location?address-city=Ann Arbor</v>
       </c>
       <c r="AA94" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B94&amp; " resources for the state"</f>
-        <v>Fetches a bundle of all Location resources for the state</v>
+        <f>"Fetches a bundle of all "&amp;B94&amp; " resources for the city"</f>
+        <v>Fetches a bundle of all Location resources for the city</v>
       </c>
       <c r="AB94" t="str">
         <f t="shared" si="57"/>
-        <v>SearchParameter-us-core-location-address-state.html</v>
+        <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
     <row r="95" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>250</v>
       </c>
       <c r="C95" t="s">
-        <v>253</v>
+        <v>315</v>
       </c>
       <c r="D95" t="s">
         <v>70</v>
@@ -8061,7 +8065,7 @@
       </c>
       <c r="L95" t="str">
         <f t="shared" si="56"/>
-        <v>Location.address-postalcode</v>
+        <v>Location.address-state</v>
       </c>
       <c r="M95" t="s">
         <v>56</v>
@@ -8070,40 +8074,39 @@
         <v>56</v>
       </c>
       <c r="Y95" t="s">
-        <v>258</v>
-      </c>
-      <c r="Z95" s="4" t="str">
-        <f>"GET [base]/"&amp;B95&amp;"?address-postalcode=48104"</f>
-        <v>GET [base]/Location?address-postalcode=48104</v>
+        <v>257</v>
+      </c>
+      <c r="Z95" s="4" t="s">
+        <v>259</v>
       </c>
       <c r="AA95" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B95&amp; " resources for the ZIP code"</f>
-        <v>Fetches a bundle of all Location resources for the ZIP code</v>
+        <f>"Fetches a bundle of all "&amp;B95&amp; " resources for the state"</f>
+        <v>Fetches a bundle of all Location resources for the state</v>
       </c>
       <c r="AB95" t="str">
         <f t="shared" si="57"/>
-        <v>SearchParameter-us-core-location-address-postalcode.html</v>
+        <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
     <row r="96" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C96" t="s">
-        <v>23</v>
+        <v>253</v>
       </c>
       <c r="D96" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="E96" t="b">
         <v>1</v>
       </c>
       <c r="G96" t="str">
         <f t="shared" si="45"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H96" t="s">
         <v>56</v>
@@ -8116,7 +8119,7 @@
       </c>
       <c r="L96" t="str">
         <f t="shared" si="56"/>
-        <v>Organization.name</v>
+        <v>Location.address-postalcode</v>
       </c>
       <c r="M96" t="s">
         <v>56</v>
@@ -8125,30 +8128,30 @@
         <v>56</v>
       </c>
       <c r="Y96" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="Z96" s="4" t="str">
-        <f>"GET [base]/"&amp;B96&amp;"?name=Health"</f>
-        <v>GET [base]/Organization?name=Health</v>
+        <f>"GET [base]/"&amp;B96&amp;"?address-postalcode=48104"</f>
+        <v>GET [base]/Location?address-postalcode=48104</v>
       </c>
       <c r="AA96" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B96&amp; " resources that match the name"</f>
-        <v>Fetches a bundle of all Organization resources that match the name</v>
+        <f>"Fetches a bundle of all "&amp;B96&amp; " resources for the ZIP code"</f>
+        <v>Fetches a bundle of all Location resources for the ZIP code</v>
       </c>
       <c r="AB96" t="str">
         <f t="shared" si="57"/>
-        <v>SearchParameter-us-core-organization-name.html</v>
+        <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
     <row r="97" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>260</v>
       </c>
       <c r="C97" t="s">
-        <v>86</v>
+        <v>23</v>
       </c>
       <c r="D97" t="s">
         <v>12</v>
@@ -8171,7 +8174,7 @@
       </c>
       <c r="L97" t="str">
         <f t="shared" si="56"/>
-        <v>Organization.address</v>
+        <v>Organization.name</v>
       </c>
       <c r="M97" t="s">
         <v>56</v>
@@ -8180,40 +8183,40 @@
         <v>56</v>
       </c>
       <c r="Y97" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Z97" s="4" t="str">
-        <f>"GET [base]/"&amp;B97&amp;"?address=Arbor"</f>
-        <v>GET [base]/Organization?address=Arbor</v>
+        <f>"GET [base]/"&amp;B97&amp;"?name=Health"</f>
+        <v>GET [base]/Organization?name=Health</v>
       </c>
       <c r="AA97" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B97&amp; " resources that match the address string"</f>
-        <v>Fetches a bundle of all Organization resources that match the address string</v>
+        <f>"Fetches a bundle of all "&amp;B97&amp; " resources that match the name"</f>
+        <v>Fetches a bundle of all Organization resources that match the name</v>
       </c>
       <c r="AB97" t="str">
         <f t="shared" si="57"/>
-        <v>SearchParameter-us-core-organization-address.html</v>
+        <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
     <row r="98" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C98" t="s">
-        <v>251</v>
+        <v>86</v>
       </c>
       <c r="D98" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="E98" t="b">
         <v>1</v>
       </c>
       <c r="G98" t="str">
         <f t="shared" si="45"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!organization</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization</v>
       </c>
       <c r="H98" t="s">
         <v>56</v>
@@ -8226,7 +8229,7 @@
       </c>
       <c r="L98" t="str">
         <f t="shared" si="56"/>
-        <v>!Organization.address-city</v>
+        <v>Organization.address</v>
       </c>
       <c r="M98" t="s">
         <v>56</v>
@@ -8235,30 +8238,30 @@
         <v>56</v>
       </c>
       <c r="Y98" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Z98" s="4" t="str">
-        <f>"GET [base]/"&amp;B98&amp;"?address-city=Ann Arbor"</f>
-        <v>GET [base]/!Organization?address-city=Ann Arbor</v>
+        <f>"GET [base]/"&amp;B98&amp;"?address=Arbor"</f>
+        <v>GET [base]/Organization?address=Arbor</v>
       </c>
       <c r="AA98" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B98&amp; " resources for the city"</f>
-        <v>Fetches a bundle of all !Organization resources for the city</v>
+        <f>"Fetches a bundle of all "&amp;B98&amp; " resources that match the address string"</f>
+        <v>Fetches a bundle of all Organization resources that match the address string</v>
       </c>
       <c r="AB98" t="str">
         <f t="shared" si="57"/>
-        <v>SearchParameter-us-core-!organization-address-city.html</v>
+        <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
     <row r="99" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B99" t="s">
         <v>266</v>
       </c>
       <c r="C99" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D99" t="s">
         <v>70</v>
@@ -8281,7 +8284,7 @@
       </c>
       <c r="L99" t="str">
         <f t="shared" si="56"/>
-        <v>!Organization.adress-state</v>
+        <v>!Organization.address-city</v>
       </c>
       <c r="M99" t="s">
         <v>56</v>
@@ -8290,30 +8293,30 @@
         <v>56</v>
       </c>
       <c r="Y99" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="Z99" s="4" t="str">
-        <f>"GET [base]/"&amp;B99&amp;"?address-state=MI"</f>
-        <v>GET [base]/!Organization?address-state=MI</v>
+        <f>"GET [base]/"&amp;B99&amp;"?address-city=Ann Arbor"</f>
+        <v>GET [base]/!Organization?address-city=Ann Arbor</v>
       </c>
       <c r="AA99" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B99&amp; " resources for the state"</f>
-        <v>Fetches a bundle of all !Organization resources for the state</v>
+        <f>"Fetches a bundle of all "&amp;B99&amp; " resources for the city"</f>
+        <v>Fetches a bundle of all !Organization resources for the city</v>
       </c>
       <c r="AB99" t="str">
         <f t="shared" si="57"/>
-        <v>SearchParameter-us-core-!organization-adress-state.html</v>
+        <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
     <row r="100" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>266</v>
       </c>
       <c r="C100" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D100" t="s">
         <v>70</v>
@@ -8336,7 +8339,7 @@
       </c>
       <c r="L100" t="str">
         <f t="shared" si="56"/>
-        <v>!Organization.address-postalcode</v>
+        <v>!Organization.adress-state</v>
       </c>
       <c r="M100" t="s">
         <v>56</v>
@@ -8345,40 +8348,40 @@
         <v>56</v>
       </c>
       <c r="Y100" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="Z100" s="4" t="str">
-        <f>"GET [base]/"&amp;B100&amp;"?address-postalcode=48104"</f>
-        <v>GET [base]/!Organization?address-postalcode=48104</v>
+        <f>"GET [base]/"&amp;B100&amp;"?address-state=MI"</f>
+        <v>GET [base]/!Organization?address-state=MI</v>
       </c>
       <c r="AA100" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B100&amp; " resources for the ZIP code"</f>
-        <v>Fetches a bundle of all !Organization resources for the ZIP code</v>
+        <f>"Fetches a bundle of all "&amp;B100&amp; " resources for the state"</f>
+        <v>Fetches a bundle of all !Organization resources for the state</v>
       </c>
       <c r="AB100" t="str">
         <f t="shared" si="57"/>
-        <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
+        <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
     <row r="101" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C101" t="s">
-        <v>23</v>
+        <v>253</v>
       </c>
       <c r="D101" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="E101" t="b">
         <v>1</v>
       </c>
       <c r="G101" t="str">
         <f t="shared" si="45"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!organization</v>
       </c>
       <c r="H101" t="s">
         <v>56</v>
@@ -8391,7 +8394,7 @@
       </c>
       <c r="L101" t="str">
         <f t="shared" si="56"/>
-        <v>Practitioner.name</v>
+        <v>!Organization.address-postalcode</v>
       </c>
       <c r="M101" t="s">
         <v>56</v>
@@ -8399,40 +8402,37 @@
       <c r="O101" t="s">
         <v>56</v>
       </c>
-      <c r="Y101" s="4" t="s">
-        <v>268</v>
+      <c r="Y101" t="s">
+        <v>265</v>
       </c>
       <c r="Z101" s="4" t="str">
-        <f>"GET [base]/"&amp;B101&amp;"?name=Smith"</f>
-        <v>GET [base]/Practitioner?name=Smith</v>
+        <f>"GET [base]/"&amp;B101&amp;"?address-postalcode=48104"</f>
+        <v>GET [base]/!Organization?address-postalcode=48104</v>
       </c>
       <c r="AA101" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B101&amp;" resources matching the name"</f>
-        <v>Fetches a bundle of all Practitioner resources matching the name</v>
+        <f>"Fetches a bundle of all "&amp;B101&amp; " resources for the ZIP code"</f>
+        <v>Fetches a bundle of all !Organization resources for the ZIP code</v>
       </c>
       <c r="AB101" t="str">
-        <f t="shared" ref="AB101:AB102" si="59">"SearchParameter-us-core-"&amp;LOWER((B101)&amp;"-"&amp;SUBSTITUTE(C101,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-practitioner-name.html</v>
+        <f t="shared" si="57"/>
+        <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
     <row r="102" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>267</v>
       </c>
       <c r="C102" t="s">
-        <v>77</v>
+        <v>23</v>
       </c>
       <c r="D102" t="s">
         <v>12</v>
       </c>
       <c r="E102" t="b">
         <v>1</v>
-      </c>
-      <c r="F102" s="1" t="s">
-        <v>503</v>
       </c>
       <c r="G102" t="str">
         <f t="shared" si="45"/>
@@ -8445,11 +8445,11 @@
         <v>56</v>
       </c>
       <c r="K102" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="L102" t="str">
         <f t="shared" si="56"/>
-        <v>Practitioner.identifier</v>
+        <v>Practitioner.name</v>
       </c>
       <c r="M102" t="s">
         <v>56</v>
@@ -8458,30 +8458,30 @@
         <v>56</v>
       </c>
       <c r="Y102" s="4" t="s">
-        <v>322</v>
+        <v>268</v>
       </c>
       <c r="Z102" s="4" t="str">
-        <f>"GET [base]/"&amp;B102&amp;"?dentifier=http://hl7.org/fhir/sid/us-npi\|97860456"</f>
-        <v>GET [base]/Practitioner?dentifier=http://hl7.org/fhir/sid/us-npi\|97860456</v>
+        <f>"GET [base]/"&amp;B102&amp;"?name=Smith"</f>
+        <v>GET [base]/Practitioner?name=Smith</v>
       </c>
       <c r="AA102" s="10" t="str">
-        <f>"Fetches a bundle containing any "&amp;B102&amp;" resources matching the identifier"</f>
-        <v>Fetches a bundle containing any Practitioner resources matching the identifier</v>
+        <f>"Fetches a bundle of all "&amp;B102&amp;" resources matching the name"</f>
+        <v>Fetches a bundle of all Practitioner resources matching the name</v>
       </c>
       <c r="AB102" t="str">
-        <f t="shared" si="59"/>
-        <v>SearchParameter-us-core-practitioner-identifier.html</v>
+        <f t="shared" ref="AB102:AB103" si="61">"SearchParameter-us-core-"&amp;LOWER((B102)&amp;"-"&amp;SUBSTITUTE(C102,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
     <row r="103" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C103" t="s">
-        <v>270</v>
+        <v>77</v>
       </c>
       <c r="D103" t="s">
         <v>12</v>
@@ -8494,7 +8494,7 @@
       </c>
       <c r="G103" t="str">
         <f t="shared" si="45"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
       </c>
       <c r="H103" t="s">
         <v>56</v>
@@ -8507,7 +8507,7 @@
       </c>
       <c r="L103" t="str">
         <f t="shared" si="56"/>
-        <v>PractitionerRole.specialty</v>
+        <v>Practitioner.identifier</v>
       </c>
       <c r="M103" t="s">
         <v>56</v>
@@ -8515,34 +8515,31 @@
       <c r="O103" t="s">
         <v>56</v>
       </c>
-      <c r="X103" t="s">
-        <v>273</v>
-      </c>
       <c r="Y103" s="4" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Z103" s="4" t="str">
-        <f>"GET [base]/"&amp;B103&amp;"?specialty=http://nucc.org/provider-taxonomy\|208D0000X"</f>
-        <v>GET [base]/PractitionerRole?specialty=http://nucc.org/provider-taxonomy\|208D0000X</v>
+        <f>"GET [base]/"&amp;B103&amp;"?dentifier=http://hl7.org/fhir/sid/us-npi\|97860456"</f>
+        <v>GET [base]/Practitioner?dentifier=http://hl7.org/fhir/sid/us-npi\|97860456</v>
       </c>
       <c r="AA103" s="10" t="str">
-        <f>"Fetches a bundle containing  "&amp;B103&amp;" resources matching the specialty"</f>
-        <v>Fetches a bundle containing  PractitionerRole resources matching the specialty</v>
+        <f>"Fetches a bundle containing any "&amp;B103&amp;" resources matching the identifier"</f>
+        <v>Fetches a bundle containing any Practitioner resources matching the identifier</v>
       </c>
       <c r="AB103" t="str">
-        <f t="shared" ref="AB103" si="60">"SearchParameter-us-core-"&amp;LOWER((B103)&amp;"-"&amp;SUBSTITUTE(C103,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
+        <f t="shared" si="61"/>
+        <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
     <row r="104" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B104" t="s">
         <v>269</v>
       </c>
       <c r="C104" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D104" t="s">
         <v>12</v>
@@ -8551,7 +8548,7 @@
         <v>1</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="G104" t="str">
         <f t="shared" si="45"/>
@@ -8564,62 +8561,59 @@
         <v>56</v>
       </c>
       <c r="K104" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="L104" t="str">
         <f t="shared" si="56"/>
-        <v>PractitionerRole.practitioner</v>
+        <v>PractitionerRole.specialty</v>
       </c>
       <c r="M104" t="s">
         <v>56</v>
       </c>
       <c r="O104" t="s">
         <v>56</v>
-      </c>
-      <c r="U104" t="s">
-        <v>272</v>
       </c>
       <c r="X104" t="s">
         <v>273</v>
       </c>
       <c r="Y104" s="4" t="s">
-        <v>274</v>
+        <v>323</v>
       </c>
       <c r="Z104" s="4" t="str">
-        <f>_xlfn.CONCAT("GET [base]/",B104,"?practitioner.identifier=http://hl7.org/fhir/sid/us-npi\|97860456&amp;_include=PractitionerRole:practitioner","&amp;_include=PractitionerRole?endpoint~GET [base]/PractitionerRole?practitioner.name=Henry&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint")</f>
-        <v>GET [base]/PractitionerRole?practitioner.identifier=http://hl7.org/fhir/sid/us-npi\|97860456&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint~GET [base]/PractitionerRole?practitioner.name=Henry&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint</v>
+        <f>"GET [base]/"&amp;B104&amp;"?specialty=http://nucc.org/provider-taxonomy\|208D0000X"</f>
+        <v>GET [base]/PractitionerRole?specialty=http://nucc.org/provider-taxonomy\|208D0000X</v>
       </c>
       <c r="AA104" s="10" t="str">
-        <f>"Fetches a bundle containing  "&amp;B104&amp;" resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint."</f>
-        <v>Fetches a bundle containing  PractitionerRole resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint.</v>
+        <f>"Fetches a bundle containing  "&amp;B104&amp;" resources matching the specialty"</f>
+        <v>Fetches a bundle containing  PractitionerRole resources matching the specialty</v>
       </c>
       <c r="AB104" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B104)&amp;"-"&amp;SUBSTITUTE(C104,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
+        <f t="shared" ref="AB104" si="62">"SearchParameter-us-core-"&amp;LOWER((B104)&amp;"-"&amp;SUBSTITUTE(C104,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
     <row r="105" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>49</v>
+        <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>575</v>
+        <v>269</v>
       </c>
       <c r="C105" t="s">
-        <v>62</v>
+        <v>271</v>
       </c>
       <c r="D105" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E105" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="G105" t="str">
         <f t="shared" si="45"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
       </c>
       <c r="H105" t="s">
         <v>56</v>
@@ -8628,50 +8622,61 @@
         <v>56</v>
       </c>
       <c r="K105" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="L105" t="str">
         <f t="shared" si="56"/>
-        <v>ServiceRequest.status</v>
+        <v>PractitionerRole.practitioner</v>
       </c>
       <c r="M105" t="s">
         <v>56</v>
       </c>
-      <c r="N105" t="s">
-        <v>12</v>
-      </c>
       <c r="O105" t="s">
         <v>56</v>
       </c>
-      <c r="Y105" s="4"/>
-      <c r="Z105" s="4"/>
-      <c r="AA105" s="10"/>
+      <c r="U105" t="s">
+        <v>272</v>
+      </c>
+      <c r="X105" t="s">
+        <v>273</v>
+      </c>
+      <c r="Y105" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="Z105" s="4" t="str">
+        <f>_xlfn.CONCAT("GET [base]/",B105,"?practitioner.identifier=http://hl7.org/fhir/sid/us-npi\|97860456&amp;_include=PractitionerRole:practitioner","&amp;_include=PractitionerRole?endpoint~GET [base]/PractitionerRole?practitioner.name=Henry&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint")</f>
+        <v>GET [base]/PractitionerRole?practitioner.identifier=http://hl7.org/fhir/sid/us-npi\|97860456&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint~GET [base]/PractitionerRole?practitioner.name=Henry&amp;_include=PractitionerRole:practitioner&amp;_include=PractitionerRole?endpoint</v>
+      </c>
+      <c r="AA105" s="10" t="str">
+        <f>"Fetches a bundle containing  "&amp;B105&amp;" resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint."</f>
+        <v>Fetches a bundle containing  PractitionerRole resources matching the chained parameter practitioner.name or practitioner.identifier. SHOULD support the _include for PractionerRole.practitioner and PractitionerRole.endpoint.</v>
+      </c>
       <c r="AB105" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B105)&amp;"-"&amp;C105&amp;".html")</f>
-        <v>SearchParameter-us-core-servicerequest-status.html</v>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B105)&amp;"-"&amp;SUBSTITUTE(C105,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
     <row r="106" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>50</v>
+        <v>105</v>
       </c>
       <c r="B106" t="s">
         <v>575</v>
       </c>
       <c r="C106" t="s">
-        <v>90</v>
+        <v>62</v>
       </c>
       <c r="D106" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E106" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="G106" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B106)</f>
+        <f t="shared" si="45"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H106" t="s">
@@ -8681,56 +8686,50 @@
         <v>56</v>
       </c>
       <c r="K106" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="L106" t="str">
         <f t="shared" si="56"/>
-        <v>ServiceRequest.patient</v>
+        <v>ServiceRequest.status</v>
       </c>
       <c r="M106" t="s">
         <v>56</v>
       </c>
+      <c r="N106" t="s">
+        <v>12</v>
+      </c>
       <c r="O106" t="s">
         <v>56</v>
       </c>
-      <c r="Y106" t="str">
-        <f>"support searching for all "&amp;LOWER(B106)&amp;"s for a patient"</f>
-        <v>support searching for all servicerequests for a patient</v>
-      </c>
-      <c r="Z106" s="4" t="str">
-        <f>"GET [base]/"&amp;B106&amp;"?patient=1137192"</f>
-        <v>GET [base]/ServiceRequest?patient=1137192</v>
-      </c>
-      <c r="AA106" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B106&amp; " resources for the specified patient"</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient</v>
-      </c>
+      <c r="Y106" s="4"/>
+      <c r="Z106" s="4"/>
+      <c r="AA106" s="10"/>
       <c r="AB106" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B106)&amp;"-"&amp;C106&amp;".html")</f>
-        <v>SearchParameter-us-core-servicerequest-patient.html</v>
+        <v>SearchParameter-us-core-servicerequest-status.html</v>
       </c>
     </row>
     <row r="107" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="B107" t="s">
         <v>575</v>
       </c>
       <c r="C107" t="s">
-        <v>140</v>
+        <v>90</v>
       </c>
       <c r="D107" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E107" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="G107" t="str">
-        <f t="shared" ref="G107:G125" si="61">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B107)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B107)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H107" t="s">
@@ -8740,11 +8739,11 @@
         <v>56</v>
       </c>
       <c r="K107" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="L107" t="str">
         <f t="shared" si="56"/>
-        <v>ServiceRequest.category</v>
+        <v>ServiceRequest.patient</v>
       </c>
       <c r="M107" t="s">
         <v>56</v>
@@ -8752,23 +8751,32 @@
       <c r="O107" t="s">
         <v>56</v>
       </c>
-      <c r="Y107" s="4"/>
-      <c r="Z107" s="4"/>
-      <c r="AA107" s="10"/>
+      <c r="Y107" t="str">
+        <f>"support searching for all "&amp;LOWER(B107)&amp;"s for a patient"</f>
+        <v>support searching for all servicerequests for a patient</v>
+      </c>
+      <c r="Z107" s="4" t="str">
+        <f>"GET [base]/"&amp;B107&amp;"?patient=1137192"</f>
+        <v>GET [base]/ServiceRequest?patient=1137192</v>
+      </c>
+      <c r="AA107" s="10" t="str">
+        <f>"Fetches a bundle of all "&amp;B107&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient</v>
+      </c>
       <c r="AB107" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B107)&amp;"-"&amp;C107&amp;".html")</f>
-        <v>SearchParameter-us-core-servicerequest-category.html</v>
+        <v>SearchParameter-us-core-servicerequest-patient.html</v>
       </c>
     </row>
     <row r="108" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108">
-        <v>52</v>
+        <v>107</v>
       </c>
       <c r="B108" t="s">
         <v>575</v>
       </c>
       <c r="C108" t="s">
-        <v>26</v>
+        <v>140</v>
       </c>
       <c r="D108" t="s">
         <v>30</v>
@@ -8780,7 +8788,7 @@
         <v>503</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" ref="G108:G126" si="63">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B108)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H108" t="s">
@@ -8794,13 +8802,10 @@
       </c>
       <c r="L108" t="str">
         <f t="shared" si="56"/>
-        <v>ServiceRequest.code</v>
+        <v>ServiceRequest.category</v>
       </c>
       <c r="M108" t="s">
         <v>56</v>
-      </c>
-      <c r="N108" t="s">
-        <v>70</v>
       </c>
       <c r="O108" t="s">
         <v>56</v>
@@ -8810,18 +8815,18 @@
       <c r="AA108" s="10"/>
       <c r="AB108" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B108)&amp;"-"&amp;C108&amp;".html")</f>
-        <v>SearchParameter-us-core-servicerequest-code.html</v>
+        <v>SearchParameter-us-core-servicerequest-category.html</v>
       </c>
     </row>
     <row r="109" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109">
-        <v>53</v>
+        <v>108</v>
       </c>
       <c r="B109" t="s">
         <v>575</v>
       </c>
       <c r="C109" t="s">
-        <v>582</v>
+        <v>26</v>
       </c>
       <c r="D109" t="s">
         <v>30</v>
@@ -8830,10 +8835,10 @@
         <v>0</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H109" t="s">
@@ -8843,48 +8848,50 @@
         <v>56</v>
       </c>
       <c r="K109" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="L109" t="str">
         <f t="shared" si="56"/>
-        <v>ServiceRequest.authored</v>
+        <v>ServiceRequest.code</v>
       </c>
       <c r="M109" t="s">
         <v>56</v>
       </c>
+      <c r="N109" t="s">
+        <v>70</v>
+      </c>
       <c r="O109" t="s">
         <v>56</v>
       </c>
-      <c r="P109" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="S109" t="s">
-        <v>93</v>
-      </c>
+      <c r="Y109" s="4"/>
+      <c r="Z109" s="4"/>
       <c r="AA109" s="10"/>
       <c r="AB109" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B109)&amp;"-"&amp;C109&amp;".html")</f>
-        <v>SearchParameter-us-core-servicerequest-authored.html</v>
+        <v>SearchParameter-us-core-servicerequest-code.html</v>
       </c>
     </row>
     <row r="110" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110">
-        <v>20</v>
+        <v>109</v>
       </c>
       <c r="B110" t="s">
         <v>575</v>
       </c>
       <c r="C110" t="s">
-        <v>55</v>
+        <v>582</v>
       </c>
       <c r="D110" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E110" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>501</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H110" t="s">
@@ -8894,11 +8901,11 @@
         <v>56</v>
       </c>
       <c r="K110" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="L110" t="str">
         <f t="shared" si="56"/>
-        <v>ServiceRequest._id</v>
+        <v>ServiceRequest.authored</v>
       </c>
       <c r="M110" t="s">
         <v>56</v>
@@ -8906,40 +8913,40 @@
       <c r="O110" t="s">
         <v>56</v>
       </c>
-      <c r="Y110" s="4" t="s">
-        <v>580</v>
-      </c>
-      <c r="Z110" s="4" t="s">
-        <v>581</v>
-      </c>
+      <c r="P110" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="S110" t="s">
+        <v>93</v>
+      </c>
+      <c r="AA110" s="10"/>
       <c r="AB110" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B110)&amp;"-"&amp;SUBSTITUTE(C110,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-servicerequest-id.html</v>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B110)&amp;"-"&amp;C110&amp;".html")</f>
+        <v>SearchParameter-us-core-servicerequest-authored.html</v>
       </c>
     </row>
     <row r="111" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111">
-        <v>56</v>
+        <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>180</v>
+        <v>575</v>
       </c>
       <c r="C111" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="D111" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E111" t="b">
-        <v>0</v>
-      </c>
-      <c r="F111" s="1"/>
+        <v>1</v>
+      </c>
       <c r="G111" t="str">
-        <f t="shared" si="61"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
+        <f t="shared" si="63"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H111" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="J111" t="s">
         <v>56</v>
@@ -8949,7 +8956,7 @@
       </c>
       <c r="L111" t="str">
         <f t="shared" si="56"/>
-        <v>Goal.description</v>
+        <v>ServiceRequest._id</v>
       </c>
       <c r="M111" t="s">
         <v>56</v>
@@ -8957,34 +8964,40 @@
       <c r="O111" t="s">
         <v>56</v>
       </c>
-      <c r="AA111" s="10"/>
+      <c r="Y111" s="4" t="s">
+        <v>580</v>
+      </c>
+      <c r="Z111" s="4" t="s">
+        <v>581</v>
+      </c>
       <c r="AB111" t="str">
-        <f t="shared" ref="AB111" si="62">"SearchParameter-us-core-"&amp;LOWER((B111)&amp;"-"&amp;C111&amp;".html")</f>
-        <v>SearchParameter-us-core-goal-description.html</v>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B111)&amp;"-"&amp;SUBSTITUTE(C111,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-servicerequest-id.html</v>
       </c>
     </row>
     <row r="112" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112">
-        <v>20</v>
+        <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>598</v>
+        <v>180</v>
       </c>
       <c r="C112" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="D112" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E112" t="b">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="F112" s="1"/>
       <c r="G112" t="str">
-        <f t="shared" si="61"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
+        <f t="shared" si="63"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="H112" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="J112" t="s">
         <v>56</v>
@@ -8994,47 +9007,38 @@
       </c>
       <c r="L112" t="str">
         <f t="shared" si="56"/>
-        <v>RelatedPerson._id</v>
+        <v>Goal.description</v>
       </c>
       <c r="M112" t="s">
         <v>56</v>
       </c>
       <c r="O112" t="s">
         <v>56</v>
-      </c>
-      <c r="Y112" s="4" t="s">
-        <v>602</v>
-      </c>
-      <c r="Z112" s="4" t="s">
-        <v>603</v>
       </c>
       <c r="AA112" s="10"/>
       <c r="AB112" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B112)&amp;"-"&amp;SUBSTITUTE(C112,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-relatedperson-id.html</v>
+        <f t="shared" ref="AB112" si="64">"SearchParameter-us-core-"&amp;LOWER((B112)&amp;"-"&amp;C112&amp;".html")</f>
+        <v>SearchParameter-us-core-goal-description.html</v>
       </c>
     </row>
     <row r="113" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113">
-        <v>79</v>
+        <v>112</v>
       </c>
       <c r="B113" t="s">
         <v>598</v>
       </c>
       <c r="C113" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="D113" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="E113" t="b">
         <v>1</v>
       </c>
-      <c r="F113" s="1" t="s">
-        <v>500</v>
-      </c>
       <c r="G113" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
       </c>
       <c r="H113" t="s">
@@ -9044,11 +9048,11 @@
         <v>56</v>
       </c>
       <c r="K113" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="L113" t="str">
-        <f>B113&amp;"."&amp;C113</f>
-        <v>RelatedPerson.patient</v>
+        <f t="shared" si="56"/>
+        <v>RelatedPerson._id</v>
       </c>
       <c r="M113" t="s">
         <v>56</v>
@@ -9056,32 +9060,27 @@
       <c r="O113" t="s">
         <v>56</v>
       </c>
-      <c r="Y113" t="str">
-        <f>"support searching for all "&amp;LOWER(B113)&amp;"s for a patient"</f>
-        <v>support searching for all relatedpersons for a patient</v>
-      </c>
-      <c r="Z113" s="4" t="str">
-        <f>"GET [base]/"&amp;B113&amp;"?"&amp;C113&amp;"=1032702"</f>
-        <v>GET [base]/RelatedPerson?patient=1032702</v>
-      </c>
-      <c r="AA113" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B113&amp; " resources for the specified patient"</f>
-        <v>Fetches a bundle of all RelatedPerson resources for the specified patient</v>
-      </c>
+      <c r="Y113" s="4" t="s">
+        <v>602</v>
+      </c>
+      <c r="Z113" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="AA113" s="10"/>
       <c r="AB113" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B113)&amp;"-"&amp;C113&amp;".html")</f>
-        <v>SearchParameter-us-core-relatedperson-patient.html</v>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B113)&amp;"-"&amp;SUBSTITUTE(C113,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-relatedperson-id.html</v>
       </c>
     </row>
     <row r="114" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114">
-        <v>26</v>
+        <v>113</v>
       </c>
       <c r="B114" t="s">
         <v>598</v>
       </c>
       <c r="C114" t="s">
-        <v>23</v>
+        <v>90</v>
       </c>
       <c r="D114" t="s">
         <v>70</v>
@@ -9089,25 +9088,25 @@
       <c r="E114" t="b">
         <v>1</v>
       </c>
+      <c r="F114" s="1" t="s">
+        <v>500</v>
+      </c>
       <c r="G114" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
       </c>
       <c r="H114" t="s">
         <v>56</v>
       </c>
-      <c r="I114" t="s">
-        <v>56</v>
-      </c>
       <c r="J114" t="s">
         <v>56</v>
       </c>
       <c r="K114" t="s">
-        <v>64</v>
+        <v>91</v>
       </c>
       <c r="L114" t="str">
         <f>B114&amp;"."&amp;C114</f>
-        <v>RelatedPerson.name</v>
+        <v>RelatedPerson.patient</v>
       </c>
       <c r="M114" t="s">
         <v>56</v>
@@ -9115,54 +9114,58 @@
       <c r="O114" t="s">
         <v>56</v>
       </c>
-      <c r="Y114" s="4" t="s">
-        <v>717</v>
+      <c r="Y114" t="str">
+        <f>"support searching for all "&amp;LOWER(B114)&amp;"s for a patient"</f>
+        <v>support searching for all relatedpersons for a patient</v>
       </c>
       <c r="Z114" s="4" t="str">
-        <f>"GET [base]/"&amp;B114&amp;"?"&amp;C114&amp;"=Mary Shaw"</f>
-        <v>GET [base]/RelatedPerson?name=Mary Shaw</v>
+        <f>"GET [base]/"&amp;B114&amp;"?"&amp;C114&amp;"=1032702"</f>
+        <v>GET [base]/RelatedPerson?patient=1032702</v>
       </c>
       <c r="AA114" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B114&amp;" resources matching the name"</f>
-        <v>Fetches a bundle of all RelatedPerson resources matching the name</v>
+        <f>"Fetches a bundle of all "&amp;B114&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all RelatedPerson resources for the specified patient</v>
       </c>
       <c r="AB114" t="str">
-        <f t="shared" ref="AB114" si="63">"SearchParameter-us-core-"&amp;LOWER((B114)&amp;"-"&amp;SUBSTITUTE(C114,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-relatedperson-name.html</v>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B114)&amp;"-"&amp;C114&amp;".html")</f>
+        <v>SearchParameter-us-core-relatedperson-patient.html</v>
       </c>
     </row>
     <row r="115" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>626</v>
+        <v>598</v>
       </c>
       <c r="C115" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="D115" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="E115" t="b">
         <v>1</v>
       </c>
       <c r="G115" t="str">
-        <f t="shared" si="61"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <f t="shared" si="63"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
       </c>
       <c r="H115" t="s">
         <v>56</v>
       </c>
+      <c r="I115" t="s">
+        <v>56</v>
+      </c>
       <c r="J115" t="s">
         <v>56</v>
       </c>
       <c r="K115" t="s">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="L115" t="str">
-        <f t="shared" ref="L115:L125" si="64">B115&amp;"."&amp;C115</f>
-        <v>QuestionnaireResponse._id</v>
+        <f>B115&amp;"."&amp;C115</f>
+        <v>RelatedPerson.name</v>
       </c>
       <c r="M115" t="s">
         <v>56</v>
@@ -9170,27 +9173,31 @@
       <c r="O115" t="s">
         <v>56</v>
       </c>
-      <c r="Y115" s="4" t="str">
-        <f>"support fetching a "&amp;B115</f>
-        <v>support fetching a QuestionnaireResponse</v>
-      </c>
-      <c r="Z115" s="4" t="s">
-        <v>643</v>
+      <c r="Y115" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="Z115" s="4" t="str">
+        <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
+        <v>GET [base]/RelatedPerson?name=Mary Shaw</v>
+      </c>
+      <c r="AA115" s="10" t="str">
+        <f>"Fetches a bundle of all "&amp;B115&amp;" resources matching the name"</f>
+        <v>Fetches a bundle of all RelatedPerson resources matching the name</v>
       </c>
       <c r="AB115" t="str">
-        <f t="shared" ref="AB115:AB121" si="65">"SearchParameter-us-core-"&amp;LOWER((B115)&amp;"-"&amp;SUBSTITUTE(C115,"_","")&amp;".html")</f>
-        <v>SearchParameter-us-core-questionnaireresponse-id.html</v>
+        <f t="shared" ref="AB115" si="65">"SearchParameter-us-core-"&amp;LOWER((B115)&amp;"-"&amp;SUBSTITUTE(C115,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-relatedperson-name.html</v>
       </c>
     </row>
     <row r="116" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="B116" t="s">
         <v>626</v>
       </c>
       <c r="C116" t="s">
-        <v>90</v>
+        <v>55</v>
       </c>
       <c r="D116" t="s">
         <v>12</v>
@@ -9198,11 +9205,8 @@
       <c r="E116" t="b">
         <v>1</v>
       </c>
-      <c r="F116" s="1" t="s">
-        <v>500</v>
-      </c>
       <c r="G116" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H116" t="s">
@@ -9212,11 +9216,11 @@
         <v>56</v>
       </c>
       <c r="K116" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="L116" t="str">
-        <f t="shared" si="64"/>
-        <v>QuestionnaireResponse.patient</v>
+        <f t="shared" ref="L116:L126" si="66">B116&amp;"."&amp;C116</f>
+        <v>QuestionnaireResponse._id</v>
       </c>
       <c r="M116" t="s">
         <v>56</v>
@@ -9224,44 +9228,39 @@
       <c r="O116" t="s">
         <v>56</v>
       </c>
-      <c r="Y116" t="str">
-        <f>"support searching for all "&amp;LOWER(B116)&amp;"s for a patient"</f>
-        <v>support searching for all questionnaireresponses for a patient</v>
-      </c>
-      <c r="Z116" s="4" t="str">
-        <f>"GET [base]/"&amp;B116&amp;"?patient=1032702"</f>
-        <v>GET [base]/QuestionnaireResponse?patient=1032702</v>
-      </c>
-      <c r="AA116" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B116&amp; " resources for the specified patient"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient</v>
+      <c r="Y116" s="4" t="str">
+        <f>"support fetching a "&amp;B116</f>
+        <v>support fetching a QuestionnaireResponse</v>
+      </c>
+      <c r="Z116" s="4" t="s">
+        <v>643</v>
       </c>
       <c r="AB116" t="str">
-        <f t="shared" si="65"/>
-        <v>SearchParameter-us-core-questionnaireresponse-patient.html</v>
+        <f t="shared" ref="AB116:AB122" si="67">"SearchParameter-us-core-"&amp;LOWER((B116)&amp;"-"&amp;SUBSTITUTE(C116,"_","")&amp;".html")</f>
+        <v>SearchParameter-us-core-questionnaireresponse-id.html</v>
       </c>
     </row>
     <row r="117" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="B117" t="s">
         <v>626</v>
       </c>
       <c r="C117" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="D117" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E117" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H117" t="s">
@@ -9271,38 +9270,44 @@
         <v>56</v>
       </c>
       <c r="K117" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="L117" t="str">
-        <f t="shared" si="64"/>
-        <v>QuestionnaireResponse.status</v>
+        <f t="shared" si="66"/>
+        <v>QuestionnaireResponse.patient</v>
       </c>
       <c r="M117" t="s">
         <v>56</v>
       </c>
-      <c r="N117" t="s">
-        <v>12</v>
-      </c>
       <c r="O117" t="s">
         <v>56</v>
       </c>
-      <c r="Y117" s="20" t="s">
-        <v>640</v>
+      <c r="Y117" t="str">
+        <f>"support searching for all "&amp;LOWER(B117)&amp;"s for a patient"</f>
+        <v>support searching for all questionnaireresponses for a patient</v>
+      </c>
+      <c r="Z117" s="4" t="str">
+        <f>"GET [base]/"&amp;B117&amp;"?patient=1032702"</f>
+        <v>GET [base]/QuestionnaireResponse?patient=1032702</v>
+      </c>
+      <c r="AA117" s="10" t="str">
+        <f>"Fetches a bundle of all "&amp;B117&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient</v>
       </c>
       <c r="AB117" t="str">
-        <f t="shared" si="65"/>
-        <v>SearchParameter-us-core-questionnaireresponse-status.html</v>
+        <f t="shared" si="67"/>
+        <v>SearchParameter-us-core-questionnaireresponse-patient.html</v>
       </c>
     </row>
     <row r="118" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="B118" t="s">
         <v>626</v>
       </c>
       <c r="C118" t="s">
-        <v>636</v>
+        <v>62</v>
       </c>
       <c r="D118" t="s">
         <v>30</v>
@@ -9314,7 +9319,7 @@
         <v>503</v>
       </c>
       <c r="G118" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H118" t="s">
@@ -9326,32 +9331,36 @@
       <c r="K118" t="s">
         <v>57</v>
       </c>
-      <c r="L118" t="s">
-        <v>638</v>
+      <c r="L118" t="str">
+        <f t="shared" si="66"/>
+        <v>QuestionnaireResponse.status</v>
       </c>
       <c r="M118" t="s">
         <v>56</v>
       </c>
+      <c r="N118" t="s">
+        <v>12</v>
+      </c>
       <c r="O118" t="s">
         <v>56</v>
       </c>
       <c r="Y118" s="20" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="AB118" t="str">
-        <f t="shared" si="65"/>
-        <v>SearchParameter-us-core-questionnaireresponse-tag.html</v>
+        <f t="shared" si="67"/>
+        <v>SearchParameter-us-core-questionnaireresponse-status.html</v>
       </c>
     </row>
     <row r="119" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="B119" t="s">
         <v>626</v>
       </c>
       <c r="C119" t="s">
-        <v>582</v>
+        <v>636</v>
       </c>
       <c r="D119" t="s">
         <v>30</v>
@@ -9360,10 +9369,10 @@
         <v>0</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H119" t="s">
@@ -9373,11 +9382,10 @@
         <v>56</v>
       </c>
       <c r="K119" t="s">
-        <v>79</v>
-      </c>
-      <c r="L119" t="str">
-        <f t="shared" si="64"/>
-        <v>QuestionnaireResponse.authored</v>
+        <v>57</v>
+      </c>
+      <c r="L119" t="s">
+        <v>638</v>
       </c>
       <c r="M119" t="s">
         <v>56</v>
@@ -9385,29 +9393,23 @@
       <c r="O119" t="s">
         <v>56</v>
       </c>
-      <c r="P119" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="S119" t="s">
-        <v>93</v>
-      </c>
       <c r="Y119" s="20" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="AB119" t="str">
-        <f t="shared" si="65"/>
-        <v>SearchParameter-us-core-questionnaireresponse-authored.html</v>
+        <f t="shared" si="67"/>
+        <v>SearchParameter-us-core-questionnaireresponse-tag.html</v>
       </c>
     </row>
     <row r="120" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="B120" t="s">
         <v>626</v>
       </c>
       <c r="C120" t="s">
-        <v>637</v>
+        <v>582</v>
       </c>
       <c r="D120" t="s">
         <v>30</v>
@@ -9416,10 +9418,10 @@
         <v>0</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H120" t="s">
@@ -9429,11 +9431,11 @@
         <v>56</v>
       </c>
       <c r="K120" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="L120" t="str">
-        <f t="shared" si="64"/>
-        <v>QuestionnaireResponse.questionnaire</v>
+        <f t="shared" si="66"/>
+        <v>QuestionnaireResponse.authored</v>
       </c>
       <c r="M120" t="s">
         <v>56</v>
@@ -9441,41 +9443,44 @@
       <c r="O120" t="s">
         <v>56</v>
       </c>
+      <c r="P120" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="S120" t="s">
+        <v>93</v>
+      </c>
       <c r="Y120" s="20" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="AB120" t="str">
-        <f t="shared" si="65"/>
-        <v>SearchParameter-us-core-questionnaireresponse-questionnaire.html</v>
+        <f t="shared" si="67"/>
+        <v>SearchParameter-us-core-questionnaireresponse-authored.html</v>
       </c>
     </row>
     <row r="121" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>675</v>
+        <v>626</v>
       </c>
       <c r="C121" t="s">
-        <v>90</v>
+        <v>637</v>
       </c>
       <c r="D121" t="s">
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="E121" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F121" s="1" t="s">
         <v>500</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="61"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-coverage</v>
+        <f t="shared" si="63"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H121" t="s">
-        <v>56</v>
-      </c>
-      <c r="I121" t="s">
         <v>56</v>
       </c>
       <c r="J121" t="s">
@@ -9485,8 +9490,8 @@
         <v>91</v>
       </c>
       <c r="L121" t="str">
-        <f t="shared" si="64"/>
-        <v>Coverage.patient</v>
+        <f t="shared" si="66"/>
+        <v>QuestionnaireResponse.questionnaire</v>
       </c>
       <c r="M121" t="s">
         <v>56</v>
@@ -9494,44 +9499,36 @@
       <c r="O121" t="s">
         <v>56</v>
       </c>
-      <c r="Y121" t="s">
-        <v>677</v>
-      </c>
-      <c r="Z121" s="4" t="str">
-        <f>"GET [base]/"&amp;B121&amp;"?patient=1137192"</f>
-        <v>GET [base]/Coverage?patient=1137192</v>
-      </c>
-      <c r="AA121" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B121&amp; " resources for the specified patient"</f>
-        <v>Fetches a bundle of all Coverage resources for the specified patient</v>
+      <c r="Y121" s="20" t="s">
+        <v>642</v>
       </c>
       <c r="AB121" t="str">
-        <f t="shared" si="65"/>
-        <v>SearchParameter-us-core-coverage-patient.html</v>
+        <f t="shared" si="67"/>
+        <v>SearchParameter-us-core-questionnaireresponse-questionnaire.html</v>
       </c>
     </row>
     <row r="122" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>691</v>
+        <v>674</v>
       </c>
       <c r="C122" t="s">
-        <v>62</v>
+        <v>90</v>
       </c>
       <c r="D122" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="E122" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="61"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+        <f t="shared" si="63"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-coverage</v>
       </c>
       <c r="H122" t="s">
         <v>56</v>
@@ -9543,38 +9540,43 @@
         <v>56</v>
       </c>
       <c r="K122" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="L122" t="str">
-        <f t="shared" si="64"/>
-        <v>MedicationDispense.status</v>
+        <f t="shared" si="66"/>
+        <v>Coverage.patient</v>
       </c>
       <c r="M122" t="s">
         <v>56</v>
       </c>
-      <c r="N122" t="s">
-        <v>12</v>
-      </c>
       <c r="O122" t="s">
         <v>56</v>
       </c>
-      <c r="Y122" s="4"/>
-      <c r="Z122" s="4"/>
-      <c r="AA122" s="10"/>
+      <c r="Y122" t="s">
+        <v>676</v>
+      </c>
+      <c r="Z122" s="4" t="str">
+        <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
+        <v>GET [base]/Coverage?patient=1137192</v>
+      </c>
+      <c r="AA122" s="10" t="str">
+        <f>"Fetches a bundle of all "&amp;B122&amp; " resources for the specified patient"</f>
+        <v>Fetches a bundle of all Coverage resources for the specified patient</v>
+      </c>
       <c r="AB122" t="str">
-        <f t="shared" ref="AB122:AB125" si="66">"SearchParameter-us-core-"&amp;LOWER((B122)&amp;"-"&amp;C122&amp;".html")</f>
-        <v>SearchParameter-us-core-medicationdispense-status.html</v>
+        <f t="shared" si="67"/>
+        <v>SearchParameter-us-core-coverage-patient.html</v>
       </c>
     </row>
     <row r="123" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C123" t="s">
-        <v>13</v>
+        <v>62</v>
       </c>
       <c r="D123" t="s">
         <v>30</v>
@@ -9586,7 +9588,7 @@
         <v>503</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="61"/>
+        <f t="shared" si="63"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="H123" t="s">
@@ -9602,8 +9604,8 @@
         <v>57</v>
       </c>
       <c r="L123" t="str">
-        <f t="shared" si="64"/>
-        <v>MedicationDispense.type</v>
+        <f t="shared" si="66"/>
+        <v>MedicationDispense.status</v>
       </c>
       <c r="M123" t="s">
         <v>56</v>
@@ -9618,129 +9620,185 @@
       <c r="Z123" s="4"/>
       <c r="AA123" s="10"/>
       <c r="AB123" t="str">
+        <f t="shared" ref="AB123:AB126" si="68">"SearchParameter-us-core-"&amp;LOWER((B123)&amp;"-"&amp;C123&amp;".html")</f>
+        <v>SearchParameter-us-core-medicationdispense-status.html</v>
+      </c>
+    </row>
+    <row r="124" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124">
+        <v>123</v>
+      </c>
+      <c r="B124" t="s">
+        <v>690</v>
+      </c>
+      <c r="C124" t="s">
+        <v>13</v>
+      </c>
+      <c r="D124" t="s">
+        <v>30</v>
+      </c>
+      <c r="E124" t="b">
+        <v>0</v>
+      </c>
+      <c r="F124" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="G124" t="str">
+        <f t="shared" si="63"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+      </c>
+      <c r="H124" t="s">
+        <v>56</v>
+      </c>
+      <c r="I124" t="s">
+        <v>56</v>
+      </c>
+      <c r="J124" t="s">
+        <v>56</v>
+      </c>
+      <c r="K124" t="s">
+        <v>57</v>
+      </c>
+      <c r="L124" t="str">
         <f t="shared" si="66"/>
+        <v>MedicationDispense.type</v>
+      </c>
+      <c r="M124" t="s">
+        <v>56</v>
+      </c>
+      <c r="N124" t="s">
+        <v>12</v>
+      </c>
+      <c r="O124" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y124" s="4"/>
+      <c r="Z124" s="4"/>
+      <c r="AA124" s="10"/>
+      <c r="AB124" t="str">
+        <f t="shared" si="68"/>
         <v>SearchParameter-us-core-medicationdispense-type.html</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A124">
-        <v>89</v>
-      </c>
-      <c r="B124" t="s">
+    <row r="125" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A125">
+        <v>124</v>
+      </c>
+      <c r="B125" t="s">
+        <v>690</v>
+      </c>
+      <c r="C125" t="s">
+        <v>90</v>
+      </c>
+      <c r="D125" t="s">
+        <v>12</v>
+      </c>
+      <c r="E125" t="b">
+        <v>1</v>
+      </c>
+      <c r="F125" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="G125" t="str">
+        <f t="shared" si="63"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+      </c>
+      <c r="H125" t="s">
+        <v>56</v>
+      </c>
+      <c r="I125" t="s">
+        <v>56</v>
+      </c>
+      <c r="J125" t="s">
+        <v>56</v>
+      </c>
+      <c r="K125" t="s">
+        <v>91</v>
+      </c>
+      <c r="L125" t="str">
+        <f t="shared" si="66"/>
+        <v>MedicationDispense.patient</v>
+      </c>
+      <c r="M125" t="s">
+        <v>56</v>
+      </c>
+      <c r="O125" t="s">
+        <v>56</v>
+      </c>
+      <c r="X125" s="6" t="s">
         <v>691</v>
       </c>
-      <c r="C124" t="s">
-        <v>90</v>
-      </c>
-      <c r="D124" t="s">
-        <v>12</v>
-      </c>
-      <c r="E124" t="b">
-        <v>1</v>
-      </c>
-      <c r="F124" s="1" t="s">
-        <v>500</v>
-      </c>
-      <c r="G124" t="str">
-        <f t="shared" si="61"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
-      </c>
-      <c r="H124" t="s">
-        <v>56</v>
-      </c>
-      <c r="I124" t="s">
-        <v>56</v>
-      </c>
-      <c r="J124" t="s">
-        <v>56</v>
-      </c>
-      <c r="K124" t="s">
-        <v>91</v>
-      </c>
-      <c r="L124" t="str">
-        <f t="shared" si="64"/>
-        <v>MedicationDispense.patient</v>
-      </c>
-      <c r="M124" t="s">
-        <v>56</v>
-      </c>
-      <c r="O124" t="s">
-        <v>56</v>
-      </c>
-      <c r="X124" s="6" t="s">
-        <v>692</v>
-      </c>
-      <c r="Z124" s="10" t="s">
-        <v>700</v>
-      </c>
-      <c r="AA124" s="10" t="str">
-        <f>"Fetches a bundle of all "&amp;B124&amp; " resources for the specified patient."</f>
+      <c r="Z125" s="10" t="s">
+        <v>699</v>
+      </c>
+      <c r="AA125" s="10" t="str">
+        <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient.</v>
       </c>
-      <c r="AB124" t="str">
+      <c r="AB125" t="str">
+        <f t="shared" si="68"/>
+        <v>SearchParameter-us-core-medicationdispense-patient.html</v>
+      </c>
+    </row>
+    <row r="126" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A126">
+        <v>125</v>
+      </c>
+      <c r="B126" t="s">
+        <v>697</v>
+      </c>
+      <c r="C126" t="s">
+        <v>698</v>
+      </c>
+      <c r="D126" t="s">
+        <v>30</v>
+      </c>
+      <c r="E126" t="b">
+        <v>0</v>
+      </c>
+      <c r="F126" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="G126" t="str">
+        <f t="shared" si="63"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
+      </c>
+      <c r="H126" t="s">
+        <v>56</v>
+      </c>
+      <c r="I126" t="s">
+        <v>56</v>
+      </c>
+      <c r="J126" t="s">
+        <v>56</v>
+      </c>
+      <c r="K126" t="s">
+        <v>79</v>
+      </c>
+      <c r="L126" t="str">
         <f t="shared" si="66"/>
-        <v>SearchParameter-us-core-medicationdispense-patient.html</v>
-      </c>
-    </row>
-    <row r="125" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A125">
-        <v>61</v>
-      </c>
-      <c r="B125" t="s">
-        <v>698</v>
-      </c>
-      <c r="C125" t="s">
-        <v>699</v>
-      </c>
-      <c r="D125" t="s">
-        <v>30</v>
-      </c>
-      <c r="E125" t="b">
-        <v>0</v>
-      </c>
-      <c r="F125" s="1" t="s">
-        <v>501</v>
-      </c>
-      <c r="G125" t="str">
-        <f t="shared" si="61"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
-      </c>
-      <c r="H125" t="s">
-        <v>56</v>
-      </c>
-      <c r="I125" t="s">
-        <v>56</v>
-      </c>
-      <c r="J125" t="s">
-        <v>56</v>
-      </c>
-      <c r="K125" t="s">
-        <v>79</v>
-      </c>
-      <c r="L125" t="str">
-        <f t="shared" si="64"/>
         <v>!MedicationDispense.whenHandedOver</v>
       </c>
-      <c r="M125" t="s">
-        <v>56</v>
-      </c>
-      <c r="O125" t="s">
-        <v>56</v>
-      </c>
-      <c r="P125" t="s">
-        <v>70</v>
-      </c>
-      <c r="S125" t="s">
+      <c r="M126" t="s">
+        <v>56</v>
+      </c>
+      <c r="O126" t="s">
+        <v>56</v>
+      </c>
+      <c r="P126" t="s">
+        <v>70</v>
+      </c>
+      <c r="S126" t="s">
         <v>93</v>
       </c>
-      <c r="AA125" s="10"/>
-      <c r="AB125" t="str">
-        <f t="shared" si="66"/>
+      <c r="AA126" s="10"/>
+      <c r="AB126" t="str">
+        <f t="shared" si="68"/>
         <v>SearchParameter-us-core-!medicationdispense-whenhandedover.html</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB120" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
+  <autoFilter ref="A1:AB126" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA38">
     <sortCondition ref="B1"/>
   </sortState>
@@ -9752,13 +9810,13 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K106"/>
+  <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="J37" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C77" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J69" sqref="J69"/>
+      <selection pane="bottomRight" activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -10209,7 +10267,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -10240,7 +10298,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
         <v>157</v>
@@ -10266,7 +10324,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
@@ -10297,7 +10355,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
@@ -10328,7 +10386,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B21" t="s">
         <v>157</v>
@@ -10619,7 +10677,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>21</v>
@@ -10629,7 +10687,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="F32" t="s">
         <v>70</v>
@@ -10638,10 +10696,10 @@
         <v>134</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" ref="K32" si="7">"Fetches a bundle of all "&amp;B32&amp;" resources matching the specified "&amp;SUBSTITUTE(D32,","," and ")</f>
@@ -10650,7 +10708,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B33" t="s">
         <v>21</v>
@@ -10681,7 +10739,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>21</v>
@@ -10712,7 +10770,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>21</v>
@@ -10743,7 +10801,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B36" t="s">
         <v>138</v>
@@ -10776,7 +10834,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>138</v>
@@ -10828,7 +10886,7 @@
         <v>150</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>556</v>
@@ -10896,7 +10954,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>138</v>
@@ -10926,7 +10984,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>138</v>
@@ -10956,7 +11014,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B43" t="s">
         <v>138</v>
@@ -10986,7 +11044,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>20</v>
@@ -11016,7 +11074,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>161</v>
@@ -11047,7 +11105,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B46" t="s">
         <v>161</v>
@@ -11078,7 +11136,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>179</v>
@@ -11108,7 +11166,7 @@
     </row>
     <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>179</v>
@@ -11141,7 +11199,7 @@
     </row>
     <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>179</v>
@@ -11171,7 +11229,7 @@
     </row>
     <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>179</v>
@@ -11204,7 +11262,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>179</v>
@@ -11234,7 +11292,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B52" t="s">
         <v>179</v>
@@ -11264,7 +11322,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>179</v>
@@ -11294,7 +11352,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>179</v>
@@ -11324,7 +11382,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>179</v>
@@ -11354,7 +11412,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B56" t="s">
         <v>179</v>
@@ -11384,7 +11442,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>180</v>
@@ -11415,7 +11473,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>180</v>
@@ -11446,7 +11504,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B59" t="s">
         <v>181</v>
@@ -11479,7 +11537,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B60" t="s">
         <v>181</v>
@@ -11512,7 +11570,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B61" t="s">
         <v>181</v>
@@ -11545,7 +11603,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B62" t="s">
         <v>181</v>
@@ -11578,7 +11636,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>435</v>
@@ -11608,9 +11666,8 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A64" t="e">
-        <f>SUBTOTAL(9,#REF!)</f>
-        <v>#REF!</v>
+      <c r="A64">
+        <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>435</v>
@@ -11640,7 +11697,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>182</v>
@@ -11671,7 +11728,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>182</v>
@@ -11702,7 +11759,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>182</v>
@@ -11733,7 +11790,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>183</v>
@@ -11765,7 +11822,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="B69" t="s">
         <v>183</v>
@@ -11798,7 +11855,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="B70" t="s">
         <v>183</v>
@@ -11828,7 +11885,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="B71" t="s">
         <v>183</v>
@@ -11861,7 +11918,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="B72" t="s">
         <v>183</v>
@@ -11891,7 +11948,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="B73" t="s">
         <v>320</v>
@@ -11921,7 +11978,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>88</v>
+        <v>73</v>
       </c>
       <c r="B74" t="s">
         <v>234</v>
@@ -11954,7 +12011,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>89</v>
+        <v>74</v>
       </c>
       <c r="B75" t="s">
         <v>234</v>
@@ -11986,7 +12043,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B76" t="s">
         <v>234</v>
@@ -12018,7 +12075,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B77" t="s">
         <v>234</v>
@@ -12049,8 +12106,8 @@
       </c>
     </row>
     <row r="78" spans="1:11" ht="136" x14ac:dyDescent="0.2">
-      <c r="A78" t="s">
-        <v>644</v>
+      <c r="A78">
+        <v>77</v>
       </c>
       <c r="B78" t="s">
         <v>248</v>
@@ -12083,7 +12140,7 @@
     </row>
     <row r="79" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>97</v>
+        <v>78</v>
       </c>
       <c r="B79" t="s">
         <v>183</v>
@@ -12116,7 +12173,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>183</v>
@@ -12149,7 +12206,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="B81" t="s">
         <v>183</v>
@@ -12182,7 +12239,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="B82" t="s">
         <v>183</v>
@@ -12215,7 +12272,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="B83" t="s">
         <v>183</v>
@@ -12248,7 +12305,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="B84" t="s">
         <v>183</v>
@@ -12278,7 +12335,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>107</v>
+        <v>84</v>
       </c>
       <c r="B85" t="s">
         <v>178</v>
@@ -12309,7 +12366,7 @@
     </row>
     <row r="86" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>108</v>
+        <v>85</v>
       </c>
       <c r="B86" t="s">
         <v>290</v>
@@ -12338,7 +12395,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
-        <v>109</v>
+        <v>86</v>
       </c>
       <c r="B87" t="s">
         <v>178</v>
@@ -12371,7 +12428,7 @@
     </row>
     <row r="88" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88">
-        <v>110</v>
+        <v>87</v>
       </c>
       <c r="B88" t="s">
         <v>178</v>
@@ -12404,7 +12461,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
-        <v>111</v>
+        <v>88</v>
       </c>
       <c r="B89" t="s">
         <v>178</v>
@@ -12434,7 +12491,7 @@
     </row>
     <row r="90" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90">
-        <v>112</v>
+        <v>89</v>
       </c>
       <c r="B90" t="s">
         <v>178</v>
@@ -12465,7 +12522,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
-        <v>115</v>
+        <v>90</v>
       </c>
       <c r="B91" t="s">
         <v>249</v>
@@ -12494,17 +12551,16 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>249</v>
+      </c>
+      <c r="C92" t="s">
+        <v>429</v>
+      </c>
+      <c r="D92" t="s">
         <v>116</v>
-      </c>
-      <c r="B92" t="s">
-        <v>248</v>
-      </c>
-      <c r="C92" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B92)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
-      </c>
-      <c r="D92" t="s">
-        <v>567</v>
       </c>
       <c r="F92" t="s">
         <v>70</v>
@@ -12513,28 +12569,28 @@
         <v>106</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>568</v>
+        <v>717</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>569</v>
+        <v>718</v>
       </c>
       <c r="K92" s="4" t="s">
-        <v>570</v>
+        <v>719</v>
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>575</v>
+        <v>248</v>
       </c>
       <c r="C93" t="str">
-        <f t="shared" ref="C93:C106" si="12">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B93)</f>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B93)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D93" t="s">
-        <v>116</v>
+        <v>567</v>
       </c>
       <c r="F93" t="s">
         <v>70</v>
@@ -12543,50 +12599,49 @@
         <v>106</v>
       </c>
       <c r="I93" s="4" t="s">
-        <v>303</v>
+        <v>568</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>577</v>
-      </c>
-      <c r="K93" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
+        <v>569</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>570</v>
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94">
-        <v>118</v>
+        <v>93</v>
       </c>
       <c r="B94" t="s">
         <v>575</v>
       </c>
       <c r="C94" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="C94:C107" si="12">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B94)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D94" t="s">
-        <v>145</v>
+        <v>116</v>
       </c>
       <c r="F94" t="s">
-        <v>12</v>
+        <v>70</v>
       </c>
       <c r="G94" t="s">
         <v>106</v>
       </c>
       <c r="I94" s="4" t="s">
-        <v>198</v>
+        <v>303</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="K94" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient and  a category code"</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
+        <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified "&amp;SUBSTITUTE(D94,","," and ")</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="B95" t="s">
         <v>575</v>
@@ -12596,7 +12651,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D95" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F95" t="s">
         <v>12</v>
@@ -12605,19 +12660,19 @@
         <v>106</v>
       </c>
       <c r="I95" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>587</v>
+        <v>579</v>
       </c>
       <c r="K95" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
+        <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and  a category code"</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="B96" t="s">
         <v>575</v>
@@ -12627,28 +12682,28 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D96" t="s">
-        <v>583</v>
+        <v>147</v>
       </c>
       <c r="F96" t="s">
         <v>12</v>
       </c>
       <c r="G96" t="s">
-        <v>218</v>
+        <v>106</v>
       </c>
       <c r="I96" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>578</v>
+        <v>587</v>
       </c>
       <c r="K96" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and date and a category code"</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
+        <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="B97" t="s">
         <v>575</v>
@@ -12658,69 +12713,69 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D97" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F97" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="G97" t="s">
         <v>218</v>
       </c>
       <c r="I97" s="4" t="s">
-        <v>576</v>
+        <v>201</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="K97" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
-        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
+        <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient and date and a category code"</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98">
-        <v>122</v>
+        <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>180</v>
+        <v>575</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="12"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D98" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="F98" t="s">
         <v>70</v>
       </c>
       <c r="G98" t="s">
-        <v>106</v>
+        <v>218</v>
       </c>
       <c r="I98" s="4" t="s">
-        <v>589</v>
+        <v>576</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
       <c r="K98" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified "&amp;SUBSTITUTE(D98,","," and ")</f>
-        <v>Fetches a bundle of all Goal resources for the specified patient and description</v>
+        <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99">
-        <v>123</v>
+        <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>626</v>
+        <v>180</v>
       </c>
       <c r="C99" t="str">
         <f t="shared" si="12"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D99" t="s">
-        <v>116</v>
+        <v>588</v>
       </c>
       <c r="F99" t="s">
         <v>70</v>
@@ -12728,20 +12783,20 @@
       <c r="G99" t="s">
         <v>106</v>
       </c>
-      <c r="I99" t="s">
-        <v>650</v>
+      <c r="I99" s="4" t="s">
+        <v>589</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>651</v>
+        <v>590</v>
       </c>
       <c r="K99" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified "&amp;SUBSTITUTE(D99,","," and ")</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and status</v>
+        <v>Fetches a bundle of all Goal resources for the specified patient and description</v>
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100">
-        <v>124</v>
+        <v>99</v>
       </c>
       <c r="B100" t="s">
         <v>626</v>
@@ -12751,7 +12806,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D100" t="s">
-        <v>645</v>
+        <v>116</v>
       </c>
       <c r="F100" t="s">
         <v>70</v>
@@ -12759,23 +12814,20 @@
       <c r="G100" t="s">
         <v>106</v>
       </c>
-      <c r="H100" t="s">
+      <c r="I100" t="s">
         <v>649</v>
       </c>
-      <c r="I100" t="s">
+      <c r="J100" s="4" t="s">
         <v>650</v>
       </c>
-      <c r="J100" s="4" t="s">
-        <v>652</v>
-      </c>
-      <c r="K100" t="str">
-        <f>"Fetches a bundle of all "&amp;B100&amp;" resources for the specified "&amp;SUBSTITUTE(D100,","," and  ") &amp; "= 'sdoh'"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
+      <c r="K100" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B100&amp;" resources for the specified "&amp;SUBSTITUTE(D100,","," and ")</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and status</v>
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101">
-        <v>125</v>
+        <v>100</v>
       </c>
       <c r="B101" t="s">
         <v>626</v>
@@ -12785,28 +12837,31 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D101" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="F101" t="s">
         <v>70</v>
       </c>
       <c r="G101" t="s">
-        <v>149</v>
+        <v>106</v>
+      </c>
+      <c r="H101" t="s">
+        <v>648</v>
       </c>
       <c r="I101" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J101" s="4" t="s">
-        <v>653</v>
-      </c>
-      <c r="K101" s="4" t="str">
-        <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient and date"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and date</v>
+        <v>651</v>
+      </c>
+      <c r="K101" t="str">
+        <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified "&amp;SUBSTITUTE(D101,","," and  ") &amp; "= 'sdoh'"</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102">
-        <v>126</v>
+        <v>101</v>
       </c>
       <c r="B102" t="s">
         <v>626</v>
@@ -12815,32 +12870,29 @@
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
-      <c r="D102" s="18" t="s">
-        <v>647</v>
+      <c r="D102" t="s">
+        <v>645</v>
       </c>
       <c r="F102" t="s">
         <v>70</v>
       </c>
       <c r="G102" t="s">
-        <v>218</v>
-      </c>
-      <c r="H102" t="s">
+        <v>149</v>
+      </c>
+      <c r="I102" t="s">
         <v>649</v>
       </c>
-      <c r="I102" t="s">
-        <v>650</v>
-      </c>
       <c r="J102" s="4" t="s">
-        <v>654</v>
-      </c>
-      <c r="K102" t="str">
-        <f>"Fetches a bundle of all "&amp;B102&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
+        <v>652</v>
+      </c>
+      <c r="K102" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B102&amp;" resources for the specified patient and date"</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and date</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103">
-        <v>127</v>
+        <v>102</v>
       </c>
       <c r="B103" t="s">
         <v>626</v>
@@ -12850,73 +12902,72 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D103" s="18" t="s">
+        <v>646</v>
+      </c>
+      <c r="F103" t="s">
+        <v>70</v>
+      </c>
+      <c r="G103" t="s">
+        <v>218</v>
+      </c>
+      <c r="H103" t="s">
         <v>648</v>
       </c>
-      <c r="F103" t="s">
-        <v>70</v>
-      </c>
-      <c r="G103" t="s">
-        <v>91</v>
-      </c>
       <c r="I103" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="J103" s="4" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="K103" t="str">
-        <f>"Fetches a bundle of all "&amp;B103&amp;" resources for the specified patient that have been completed against a specified form."</f>
-        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B103&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104">
-        <v>129</v>
-      </c>
-      <c r="B104" s="18" t="s">
-        <v>691</v>
+        <v>103</v>
+      </c>
+      <c r="B104" t="s">
+        <v>626</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="12"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>116</v>
-      </c>
-      <c r="E104" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="F104" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="G104" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="H104" s="18"/>
-      <c r="I104" s="4" t="s">
-        <v>702</v>
+        <v>647</v>
+      </c>
+      <c r="F104" t="s">
+        <v>70</v>
+      </c>
+      <c r="G104" t="s">
+        <v>91</v>
+      </c>
+      <c r="I104" t="s">
+        <v>649</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>701</v>
+        <v>654</v>
       </c>
       <c r="K104" t="str">
-        <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
-        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed)).</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
+        <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient that have been completed against a specified form."</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105">
-        <v>129</v>
+        <v>104</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E105" s="18" t="s">
         <v>56</v>
@@ -12929,29 +12980,29 @@
       </c>
       <c r="H105" s="18"/>
       <c r="I105" s="4" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="J105" s="4" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="K105" t="str">
-        <f>"Fetches a bundle of all "&amp;B105&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
-        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed).</v>
+        <f>"Fetches a bundle of all "&amp;B105&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed)).</v>
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106">
-        <v>130</v>
+        <v>105</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>698</v>
+        <v>690</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="12"/>
-        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>696</v>
+        <v>117</v>
       </c>
       <c r="E106" s="18" t="s">
         <v>56</v>
@@ -12960,23 +13011,58 @@
         <v>70</v>
       </c>
       <c r="G106" s="18" t="s">
-        <v>149</v>
+        <v>106</v>
       </c>
       <c r="H106" s="18"/>
       <c r="I106" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="J106" s="4" t="s">
+        <v>703</v>
+      </c>
+      <c r="K106" t="str">
+        <f>"Fetches a bundle of all "&amp;B106&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed).</v>
+      </c>
+    </row>
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A107">
+        <v>106</v>
+      </c>
+      <c r="B107" s="18" t="s">
         <v>697</v>
       </c>
-      <c r="J106" s="4" t="s">
+      <c r="C107" t="str">
+        <f t="shared" si="12"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
+      </c>
+      <c r="D107" s="18" t="s">
         <v>695</v>
       </c>
-      <c r="K106" t="str">
-        <f>"Fetches a bundle of all "&amp;B105&amp;" resources for the specified patient for a given dispense and date or range"</f>
+      <c r="E107" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="F107" s="18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G107" s="18" t="s">
+        <v>149</v>
+      </c>
+      <c r="H107" s="18"/>
+      <c r="I107" s="4" t="s">
+        <v>696</v>
+      </c>
+      <c r="J107" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="K107" t="str">
+        <f>"Fetches a bundle of all "&amp;B106&amp;" resources for the specified patient for a given dispense and date or range"</f>
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient for a given dispense and date or range</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K97" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K134">
+  <autoFilter ref="A1:K107" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K135">
     <sortCondition ref="A1"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13020,7 +13106,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13036,7 +13122,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -13052,7 +13138,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13299,7 +13385,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B5" t="s">
         <v>614</v>
@@ -13313,7 +13399,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="B6" t="s">
         <v>620</v>
@@ -13327,16 +13413,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>672</v>
+      </c>
+      <c r="B7" t="s">
         <v>673</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>674</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13397,7 +13483,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="B12" t="s">
         <v>365</v>
@@ -13565,16 +13651,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>688</v>
+      </c>
+      <c r="B24" t="s">
         <v>689</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
         <v>690</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>691</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13593,10 +13679,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B26" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -13607,10 +13693,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B27" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -13621,10 +13707,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="B28" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -13876,7 +13962,7 @@
         <v>495</v>
       </c>
       <c r="B46" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -14041,16 +14127,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
+        <v>683</v>
+      </c>
+      <c r="B58" t="s">
         <v>684</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
         <v>685</v>
-      </c>
-      <c r="D58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" t="s">
-        <v>686</v>
       </c>
     </row>
   </sheetData>
@@ -14221,7 +14307,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="T4" t="s">
         <v>19</v>
@@ -14250,7 +14336,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="T5" t="s">
         <v>19</v>
@@ -14267,7 +14353,7 @@
     </row>
     <row r="6" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -14293,7 +14379,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="T7" t="s">
         <v>19</v>
@@ -14337,7 +14423,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14360,7 +14446,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="T10" t="s">
         <v>19</v>
@@ -14403,7 +14489,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="T12" t="s">
         <v>19</v>
@@ -14487,13 +14573,13 @@
     </row>
     <row r="16" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="T16" t="s">
         <v>19</v>
@@ -14505,7 +14591,7 @@
         <v>70</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="X16" s="15" t="s">
         <v>449</v>
@@ -14551,7 +14637,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="T18" t="s">
         <v>19</v>
@@ -14574,7 +14660,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="T19" t="s">
         <v>19</v>
@@ -14593,7 +14679,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="T20" t="s">
         <v>19</v>
@@ -14657,7 +14743,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="T23" t="s">
         <v>19</v>
@@ -14680,7 +14766,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="T24" t="s">
         <v>19</v>
@@ -14754,7 +14840,7 @@
     </row>
     <row r="28" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -14840,7 +14926,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -14918,7 +15004,7 @@
         <v>371</v>
       </c>
       <c r="F1" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="G1" t="s">
         <v>372</v>
@@ -14948,7 +15034,7 @@
         <v>379</v>
       </c>
       <c r="P1" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="Q1" t="s">
         <v>380</v>
@@ -14990,10 +15076,10 @@
         <v>601</v>
       </c>
       <c r="AD1" t="s">
+        <v>686</v>
+      </c>
+      <c r="AE1" t="s">
         <v>687</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>688</v>
       </c>
       <c r="AF1" t="s">
         <v>448</v>

</xml_diff>

<commit_message>
Remove Bulk Dependency FHIR-39377,Change Condition patient + category search to SHALL support FHIR-37918
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51879F10-E165-C642-B5D0-6A95D3AD4594}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA59F2E-0F24-E64B-B220-1B0C07C00C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1742,9 +1742,6 @@
     <t>application/json-patch+json</t>
   </si>
   <si>
-    <t>Bulk Data Access IG</t>
-  </si>
-  <si>
     <t>SMART Application Launch Framework Implementation Guide</t>
   </si>
   <si>
@@ -2398,12 +2395,15 @@
   <si>
     <t>Fetches a bundle of all Device resources for the specified patient and status</t>
   </si>
+  <si>
+    <t>!Bulk Data Access IG</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2499,6 +2499,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -2546,12 +2554,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2583,12 +2592,15 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2962,7 +2974,7 @@
         <v>466</v>
       </c>
       <c r="B2" t="s">
-        <v>655</v>
+        <v>654</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2994,7 +3006,7 @@
         <v>68</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -3010,12 +3022,12 @@
         <v>469</v>
       </c>
       <c r="B8" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
       <c r="B9" t="b">
         <v>1</v>
@@ -3080,7 +3092,7 @@
         <v>41</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>32</v>
@@ -4036,7 +4048,7 @@
         <v>22</v>
       </c>
       <c r="C19" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="D19" t="s">
         <v>30</v>
@@ -4194,7 +4206,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="D22" t="s">
         <v>30</v>
@@ -4341,7 +4353,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="D25" t="s">
         <v>30</v>
@@ -4400,7 +4412,7 @@
         <v>0</v>
       </c>
       <c r="F26" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
       <c r="G26" t="str">
         <f t="shared" si="1"/>
@@ -4618,7 +4630,7 @@
         <v>56</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Z30" t="s">
         <v>173</v>
@@ -4640,7 +4652,7 @@
         <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -4665,19 +4677,19 @@
         <v>57</v>
       </c>
       <c r="L31" t="s">
+        <v>705</v>
+      </c>
+      <c r="M31" t="s">
+        <v>56</v>
+      </c>
+      <c r="O31" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>706</v>
       </c>
-      <c r="M31" t="s">
-        <v>56</v>
-      </c>
-      <c r="O31" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>707</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>708</v>
       </c>
       <c r="AA31" s="10" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -5072,7 +5084,7 @@
         <v>138</v>
       </c>
       <c r="C40" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
       <c r="D40" t="s">
         <v>30</v>
@@ -5126,7 +5138,7 @@
         <v>138</v>
       </c>
       <c r="C41" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="D41" t="s">
         <v>30</v>
@@ -5180,7 +5192,7 @@
         <v>138</v>
       </c>
       <c r="C42" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="D42" t="s">
         <v>30</v>
@@ -5319,7 +5331,7 @@
         <v>56</v>
       </c>
       <c r="Y44" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="Z44" s="4" t="str">
         <f>"GET [base]/"&amp;B44&amp;"?patient=1137192"</f>
@@ -7526,7 +7538,7 @@
         <v>56</v>
       </c>
       <c r="X85" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="Y85" t="str">
         <f>"support searching for all "&amp;LOWER(B85)&amp;"s for a patient"</f>
@@ -7659,7 +7671,7 @@
         <v>248</v>
       </c>
       <c r="C88" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="D88" t="s">
         <v>70</v>
@@ -7697,7 +7709,7 @@
         <v>56</v>
       </c>
       <c r="Y88" s="4" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="Z88" s="4" t="str">
         <f>"GET [base]/"&amp;B88&amp;"?"&amp;C88&amp;"=http://snomed.info/sct\|17561000"</f>
@@ -8661,7 +8673,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C106" t="s">
         <v>62</v>
@@ -8714,7 +8726,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C107" t="s">
         <v>90</v>
@@ -8773,7 +8785,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C108" t="s">
         <v>140</v>
@@ -8823,7 +8835,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C109" t="s">
         <v>26</v>
@@ -8876,10 +8888,10 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C110" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D110" t="s">
         <v>30</v>
@@ -8930,7 +8942,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C111" t="s">
         <v>55</v>
@@ -8965,10 +8977,10 @@
         <v>56</v>
       </c>
       <c r="Y111" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="Z111" s="4" t="s">
         <v>580</v>
-      </c>
-      <c r="Z111" s="4" t="s">
-        <v>581</v>
       </c>
       <c r="AB111" t="str">
         <f>"SearchParameter-us-core-"&amp;LOWER((B111)&amp;"-"&amp;SUBSTITUTE(C111,"_","")&amp;".html")</f>
@@ -9026,7 +9038,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C113" t="s">
         <v>55</v>
@@ -9061,10 +9073,10 @@
         <v>56</v>
       </c>
       <c r="Y113" s="4" t="s">
+        <v>601</v>
+      </c>
+      <c r="Z113" s="4" t="s">
         <v>602</v>
-      </c>
-      <c r="Z113" s="4" t="s">
-        <v>603</v>
       </c>
       <c r="AA113" s="10"/>
       <c r="AB113" t="str">
@@ -9077,7 +9089,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C114" t="s">
         <v>90</v>
@@ -9136,7 +9148,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="C115" t="s">
         <v>23</v>
@@ -9174,7 +9186,7 @@
         <v>56</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9194,7 +9206,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C116" t="s">
         <v>55</v>
@@ -9233,7 +9245,7 @@
         <v>support fetching a QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" ref="AB116:AB122" si="67">"SearchParameter-us-core-"&amp;LOWER((B116)&amp;"-"&amp;SUBSTITUTE(C116,"_","")&amp;".html")</f>
@@ -9245,7 +9257,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C117" t="s">
         <v>90</v>
@@ -9304,7 +9316,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C118" t="s">
         <v>62</v>
@@ -9345,7 +9357,7 @@
         <v>56</v>
       </c>
       <c r="Y118" s="20" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="67"/>
@@ -9357,10 +9369,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C119" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="D119" t="s">
         <v>30</v>
@@ -9385,16 +9397,16 @@
         <v>57</v>
       </c>
       <c r="L119" t="s">
+        <v>637</v>
+      </c>
+      <c r="M119" t="s">
+        <v>56</v>
+      </c>
+      <c r="O119" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y119" s="20" t="s">
         <v>638</v>
-      </c>
-      <c r="M119" t="s">
-        <v>56</v>
-      </c>
-      <c r="O119" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y119" s="20" t="s">
-        <v>639</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="67"/>
@@ -9406,10 +9418,10 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C120" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="D120" t="s">
         <v>30</v>
@@ -9450,7 +9462,7 @@
         <v>93</v>
       </c>
       <c r="Y120" s="20" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="67"/>
@@ -9462,10 +9474,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C121" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="D121" t="s">
         <v>30</v>
@@ -9500,7 +9512,7 @@
         <v>56</v>
       </c>
       <c r="Y121" s="20" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="67"/>
@@ -9512,7 +9524,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="C122" t="s">
         <v>90</v>
@@ -9553,7 +9565,7 @@
         <v>56</v>
       </c>
       <c r="Y122" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9573,7 +9585,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C123" t="s">
         <v>62</v>
@@ -9629,7 +9641,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C124" t="s">
         <v>13</v>
@@ -9685,7 +9697,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C125" t="s">
         <v>90</v>
@@ -9726,10 +9738,10 @@
         <v>56</v>
       </c>
       <c r="X125" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="Z125" s="10" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="AA125" s="10" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9745,10 +9757,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>696</v>
+      </c>
+      <c r="C126" t="s">
         <v>697</v>
-      </c>
-      <c r="C126" t="s">
-        <v>698</v>
       </c>
       <c r="D126" t="s">
         <v>30</v>
@@ -9810,13 +9822,14 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K107"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C77" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="G36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B105" sqref="B105"/>
+      <selection pane="bottomRight" activeCell="H114" sqref="H114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9847,7 +9860,7 @@
         <v>96</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>97</v>
@@ -9868,7 +9881,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9893,7 +9906,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9918,7 +9931,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9943,7 +9956,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9968,7 +9981,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -9999,7 +10012,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10024,7 +10037,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -10049,7 +10062,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -10075,7 +10088,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -10102,7 +10115,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10128,7 +10141,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10153,7 +10166,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10184,7 +10197,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10209,7 +10222,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10234,7 +10247,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10265,7 +10278,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10277,7 +10290,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="F17" t="s">
         <v>70</v>
@@ -10289,14 +10302,14 @@
         <v>305</v>
       </c>
       <c r="J17" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and location</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10322,7 +10335,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10353,7 +10366,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10365,7 +10378,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="F20" t="s">
         <v>70</v>
@@ -10377,14 +10390,14 @@
         <v>310</v>
       </c>
       <c r="J20" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="1"/>
         <v>Fetches a bundle of all Encounter resources matching the specified patient and discharge-disposition</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -10411,7 +10424,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -10437,7 +10450,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -10462,7 +10475,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10488,7 +10501,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10515,7 +10528,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10542,7 +10555,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -10569,7 +10582,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10594,7 +10607,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10619,7 +10632,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -10644,7 +10657,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -10675,7 +10688,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -10687,7 +10700,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="F32" t="s">
         <v>70</v>
@@ -10696,17 +10709,17 @@
         <v>134</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" ref="K32" si="7">"Fetches a bundle of all "&amp;B32&amp;" resources matching the specified "&amp;SUBSTITUTE(D32,","," and ")</f>
         <v>Fetches a bundle of all Patient resources matching the specified death-date and family</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -10737,7 +10750,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -10768,7 +10781,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -10799,7 +10812,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10829,7 +10842,7 @@
         <v>330</v>
       </c>
       <c r="K36" s="4" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
@@ -10847,7 +10860,7 @@
         <v>145</v>
       </c>
       <c r="F37" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="G37" t="s">
         <v>106</v>
@@ -10874,7 +10887,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F38" t="s">
         <v>70</v>
@@ -10886,10 +10899,10 @@
         <v>150</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="K38" s="4" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
@@ -10946,7 +10959,7 @@
         <v>153</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="K40" s="4" t="s">
         <v>156</v>
@@ -10964,7 +10977,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="F41" t="s">
         <v>70</v>
@@ -10976,7 +10989,7 @@
         <v>153</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="K41" s="4" t="s">
         <v>156</v>
@@ -10994,7 +11007,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="F42" t="s">
         <v>70</v>
@@ -11006,7 +11019,7 @@
         <v>153</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="K42" s="4" t="s">
         <v>156</v>
@@ -11024,7 +11037,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="F43" t="s">
         <v>70</v>
@@ -11036,13 +11049,13 @@
         <v>153</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="K43" s="4" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -11072,7 +11085,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -11103,7 +11116,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -11134,7 +11147,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -11164,7 +11177,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11197,7 +11210,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11227,7 +11240,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -11260,7 +11273,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -11290,7 +11303,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -11320,7 +11333,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -11350,7 +11363,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -11380,7 +11393,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -11410,7 +11423,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code specified in US Core DiagnosticReport Category Codes</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -11440,7 +11453,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -11471,7 +11484,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -11502,7 +11515,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -11535,7 +11548,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -11568,7 +11581,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -11601,7 +11614,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -11634,7 +11647,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -11665,7 +11678,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -11695,7 +11708,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -11726,7 +11739,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -11757,7 +11770,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -11788,7 +11801,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -11820,7 +11833,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -11853,7 +11866,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -11883,7 +11896,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -11916,7 +11929,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -11946,7 +11959,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -11976,7 +11989,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -12009,7 +12022,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -12041,7 +12054,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -12073,7 +12086,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -12105,7 +12118,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="136" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="136" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -12129,16 +12142,16 @@
         <v>311</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="K78" s="10" t="s">
-        <v>574</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -12171,7 +12184,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code.</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -12204,7 +12217,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and category and status</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -12237,7 +12250,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -12270,7 +12283,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -12303,7 +12316,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `vital-signs`</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -12333,7 +12346,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -12364,7 +12377,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -12393,7 +12406,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -12426,7 +12439,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -12459,7 +12472,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -12489,7 +12502,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -12520,7 +12533,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -12549,7 +12562,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -12569,16 +12582,16 @@
         <v>106</v>
       </c>
       <c r="I92" s="4" t="s">
+        <v>716</v>
+      </c>
+      <c r="J92" s="4" t="s">
         <v>717</v>
       </c>
-      <c r="J92" s="4" t="s">
+      <c r="K92" s="4" t="s">
         <v>718</v>
       </c>
-      <c r="K92" s="4" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -12590,7 +12603,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D93" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F93" t="s">
         <v>70</v>
@@ -12599,21 +12612,21 @@
         <v>106</v>
       </c>
       <c r="I93" s="4" t="s">
+        <v>567</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="J93" s="4" t="s">
+      <c r="K93" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="K93" s="4" t="s">
-        <v>570</v>
-      </c>
-    </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="94" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" ref="C94:C107" si="12">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B94)</f>
@@ -12632,19 +12645,19 @@
         <v>303</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="K94" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified "&amp;SUBSTITUTE(D94,","," and ")</f>
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="12"/>
@@ -12663,19 +12676,19 @@
         <v>198</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="K95" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and  a category code"</f>
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="12"/>
@@ -12694,26 +12707,26 @@
         <v>199</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="K96" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C97" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D97" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="F97" t="s">
         <v>12</v>
@@ -12725,26 +12738,26 @@
         <v>201</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="K97" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient and date and a category code"</f>
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="C98" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D98" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="F98" t="s">
         <v>70</v>
@@ -12753,17 +12766,17 @@
         <v>218</v>
       </c>
       <c r="I98" s="4" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
       <c r="K98" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -12775,7 +12788,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D99" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
       <c r="F99" t="s">
         <v>70</v>
@@ -12784,22 +12797,22 @@
         <v>106</v>
       </c>
       <c r="I99" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>589</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>590</v>
       </c>
       <c r="K99" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified "&amp;SUBSTITUTE(D99,","," and ")</f>
         <v>Fetches a bundle of all Goal resources for the specified patient and description</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C100" t="str">
         <f t="shared" si="12"/>
@@ -12815,29 +12828,29 @@
         <v>106</v>
       </c>
       <c r="I100" t="s">
+        <v>648</v>
+      </c>
+      <c r="J100" s="4" t="s">
         <v>649</v>
-      </c>
-      <c r="J100" s="4" t="s">
-        <v>650</v>
       </c>
       <c r="K100" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B100&amp;" resources for the specified "&amp;SUBSTITUTE(D100,","," and ")</f>
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C101" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D101" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="F101" t="s">
         <v>70</v>
@@ -12846,32 +12859,32 @@
         <v>106</v>
       </c>
       <c r="H101" t="s">
+        <v>647</v>
+      </c>
+      <c r="I101" t="s">
         <v>648</v>
       </c>
-      <c r="I101" t="s">
-        <v>649</v>
-      </c>
       <c r="J101" s="4" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="K101" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified "&amp;SUBSTITUTE(D101,","," and  ") &amp; "= 'sdoh'"</f>
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D102" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="F102" t="s">
         <v>70</v>
@@ -12880,29 +12893,29 @@
         <v>149</v>
       </c>
       <c r="I102" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J102" s="4" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
       <c r="K102" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B102&amp;" resources for the specified patient and date"</f>
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C103" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D103" s="18" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="F103" t="s">
         <v>70</v>
@@ -12911,32 +12924,32 @@
         <v>218</v>
       </c>
       <c r="H103" t="s">
+        <v>647</v>
+      </c>
+      <c r="I103" t="s">
         <v>648</v>
       </c>
-      <c r="I103" t="s">
-        <v>649</v>
-      </c>
       <c r="J103" s="4" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="K103" t="str">
         <f>"Fetches a bundle of all "&amp;B103&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
         <v>Fetches a bundle of all QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="C104" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D104" s="18" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="F104" t="s">
         <v>70</v>
@@ -12945,22 +12958,22 @@
         <v>91</v>
       </c>
       <c r="I104" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="J104" s="4" t="s">
-        <v>654</v>
+        <v>653</v>
       </c>
       <c r="K104" t="str">
         <f>"Fetches a bundle of all "&amp;B104&amp;" resources for the specified patient that have been completed against a specified form."</f>
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:11" ht="151" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
       <c r="B105" s="18" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C105" t="str">
         <f t="shared" si="12"/>
@@ -12980,22 +12993,22 @@
       </c>
       <c r="H105" s="18"/>
       <c r="I105" s="4" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="J105" s="4" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="K105" t="str">
         <f>"Fetches a bundle of all "&amp;B105&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed)).</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
       <c r="B106" s="18" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="C106" t="str">
         <f t="shared" si="12"/>
@@ -13015,29 +13028,29 @@
       </c>
       <c r="H106" s="18"/>
       <c r="I106" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="J106" s="4" t="s">
         <v>702</v>
-      </c>
-      <c r="J106" s="4" t="s">
-        <v>703</v>
       </c>
       <c r="K106" t="str">
         <f>"Fetches a bundle of all "&amp;B106&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed).</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
       <c r="B107" s="18" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C107" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D107" s="18" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E107" s="18" t="s">
         <v>56</v>
@@ -13050,10 +13063,10 @@
       </c>
       <c r="H107" s="18"/>
       <c r="I107" s="4" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="J107" s="4" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="K107" t="str">
         <f>"Fetches a bundle of all "&amp;B106&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -13061,7 +13074,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K107" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
+  <autoFilter ref="A1:K107" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Condition"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K135">
     <sortCondition ref="A1"/>
   </sortState>
@@ -13106,7 +13125,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13122,7 +13141,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -13138,7 +13157,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13146,7 +13165,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -13191,7 +13210,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13217,29 +13236,29 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="B2" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
       <c r="C2" t="s">
+        <v>540</v>
+      </c>
+      <c r="D2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>719</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>539</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>541</v>
       </c>
-      <c r="D2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>534</v>
-      </c>
-      <c r="B3" t="s">
-        <v>540</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>542</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="D3" s="24" t="s">
         <v>70</v>
       </c>
     </row>
@@ -13252,7 +13271,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EBB963-62EF-8346-A79F-04E3300CC06A}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -13290,13 +13309,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="F2" t="s">
         <v>12</v>
@@ -13311,8 +13330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13385,10 +13404,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="B5" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -13399,10 +13418,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="B6" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -13413,16 +13432,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>671</v>
+      </c>
+      <c r="B7" t="s">
         <v>672</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>673</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>674</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13482,8 +13501,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
-        <v>714</v>
+      <c r="A12" s="23" t="s">
+        <v>713</v>
       </c>
       <c r="B12" t="s">
         <v>365</v>
@@ -13496,91 +13515,91 @@
       </c>
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="21" t="s">
+      <c r="A13" s="22" t="s">
+        <v>627</v>
+      </c>
+      <c r="B13" t="s">
+        <v>607</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
         <v>628</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
+        <v>615</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" t="s">
         <v>608</v>
       </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E13" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="21" t="s">
+    </row>
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
         <v>629</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>616</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-      <c r="E14" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="21" t="s">
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
         <v>630</v>
       </c>
-      <c r="B15" t="s">
-        <v>617</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="21" t="s">
+      <c r="B16" t="s">
+        <v>618</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
         <v>631</v>
       </c>
-      <c r="B16" t="s">
-        <v>619</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="B17" t="s">
+        <v>620</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="22" t="s">
         <v>632</v>
       </c>
-      <c r="B17" t="s">
-        <v>621</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" t="s">
-        <v>609</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="21" t="s">
-        <v>633</v>
-      </c>
       <c r="B18" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
       </c>
       <c r="E18" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="19" t="s">
+      <c r="A19" s="21" t="s">
         <v>359</v>
       </c>
       <c r="B19" t="s">
@@ -13651,16 +13670,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>687</v>
+      </c>
+      <c r="B24" t="s">
         <v>688</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
         <v>689</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>690</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13679,10 +13698,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="B26" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -13693,10 +13712,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="B27" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -13707,10 +13726,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B28" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -13721,10 +13740,10 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="19" t="s">
+        <v>609</v>
+      </c>
+      <c r="B29" t="s">
         <v>610</v>
-      </c>
-      <c r="B29" t="s">
-        <v>611</v>
       </c>
       <c r="D29" t="s">
         <v>12</v>
@@ -13749,10 +13768,10 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="19" t="s">
+        <v>611</v>
+      </c>
+      <c r="B31" t="s">
         <v>612</v>
-      </c>
-      <c r="B31" t="s">
-        <v>613</v>
       </c>
       <c r="D31" t="s">
         <v>12</v>
@@ -13833,10 +13852,10 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="19" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="B37" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="D37" t="s">
         <v>12</v>
@@ -13889,10 +13908,10 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="19" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="B41" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="D41" t="s">
         <v>12</v>
@@ -13917,10 +13936,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="19" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B43" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -13931,10 +13950,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="19" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="B44" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -13962,7 +13981,7 @@
         <v>495</v>
       </c>
       <c r="B46" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -14085,58 +14104,58 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="19" t="s">
+        <v>623</v>
+      </c>
+      <c r="B55" t="s">
         <v>624</v>
       </c>
-      <c r="B55" t="s">
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" t="s">
         <v>625</v>
-      </c>
-      <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
-        <v>626</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="19" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="B56" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="D56" t="s">
         <v>12</v>
       </c>
       <c r="E56" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="19" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="B57" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="D57" t="s">
         <v>12</v>
       </c>
       <c r="E57" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="19" t="s">
+        <v>682</v>
+      </c>
+      <c r="B58" t="s">
         <v>683</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
         <v>684</v>
-      </c>
-      <c r="D58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" t="s">
-        <v>685</v>
       </c>
     </row>
   </sheetData>
@@ -14144,8 +14163,11 @@
     <sortCondition ref="E2:E43"/>
     <sortCondition ref="B2:B43"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="A19" r:id="rId1" xr:uid="{989800B5-A1D9-4349-9DD7-B6144EA2265D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -14307,7 +14329,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="T4" t="s">
         <v>19</v>
@@ -14316,10 +14338,10 @@
         <v>70</v>
       </c>
       <c r="V4" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="W4" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="X4" s="15" t="s">
         <v>449</v>
@@ -14336,7 +14358,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="T5" t="s">
         <v>19</v>
@@ -14353,7 +14375,7 @@
     </row>
     <row r="6" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -14379,7 +14401,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="T7" t="s">
         <v>19</v>
@@ -14423,7 +14445,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14446,7 +14468,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="T10" t="s">
         <v>19</v>
@@ -14489,7 +14511,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="T12" t="s">
         <v>19</v>
@@ -14573,13 +14595,13 @@
     </row>
     <row r="16" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="T16" t="s">
         <v>19</v>
@@ -14591,7 +14613,7 @@
         <v>70</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="X16" s="15" t="s">
         <v>449</v>
@@ -14637,7 +14659,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="T18" t="s">
         <v>19</v>
@@ -14660,7 +14682,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="T19" t="s">
         <v>19</v>
@@ -14679,7 +14701,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="T20" t="s">
         <v>19</v>
@@ -14743,7 +14765,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="T23" t="s">
         <v>19</v>
@@ -14766,7 +14788,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="T24" t="s">
         <v>19</v>
@@ -14777,13 +14799,13 @@
     </row>
     <row r="25" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
       <c r="B25" t="s">
         <v>70</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="T25" t="s">
         <v>19</v>
@@ -14800,7 +14822,7 @@
     </row>
     <row r="26" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="B26" t="s">
         <v>12</v>
@@ -14820,7 +14842,7 @@
     </row>
     <row r="27" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="B27" t="s">
         <v>12</v>
@@ -14840,7 +14862,7 @@
     </row>
     <row r="28" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -14926,7 +14948,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -15004,7 +15026,7 @@
         <v>371</v>
       </c>
       <c r="F1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="G1" t="s">
         <v>372</v>
@@ -15034,7 +15056,7 @@
         <v>379</v>
       </c>
       <c r="P1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="Q1" t="s">
         <v>380</v>
@@ -15067,19 +15089,19 @@
         <v>439</v>
       </c>
       <c r="AA1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="AB1" t="s">
+        <v>599</v>
+      </c>
+      <c r="AC1" t="s">
         <v>600</v>
       </c>
-      <c r="AC1" t="s">
-        <v>601</v>
-      </c>
       <c r="AD1" t="s">
+        <v>685</v>
+      </c>
+      <c r="AE1" t="s">
         <v>686</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>687</v>
       </c>
       <c r="AF1" t="s">
         <v>448</v>

</xml_diff>

<commit_message>
Clarify organization responsible for the DocumentReference FHIR-36654, Clarify Device UDI-PI requirements FHIR-36657
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB6047C6-687F-4A45-9346-17C110E49257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F6881EC-287A-3B48-A0C6-72F866881870}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="ops" sheetId="5" r:id="rId7"/>
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
     <sheet name="rest_interactions" sheetId="11" r:id="rId9"/>
-    <sheet name="sps" sheetId="7" r:id="rId10"/>
+    <sheet name="sps" sheetId="14" r:id="rId10"/>
     <sheet name="sp_combos" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames>
@@ -49,12 +49,12 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>tc={9A91E9C9-8B21-8546-B0F6-E258B9D2B6FF}</author>
-    <author>tc={2FB8FCA2-BD31-DF4C-95E0-15548A47CED8}</author>
-    <author>tc={B335108E-FDC9-AC41-96F3-657CAF0CB14F}</author>
+    <author>tc={FB93E46D-3D13-4645-A003-7A1F153E1DB9}</author>
+    <author>tc={738109A7-92A0-7248-ACDE-F9875EAC079A}</author>
+    <author>tc={DCDC06BA-7148-9843-A6EA-EC4B7F1297F8}</author>
   </authors>
   <commentList>
-    <comment ref="L40" authorId="0" shapeId="0" xr:uid="{9A91E9C9-8B21-8546-B0F6-E258B9D2B6FF}">
+    <comment ref="L40" authorId="0" shapeId="0" xr:uid="{FB93E46D-3D13-4645-A003-7A1F153E1DB9}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -62,7 +62,7 @@
     where does this show up?</t>
       </text>
     </comment>
-    <comment ref="Z44" authorId="1" shapeId="0" xr:uid="{2FB8FCA2-BD31-DF4C-95E0-15548A47CED8}">
+    <comment ref="Z44" authorId="1" shapeId="0" xr:uid="{738109A7-92A0-7248-ACDE-F9875EAC079A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -70,7 +70,7 @@
     do i need this?</t>
       </text>
     </comment>
-    <comment ref="AA44" authorId="2" shapeId="0" xr:uid="{B335108E-FDC9-AC41-96F3-657CAF0CB14F}">
+    <comment ref="AA44" authorId="2" shapeId="0" xr:uid="{DCDC06BA-7148-9843-A6EA-EC4B7F1297F8}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -2116,15 +2116,6 @@
     <t>* Based upon the ONC U.S. Core Data for Interoperability (USCDI) requirements, CVX vaccine codes are required and the NDC vaccine codes **SHOULD** be supported as translations to them.</t>
   </si>
   <si>
-    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
-* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
-    *  Although both are marked as must support, the server system is not required to support both an address and inline base64 encoded data, but **SHALL** support at least one of these elements.
-    *  The client application **SHALL** support both elements.
-    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or other endpoint.
-        * If the endpoint is outside of the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
-* The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
-  </si>
-  <si>
     <t>* Implantable medical devices that have UDI information **SHALL** represent the UDI code in `Device.udiCarrier.carrierHRF`.
    - All of the five UDI-PI elements that are present in the UDI code **SHALL** be represented in the corresponding US Core Implantable Device Profile element.
    UDI may not be present in all scenarios such as historical implantable devices, patient reported implant information, payer reported devices, or improperly documented implants. If UDI is not present and the manufacturer and/or model number information is available, they **SHOULD** be included to support historical reports of implantable medical devices as follows:
@@ -2358,6 +2349,15 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable</t>
+  </si>
+  <si>
+    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
+* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
+    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
+    *  The client application **SHALL** support both elements.
+    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
+        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
+* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
   </si>
 </sst>
 </file>
@@ -2873,13 +2873,13 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="L40" dT="2021-11-06T02:36:52.48" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{9A91E9C9-8B21-8546-B0F6-E258B9D2B6FF}">
+  <threadedComment ref="L40" dT="2021-11-06T02:36:52.48" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{FB93E46D-3D13-4645-A003-7A1F153E1DB9}">
     <text>where does this show up?</text>
   </threadedComment>
-  <threadedComment ref="Z44" dT="2021-11-06T02:39:25.62" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{2FB8FCA2-BD31-DF4C-95E0-15548A47CED8}">
+  <threadedComment ref="Z44" dT="2021-11-06T02:39:25.62" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{738109A7-92A0-7248-ACDE-F9875EAC079A}">
     <text>do i need this?</text>
   </threadedComment>
-  <threadedComment ref="AA44" dT="2021-11-06T02:40:08.93" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{B335108E-FDC9-AC41-96F3-657CAF0CB14F}">
+  <threadedComment ref="AA44" dT="2021-11-06T02:40:08.93" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{DCDC06BA-7148-9843-A6EA-EC4B7F1297F8}">
     <text>do I need this?</text>
   </threadedComment>
 </ThreadedComments>
@@ -2993,14 +2993,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9F73F9-34B4-C04F-A2E4-99114F8B7BF7}">
   <dimension ref="A1:AB126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C90" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G130" sqref="G130"/>
+      <selection pane="bottomRight" activeCell="F128" sqref="F128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3149,7 +3149,7 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="9"/>
       <c r="AB2" t="str">
-        <f t="shared" ref="AB2:AB4" si="0">"SearchParameter-us-core-"&amp;LOWER((B2)&amp;"-"&amp;C2&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B2)&amp;"-"&amp;C2&amp;".html")</f>
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
@@ -3170,7 +3170,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="str">
-        <f t="shared" ref="G3:G74" si="1">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B3)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B3)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example code search</v>
       </c>
       <c r="H3" t="s">
@@ -3196,7 +3196,7 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="9"/>
       <c r="AB3" t="str">
-        <f t="shared" si="0"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B3)&amp;"-"&amp;C3&amp;".html")</f>
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
@@ -3217,7 +3217,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B4)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example date search</v>
       </c>
       <c r="H4" t="s">
@@ -3247,7 +3247,7 @@
       </c>
       <c r="AA4" s="9"/>
       <c r="AB4" t="str">
-        <f t="shared" si="0"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B4)&amp;"-"&amp;C4&amp;".html")</f>
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
@@ -3271,7 +3271,7 @@
         <v>486</v>
       </c>
       <c r="G5" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B5)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example patient search</v>
       </c>
       <c r="H5" t="s">
@@ -3327,7 +3327,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B6)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example status search</v>
       </c>
       <c r="H6" t="s">
@@ -3340,7 +3340,7 @@
         <v>57</v>
       </c>
       <c r="L6" t="str">
-        <f t="shared" ref="L6" si="2">B6&amp;"."&amp;C6</f>
+        <f>B6&amp;"."&amp;C6</f>
         <v>!EXAMPLE STATUS SEARCH.status</v>
       </c>
       <c r="M6" t="s">
@@ -3353,7 +3353,7 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="9"/>
       <c r="AB6" t="str">
-        <f t="shared" ref="AB6" si="3">"SearchParameter-us-core-"&amp;LOWER((B6)&amp;"-"&amp;C6&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B6)&amp;"-"&amp;C6&amp;".html")</f>
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
@@ -3374,7 +3374,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B7)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="H7" t="s">
@@ -3387,7 +3387,7 @@
         <v>64</v>
       </c>
       <c r="L7" t="str">
-        <f t="shared" ref="L7:L24" si="4">B7&amp;"."&amp;C7</f>
+        <f>B7&amp;"."&amp;C7</f>
         <v>!Patient.address</v>
       </c>
       <c r="M7" t="s">
@@ -3425,7 +3425,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B8)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="H8" t="s">
@@ -3438,7 +3438,7 @@
         <v>64</v>
       </c>
       <c r="L8" t="str">
-        <f t="shared" si="4"/>
+        <f>B8&amp;"."&amp;C8</f>
         <v>!Patient.telecom</v>
       </c>
       <c r="M8" t="s">
@@ -3455,7 +3455,7 @@
       </c>
       <c r="AA8" s="9"/>
       <c r="AB8" t="str">
-        <f t="shared" ref="AB8:AB47" si="5">"SearchParameter-us-core-"&amp;LOWER((B8)&amp;"-"&amp;C8&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B8)&amp;"-"&amp;C8&amp;".html")</f>
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
@@ -3479,7 +3479,7 @@
         <v>489</v>
       </c>
       <c r="G9" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B9)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="H9" t="s">
@@ -3492,7 +3492,7 @@
         <v>57</v>
       </c>
       <c r="L9" t="str">
-        <f t="shared" si="4"/>
+        <f>B9&amp;"."&amp;C9</f>
         <v>AllergyIntolerance.clinical-status</v>
       </c>
       <c r="M9" t="s">
@@ -3504,7 +3504,7 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="9"/>
       <c r="AB9" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B9)&amp;"-"&amp;C9&amp;".html")</f>
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
@@ -3528,7 +3528,7 @@
         <v>486</v>
       </c>
       <c r="G10" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B10)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="H10" t="s">
@@ -3541,7 +3541,7 @@
         <v>91</v>
       </c>
       <c r="L10" t="str">
-        <f t="shared" si="4"/>
+        <f>B10&amp;"."&amp;C10</f>
         <v>AllergyIntolerance.patient</v>
       </c>
       <c r="M10" t="s">
@@ -3586,7 +3586,7 @@
         <v>489</v>
       </c>
       <c r="G11" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B11)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H11" t="s">
@@ -3599,7 +3599,7 @@
         <v>57</v>
       </c>
       <c r="L11" t="str">
-        <f t="shared" si="4"/>
+        <f>B11&amp;"."&amp;C11</f>
         <v>Condition.category</v>
       </c>
       <c r="M11" t="s">
@@ -3612,7 +3612,7 @@
       <c r="Z11" s="4"/>
       <c r="AA11" s="9"/>
       <c r="AB11" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B11)&amp;"-"&amp;C11&amp;".html")</f>
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
@@ -3636,7 +3636,7 @@
         <v>489</v>
       </c>
       <c r="G12" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B12)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H12" t="s">
@@ -3649,7 +3649,7 @@
         <v>57</v>
       </c>
       <c r="L12" t="str">
-        <f t="shared" si="4"/>
+        <f>B12&amp;"."&amp;C12</f>
         <v>Condition.clinical-status</v>
       </c>
       <c r="M12" t="s">
@@ -3660,7 +3660,7 @@
       </c>
       <c r="AA12" s="9"/>
       <c r="AB12" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B12)&amp;"-"&amp;C12&amp;".html")</f>
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
@@ -3684,7 +3684,7 @@
         <v>486</v>
       </c>
       <c r="G13" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B13)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H13" t="s">
@@ -3697,7 +3697,7 @@
         <v>91</v>
       </c>
       <c r="L13" t="str">
-        <f t="shared" si="4"/>
+        <f>B13&amp;"."&amp;C13</f>
         <v>Condition.patient</v>
       </c>
       <c r="M13" t="s">
@@ -3718,7 +3718,7 @@
         <v>Fetches a bundle of all Condition resources for the specified patient</v>
       </c>
       <c r="AB13" t="str">
-        <f t="shared" ref="AB13:AB14" si="6">"SearchParameter-us-core-"&amp;LOWER((B13)&amp;"-"&amp;SUBSTITUTE(C13,"_","")&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B13)&amp;"-"&amp;SUBSTITUTE(C13,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
@@ -3739,7 +3739,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B14)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H14" t="s">
@@ -3752,7 +3752,7 @@
         <v>57</v>
       </c>
       <c r="L14" t="str">
-        <f t="shared" si="4"/>
+        <f>B14&amp;"."&amp;C14</f>
         <v>Encounter._id</v>
       </c>
       <c r="M14" t="s">
@@ -3771,7 +3771,7 @@
         <v>171</v>
       </c>
       <c r="AB14" t="str">
-        <f t="shared" si="6"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B14)&amp;"-"&amp;SUBSTITUTE(C14,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
@@ -3795,7 +3795,7 @@
         <v>489</v>
       </c>
       <c r="G15" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B15)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H15" t="s">
@@ -3808,7 +3808,7 @@
         <v>57</v>
       </c>
       <c r="L15" t="str">
-        <f t="shared" si="4"/>
+        <f>B15&amp;"."&amp;C15</f>
         <v>Encounter.class</v>
       </c>
       <c r="M15" t="s">
@@ -3821,7 +3821,7 @@
       <c r="Z15" s="4"/>
       <c r="AA15" s="9"/>
       <c r="AB15" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B15)&amp;"-"&amp;C15&amp;".html")</f>
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
@@ -3845,7 +3845,7 @@
         <v>487</v>
       </c>
       <c r="G16" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B16)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H16" t="s">
@@ -3858,7 +3858,7 @@
         <v>79</v>
       </c>
       <c r="L16" t="str">
-        <f t="shared" si="4"/>
+        <f>B16&amp;"."&amp;C16</f>
         <v>Encounter.date</v>
       </c>
       <c r="M16" t="s">
@@ -3875,7 +3875,7 @@
       </c>
       <c r="AA16" s="9"/>
       <c r="AB16" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B16)&amp;"-"&amp;C16&amp;".html")</f>
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
@@ -3899,7 +3899,7 @@
         <v>489</v>
       </c>
       <c r="G17" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B17)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H17" t="s">
@@ -3912,7 +3912,7 @@
         <v>57</v>
       </c>
       <c r="L17" t="str">
-        <f t="shared" si="4"/>
+        <f>B17&amp;"."&amp;C17</f>
         <v>Encounter.identifier</v>
       </c>
       <c r="M17" t="s">
@@ -3932,7 +3932,7 @@
         <v>Fetches a bundle containing any Encounter resources matching the identifier</v>
       </c>
       <c r="AB17" t="str">
-        <f t="shared" ref="AB17:AB18" si="7">"SearchParameter-us-core-"&amp;LOWER((B17)&amp;"-"&amp;SUBSTITUTE(C17,"_","")&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B17)&amp;"-"&amp;SUBSTITUTE(C17,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
@@ -3956,7 +3956,7 @@
         <v>486</v>
       </c>
       <c r="G18" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B18)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H18" t="s">
@@ -3969,7 +3969,7 @@
         <v>91</v>
       </c>
       <c r="L18" t="str">
-        <f t="shared" si="4"/>
+        <f>B18&amp;"."&amp;C18</f>
         <v>Encounter.patient</v>
       </c>
       <c r="M18" t="s">
@@ -3990,7 +3990,7 @@
         <v>Fetches a bundle of all Encounter resources for the specified patient</v>
       </c>
       <c r="AB18" t="str">
-        <f t="shared" si="7"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B18)&amp;"-"&amp;SUBSTITUTE(C18,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
@@ -4014,7 +4014,7 @@
         <v>486</v>
       </c>
       <c r="G19" t="str">
-        <f t="shared" ref="G19" si="8">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B19)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B19)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H19" t="s">
@@ -4027,7 +4027,7 @@
         <v>91</v>
       </c>
       <c r="L19" t="str">
-        <f t="shared" ref="L19" si="9">B19&amp;"."&amp;C19</f>
+        <f>B19&amp;"."&amp;C19</f>
         <v>Encounter.location</v>
       </c>
       <c r="M19" t="s">
@@ -4048,7 +4048,7 @@
         <v>Fetches a bundle of all Encounter resources for the specified patient</v>
       </c>
       <c r="AB19" t="str">
-        <f t="shared" ref="AB19" si="10">"SearchParameter-us-core-"&amp;LOWER((B19)&amp;"-"&amp;SUBSTITUTE(C19,"_","")&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B19)&amp;"-"&amp;SUBSTITUTE(C19,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-encounter-location.html</v>
       </c>
     </row>
@@ -4072,7 +4072,7 @@
         <v>489</v>
       </c>
       <c r="G20" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B20)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H20" t="s">
@@ -4085,7 +4085,7 @@
         <v>57</v>
       </c>
       <c r="L20" t="str">
-        <f t="shared" si="4"/>
+        <f>B20&amp;"."&amp;C20</f>
         <v>Encounter.status</v>
       </c>
       <c r="M20" t="s">
@@ -4098,7 +4098,7 @@
       <c r="Z20" s="4"/>
       <c r="AA20" s="9"/>
       <c r="AB20" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B20)&amp;"-"&amp;C20&amp;".html")</f>
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
@@ -4122,7 +4122,7 @@
         <v>489</v>
       </c>
       <c r="G21" t="str">
-        <f t="shared" ref="G21" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H21" t="s">
@@ -4135,7 +4135,7 @@
         <v>57</v>
       </c>
       <c r="L21" t="str">
-        <f t="shared" ref="L21" si="12">B21&amp;"."&amp;C21</f>
+        <f>B21&amp;"."&amp;C21</f>
         <v>Encounter.type</v>
       </c>
       <c r="M21" t="s">
@@ -4148,7 +4148,7 @@
       <c r="Z21" s="4"/>
       <c r="AA21" s="9"/>
       <c r="AB21" t="str">
-        <f t="shared" ref="AB21" si="13">"SearchParameter-us-core-"&amp;LOWER((B21)&amp;"-"&amp;C21&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B21)&amp;"-"&amp;C21&amp;".html")</f>
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
@@ -4172,7 +4172,7 @@
         <v>489</v>
       </c>
       <c r="G22" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B22)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H22" t="s">
@@ -4185,7 +4185,7 @@
         <v>57</v>
       </c>
       <c r="L22" t="str">
-        <f t="shared" si="4"/>
+        <f>B22&amp;"."&amp;C22</f>
         <v>Encounter.discharge-disposition</v>
       </c>
       <c r="M22" t="s">
@@ -4198,7 +4198,7 @@
       <c r="Z22" s="4"/>
       <c r="AA22" s="9"/>
       <c r="AB22" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B22)&amp;"-"&amp;C22&amp;".html")</f>
         <v>SearchParameter-us-core-encounter-discharge-disposition.html</v>
       </c>
     </row>
@@ -4219,7 +4219,7 @@
         <v>1</v>
       </c>
       <c r="G23" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B23)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H23" t="s">
@@ -4235,7 +4235,7 @@
         <v>57</v>
       </c>
       <c r="L23" t="str">
-        <f t="shared" si="4"/>
+        <f>B23&amp;"."&amp;C23</f>
         <v>Patient._id</v>
       </c>
       <c r="M23" t="s">
@@ -4275,7 +4275,7 @@
         <v>488</v>
       </c>
       <c r="G24" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B24)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H24" t="s">
@@ -4288,7 +4288,7 @@
         <v>79</v>
       </c>
       <c r="L24" t="str">
-        <f t="shared" si="4"/>
+        <f>B24&amp;"."&amp;C24</f>
         <v>Patient.birthdate</v>
       </c>
       <c r="M24" t="s">
@@ -4298,7 +4298,7 @@
         <v>56</v>
       </c>
       <c r="AB24" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B24)&amp;"-"&amp;C24&amp;".html")</f>
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
@@ -4310,7 +4310,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D25" t="s">
         <v>30</v>
@@ -4322,7 +4322,7 @@
         <v>488</v>
       </c>
       <c r="G25" t="str">
-        <f t="shared" ref="G25" si="14">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B25)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B25)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H25" t="s">
@@ -4338,7 +4338,7 @@
         <v>79</v>
       </c>
       <c r="L25" t="str">
-        <f t="shared" ref="L25" si="15">B25&amp;"."&amp;C25</f>
+        <f>B25&amp;"."&amp;C25</f>
         <v>Patient.death-date</v>
       </c>
       <c r="M25" t="s">
@@ -4348,7 +4348,7 @@
         <v>56</v>
       </c>
       <c r="AB25" t="str">
-        <f t="shared" ref="AB25" si="16">"SearchParameter-us-core-"&amp;LOWER((B25)&amp;"-"&amp;C25&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B25)&amp;"-"&amp;C25&amp;".html")</f>
         <v>SearchParameter-us-core-patient-death-date.html</v>
       </c>
     </row>
@@ -4372,7 +4372,7 @@
         <v>519</v>
       </c>
       <c r="G26" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B26)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H26" t="s">
@@ -4394,7 +4394,7 @@
         <v>56</v>
       </c>
       <c r="AB26" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B26)&amp;"-"&amp;C26&amp;".html")</f>
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
@@ -4418,7 +4418,7 @@
         <v>489</v>
       </c>
       <c r="G27" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B27)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H27" t="s">
@@ -4442,7 +4442,7 @@
       </c>
       <c r="AA27" s="9"/>
       <c r="AB27" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B27)&amp;"-"&amp;C27&amp;".html")</f>
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
@@ -4463,7 +4463,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B28)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H28" t="s">
@@ -4486,7 +4486,7 @@
       </c>
       <c r="AA28" s="9"/>
       <c r="AB28" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B28)&amp;"-"&amp;C28&amp;".html")</f>
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
@@ -4510,7 +4510,7 @@
         <v>489</v>
       </c>
       <c r="G29" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B29)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H29" t="s">
@@ -4543,7 +4543,7 @@
         <v>Fetches a bundle containing any Patient resources matching the identifier</v>
       </c>
       <c r="AB29" t="str">
-        <f t="shared" ref="AB29:AB30" si="17">"SearchParameter-us-core-"&amp;LOWER((B29)&amp;"-"&amp;SUBSTITUTE(C29,"_","")&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B29)&amp;"-"&amp;SUBSTITUTE(C29,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
@@ -4564,7 +4564,7 @@
         <v>1</v>
       </c>
       <c r="G30" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B30)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H30" t="s">
@@ -4587,7 +4587,7 @@
         <v>56</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="Z30" t="s">
         <v>173</v>
@@ -4597,7 +4597,7 @@
         <v>Fetches a bundle of all Patient resources matching the name</v>
       </c>
       <c r="AB30" t="str">
-        <f t="shared" si="17"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B30)&amp;"-"&amp;SUBSTITUTE(C30,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
@@ -4609,7 +4609,7 @@
         <v>85</v>
       </c>
       <c r="C31" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -4618,7 +4618,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="str">
-        <f t="shared" ref="G31" si="18">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B31)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B31)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="H31" t="s">
@@ -4634,26 +4634,26 @@
         <v>57</v>
       </c>
       <c r="L31" t="s">
+        <v>687</v>
+      </c>
+      <c r="M31" t="s">
+        <v>56</v>
+      </c>
+      <c r="O31" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>688</v>
       </c>
-      <c r="M31" t="s">
-        <v>56</v>
-      </c>
-      <c r="O31" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>689</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>690</v>
       </c>
       <c r="AA31" s="9" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
         <v>Fetches a bundle of all !Patient resources matching the name</v>
       </c>
       <c r="AB31" t="str">
-        <f t="shared" ref="AB31" si="19">"SearchParameter-us-core-"&amp;LOWER((B31)&amp;"-"&amp;SUBSTITUTE(C31,"_","")&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B31)&amp;"-"&amp;SUBSTITUTE(C31,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-!patient-tribal-affiliation.html</v>
       </c>
     </row>
@@ -4674,7 +4674,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B32)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="H32" t="s">
@@ -4696,7 +4696,7 @@
         <v>56</v>
       </c>
       <c r="AB32" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B32)&amp;"-"&amp;C32&amp;".html")</f>
         <v>SearchParameter-us-core-!questionnaire-_id.html</v>
       </c>
     </row>
@@ -4717,7 +4717,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B33)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="H33" t="s">
@@ -4730,7 +4730,7 @@
         <v>72</v>
       </c>
       <c r="L33" t="str">
-        <f t="shared" ref="L33:L47" si="20">B33&amp;"."&amp;C33</f>
+        <f>B33&amp;"."&amp;C33</f>
         <v>!Questionnaire.context-type-value</v>
       </c>
       <c r="M33" t="s">
@@ -4740,7 +4740,7 @@
         <v>56</v>
       </c>
       <c r="AB33" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B33)&amp;"-"&amp;C33&amp;".html")</f>
         <v>SearchParameter-us-core-!questionnaire-context-type-value.html</v>
       </c>
     </row>
@@ -4761,7 +4761,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B34)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="H34" t="s">
@@ -4774,7 +4774,7 @@
         <v>64</v>
       </c>
       <c r="L34" t="str">
-        <f t="shared" si="20"/>
+        <f>B34&amp;"."&amp;C34</f>
         <v>!Questionnaire.publisher</v>
       </c>
       <c r="M34" t="s">
@@ -4787,7 +4787,7 @@
         <v>69</v>
       </c>
       <c r="AB34" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B34)&amp;"-"&amp;C34&amp;".html")</f>
         <v>SearchParameter-us-core-!questionnaire-publisher.html</v>
       </c>
     </row>
@@ -4808,7 +4808,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B35)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="H35" t="s">
@@ -4821,7 +4821,7 @@
         <v>57</v>
       </c>
       <c r="L35" t="str">
-        <f t="shared" si="20"/>
+        <f>B35&amp;"."&amp;C35</f>
         <v>!Questionnaire.status</v>
       </c>
       <c r="M35" t="s">
@@ -4831,7 +4831,7 @@
         <v>56</v>
       </c>
       <c r="AB35" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B35)&amp;"-"&amp;C35&amp;".html")</f>
         <v>SearchParameter-us-core-!questionnaire-status.html</v>
       </c>
     </row>
@@ -4852,7 +4852,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B36)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="H36" t="s">
@@ -4865,7 +4865,7 @@
         <v>64</v>
       </c>
       <c r="L36" t="str">
-        <f t="shared" si="20"/>
+        <f>B36&amp;"."&amp;C36</f>
         <v>!Questionnaire.title</v>
       </c>
       <c r="M36" t="s">
@@ -4887,7 +4887,7 @@
         <v>65</v>
       </c>
       <c r="AB36" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B36)&amp;"-"&amp;C36&amp;".html")</f>
         <v>SearchParameter-us-core-!questionnaire-title.html</v>
       </c>
     </row>
@@ -4908,7 +4908,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B37)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="H37" t="s">
@@ -4921,7 +4921,7 @@
         <v>61</v>
       </c>
       <c r="L37" t="str">
-        <f t="shared" si="20"/>
+        <f>B37&amp;"."&amp;C37</f>
         <v>!Questionnaire.url</v>
       </c>
       <c r="M37" t="s">
@@ -4931,7 +4931,7 @@
         <v>56</v>
       </c>
       <c r="AB37" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B37)&amp;"-"&amp;C37&amp;".html")</f>
         <v>SearchParameter-us-core-!questionnaire-url.html</v>
       </c>
     </row>
@@ -4952,7 +4952,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B38)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="H38" t="s">
@@ -4965,7 +4965,7 @@
         <v>57</v>
       </c>
       <c r="L38" t="str">
-        <f t="shared" si="20"/>
+        <f>B38&amp;"."&amp;C38</f>
         <v>!Questionnaire.version</v>
       </c>
       <c r="M38" t="s">
@@ -4975,7 +4975,7 @@
         <v>56</v>
       </c>
       <c r="AB38" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B38)&amp;"-"&amp;C38&amp;".html")</f>
         <v>SearchParameter-us-core-!questionnaire-version.html</v>
       </c>
     </row>
@@ -4999,7 +4999,7 @@
         <v>487</v>
       </c>
       <c r="G39" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B39)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H39" t="s">
@@ -5012,7 +5012,7 @@
         <v>79</v>
       </c>
       <c r="L39" t="str">
-        <f t="shared" si="20"/>
+        <f>B39&amp;"."&amp;C39</f>
         <v>Condition.onset-date</v>
       </c>
       <c r="M39" t="s">
@@ -5029,7 +5029,7 @@
       </c>
       <c r="AA39" s="9"/>
       <c r="AB39" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B39)&amp;"-"&amp;C39&amp;".html")</f>
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
@@ -5053,7 +5053,7 @@
         <v>487</v>
       </c>
       <c r="G40" t="str">
-        <f t="shared" ref="G40:G42" si="21">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B40)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B40)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H40" t="s">
@@ -5066,7 +5066,7 @@
         <v>79</v>
       </c>
       <c r="L40" t="str">
-        <f t="shared" ref="L40:L42" si="22">B40&amp;"."&amp;C40</f>
+        <f>B40&amp;"."&amp;C40</f>
         <v>Condition.asserted-date</v>
       </c>
       <c r="M40" t="s">
@@ -5083,7 +5083,7 @@
       </c>
       <c r="AA40" s="9"/>
       <c r="AB40" t="str">
-        <f t="shared" ref="AB40:AB42" si="23">"SearchParameter-us-core-"&amp;LOWER((B40)&amp;"-"&amp;C40&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B40)&amp;"-"&amp;C40&amp;".html")</f>
         <v>SearchParameter-us-core-condition-asserted-date.html</v>
       </c>
     </row>
@@ -5107,7 +5107,7 @@
         <v>487</v>
       </c>
       <c r="G41" t="str">
-        <f t="shared" si="21"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B41)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H41" t="s">
@@ -5120,7 +5120,7 @@
         <v>79</v>
       </c>
       <c r="L41" t="str">
-        <f t="shared" si="22"/>
+        <f>B41&amp;"."&amp;C41</f>
         <v>Condition.recorded-date</v>
       </c>
       <c r="M41" t="s">
@@ -5137,7 +5137,7 @@
       </c>
       <c r="AA41" s="9"/>
       <c r="AB41" t="str">
-        <f t="shared" si="23"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B41)&amp;"-"&amp;C41&amp;".html")</f>
         <v>SearchParameter-us-core-condition-recorded-date.html</v>
       </c>
     </row>
@@ -5161,7 +5161,7 @@
         <v>487</v>
       </c>
       <c r="G42" t="str">
-        <f t="shared" si="21"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B42)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H42" t="s">
@@ -5174,7 +5174,7 @@
         <v>79</v>
       </c>
       <c r="L42" t="str">
-        <f t="shared" si="22"/>
+        <f>B42&amp;"."&amp;C42</f>
         <v>Condition.abatement-date</v>
       </c>
       <c r="M42" t="s">
@@ -5191,7 +5191,7 @@
       </c>
       <c r="AA42" s="9"/>
       <c r="AB42" t="str">
-        <f t="shared" si="23"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B42)&amp;"-"&amp;C42&amp;".html")</f>
         <v>SearchParameter-us-core-condition-abatement-date.html</v>
       </c>
     </row>
@@ -5215,7 +5215,7 @@
         <v>489</v>
       </c>
       <c r="G43" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B43)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H43" t="s">
@@ -5228,7 +5228,7 @@
         <v>57</v>
       </c>
       <c r="L43" t="str">
-        <f t="shared" si="20"/>
+        <f>B43&amp;"."&amp;C43</f>
         <v>Condition.code</v>
       </c>
       <c r="M43" t="s">
@@ -5241,7 +5241,7 @@
       <c r="Z43" s="4"/>
       <c r="AA43" s="9"/>
       <c r="AB43" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B43)&amp;"-"&amp;C43&amp;".html")</f>
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
@@ -5265,7 +5265,7 @@
         <v>486</v>
       </c>
       <c r="G44" t="str">
-        <f t="shared" ref="G44" si="24">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B44)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B44)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H44" t="s">
@@ -5278,7 +5278,7 @@
         <v>91</v>
       </c>
       <c r="L44" t="str">
-        <f t="shared" si="20"/>
+        <f>B44&amp;"."&amp;C44</f>
         <v>Condition.encounter</v>
       </c>
       <c r="M44" t="s">
@@ -5299,7 +5299,7 @@
         <v>Fetches a bundle of all Condition resources for the specified patient</v>
       </c>
       <c r="AB44" t="str">
-        <f t="shared" ref="AB44" si="25">"SearchParameter-us-core-"&amp;LOWER((B44)&amp;"-"&amp;SUBSTITUTE(C44,"_","")&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B44)&amp;"-"&amp;SUBSTITUTE(C44,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-condition-encounter.html</v>
       </c>
     </row>
@@ -5323,7 +5323,7 @@
         <v>486</v>
       </c>
       <c r="G45" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B45)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="H45" t="s">
@@ -5336,7 +5336,7 @@
         <v>91</v>
       </c>
       <c r="L45" t="str">
-        <f t="shared" si="20"/>
+        <f>B45&amp;"."&amp;C45</f>
         <v>Immunization.patient</v>
       </c>
       <c r="M45" t="s">
@@ -5382,7 +5382,7 @@
         <v>489</v>
       </c>
       <c r="G46" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B46)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="H46" t="s">
@@ -5395,7 +5395,7 @@
         <v>57</v>
       </c>
       <c r="L46" t="str">
-        <f t="shared" si="20"/>
+        <f>B46&amp;"."&amp;C46</f>
         <v>Immunization.status</v>
       </c>
       <c r="M46" t="s">
@@ -5408,7 +5408,7 @@
       <c r="Z46" s="4"/>
       <c r="AA46" s="9"/>
       <c r="AB46" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B46)&amp;"-"&amp;C46&amp;".html")</f>
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
@@ -5432,7 +5432,7 @@
         <v>487</v>
       </c>
       <c r="G47" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B47)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="H47" t="s">
@@ -5445,7 +5445,7 @@
         <v>79</v>
       </c>
       <c r="L47" t="str">
-        <f t="shared" si="20"/>
+        <f>B47&amp;"."&amp;C47</f>
         <v>Immunization.date</v>
       </c>
       <c r="M47" t="s">
@@ -5462,7 +5462,7 @@
       </c>
       <c r="AA47" s="9"/>
       <c r="AB47" t="str">
-        <f t="shared" si="5"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B47)&amp;"-"&amp;C47&amp;".html")</f>
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
@@ -5483,7 +5483,7 @@
         <v>1</v>
       </c>
       <c r="G48" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B48)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H48" t="s">
@@ -5515,7 +5515,7 @@
         <v>277</v>
       </c>
       <c r="AB48" t="str">
-        <f t="shared" ref="AB48" si="26">"SearchParameter-us-core-"&amp;LOWER((B48)&amp;"-"&amp;C48&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B48)&amp;"-"&amp;C48&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
@@ -5539,7 +5539,7 @@
         <v>489</v>
       </c>
       <c r="G49" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B49)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H49" t="s">
@@ -5552,7 +5552,7 @@
         <v>57</v>
       </c>
       <c r="L49" t="str">
-        <f t="shared" ref="L49:L75" si="27">B49&amp;"."&amp;C49</f>
+        <f>B49&amp;"."&amp;C49</f>
         <v>DocumentReference.status</v>
       </c>
       <c r="M49" t="s">
@@ -5568,7 +5568,7 @@
       <c r="Z49" s="4"/>
       <c r="AA49" s="9"/>
       <c r="AB49" t="str">
-        <f t="shared" ref="AB49:AB78" si="28">"SearchParameter-us-core-"&amp;LOWER((B49)&amp;"-"&amp;C49&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B49)&amp;"-"&amp;C49&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
@@ -5592,7 +5592,7 @@
         <v>486</v>
       </c>
       <c r="G50" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B50)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H50" t="s">
@@ -5605,7 +5605,7 @@
         <v>91</v>
       </c>
       <c r="L50" t="str">
-        <f t="shared" si="27"/>
+        <f>B50&amp;"."&amp;C50</f>
         <v>DocumentReference.patient</v>
       </c>
       <c r="M50" t="s">
@@ -5627,7 +5627,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient. See the implementation notes above for how to access the actual document.</v>
       </c>
       <c r="AB50" t="str">
-        <f t="shared" ref="AB50:AB53" si="29">"SearchParameter-us-core-"&amp;LOWER((B50)&amp;"-"&amp;C50&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B50)&amp;"-"&amp;C50&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
@@ -5651,7 +5651,7 @@
         <v>489</v>
       </c>
       <c r="G51" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B51)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H51" t="s">
@@ -5664,7 +5664,7 @@
         <v>57</v>
       </c>
       <c r="L51" t="str">
-        <f t="shared" ref="L51:L53" si="30">B51&amp;"."&amp;C51</f>
+        <f>B51&amp;"."&amp;C51</f>
         <v>DocumentReference.category</v>
       </c>
       <c r="M51" t="s">
@@ -5677,7 +5677,7 @@
       <c r="Z51" s="4"/>
       <c r="AA51" s="9"/>
       <c r="AB51" t="str">
-        <f t="shared" si="29"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B51)&amp;"-"&amp;C51&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
@@ -5701,7 +5701,7 @@
         <v>489</v>
       </c>
       <c r="G52" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B52)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H52" t="s">
@@ -5714,7 +5714,7 @@
         <v>57</v>
       </c>
       <c r="L52" t="str">
-        <f t="shared" si="30"/>
+        <f>B52&amp;"."&amp;C52</f>
         <v>DocumentReference.type</v>
       </c>
       <c r="M52" t="s">
@@ -5727,7 +5727,7 @@
       <c r="Z52" s="4"/>
       <c r="AA52" s="9"/>
       <c r="AB52" t="str">
-        <f t="shared" si="29"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B52)&amp;"-"&amp;C52&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
@@ -5751,7 +5751,7 @@
         <v>487</v>
       </c>
       <c r="G53" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B53)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H53" t="s">
@@ -5764,7 +5764,7 @@
         <v>79</v>
       </c>
       <c r="L53" t="str">
-        <f t="shared" si="30"/>
+        <f>B53&amp;"."&amp;C53</f>
         <v>DocumentReference.date</v>
       </c>
       <c r="M53" t="s">
@@ -5781,7 +5781,7 @@
       </c>
       <c r="AA53" s="9"/>
       <c r="AB53" t="str">
-        <f t="shared" si="29"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B53)&amp;"-"&amp;C53&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
@@ -5805,7 +5805,7 @@
         <v>487</v>
       </c>
       <c r="G54" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B54)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H54" t="s">
@@ -5834,7 +5834,7 @@
       </c>
       <c r="AA54" s="9"/>
       <c r="AB54" t="str">
-        <f t="shared" ref="AB54" si="31">"SearchParameter-us-core-"&amp;LOWER((B54)&amp;"-"&amp;C54&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B54)&amp;"-"&amp;C54&amp;".html")</f>
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
@@ -5858,7 +5858,7 @@
         <v>489</v>
       </c>
       <c r="G55" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B55)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="H55" t="s">
@@ -5871,7 +5871,7 @@
         <v>57</v>
       </c>
       <c r="L55" t="str">
-        <f t="shared" ref="L55:L59" si="32">B55&amp;"."&amp;C55</f>
+        <f>B55&amp;"."&amp;C55</f>
         <v>DiagnosticReport.status</v>
       </c>
       <c r="M55" t="s">
@@ -5924,7 +5924,7 @@
         <v>91</v>
       </c>
       <c r="L56" t="str">
-        <f t="shared" si="32"/>
+        <f>B56&amp;"."&amp;C56</f>
         <v>DiagnosticReport.patient</v>
       </c>
       <c r="M56" t="s">
@@ -5970,7 +5970,7 @@
         <v>489</v>
       </c>
       <c r="G57" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B57)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="H57" t="s">
@@ -5983,7 +5983,7 @@
         <v>57</v>
       </c>
       <c r="L57" t="str">
-        <f t="shared" si="32"/>
+        <f>B57&amp;"."&amp;C57</f>
         <v>DiagnosticReport.category</v>
       </c>
       <c r="M57" t="s">
@@ -6020,7 +6020,7 @@
         <v>489</v>
       </c>
       <c r="G58" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B58)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="H58" t="s">
@@ -6033,7 +6033,7 @@
         <v>57</v>
       </c>
       <c r="L58" t="str">
-        <f t="shared" si="32"/>
+        <f>B58&amp;"."&amp;C58</f>
         <v>DiagnosticReport.code</v>
       </c>
       <c r="M58" t="s">
@@ -6073,7 +6073,7 @@
         <v>487</v>
       </c>
       <c r="G59" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B59)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="H59" t="s">
@@ -6086,7 +6086,7 @@
         <v>79</v>
       </c>
       <c r="L59" t="str">
-        <f t="shared" si="32"/>
+        <f>B59&amp;"."&amp;C59</f>
         <v>DiagnosticReport.date</v>
       </c>
       <c r="M59" t="s">
@@ -6127,7 +6127,7 @@
         <v>489</v>
       </c>
       <c r="G60" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B60)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="H60" t="s">
@@ -6140,7 +6140,7 @@
         <v>57</v>
       </c>
       <c r="L60" t="str">
-        <f t="shared" si="27"/>
+        <f>B60&amp;"."&amp;C60</f>
         <v>Goal.lifecycle-status</v>
       </c>
       <c r="M60" t="s">
@@ -6153,7 +6153,7 @@
       <c r="Z60" s="4"/>
       <c r="AA60" s="9"/>
       <c r="AB60" t="str">
-        <f t="shared" si="28"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B60)&amp;"-"&amp;C60&amp;".html")</f>
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
@@ -6177,7 +6177,7 @@
         <v>486</v>
       </c>
       <c r="G61" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B61)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="H61" t="s">
@@ -6190,7 +6190,7 @@
         <v>91</v>
       </c>
       <c r="L61" t="str">
-        <f t="shared" si="27"/>
+        <f>B61&amp;"."&amp;C61</f>
         <v>Goal.patient</v>
       </c>
       <c r="M61" t="s">
@@ -6212,7 +6212,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient</v>
       </c>
       <c r="AB61" t="str">
-        <f t="shared" ref="AB61:AB62" si="33">"SearchParameter-us-core-"&amp;LOWER((B61)&amp;"-"&amp;C61&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B61)&amp;"-"&amp;C61&amp;".html")</f>
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
@@ -6236,7 +6236,7 @@
         <v>488</v>
       </c>
       <c r="G62" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B62)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="H62" t="s">
@@ -6249,7 +6249,7 @@
         <v>79</v>
       </c>
       <c r="L62" t="str">
-        <f t="shared" ref="L62" si="34">B62&amp;"."&amp;C62</f>
+        <f>B62&amp;"."&amp;C62</f>
         <v>Goal.target-date</v>
       </c>
       <c r="M62" t="s">
@@ -6266,7 +6266,7 @@
       </c>
       <c r="AA62" s="9"/>
       <c r="AB62" t="str">
-        <f t="shared" si="33"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B62)&amp;"-"&amp;C62&amp;".html")</f>
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
@@ -6290,7 +6290,7 @@
         <v>489</v>
       </c>
       <c r="G63" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B63)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H63" t="s">
@@ -6303,7 +6303,7 @@
         <v>57</v>
       </c>
       <c r="L63" t="str">
-        <f t="shared" si="27"/>
+        <f>B63&amp;"."&amp;C63</f>
         <v>MedicationRequest.status</v>
       </c>
       <c r="M63" t="s">
@@ -6319,7 +6319,7 @@
       <c r="Z63" s="4"/>
       <c r="AA63" s="9"/>
       <c r="AB63" t="str">
-        <f t="shared" si="28"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B63)&amp;"-"&amp;C63&amp;".html")</f>
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
@@ -6343,7 +6343,7 @@
         <v>489</v>
       </c>
       <c r="G64" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B64)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H64" t="s">
@@ -6356,7 +6356,7 @@
         <v>57</v>
       </c>
       <c r="L64" t="str">
-        <f t="shared" ref="L64" si="35">B64&amp;"."&amp;C64</f>
+        <f>B64&amp;"."&amp;C64</f>
         <v>MedicationRequest.intent</v>
       </c>
       <c r="M64" t="s">
@@ -6372,7 +6372,7 @@
       <c r="Z64" s="4"/>
       <c r="AA64" s="9"/>
       <c r="AB64" t="str">
-        <f t="shared" ref="AB64" si="36">"SearchParameter-us-core-"&amp;LOWER((B64)&amp;"-"&amp;C64&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B64)&amp;"-"&amp;C64&amp;".html")</f>
         <v>SearchParameter-us-core-medicationrequest-intent.html</v>
       </c>
     </row>
@@ -6396,7 +6396,7 @@
         <v>486</v>
       </c>
       <c r="G65" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B65)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H65" t="s">
@@ -6409,7 +6409,7 @@
         <v>91</v>
       </c>
       <c r="L65" t="str">
-        <f t="shared" si="27"/>
+        <f>B65&amp;"."&amp;C65</f>
         <v>MedicationRequest.patient</v>
       </c>
       <c r="M65" t="s">
@@ -6425,7 +6425,7 @@
       <c r="Z65" s="9"/>
       <c r="AA65" s="9"/>
       <c r="AB65" t="str">
-        <f t="shared" ref="AB65" si="37">"SearchParameter-us-core-"&amp;LOWER((B65)&amp;"-"&amp;C65&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B65)&amp;"-"&amp;C65&amp;".html")</f>
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
@@ -6449,7 +6449,7 @@
         <v>486</v>
       </c>
       <c r="G66" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B66)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H66" t="s">
@@ -6462,7 +6462,7 @@
         <v>91</v>
       </c>
       <c r="L66" t="str">
-        <f t="shared" ref="L66" si="38">B66&amp;"."&amp;C66</f>
+        <f>B66&amp;"."&amp;C66</f>
         <v>MedicationRequest.encounter</v>
       </c>
       <c r="M66" t="s">
@@ -6476,7 +6476,7 @@
       <c r="Z66" s="9"/>
       <c r="AA66" s="9"/>
       <c r="AB66" t="str">
-        <f t="shared" ref="AB66" si="39">"SearchParameter-us-core-"&amp;LOWER((B66)&amp;"-"&amp;C66&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B66)&amp;"-"&amp;C66&amp;".html")</f>
         <v>SearchParameter-us-core-medicationrequest-encounter.html</v>
       </c>
     </row>
@@ -6500,7 +6500,7 @@
         <v>487</v>
       </c>
       <c r="G67" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B67)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H67" t="s">
@@ -6513,7 +6513,7 @@
         <v>79</v>
       </c>
       <c r="L67" t="str">
-        <f t="shared" ref="L67" si="40">B67&amp;"."&amp;C67</f>
+        <f>B67&amp;"."&amp;C67</f>
         <v>MedicationRequest.authoredon</v>
       </c>
       <c r="M67" t="s">
@@ -6530,7 +6530,7 @@
       </c>
       <c r="AA67" s="9"/>
       <c r="AB67" t="str">
-        <f t="shared" si="28"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B67)&amp;"-"&amp;C67&amp;".html")</f>
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
@@ -6554,7 +6554,7 @@
         <v>489</v>
       </c>
       <c r="G68" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B68)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="H68" t="s">
@@ -6607,7 +6607,7 @@
         <v>486</v>
       </c>
       <c r="G69" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B69)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="H69" t="s">
@@ -6620,7 +6620,7 @@
         <v>91</v>
       </c>
       <c r="L69" t="str">
-        <f t="shared" si="27"/>
+        <f>B69&amp;"."&amp;C69</f>
         <v>!MedicationStatement.patient</v>
       </c>
       <c r="M69" t="s">
@@ -6641,7 +6641,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient.W63+X63 Mandatory for client to support the _include parameter. Optional for server to support the _include parameter.</v>
       </c>
       <c r="AB69" t="str">
-        <f t="shared" ref="AB69:AB70" si="41">"SearchParameter-us-core-"&amp;LOWER((B69)&amp;"-"&amp;C69&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B69)&amp;"-"&amp;C69&amp;".html")</f>
         <v>SearchParameter-us-core-!medicationstatement-patient.html</v>
       </c>
     </row>
@@ -6665,7 +6665,7 @@
         <v>487</v>
       </c>
       <c r="G70" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B70)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="H70" t="s">
@@ -6678,7 +6678,7 @@
         <v>79</v>
       </c>
       <c r="L70" t="str">
-        <f t="shared" ref="L70" si="42">B70&amp;"."&amp;C70</f>
+        <f>B70&amp;"."&amp;C70</f>
         <v>!MedicationStatement.effective</v>
       </c>
       <c r="M70" t="s">
@@ -6695,7 +6695,7 @@
       </c>
       <c r="AA70" s="9"/>
       <c r="AB70" t="str">
-        <f t="shared" si="41"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B70)&amp;"-"&amp;C70&amp;".html")</f>
         <v>SearchParameter-us-core-!medicationstatement-effective.html</v>
       </c>
     </row>
@@ -6719,7 +6719,7 @@
         <v>489</v>
       </c>
       <c r="G71" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B71)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="H71" t="s">
@@ -6732,7 +6732,7 @@
         <v>57</v>
       </c>
       <c r="L71" t="str">
-        <f t="shared" si="27"/>
+        <f>B71&amp;"."&amp;C71</f>
         <v>Procedure.status</v>
       </c>
       <c r="M71" t="s">
@@ -6748,7 +6748,7 @@
       <c r="Z71" s="4"/>
       <c r="AA71" s="9"/>
       <c r="AB71" t="str">
-        <f t="shared" si="28"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B71)&amp;"-"&amp;C71&amp;".html")</f>
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
@@ -6772,7 +6772,7 @@
         <v>486</v>
       </c>
       <c r="G72" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B72)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="H72" t="s">
@@ -6785,7 +6785,7 @@
         <v>91</v>
       </c>
       <c r="L72" t="str">
-        <f t="shared" si="27"/>
+        <f>B72&amp;"."&amp;C72</f>
         <v>Procedure.patient</v>
       </c>
       <c r="M72" t="s">
@@ -6806,7 +6806,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient</v>
       </c>
       <c r="AB72" t="str">
-        <f t="shared" ref="AB72:AB74" si="43">"SearchParameter-us-core-"&amp;LOWER((B72)&amp;"-"&amp;C72&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B72)&amp;"-"&amp;C72&amp;".html")</f>
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
@@ -6830,7 +6830,7 @@
         <v>487</v>
       </c>
       <c r="G73" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B73)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="H73" t="s">
@@ -6843,7 +6843,7 @@
         <v>79</v>
       </c>
       <c r="L73" t="str">
-        <f t="shared" ref="L73:L74" si="44">B73&amp;"."&amp;C73</f>
+        <f>B73&amp;"."&amp;C73</f>
         <v>Procedure.date</v>
       </c>
       <c r="M73" t="s">
@@ -6860,7 +6860,7 @@
       </c>
       <c r="AA73" s="9"/>
       <c r="AB73" t="str">
-        <f t="shared" si="43"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B73)&amp;"-"&amp;C73&amp;".html")</f>
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
@@ -6884,7 +6884,7 @@
         <v>489</v>
       </c>
       <c r="G74" t="str">
-        <f t="shared" si="1"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B74)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="H74" t="s">
@@ -6897,7 +6897,7 @@
         <v>57</v>
       </c>
       <c r="L74" t="str">
-        <f t="shared" si="44"/>
+        <f>B74&amp;"."&amp;C74</f>
         <v>Procedure.code</v>
       </c>
       <c r="M74" t="s">
@@ -6913,7 +6913,7 @@
       <c r="Z74" s="4"/>
       <c r="AA74" s="9"/>
       <c r="AB74" t="str">
-        <f t="shared" si="43"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B74)&amp;"-"&amp;C74&amp;".html")</f>
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
@@ -6937,7 +6937,7 @@
         <v>489</v>
       </c>
       <c r="G75" t="str">
-        <f t="shared" ref="G75:G106" si="45">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B75)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B75)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H75" t="s">
@@ -6950,7 +6950,7 @@
         <v>57</v>
       </c>
       <c r="L75" t="str">
-        <f t="shared" si="27"/>
+        <f>B75&amp;"."&amp;C75</f>
         <v>Observation.status</v>
       </c>
       <c r="M75" t="s">
@@ -6966,7 +6966,7 @@
       <c r="Z75" s="4"/>
       <c r="AA75" s="9"/>
       <c r="AB75" t="str">
-        <f t="shared" si="28"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B75)&amp;"-"&amp;C75&amp;".html")</f>
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
@@ -6990,7 +6990,7 @@
         <v>489</v>
       </c>
       <c r="G76" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B76)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H76" t="s">
@@ -7003,7 +7003,7 @@
         <v>57</v>
       </c>
       <c r="L76" t="str">
-        <f t="shared" ref="L76:L78" si="46">B76&amp;"."&amp;C76</f>
+        <f>B76&amp;"."&amp;C76</f>
         <v>Observation.category</v>
       </c>
       <c r="M76" t="s">
@@ -7016,7 +7016,7 @@
       <c r="Z76" s="4"/>
       <c r="AA76" s="9"/>
       <c r="AB76" t="str">
-        <f t="shared" si="28"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B76)&amp;"-"&amp;C76&amp;".html")</f>
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
@@ -7040,7 +7040,7 @@
         <v>489</v>
       </c>
       <c r="G77" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B77)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H77" t="s">
@@ -7053,7 +7053,7 @@
         <v>57</v>
       </c>
       <c r="L77" t="str">
-        <f t="shared" si="46"/>
+        <f>B77&amp;"."&amp;C77</f>
         <v>Observation.code</v>
       </c>
       <c r="M77" t="s">
@@ -7069,7 +7069,7 @@
       <c r="Z77" s="4"/>
       <c r="AA77" s="9"/>
       <c r="AB77" t="str">
-        <f t="shared" si="28"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B77)&amp;"-"&amp;C77&amp;".html")</f>
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
@@ -7093,7 +7093,7 @@
         <v>487</v>
       </c>
       <c r="G78" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B78)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H78" t="s">
@@ -7106,7 +7106,7 @@
         <v>79</v>
       </c>
       <c r="L78" t="str">
-        <f t="shared" si="46"/>
+        <f>B78&amp;"."&amp;C78</f>
         <v>Observation.date</v>
       </c>
       <c r="M78" t="s">
@@ -7123,7 +7123,7 @@
       </c>
       <c r="AA78" s="9"/>
       <c r="AB78" t="str">
-        <f t="shared" si="28"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B78)&amp;"-"&amp;C78&amp;".html")</f>
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
@@ -7147,7 +7147,7 @@
         <v>486</v>
       </c>
       <c r="G79" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B79)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H79" t="s">
@@ -7206,7 +7206,7 @@
         <v>489</v>
       </c>
       <c r="G80" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B80)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="H80" t="s">
@@ -7219,7 +7219,7 @@
         <v>57</v>
       </c>
       <c r="L80" t="str">
-        <f t="shared" ref="L80:L82" si="47">B80&amp;"."&amp;C80</f>
+        <f>B80&amp;"."&amp;C80</f>
         <v>CarePlan.category</v>
       </c>
       <c r="M80" t="s">
@@ -7232,7 +7232,7 @@
       <c r="Z80" s="4"/>
       <c r="AA80" s="9"/>
       <c r="AB80" t="str">
-        <f t="shared" ref="AB80:AB82" si="48">"SearchParameter-us-core-"&amp;LOWER((B80)&amp;"-"&amp;C80&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B80)&amp;"-"&amp;C80&amp;".html")</f>
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
@@ -7256,7 +7256,7 @@
         <v>489</v>
       </c>
       <c r="G81" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B81)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!careplan</v>
       </c>
       <c r="H81" t="s">
@@ -7269,7 +7269,7 @@
         <v>57</v>
       </c>
       <c r="L81" t="str">
-        <f t="shared" si="47"/>
+        <f>B81&amp;"."&amp;C81</f>
         <v>!CarePlan.code</v>
       </c>
       <c r="M81" t="s">
@@ -7282,7 +7282,7 @@
       <c r="Z81" s="4"/>
       <c r="AA81" s="9"/>
       <c r="AB81" t="str">
-        <f t="shared" si="48"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B81)&amp;"-"&amp;C81&amp;".html")</f>
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
@@ -7306,7 +7306,7 @@
         <v>487</v>
       </c>
       <c r="G82" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B82)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="H82" t="s">
@@ -7319,7 +7319,7 @@
         <v>79</v>
       </c>
       <c r="L82" t="str">
-        <f t="shared" si="47"/>
+        <f>B82&amp;"."&amp;C82</f>
         <v>CarePlan.date</v>
       </c>
       <c r="M82" t="s">
@@ -7336,7 +7336,7 @@
       </c>
       <c r="AA82" s="9"/>
       <c r="AB82" t="str">
-        <f t="shared" si="48"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B82)&amp;"-"&amp;C82&amp;".html")</f>
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
@@ -7360,7 +7360,7 @@
         <v>486</v>
       </c>
       <c r="G83" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B83)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="H83" t="s">
@@ -7419,7 +7419,7 @@
         <v>489</v>
       </c>
       <c r="G84" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B84)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="H84" t="s">
@@ -7432,7 +7432,7 @@
         <v>57</v>
       </c>
       <c r="L84" t="str">
-        <f t="shared" ref="L84" si="49">B84&amp;"."&amp;C84</f>
+        <f>B84&amp;"."&amp;C84</f>
         <v>CarePlan.status</v>
       </c>
       <c r="M84" t="s">
@@ -7448,7 +7448,7 @@
       <c r="Z84" s="4"/>
       <c r="AA84" s="9"/>
       <c r="AB84" t="str">
-        <f t="shared" ref="AB84" si="50">"SearchParameter-us-core-"&amp;LOWER((B84)&amp;"-"&amp;C84&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B84)&amp;"-"&amp;C84&amp;".html")</f>
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
@@ -7472,7 +7472,7 @@
         <v>486</v>
       </c>
       <c r="G85" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B85)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="H85" t="s">
@@ -7531,7 +7531,7 @@
         <v>1</v>
       </c>
       <c r="G86" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B86)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
       </c>
       <c r="H86" t="s">
@@ -7544,7 +7544,7 @@
         <v>57</v>
       </c>
       <c r="L86" t="str">
-        <f t="shared" ref="L86:L87" si="51">B86&amp;"."&amp;C86</f>
+        <f>B86&amp;"."&amp;C86</f>
         <v>Practitioner._id</v>
       </c>
       <c r="M86" t="s">
@@ -7587,7 +7587,7 @@
         <v>489</v>
       </c>
       <c r="G87" t="str">
-        <f t="shared" ref="G87" si="52">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B87)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B87)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="H87" t="s">
@@ -7600,7 +7600,7 @@
         <v>57</v>
       </c>
       <c r="L87" t="str">
-        <f t="shared" si="51"/>
+        <f>B87&amp;"."&amp;C87</f>
         <v>CareTeam.status</v>
       </c>
       <c r="M87" t="s">
@@ -7616,7 +7616,7 @@
       <c r="Z87" s="4"/>
       <c r="AA87" s="9"/>
       <c r="AB87" t="str">
-        <f t="shared" ref="AB87" si="53">"SearchParameter-us-core-"&amp;LOWER((B87)&amp;"-"&amp;C87&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B87)&amp;"-"&amp;C87&amp;".html")</f>
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
@@ -7640,7 +7640,7 @@
         <v>489</v>
       </c>
       <c r="G88" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B88)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="H88" t="s">
@@ -7653,7 +7653,7 @@
         <v>57</v>
       </c>
       <c r="L88" t="str">
-        <f t="shared" ref="L88" si="54">B88&amp;"."&amp;C88</f>
+        <f>B88&amp;"."&amp;C88</f>
         <v>CareTeam.role</v>
       </c>
       <c r="M88" t="s">
@@ -7674,7 +7674,7 @@
       </c>
       <c r="AA88" s="9"/>
       <c r="AB88" t="str">
-        <f t="shared" ref="AB88" si="55">"SearchParameter-us-core-"&amp;LOWER((B88)&amp;"-"&amp;C88&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B88)&amp;"-"&amp;C88&amp;".html")</f>
         <v>SearchParameter-us-core-careteam-role.html</v>
       </c>
     </row>
@@ -7711,7 +7711,7 @@
         <v>91</v>
       </c>
       <c r="L89" t="str">
-        <f t="shared" ref="L89:L113" si="56">B89&amp;"."&amp;C89</f>
+        <f>B89&amp;"."&amp;C89</f>
         <v>Device.patient</v>
       </c>
       <c r="M89" t="s">
@@ -7733,7 +7733,7 @@
         <v>Fetches a bundle of all Device resources for the specified patient</v>
       </c>
       <c r="AB89" t="str">
-        <f t="shared" ref="AB89:AB101" si="57">"SearchParameter-us-core-"&amp;LOWER((B89)&amp;"-"&amp;C89&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B89)&amp;"-"&amp;C89&amp;".html")</f>
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
@@ -7757,7 +7757,7 @@
         <v>489</v>
       </c>
       <c r="G90" t="str">
-        <f t="shared" ref="G90:G91" si="58">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B90)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B90)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</v>
       </c>
       <c r="H90" t="s">
@@ -7770,7 +7770,7 @@
         <v>57</v>
       </c>
       <c r="L90" t="str">
-        <f t="shared" ref="L90" si="59">B90&amp;"."&amp;C90</f>
+        <f>B90&amp;"."&amp;C90</f>
         <v>Device.type</v>
       </c>
       <c r="M90" t="s">
@@ -7782,7 +7782,7 @@
       <c r="Z90" s="4"/>
       <c r="AA90" s="9"/>
       <c r="AB90" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B90)&amp;"-"&amp;C90&amp;".html")</f>
         <v>SearchParameter-us-core-device-type.html</v>
       </c>
     </row>
@@ -7806,7 +7806,7 @@
         <v>489</v>
       </c>
       <c r="G91" t="str">
-        <f t="shared" si="58"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B91)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</v>
       </c>
       <c r="H91" t="s">
@@ -7819,7 +7819,7 @@
         <v>57</v>
       </c>
       <c r="L91" t="str">
-        <f t="shared" ref="L91" si="60">B91&amp;"."&amp;C91</f>
+        <f>B91&amp;"."&amp;C91</f>
         <v>Device.status</v>
       </c>
       <c r="M91" t="s">
@@ -7834,7 +7834,7 @@
       <c r="Z91" s="4"/>
       <c r="AA91" s="9"/>
       <c r="AB91" t="str">
-        <f t="shared" ref="AB91" si="61">"SearchParameter-us-core-"&amp;LOWER((B91)&amp;"-"&amp;C91&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B91)&amp;"-"&amp;C91&amp;".html")</f>
         <v>SearchParameter-us-core-device-status.html</v>
       </c>
     </row>
@@ -7855,7 +7855,7 @@
         <v>1</v>
       </c>
       <c r="G92" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B92)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H92" t="s">
@@ -7868,7 +7868,7 @@
         <v>64</v>
       </c>
       <c r="L92" t="str">
-        <f t="shared" si="56"/>
+        <f>B92&amp;"."&amp;C92</f>
         <v>Location.name</v>
       </c>
       <c r="M92" t="s">
@@ -7889,7 +7889,7 @@
         <v>Fetches a bundle of all Location resources that match the name</v>
       </c>
       <c r="AB92" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B92)&amp;"-"&amp;C92&amp;".html")</f>
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
@@ -7910,7 +7910,7 @@
         <v>1</v>
       </c>
       <c r="G93" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B93)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H93" t="s">
@@ -7923,7 +7923,7 @@
         <v>64</v>
       </c>
       <c r="L93" t="str">
-        <f t="shared" si="56"/>
+        <f>B93&amp;"."&amp;C93</f>
         <v>Location.address</v>
       </c>
       <c r="M93" t="s">
@@ -7944,7 +7944,7 @@
         <v>Fetches a bundle of all Location resources that match the address string</v>
       </c>
       <c r="AB93" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B93)&amp;"-"&amp;C93&amp;".html")</f>
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
@@ -7965,7 +7965,7 @@
         <v>1</v>
       </c>
       <c r="G94" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B94)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H94" t="s">
@@ -7978,7 +7978,7 @@
         <v>64</v>
       </c>
       <c r="L94" t="str">
-        <f t="shared" si="56"/>
+        <f>B94&amp;"."&amp;C94</f>
         <v>Location.address-city</v>
       </c>
       <c r="M94" t="s">
@@ -7999,7 +7999,7 @@
         <v>Fetches a bundle of all Location resources for the city</v>
       </c>
       <c r="AB94" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B94)&amp;"-"&amp;C94&amp;".html")</f>
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
@@ -8020,7 +8020,7 @@
         <v>1</v>
       </c>
       <c r="G95" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B95)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H95" t="s">
@@ -8033,7 +8033,7 @@
         <v>64</v>
       </c>
       <c r="L95" t="str">
-        <f t="shared" si="56"/>
+        <f>B95&amp;"."&amp;C95</f>
         <v>Location.address-state</v>
       </c>
       <c r="M95" t="s">
@@ -8053,7 +8053,7 @@
         <v>Fetches a bundle of all Location resources for the state</v>
       </c>
       <c r="AB95" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B95)&amp;"-"&amp;C95&amp;".html")</f>
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
@@ -8074,7 +8074,7 @@
         <v>1</v>
       </c>
       <c r="G96" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B96)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H96" t="s">
@@ -8087,7 +8087,7 @@
         <v>64</v>
       </c>
       <c r="L96" t="str">
-        <f t="shared" si="56"/>
+        <f>B96&amp;"."&amp;C96</f>
         <v>Location.address-postalcode</v>
       </c>
       <c r="M96" t="s">
@@ -8108,7 +8108,7 @@
         <v>Fetches a bundle of all Location resources for the ZIP code</v>
       </c>
       <c r="AB96" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B96)&amp;"-"&amp;C96&amp;".html")</f>
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
@@ -8129,7 +8129,7 @@
         <v>1</v>
       </c>
       <c r="G97" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B97)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization</v>
       </c>
       <c r="H97" t="s">
@@ -8142,7 +8142,7 @@
         <v>64</v>
       </c>
       <c r="L97" t="str">
-        <f t="shared" si="56"/>
+        <f>B97&amp;"."&amp;C97</f>
         <v>Organization.name</v>
       </c>
       <c r="M97" t="s">
@@ -8163,7 +8163,7 @@
         <v>Fetches a bundle of all Organization resources that match the name</v>
       </c>
       <c r="AB97" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B97)&amp;"-"&amp;C97&amp;".html")</f>
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
@@ -8184,7 +8184,7 @@
         <v>1</v>
       </c>
       <c r="G98" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B98)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization</v>
       </c>
       <c r="H98" t="s">
@@ -8197,7 +8197,7 @@
         <v>64</v>
       </c>
       <c r="L98" t="str">
-        <f t="shared" si="56"/>
+        <f>B98&amp;"."&amp;C98</f>
         <v>Organization.address</v>
       </c>
       <c r="M98" t="s">
@@ -8218,7 +8218,7 @@
         <v>Fetches a bundle of all Organization resources that match the address string</v>
       </c>
       <c r="AB98" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B98)&amp;"-"&amp;C98&amp;".html")</f>
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
@@ -8239,7 +8239,7 @@
         <v>1</v>
       </c>
       <c r="G99" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B99)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!organization</v>
       </c>
       <c r="H99" t="s">
@@ -8252,7 +8252,7 @@
         <v>64</v>
       </c>
       <c r="L99" t="str">
-        <f t="shared" si="56"/>
+        <f>B99&amp;"."&amp;C99</f>
         <v>!Organization.address-city</v>
       </c>
       <c r="M99" t="s">
@@ -8273,7 +8273,7 @@
         <v>Fetches a bundle of all !Organization resources for the city</v>
       </c>
       <c r="AB99" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B99)&amp;"-"&amp;C99&amp;".html")</f>
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
@@ -8294,7 +8294,7 @@
         <v>1</v>
       </c>
       <c r="G100" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B100)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!organization</v>
       </c>
       <c r="H100" t="s">
@@ -8307,7 +8307,7 @@
         <v>64</v>
       </c>
       <c r="L100" t="str">
-        <f t="shared" si="56"/>
+        <f>B100&amp;"."&amp;C100</f>
         <v>!Organization.adress-state</v>
       </c>
       <c r="M100" t="s">
@@ -8328,7 +8328,7 @@
         <v>Fetches a bundle of all !Organization resources for the state</v>
       </c>
       <c r="AB100" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B100)&amp;"-"&amp;C100&amp;".html")</f>
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
@@ -8349,7 +8349,7 @@
         <v>1</v>
       </c>
       <c r="G101" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B101)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!organization</v>
       </c>
       <c r="H101" t="s">
@@ -8362,7 +8362,7 @@
         <v>64</v>
       </c>
       <c r="L101" t="str">
-        <f t="shared" si="56"/>
+        <f>B101&amp;"."&amp;C101</f>
         <v>!Organization.address-postalcode</v>
       </c>
       <c r="M101" t="s">
@@ -8383,7 +8383,7 @@
         <v>Fetches a bundle of all !Organization resources for the ZIP code</v>
       </c>
       <c r="AB101" t="str">
-        <f t="shared" si="57"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B101)&amp;"-"&amp;C101&amp;".html")</f>
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
@@ -8404,7 +8404,7 @@
         <v>1</v>
       </c>
       <c r="G102" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B102)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
       </c>
       <c r="H102" t="s">
@@ -8417,7 +8417,7 @@
         <v>64</v>
       </c>
       <c r="L102" t="str">
-        <f t="shared" si="56"/>
+        <f>B102&amp;"."&amp;C102</f>
         <v>Practitioner.name</v>
       </c>
       <c r="M102" t="s">
@@ -8438,7 +8438,7 @@
         <v>Fetches a bundle of all Practitioner resources matching the name</v>
       </c>
       <c r="AB102" t="str">
-        <f t="shared" ref="AB102:AB103" si="62">"SearchParameter-us-core-"&amp;LOWER((B102)&amp;"-"&amp;SUBSTITUTE(C102,"_","")&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B102)&amp;"-"&amp;SUBSTITUTE(C102,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
@@ -8462,7 +8462,7 @@
         <v>489</v>
       </c>
       <c r="G103" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B103)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
       </c>
       <c r="H103" t="s">
@@ -8475,7 +8475,7 @@
         <v>57</v>
       </c>
       <c r="L103" t="str">
-        <f t="shared" si="56"/>
+        <f>B103&amp;"."&amp;C103</f>
         <v>Practitioner.identifier</v>
       </c>
       <c r="M103" t="s">
@@ -8496,7 +8496,7 @@
         <v>Fetches a bundle containing any Practitioner resources matching the identifier</v>
       </c>
       <c r="AB103" t="str">
-        <f t="shared" si="62"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B103)&amp;"-"&amp;SUBSTITUTE(C103,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
@@ -8520,7 +8520,7 @@
         <v>489</v>
       </c>
       <c r="G104" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B104)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
       </c>
       <c r="H104" t="s">
@@ -8533,7 +8533,7 @@
         <v>57</v>
       </c>
       <c r="L104" t="str">
-        <f t="shared" si="56"/>
+        <f>B104&amp;"."&amp;C104</f>
         <v>PractitionerRole.specialty</v>
       </c>
       <c r="M104" t="s">
@@ -8557,7 +8557,7 @@
         <v>Fetches a bundle containing  PractitionerRole resources matching the specialty</v>
       </c>
       <c r="AB104" t="str">
-        <f t="shared" ref="AB104" si="63">"SearchParameter-us-core-"&amp;LOWER((B104)&amp;"-"&amp;SUBSTITUTE(C104,"_","")&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B104)&amp;"-"&amp;SUBSTITUTE(C104,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
@@ -8581,7 +8581,7 @@
         <v>486</v>
       </c>
       <c r="G105" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
       </c>
       <c r="H105" t="s">
@@ -8594,7 +8594,7 @@
         <v>91</v>
       </c>
       <c r="L105" t="str">
-        <f t="shared" si="56"/>
+        <f>B105&amp;"."&amp;C105</f>
         <v>PractitionerRole.practitioner</v>
       </c>
       <c r="M105" t="s">
@@ -8645,7 +8645,7 @@
         <v>489</v>
       </c>
       <c r="G106" t="str">
-        <f t="shared" si="45"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B106)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H106" t="s">
@@ -8658,7 +8658,7 @@
         <v>57</v>
       </c>
       <c r="L106" t="str">
-        <f t="shared" si="56"/>
+        <f>B106&amp;"."&amp;C106</f>
         <v>ServiceRequest.status</v>
       </c>
       <c r="M106" t="s">
@@ -8711,7 +8711,7 @@
         <v>91</v>
       </c>
       <c r="L107" t="str">
-        <f t="shared" si="56"/>
+        <f>B107&amp;"."&amp;C107</f>
         <v>ServiceRequest.patient</v>
       </c>
       <c r="M107" t="s">
@@ -8757,7 +8757,7 @@
         <v>489</v>
       </c>
       <c r="G108" t="str">
-        <f t="shared" ref="G108:G126" si="64">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B108)</f>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B108)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H108" t="s">
@@ -8770,7 +8770,7 @@
         <v>57</v>
       </c>
       <c r="L108" t="str">
-        <f t="shared" si="56"/>
+        <f>B108&amp;"."&amp;C108</f>
         <v>ServiceRequest.category</v>
       </c>
       <c r="M108" t="s">
@@ -8807,7 +8807,7 @@
         <v>489</v>
       </c>
       <c r="G109" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B109)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H109" t="s">
@@ -8820,7 +8820,7 @@
         <v>57</v>
       </c>
       <c r="L109" t="str">
-        <f t="shared" si="56"/>
+        <f>B109&amp;"."&amp;C109</f>
         <v>ServiceRequest.code</v>
       </c>
       <c r="M109" t="s">
@@ -8860,7 +8860,7 @@
         <v>487</v>
       </c>
       <c r="G110" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B110)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H110" t="s">
@@ -8873,7 +8873,7 @@
         <v>79</v>
       </c>
       <c r="L110" t="str">
-        <f t="shared" si="56"/>
+        <f>B110&amp;"."&amp;C110</f>
         <v>ServiceRequest.authored</v>
       </c>
       <c r="M110" t="s">
@@ -8911,7 +8911,7 @@
         <v>1</v>
       </c>
       <c r="G111" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B111)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H111" t="s">
@@ -8924,7 +8924,7 @@
         <v>57</v>
       </c>
       <c r="L111" t="str">
-        <f t="shared" si="56"/>
+        <f>B111&amp;"."&amp;C111</f>
         <v>ServiceRequest._id</v>
       </c>
       <c r="M111" t="s">
@@ -8962,7 +8962,7 @@
       </c>
       <c r="F112" s="1"/>
       <c r="G112" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B112)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="H112" t="s">
@@ -8975,7 +8975,7 @@
         <v>57</v>
       </c>
       <c r="L112" t="str">
-        <f t="shared" si="56"/>
+        <f>B112&amp;"."&amp;C112</f>
         <v>Goal.description</v>
       </c>
       <c r="M112" t="s">
@@ -8986,7 +8986,7 @@
       </c>
       <c r="AA112" s="9"/>
       <c r="AB112" t="str">
-        <f t="shared" ref="AB112" si="65">"SearchParameter-us-core-"&amp;LOWER((B112)&amp;"-"&amp;C112&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B112)&amp;"-"&amp;C112&amp;".html")</f>
         <v>SearchParameter-us-core-goal-description.html</v>
       </c>
     </row>
@@ -9007,7 +9007,7 @@
         <v>1</v>
       </c>
       <c r="G113" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B113)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
       </c>
       <c r="H113" t="s">
@@ -9020,7 +9020,7 @@
         <v>57</v>
       </c>
       <c r="L113" t="str">
-        <f t="shared" si="56"/>
+        <f>B113&amp;"."&amp;C113</f>
         <v>RelatedPerson._id</v>
       </c>
       <c r="M113" t="s">
@@ -9061,7 +9061,7 @@
         <v>486</v>
       </c>
       <c r="G114" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B114)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
       </c>
       <c r="H114" t="s">
@@ -9117,7 +9117,7 @@
         <v>1</v>
       </c>
       <c r="G115" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B115)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
       </c>
       <c r="H115" t="s">
@@ -9143,7 +9143,7 @@
         <v>56</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9154,7 +9154,7 @@
         <v>Fetches a bundle of all RelatedPerson resources matching the name</v>
       </c>
       <c r="AB115" t="str">
-        <f t="shared" ref="AB115" si="66">"SearchParameter-us-core-"&amp;LOWER((B115)&amp;"-"&amp;SUBSTITUTE(C115,"_","")&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B115)&amp;"-"&amp;SUBSTITUTE(C115,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-relatedperson-name.html</v>
       </c>
     </row>
@@ -9175,7 +9175,7 @@
         <v>1</v>
       </c>
       <c r="G116" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B116)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H116" t="s">
@@ -9188,7 +9188,7 @@
         <v>57</v>
       </c>
       <c r="L116" t="str">
-        <f t="shared" ref="L116:L126" si="67">B116&amp;"."&amp;C116</f>
+        <f>B116&amp;"."&amp;C116</f>
         <v>QuestionnaireResponse._id</v>
       </c>
       <c r="M116" t="s">
@@ -9205,7 +9205,7 @@
         <v>625</v>
       </c>
       <c r="AB116" t="str">
-        <f t="shared" ref="AB116:AB122" si="68">"SearchParameter-us-core-"&amp;LOWER((B116)&amp;"-"&amp;SUBSTITUTE(C116,"_","")&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B116)&amp;"-"&amp;SUBSTITUTE(C116,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-questionnaireresponse-id.html</v>
       </c>
     </row>
@@ -9229,7 +9229,7 @@
         <v>486</v>
       </c>
       <c r="G117" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B117)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H117" t="s">
@@ -9242,7 +9242,7 @@
         <v>91</v>
       </c>
       <c r="L117" t="str">
-        <f t="shared" si="67"/>
+        <f>B117&amp;"."&amp;C117</f>
         <v>QuestionnaireResponse.patient</v>
       </c>
       <c r="M117" t="s">
@@ -9264,7 +9264,7 @@
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient</v>
       </c>
       <c r="AB117" t="str">
-        <f t="shared" si="68"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B117)&amp;"-"&amp;SUBSTITUTE(C117,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-questionnaireresponse-patient.html</v>
       </c>
     </row>
@@ -9288,7 +9288,7 @@
         <v>489</v>
       </c>
       <c r="G118" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B118)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H118" t="s">
@@ -9301,7 +9301,7 @@
         <v>57</v>
       </c>
       <c r="L118" t="str">
-        <f t="shared" si="67"/>
+        <f>B118&amp;"."&amp;C118</f>
         <v>QuestionnaireResponse.status</v>
       </c>
       <c r="M118" t="s">
@@ -9317,7 +9317,7 @@
         <v>622</v>
       </c>
       <c r="AB118" t="str">
-        <f t="shared" si="68"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B118)&amp;"-"&amp;SUBSTITUTE(C118,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-questionnaireresponse-status.html</v>
       </c>
     </row>
@@ -9341,7 +9341,7 @@
         <v>489</v>
       </c>
       <c r="G119" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B119)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H119" t="s">
@@ -9366,7 +9366,7 @@
         <v>621</v>
       </c>
       <c r="AB119" t="str">
-        <f t="shared" si="68"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B119)&amp;"-"&amp;SUBSTITUTE(C119,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-questionnaireresponse-tag.html</v>
       </c>
     </row>
@@ -9390,7 +9390,7 @@
         <v>487</v>
       </c>
       <c r="G120" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B120)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H120" t="s">
@@ -9403,7 +9403,7 @@
         <v>79</v>
       </c>
       <c r="L120" t="str">
-        <f t="shared" si="67"/>
+        <f>B120&amp;"."&amp;C120</f>
         <v>QuestionnaireResponse.authored</v>
       </c>
       <c r="M120" t="s">
@@ -9422,7 +9422,7 @@
         <v>623</v>
       </c>
       <c r="AB120" t="str">
-        <f t="shared" si="68"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B120)&amp;"-"&amp;SUBSTITUTE(C120,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-questionnaireresponse-authored.html</v>
       </c>
     </row>
@@ -9446,7 +9446,7 @@
         <v>486</v>
       </c>
       <c r="G121" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B121)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="H121" t="s">
@@ -9459,7 +9459,7 @@
         <v>91</v>
       </c>
       <c r="L121" t="str">
-        <f t="shared" si="67"/>
+        <f>B121&amp;"."&amp;C121</f>
         <v>QuestionnaireResponse.questionnaire</v>
       </c>
       <c r="M121" t="s">
@@ -9472,7 +9472,7 @@
         <v>624</v>
       </c>
       <c r="AB121" t="str">
-        <f t="shared" si="68"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B121)&amp;"-"&amp;SUBSTITUTE(C121,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-questionnaireresponse-questionnaire.html</v>
       </c>
     </row>
@@ -9481,7 +9481,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="C122" t="s">
         <v>90</v>
@@ -9496,7 +9496,7 @@
         <v>486</v>
       </c>
       <c r="G122" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B122)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-coverage</v>
       </c>
       <c r="H122" t="s">
@@ -9512,7 +9512,7 @@
         <v>91</v>
       </c>
       <c r="L122" t="str">
-        <f t="shared" si="67"/>
+        <f>B122&amp;"."&amp;C122</f>
         <v>Coverage.patient</v>
       </c>
       <c r="M122" t="s">
@@ -9522,7 +9522,7 @@
         <v>56</v>
       </c>
       <c r="Y122" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9533,7 +9533,7 @@
         <v>Fetches a bundle of all Coverage resources for the specified patient</v>
       </c>
       <c r="AB122" t="str">
-        <f t="shared" si="68"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B122)&amp;"-"&amp;SUBSTITUTE(C122,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-coverage-patient.html</v>
       </c>
     </row>
@@ -9542,7 +9542,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C123" t="s">
         <v>62</v>
@@ -9557,7 +9557,7 @@
         <v>489</v>
       </c>
       <c r="G123" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B123)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="H123" t="s">
@@ -9573,7 +9573,7 @@
         <v>57</v>
       </c>
       <c r="L123" t="str">
-        <f t="shared" si="67"/>
+        <f>B123&amp;"."&amp;C123</f>
         <v>MedicationDispense.status</v>
       </c>
       <c r="M123" t="s">
@@ -9589,7 +9589,7 @@
       <c r="Z123" s="4"/>
       <c r="AA123" s="9"/>
       <c r="AB123" t="str">
-        <f t="shared" ref="AB123:AB126" si="69">"SearchParameter-us-core-"&amp;LOWER((B123)&amp;"-"&amp;C123&amp;".html")</f>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B123)&amp;"-"&amp;C123&amp;".html")</f>
         <v>SearchParameter-us-core-medicationdispense-status.html</v>
       </c>
     </row>
@@ -9598,7 +9598,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C124" t="s">
         <v>13</v>
@@ -9613,7 +9613,7 @@
         <v>489</v>
       </c>
       <c r="G124" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B124)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="H124" t="s">
@@ -9629,7 +9629,7 @@
         <v>57</v>
       </c>
       <c r="L124" t="str">
-        <f t="shared" si="67"/>
+        <f>B124&amp;"."&amp;C124</f>
         <v>MedicationDispense.type</v>
       </c>
       <c r="M124" t="s">
@@ -9645,7 +9645,7 @@
       <c r="Z124" s="4"/>
       <c r="AA124" s="9"/>
       <c r="AB124" t="str">
-        <f t="shared" si="69"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B124)&amp;"-"&amp;C124&amp;".html")</f>
         <v>SearchParameter-us-core-medicationdispense-type.html</v>
       </c>
     </row>
@@ -9654,7 +9654,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C125" t="s">
         <v>90</v>
@@ -9669,7 +9669,7 @@
         <v>486</v>
       </c>
       <c r="G125" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B125)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="H125" t="s">
@@ -9685,7 +9685,7 @@
         <v>91</v>
       </c>
       <c r="L125" t="str">
-        <f t="shared" si="67"/>
+        <f>B125&amp;"."&amp;C125</f>
         <v>MedicationDispense.patient</v>
       </c>
       <c r="M125" t="s">
@@ -9695,17 +9695,17 @@
         <v>56</v>
       </c>
       <c r="X125" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="Z125" s="9" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="AA125" s="9" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient.</v>
       </c>
       <c r="AB125" t="str">
-        <f t="shared" si="69"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B125)&amp;"-"&amp;C125&amp;".html")</f>
         <v>SearchParameter-us-core-medicationdispense-patient.html</v>
       </c>
     </row>
@@ -9714,10 +9714,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>678</v>
+      </c>
+      <c r="C126" t="s">
         <v>679</v>
-      </c>
-      <c r="C126" t="s">
-        <v>680</v>
       </c>
       <c r="D126" t="s">
         <v>30</v>
@@ -9729,7 +9729,7 @@
         <v>487</v>
       </c>
       <c r="G126" t="str">
-        <f t="shared" si="64"/>
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B126)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="H126" t="s">
@@ -9745,7 +9745,7 @@
         <v>79</v>
       </c>
       <c r="L126" t="str">
-        <f t="shared" si="67"/>
+        <f>B126&amp;"."&amp;C126</f>
         <v>!MedicationDispense.whenHandedOver</v>
       </c>
       <c r="M126" t="s">
@@ -9762,15 +9762,12 @@
       </c>
       <c r="AA126" s="9"/>
       <c r="AB126" t="str">
-        <f t="shared" si="69"/>
+        <f>"SearchParameter-us-core-"&amp;LOWER((B126)&amp;"-"&amp;C126&amp;".html")</f>
         <v>SearchParameter-us-core-!medicationdispense-whenhandedover.html</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:AB126" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:AA38">
-    <sortCondition ref="B1"/>
-  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -10656,7 +10653,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="F32" t="s">
         <v>70</v>
@@ -10665,10 +10662,10 @@
         <v>134</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" ref="K32" si="7">"Fetches a bundle of all "&amp;B32&amp;" resources matching the specified "&amp;SUBSTITUTE(D32,","," and ")</f>
@@ -10858,7 +10855,7 @@
         <v>150</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>538</v>
@@ -11114,7 +11111,7 @@
         <v>179</v>
       </c>
       <c r="C47" s="22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D47" t="s">
         <v>116</v>
@@ -11144,7 +11141,7 @@
         <v>179</v>
       </c>
       <c r="C48" s="22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D48" t="s">
         <v>145</v>
@@ -11177,7 +11174,7 @@
         <v>179</v>
       </c>
       <c r="C49" s="22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D49" t="s">
         <v>147</v>
@@ -11207,7 +11204,7 @@
         <v>179</v>
       </c>
       <c r="C50" s="22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D50" t="s">
         <v>194</v>
@@ -11240,7 +11237,7 @@
         <v>179</v>
       </c>
       <c r="C51" s="22" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="D51" t="s">
         <v>218</v>
@@ -11618,7 +11615,7 @@
         <v>183</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D63" t="s">
         <v>235</v>
@@ -11650,7 +11647,7 @@
         <v>183</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D64" t="s">
         <v>145</v>
@@ -11683,7 +11680,7 @@
         <v>183</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D65" t="s">
         <v>147</v>
@@ -11713,7 +11710,7 @@
         <v>183</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D66" t="s">
         <v>194</v>
@@ -11746,7 +11743,7 @@
         <v>183</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D67" t="s">
         <v>218</v>
@@ -11776,7 +11773,7 @@
         <v>310</v>
       </c>
       <c r="C68" s="22" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="D68" t="s">
         <v>116</v>
@@ -12155,7 +12152,7 @@
         <v>247</v>
       </c>
       <c r="C80" s="22" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="D80" t="s">
         <v>118</v>
@@ -12184,7 +12181,7 @@
         <v>247</v>
       </c>
       <c r="C81" s="22" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="D81" t="s">
         <v>116</v>
@@ -12199,13 +12196,13 @@
         <v>106</v>
       </c>
       <c r="I81" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>699</v>
       </c>
-      <c r="J81" s="4" t="s">
+      <c r="K81" s="4" t="s">
         <v>700</v>
-      </c>
-      <c r="K81" s="4" t="s">
-        <v>701</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -12590,7 +12587,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="12"/>
@@ -12610,10 +12607,10 @@
       </c>
       <c r="H94" s="17"/>
       <c r="I94" s="4" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12625,7 +12622,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="17" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="12"/>
@@ -12645,10 +12642,10 @@
       </c>
       <c r="H95" s="17"/>
       <c r="I95" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>684</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>685</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12660,14 +12657,14 @@
         <v>95</v>
       </c>
       <c r="B96" s="17" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D96" s="17" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E96" s="17" t="s">
         <v>56</v>
@@ -12680,10 +12677,10 @@
       </c>
       <c r="H96" s="17"/>
       <c r="I96" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12736,7 +12733,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>652</v>
+        <v>651</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -12752,7 +12749,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -12861,7 +12858,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B3" s="23" t="s">
         <v>522</v>
@@ -13015,7 +13012,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B5" t="s">
         <v>596</v>
@@ -13029,7 +13026,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>651</v>
+        <v>650</v>
       </c>
       <c r="B6" t="s">
         <v>602</v>
@@ -13043,16 +13040,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>653</v>
+      </c>
+      <c r="B7" t="s">
         <v>654</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>655</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>656</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13113,7 +13110,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B12" t="s">
         <v>354</v>
@@ -13281,16 +13278,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>669</v>
+      </c>
+      <c r="B24" t="s">
         <v>670</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
         <v>671</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13309,10 +13306,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="B26" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -13323,10 +13320,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="B27" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -13337,10 +13334,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="B28" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -13592,7 +13589,7 @@
         <v>481</v>
       </c>
       <c r="B46" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -13757,16 +13754,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
+        <v>664</v>
+      </c>
+      <c r="B58" t="s">
         <v>665</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
         <v>666</v>
-      </c>
-      <c r="D58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" t="s">
-        <v>667</v>
       </c>
     </row>
   </sheetData>
@@ -13786,14 +13783,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y65"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B24" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.5" customWidth="1"/>
     <col min="2" max="2" width="25.33203125" customWidth="1"/>
@@ -13809,7 +13803,7 @@
     <col min="22" max="25" width="38.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -13886,7 +13880,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="25.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -13909,7 +13903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="163" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>232</v>
       </c>
@@ -13932,7 +13926,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="279" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>246</v>
       </c>
@@ -13940,7 +13934,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="T4" t="s">
         <v>19</v>
@@ -13961,7 +13955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>138</v>
       </c>
@@ -13969,7 +13963,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="T5" t="s">
         <v>19</v>
@@ -13984,9 +13978,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -14004,7 +13998,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>247</v>
       </c>
@@ -14012,7 +14006,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="T7" t="s">
         <v>19</v>
@@ -14027,7 +14021,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>179</v>
       </c>
@@ -14048,7 +14042,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>178</v>
       </c>
@@ -14056,7 +14050,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>645</v>
+        <v>706</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14071,7 +14065,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -14079,7 +14073,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="T10" t="s">
         <v>19</v>
@@ -14094,7 +14088,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>180</v>
       </c>
@@ -14114,7 +14108,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>161</v>
       </c>
@@ -14137,7 +14131,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>248</v>
       </c>
@@ -14156,7 +14150,7 @@
       <c r="X13" s="14"/>
       <c r="Y13" s="14"/>
     </row>
-    <row r="14" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>343</v>
       </c>
@@ -14175,7 +14169,7 @@
       <c r="X14" s="14"/>
       <c r="Y14" s="14"/>
     </row>
-    <row r="15" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>181</v>
       </c>
@@ -14204,15 +14198,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="T16" t="s">
         <v>19</v>
@@ -14224,7 +14218,7 @@
         <v>70</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="X16" s="14" t="s">
         <v>435</v>
@@ -14233,7 +14227,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>421</v>
       </c>
@@ -14262,7 +14256,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>183</v>
       </c>
@@ -14285,7 +14279,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>258</v>
       </c>
@@ -14304,7 +14298,7 @@
       <c r="X19" s="14"/>
       <c r="Y19" s="14"/>
     </row>
-    <row r="20" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -14327,7 +14321,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>265</v>
       </c>
@@ -14343,7 +14337,7 @@
       <c r="X21" s="14"/>
       <c r="Y21" s="14"/>
     </row>
-    <row r="22" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>267</v>
       </c>
@@ -14368,7 +14362,7 @@
       <c r="X22" s="14"/>
       <c r="Y22" s="14"/>
     </row>
-    <row r="23" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>182</v>
       </c>
@@ -14391,7 +14385,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="409.6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>422</v>
       </c>
@@ -14399,7 +14393,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="T24" t="s">
         <v>19</v>
@@ -14408,7 +14402,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>608</v>
       </c>
@@ -14431,7 +14425,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>580</v>
       </c>
@@ -14451,7 +14445,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>557</v>
       </c>
@@ -14471,9 +14465,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -14487,7 +14481,7 @@
       <c r="X28" s="14"/>
       <c r="Y28" s="14"/>
     </row>
-    <row r="29" spans="1:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>432</v>
       </c>
@@ -14495,12 +14489,12 @@
         <v>70</v>
       </c>
     </row>
-    <row r="62" spans="22:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="22:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="V62" s="6"/>
       <c r="X62" s="6"/>
       <c r="Y62" s="6"/>
     </row>
-    <row r="65" spans="25:25" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="25:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y65" s="6"/>
     </row>
   </sheetData>
@@ -14637,7 +14631,7 @@
         <v>360</v>
       </c>
       <c r="F1" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
       <c r="G1" t="s">
         <v>361</v>
@@ -14667,7 +14661,7 @@
         <v>368</v>
       </c>
       <c r="P1" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="Q1" t="s">
         <v>369</v>
@@ -14709,10 +14703,10 @@
         <v>583</v>
       </c>
       <c r="AD1" t="s">
+        <v>667</v>
+      </c>
+      <c r="AE1" t="s">
         <v>668</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>669</v>
       </c>
       <c r="AF1" t="s">
         <v>434</v>

</xml_diff>

<commit_message>
qa changes update sp list
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{457BDA4A-8BA4-2C48-A2CF-37F3827468C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEAC2DB-7E17-9A42-AB18-307DECD7B951}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33980" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2677" uniqueCount="710">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2678" uniqueCount="709">
   <si>
     <t>Element</t>
   </si>
@@ -2319,9 +2319,6 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-implantable</t>
   </si>
   <si>
     <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
@@ -2525,7 +2522,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2557,7 +2554,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFill="1"/>
   </cellXfs>
@@ -3045,13 +3041,14 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9F73F9-34B4-C04F-A2E4-99114F8B7BF7}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AB126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C90" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B116" sqref="B116"/>
+      <selection pane="bottomRight" activeCell="G130" sqref="G130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3157,7 +3154,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:28" ht="19" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3174,7 +3171,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
+        <f t="shared" ref="G2:G33" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example category search</v>
       </c>
       <c r="H2" t="s">
@@ -3187,7 +3184,7 @@
         <v>57</v>
       </c>
       <c r="L2" t="str">
-        <f>B2&amp;"."&amp;C2</f>
+        <f t="shared" ref="L2:L25" si="1">B2&amp;"."&amp;C2</f>
         <v>!EXAMPLE CATEGORY SEARCH.category</v>
       </c>
       <c r="M2" t="s">
@@ -3200,11 +3197,11 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="9"/>
       <c r="AB2" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B2)&amp;"-"&amp;C2&amp;".html")</f>
+        <f t="shared" ref="AB2:AB9" si="2">"SearchParameter-us-core-"&amp;LOWER((B2)&amp;"-"&amp;C2&amp;".html")</f>
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3221,7 +3218,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B3)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example code search</v>
       </c>
       <c r="H3" t="s">
@@ -3234,7 +3231,7 @@
         <v>57</v>
       </c>
       <c r="L3" t="str">
-        <f>B3&amp;"."&amp;C3</f>
+        <f t="shared" si="1"/>
         <v>!EXAMPLE CODE SEARCH.code</v>
       </c>
       <c r="M3" t="s">
@@ -3247,11 +3244,11 @@
       <c r="Z3" s="4"/>
       <c r="AA3" s="9"/>
       <c r="AB3" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B3)&amp;"-"&amp;C3&amp;".html")</f>
+        <f t="shared" si="2"/>
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3268,7 +3265,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B4)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example date search</v>
       </c>
       <c r="H4" t="s">
@@ -3281,7 +3278,7 @@
         <v>78</v>
       </c>
       <c r="L4" t="str">
-        <f>B4&amp;"."&amp;C4</f>
+        <f t="shared" si="1"/>
         <v>!EXAMPLE DATE SEARCH.date</v>
       </c>
       <c r="M4" t="s">
@@ -3298,11 +3295,11 @@
       </c>
       <c r="AA4" s="9"/>
       <c r="AB4" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B4)&amp;"-"&amp;C4&amp;".html")</f>
+        <f t="shared" si="2"/>
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3322,7 +3319,7 @@
         <v>485</v>
       </c>
       <c r="G5" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B5)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example patient search</v>
       </c>
       <c r="H5" t="s">
@@ -3335,7 +3332,7 @@
         <v>90</v>
       </c>
       <c r="L5" t="str">
-        <f>B5&amp;"."&amp;C5</f>
+        <f t="shared" si="1"/>
         <v>!EXAMPLE PATIENT SEARCH.patient</v>
       </c>
       <c r="M5" t="s">
@@ -3357,11 +3354,11 @@
         <v>Fetches a bundle of all !EXAMPLE PATIENT SEARCH resources for the specified patient</v>
       </c>
       <c r="AB5" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B5)&amp;"-"&amp;C5&amp;".html")</f>
+        <f t="shared" si="2"/>
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3378,7 +3375,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B6)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!example status search</v>
       </c>
       <c r="H6" t="s">
@@ -3391,7 +3388,7 @@
         <v>57</v>
       </c>
       <c r="L6" t="str">
-        <f>B6&amp;"."&amp;C6</f>
+        <f t="shared" si="1"/>
         <v>!EXAMPLE STATUS SEARCH.status</v>
       </c>
       <c r="M6" t="s">
@@ -3404,11 +3401,11 @@
       <c r="Z6" s="4"/>
       <c r="AA6" s="9"/>
       <c r="AB6" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B6)&amp;"-"&amp;C6&amp;".html")</f>
+        <f t="shared" si="2"/>
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3425,7 +3422,7 @@
         <v>0</v>
       </c>
       <c r="G7" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B7)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="H7" t="s">
@@ -3438,7 +3435,7 @@
         <v>63</v>
       </c>
       <c r="L7" t="str">
-        <f>B7&amp;"."&amp;C7</f>
+        <f t="shared" si="1"/>
         <v>!Patient.address</v>
       </c>
       <c r="M7" t="s">
@@ -3455,11 +3452,11 @@
       </c>
       <c r="AA7" s="9"/>
       <c r="AB7" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B7)&amp;"-"&amp;C7&amp;".html")</f>
+        <f t="shared" si="2"/>
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3476,7 +3473,7 @@
         <v>0</v>
       </c>
       <c r="G8" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B8)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="H8" t="s">
@@ -3489,7 +3486,7 @@
         <v>63</v>
       </c>
       <c r="L8" t="str">
-        <f>B8&amp;"."&amp;C8</f>
+        <f t="shared" si="1"/>
         <v>!Patient.telecom</v>
       </c>
       <c r="M8" t="s">
@@ -3506,11 +3503,11 @@
       </c>
       <c r="AA8" s="9"/>
       <c r="AB8" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B8)&amp;"-"&amp;C8&amp;".html")</f>
+        <f t="shared" si="2"/>
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3530,7 +3527,7 @@
         <v>488</v>
       </c>
       <c r="G9" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B9)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="H9" t="s">
@@ -3543,7 +3540,7 @@
         <v>57</v>
       </c>
       <c r="L9" t="str">
-        <f>B9&amp;"."&amp;C9</f>
+        <f t="shared" si="1"/>
         <v>AllergyIntolerance.clinical-status</v>
       </c>
       <c r="M9" t="s">
@@ -3555,11 +3552,11 @@
       <c r="Z9" s="4"/>
       <c r="AA9" s="9"/>
       <c r="AB9" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B9)&amp;"-"&amp;C9&amp;".html")</f>
+        <f t="shared" si="2"/>
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3579,7 +3576,7 @@
         <v>485</v>
       </c>
       <c r="G10" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B10)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="H10" t="s">
@@ -3592,7 +3589,7 @@
         <v>90</v>
       </c>
       <c r="L10" t="str">
-        <f>B10&amp;"."&amp;C10</f>
+        <f t="shared" si="1"/>
         <v>AllergyIntolerance.patient</v>
       </c>
       <c r="M10" t="s">
@@ -3617,7 +3614,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3637,7 +3634,7 @@
         <v>488</v>
       </c>
       <c r="G11" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B11)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H11" t="s">
@@ -3650,7 +3647,7 @@
         <v>57</v>
       </c>
       <c r="L11" t="str">
-        <f>B11&amp;"."&amp;C11</f>
+        <f t="shared" si="1"/>
         <v>Condition.category</v>
       </c>
       <c r="M11" t="s">
@@ -3667,7 +3664,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3687,7 +3684,7 @@
         <v>488</v>
       </c>
       <c r="G12" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B12)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H12" t="s">
@@ -3700,7 +3697,7 @@
         <v>57</v>
       </c>
       <c r="L12" t="str">
-        <f>B12&amp;"."&amp;C12</f>
+        <f t="shared" si="1"/>
         <v>Condition.clinical-status</v>
       </c>
       <c r="M12" t="s">
@@ -3715,7 +3712,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3735,7 +3732,7 @@
         <v>485</v>
       </c>
       <c r="G13" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B13)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H13" t="s">
@@ -3748,7 +3745,7 @@
         <v>90</v>
       </c>
       <c r="L13" t="str">
-        <f>B13&amp;"."&amp;C13</f>
+        <f t="shared" si="1"/>
         <v>Condition.patient</v>
       </c>
       <c r="M13" t="s">
@@ -3773,7 +3770,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3790,7 +3787,7 @@
         <v>1</v>
       </c>
       <c r="G14" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B14)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H14" t="s">
@@ -3803,7 +3800,7 @@
         <v>57</v>
       </c>
       <c r="L14" t="str">
-        <f>B14&amp;"."&amp;C14</f>
+        <f t="shared" si="1"/>
         <v>Encounter._id</v>
       </c>
       <c r="M14" t="s">
@@ -3826,7 +3823,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3846,7 +3843,7 @@
         <v>488</v>
       </c>
       <c r="G15" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B15)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H15" t="s">
@@ -3859,7 +3856,7 @@
         <v>57</v>
       </c>
       <c r="L15" t="str">
-        <f>B15&amp;"."&amp;C15</f>
+        <f t="shared" si="1"/>
         <v>Encounter.class</v>
       </c>
       <c r="M15" t="s">
@@ -3876,7 +3873,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3896,7 +3893,7 @@
         <v>486</v>
       </c>
       <c r="G16" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B16)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H16" t="s">
@@ -3909,7 +3906,7 @@
         <v>78</v>
       </c>
       <c r="L16" t="str">
-        <f>B16&amp;"."&amp;C16</f>
+        <f t="shared" si="1"/>
         <v>Encounter.date</v>
       </c>
       <c r="M16" t="s">
@@ -3930,7 +3927,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -3950,7 +3947,7 @@
         <v>488</v>
       </c>
       <c r="G17" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B17)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H17" t="s">
@@ -3963,7 +3960,7 @@
         <v>57</v>
       </c>
       <c r="L17" t="str">
-        <f>B17&amp;"."&amp;C17</f>
+        <f t="shared" si="1"/>
         <v>Encounter.identifier</v>
       </c>
       <c r="M17" t="s">
@@ -3987,7 +3984,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4007,7 +4004,7 @@
         <v>485</v>
       </c>
       <c r="G18" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B18)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H18" t="s">
@@ -4020,7 +4017,7 @@
         <v>90</v>
       </c>
       <c r="L18" t="str">
-        <f>B18&amp;"."&amp;C18</f>
+        <f t="shared" si="1"/>
         <v>Encounter.patient</v>
       </c>
       <c r="M18" t="s">
@@ -4045,7 +4042,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4065,7 +4062,7 @@
         <v>485</v>
       </c>
       <c r="G19" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B19)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H19" t="s">
@@ -4078,7 +4075,7 @@
         <v>90</v>
       </c>
       <c r="L19" t="str">
-        <f>B19&amp;"."&amp;C19</f>
+        <f t="shared" si="1"/>
         <v>Encounter.location</v>
       </c>
       <c r="M19" t="s">
@@ -4103,7 +4100,7 @@
         <v>SearchParameter-us-core-encounter-location.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4123,7 +4120,7 @@
         <v>488</v>
       </c>
       <c r="G20" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B20)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H20" t="s">
@@ -4136,7 +4133,7 @@
         <v>57</v>
       </c>
       <c r="L20" t="str">
-        <f>B20&amp;"."&amp;C20</f>
+        <f t="shared" si="1"/>
         <v>Encounter.status</v>
       </c>
       <c r="M20" t="s">
@@ -4153,7 +4150,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4173,7 +4170,7 @@
         <v>488</v>
       </c>
       <c r="G21" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B21)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H21" t="s">
@@ -4186,7 +4183,7 @@
         <v>57</v>
       </c>
       <c r="L21" t="str">
-        <f>B21&amp;"."&amp;C21</f>
+        <f t="shared" si="1"/>
         <v>Encounter.type</v>
       </c>
       <c r="M21" t="s">
@@ -4203,7 +4200,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4223,7 +4220,7 @@
         <v>488</v>
       </c>
       <c r="G22" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B22)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="H22" t="s">
@@ -4236,7 +4233,7 @@
         <v>57</v>
       </c>
       <c r="L22" t="str">
-        <f>B22&amp;"."&amp;C22</f>
+        <f t="shared" si="1"/>
         <v>Encounter.discharge-disposition</v>
       </c>
       <c r="M22" t="s">
@@ -4253,7 +4250,7 @@
         <v>SearchParameter-us-core-encounter-discharge-disposition.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4270,7 +4267,7 @@
         <v>1</v>
       </c>
       <c r="G23" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B23)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H23" t="s">
@@ -4286,7 +4283,7 @@
         <v>57</v>
       </c>
       <c r="L23" t="str">
-        <f>B23&amp;"."&amp;C23</f>
+        <f t="shared" si="1"/>
         <v>Patient._id</v>
       </c>
       <c r="M23" t="s">
@@ -4306,7 +4303,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4326,7 +4323,7 @@
         <v>487</v>
       </c>
       <c r="G24" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B24)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H24" t="s">
@@ -4339,7 +4336,7 @@
         <v>78</v>
       </c>
       <c r="L24" t="str">
-        <f>B24&amp;"."&amp;C24</f>
+        <f t="shared" si="1"/>
         <v>Patient.birthdate</v>
       </c>
       <c r="M24" t="s">
@@ -4353,7 +4350,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4373,7 +4370,7 @@
         <v>487</v>
       </c>
       <c r="G25" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B25)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H25" t="s">
@@ -4389,7 +4386,7 @@
         <v>78</v>
       </c>
       <c r="L25" t="str">
-        <f>B25&amp;"."&amp;C25</f>
+        <f t="shared" si="1"/>
         <v>Patient.death-date</v>
       </c>
       <c r="M25" t="s">
@@ -4403,7 +4400,7 @@
         <v>SearchParameter-us-core-patient-death-date.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4423,7 +4420,7 @@
         <v>518</v>
       </c>
       <c r="G26" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B26)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H26" t="s">
@@ -4449,7 +4446,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4469,7 +4466,7 @@
         <v>488</v>
       </c>
       <c r="G27" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B27)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H27" t="s">
@@ -4497,7 +4494,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4514,7 +4511,7 @@
         <v>0</v>
       </c>
       <c r="G28" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B28)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H28" t="s">
@@ -4541,7 +4538,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4561,7 +4558,7 @@
         <v>488</v>
       </c>
       <c r="G29" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B29)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H29" t="s">
@@ -4598,7 +4595,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4615,7 +4612,7 @@
         <v>1</v>
       </c>
       <c r="G30" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B30)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="H30" t="s">
@@ -4652,7 +4649,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4669,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="G31" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B31)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="H31" t="s">
@@ -4708,12 +4705,12 @@
         <v>SearchParameter-us-core-!patient-tribal-affiliation.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C32" t="s">
         <v>55</v>
@@ -4725,7 +4722,7 @@
         <v>0</v>
       </c>
       <c r="G32" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B32)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!!questionnaire</v>
       </c>
       <c r="H32" t="s">
@@ -4738,7 +4735,7 @@
         <v>57</v>
       </c>
       <c r="L32" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="M32" t="s">
         <v>56</v>
@@ -4747,16 +4744,16 @@
         <v>56</v>
       </c>
       <c r="AB32" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B32)&amp;"-"&amp;C32&amp;".html")</f>
+        <f t="shared" ref="AB32:AB43" si="3">"SearchParameter-us-core-"&amp;LOWER((B32)&amp;"-"&amp;C32&amp;".html")</f>
         <v>SearchParameter-us-core-!!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C33" t="s">
         <v>70</v>
@@ -4768,7 +4765,7 @@
         <v>0</v>
       </c>
       <c r="G33" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B33)</f>
+        <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!!questionnaire</v>
       </c>
       <c r="H33" t="s">
@@ -4781,7 +4778,7 @@
         <v>71</v>
       </c>
       <c r="L33" t="str">
-        <f>B33&amp;"."&amp;C33</f>
+        <f t="shared" ref="L33:L47" si="4">B33&amp;"."&amp;C33</f>
         <v>!!Questionnaire.context-type-value</v>
       </c>
       <c r="M33" t="s">
@@ -4791,16 +4788,16 @@
         <v>56</v>
       </c>
       <c r="AB33" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B33)&amp;"-"&amp;C33&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-!!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C34" t="s">
         <v>67</v>
@@ -4812,7 +4809,7 @@
         <v>0</v>
       </c>
       <c r="G34" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B34)</f>
+        <f t="shared" ref="G34:G65" si="5">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B34)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!!questionnaire</v>
       </c>
       <c r="H34" t="s">
@@ -4825,7 +4822,7 @@
         <v>63</v>
       </c>
       <c r="L34" t="str">
-        <f>B34&amp;"."&amp;C34</f>
+        <f t="shared" si="4"/>
         <v>!!Questionnaire.publisher</v>
       </c>
       <c r="M34" t="s">
@@ -4838,16 +4835,16 @@
         <v>68</v>
       </c>
       <c r="AB34" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B34)&amp;"-"&amp;C34&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-!!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C35" t="s">
         <v>61</v>
@@ -4859,7 +4856,7 @@
         <v>0</v>
       </c>
       <c r="G35" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B35)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!!questionnaire</v>
       </c>
       <c r="H35" t="s">
@@ -4872,7 +4869,7 @@
         <v>57</v>
       </c>
       <c r="L35" t="str">
-        <f>B35&amp;"."&amp;C35</f>
+        <f t="shared" si="4"/>
         <v>!!Questionnaire.status</v>
       </c>
       <c r="M35" t="s">
@@ -4882,16 +4879,16 @@
         <v>56</v>
       </c>
       <c r="AB35" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B35)&amp;"-"&amp;C35&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-!!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C36" t="s">
         <v>62</v>
@@ -4903,7 +4900,7 @@
         <v>0</v>
       </c>
       <c r="G36" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B36)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!!questionnaire</v>
       </c>
       <c r="H36" t="s">
@@ -4916,7 +4913,7 @@
         <v>63</v>
       </c>
       <c r="L36" t="str">
-        <f>B36&amp;"."&amp;C36</f>
+        <f t="shared" si="4"/>
         <v>!!Questionnaire.title</v>
       </c>
       <c r="M36" t="s">
@@ -4938,16 +4935,16 @@
         <v>64</v>
       </c>
       <c r="AB36" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B36)&amp;"-"&amp;C36&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-!!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C37" t="s">
         <v>59</v>
@@ -4959,7 +4956,7 @@
         <v>0</v>
       </c>
       <c r="G37" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B37)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!!questionnaire</v>
       </c>
       <c r="H37" t="s">
@@ -4972,7 +4969,7 @@
         <v>60</v>
       </c>
       <c r="L37" t="str">
-        <f>B37&amp;"."&amp;C37</f>
+        <f t="shared" si="4"/>
         <v>!!Questionnaire.url</v>
       </c>
       <c r="M37" t="s">
@@ -4982,16 +4979,16 @@
         <v>56</v>
       </c>
       <c r="AB37" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B37)&amp;"-"&amp;C37&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-!!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="C38" t="s">
         <v>66</v>
@@ -5003,7 +5000,7 @@
         <v>0</v>
       </c>
       <c r="G38" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B38)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!!questionnaire</v>
       </c>
       <c r="H38" t="s">
@@ -5016,7 +5013,7 @@
         <v>57</v>
       </c>
       <c r="L38" t="str">
-        <f>B38&amp;"."&amp;C38</f>
+        <f t="shared" si="4"/>
         <v>!!Questionnaire.version</v>
       </c>
       <c r="M38" t="s">
@@ -5026,11 +5023,11 @@
         <v>56</v>
       </c>
       <c r="AB38" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B38)&amp;"-"&amp;C38&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-!!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5050,7 +5047,7 @@
         <v>486</v>
       </c>
       <c r="G39" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B39)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H39" t="s">
@@ -5063,7 +5060,7 @@
         <v>78</v>
       </c>
       <c r="L39" t="str">
-        <f>B39&amp;"."&amp;C39</f>
+        <f t="shared" si="4"/>
         <v>Condition.onset-date</v>
       </c>
       <c r="M39" t="s">
@@ -5080,11 +5077,11 @@
       </c>
       <c r="AA39" s="9"/>
       <c r="AB39" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B39)&amp;"-"&amp;C39&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5104,7 +5101,7 @@
         <v>486</v>
       </c>
       <c r="G40" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B40)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H40" t="s">
@@ -5117,7 +5114,7 @@
         <v>78</v>
       </c>
       <c r="L40" t="str">
-        <f>B40&amp;"."&amp;C40</f>
+        <f t="shared" si="4"/>
         <v>Condition.asserted-date</v>
       </c>
       <c r="M40" t="s">
@@ -5134,11 +5131,11 @@
       </c>
       <c r="AA40" s="9"/>
       <c r="AB40" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B40)&amp;"-"&amp;C40&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-condition-asserted-date.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5158,7 +5155,7 @@
         <v>486</v>
       </c>
       <c r="G41" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B41)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H41" t="s">
@@ -5171,7 +5168,7 @@
         <v>78</v>
       </c>
       <c r="L41" t="str">
-        <f>B41&amp;"."&amp;C41</f>
+        <f t="shared" si="4"/>
         <v>Condition.recorded-date</v>
       </c>
       <c r="M41" t="s">
@@ -5188,11 +5185,11 @@
       </c>
       <c r="AA41" s="9"/>
       <c r="AB41" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B41)&amp;"-"&amp;C41&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-condition-recorded-date.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5212,7 +5209,7 @@
         <v>486</v>
       </c>
       <c r="G42" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B42)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H42" t="s">
@@ -5225,7 +5222,7 @@
         <v>78</v>
       </c>
       <c r="L42" t="str">
-        <f>B42&amp;"."&amp;C42</f>
+        <f t="shared" si="4"/>
         <v>Condition.abatement-date</v>
       </c>
       <c r="M42" t="s">
@@ -5242,11 +5239,11 @@
       </c>
       <c r="AA42" s="9"/>
       <c r="AB42" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B42)&amp;"-"&amp;C42&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-condition-abatement-date.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5266,7 +5263,7 @@
         <v>488</v>
       </c>
       <c r="G43" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B43)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H43" t="s">
@@ -5279,7 +5276,7 @@
         <v>57</v>
       </c>
       <c r="L43" t="str">
-        <f>B43&amp;"."&amp;C43</f>
+        <f t="shared" si="4"/>
         <v>Condition.code</v>
       </c>
       <c r="M43" t="s">
@@ -5292,11 +5289,11 @@
       <c r="Z43" s="4"/>
       <c r="AA43" s="9"/>
       <c r="AB43" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B43)&amp;"-"&amp;C43&amp;".html")</f>
+        <f t="shared" si="3"/>
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5316,7 +5313,7 @@
         <v>485</v>
       </c>
       <c r="G44" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B44)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="H44" t="s">
@@ -5329,7 +5326,7 @@
         <v>90</v>
       </c>
       <c r="L44" t="str">
-        <f>B44&amp;"."&amp;C44</f>
+        <f t="shared" si="4"/>
         <v>Condition.encounter</v>
       </c>
       <c r="M44" t="s">
@@ -5354,7 +5351,7 @@
         <v>SearchParameter-us-core-condition-encounter.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5374,7 +5371,7 @@
         <v>485</v>
       </c>
       <c r="G45" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B45)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="H45" t="s">
@@ -5387,7 +5384,7 @@
         <v>90</v>
       </c>
       <c r="L45" t="str">
-        <f>B45&amp;"."&amp;C45</f>
+        <f t="shared" si="4"/>
         <v>Immunization.patient</v>
       </c>
       <c r="M45" t="s">
@@ -5413,7 +5410,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5433,7 +5430,7 @@
         <v>488</v>
       </c>
       <c r="G46" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B46)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="H46" t="s">
@@ -5446,7 +5443,7 @@
         <v>57</v>
       </c>
       <c r="L46" t="str">
-        <f>B46&amp;"."&amp;C46</f>
+        <f t="shared" si="4"/>
         <v>Immunization.status</v>
       </c>
       <c r="M46" t="s">
@@ -5459,11 +5456,11 @@
       <c r="Z46" s="4"/>
       <c r="AA46" s="9"/>
       <c r="AB46" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B46)&amp;"-"&amp;C46&amp;".html")</f>
+        <f t="shared" ref="AB46:AB85" si="6">"SearchParameter-us-core-"&amp;LOWER((B46)&amp;"-"&amp;C46&amp;".html")</f>
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5483,7 +5480,7 @@
         <v>486</v>
       </c>
       <c r="G47" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B47)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="H47" t="s">
@@ -5496,7 +5493,7 @@
         <v>78</v>
       </c>
       <c r="L47" t="str">
-        <f>B47&amp;"."&amp;C47</f>
+        <f t="shared" si="4"/>
         <v>Immunization.date</v>
       </c>
       <c r="M47" t="s">
@@ -5513,11 +5510,11 @@
       </c>
       <c r="AA47" s="9"/>
       <c r="AB47" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B47)&amp;"-"&amp;C47&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5534,7 +5531,7 @@
         <v>1</v>
       </c>
       <c r="G48" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B48)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H48" t="s">
@@ -5566,11 +5563,11 @@
         <v>276</v>
       </c>
       <c r="AB48" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B48)&amp;"-"&amp;C48&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5590,7 +5587,7 @@
         <v>488</v>
       </c>
       <c r="G49" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B49)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H49" t="s">
@@ -5619,11 +5616,11 @@
       <c r="Z49" s="4"/>
       <c r="AA49" s="9"/>
       <c r="AB49" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B49)&amp;"-"&amp;C49&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5643,7 +5640,7 @@
         <v>485</v>
       </c>
       <c r="G50" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B50)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H50" t="s">
@@ -5678,11 +5675,11 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient. See the implementation notes above for how to access the actual document.</v>
       </c>
       <c r="AB50" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B50)&amp;"-"&amp;C50&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5702,7 +5699,7 @@
         <v>488</v>
       </c>
       <c r="G51" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B51)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H51" t="s">
@@ -5728,11 +5725,11 @@
       <c r="Z51" s="4"/>
       <c r="AA51" s="9"/>
       <c r="AB51" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B51)&amp;"-"&amp;C51&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5752,7 +5749,7 @@
         <v>488</v>
       </c>
       <c r="G52" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B52)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H52" t="s">
@@ -5778,11 +5775,11 @@
       <c r="Z52" s="4"/>
       <c r="AA52" s="9"/>
       <c r="AB52" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B52)&amp;"-"&amp;C52&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5802,7 +5799,7 @@
         <v>486</v>
       </c>
       <c r="G53" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B53)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H53" t="s">
@@ -5832,11 +5829,11 @@
       </c>
       <c r="AA53" s="9"/>
       <c r="AB53" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B53)&amp;"-"&amp;C53&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5856,7 +5853,7 @@
         <v>486</v>
       </c>
       <c r="G54" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B54)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="H54" t="s">
@@ -5885,11 +5882,11 @@
       </c>
       <c r="AA54" s="9"/>
       <c r="AB54" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B54)&amp;"-"&amp;C54&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5909,7 +5906,7 @@
         <v>488</v>
       </c>
       <c r="G55" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B55)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="H55" t="s">
@@ -5922,7 +5919,7 @@
         <v>57</v>
       </c>
       <c r="L55" t="str">
-        <f>B55&amp;"."&amp;C55</f>
+        <f t="shared" ref="L55:L86" si="7">B55&amp;"."&amp;C55</f>
         <v>DiagnosticReport.status</v>
       </c>
       <c r="M55" t="s">
@@ -5938,11 +5935,11 @@
       <c r="Z55" s="4"/>
       <c r="AA55" s="9"/>
       <c r="AB55" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B55)&amp;"-"&amp;C55&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -5962,7 +5959,7 @@
         <v>485</v>
       </c>
       <c r="G56" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B56)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="H56" t="s">
@@ -5975,7 +5972,7 @@
         <v>90</v>
       </c>
       <c r="L56" t="str">
-        <f>B56&amp;"."&amp;C56</f>
+        <f t="shared" si="7"/>
         <v>DiagnosticReport.patient</v>
       </c>
       <c r="M56" t="s">
@@ -5997,11 +5994,11 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient</v>
       </c>
       <c r="AB56" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B56)&amp;"-"&amp;C56&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6021,7 +6018,7 @@
         <v>488</v>
       </c>
       <c r="G57" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B57)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="H57" t="s">
@@ -6034,7 +6031,7 @@
         <v>57</v>
       </c>
       <c r="L57" t="str">
-        <f>B57&amp;"."&amp;C57</f>
+        <f t="shared" si="7"/>
         <v>DiagnosticReport.category</v>
       </c>
       <c r="M57" t="s">
@@ -6047,11 +6044,11 @@
       <c r="Z57" s="4"/>
       <c r="AA57" s="9"/>
       <c r="AB57" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B57)&amp;"-"&amp;C57&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6071,7 +6068,7 @@
         <v>488</v>
       </c>
       <c r="G58" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B58)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="H58" t="s">
@@ -6084,7 +6081,7 @@
         <v>57</v>
       </c>
       <c r="L58" t="str">
-        <f>B58&amp;"."&amp;C58</f>
+        <f t="shared" si="7"/>
         <v>DiagnosticReport.code</v>
       </c>
       <c r="M58" t="s">
@@ -6100,11 +6097,11 @@
       <c r="Z58" s="4"/>
       <c r="AA58" s="9"/>
       <c r="AB58" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B58)&amp;"-"&amp;C58&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -6124,7 +6121,7 @@
         <v>486</v>
       </c>
       <c r="G59" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B59)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="H59" t="s">
@@ -6137,7 +6134,7 @@
         <v>78</v>
       </c>
       <c r="L59" t="str">
-        <f>B59&amp;"."&amp;C59</f>
+        <f t="shared" si="7"/>
         <v>DiagnosticReport.date</v>
       </c>
       <c r="M59" t="s">
@@ -6154,11 +6151,11 @@
       </c>
       <c r="AA59" s="9"/>
       <c r="AB59" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B59)&amp;"-"&amp;C59&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -6178,7 +6175,7 @@
         <v>488</v>
       </c>
       <c r="G60" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B60)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="H60" t="s">
@@ -6191,7 +6188,7 @@
         <v>57</v>
       </c>
       <c r="L60" t="str">
-        <f>B60&amp;"."&amp;C60</f>
+        <f t="shared" si="7"/>
         <v>Goal.lifecycle-status</v>
       </c>
       <c r="M60" t="s">
@@ -6204,11 +6201,11 @@
       <c r="Z60" s="4"/>
       <c r="AA60" s="9"/>
       <c r="AB60" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B60)&amp;"-"&amp;C60&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -6228,7 +6225,7 @@
         <v>485</v>
       </c>
       <c r="G61" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B61)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="H61" t="s">
@@ -6241,7 +6238,7 @@
         <v>90</v>
       </c>
       <c r="L61" t="str">
-        <f>B61&amp;"."&amp;C61</f>
+        <f t="shared" si="7"/>
         <v>Goal.patient</v>
       </c>
       <c r="M61" t="s">
@@ -6263,11 +6260,11 @@
         <v>Fetches a bundle of all Goal resources for the specified patient</v>
       </c>
       <c r="AB61" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B61)&amp;"-"&amp;C61&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6287,7 +6284,7 @@
         <v>487</v>
       </c>
       <c r="G62" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B62)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="H62" t="s">
@@ -6300,7 +6297,7 @@
         <v>78</v>
       </c>
       <c r="L62" t="str">
-        <f>B62&amp;"."&amp;C62</f>
+        <f t="shared" si="7"/>
         <v>Goal.target-date</v>
       </c>
       <c r="M62" t="s">
@@ -6317,11 +6314,11 @@
       </c>
       <c r="AA62" s="9"/>
       <c r="AB62" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B62)&amp;"-"&amp;C62&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6341,7 +6338,7 @@
         <v>488</v>
       </c>
       <c r="G63" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B63)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H63" t="s">
@@ -6354,7 +6351,7 @@
         <v>57</v>
       </c>
       <c r="L63" t="str">
-        <f>B63&amp;"."&amp;C63</f>
+        <f t="shared" si="7"/>
         <v>MedicationRequest.status</v>
       </c>
       <c r="M63" t="s">
@@ -6370,11 +6367,11 @@
       <c r="Z63" s="4"/>
       <c r="AA63" s="9"/>
       <c r="AB63" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B63)&amp;"-"&amp;C63&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6394,7 +6391,7 @@
         <v>488</v>
       </c>
       <c r="G64" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B64)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H64" t="s">
@@ -6407,7 +6404,7 @@
         <v>57</v>
       </c>
       <c r="L64" t="str">
-        <f>B64&amp;"."&amp;C64</f>
+        <f t="shared" si="7"/>
         <v>MedicationRequest.intent</v>
       </c>
       <c r="M64" t="s">
@@ -6423,11 +6420,11 @@
       <c r="Z64" s="4"/>
       <c r="AA64" s="9"/>
       <c r="AB64" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B64)&amp;"-"&amp;C64&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-medicationrequest-intent.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6447,7 +6444,7 @@
         <v>485</v>
       </c>
       <c r="G65" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B65)</f>
+        <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H65" t="s">
@@ -6460,7 +6457,7 @@
         <v>90</v>
       </c>
       <c r="L65" t="str">
-        <f>B65&amp;"."&amp;C65</f>
+        <f t="shared" si="7"/>
         <v>MedicationRequest.patient</v>
       </c>
       <c r="M65" t="s">
@@ -6476,11 +6473,11 @@
       <c r="Z65" s="9"/>
       <c r="AA65" s="9"/>
       <c r="AB65" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B65)&amp;"-"&amp;C65&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6500,7 +6497,7 @@
         <v>485</v>
       </c>
       <c r="G66" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B66)</f>
+        <f t="shared" ref="G66:G97" si="8">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B66)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H66" t="s">
@@ -6513,7 +6510,7 @@
         <v>90</v>
       </c>
       <c r="L66" t="str">
-        <f>B66&amp;"."&amp;C66</f>
+        <f t="shared" si="7"/>
         <v>MedicationRequest.encounter</v>
       </c>
       <c r="M66" t="s">
@@ -6527,11 +6524,11 @@
       <c r="Z66" s="9"/>
       <c r="AA66" s="9"/>
       <c r="AB66" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B66)&amp;"-"&amp;C66&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-medicationrequest-encounter.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6551,7 +6548,7 @@
         <v>486</v>
       </c>
       <c r="G67" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B67)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="H67" t="s">
@@ -6564,7 +6561,7 @@
         <v>78</v>
       </c>
       <c r="L67" t="str">
-        <f>B67&amp;"."&amp;C67</f>
+        <f t="shared" si="7"/>
         <v>MedicationRequest.authoredon</v>
       </c>
       <c r="M67" t="s">
@@ -6581,11 +6578,11 @@
       </c>
       <c r="AA67" s="9"/>
       <c r="AB67" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B67)&amp;"-"&amp;C67&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6605,7 +6602,7 @@
         <v>488</v>
       </c>
       <c r="G68" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B68)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="H68" t="s">
@@ -6618,7 +6615,7 @@
         <v>57</v>
       </c>
       <c r="L68" t="str">
-        <f>B68&amp;"."&amp;C68</f>
+        <f t="shared" si="7"/>
         <v>!MedicationStatement.status</v>
       </c>
       <c r="M68" t="s">
@@ -6634,11 +6631,11 @@
       <c r="Z68" s="4"/>
       <c r="AA68" s="9"/>
       <c r="AB68" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B68)&amp;"-"&amp;C68&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-!medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6658,7 +6655,7 @@
         <v>485</v>
       </c>
       <c r="G69" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B69)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="H69" t="s">
@@ -6671,7 +6668,7 @@
         <v>90</v>
       </c>
       <c r="L69" t="str">
-        <f>B69&amp;"."&amp;C69</f>
+        <f t="shared" si="7"/>
         <v>!MedicationStatement.patient</v>
       </c>
       <c r="M69" t="s">
@@ -6692,11 +6689,11 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient.W63+X63 Mandatory for client to support the _include parameter. Optional for server to support the _include parameter.</v>
       </c>
       <c r="AB69" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B69)&amp;"-"&amp;C69&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-!medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6716,7 +6713,7 @@
         <v>486</v>
       </c>
       <c r="G70" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B70)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="H70" t="s">
@@ -6729,7 +6726,7 @@
         <v>78</v>
       </c>
       <c r="L70" t="str">
-        <f>B70&amp;"."&amp;C70</f>
+        <f t="shared" si="7"/>
         <v>!MedicationStatement.effective</v>
       </c>
       <c r="M70" t="s">
@@ -6746,11 +6743,11 @@
       </c>
       <c r="AA70" s="9"/>
       <c r="AB70" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B70)&amp;"-"&amp;C70&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-!medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6770,7 +6767,7 @@
         <v>488</v>
       </c>
       <c r="G71" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B71)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="H71" t="s">
@@ -6783,7 +6780,7 @@
         <v>57</v>
       </c>
       <c r="L71" t="str">
-        <f>B71&amp;"."&amp;C71</f>
+        <f t="shared" si="7"/>
         <v>Procedure.status</v>
       </c>
       <c r="M71" t="s">
@@ -6799,11 +6796,11 @@
       <c r="Z71" s="4"/>
       <c r="AA71" s="9"/>
       <c r="AB71" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B71)&amp;"-"&amp;C71&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6823,7 +6820,7 @@
         <v>485</v>
       </c>
       <c r="G72" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B72)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="H72" t="s">
@@ -6836,7 +6833,7 @@
         <v>90</v>
       </c>
       <c r="L72" t="str">
-        <f>B72&amp;"."&amp;C72</f>
+        <f t="shared" si="7"/>
         <v>Procedure.patient</v>
       </c>
       <c r="M72" t="s">
@@ -6857,11 +6854,11 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient</v>
       </c>
       <c r="AB72" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B72)&amp;"-"&amp;C72&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6881,7 +6878,7 @@
         <v>486</v>
       </c>
       <c r="G73" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B73)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="H73" t="s">
@@ -6894,7 +6891,7 @@
         <v>78</v>
       </c>
       <c r="L73" t="str">
-        <f>B73&amp;"."&amp;C73</f>
+        <f t="shared" si="7"/>
         <v>Procedure.date</v>
       </c>
       <c r="M73" t="s">
@@ -6911,11 +6908,11 @@
       </c>
       <c r="AA73" s="9"/>
       <c r="AB73" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B73)&amp;"-"&amp;C73&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -6935,7 +6932,7 @@
         <v>488</v>
       </c>
       <c r="G74" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B74)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="H74" t="s">
@@ -6948,7 +6945,7 @@
         <v>57</v>
       </c>
       <c r="L74" t="str">
-        <f>B74&amp;"."&amp;C74</f>
+        <f t="shared" si="7"/>
         <v>Procedure.code</v>
       </c>
       <c r="M74" t="s">
@@ -6964,11 +6961,11 @@
       <c r="Z74" s="4"/>
       <c r="AA74" s="9"/>
       <c r="AB74" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B74)&amp;"-"&amp;C74&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -6988,7 +6985,7 @@
         <v>488</v>
       </c>
       <c r="G75" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B75)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H75" t="s">
@@ -7001,7 +6998,7 @@
         <v>57</v>
       </c>
       <c r="L75" t="str">
-        <f>B75&amp;"."&amp;C75</f>
+        <f t="shared" si="7"/>
         <v>Observation.status</v>
       </c>
       <c r="M75" t="s">
@@ -7017,11 +7014,11 @@
       <c r="Z75" s="4"/>
       <c r="AA75" s="9"/>
       <c r="AB75" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B75)&amp;"-"&amp;C75&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -7041,7 +7038,7 @@
         <v>488</v>
       </c>
       <c r="G76" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B76)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H76" t="s">
@@ -7054,7 +7051,7 @@
         <v>57</v>
       </c>
       <c r="L76" t="str">
-        <f>B76&amp;"."&amp;C76</f>
+        <f t="shared" si="7"/>
         <v>Observation.category</v>
       </c>
       <c r="M76" t="s">
@@ -7067,11 +7064,11 @@
       <c r="Z76" s="4"/>
       <c r="AA76" s="9"/>
       <c r="AB76" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B76)&amp;"-"&amp;C76&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -7091,7 +7088,7 @@
         <v>488</v>
       </c>
       <c r="G77" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B77)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H77" t="s">
@@ -7104,7 +7101,7 @@
         <v>57</v>
       </c>
       <c r="L77" t="str">
-        <f>B77&amp;"."&amp;C77</f>
+        <f t="shared" si="7"/>
         <v>Observation.code</v>
       </c>
       <c r="M77" t="s">
@@ -7120,11 +7117,11 @@
       <c r="Z77" s="4"/>
       <c r="AA77" s="9"/>
       <c r="AB77" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B77)&amp;"-"&amp;C77&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -7144,7 +7141,7 @@
         <v>486</v>
       </c>
       <c r="G78" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B78)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H78" t="s">
@@ -7157,7 +7154,7 @@
         <v>78</v>
       </c>
       <c r="L78" t="str">
-        <f>B78&amp;"."&amp;C78</f>
+        <f t="shared" si="7"/>
         <v>Observation.date</v>
       </c>
       <c r="M78" t="s">
@@ -7174,11 +7171,11 @@
       </c>
       <c r="AA78" s="9"/>
       <c r="AB78" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B78)&amp;"-"&amp;C78&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -7198,7 +7195,7 @@
         <v>485</v>
       </c>
       <c r="G79" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B79)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</v>
       </c>
       <c r="H79" t="s">
@@ -7211,7 +7208,7 @@
         <v>90</v>
       </c>
       <c r="L79" t="str">
-        <f>B79&amp;"."&amp;C79</f>
+        <f t="shared" si="7"/>
         <v>Observation.patient</v>
       </c>
       <c r="M79" t="s">
@@ -7233,11 +7230,11 @@
         <v>Fetches a bundle of all Observation resources for the specified patient</v>
       </c>
       <c r="AB79" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B79)&amp;"-"&amp;C79&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -7257,7 +7254,7 @@
         <v>488</v>
       </c>
       <c r="G80" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B80)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="H80" t="s">
@@ -7270,7 +7267,7 @@
         <v>57</v>
       </c>
       <c r="L80" t="str">
-        <f>B80&amp;"."&amp;C80</f>
+        <f t="shared" si="7"/>
         <v>CarePlan.category</v>
       </c>
       <c r="M80" t="s">
@@ -7283,11 +7280,11 @@
       <c r="Z80" s="4"/>
       <c r="AA80" s="9"/>
       <c r="AB80" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B80)&amp;"-"&amp;C80&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -7307,7 +7304,7 @@
         <v>488</v>
       </c>
       <c r="G81" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B81)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!careplan</v>
       </c>
       <c r="H81" t="s">
@@ -7320,7 +7317,7 @@
         <v>57</v>
       </c>
       <c r="L81" t="str">
-        <f>B81&amp;"."&amp;C81</f>
+        <f t="shared" si="7"/>
         <v>!CarePlan.code</v>
       </c>
       <c r="M81" t="s">
@@ -7333,11 +7330,11 @@
       <c r="Z81" s="4"/>
       <c r="AA81" s="9"/>
       <c r="AB81" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B81)&amp;"-"&amp;C81&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -7357,7 +7354,7 @@
         <v>486</v>
       </c>
       <c r="G82" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B82)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="H82" t="s">
@@ -7370,7 +7367,7 @@
         <v>78</v>
       </c>
       <c r="L82" t="str">
-        <f>B82&amp;"."&amp;C82</f>
+        <f t="shared" si="7"/>
         <v>CarePlan.date</v>
       </c>
       <c r="M82" t="s">
@@ -7387,11 +7384,11 @@
       </c>
       <c r="AA82" s="9"/>
       <c r="AB82" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B82)&amp;"-"&amp;C82&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -7411,7 +7408,7 @@
         <v>485</v>
       </c>
       <c r="G83" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B83)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="H83" t="s">
@@ -7424,7 +7421,7 @@
         <v>90</v>
       </c>
       <c r="L83" t="str">
-        <f>B83&amp;"."&amp;C83</f>
+        <f t="shared" si="7"/>
         <v>CarePlan.patient</v>
       </c>
       <c r="M83" t="s">
@@ -7446,11 +7443,11 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient</v>
       </c>
       <c r="AB83" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B83)&amp;"-"&amp;C83&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -7470,7 +7467,7 @@
         <v>488</v>
       </c>
       <c r="G84" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B84)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careplan</v>
       </c>
       <c r="H84" t="s">
@@ -7483,7 +7480,7 @@
         <v>57</v>
       </c>
       <c r="L84" t="str">
-        <f>B84&amp;"."&amp;C84</f>
+        <f t="shared" si="7"/>
         <v>CarePlan.status</v>
       </c>
       <c r="M84" t="s">
@@ -7499,11 +7496,11 @@
       <c r="Z84" s="4"/>
       <c r="AA84" s="9"/>
       <c r="AB84" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B84)&amp;"-"&amp;C84&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -7523,7 +7520,7 @@
         <v>485</v>
       </c>
       <c r="G85" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B85)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="H85" t="s">
@@ -7536,7 +7533,7 @@
         <v>90</v>
       </c>
       <c r="L85" t="str">
-        <f>B85&amp;"."&amp;C85</f>
+        <f t="shared" si="7"/>
         <v>CareTeam.patient</v>
       </c>
       <c r="M85" t="s">
@@ -7561,11 +7558,11 @@
         <v>Fetches a bundle of all CareTeam resources for the specified patient</v>
       </c>
       <c r="AB85" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B85)&amp;"-"&amp;C85&amp;".html")</f>
+        <f t="shared" si="6"/>
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -7582,7 +7579,7 @@
         <v>1</v>
       </c>
       <c r="G86" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B86)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
       </c>
       <c r="H86" t="s">
@@ -7595,7 +7592,7 @@
         <v>57</v>
       </c>
       <c r="L86" t="str">
-        <f>B86&amp;"."&amp;C86</f>
+        <f t="shared" si="7"/>
         <v>Practitioner._id</v>
       </c>
       <c r="M86" t="s">
@@ -7618,7 +7615,7 @@
         <v>SearchParameter-us-core-practitioner-id.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -7638,7 +7635,7 @@
         <v>488</v>
       </c>
       <c r="G87" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B87)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="H87" t="s">
@@ -7651,7 +7648,7 @@
         <v>57</v>
       </c>
       <c r="L87" t="str">
-        <f>B87&amp;"."&amp;C87</f>
+        <f t="shared" ref="L87:L118" si="9">B87&amp;"."&amp;C87</f>
         <v>CareTeam.status</v>
       </c>
       <c r="M87" t="s">
@@ -7667,11 +7664,11 @@
       <c r="Z87" s="4"/>
       <c r="AA87" s="9"/>
       <c r="AB87" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B87)&amp;"-"&amp;C87&amp;".html")</f>
+        <f t="shared" ref="AB87:AB101" si="10">"SearchParameter-us-core-"&amp;LOWER((B87)&amp;"-"&amp;C87&amp;".html")</f>
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -7691,7 +7688,7 @@
         <v>488</v>
       </c>
       <c r="G88" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B88)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="H88" t="s">
@@ -7704,7 +7701,7 @@
         <v>57</v>
       </c>
       <c r="L88" t="str">
-        <f>B88&amp;"."&amp;C88</f>
+        <f t="shared" si="9"/>
         <v>CareTeam.role</v>
       </c>
       <c r="M88" t="s">
@@ -7725,11 +7722,11 @@
       </c>
       <c r="AA88" s="9"/>
       <c r="AB88" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B88)&amp;"-"&amp;C88&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-careteam-role.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:28" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -7749,7 +7746,7 @@
         <v>485</v>
       </c>
       <c r="G89" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B89)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</v>
       </c>
       <c r="H89" t="s">
@@ -7762,7 +7759,7 @@
         <v>90</v>
       </c>
       <c r="L89" t="str">
-        <f>B89&amp;"."&amp;C89</f>
+        <f t="shared" si="9"/>
         <v>Device.patient</v>
       </c>
       <c r="M89" t="s">
@@ -7784,7 +7781,7 @@
         <v>Fetches a bundle of all Device resources for the specified patient</v>
       </c>
       <c r="AB89" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B89)&amp;"-"&amp;C89&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
@@ -7808,7 +7805,7 @@
         <v>488</v>
       </c>
       <c r="G90" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B90)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</v>
       </c>
       <c r="H90" t="s">
@@ -7821,7 +7818,7 @@
         <v>57</v>
       </c>
       <c r="L90" t="str">
-        <f>B90&amp;"."&amp;C90</f>
+        <f t="shared" si="9"/>
         <v>Device.type</v>
       </c>
       <c r="M90" t="s">
@@ -7833,7 +7830,7 @@
       <c r="Z90" s="4"/>
       <c r="AA90" s="9"/>
       <c r="AB90" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B90)&amp;"-"&amp;C90&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-device-type.html</v>
       </c>
     </row>
@@ -7857,10 +7854,13 @@
         <v>488</v>
       </c>
       <c r="G91" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B91)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</v>
       </c>
       <c r="H91" t="s">
+        <v>56</v>
+      </c>
+      <c r="I91" t="s">
         <v>56</v>
       </c>
       <c r="J91" t="s">
@@ -7870,7 +7870,7 @@
         <v>57</v>
       </c>
       <c r="L91" t="str">
-        <f>B91&amp;"."&amp;C91</f>
+        <f t="shared" si="9"/>
         <v>Device.status</v>
       </c>
       <c r="M91" t="s">
@@ -7885,11 +7885,11 @@
       <c r="Z91" s="4"/>
       <c r="AA91" s="9"/>
       <c r="AB91" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B91)&amp;"-"&amp;C91&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-device-status.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -7906,7 +7906,7 @@
         <v>1</v>
       </c>
       <c r="G92" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B92)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H92" t="s">
@@ -7919,7 +7919,7 @@
         <v>63</v>
       </c>
       <c r="L92" t="str">
-        <f>B92&amp;"."&amp;C92</f>
+        <f t="shared" si="9"/>
         <v>Location.name</v>
       </c>
       <c r="M92" t="s">
@@ -7940,11 +7940,11 @@
         <v>Fetches a bundle of all Location resources that match the name</v>
       </c>
       <c r="AB92" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B92)&amp;"-"&amp;C92&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -7961,7 +7961,7 @@
         <v>1</v>
       </c>
       <c r="G93" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B93)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H93" t="s">
@@ -7974,7 +7974,7 @@
         <v>63</v>
       </c>
       <c r="L93" t="str">
-        <f>B93&amp;"."&amp;C93</f>
+        <f t="shared" si="9"/>
         <v>Location.address</v>
       </c>
       <c r="M93" t="s">
@@ -7995,11 +7995,11 @@
         <v>Fetches a bundle of all Location resources that match the address string</v>
       </c>
       <c r="AB93" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B93)&amp;"-"&amp;C93&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8016,7 +8016,7 @@
         <v>1</v>
       </c>
       <c r="G94" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B94)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H94" t="s">
@@ -8029,7 +8029,7 @@
         <v>63</v>
       </c>
       <c r="L94" t="str">
-        <f>B94&amp;"."&amp;C94</f>
+        <f t="shared" si="9"/>
         <v>Location.address-city</v>
       </c>
       <c r="M94" t="s">
@@ -8050,11 +8050,11 @@
         <v>Fetches a bundle of all Location resources for the city</v>
       </c>
       <c r="AB94" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B94)&amp;"-"&amp;C94&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8071,7 +8071,7 @@
         <v>1</v>
       </c>
       <c r="G95" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B95)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H95" t="s">
@@ -8084,7 +8084,7 @@
         <v>63</v>
       </c>
       <c r="L95" t="str">
-        <f>B95&amp;"."&amp;C95</f>
+        <f t="shared" si="9"/>
         <v>Location.address-state</v>
       </c>
       <c r="M95" t="s">
@@ -8104,11 +8104,11 @@
         <v>Fetches a bundle of all Location resources for the state</v>
       </c>
       <c r="AB95" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B95)&amp;"-"&amp;C95&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="96" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8125,7 +8125,7 @@
         <v>1</v>
       </c>
       <c r="G96" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B96)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-location</v>
       </c>
       <c r="H96" t="s">
@@ -8138,7 +8138,7 @@
         <v>63</v>
       </c>
       <c r="L96" t="str">
-        <f>B96&amp;"."&amp;C96</f>
+        <f t="shared" si="9"/>
         <v>Location.address-postalcode</v>
       </c>
       <c r="M96" t="s">
@@ -8159,11 +8159,11 @@
         <v>Fetches a bundle of all Location resources for the ZIP code</v>
       </c>
       <c r="AB96" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B96)&amp;"-"&amp;C96&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="97" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8180,7 +8180,7 @@
         <v>1</v>
       </c>
       <c r="G97" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B97)</f>
+        <f t="shared" si="8"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization</v>
       </c>
       <c r="H97" t="s">
@@ -8193,7 +8193,7 @@
         <v>63</v>
       </c>
       <c r="L97" t="str">
-        <f>B97&amp;"."&amp;C97</f>
+        <f t="shared" si="9"/>
         <v>Organization.name</v>
       </c>
       <c r="M97" t="s">
@@ -8214,11 +8214,11 @@
         <v>Fetches a bundle of all Organization resources that match the name</v>
       </c>
       <c r="AB97" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B97)&amp;"-"&amp;C97&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8235,7 +8235,7 @@
         <v>1</v>
       </c>
       <c r="G98" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B98)</f>
+        <f t="shared" ref="G98:G126" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B98)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-organization</v>
       </c>
       <c r="H98" t="s">
@@ -8248,7 +8248,7 @@
         <v>63</v>
       </c>
       <c r="L98" t="str">
-        <f>B98&amp;"."&amp;C98</f>
+        <f t="shared" si="9"/>
         <v>Organization.address</v>
       </c>
       <c r="M98" t="s">
@@ -8269,11 +8269,11 @@
         <v>Fetches a bundle of all Organization resources that match the address string</v>
       </c>
       <c r="AB98" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B98)&amp;"-"&amp;C98&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="99" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8290,7 +8290,7 @@
         <v>1</v>
       </c>
       <c r="G99" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B99)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!organization</v>
       </c>
       <c r="H99" t="s">
@@ -8303,7 +8303,7 @@
         <v>63</v>
       </c>
       <c r="L99" t="str">
-        <f>B99&amp;"."&amp;C99</f>
+        <f t="shared" si="9"/>
         <v>!Organization.address-city</v>
       </c>
       <c r="M99" t="s">
@@ -8324,11 +8324,11 @@
         <v>Fetches a bundle of all !Organization resources for the city</v>
       </c>
       <c r="AB99" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B99)&amp;"-"&amp;C99&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -8345,7 +8345,7 @@
         <v>1</v>
       </c>
       <c r="G100" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B100)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!organization</v>
       </c>
       <c r="H100" t="s">
@@ -8358,7 +8358,7 @@
         <v>63</v>
       </c>
       <c r="L100" t="str">
-        <f>B100&amp;"."&amp;C100</f>
+        <f t="shared" si="9"/>
         <v>!Organization.adress-state</v>
       </c>
       <c r="M100" t="s">
@@ -8379,11 +8379,11 @@
         <v>Fetches a bundle of all !Organization resources for the state</v>
       </c>
       <c r="AB100" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B100)&amp;"-"&amp;C100&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -8400,7 +8400,7 @@
         <v>1</v>
       </c>
       <c r="G101" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B101)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!organization</v>
       </c>
       <c r="H101" t="s">
@@ -8413,7 +8413,7 @@
         <v>63</v>
       </c>
       <c r="L101" t="str">
-        <f>B101&amp;"."&amp;C101</f>
+        <f t="shared" si="9"/>
         <v>!Organization.address-postalcode</v>
       </c>
       <c r="M101" t="s">
@@ -8434,11 +8434,11 @@
         <v>Fetches a bundle of all !Organization resources for the ZIP code</v>
       </c>
       <c r="AB101" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B101)&amp;"-"&amp;C101&amp;".html")</f>
+        <f t="shared" si="10"/>
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -8455,7 +8455,7 @@
         <v>1</v>
       </c>
       <c r="G102" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B102)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
       </c>
       <c r="H102" t="s">
@@ -8468,7 +8468,7 @@
         <v>63</v>
       </c>
       <c r="L102" t="str">
-        <f>B102&amp;"."&amp;C102</f>
+        <f t="shared" si="9"/>
         <v>Practitioner.name</v>
       </c>
       <c r="M102" t="s">
@@ -8493,7 +8493,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -8513,7 +8513,7 @@
         <v>488</v>
       </c>
       <c r="G103" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B103)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitioner</v>
       </c>
       <c r="H103" t="s">
@@ -8526,7 +8526,7 @@
         <v>57</v>
       </c>
       <c r="L103" t="str">
-        <f>B103&amp;"."&amp;C103</f>
+        <f t="shared" si="9"/>
         <v>Practitioner.identifier</v>
       </c>
       <c r="M103" t="s">
@@ -8551,7 +8551,7 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -8571,7 +8571,7 @@
         <v>488</v>
       </c>
       <c r="G104" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B104)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
       </c>
       <c r="H104" t="s">
@@ -8584,7 +8584,7 @@
         <v>57</v>
       </c>
       <c r="L104" t="str">
-        <f>B104&amp;"."&amp;C104</f>
+        <f t="shared" si="9"/>
         <v>PractitionerRole.specialty</v>
       </c>
       <c r="M104" t="s">
@@ -8612,7 +8612,7 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="105" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -8632,7 +8632,7 @@
         <v>485</v>
       </c>
       <c r="G105" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B105)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-practitionerrole</v>
       </c>
       <c r="H105" t="s">
@@ -8645,7 +8645,7 @@
         <v>90</v>
       </c>
       <c r="L105" t="str">
-        <f>B105&amp;"."&amp;C105</f>
+        <f t="shared" si="9"/>
         <v>PractitionerRole.practitioner</v>
       </c>
       <c r="M105" t="s">
@@ -8676,7 +8676,7 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="106" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -8696,7 +8696,7 @@
         <v>488</v>
       </c>
       <c r="G106" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B106)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H106" t="s">
@@ -8709,7 +8709,7 @@
         <v>57</v>
       </c>
       <c r="L106" t="str">
-        <f>B106&amp;"."&amp;C106</f>
+        <f t="shared" si="9"/>
         <v>ServiceRequest.status</v>
       </c>
       <c r="M106" t="s">
@@ -8729,7 +8729,7 @@
         <v>SearchParameter-us-core-servicerequest-status.html</v>
       </c>
     </row>
-    <row r="107" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -8749,7 +8749,7 @@
         <v>485</v>
       </c>
       <c r="G107" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B107)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H107" t="s">
@@ -8762,7 +8762,7 @@
         <v>90</v>
       </c>
       <c r="L107" t="str">
-        <f>B107&amp;"."&amp;C107</f>
+        <f t="shared" si="9"/>
         <v>ServiceRequest.patient</v>
       </c>
       <c r="M107" t="s">
@@ -8788,7 +8788,7 @@
         <v>SearchParameter-us-core-servicerequest-patient.html</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -8808,7 +8808,7 @@
         <v>488</v>
       </c>
       <c r="G108" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B108)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H108" t="s">
@@ -8821,7 +8821,7 @@
         <v>57</v>
       </c>
       <c r="L108" t="str">
-        <f>B108&amp;"."&amp;C108</f>
+        <f t="shared" si="9"/>
         <v>ServiceRequest.category</v>
       </c>
       <c r="M108" t="s">
@@ -8838,7 +8838,7 @@
         <v>SearchParameter-us-core-servicerequest-category.html</v>
       </c>
     </row>
-    <row r="109" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -8858,7 +8858,7 @@
         <v>488</v>
       </c>
       <c r="G109" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B109)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H109" t="s">
@@ -8871,7 +8871,7 @@
         <v>57</v>
       </c>
       <c r="L109" t="str">
-        <f>B109&amp;"."&amp;C109</f>
+        <f t="shared" si="9"/>
         <v>ServiceRequest.code</v>
       </c>
       <c r="M109" t="s">
@@ -8891,7 +8891,7 @@
         <v>SearchParameter-us-core-servicerequest-code.html</v>
       </c>
     </row>
-    <row r="110" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -8911,7 +8911,7 @@
         <v>486</v>
       </c>
       <c r="G110" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B110)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H110" t="s">
@@ -8924,7 +8924,7 @@
         <v>78</v>
       </c>
       <c r="L110" t="str">
-        <f>B110&amp;"."&amp;C110</f>
+        <f t="shared" si="9"/>
         <v>ServiceRequest.authored</v>
       </c>
       <c r="M110" t="s">
@@ -8945,7 +8945,7 @@
         <v>SearchParameter-us-core-servicerequest-authored.html</v>
       </c>
     </row>
-    <row r="111" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -8962,7 +8962,7 @@
         <v>1</v>
       </c>
       <c r="G111" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B111)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="H111" t="s">
@@ -8975,7 +8975,7 @@
         <v>57</v>
       </c>
       <c r="L111" t="str">
-        <f>B111&amp;"."&amp;C111</f>
+        <f t="shared" si="9"/>
         <v>ServiceRequest._id</v>
       </c>
       <c r="M111" t="s">
@@ -8995,7 +8995,7 @@
         <v>SearchParameter-us-core-servicerequest-id.html</v>
       </c>
     </row>
-    <row r="112" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -9013,7 +9013,7 @@
       </c>
       <c r="F112" s="1"/>
       <c r="G112" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B112)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="H112" t="s">
@@ -9026,7 +9026,7 @@
         <v>57</v>
       </c>
       <c r="L112" t="str">
-        <f>B112&amp;"."&amp;C112</f>
+        <f t="shared" si="9"/>
         <v>Goal.description</v>
       </c>
       <c r="M112" t="s">
@@ -9041,7 +9041,7 @@
         <v>SearchParameter-us-core-goal-description.html</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -9058,7 +9058,7 @@
         <v>1</v>
       </c>
       <c r="G113" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B113)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
       </c>
       <c r="H113" t="s">
@@ -9071,7 +9071,7 @@
         <v>57</v>
       </c>
       <c r="L113" t="str">
-        <f>B113&amp;"."&amp;C113</f>
+        <f t="shared" si="9"/>
         <v>RelatedPerson._id</v>
       </c>
       <c r="M113" t="s">
@@ -9092,7 +9092,7 @@
         <v>SearchParameter-us-core-relatedperson-id.html</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -9112,7 +9112,7 @@
         <v>485</v>
       </c>
       <c r="G114" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B114)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
       </c>
       <c r="H114" t="s">
@@ -9125,7 +9125,7 @@
         <v>90</v>
       </c>
       <c r="L114" t="str">
-        <f>B114&amp;"."&amp;C114</f>
+        <f t="shared" si="9"/>
         <v>RelatedPerson.patient</v>
       </c>
       <c r="M114" t="s">
@@ -9151,7 +9151,7 @@
         <v>SearchParameter-us-core-relatedperson-patient.html</v>
       </c>
     </row>
-    <row r="115" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -9168,7 +9168,7 @@
         <v>1</v>
       </c>
       <c r="G115" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B115)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-relatedperson</v>
       </c>
       <c r="H115" t="s">
@@ -9184,7 +9184,7 @@
         <v>63</v>
       </c>
       <c r="L115" t="str">
-        <f>B115&amp;"."&amp;C115</f>
+        <f t="shared" si="9"/>
         <v>RelatedPerson.name</v>
       </c>
       <c r="M115" t="s">
@@ -9205,16 +9205,16 @@
         <v>Fetches a bundle of all RelatedPerson resources matching the name</v>
       </c>
       <c r="AB115" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B115)&amp;"-"&amp;SUBSTITUTE(C115,"_","")&amp;".html")</f>
+        <f t="shared" ref="AB115:AB122" si="12">"SearchParameter-us-core-"&amp;LOWER((B115)&amp;"-"&amp;SUBSTITUTE(C115,"_","")&amp;".html")</f>
         <v>SearchParameter-us-core-relatedperson-name.html</v>
       </c>
     </row>
-    <row r="116" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C116" t="s">
         <v>55</v>
@@ -9226,7 +9226,7 @@
         <v>1</v>
       </c>
       <c r="G116" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B116)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H116" t="s">
@@ -9239,7 +9239,7 @@
         <v>57</v>
       </c>
       <c r="L116" t="str">
-        <f>B116&amp;"."&amp;C116</f>
+        <f t="shared" si="9"/>
         <v>!QuestionnaireResponse._id</v>
       </c>
       <c r="M116" t="s">
@@ -9253,19 +9253,19 @@
         <v>support fetching a !QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="AB116" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B116)&amp;"-"&amp;SUBSTITUTE(C116,"_","")&amp;".html")</f>
+        <f t="shared" si="12"/>
         <v>SearchParameter-us-core-!questionnaireresponse-id.html</v>
       </c>
     </row>
-    <row r="117" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C117" t="s">
         <v>89</v>
@@ -9280,7 +9280,7 @@
         <v>485</v>
       </c>
       <c r="G117" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B117)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H117" t="s">
@@ -9293,7 +9293,7 @@
         <v>90</v>
       </c>
       <c r="L117" t="str">
-        <f>B117&amp;"."&amp;C117</f>
+        <f t="shared" si="9"/>
         <v>!QuestionnaireResponse.patient</v>
       </c>
       <c r="M117" t="s">
@@ -9315,16 +9315,16 @@
         <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient</v>
       </c>
       <c r="AB117" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B117)&amp;"-"&amp;SUBSTITUTE(C117,"_","")&amp;".html")</f>
+        <f t="shared" si="12"/>
         <v>SearchParameter-us-core-!questionnaireresponse-patient.html</v>
       </c>
     </row>
-    <row r="118" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C118" t="s">
         <v>61</v>
@@ -9339,7 +9339,7 @@
         <v>488</v>
       </c>
       <c r="G118" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B118)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H118" t="s">
@@ -9352,7 +9352,7 @@
         <v>57</v>
       </c>
       <c r="L118" t="str">
-        <f>B118&amp;"."&amp;C118</f>
+        <f t="shared" si="9"/>
         <v>!QuestionnaireResponse.status</v>
       </c>
       <c r="M118" t="s">
@@ -9365,19 +9365,19 @@
         <v>56</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="AB118" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B118)&amp;"-"&amp;SUBSTITUTE(C118,"_","")&amp;".html")</f>
+        <f t="shared" si="12"/>
         <v>SearchParameter-us-core-!questionnaireresponse-status.html</v>
       </c>
     </row>
-    <row r="119" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C119" t="s">
         <v>615</v>
@@ -9392,7 +9392,7 @@
         <v>488</v>
       </c>
       <c r="G119" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B119)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H119" t="s">
@@ -9405,28 +9405,28 @@
         <v>57</v>
       </c>
       <c r="L119" t="s">
+        <v>705</v>
+      </c>
+      <c r="M119" t="s">
+        <v>56</v>
+      </c>
+      <c r="O119" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>706</v>
       </c>
-      <c r="M119" t="s">
-        <v>56</v>
-      </c>
-      <c r="O119" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>707</v>
-      </c>
       <c r="AB119" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B119)&amp;"-"&amp;SUBSTITUTE(C119,"_","")&amp;".html")</f>
+        <f t="shared" si="12"/>
         <v>SearchParameter-us-core-!questionnaireresponse-tag.html</v>
       </c>
     </row>
-    <row r="120" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C120" t="s">
         <v>562</v>
@@ -9441,7 +9441,7 @@
         <v>486</v>
       </c>
       <c r="G120" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B120)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H120" t="s">
@@ -9454,7 +9454,7 @@
         <v>78</v>
       </c>
       <c r="L120" t="str">
-        <f>B120&amp;"."&amp;C120</f>
+        <f t="shared" ref="L120:L126" si="13">B120&amp;"."&amp;C120</f>
         <v>!QuestionnaireResponse.authored</v>
       </c>
       <c r="M120" t="s">
@@ -9470,19 +9470,19 @@
         <v>92</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="AB120" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B120)&amp;"-"&amp;SUBSTITUTE(C120,"_","")&amp;".html")</f>
+        <f t="shared" si="12"/>
         <v>SearchParameter-us-core-!questionnaireresponse-authored.html</v>
       </c>
     </row>
-    <row r="121" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C121" t="s">
         <v>616</v>
@@ -9497,7 +9497,7 @@
         <v>485</v>
       </c>
       <c r="G121" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B121)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="H121" t="s">
@@ -9510,7 +9510,7 @@
         <v>90</v>
       </c>
       <c r="L121" t="str">
-        <f>B121&amp;"."&amp;C121</f>
+        <f t="shared" si="13"/>
         <v>!QuestionnaireResponse.questionnaire</v>
       </c>
       <c r="M121" t="s">
@@ -9520,14 +9520,14 @@
         <v>56</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="AB121" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B121)&amp;"-"&amp;SUBSTITUTE(C121,"_","")&amp;".html")</f>
+        <f t="shared" si="12"/>
         <v>SearchParameter-us-core-!questionnaireresponse-questionnaire.html</v>
       </c>
     </row>
-    <row r="122" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -9547,7 +9547,7 @@
         <v>485</v>
       </c>
       <c r="G122" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B122)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-coverage</v>
       </c>
       <c r="H122" t="s">
@@ -9563,7 +9563,7 @@
         <v>90</v>
       </c>
       <c r="L122" t="str">
-        <f>B122&amp;"."&amp;C122</f>
+        <f t="shared" si="13"/>
         <v>Coverage.patient</v>
       </c>
       <c r="M122" t="s">
@@ -9584,11 +9584,11 @@
         <v>Fetches a bundle of all Coverage resources for the specified patient</v>
       </c>
       <c r="AB122" t="str">
-        <f>"SearchParameter-us-core-"&amp;LOWER((B122)&amp;"-"&amp;SUBSTITUTE(C122,"_","")&amp;".html")</f>
+        <f t="shared" si="12"/>
         <v>SearchParameter-us-core-coverage-patient.html</v>
       </c>
     </row>
-    <row r="123" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -9608,7 +9608,7 @@
         <v>488</v>
       </c>
       <c r="G123" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B123)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="H123" t="s">
@@ -9624,7 +9624,7 @@
         <v>57</v>
       </c>
       <c r="L123" t="str">
-        <f>B123&amp;"."&amp;C123</f>
+        <f t="shared" si="13"/>
         <v>MedicationDispense.status</v>
       </c>
       <c r="M123" t="s">
@@ -9644,7 +9644,7 @@
         <v>SearchParameter-us-core-medicationdispense-status.html</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -9664,7 +9664,7 @@
         <v>488</v>
       </c>
       <c r="G124" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B124)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="H124" t="s">
@@ -9680,7 +9680,7 @@
         <v>57</v>
       </c>
       <c r="L124" t="str">
-        <f>B124&amp;"."&amp;C124</f>
+        <f t="shared" si="13"/>
         <v>MedicationDispense.type</v>
       </c>
       <c r="M124" t="s">
@@ -9700,7 +9700,7 @@
         <v>SearchParameter-us-core-medicationdispense-type.html</v>
       </c>
     </row>
-    <row r="125" spans="1:28" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:28" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -9720,7 +9720,7 @@
         <v>485</v>
       </c>
       <c r="G125" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B125)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="H125" t="s">
@@ -9736,7 +9736,7 @@
         <v>90</v>
       </c>
       <c r="L125" t="str">
-        <f>B125&amp;"."&amp;C125</f>
+        <f t="shared" si="13"/>
         <v>MedicationDispense.patient</v>
       </c>
       <c r="M125" t="s">
@@ -9760,7 +9760,7 @@
         <v>SearchParameter-us-core-medicationdispense-patient.html</v>
       </c>
     </row>
-    <row r="126" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -9780,7 +9780,7 @@
         <v>486</v>
       </c>
       <c r="G126" t="str">
-        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B126)</f>
+        <f t="shared" si="11"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="H126" t="s">
@@ -9796,7 +9796,7 @@
         <v>78</v>
       </c>
       <c r="L126" t="str">
-        <f>B126&amp;"."&amp;C126</f>
+        <f t="shared" si="13"/>
         <v>!MedicationDispense.whenHandedOver</v>
       </c>
       <c r="M126" t="s">
@@ -9818,7 +9818,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB126" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
+  <autoFilter ref="A1:AB126" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Device"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
@@ -9832,13 +9838,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:K96"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C73" activePane="bottomRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C99" sqref="C99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -9890,7 +9894,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -9915,7 +9919,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -9940,7 +9944,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -9965,7 +9969,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -9990,7 +9994,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10021,7 +10025,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10046,7 +10050,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -10071,7 +10075,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -10097,7 +10101,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -10124,7 +10128,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10150,7 +10154,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10175,7 +10179,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10206,7 +10210,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10231,7 +10235,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10256,7 +10260,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10287,7 +10291,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10318,7 +10322,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and location</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10344,7 +10348,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10375,7 +10379,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10406,7 +10410,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and discharge-disposition</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -10433,7 +10437,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -10459,7 +10463,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -10484,7 +10488,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10510,7 +10514,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10537,7 +10541,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10564,7 +10568,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -10591,7 +10595,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10616,7 +10620,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10641,7 +10645,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -10666,7 +10670,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -10697,7 +10701,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -10728,7 +10732,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified death-date and family</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -10759,7 +10763,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -10790,7 +10794,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -10821,7 +10825,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10854,7 +10858,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -10887,7 +10891,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -10917,7 +10921,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -10947,7 +10951,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -10977,7 +10981,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -11007,7 +11011,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -11037,7 +11041,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -11067,7 +11071,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -11097,7 +11101,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -11128,7 +11132,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -11159,14 +11163,14 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
       <c r="B47" t="s">
         <v>178</v>
       </c>
-      <c r="C47" s="21" t="s">
+      <c r="C47" t="s">
         <v>694</v>
       </c>
       <c r="D47" t="s">
@@ -11189,14 +11193,14 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>178</v>
       </c>
-      <c r="C48" s="21" t="s">
+      <c r="C48" t="s">
         <v>694</v>
       </c>
       <c r="D48" t="s">
@@ -11222,14 +11226,14 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>178</v>
       </c>
-      <c r="C49" s="21" t="s">
+      <c r="C49" t="s">
         <v>694</v>
       </c>
       <c r="D49" t="s">
@@ -11252,14 +11256,14 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" ht="17" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>178</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C50" t="s">
         <v>694</v>
       </c>
       <c r="D50" t="s">
@@ -11285,14 +11289,14 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
       <c r="B51" t="s">
         <v>178</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C51" t="s">
         <v>694</v>
       </c>
       <c r="D51" t="s">
@@ -11315,7 +11319,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -11346,7 +11350,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -11377,7 +11381,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -11410,7 +11414,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -11443,7 +11447,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -11476,7 +11480,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -11509,7 +11513,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -11540,7 +11544,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -11570,7 +11574,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -11601,7 +11605,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -11632,7 +11636,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -11663,14 +11667,14 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>182</v>
       </c>
-      <c r="C63" s="21" t="s">
+      <c r="C63" t="s">
         <v>695</v>
       </c>
       <c r="D63" t="s">
@@ -11695,14 +11699,14 @@
         <v>310</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
       <c r="B64" t="s">
         <v>182</v>
       </c>
-      <c r="C64" s="21" t="s">
+      <c r="C64" t="s">
         <v>695</v>
       </c>
       <c r="D64" t="s">
@@ -11728,14 +11732,14 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
       <c r="B65" t="s">
         <v>182</v>
       </c>
-      <c r="C65" s="21" t="s">
+      <c r="C65" t="s">
         <v>695</v>
       </c>
       <c r="D65" t="s">
@@ -11758,14 +11762,14 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
       <c r="B66" t="s">
         <v>182</v>
       </c>
-      <c r="C66" s="21" t="s">
+      <c r="C66" t="s">
         <v>695</v>
       </c>
       <c r="D66" t="s">
@@ -11791,14 +11795,14 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
       <c r="B67" t="s">
         <v>182</v>
       </c>
-      <c r="C67" s="21" t="s">
+      <c r="C67" t="s">
         <v>695</v>
       </c>
       <c r="D67" t="s">
@@ -11821,14 +11825,14 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
       <c r="B68" t="s">
         <v>309</v>
       </c>
-      <c r="C68" s="21" t="s">
+      <c r="C68" t="s">
         <v>695</v>
       </c>
       <c r="D68" t="s">
@@ -11851,7 +11855,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -11884,7 +11888,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -11916,7 +11920,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -11948,7 +11952,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -11980,7 +11984,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="136" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" ht="137" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -12013,7 +12017,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -12044,7 +12048,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -12073,7 +12077,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -12106,7 +12110,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -12139,7 +12143,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" ht="16" hidden="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -12169,7 +12173,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" ht="20.25" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -12200,15 +12204,15 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
       <c r="B80" t="s">
         <v>246</v>
       </c>
-      <c r="C80" s="21" t="s">
-        <v>696</v>
+      <c r="C80" t="s">
+        <v>693</v>
       </c>
       <c r="D80" t="s">
         <v>117</v>
@@ -12236,7 +12240,7 @@
       <c r="B81" t="s">
         <v>246</v>
       </c>
-      <c r="C81" s="21" t="s">
+      <c r="C81" t="s">
         <v>693</v>
       </c>
       <c r="D81" t="s">
@@ -12261,7 +12265,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -12291,7 +12295,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -12322,7 +12326,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -12353,7 +12357,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -12384,7 +12388,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -12415,7 +12419,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -12446,7 +12450,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -12477,7 +12481,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and description</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -12508,7 +12512,7 @@
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -12542,7 +12546,7 @@
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -12573,7 +12577,7 @@
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -12607,7 +12611,7 @@
         <v>Fetches a bundle of all QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -12638,7 +12642,7 @@
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:11" ht="151" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -12673,7 +12677,7 @@
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed)).</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -12708,7 +12712,7 @@
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed).</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -12744,7 +12748,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
+  <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="Device"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K124">
     <sortCondition ref="A1"/>
   </sortState>
@@ -12905,24 +12915,24 @@
       <c r="B2" t="s">
         <v>572</v>
       </c>
-      <c r="C2" s="23" t="s">
-        <v>699</v>
+      <c r="C2" s="22" t="s">
+        <v>698</v>
       </c>
       <c r="D2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>692</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>521</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="21" t="s">
         <v>522</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>69</v>
       </c>
     </row>
@@ -13168,7 +13178,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="21" t="s">
+      <c r="A12" t="s">
         <v>686</v>
       </c>
       <c r="B12" t="s">
@@ -13266,7 +13276,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="21" t="s">
+      <c r="A19" t="s">
         <v>347</v>
       </c>
       <c r="B19" t="s">
@@ -13771,7 +13781,7 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="B55" t="s">
         <v>604</v>
@@ -14116,7 +14126,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14395,7 +14405,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="T21" t="s">
         <v>19</v>
@@ -14473,7 +14483,7 @@
     </row>
     <row r="25" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B25" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Add USCDI V3 Requirements FHIR-38702 simple observations for assessments
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F4694A-2535-4A49-8C49-ADCC875BA8CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46F3CF16-8F17-B44D-A7F0-B7260BA2C370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33980" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51160" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1926,9 +1926,6 @@
     <t>US Core Birth Sex Extension</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-survey</t>
-  </si>
-  <si>
     <t>US Core Gender Identity Extension</t>
   </si>
   <si>
@@ -2365,6 +2362,9 @@
   </si>
   <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-clinical-result</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation-screening-assessment</t>
   </si>
 </sst>
 </file>
@@ -2556,7 +2556,7 @@
     <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFill="1"/>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="3" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2986,7 +2986,7 @@
         <v>451</v>
       </c>
       <c r="B2" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -4368,7 +4368,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="D25" t="s">
         <v>30</v>
@@ -4645,7 +4645,7 @@
         <v>56</v>
       </c>
       <c r="Y30" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="Z30" t="s">
         <v>172</v>
@@ -4667,7 +4667,7 @@
         <v>84</v>
       </c>
       <c r="C31" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="D31" t="s">
         <v>30</v>
@@ -4692,19 +4692,19 @@
         <v>57</v>
       </c>
       <c r="L31" t="s">
+        <v>673</v>
+      </c>
+      <c r="M31" t="s">
+        <v>56</v>
+      </c>
+      <c r="O31" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y31" s="4" t="s">
         <v>674</v>
       </c>
-      <c r="M31" t="s">
-        <v>56</v>
-      </c>
-      <c r="O31" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y31" s="4" t="s">
+      <c r="Z31" t="s">
         <v>675</v>
-      </c>
-      <c r="Z31" t="s">
-        <v>676</v>
       </c>
       <c r="AA31" s="9" t="str">
         <f>"Fetches a bundle of all "&amp;B31&amp;" resources matching the name"</f>
@@ -4720,7 +4720,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C32" t="s">
         <v>55</v>
@@ -4745,7 +4745,7 @@
         <v>57</v>
       </c>
       <c r="L32" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="M32" t="s">
         <v>56</v>
@@ -4763,7 +4763,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C33" t="s">
         <v>70</v>
@@ -4807,7 +4807,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C34" t="s">
         <v>67</v>
@@ -4854,7 +4854,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C35" t="s">
         <v>61</v>
@@ -4898,7 +4898,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C36" t="s">
         <v>62</v>
@@ -4954,7 +4954,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C37" t="s">
         <v>59</v>
@@ -4998,7 +4998,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="C38" t="s">
         <v>66</v>
@@ -9204,7 +9204,7 @@
         <v>56</v>
       </c>
       <c r="Y115" s="4" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="Z115" s="4" t="str">
         <f>"GET [base]/"&amp;B115&amp;"?"&amp;C115&amp;"=Mary Shaw"</f>
@@ -9224,7 +9224,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C116" t="s">
         <v>55</v>
@@ -9263,7 +9263,7 @@
         <v>support fetching a !QuestionnaireResponse</v>
       </c>
       <c r="Z116" s="4" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="AB116" t="str">
         <f t="shared" si="12"/>
@@ -9275,7 +9275,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C117" t="s">
         <v>89</v>
@@ -9334,7 +9334,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C118" t="s">
         <v>61</v>
@@ -9375,7 +9375,7 @@
         <v>56</v>
       </c>
       <c r="Y118" s="19" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="AB118" t="str">
         <f t="shared" si="12"/>
@@ -9387,10 +9387,10 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C119" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="D119" t="s">
         <v>30</v>
@@ -9415,16 +9415,16 @@
         <v>57</v>
       </c>
       <c r="L119" t="s">
+        <v>700</v>
+      </c>
+      <c r="M119" t="s">
+        <v>56</v>
+      </c>
+      <c r="O119" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y119" s="19" t="s">
         <v>701</v>
-      </c>
-      <c r="M119" t="s">
-        <v>56</v>
-      </c>
-      <c r="O119" t="s">
-        <v>56</v>
-      </c>
-      <c r="Y119" s="19" t="s">
-        <v>702</v>
       </c>
       <c r="AB119" t="str">
         <f t="shared" si="12"/>
@@ -9436,7 +9436,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C120" t="s">
         <v>562</v>
@@ -9480,7 +9480,7 @@
         <v>92</v>
       </c>
       <c r="Y120" s="19" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="AB120" t="str">
         <f t="shared" si="12"/>
@@ -9492,10 +9492,10 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C121" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="D121" t="s">
         <v>30</v>
@@ -9530,7 +9530,7 @@
         <v>56</v>
       </c>
       <c r="Y121" s="19" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="AB121" t="str">
         <f t="shared" si="12"/>
@@ -9542,7 +9542,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="C122" t="s">
         <v>89</v>
@@ -9583,7 +9583,7 @@
         <v>56</v>
       </c>
       <c r="Y122" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="Z122" s="4" t="str">
         <f>"GET [base]/"&amp;B122&amp;"?patient=1137192"</f>
@@ -9603,7 +9603,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C123" t="s">
         <v>61</v>
@@ -9659,7 +9659,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C124" t="s">
         <v>13</v>
@@ -9715,7 +9715,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C125" t="s">
         <v>89</v>
@@ -9756,10 +9756,10 @@
         <v>56</v>
       </c>
       <c r="X125" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="Z125" s="9" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="AA125" s="9" t="str">
         <f>"Fetches a bundle of all "&amp;B125&amp; " resources for the specified patient."</f>
@@ -9775,10 +9775,10 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
+        <v>664</v>
+      </c>
+      <c r="C126" t="s">
         <v>665</v>
-      </c>
-      <c r="C126" t="s">
-        <v>666</v>
       </c>
       <c r="D126" t="s">
         <v>30</v>
@@ -10716,7 +10716,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="F32" t="s">
         <v>69</v>
@@ -10725,10 +10725,10 @@
         <v>133</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="J32" s="4" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" ref="K32" si="7">"Fetches a bundle of all "&amp;B32&amp;" resources matching the specified "&amp;SUBSTITUTE(D32,","," and ")</f>
@@ -10918,7 +10918,7 @@
         <v>149</v>
       </c>
       <c r="J38" s="4" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="K38" s="4" t="s">
         <v>536</v>
@@ -11174,7 +11174,7 @@
         <v>178</v>
       </c>
       <c r="C47" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D47" t="s">
         <v>115</v>
@@ -11204,7 +11204,7 @@
         <v>178</v>
       </c>
       <c r="C48" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D48" t="s">
         <v>144</v>
@@ -11237,7 +11237,7 @@
         <v>178</v>
       </c>
       <c r="C49" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D49" t="s">
         <v>146</v>
@@ -11267,7 +11267,7 @@
         <v>178</v>
       </c>
       <c r="C50" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D50" t="s">
         <v>193</v>
@@ -11300,7 +11300,7 @@
         <v>178</v>
       </c>
       <c r="C51" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D51" t="s">
         <v>217</v>
@@ -11678,7 +11678,7 @@
         <v>182</v>
       </c>
       <c r="C63" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D63" t="s">
         <v>234</v>
@@ -11710,7 +11710,7 @@
         <v>182</v>
       </c>
       <c r="C64" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D64" t="s">
         <v>144</v>
@@ -11743,7 +11743,7 @@
         <v>182</v>
       </c>
       <c r="C65" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D65" t="s">
         <v>146</v>
@@ -11773,7 +11773,7 @@
         <v>182</v>
       </c>
       <c r="C66" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D66" t="s">
         <v>193</v>
@@ -11806,7 +11806,7 @@
         <v>182</v>
       </c>
       <c r="C67" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D67" t="s">
         <v>217</v>
@@ -11836,7 +11836,7 @@
         <v>309</v>
       </c>
       <c r="C68" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="D68" t="s">
         <v>115</v>
@@ -12215,7 +12215,7 @@
         <v>246</v>
       </c>
       <c r="C80" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D80" t="s">
         <v>117</v>
@@ -12244,7 +12244,7 @@
         <v>246</v>
       </c>
       <c r="C81" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="D81" t="s">
         <v>115</v>
@@ -12259,13 +12259,13 @@
         <v>105</v>
       </c>
       <c r="I81" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="J81" s="4" t="s">
         <v>685</v>
       </c>
-      <c r="J81" s="4" t="s">
+      <c r="K81" s="4" t="s">
         <v>686</v>
-      </c>
-      <c r="K81" s="4" t="s">
-        <v>687</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -12489,7 +12489,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C89" t="str">
         <f t="shared" si="12"/>
@@ -12505,10 +12505,10 @@
         <v>105</v>
       </c>
       <c r="I89" t="s">
+        <v>617</v>
+      </c>
+      <c r="J89" s="4" t="s">
         <v>618</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>619</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified "&amp;SUBSTITUTE(D89,","," and ")</f>
@@ -12520,14 +12520,14 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C90" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D90" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="F90" t="s">
         <v>69</v>
@@ -12536,13 +12536,13 @@
         <v>105</v>
       </c>
       <c r="H90" t="s">
+        <v>616</v>
+      </c>
+      <c r="I90" t="s">
         <v>617</v>
       </c>
-      <c r="I90" t="s">
-        <v>618</v>
-      </c>
       <c r="J90" s="4" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="K90" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified "&amp;SUBSTITUTE(D90,","," and  ") &amp; "= 'sdoh'"</f>
@@ -12554,14 +12554,14 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C91" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D91" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="F91" t="s">
         <v>69</v>
@@ -12570,10 +12570,10 @@
         <v>148</v>
       </c>
       <c r="I91" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date"</f>
@@ -12585,14 +12585,14 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C92" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D92" s="17" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F92" t="s">
         <v>69</v>
@@ -12601,13 +12601,13 @@
         <v>216</v>
       </c>
       <c r="H92" t="s">
+        <v>616</v>
+      </c>
+      <c r="I92" t="s">
         <v>617</v>
       </c>
-      <c r="I92" t="s">
-        <v>618</v>
-      </c>
       <c r="J92" s="4" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="K92" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -12619,14 +12619,14 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="C93" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D93" s="17" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F93" t="s">
         <v>69</v>
@@ -12635,10 +12635,10 @@
         <v>90</v>
       </c>
       <c r="I93" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="K93" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -12650,7 +12650,7 @@
         <v>93</v>
       </c>
       <c r="B94" s="17" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="12"/>
@@ -12670,10 +12670,10 @@
       </c>
       <c r="H94" s="17"/>
       <c r="I94" s="4" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -12685,7 +12685,7 @@
         <v>94</v>
       </c>
       <c r="B95" s="17" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="C95" t="str">
         <f t="shared" si="12"/>
@@ -12705,10 +12705,10 @@
       </c>
       <c r="H95" s="17"/>
       <c r="I95" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>670</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>671</v>
       </c>
       <c r="K95" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -12720,14 +12720,14 @@
         <v>95</v>
       </c>
       <c r="B96" s="17" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="12"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D96" s="17" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E96" s="17" t="s">
         <v>56</v>
@@ -12740,10 +12740,10 @@
       </c>
       <c r="H96" s="17"/>
       <c r="I96" s="4" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -12771,7 +12771,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -12801,7 +12801,7 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -12817,7 +12817,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -12833,7 +12833,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -12918,7 +12918,7 @@
         <v>572</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="D2" t="s">
         <v>69</v>
@@ -12926,7 +12926,7 @@
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="B3" s="21" t="s">
         <v>521</v>
@@ -12950,8 +12950,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EBB963-62EF-8346-A79F-04E3300CC06A}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S48" sqref="S48"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13009,8 +13009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView topLeftCell="A12" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13083,7 +13083,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="B5" t="s">
         <v>590</v>
@@ -13097,10 +13097,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="B6" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -13111,16 +13111,16 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>639</v>
+      </c>
+      <c r="B7" t="s">
         <v>640</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
         <v>641</v>
-      </c>
-      <c r="D7" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" t="s">
-        <v>642</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
@@ -13181,7 +13181,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="B12" t="s">
         <v>353</v>
@@ -13195,7 +13195,7 @@
     </row>
     <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="B13" t="s">
         <v>586</v>
@@ -13209,7 +13209,7 @@
     </row>
     <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="B14" t="s">
         <v>592</v>
@@ -13223,7 +13223,7 @@
     </row>
     <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="B15" t="s">
         <v>593</v>
@@ -13237,10 +13237,10 @@
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="B16" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="D16" t="s">
         <v>12</v>
@@ -13251,10 +13251,10 @@
     </row>
     <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="B17" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="D17" t="s">
         <v>12</v>
@@ -13265,10 +13265,10 @@
     </row>
     <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="B18" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D18" t="s">
         <v>12</v>
@@ -13349,16 +13349,16 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
+        <v>655</v>
+      </c>
+      <c r="B24" t="s">
         <v>656</v>
       </c>
-      <c r="B24" t="s">
+      <c r="D24" t="s">
+        <v>12</v>
+      </c>
+      <c r="E24" t="s">
         <v>657</v>
-      </c>
-      <c r="D24" t="s">
-        <v>12</v>
-      </c>
-      <c r="E24" t="s">
-        <v>658</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -13377,10 +13377,10 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>649</v>
+        <v>648</v>
       </c>
       <c r="B26" t="s">
-        <v>645</v>
+        <v>644</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -13391,10 +13391,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
       <c r="B27" t="s">
-        <v>646</v>
+        <v>645</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -13405,10 +13405,10 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="B28" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="D28" t="s">
         <v>12</v>
@@ -13419,7 +13419,7 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="B29" t="s">
         <v>588</v>
@@ -13447,7 +13447,7 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="B31" t="s">
         <v>589</v>
@@ -13586,8 +13586,8 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" s="18" t="s">
-        <v>594</v>
+      <c r="A41" s="23" t="s">
+        <v>708</v>
       </c>
       <c r="B41" t="s">
         <v>585</v>
@@ -13615,10 +13615,10 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="B43" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
       <c r="D43" t="s">
         <v>12</v>
@@ -13629,10 +13629,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="23" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="B44" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -13660,7 +13660,7 @@
         <v>480</v>
       </c>
       <c r="B46" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="D46" t="s">
         <v>12</v>
@@ -13783,16 +13783,16 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="18" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="B55" t="s">
+        <v>599</v>
+      </c>
+      <c r="D55" t="s">
+        <v>12</v>
+      </c>
+      <c r="E55" t="s">
         <v>600</v>
-      </c>
-      <c r="D55" t="s">
-        <v>12</v>
-      </c>
-      <c r="E55" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -13825,16 +13825,16 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
+        <v>650</v>
+      </c>
+      <c r="B58" t="s">
         <v>651</v>
       </c>
-      <c r="B58" t="s">
+      <c r="D58" t="s">
+        <v>12</v>
+      </c>
+      <c r="E58" t="s">
         <v>652</v>
-      </c>
-      <c r="D58" t="s">
-        <v>12</v>
-      </c>
-      <c r="E58" t="s">
-        <v>653</v>
       </c>
     </row>
   </sheetData>
@@ -13852,12 +13852,8 @@
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <hyperlinks>
-    <hyperlink ref="A31" r:id="rId1" xr:uid="{B6435404-5F1C-F845-8B4E-267AEEF8CB8D}"/>
-    <hyperlink ref="A44" r:id="rId2" xr:uid="{26587682-6FC3-6246-8C01-D010FEEB473C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -14016,7 +14012,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="T4" t="s">
         <v>19</v>
@@ -14045,7 +14041,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="T5" t="s">
         <v>19</v>
@@ -14062,7 +14058,7 @@
     </row>
     <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -14088,7 +14084,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="T7" t="s">
         <v>19</v>
@@ -14132,7 +14128,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14155,7 +14151,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="T10" t="s">
         <v>19</v>
@@ -14198,7 +14194,7 @@
         <v>12</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="T12" t="s">
         <v>19</v>
@@ -14282,13 +14278,13 @@
     </row>
     <row r="16" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>658</v>
+        <v>657</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="T16" t="s">
         <v>19</v>
@@ -14300,7 +14296,7 @@
         <v>69</v>
       </c>
       <c r="W16" s="6" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="X16" s="14" t="s">
         <v>434</v>
@@ -14346,7 +14342,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="T18" t="s">
         <v>19</v>
@@ -14369,7 +14365,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
       <c r="T19" t="s">
         <v>19</v>
@@ -14388,7 +14384,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
       <c r="T20" t="s">
         <v>19</v>
@@ -14411,7 +14407,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="T21" t="s">
         <v>19</v>
@@ -14455,7 +14451,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="T23" t="s">
         <v>19</v>
@@ -14478,7 +14474,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="T24" t="s">
         <v>19</v>
@@ -14489,13 +14485,13 @@
     </row>
     <row r="25" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="B25" t="s">
         <v>69</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="T25" t="s">
         <v>19</v>
@@ -14552,7 +14548,7 @@
     </row>
     <row r="28" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -14643,7 +14639,7 @@
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="64" x14ac:dyDescent="0.2">
@@ -14721,7 +14717,7 @@
         <v>359</v>
       </c>
       <c r="F1" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="G1" t="s">
         <v>360</v>
@@ -14751,7 +14747,7 @@
         <v>367</v>
       </c>
       <c r="P1" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="Q1" t="s">
         <v>368</v>
@@ -14784,7 +14780,7 @@
         <v>424</v>
       </c>
       <c r="AA1" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="AB1" t="s">
         <v>578</v>
@@ -14793,10 +14789,10 @@
         <v>579</v>
       </c>
       <c r="AD1" t="s">
+        <v>653</v>
+      </c>
+      <c r="AE1" t="s">
         <v>654</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>655</v>
       </c>
       <c r="AF1" t="s">
         <v>433</v>

</xml_diff>

<commit_message>
Change RelatedPerson search to combination of Patient + Name [FHIR-39791]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\US-Core\input\resources_spreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01546C9B-E402-4652-A2E6-FD61AF13DC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC76624C-37E9-424E-8C72-EE613AF3F53C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34140" yWindow="500" windowWidth="34120" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -26,8 +26,8 @@
     <sheet name="sp_combos" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$96</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$128</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2703" uniqueCount="715">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2705" uniqueCount="719">
   <si>
     <t>Element</t>
   </si>
@@ -2385,12 +2385,24 @@
   <si>
     <t>Fetches a bundle of all Condition resources for the specified patient and all "active" statuses (active,relapse,remission). This will *exclude* diagnoses and health concerns without a clinicalStatus specified.</t>
   </si>
+  <si>
+    <t>patient,name</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>reference,string</t>
+  </si>
+  <si>
+    <t>GET [base]/RelatedPerson?patient=1137192&amp;name=van%20Putten</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2541,7 +2553,7 @@
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2575,6 +2587,7 @@
     <xf numFmtId="49" fontId="13" fillId="2" borderId="0" xfId="2" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -3016,12 +3029,12 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -3029,7 +3042,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>450</v>
       </c>
@@ -3037,7 +3050,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>451</v>
       </c>
@@ -3045,7 +3058,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>446</v>
       </c>
@@ -3053,7 +3066,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>448</v>
       </c>
@@ -3061,7 +3074,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -3069,7 +3082,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>452</v>
       </c>
@@ -3077,7 +3090,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>453</v>
       </c>
@@ -3085,7 +3098,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>516</v>
       </c>
@@ -3100,33 +3113,34 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9F73F9-34B4-C04F-A2E4-99114F8B7BF7}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AB128"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C72" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A108" sqref="A108"/>
+      <selection pane="bottomRight" activeCell="K114" sqref="K114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.95" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="33.42578125" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.5" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="37.83203125" customWidth="1"/>
     <col min="7" max="7" width="60" customWidth="1"/>
-    <col min="10" max="10" width="14.28515625" customWidth="1"/>
-    <col min="12" max="12" width="31.140625" customWidth="1"/>
-    <col min="13" max="24" width="13.28515625" customWidth="1"/>
-    <col min="25" max="25" width="85.28515625" customWidth="1"/>
-    <col min="26" max="26" width="90.7109375" customWidth="1"/>
-    <col min="27" max="27" width="83.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.140625" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" customWidth="1"/>
+    <col min="12" max="12" width="31.1640625" customWidth="1"/>
+    <col min="13" max="24" width="13.33203125" customWidth="1"/>
+    <col min="25" max="25" width="85.33203125" customWidth="1"/>
+    <col min="26" max="26" width="90.6640625" customWidth="1"/>
+    <col min="27" max="27" width="83.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="18.95" customHeight="1" thickBot="1">
+    <row r="1" spans="1:28" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>140</v>
       </c>
@@ -3212,7 +3226,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="18.95" customHeight="1" thickTop="1">
+    <row r="2" spans="1:28" ht="19" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3259,7 +3273,7 @@
         <v>SearchParameter-us-core-!example category search-category.html</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="18.95" customHeight="1">
+    <row r="3" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3306,7 +3320,7 @@
         <v>SearchParameter-us-core-!example code search-code.html</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="18.95" customHeight="1">
+    <row r="4" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3357,7 +3371,7 @@
         <v>SearchParameter-us-core-!example date search-date.html</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="18.95" customHeight="1">
+    <row r="5" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3416,7 +3430,7 @@
         <v>SearchParameter-us-core-!example patient search-patient.html</v>
       </c>
     </row>
-    <row r="6" spans="1:28" ht="18.95" customHeight="1">
+    <row r="6" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3463,7 +3477,7 @@
         <v>SearchParameter-us-core-!example status search-status.html</v>
       </c>
     </row>
-    <row r="7" spans="1:28" ht="18.95" customHeight="1">
+    <row r="7" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3514,7 +3528,7 @@
         <v>SearchParameter-us-core-!patient-address.html</v>
       </c>
     </row>
-    <row r="8" spans="1:28" ht="18.95" customHeight="1">
+    <row r="8" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3565,7 +3579,7 @@
         <v>SearchParameter-us-core-!patient-telecom.html</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="18.95" customHeight="1">
+    <row r="9" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3614,7 +3628,7 @@
         <v>SearchParameter-us-core-allergyintolerance-clinical-status.html</v>
       </c>
     </row>
-    <row r="10" spans="1:28" ht="18.95" customHeight="1">
+    <row r="10" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3672,7 +3686,7 @@
         <v>SearchParameter-us-core-allergyintolerance-patient.html</v>
       </c>
     </row>
-    <row r="11" spans="1:28" ht="18.95" customHeight="1">
+    <row r="11" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3722,7 +3736,7 @@
         <v>SearchParameter-us-core-condition-category.html</v>
       </c>
     </row>
-    <row r="12" spans="1:28" ht="18.95" customHeight="1">
+    <row r="12" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3770,7 +3784,7 @@
         <v>SearchParameter-us-core-condition-clinical-status.html</v>
       </c>
     </row>
-    <row r="13" spans="1:28" ht="18.95" customHeight="1">
+    <row r="13" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3828,7 +3842,7 @@
         <v>SearchParameter-us-core-condition-patient.html</v>
       </c>
     </row>
-    <row r="14" spans="1:28" ht="18.95" customHeight="1">
+    <row r="14" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -3881,7 +3895,7 @@
         <v>SearchParameter-us-core-encounter-id.html</v>
       </c>
     </row>
-    <row r="15" spans="1:28" ht="18.95" customHeight="1">
+    <row r="15" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -3931,7 +3945,7 @@
         <v>SearchParameter-us-core-encounter-class.html</v>
       </c>
     </row>
-    <row r="16" spans="1:28" ht="18.95" customHeight="1">
+    <row r="16" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -3985,7 +3999,7 @@
         <v>SearchParameter-us-core-encounter-date.html</v>
       </c>
     </row>
-    <row r="17" spans="1:28" ht="18.95" customHeight="1">
+    <row r="17" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4042,7 +4056,7 @@
         <v>SearchParameter-us-core-encounter-identifier.html</v>
       </c>
     </row>
-    <row r="18" spans="1:28" ht="18.95" customHeight="1">
+    <row r="18" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4100,7 +4114,7 @@
         <v>SearchParameter-us-core-encounter-patient.html</v>
       </c>
     </row>
-    <row r="19" spans="1:28" ht="18.95" customHeight="1">
+    <row r="19" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4158,7 +4172,7 @@
         <v>SearchParameter-us-core-encounter-location.html</v>
       </c>
     </row>
-    <row r="20" spans="1:28" ht="18.95" customHeight="1">
+    <row r="20" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4208,7 +4222,7 @@
         <v>SearchParameter-us-core-encounter-status.html</v>
       </c>
     </row>
-    <row r="21" spans="1:28" ht="18.95" customHeight="1">
+    <row r="21" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4258,7 +4272,7 @@
         <v>SearchParameter-us-core-encounter-type.html</v>
       </c>
     </row>
-    <row r="22" spans="1:28" ht="18.95" customHeight="1">
+    <row r="22" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4308,7 +4322,7 @@
         <v>SearchParameter-us-core-encounter-discharge-disposition.html</v>
       </c>
     </row>
-    <row r="23" spans="1:28" ht="18.95" customHeight="1">
+    <row r="23" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4358,7 +4372,7 @@
         <v>SearchParameter-us-core-patient-id.html</v>
       </c>
     </row>
-    <row r="24" spans="1:28" ht="18.95" customHeight="1">
+    <row r="24" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4405,7 +4419,7 @@
         <v>SearchParameter-us-core-patient-birthdate.html</v>
       </c>
     </row>
-    <row r="25" spans="1:28" ht="18.95" customHeight="1">
+    <row r="25" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4452,7 +4466,7 @@
         <v>SearchParameter-us-core-patient-death-date.html</v>
       </c>
     </row>
-    <row r="26" spans="1:28" ht="18.95" customHeight="1">
+    <row r="26" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4498,7 +4512,7 @@
         <v>SearchParameter-us-core-patient-family.html</v>
       </c>
     </row>
-    <row r="27" spans="1:28" ht="18.95" customHeight="1">
+    <row r="27" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4546,7 +4560,7 @@
         <v>SearchParameter-us-core-patient-gender.html</v>
       </c>
     </row>
-    <row r="28" spans="1:28" ht="18.95" customHeight="1">
+    <row r="28" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4590,7 +4604,7 @@
         <v>SearchParameter-us-core-patient-given.html</v>
       </c>
     </row>
-    <row r="29" spans="1:28" ht="18.95" customHeight="1">
+    <row r="29" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4647,7 +4661,7 @@
         <v>SearchParameter-us-core-patient-identifier.html</v>
       </c>
     </row>
-    <row r="30" spans="1:28" ht="18.95" customHeight="1">
+    <row r="30" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4701,7 +4715,7 @@
         <v>SearchParameter-us-core-patient-name.html</v>
       </c>
     </row>
-    <row r="31" spans="1:28" ht="18.95" customHeight="1">
+    <row r="31" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4754,7 +4768,7 @@
         <v>SearchParameter-us-core-!patient-tribal-affiliation.html</v>
       </c>
     </row>
-    <row r="32" spans="1:28" ht="18.95" customHeight="1">
+    <row r="32" spans="1:28" ht="19" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4797,7 +4811,7 @@
         <v>SearchParameter-us-core-!!questionnaire-_id.html</v>
       </c>
     </row>
-    <row r="33" spans="1:28" ht="18.95" customHeight="1">
+    <row r="33" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4841,7 +4855,7 @@
         <v>SearchParameter-us-core-!!questionnaire-context-type-value.html</v>
       </c>
     </row>
-    <row r="34" spans="1:28" ht="18.95" customHeight="1">
+    <row r="34" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4888,7 +4902,7 @@
         <v>SearchParameter-us-core-!!questionnaire-publisher.html</v>
       </c>
     </row>
-    <row r="35" spans="1:28" ht="18.95" customHeight="1">
+    <row r="35" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4932,7 +4946,7 @@
         <v>SearchParameter-us-core-!!questionnaire-status.html</v>
       </c>
     </row>
-    <row r="36" spans="1:28" ht="18.95" customHeight="1">
+    <row r="36" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4988,7 +5002,7 @@
         <v>SearchParameter-us-core-!!questionnaire-title.html</v>
       </c>
     </row>
-    <row r="37" spans="1:28" ht="18.95" customHeight="1">
+    <row r="37" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -5032,7 +5046,7 @@
         <v>SearchParameter-us-core-!!questionnaire-url.html</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="18.95" customHeight="1">
+    <row r="38" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -5076,7 +5090,7 @@
         <v>SearchParameter-us-core-!!questionnaire-version.html</v>
       </c>
     </row>
-    <row r="39" spans="1:28" ht="18.95" customHeight="1">
+    <row r="39" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -5130,7 +5144,7 @@
         <v>SearchParameter-us-core-condition-onset-date.html</v>
       </c>
     </row>
-    <row r="40" spans="1:28" ht="18.95" customHeight="1">
+    <row r="40" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -5184,7 +5198,7 @@
         <v>SearchParameter-us-core-condition-asserted-date.html</v>
       </c>
     </row>
-    <row r="41" spans="1:28" ht="18.95" customHeight="1">
+    <row r="41" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -5238,7 +5252,7 @@
         <v>SearchParameter-us-core-condition-recorded-date.html</v>
       </c>
     </row>
-    <row r="42" spans="1:28" ht="18.95" customHeight="1">
+    <row r="42" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -5292,7 +5306,7 @@
         <v>SearchParameter-us-core-condition-abatement-date.html</v>
       </c>
     </row>
-    <row r="43" spans="1:28" ht="18.95" customHeight="1">
+    <row r="43" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -5342,7 +5356,7 @@
         <v>SearchParameter-us-core-condition-code.html</v>
       </c>
     </row>
-    <row r="44" spans="1:28" ht="18.95" customHeight="1">
+    <row r="44" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -5400,7 +5414,7 @@
         <v>SearchParameter-us-core-condition-encounter.html</v>
       </c>
     </row>
-    <row r="45" spans="1:28" ht="18.95" customHeight="1">
+    <row r="45" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -5459,7 +5473,7 @@
         <v>SearchParameter-us-core-immunization-patient.html</v>
       </c>
     </row>
-    <row r="46" spans="1:28" ht="18.95" customHeight="1">
+    <row r="46" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -5509,7 +5523,7 @@
         <v>SearchParameter-us-core-immunization-status.html</v>
       </c>
     </row>
-    <row r="47" spans="1:28" ht="18.95" customHeight="1">
+    <row r="47" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -5563,7 +5577,7 @@
         <v>SearchParameter-us-core-immunization-date.html</v>
       </c>
     </row>
-    <row r="48" spans="1:28" ht="18.95" customHeight="1">
+    <row r="48" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -5616,7 +5630,7 @@
         <v>SearchParameter-us-core-documentreference-_id.html</v>
       </c>
     </row>
-    <row r="49" spans="1:28" ht="18.95" customHeight="1">
+    <row r="49" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -5669,7 +5683,7 @@
         <v>SearchParameter-us-core-documentreference-status.html</v>
       </c>
     </row>
-    <row r="50" spans="1:28" ht="18.95" customHeight="1">
+    <row r="50" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -5728,7 +5742,7 @@
         <v>SearchParameter-us-core-documentreference-patient.html</v>
       </c>
     </row>
-    <row r="51" spans="1:28" ht="18.95" customHeight="1">
+    <row r="51" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -5778,7 +5792,7 @@
         <v>SearchParameter-us-core-documentreference-category.html</v>
       </c>
     </row>
-    <row r="52" spans="1:28" ht="18.95" customHeight="1">
+    <row r="52" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -5828,7 +5842,7 @@
         <v>SearchParameter-us-core-documentreference-type.html</v>
       </c>
     </row>
-    <row r="53" spans="1:28" ht="18.95" customHeight="1">
+    <row r="53" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -5882,7 +5896,7 @@
         <v>SearchParameter-us-core-documentreference-date.html</v>
       </c>
     </row>
-    <row r="54" spans="1:28" ht="18.95" customHeight="1">
+    <row r="54" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -5935,7 +5949,7 @@
         <v>SearchParameter-us-core-documentreference-period.html</v>
       </c>
     </row>
-    <row r="55" spans="1:28" ht="18.95" customHeight="1">
+    <row r="55" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -5988,7 +6002,7 @@
         <v>SearchParameter-us-core-diagnosticreport-status.html</v>
       </c>
     </row>
-    <row r="56" spans="1:28" ht="18.95" customHeight="1">
+    <row r="56" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -6047,7 +6061,7 @@
         <v>SearchParameter-us-core-diagnosticreport-patient.html</v>
       </c>
     </row>
-    <row r="57" spans="1:28" ht="18.95" customHeight="1">
+    <row r="57" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -6097,7 +6111,7 @@
         <v>SearchParameter-us-core-diagnosticreport-category.html</v>
       </c>
     </row>
-    <row r="58" spans="1:28" ht="18.95" customHeight="1">
+    <row r="58" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -6150,7 +6164,7 @@
         <v>SearchParameter-us-core-diagnosticreport-code.html</v>
       </c>
     </row>
-    <row r="59" spans="1:28" ht="18.95" customHeight="1">
+    <row r="59" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -6204,7 +6218,7 @@
         <v>SearchParameter-us-core-diagnosticreport-date.html</v>
       </c>
     </row>
-    <row r="60" spans="1:28" ht="18.95" customHeight="1">
+    <row r="60" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -6254,7 +6268,7 @@
         <v>SearchParameter-us-core-goal-lifecycle-status.html</v>
       </c>
     </row>
-    <row r="61" spans="1:28" ht="18.95" customHeight="1">
+    <row r="61" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -6313,7 +6327,7 @@
         <v>SearchParameter-us-core-goal-patient.html</v>
       </c>
     </row>
-    <row r="62" spans="1:28" ht="18.95" customHeight="1">
+    <row r="62" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -6367,7 +6381,7 @@
         <v>SearchParameter-us-core-goal-target-date.html</v>
       </c>
     </row>
-    <row r="63" spans="1:28" ht="18.95" customHeight="1">
+    <row r="63" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -6420,7 +6434,7 @@
         <v>SearchParameter-us-core-medicationrequest-status.html</v>
       </c>
     </row>
-    <row r="64" spans="1:28" ht="18.95" customHeight="1">
+    <row r="64" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -6473,7 +6487,7 @@
         <v>SearchParameter-us-core-medicationrequest-intent.html</v>
       </c>
     </row>
-    <row r="65" spans="1:28" ht="18.95" customHeight="1">
+    <row r="65" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -6526,7 +6540,7 @@
         <v>SearchParameter-us-core-medicationrequest-patient.html</v>
       </c>
     </row>
-    <row r="66" spans="1:28" ht="18.95" customHeight="1">
+    <row r="66" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -6577,7 +6591,7 @@
         <v>SearchParameter-us-core-medicationrequest-encounter.html</v>
       </c>
     </row>
-    <row r="67" spans="1:28" ht="18.95" customHeight="1">
+    <row r="67" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -6631,7 +6645,7 @@
         <v>SearchParameter-us-core-medicationrequest-authoredon.html</v>
       </c>
     </row>
-    <row r="68" spans="1:28" ht="18.95" customHeight="1">
+    <row r="68" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -6684,7 +6698,7 @@
         <v>SearchParameter-us-core-!medicationstatement-status.html</v>
       </c>
     </row>
-    <row r="69" spans="1:28" ht="18.95" customHeight="1">
+    <row r="69" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -6742,7 +6756,7 @@
         <v>SearchParameter-us-core-!medicationstatement-patient.html</v>
       </c>
     </row>
-    <row r="70" spans="1:28" ht="18.95" customHeight="1">
+    <row r="70" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -6796,7 +6810,7 @@
         <v>SearchParameter-us-core-!medicationstatement-effective.html</v>
       </c>
     </row>
-    <row r="71" spans="1:28" ht="18.95" customHeight="1">
+    <row r="71" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -6849,7 +6863,7 @@
         <v>SearchParameter-us-core-procedure-status.html</v>
       </c>
     </row>
-    <row r="72" spans="1:28" ht="18.95" customHeight="1">
+    <row r="72" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -6907,7 +6921,7 @@
         <v>SearchParameter-us-core-procedure-patient.html</v>
       </c>
     </row>
-    <row r="73" spans="1:28" ht="18.95" customHeight="1">
+    <row r="73" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -6961,7 +6975,7 @@
         <v>SearchParameter-us-core-procedure-date.html</v>
       </c>
     </row>
-    <row r="74" spans="1:28" ht="18.95" customHeight="1">
+    <row r="74" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -7014,7 +7028,7 @@
         <v>SearchParameter-us-core-procedure-code.html</v>
       </c>
     </row>
-    <row r="75" spans="1:28" ht="18.95" customHeight="1">
+    <row r="75" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -7067,7 +7081,7 @@
         <v>SearchParameter-us-core-observation-status.html</v>
       </c>
     </row>
-    <row r="76" spans="1:28" ht="18.95" customHeight="1">
+    <row r="76" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -7117,7 +7131,7 @@
         <v>SearchParameter-us-core-observation-category.html</v>
       </c>
     </row>
-    <row r="77" spans="1:28" ht="18.95" customHeight="1">
+    <row r="77" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -7170,7 +7184,7 @@
         <v>SearchParameter-us-core-observation-code.html</v>
       </c>
     </row>
-    <row r="78" spans="1:28" ht="18.95" customHeight="1">
+    <row r="78" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -7224,7 +7238,7 @@
         <v>SearchParameter-us-core-observation-date.html</v>
       </c>
     </row>
-    <row r="79" spans="1:28" ht="18.95" customHeight="1">
+    <row r="79" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -7283,7 +7297,7 @@
         <v>SearchParameter-us-core-observation-patient.html</v>
       </c>
     </row>
-    <row r="80" spans="1:28" ht="18.95" customHeight="1">
+    <row r="80" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -7333,7 +7347,7 @@
         <v>SearchParameter-us-core-careplan-category.html</v>
       </c>
     </row>
-    <row r="81" spans="1:28" ht="18.95" customHeight="1">
+    <row r="81" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -7383,7 +7397,7 @@
         <v>SearchParameter-us-core-!careplan-code.html</v>
       </c>
     </row>
-    <row r="82" spans="1:28" ht="18.95" customHeight="1">
+    <row r="82" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -7437,7 +7451,7 @@
         <v>SearchParameter-us-core-careplan-date.html</v>
       </c>
     </row>
-    <row r="83" spans="1:28" ht="18.95" customHeight="1">
+    <row r="83" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -7496,7 +7510,7 @@
         <v>SearchParameter-us-core-careplan-patient.html</v>
       </c>
     </row>
-    <row r="84" spans="1:28" ht="18.95" customHeight="1">
+    <row r="84" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -7549,7 +7563,7 @@
         <v>SearchParameter-us-core-careplan-status.html</v>
       </c>
     </row>
-    <row r="85" spans="1:28" ht="18.95" customHeight="1">
+    <row r="85" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -7611,7 +7625,7 @@
         <v>SearchParameter-us-core-careteam-patient.html</v>
       </c>
     </row>
-    <row r="86" spans="1:28" ht="18.95" customHeight="1">
+    <row r="86" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -7664,7 +7678,7 @@
         <v>SearchParameter-us-core-practitioner-id.html</v>
       </c>
     </row>
-    <row r="87" spans="1:28" ht="18.95" customHeight="1">
+    <row r="87" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -7717,7 +7731,7 @@
         <v>SearchParameter-us-core-careteam-status.html</v>
       </c>
     </row>
-    <row r="88" spans="1:28" ht="18.95" customHeight="1">
+    <row r="88" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -7775,7 +7789,7 @@
         <v>SearchParameter-us-core-careteam-role.html</v>
       </c>
     </row>
-    <row r="89" spans="1:28" ht="18.95" customHeight="1">
+    <row r="89" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -7834,7 +7848,7 @@
         <v>SearchParameter-us-core-device-patient.html</v>
       </c>
     </row>
-    <row r="90" spans="1:28" ht="18.95" customHeight="1">
+    <row r="90" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -7883,7 +7897,7 @@
         <v>SearchParameter-us-core-device-type.html</v>
       </c>
     </row>
-    <row r="91" spans="1:28" ht="18.95" customHeight="1">
+    <row r="91" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -7935,7 +7949,7 @@
         <v>SearchParameter-us-core-device-status.html</v>
       </c>
     </row>
-    <row r="92" spans="1:28" ht="18.95" customHeight="1">
+    <row r="92" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -7990,7 +8004,7 @@
         <v>SearchParameter-us-core-location-name.html</v>
       </c>
     </row>
-    <row r="93" spans="1:28" ht="18.95" customHeight="1">
+    <row r="93" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -8045,7 +8059,7 @@
         <v>SearchParameter-us-core-location-address.html</v>
       </c>
     </row>
-    <row r="94" spans="1:28" ht="18.95" customHeight="1">
+    <row r="94" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -8100,7 +8114,7 @@
         <v>SearchParameter-us-core-location-address-city.html</v>
       </c>
     </row>
-    <row r="95" spans="1:28" ht="18.95" customHeight="1">
+    <row r="95" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -8154,7 +8168,7 @@
         <v>SearchParameter-us-core-location-address-state.html</v>
       </c>
     </row>
-    <row r="96" spans="1:28" ht="18.95" customHeight="1">
+    <row r="96" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -8209,7 +8223,7 @@
         <v>SearchParameter-us-core-location-address-postalcode.html</v>
       </c>
     </row>
-    <row r="97" spans="1:28" ht="18.95" customHeight="1">
+    <row r="97" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -8264,7 +8278,7 @@
         <v>SearchParameter-us-core-organization-name.html</v>
       </c>
     </row>
-    <row r="98" spans="1:28" ht="18.95" customHeight="1">
+    <row r="98" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -8319,7 +8333,7 @@
         <v>SearchParameter-us-core-organization-address.html</v>
       </c>
     </row>
-    <row r="99" spans="1:28" ht="18.95" customHeight="1">
+    <row r="99" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -8374,7 +8388,7 @@
         <v>SearchParameter-us-core-!organization-address-city.html</v>
       </c>
     </row>
-    <row r="100" spans="1:28" ht="18.95" customHeight="1">
+    <row r="100" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -8429,7 +8443,7 @@
         <v>SearchParameter-us-core-!organization-adress-state.html</v>
       </c>
     </row>
-    <row r="101" spans="1:28" ht="18.95" customHeight="1">
+    <row r="101" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -8484,7 +8498,7 @@
         <v>SearchParameter-us-core-!organization-address-postalcode.html</v>
       </c>
     </row>
-    <row r="102" spans="1:28" ht="18.95" customHeight="1">
+    <row r="102" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -8539,7 +8553,7 @@
         <v>SearchParameter-us-core-practitioner-name.html</v>
       </c>
     </row>
-    <row r="103" spans="1:28" ht="18.95" customHeight="1">
+    <row r="103" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -8597,7 +8611,7 @@
         <v>SearchParameter-us-core-practitioner-identifier.html</v>
       </c>
     </row>
-    <row r="104" spans="1:28" ht="18.95" customHeight="1">
+    <row r="104" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -8658,7 +8672,7 @@
         <v>SearchParameter-us-core-practitionerrole-specialty.html</v>
       </c>
     </row>
-    <row r="105" spans="1:28" ht="18.95" customHeight="1">
+    <row r="105" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -8722,7 +8736,7 @@
         <v>SearchParameter-us-core-practitionerrole-practitioner.html</v>
       </c>
     </row>
-    <row r="106" spans="1:28" ht="18.95" customHeight="1">
+    <row r="106" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -8775,7 +8789,7 @@
         <v>SearchParameter-us-core-servicerequest-status.html</v>
       </c>
     </row>
-    <row r="107" spans="1:28" ht="18.95" customHeight="1">
+    <row r="107" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -8834,7 +8848,7 @@
         <v>SearchParameter-us-core-servicerequest-patient.html</v>
       </c>
     </row>
-    <row r="108" spans="1:28" ht="18.95" customHeight="1">
+    <row r="108" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -8884,7 +8898,7 @@
         <v>SearchParameter-us-core-servicerequest-category.html</v>
       </c>
     </row>
-    <row r="109" spans="1:28" ht="18.95" customHeight="1">
+    <row r="109" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -8937,7 +8951,7 @@
         <v>SearchParameter-us-core-servicerequest-code.html</v>
       </c>
     </row>
-    <row r="110" spans="1:28" ht="18.95" customHeight="1">
+    <row r="110" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -8991,7 +9005,7 @@
         <v>SearchParameter-us-core-servicerequest-authored.html</v>
       </c>
     </row>
-    <row r="111" spans="1:28" ht="18.95" customHeight="1">
+    <row r="111" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -9041,7 +9055,7 @@
         <v>SearchParameter-us-core-servicerequest-id.html</v>
       </c>
     </row>
-    <row r="112" spans="1:28" ht="18.95" customHeight="1">
+    <row r="112" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -9087,7 +9101,7 @@
         <v>SearchParameter-us-core-goal-description.html</v>
       </c>
     </row>
-    <row r="113" spans="1:28" ht="18.95" customHeight="1">
+    <row r="113" spans="1:28" ht="19" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -9138,7 +9152,7 @@
         <v>SearchParameter-us-core-relatedperson-id.html</v>
       </c>
     </row>
-    <row r="114" spans="1:28" ht="18.95" customHeight="1">
+    <row r="114" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -9197,7 +9211,7 @@
         <v>SearchParameter-us-core-relatedperson-patient.html</v>
       </c>
     </row>
-    <row r="115" spans="1:28" ht="18.95" customHeight="1">
+    <row r="115" spans="1:28" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -9211,7 +9225,7 @@
         <v>69</v>
       </c>
       <c r="E115" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G115" t="str">
         <f t="shared" si="11"/>
@@ -9252,7 +9266,7 @@
         <v>SearchParameter-us-core-relatedperson-name.html</v>
       </c>
     </row>
-    <row r="116" spans="1:28" ht="18.95" customHeight="1">
+    <row r="116" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -9303,7 +9317,7 @@
         <v>SearchParameter-us-core-questionnaireresponse-id.html</v>
       </c>
     </row>
-    <row r="117" spans="1:28" ht="18.95" customHeight="1">
+    <row r="117" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -9362,7 +9376,7 @@
         <v>SearchParameter-us-core-questionnaireresponse-patient.html</v>
       </c>
     </row>
-    <row r="118" spans="1:28" ht="18.95" customHeight="1">
+    <row r="118" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -9415,7 +9429,7 @@
         <v>SearchParameter-us-core-questionnaireresponse-status.html</v>
       </c>
     </row>
-    <row r="119" spans="1:28" ht="18.95" customHeight="1">
+    <row r="119" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -9464,7 +9478,7 @@
         <v>SearchParameter-us-core-!questionnaireresponse-tag.html</v>
       </c>
     </row>
-    <row r="120" spans="1:28" ht="18.95" customHeight="1">
+    <row r="120" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -9520,7 +9534,7 @@
         <v>SearchParameter-us-core-questionnaireresponse-authored.html</v>
       </c>
     </row>
-    <row r="121" spans="1:28" ht="18.95" customHeight="1">
+    <row r="121" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -9570,7 +9584,7 @@
         <v>SearchParameter-us-core-questionnaireresponse-questionnaire.html</v>
       </c>
     </row>
-    <row r="122" spans="1:28" ht="18.95" customHeight="1">
+    <row r="122" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -9628,7 +9642,7 @@
         <v>SearchParameter-us-core-coverage-patient.html</v>
       </c>
     </row>
-    <row r="123" spans="1:28" ht="18.95" customHeight="1">
+    <row r="123" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -9681,7 +9695,7 @@
         <v>SearchParameter-us-core-medicationdispense-status.html</v>
       </c>
     </row>
-    <row r="124" spans="1:28" ht="18.95" customHeight="1">
+    <row r="124" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -9734,7 +9748,7 @@
         <v>SearchParameter-us-core-medicationdispense-type.html</v>
       </c>
     </row>
-    <row r="125" spans="1:28" ht="51" customHeight="1">
+    <row r="125" spans="1:28" ht="51" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -9791,7 +9805,7 @@
         <v>SearchParameter-us-core-medicationdispense-patient.html</v>
       </c>
     </row>
-    <row r="126" spans="1:28" ht="18.95" customHeight="1">
+    <row r="126" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -9845,7 +9859,7 @@
         <v>SearchParameter-us-core-!medicationdispense-whenhandedover.html</v>
       </c>
     </row>
-    <row r="127" spans="1:28" ht="18.95" customHeight="1">
+    <row r="127" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -9899,7 +9913,7 @@
         <v>SearchParameter-us-core-specimen-_id.html</v>
       </c>
     </row>
-    <row r="128" spans="1:28" ht="18.95" customHeight="1">
+    <row r="128" spans="1:28" ht="19" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -9959,7 +9973,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AB126" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}"/>
+  <autoFilter ref="A1:AB128" xr:uid="{1CF5B17E-E72E-48B2-A597-9C21C12723F0}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="RelatedPerson"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
@@ -9973,27 +9993,30 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:K96"/>
+  <dimension ref="A1:K97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="K74" sqref="K74"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J63" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J94" sqref="J94"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="96.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="96.5" customWidth="1"/>
     <col min="4" max="4" width="33" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" customWidth="1"/>
-    <col min="8" max="8" width="121.7109375" customWidth="1"/>
-    <col min="9" max="9" width="88.85546875" customWidth="1"/>
-    <col min="10" max="10" width="255.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="83.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="121.6640625" customWidth="1"/>
+    <col min="9" max="9" width="88.83203125" customWidth="1"/>
+    <col min="10" max="10" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="83.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" customHeight="1" thickBot="1">
+    <row r="1" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>142</v>
       </c>
@@ -10028,7 +10051,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickTop="1">
+    <row r="2" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -10053,7 +10076,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
       </c>
     </row>
-    <row r="3" spans="1:11">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -10078,7 +10101,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -10103,7 +10126,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -10128,7 +10151,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -10159,7 +10182,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -10184,7 +10207,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -10209,7 +10232,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -10235,7 +10258,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
       </c>
     </row>
-    <row r="10" spans="1:11">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -10262,7 +10285,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
       </c>
     </row>
-    <row r="11" spans="1:11">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -10288,7 +10311,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
       </c>
     </row>
-    <row r="12" spans="1:11">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -10313,7 +10336,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
       </c>
     </row>
-    <row r="13" spans="1:11">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -10344,7 +10367,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -10369,7 +10392,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -10394,7 +10417,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -10425,7 +10448,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
       </c>
     </row>
-    <row r="17" spans="1:11">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -10456,7 +10479,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and location</v>
       </c>
     </row>
-    <row r="18" spans="1:11">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -10482,7 +10505,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
       </c>
     </row>
-    <row r="19" spans="1:11">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -10513,7 +10536,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
       </c>
     </row>
-    <row r="20" spans="1:11">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -10544,7 +10567,7 @@
         <v>Fetches a bundle of all Encounter resources matching the specified patient and discharge-disposition</v>
       </c>
     </row>
-    <row r="21" spans="1:11">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -10571,7 +10594,7 @@
         <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
       </c>
     </row>
-    <row r="22" spans="1:11">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -10597,7 +10620,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
       </c>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -10622,7 +10645,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
       </c>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -10648,7 +10671,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
       </c>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -10675,7 +10698,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
       </c>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -10702,7 +10725,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -10729,7 +10752,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
       </c>
     </row>
-    <row r="28" spans="1:11">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -10754,7 +10777,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
       </c>
     </row>
-    <row r="29" spans="1:11">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -10779,7 +10802,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
       </c>
     </row>
-    <row r="30" spans="1:11">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -10804,7 +10827,7 @@
         <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
       </c>
     </row>
-    <row r="31" spans="1:11">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -10835,7 +10858,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
       </c>
     </row>
-    <row r="32" spans="1:11">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -10866,7 +10889,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified death-date and family</v>
       </c>
     </row>
-    <row r="33" spans="1:11">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -10897,7 +10920,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
       </c>
     </row>
-    <row r="34" spans="1:11">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -10928,7 +10951,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
       </c>
     </row>
-    <row r="35" spans="1:11">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -10959,7 +10982,7 @@
         <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
       </c>
     </row>
-    <row r="36" spans="1:11">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -10992,7 +11015,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="37" spans="1:11">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -11006,9 +11029,6 @@
       <c r="D37" t="s">
         <v>144</v>
       </c>
-      <c r="E37" t="s">
-        <v>56</v>
-      </c>
       <c r="F37" t="s">
         <v>12</v>
       </c>
@@ -11025,7 +11045,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="38" spans="1:11">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -11055,7 +11075,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="39" spans="1:11">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -11085,7 +11105,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="40" spans="1:11">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -11115,7 +11135,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:11">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -11145,7 +11165,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="42" spans="1:11">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -11175,7 +11195,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:11">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -11205,7 +11225,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -11235,7 +11255,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="45" spans="1:11">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -11266,7 +11286,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="46" spans="1:11">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -11297,7 +11317,7 @@
         <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="47" spans="1:11">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -11327,7 +11347,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15.75">
+    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -11360,7 +11380,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15.75">
+    <row r="49" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -11390,7 +11410,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15.75">
+    <row r="50" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -11423,7 +11443,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
       </c>
     </row>
-    <row r="51" spans="1:11">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -11453,7 +11473,7 @@
         <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="52" spans="1:11">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -11484,7 +11504,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
       </c>
     </row>
-    <row r="53" spans="1:11">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -11515,7 +11535,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
       </c>
     </row>
-    <row r="54" spans="1:11">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -11548,7 +11568,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="55" spans="1:11">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -11581,7 +11601,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="56" spans="1:11">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -11614,7 +11634,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="57" spans="1:11">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -11647,7 +11667,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="58" spans="1:11">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -11678,7 +11698,7 @@
         <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="59" spans="1:11">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -11708,7 +11728,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="60" spans="1:11">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -11739,7 +11759,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="61" spans="1:11">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -11770,7 +11790,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="62" spans="1:11">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -11801,7 +11821,7 @@
         <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
       </c>
     </row>
-    <row r="63" spans="1:11">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -11833,7 +11853,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="64" spans="1:11">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -11866,7 +11886,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="65" spans="1:11">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -11896,7 +11916,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
       </c>
     </row>
-    <row r="66" spans="1:11">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -11929,7 +11949,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
       </c>
     </row>
-    <row r="67" spans="1:11">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -11959,7 +11979,7 @@
         <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="68" spans="1:11">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -11989,7 +12009,7 @@
         <v>Fetches a bundle of all !Observation resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="69" spans="1:11">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -12022,7 +12042,7 @@
         <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
       </c>
     </row>
-    <row r="70" spans="1:11">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -12054,7 +12074,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="71" spans="1:11">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -12086,7 +12106,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:11">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -12118,7 +12138,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="143.25">
+    <row r="73" spans="1:11" ht="136" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -12151,7 +12171,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="74" spans="1:11">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -12182,7 +12202,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="20.25" customHeight="1">
+    <row r="75" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -12211,7 +12231,7 @@
         <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="76" spans="1:11">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -12244,7 +12264,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="20.25" customHeight="1">
+    <row r="77" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -12277,7 +12297,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="78" spans="1:11">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -12307,7 +12327,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="20.25" customHeight="1">
+    <row r="79" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -12338,7 +12358,7 @@
         <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
       </c>
     </row>
-    <row r="80" spans="1:11">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -12367,7 +12387,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="81" spans="1:11">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -12380,9 +12400,6 @@
       <c r="D81" t="s">
         <v>115</v>
       </c>
-      <c r="E81" t="s">
-        <v>56</v>
-      </c>
       <c r="F81" t="s">
         <v>69</v>
       </c>
@@ -12399,7 +12416,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="82" spans="1:11">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -12429,7 +12446,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="83" spans="1:11">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -12460,7 +12477,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="84" spans="1:11">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -12491,7 +12508,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
       </c>
     </row>
-    <row r="85" spans="1:11">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -12522,7 +12539,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="86" spans="1:11">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -12553,7 +12570,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
       </c>
     </row>
-    <row r="87" spans="1:11">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -12584,7 +12601,7 @@
         <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
       </c>
     </row>
-    <row r="88" spans="1:11">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -12615,7 +12632,7 @@
         <v>Fetches a bundle of all Goal resources for the specified patient and description</v>
       </c>
     </row>
-    <row r="89" spans="1:11">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -12646,7 +12663,7 @@
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and status</v>
       </c>
     </row>
-    <row r="90" spans="1:11">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -12680,7 +12697,7 @@
         <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
       </c>
     </row>
-    <row r="91" spans="1:11">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -12711,7 +12728,7 @@
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and date</v>
       </c>
     </row>
-    <row r="92" spans="1:11">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -12745,7 +12762,7 @@
         <v>Fetches a bundle of all !QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
       </c>
     </row>
-    <row r="93" spans="1:11">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -12776,7 +12793,7 @@
         <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="150.94999999999999" customHeight="1">
+    <row r="94" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -12790,9 +12807,7 @@
       <c r="D94" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="E94" s="17" t="s">
-        <v>56</v>
-      </c>
+      <c r="E94" s="17"/>
       <c r="F94" s="17" t="s">
         <v>69</v>
       </c>
@@ -12811,7 +12826,7 @@
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed)).</v>
       </c>
     </row>
-    <row r="95" spans="1:11">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -12825,9 +12840,7 @@
       <c r="D95" s="17" t="s">
         <v>116</v>
       </c>
-      <c r="E95" s="17" t="s">
-        <v>56</v>
-      </c>
+      <c r="E95" s="17"/>
       <c r="F95" s="17" t="s">
         <v>69</v>
       </c>
@@ -12846,7 +12859,7 @@
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed).</v>
       </c>
     </row>
-    <row r="96" spans="1:11">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -12860,9 +12873,7 @@
       <c r="D96" s="17" t="s">
         <v>656</v>
       </c>
-      <c r="E96" s="17" t="s">
-        <v>56</v>
-      </c>
+      <c r="E96" s="17"/>
       <c r="F96" s="17" t="s">
         <v>69</v>
       </c>
@@ -12881,19 +12892,54 @@
         <v>Fetches a bundle of all MedicationDispense resources for the specified patient for a given dispense and date or range</v>
       </c>
     </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97" s="17">
+        <v>96</v>
+      </c>
+      <c r="B97" s="17" t="s">
+        <v>575</v>
+      </c>
+      <c r="C97" s="23" t="s">
+        <v>574</v>
+      </c>
+      <c r="D97" s="17" t="s">
+        <v>715</v>
+      </c>
+      <c r="E97" s="17" t="s">
+        <v>716</v>
+      </c>
+      <c r="F97" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G97" s="17" t="s">
+        <v>717</v>
+      </c>
+      <c r="H97" s="17"/>
+      <c r="I97" s="4"/>
+      <c r="J97" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="K97" t="str">
+        <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
+        <v>Fetches a bundle of all RelatedPerson resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:K96" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
+  <autoFilter ref="A1:K97" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K124">
     <sortCondition ref="A1"/>
   </sortState>
-  <conditionalFormatting sqref="B1:B1048576">
+  <conditionalFormatting sqref="B1:B96 B98:B1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C97" r:id="rId1" xr:uid="{7BD4B001-15AD-2A41-B63E-111DE4CF26FB}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -12905,13 +12951,13 @@
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
-    <col min="2" max="2" width="95.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="95.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -12919,7 +12965,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -12927,7 +12973,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>66</v>
       </c>
@@ -12935,7 +12981,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>436</v>
       </c>
@@ -12943,7 +12989,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="255.95" customHeight="1">
+    <row r="5" spans="1:2" ht="256" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -12951,7 +12997,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -12959,7 +13005,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="351.75" customHeight="1">
+    <row r="7" spans="1:2" ht="351.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -12967,7 +13013,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="103.5" customHeight="1">
+    <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -12975,7 +13021,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>500</v>
       </c>
@@ -12983,7 +13029,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>501</v>
       </c>
@@ -12991,7 +13037,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>512</v>
       </c>
@@ -12999,7 +13045,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>513</v>
       </c>
@@ -13020,14 +13066,14 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="61.42578125" customWidth="1"/>
+    <col min="1" max="1" width="61.5" customWidth="1"/>
     <col min="2" max="2" width="71" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -13041,7 +13087,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>515</v>
       </c>
@@ -13055,7 +13101,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="21" t="s">
         <v>680</v>
       </c>
@@ -13085,16 +13131,16 @@
       <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.28515625" customWidth="1"/>
-    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" customWidth="1"/>
+    <col min="3" max="3" width="24.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="65" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.7109375" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="5" max="5" width="50.6640625" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>504</v>
       </c>
@@ -13114,7 +13160,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B2" s="17" t="b">
         <v>1</v>
       </c>
@@ -13144,16 +13190,16 @@
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" customWidth="1"/>
-    <col min="4" max="4" width="20.140625" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
+    <col min="2" max="2" width="60.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="16.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -13170,7 +13216,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>72</v>
       </c>
@@ -13184,7 +13230,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="18" t="s">
         <v>233</v>
       </c>
@@ -13198,7 +13244,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="18" t="s">
         <v>325</v>
       </c>
@@ -13212,7 +13258,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="18" t="s">
         <v>629</v>
       </c>
@@ -13226,7 +13272,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="18" t="s">
         <v>630</v>
       </c>
@@ -13240,7 +13286,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>633</v>
       </c>
@@ -13254,7 +13300,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="18" t="s">
         <v>414</v>
       </c>
@@ -13268,7 +13314,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="18" t="s">
         <v>188</v>
       </c>
@@ -13282,7 +13328,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="18" t="s">
         <v>187</v>
       </c>
@@ -13296,7 +13342,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="18" t="s">
         <v>332</v>
       </c>
@@ -13310,7 +13356,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>675</v>
       </c>
@@ -13324,7 +13370,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.75">
+    <row r="13" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
         <v>597</v>
       </c>
@@ -13338,7 +13384,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.75">
+    <row r="14" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
         <v>598</v>
       </c>
@@ -13352,7 +13398,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="15.75">
+    <row r="15" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
         <v>599</v>
       </c>
@@ -13366,7 +13412,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.75">
+    <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
         <v>600</v>
       </c>
@@ -13380,7 +13426,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.75">
+    <row r="17" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>601</v>
       </c>
@@ -13394,7 +13440,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.75">
+    <row r="18" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
         <v>602</v>
       </c>
@@ -13408,7 +13454,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>347</v>
       </c>
@@ -13422,7 +13468,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>329</v>
       </c>
@@ -13436,7 +13482,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="18" t="s">
         <v>349</v>
       </c>
@@ -13450,7 +13496,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="18" t="s">
         <v>340</v>
       </c>
@@ -13464,7 +13510,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="18" t="s">
         <v>334</v>
       </c>
@@ -13478,7 +13524,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>649</v>
       </c>
@@ -13492,7 +13538,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="18" t="s">
         <v>401</v>
       </c>
@@ -13506,7 +13552,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>642</v>
       </c>
@@ -13520,7 +13566,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>641</v>
       </c>
@@ -13534,7 +13580,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>643</v>
       </c>
@@ -13548,7 +13594,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="18" t="s">
         <v>696</v>
       </c>
@@ -13562,7 +13608,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="18" t="s">
         <v>475</v>
       </c>
@@ -13576,7 +13622,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>695</v>
       </c>
@@ -13590,7 +13636,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="18" t="s">
         <v>474</v>
       </c>
@@ -13604,7 +13650,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="18" t="s">
         <v>473</v>
       </c>
@@ -13618,7 +13664,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="18" t="s">
         <v>483</v>
       </c>
@@ -13632,7 +13678,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="18" t="s">
         <v>426</v>
       </c>
@@ -13646,7 +13692,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="18" t="s">
         <v>272</v>
       </c>
@@ -13660,7 +13706,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="37" spans="1:5">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="18" t="s">
         <v>552</v>
       </c>
@@ -13674,7 +13720,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="38" spans="1:5">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="18" t="s">
         <v>470</v>
       </c>
@@ -13688,7 +13734,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="39" spans="1:5">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="18" t="s">
         <v>471</v>
       </c>
@@ -13702,7 +13748,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="18" t="s">
         <v>469</v>
       </c>
@@ -13716,7 +13762,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>699</v>
       </c>
@@ -13730,7 +13776,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="42" spans="1:5">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="18" t="s">
         <v>468</v>
       </c>
@@ -13744,7 +13790,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="18" t="s">
         <v>697</v>
       </c>
@@ -13758,7 +13804,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>698</v>
       </c>
@@ -13772,7 +13818,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="18" t="s">
         <v>481</v>
       </c>
@@ -13786,7 +13832,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="18" t="s">
         <v>479</v>
       </c>
@@ -13800,7 +13846,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="18" t="s">
         <v>472</v>
       </c>
@@ -13814,7 +13860,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="18" t="s">
         <v>467</v>
       </c>
@@ -13828,7 +13874,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="49" spans="1:5">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="18" t="s">
         <v>336</v>
       </c>
@@ -13842,7 +13888,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="50" spans="1:5">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="18" t="s">
         <v>74</v>
       </c>
@@ -13856,7 +13902,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="18" t="s">
         <v>327</v>
       </c>
@@ -13870,7 +13916,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="52" spans="1:5">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="18" t="s">
         <v>344</v>
       </c>
@@ -13884,7 +13930,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="18" t="s">
         <v>338</v>
       </c>
@@ -13898,7 +13944,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="54" spans="1:5">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="18" t="s">
         <v>422</v>
       </c>
@@ -13912,7 +13958,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="55" spans="1:5">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>704</v>
       </c>
@@ -13926,7 +13972,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>703</v>
       </c>
@@ -13940,7 +13986,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="57" spans="1:5">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="18" t="s">
         <v>574</v>
       </c>
@@ -13954,7 +14000,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="58" spans="1:5">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="18" t="s">
         <v>564</v>
       </c>
@@ -13968,7 +14014,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="59" spans="1:5">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="18" t="s">
         <v>644</v>
       </c>
@@ -14020,23 +14066,23 @@
       <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="21" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="21" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.5" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" customWidth="1"/>
     <col min="7" max="7" width="9" customWidth="1"/>
-    <col min="8" max="14" width="17.42578125" customWidth="1"/>
-    <col min="15" max="15" width="20.42578125" customWidth="1"/>
-    <col min="16" max="19" width="17.42578125" customWidth="1"/>
-    <col min="20" max="21" width="20.42578125" customWidth="1"/>
-    <col min="22" max="25" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="14" width="17.5" customWidth="1"/>
+    <col min="15" max="15" width="20.5" customWidth="1"/>
+    <col min="16" max="19" width="17.5" customWidth="1"/>
+    <col min="20" max="21" width="20.5" customWidth="1"/>
+    <col min="22" max="25" width="38.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="21" customHeight="1" thickBot="1">
+    <row r="1" spans="1:25" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -14113,7 +14159,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="2" spans="1:25" ht="21" customHeight="1" thickTop="1">
+    <row r="2" spans="1:25" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -14136,7 +14182,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:25" ht="21" customHeight="1">
+    <row r="3" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>231</v>
       </c>
@@ -14159,7 +14205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:25" ht="21" customHeight="1">
+    <row r="4" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>245</v>
       </c>
@@ -14188,7 +14234,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:25" ht="21" customHeight="1">
+    <row r="5" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>137</v>
       </c>
@@ -14211,7 +14257,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:25" ht="21" customHeight="1">
+    <row r="6" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>635</v>
       </c>
@@ -14231,7 +14277,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:25" ht="21" customHeight="1">
+    <row r="7" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>246</v>
       </c>
@@ -14254,7 +14300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:25" ht="21" customHeight="1">
+    <row r="8" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>178</v>
       </c>
@@ -14275,7 +14321,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:25" ht="21" customHeight="1">
+    <row r="9" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>177</v>
       </c>
@@ -14298,7 +14344,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:25" ht="21" customHeight="1">
+    <row r="10" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -14321,7 +14367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:25" ht="21" customHeight="1">
+    <row r="11" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>179</v>
       </c>
@@ -14344,7 +14390,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:25" ht="21" customHeight="1">
+    <row r="12" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>160</v>
       </c>
@@ -14367,7 +14413,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:25" ht="21" customHeight="1">
+    <row r="13" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>247</v>
       </c>
@@ -14386,7 +14432,7 @@
       <c r="X13" s="14"/>
       <c r="Y13" s="14"/>
     </row>
-    <row r="14" spans="1:25" ht="21" customHeight="1">
+    <row r="14" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>342</v>
       </c>
@@ -14405,7 +14451,7 @@
       <c r="X14" s="14"/>
       <c r="Y14" s="14"/>
     </row>
-    <row r="15" spans="1:25" ht="21" customHeight="1">
+    <row r="15" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>180</v>
       </c>
@@ -14434,7 +14480,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:25" ht="21" customHeight="1">
+    <row r="16" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>651</v>
       </c>
@@ -14463,7 +14509,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:25" ht="21" customHeight="1">
+    <row r="17" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>420</v>
       </c>
@@ -14492,7 +14538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:25" ht="21" customHeight="1">
+    <row r="18" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>182</v>
       </c>
@@ -14515,7 +14561,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:25" ht="21" customHeight="1">
+    <row r="19" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>257</v>
       </c>
@@ -14534,7 +14580,7 @@
       <c r="X19" s="14"/>
       <c r="Y19" s="14"/>
     </row>
-    <row r="20" spans="1:25" ht="21" customHeight="1">
+    <row r="20" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -14557,7 +14603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:25" ht="21" customHeight="1">
+    <row r="21" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>264</v>
       </c>
@@ -14576,7 +14622,7 @@
       <c r="X21" s="14"/>
       <c r="Y21" s="14"/>
     </row>
-    <row r="22" spans="1:25" ht="21" customHeight="1">
+    <row r="22" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>266</v>
       </c>
@@ -14601,7 +14647,7 @@
       <c r="X22" s="14"/>
       <c r="Y22" s="14"/>
     </row>
-    <row r="23" spans="1:25" ht="21" customHeight="1">
+    <row r="23" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>181</v>
       </c>
@@ -14624,7 +14670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:25" ht="21" customHeight="1">
+    <row r="24" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>421</v>
       </c>
@@ -14641,7 +14687,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:25" ht="23.1" customHeight="1">
+    <row r="25" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>706</v>
       </c>
@@ -14654,7 +14700,7 @@
       <c r="X25" s="14"/>
       <c r="Y25" s="14"/>
     </row>
-    <row r="26" spans="1:25" ht="23.1" customHeight="1">
+    <row r="26" spans="1:25" ht="23" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>595</v>
       </c>
@@ -14671,7 +14717,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="27" spans="1:25" ht="21" customHeight="1">
+    <row r="27" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>575</v>
       </c>
@@ -14691,7 +14737,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:25" ht="21" customHeight="1">
+    <row r="28" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>554</v>
       </c>
@@ -14711,7 +14757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:25" ht="21" customHeight="1">
+    <row r="29" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>646</v>
       </c>
@@ -14727,7 +14773,7 @@
       <c r="X29" s="14"/>
       <c r="Y29" s="14"/>
     </row>
-    <row r="30" spans="1:25" ht="21" customHeight="1">
+    <row r="30" spans="1:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>431</v>
       </c>
@@ -14735,12 +14781,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="63" spans="22:25" ht="21" customHeight="1">
+    <row r="63" spans="22:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="V63" s="6"/>
       <c r="X63" s="6"/>
       <c r="Y63" s="6"/>
     </row>
-    <row r="66" spans="25:25" ht="21" customHeight="1">
+    <row r="66" spans="25:25" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Y66" s="6"/>
     </row>
   </sheetData>
@@ -14770,15 +14816,15 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.6640625" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" customWidth="1"/>
     <col min="5" max="5" width="89" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1">
+    <row r="1" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>23</v>
       </c>
@@ -14795,7 +14841,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="135.75" thickBot="1">
+    <row r="2" spans="1:5" ht="129" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="12" t="s">
         <v>355</v>
       </c>
@@ -14812,7 +14858,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="60">
+    <row r="3" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>429</v>
       </c>
@@ -14829,7 +14875,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="E4" s="1"/>
     </row>
   </sheetData>
@@ -14848,29 +14894,29 @@
       <selection pane="bottomRight" activeCell="R7" sqref="R7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.83203125" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="5" max="6" width="29.140625" customWidth="1"/>
-    <col min="7" max="7" width="68.7109375" customWidth="1"/>
-    <col min="8" max="8" width="58.28515625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="28.140625" customWidth="1"/>
-    <col min="15" max="15" width="17.28515625" customWidth="1"/>
-    <col min="16" max="17" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="31.28515625" customWidth="1"/>
-    <col min="23" max="23" width="22.7109375" customWidth="1"/>
-    <col min="24" max="24" width="38.28515625" customWidth="1"/>
+    <col min="5" max="6" width="29.1640625" customWidth="1"/>
+    <col min="7" max="7" width="68.6640625" customWidth="1"/>
+    <col min="8" max="8" width="58.33203125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="28.1640625" customWidth="1"/>
+    <col min="15" max="15" width="17.33203125" customWidth="1"/>
+    <col min="16" max="17" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="31.33203125" customWidth="1"/>
+    <col min="23" max="23" width="22.6640625" customWidth="1"/>
+    <col min="24" max="24" width="38.33203125" customWidth="1"/>
     <col min="25" max="25" width="23" customWidth="1"/>
-    <col min="26" max="28" width="36.42578125" customWidth="1"/>
-    <col min="29" max="29" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="17.28515625" customWidth="1"/>
+    <col min="26" max="28" width="36.5" customWidth="1"/>
+    <col min="29" max="29" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33">
+    <row r="1" spans="1:33" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -14971,7 +15017,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="2" spans="1:33" ht="75">
+    <row r="2" spans="1:33" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -15066,7 +15112,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:33">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>28</v>
       </c>
@@ -15159,7 +15205,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:33">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>29</v>
       </c>
@@ -15251,7 +15297,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:33">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>31</v>
       </c>
@@ -15343,7 +15389,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:33">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>32</v>
       </c>
@@ -15435,7 +15481,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:33">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -15527,7 +15573,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:33">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -15619,7 +15665,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:33">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>35</v>
       </c>
@@ -15711,7 +15757,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="10" spans="1:33">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>36</v>
       </c>
@@ -15816,12 +15862,12 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="51.140625" customWidth="1"/>
+    <col min="3" max="3" width="51.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -15832,7 +15878,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="59.25" customHeight="1">
+    <row r="2" spans="1:3" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>416</v>
       </c>
@@ -15841,7 +15887,7 @@
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>417</v>
       </c>
@@ -15850,7 +15896,7 @@
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>418</v>
       </c>
@@ -15859,7 +15905,7 @@
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>419</v>
       </c>

</xml_diff>

<commit_message>
Address all qa issues prior to applying 7.0.0 - ballot reconciliation changes
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B292564-8862-EB4A-8892-F4B5255E9E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EAAB5D0-40D2-144C-B991-C38CCC4A9D40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7180" yWindow="500" windowWidth="38500" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2427,9 +2427,36 @@
     Certifying Servers and Clients **SHALL** support options 1 and 2 as Additional USCDI Requirements.</t>
   </si>
   <si>
+    <t>* Due to implementer feedback, some US Core Profiles reference the PractitionerRole resource instead of the US Core PractitionerRole Profile. However the US Core PractitionerRole Profile **SHOULD** be used as the default profile if referenced by another US Core profile.</t>
+  </si>
+  <si>
+    <t>In order to access care team member's names, identifiers, locations, and contact information, the CareTeam profile supports several types of care team participants. They are represented as references to other profiles and include the following four profiles which are marked as must support:
+  1. US Core Practitioner Profile
+  1. US Core PractitionerRole Profile
+  1. US Core Patient Profile
+  1. US Core RelatedPerson Profile
+  * Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references, but **SHALL** support *at least* one of them.
+  * The client application **SHALL** support all four profile references.
+  * Bacause the *US Core PractitionerRole Profile* supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the *US Core Practitioner Profile*.
+  * Servers that supports only *US Core Practitioner Profile* **SHALL** provide implementation specific guidance how to access a provider's location and contact information using only the Practitioner resource.</t>
+  </si>
+  <si>
+    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
+* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
+    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
+    *  The client application **SHALL** support both elements.
+    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
+        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
+   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL** not contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
+* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
+  </si>
+  <si>
+    <t>7.0.0-ballot</t>
+  </si>
+  <si>
     <t xml:space="preserve">The US Core Server **SHALL**:
 1. Support the US Core Patient resource profile AND at least one additional resource profile from the list of US Core Profiles AND and all Must Support US Core Profiles and resources it references.
-     - The [Table below](#summary-of-must-support-references) summarizes the Must Support references to other US Core Profiles and FHIR resources for each US Core Profile:
+     - The [Table below](#ms-ref-table) summarizes the Must Support references to other US Core Profiles and FHIR resources for each US Core Profile:
 1. Implement the RESTful behavior according to the FHIR specification.
 1. Follow the requirements documented in the [General Requirements](general-requirements.html) and [Must Support](must-support.html) pages
 1. Return the following response classes:
@@ -2443,33 +2470,6 @@
 1. Support XML source formats for all US Core interactions.
 1. Identify the US Core profiles supported as part of the FHIR `meta.profile` attribute for each instance.
 </t>
-  </si>
-  <si>
-    <t>* Due to implementer feedback, some US Core Profiles reference the PractitionerRole resource instead of the US Core PractitionerRole Profile. However the US Core PractitionerRole Profile **SHOULD** be used as the default profile if referenced by another US Core profile.</t>
-  </si>
-  <si>
-    <t>In order to access care team member's names, identifiers, locations, and contact information, the CareTeam profile supports several types of care team participants. They are represented as references to other profiles and include the following four profiles which are marked as must support:
-  1. US Core Practitioner Profile
-  1. US Core PractitionerRole Profile
-  1. US Core Patient Profile
-  1. US Core RelatedPerson Profile
-  * Although *both* US Core Practitioner Profile and US Core PractitionerRole are must support, the server system is not required to support both types of references, but **SHALL** support *at least* one of them.
-  * The client application **SHALL** support all four profile references.
-  * Bacause the *US Core PractitionerRole Profile* supplies the provider's location and contact information and a reference to the Practitioner, server systems **SHOULD** reference it instead of the *US Core Practitioner Profile*.
-  * Servers that supports only *US Core Practitioner Profile* **SHALL** provide implementation specific guidance how to access a provider's location and contact information using only the Practitioner resource.</t>
-  </si>
-  <si>
-    <t>* The `DocumentReference.type` binding **SHALL** support at a minimum the [5 Common Clinical Notes](ValueSet-us-core-clinical-note-type.html) and may extend to the full US Core DocumentReference Type Value Set
-* The DocumentReference resources can represent the referenced content using either an address where the document can be retrieved using `DocumentReference.attachment.url` or the content as inline base64 encoded data using `DocumentReference.attachment.data`.
-    *  Although both are marked as must support, the server system is not required to support an address, and inline base64 encoded data, but **SHALL** support at least one of these elements.
-    *  The client application **SHALL** support both elements.
-    *  The `content.url` may refer to a FHIR Binary Resource (i.e. [base]/Binary/[id]), FHIR Document Bundle (i.e [base]/Bundle/[id] or another endpoint.
-        * If the endpoint is outside the FHIR base URL, it **SHOULD NOT** require additional authorization to access.
-   * If there are multiple `DocumentReference.content` element repetitions, these **SHALL** all represent the same document in different format or attachment metadata. The content element **SHALL** not contain different versions of the same content. For version handling use multiple DocumentReferences with `DocumentReference.relatesTo`
-* Every DocumentReference must have a responsible Organization. The organization responsible for the DocumentReference **SHALL** be present either in `DocumentReference.custodian` or accessible in the Provenance resource targeting the DocumentReference using `Provenance.agent.who` or `Provenance.agent.onBehalfOf`.</t>
-  </si>
-  <si>
-    <t>7.0.0-ballot</t>
   </si>
 </sst>
 </file>
@@ -2753,9 +2753,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2793,7 +2793,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2899,7 +2899,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3041,7 +3041,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -13036,8 +13036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13067,7 +13067,7 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13099,7 +13099,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>727</v>
+        <v>731</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -14329,7 +14329,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="T4" t="s">
         <v>19</v>
@@ -14445,7 +14445,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14800,7 +14800,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="T25" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Change "may" to "can" to avoid conformance verbs [FHIR-44060] Clarify Medication Adherence Extension definitions [FHIR-44076] Remove redundant sentence from Server CapabilityStatement description [FHIR-44112] Clarify the use of UCUM for Quantity datatypes in Lab Observations [FHIR-44117]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D651E09D-E38A-094F-AC56-7A268BBE3BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4507BAA2-1AC9-0141-AE16-118E1C48D3AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45260" yWindow="500" windowWidth="38500" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21520" yWindow="500" windowWidth="38500" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2375,9 +2375,6 @@
     * The client application **SHALL** support all three elements.</t>
   </si>
   <si>
-    <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ONC 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and the ONC [U.S. Core Data for Interoperability (USCDI) Version 4 July 2023](https://www.healthit.gov/sites/isa/files/2023-07/Final-USCDI-Version-4-July-2023-Final.pdf).  US Core Clients have the option of choosing from this list to access necessary data based on their local use cases and other contextual requirements.</t>
-  </si>
-  <si>
     <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-average-blood-pressure</t>
   </si>
   <si>
@@ -2470,6 +2467,9 @@
   </si>
   <si>
     <t>7.0.0</t>
+  </si>
+  <si>
+    <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ONC 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and the ONC [U.S. Core Data for Interoperability (USCDI) Version 4 July 2023](https://www.healthit.gov/sites/isa/files/2023-07/Final-USCDI-Version-4-July-2023-Final.pdf).</t>
   </si>
 </sst>
 </file>
@@ -13036,8 +13036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13067,7 +13067,7 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13083,7 +13083,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>717</v>
+        <v>731</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -13099,7 +13099,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13216,7 +13216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84EBB963-62EF-8346-A79F-04E3300CC06A}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -13725,10 +13725,10 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
+        <v>720</v>
+      </c>
+      <c r="B32" t="s">
         <v>721</v>
-      </c>
-      <c r="B32" t="s">
-        <v>722</v>
       </c>
       <c r="D32" t="s">
         <v>12</v>
@@ -13739,10 +13739,10 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
+        <v>722</v>
+      </c>
+      <c r="B33" t="s">
         <v>723</v>
-      </c>
-      <c r="B33" t="s">
-        <v>724</v>
       </c>
       <c r="D33" t="s">
         <v>12</v>
@@ -13893,10 +13893,10 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
+        <v>717</v>
+      </c>
+      <c r="B44" t="s">
         <v>718</v>
-      </c>
-      <c r="B44" t="s">
-        <v>719</v>
       </c>
       <c r="D44" t="s">
         <v>12</v>
@@ -14327,7 +14327,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="T4" t="s">
         <v>19</v>
@@ -14443,7 +14443,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14714,7 +14714,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="T21" t="s">
         <v>19</v>
@@ -14798,7 +14798,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="T25" t="s">
         <v>19</v>
@@ -14823,7 +14823,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="T26" t="s">
         <v>19</v>
@@ -14913,7 +14913,7 @@
         <v>12</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="T31" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Add reference in the profile description to the base resource for scope and usage definitions. [FHIR-43543]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C46A83-A4ED-FB44-BD1C-EF4A16CEDFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F42818E-83EF-5549-8276-107F35063250}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31540" yWindow="500" windowWidth="34140" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="660" windowWidth="34140" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -3226,8 +3226,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9F73F9-34B4-C04F-A2E4-99114F8B7BF7}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="Z28" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="Z48" sqref="Z48"/>
@@ -13398,7 +13398,7 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K128">
     <sortCondition ref="A1"/>
   </sortState>
-  <conditionalFormatting sqref="B102:B1048576 B1:B100">
+  <conditionalFormatting sqref="B1:B100 B102:B1048576">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
@@ -14556,8 +14556,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A20" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -15293,7 +15293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="225" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>541</v>
       </c>

</xml_diff>

<commit_message>
FMG QA Suggestions for US Core IG including: Update DocumentReference.content.format binding [FHIR-45302] Update code systmm URL in US Core Discharge Disposition [FHIR-45303]
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3633C36-D2A7-1144-9261-02697951A463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354E736D-0A82-CC4E-A54D-35F6E3F6D31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34100" yWindow="500" windowWidth="34140" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34100" yWindow="500" windowWidth="34140" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -23,8 +23,10 @@
     <sheet name="interactions" sheetId="6" r:id="rId8"/>
     <sheet name="rest_interactions" sheetId="11" r:id="rId9"/>
     <sheet name="sps" sheetId="14" r:id="rId10"/>
+    <sheet name="sp_combos" sheetId="15" r:id="rId11"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">sp_combos!$A$1:$K$101</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">sps!$A$1:$AB$132</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -80,8 +82,46 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={3D6593B2-8A1E-A24A-80BE-57CB27553CF1}</author>
+    <author>tc={D8B0DCD9-3CF9-B14D-BBD2-ED0D75EDCEE7}</author>
+    <author>tc={28AD8D2E-6B3A-D044-9128-B122FA094994}</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{3D6593B2-8A1E-A24A-80BE-57CB27553CF1}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    add column for include file
+Reply:
+    make this a comma separate list of profiles</t>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="1" shapeId="0" xr:uid="{D8B0DCD9-3CF9-B14D-BBD2-ED0D75EDCEE7}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    does this do anything if not delete row</t>
+      </text>
+    </comment>
+    <comment ref="I42" authorId="2" shapeId="0" xr:uid="{28AD8D2E-6B3A-D044-9128-B122FA094994}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    is column being used???</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2190" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2813" uniqueCount="740">
   <si>
     <t>Element</t>
   </si>
@@ -1668,12 +1708,833 @@
 A client **SHALL** provide a value precise to the *second + time offset*.
 A server **SHALL** support a value precise to the *second + time offset*.</t>
   </si>
+  <si>
+    <t>index</t>
+  </si>
+  <si>
+    <t>combo</t>
+  </si>
+  <si>
+    <t>combo_conf</t>
+  </si>
+  <si>
+    <t>types</t>
+  </si>
+  <si>
+    <t>fixed_kv</t>
+  </si>
+  <si>
+    <t>!Encounter</t>
+  </si>
+  <si>
+    <t>class,date</t>
+  </si>
+  <si>
+    <t>date,token</t>
+  </si>
+  <si>
+    <t>class,date,patient</t>
+  </si>
+  <si>
+    <t>date,reference,token</t>
+  </si>
+  <si>
+    <t>class,date,patient,type</t>
+  </si>
+  <si>
+    <t>class,date,type</t>
+  </si>
+  <si>
+    <t>class,patient</t>
+  </si>
+  <si>
+    <t>reference,token</t>
+  </si>
+  <si>
+    <t>support searching for all encounter for a patient by encounter class</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?patient=example1&amp;class= http://terminology.hl7.org/CodeSystem/v3-ActCode code\|AMB</t>
+  </si>
+  <si>
+    <t>class,patient,status</t>
+  </si>
+  <si>
+    <t>class,patient,status,type</t>
+  </si>
+  <si>
+    <t>class,patient,type</t>
+  </si>
+  <si>
+    <t>class,status</t>
+  </si>
+  <si>
+    <t>class,status,type</t>
+  </si>
+  <si>
+    <t>class,type</t>
+  </si>
+  <si>
+    <t>date,patient</t>
+  </si>
+  <si>
+    <t>date,reference</t>
+  </si>
+  <si>
+    <t>support searching for all encounters for a patient by date</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?patient=example1&amp;date=ge2019-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>date,patient,type</t>
+  </si>
+  <si>
+    <t>date,type</t>
+  </si>
+  <si>
+    <t>patient,type</t>
+  </si>
+  <si>
+    <t>support searching for all encounter for a patient by encounter type</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?patient=1137192&amp;type=http://www.ama-assn.org/go/cpt code\|99201</t>
+  </si>
+  <si>
+    <t>patient,location</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?patient=1137192&amp;location=Location/hospital</t>
+  </si>
+  <si>
+    <t>patient,_lastUpdated</t>
+  </si>
+  <si>
+    <t>reference,date</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?patient=1137192&amp;_lastUpdated=ge2024-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>patient,status,type</t>
+  </si>
+  <si>
+    <t>patient,status</t>
+  </si>
+  <si>
+    <t>support searching for all encounter for a patient by status (for example, all finished encounters)</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?patient=example1&amp;status=finished</t>
+  </si>
+  <si>
+    <t>patient,discharge-disposition</t>
+  </si>
+  <si>
+    <t>GET [base]/Encounter?patient=example1&amp;discharge-disposition=01</t>
+  </si>
+  <si>
+    <t>status,type</t>
+  </si>
+  <si>
+    <t>!Questionnaire</t>
+  </si>
+  <si>
+    <t>context-type-value,publisher</t>
+  </si>
+  <si>
+    <t>composite,string</t>
+  </si>
+  <si>
+    <t>context-type-value,publisher,status</t>
+  </si>
+  <si>
+    <t>composite,string,token</t>
+  </si>
+  <si>
+    <t>context-type-value,status</t>
+  </si>
+  <si>
+    <t>composite,token</t>
+  </si>
+  <si>
+    <t>publisher,status</t>
+  </si>
+  <si>
+    <t>string,token</t>
+  </si>
+  <si>
+    <t>publisher,status,version</t>
+  </si>
+  <si>
+    <t>publisher,version</t>
+  </si>
+  <si>
+    <t>status,title,version</t>
+  </si>
+  <si>
+    <t>status,version</t>
+  </si>
+  <si>
+    <t>title,version</t>
+  </si>
+  <si>
+    <t>birthdate,family</t>
+  </si>
+  <si>
+    <t>date,string</t>
+  </si>
+  <si>
+    <t>support searching for a patient by birthdate and family name</t>
+  </si>
+  <si>
+    <t>GET [base]/Patient?family=Shaw&amp;birthdate=2007-03-20</t>
+  </si>
+  <si>
+    <t>death-date,family</t>
+  </si>
+  <si>
+    <t>support searching for a patient by date of death and family name</t>
+  </si>
+  <si>
+    <t>GET [base]/Patient?family=Shaw&amp;death-date=2022-07-22</t>
+  </si>
+  <si>
+    <t>birthdate,name</t>
+  </si>
+  <si>
+    <t>support searching for a patient by birthdate and a string match of any part of name</t>
+  </si>
+  <si>
+    <t>GET [base]/Patient?name=Shaw&amp;birthdate=2007-03-20</t>
+  </si>
+  <si>
+    <t>family,gender</t>
+  </si>
+  <si>
+    <t>support searching for a patient by family name and gender</t>
+  </si>
+  <si>
+    <t>GET [base]/Patient?family=Shaw&amp;gender=female</t>
+  </si>
+  <si>
+    <t>gender,name</t>
+  </si>
+  <si>
+    <t>support searching for a patient by a string match of any part of name and gender</t>
+  </si>
+  <si>
+    <t>GET [base]/Patient?name=Shaw&amp;gender=female</t>
+  </si>
+  <si>
+    <t>patient,clinical-status</t>
+  </si>
+  <si>
+    <t>clinical-status=http://terminology.hl7.org/CodeSystem/condition-clinical|active,http://terminology.hl7.org/CodeSystem/condition-clinical|recurrance,http://terminology.hl7.org/CodeSystem/condition-clinical|remission</t>
+  </si>
+  <si>
+    <t>support searching for all *active* conditions for a patient</t>
+  </si>
+  <si>
+    <t>GET [base/Condition?patient=1032702&amp;clinical-status=http://terminology.hl7.org/CodeSystem/condition-clinical\|active,http://terminology.hl7.org/CodeSystem/condition-clinical\|recurrance,http://terminology.hl7.org/CodeSystem/condition-clinical\|remission</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Condition resources for the specified patient and all "active" statuses (active,relapse,remission). This will *exclude* diagnoses and health concerns without a clinicalStatus specified.</t>
+  </si>
+  <si>
+    <t>patient,category</t>
+  </si>
+  <si>
+    <t>support searching for all problems or health concerns or encounter diagnosis for a patient</t>
+  </si>
+  <si>
+    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|problem-list-item~GET [base]/Condition?patient=1032702&amp;category=http://hl7.org/fhir/us/core/CodeSystem/condition-category\|health-concern~GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Condition resources for the specified patient and category.</t>
+  </si>
+  <si>
+    <t>patient,category,clinical-status</t>
+  </si>
+  <si>
+    <t>support searching for all *active* problems or health concerns or  *active* encounter diagnosis for a patient</t>
+  </si>
+  <si>
+    <r>
+      <t>GET [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>base</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|problem-list-item&amp;clinical-status=http://terminology.hl7.org/CodeSystem/condition-clinical\|active,http://terminology.hl7.org/CodeSystem/condition-clinical\|recurrance,http://terminology.hl7.org/CodeSystem/condition-clinical\|remission</t>
+    </r>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Condition resources for the specified patient and category for all "active" statuses (active,relapse,remission). This will *exclude* diagnoses and health concerns without a clinicalStatus specified.</t>
+  </si>
+  <si>
+    <t>patient,category,encounter</t>
+  </si>
+  <si>
+    <t>GET [base]/Condition?patient=1032702&amp;category=http://terminology.hl7.org/CodeSystem/condition-category\|encounter-diagnosis&amp;encounter=1036</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Condition resources for the specified patient and category and encounter. When category = "encounter-diagnosis" will return the encounter diagnosis for the encounter.</t>
+  </si>
+  <si>
+    <t>patient,code</t>
+  </si>
+  <si>
+    <t>support searching for a particular condition for a patient</t>
+  </si>
+  <si>
+    <t>GET [base]/Condition?patient=1032702&amp;code=[http://snomed.info/sct\|442311008]</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Condition resources for the specified patient and code.</t>
+  </si>
+  <si>
+    <t>patient,onset-date</t>
+  </si>
+  <si>
+    <t>support searching for all conditions for a patient for a specified time period</t>
+  </si>
+  <si>
+    <t>GET [base]Condition?patient=555580&amp;onset-date=ge2018-01-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fetches a bundle of all Condition resources for the specified patient and date. </t>
+  </si>
+  <si>
+    <t>patient,asserted-date</t>
+  </si>
+  <si>
+    <t>GET [base]Condition?patient=555580&amp;asserted-date=ge2018-01-14</t>
+  </si>
+  <si>
+    <t>patient,recorded-date</t>
+  </si>
+  <si>
+    <t>GET [base]Condition?patient=555580&amp;recorded-date=ge2018-01-14</t>
+  </si>
+  <si>
+    <t>patient,abatement-date</t>
+  </si>
+  <si>
+    <t>GET [base]Condition?patient=555580&amp;abatement-date=ge2018-01-14</t>
+  </si>
+  <si>
+    <r>
+      <t>GET [</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>base</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <rFont val="Menlo"/>
+        <family val="2"/>
+      </rPr>
+      <t>]/Condition?patient=1032702&amp;_lastUpdated=ge2024-01-01T00:00:00Z</t>
+    </r>
+  </si>
+  <si>
+    <t>support searching for all *active*  or *inactive* allergies for a patient</t>
+  </si>
+  <si>
+    <t>GET [base]/AllergyIntolerance?patient=[id]&amp;clinical-status=http://terminology.hl7.org/CodeSystem/allergyintolerance-clinical\|active</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all AllergyIntolerance resources for the specified patient and status code.  This will not return any "entered in error" resources because of the conditional presence of the clinicalStatus element.</t>
+  </si>
+  <si>
+    <t>patient,date</t>
+  </si>
+  <si>
+    <t>support searching for all immunizations for a patient for a specified time period</t>
+  </si>
+  <si>
+    <t>GET [base]/Immunization?patient=1137192&amp;date=ge2019-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>support searching for all administered immunizations for a patient</t>
+  </si>
+  <si>
+    <t>GET [base]/Immunization?patient=1137192&amp;status=completed</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</t>
+  </si>
+  <si>
+    <t>support searching for all laboratory reports for a patient for a given status (for example completed reports )</t>
+  </si>
+  <si>
+    <t>GET [base]/DiagnosticReport?patient=1137192&amp;status=completed</t>
+  </si>
+  <si>
+    <t>category=http://terminology.hl7.org/CodeSystem/v2-0074|LAB</t>
+  </si>
+  <si>
+    <t>support searching for all laboratory reports</t>
+  </si>
+  <si>
+    <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://terminology.hl7.org/CodeSystem/v2-0074\|LAB</t>
+  </si>
+  <si>
+    <t>support searching for all laboratory reports by code  (for example, search for all metabolic panel reports for a patient, or search for all cbcs, metabolic panels, and urinalysis panels for a patient)</t>
+  </si>
+  <si>
+    <t>GET [base]/DiagnosticReport?patient=1032702&amp;code=http://loinc.org\|24323-8</t>
+  </si>
+  <si>
+    <t>patient,category,date</t>
+  </si>
+  <si>
+    <t>reference,token,date</t>
+  </si>
+  <si>
+    <t>support searching for all laboratory reports by date</t>
+  </si>
+  <si>
+    <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://terminology.hl7.org/CodeSystem/v2-0074\|LAB&amp;date=ge2010-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>patient,category,_lastUpdated</t>
+  </si>
+  <si>
+    <t>GET [base]/DiagnosticReport?patient=f201&amp;category=http://terminology.hl7.org/CodeSystem/v2-0074\|LAB&amp;_lastUpdated=ge2010-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>patient,code,date</t>
+  </si>
+  <si>
+    <t>support searching for laboratory reports by code and date (for example, search for all metabolic panel reports since 2019 for a patient)</t>
+  </si>
+  <si>
+    <t>GET [base]/DiagnosticReport?patient=f201&amp;code=http://loinc.org\|24323-8&amp;date=ge2019-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>patient,lifecycle-status</t>
+  </si>
+  <si>
+    <t>support searching for all goals for a patient for a given status (for example active goals)</t>
+  </si>
+  <si>
+    <t>GET [base]/Goal?patient=1137192&amp;lifecycle-status=active</t>
+  </si>
+  <si>
+    <t>patient,target-date</t>
+  </si>
+  <si>
+    <t>support searching for all goals for a patient by date</t>
+  </si>
+  <si>
+    <t>GET [base]/Goal?patient=1137192&amp;target-date=ge2015-01-14&amp;target-date=le2019-01-14</t>
+  </si>
+  <si>
+    <t>patient,intent</t>
+  </si>
+  <si>
+    <t>intent=order,plan</t>
+  </si>
+  <si>
+    <t>support searching for all medications that have been prescribed to a patient. See the [Medication List Guidance] section for guidance on accessing a patient medications. The server application represents the medication using either an inline code or a contained or external reference to the Medication resource.</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=14676&amp;intent=order,plan~GET [base]/MedicationRequest?patient=14676&amp;intent=order,plan&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent code = `order,plan`</t>
+  </si>
+  <si>
+    <t>patient,intent,status</t>
+  </si>
+  <si>
+    <t>support searching for all prescriptions for a patient for a given status (for example all active prescriptions)</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;status=active~GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;status=active&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order,plan` and status</t>
+  </si>
+  <si>
+    <t>patient,intent,encounter</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;status=active&amp;encounter=Encounter/123~GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;status=active&amp;&amp;encounter=Encounter/123&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order,plan` and encounter</t>
+  </si>
+  <si>
+    <t>patient,intent,authoredon</t>
+  </si>
+  <si>
+    <t>support searching for all prescriptions for a patient by date</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;authoredon=ge2019-01-01T00:00:00Z~GET [base]/MedicationRequest?patient=1137192&amp;intent=order,plan&amp;authoredon=ge2019-01-01T00:00:00Z&amp;_include=MedicationRequest:medication</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all MedicationRequest resources for the specified patient and intent  code = `order,plan` and authoredon date</t>
+  </si>
+  <si>
+    <t>support searching for all medications for a patient for a given status (for example all active medications)</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationStatement?patient=1137192&amp;status=active~GET [base]/MedicationStatement?patient=1137192&amp;status=active&amp;_include=MedicationStatement:medication</t>
+  </si>
+  <si>
+    <t>patient,effective</t>
+  </si>
+  <si>
+    <t>support searching for all medications for a patient by date</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationStatement?patient=1137192&amp;date=ge2019~GET [base]/MedicationRequest?patient=1137192&amp;date=ge2019&amp;_include=MedicationStatement:medication</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all MedicationStatement resources for the specified patient and date</t>
+  </si>
+  <si>
+    <t>support searching for all procedures for a patient for a given status (for example all completed procedures)</t>
+  </si>
+  <si>
+    <t>GET [base]/Procedure?patient=1137192&amp;status=completed</t>
+  </si>
+  <si>
+    <t>support searching for all procedures for a patient by date</t>
+  </si>
+  <si>
+    <t>GET [base]/Procedure?patient=1137192&amp;date=ge2019-01-14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">support searching for procedures for a patient by code and date </t>
+  </si>
+  <si>
+    <t>GET [base]/Procedure?patient=1137192&amp;date=ge2019-01-14T00:00:00Z&amp;code=http://snomed.info/sct\|35637008</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-observation</t>
+  </si>
+  <si>
+    <t>patient,category,status</t>
+  </si>
+  <si>
+    <t>category=http://terminology.hl7.org/CodeSystem/observation-category|laboratory</t>
+  </si>
+  <si>
+    <t>support searching for all laboratory results for a patient for a given status (for example all observations marked as final)</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;category={% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: '[category]'}}&amp;status=final</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Observation resources for the specified patient and category = `laboratory` and status</t>
+  </si>
+  <si>
+    <t>support searching for all laboratory results</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;amp;category={% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: &amp;#39;[category]&amp;#39;}}</t>
+  </si>
+  <si>
+    <t>support searching for all laboratory results by code (for example, search for all blood glucose lab results for a patient,  or search for all  blood glucose, urine glucose and urine ketones for a patient)</t>
+  </si>
+  <si>
+    <t>GET [base]/Observation?patient=1134281&amp;amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}}
+      {% if include.code2 %}2. GET [base]/Observation?patient=1134281&amp;amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}},http://loinc.org\|{{include.code2 | default: '[code]'}},http://loinc.org\|{{include.code3 | default: '[code]'}}{% endif %}</t>
+  </si>
+  <si>
+    <t>support searching for all laboratory results by date (for example, find all the laboratory results after 2018-03-14.)</t>
+  </si>
+  <si>
+    <t>GET [base]Observation?patient=555580&amp;category={% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: '[category]'}}&amp;date=ge2018-03-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>GET [base]Observation?patient=555580&amp;{% if include.system %}{{include.system }}\|{% endif %}{{include.category | default: '[category]'}}&amp;_lastUpdated=ge2024-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>support searching laboratory results by code and date (for example, search for all blood glucose lab results since 2019 for a patient)</t>
+  </si>
+  <si>
+    <t>GET [base]Observation?patient=555580&amp;code=http://loinc.org\|{{include.code1 | default: '[code]'}}&amp;date=ge2019-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category|assess-plan</t>
+  </si>
+  <si>
+    <t>support searching for all patient assessments and plans of treatment for a patient</t>
+  </si>
+  <si>
+    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan</t>
+  </si>
+  <si>
+    <t>support searching for all assessment and plan of treatment for a patient within a time period</t>
+  </si>
+  <si>
+    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2019-01-01T00:00:00Z~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;date=ge2018-01-01T00:00:00Z&amp;date=le2019-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan` and date</t>
+  </si>
+  <si>
+    <t>support searching for all *active* assessment and plan of treatment for a patient</t>
+  </si>
+  <si>
+    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan` and status=`active`</t>
+  </si>
+  <si>
+    <t>patient,category,status,date</t>
+  </si>
+  <si>
+    <t>support searching for all *active* assessment and plan of treatment for a patient within a time period</t>
+  </si>
+  <si>
+    <t>GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2019-01-01T00:00:00Z~GET [base]/CarePlan?patient=1137192&amp;category=http://hl7.org/fhir/us/core/CodeSystem/careplan-category\|assess-plan&amp;status=active&amp;date=ge2018-01-01T00:00:00Z&amp;date=le2019-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan` and status=`active` and date</t>
+  </si>
+  <si>
+    <t>status=active</t>
+  </si>
+  <si>
+    <t>support searching for all current care team members for a patient. DOES THIS DO ANYTHING?</t>
+  </si>
+  <si>
+    <t>GET [base]/CareTeam?patient=1137192&amp;status=active~GET [base]/CareTeam?patient=1137192&amp;status=active&amp;_include=CareTeam:participant:RelatedPerson&amp;_include=CareTeam:participant:Patient&amp;_include=CareTeam:participant:Practitioner&amp;_include=CareTeam:participant:PractitionerRole</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all CareTeam resources for the specified patient and status =`active` and may include CareTeam Patient, RelatedPerson and Practitioner and PractitionerRole participants.  
+To get Practitioner name and identifier using PractitionerRole:  
+1) Search for the careteam PractitionerRole: GET [base]/CareTeam?patient=[id]&amp;status=active&amp;_include=CareTeam:participant:PractitionerRole  
+2) using the FHIR _id from the PractitionerRole.practitioner element resource,  fetch the Practitioner resources using  GET [base]/Practitioner?_id=[id]</t>
+  </si>
+  <si>
+    <t>support searching for all documents for a patient for a given status (for example completed reports )</t>
+  </si>
+  <si>
+    <t>GET [base]/DocumentReference?patient=1235541</t>
+  </si>
+  <si>
+    <t>!DocumentReference</t>
+  </si>
+  <si>
+    <t>patient,period</t>
+  </si>
+  <si>
+    <t>category=http://hl7.org/fhir/us/core/CodeSystem/us-core-documentreference-category|clinical-note</t>
+  </si>
+  <si>
+    <t>support searching for all clinical notes for a given patient</t>
+  </si>
+  <si>
+    <t>GET [base]/DocumentReference?patient=1235541&amp;category=http://hl7.org/fhir/us/core/CodeSystem/us-core-documentreference-category\|clinical-note</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all DocumentReference resources for the specified patient and category = `clinical-note`.  See the implementation notes above for how to access the actual document.</t>
+  </si>
+  <si>
+    <t>support searching for all clinical notes for a given patient by date (for example, since 2019)</t>
+  </si>
+  <si>
+    <t>GET [base]/DocumentReference?patient=1235541&amp;category=http://hl7.org/fhir/us/core/CodeSystem/us-core-documentreference-category\|clinical-note&amp;date=ge2020-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all DocumentReference resources for the specified patient and category = `clinical=note` and date. See the implementation notes above for how to access the actual document.</t>
+  </si>
+  <si>
+    <t>support searching for a specific note type for a patient</t>
+  </si>
+  <si>
+    <t>GET [base]/DocumentReference?patient=1316024&amp;type=http://loinc.org\|18842-5</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all DocumentReference resources for the specified patient and type. See the implementation notes above for how to access the actual document.</t>
+  </si>
+  <si>
+    <t>patient,type,period</t>
+  </si>
+  <si>
+    <t>support searching for a document for a patient by type and a clinically relevent date</t>
+  </si>
+  <si>
+    <t>GET [base]/DocumentReference?patient=2169591&amp;type=http://loinc.org \|34133-9&amp;period=ge2020-01-01T00:00:00Z</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/us/core/StructureDefinition/us-core-device</t>
+  </si>
+  <si>
+    <t>support searching for a specific device type for a patient (for example, implantable devices)</t>
+  </si>
+  <si>
+    <t>GET [base]/Device?patient=1316024&amp;type=http://snomed.info/sct\|468063009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fetches a bundle of all Device resources for the specified patient and type. </t>
+  </si>
+  <si>
+    <t>support searching for all devices with a given status for a patient (for example all active devices)</t>
+  </si>
+  <si>
+    <t>GET [base]/Device?patient=1316024&amp;status=active</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all Device resources for the specified patient and status</t>
+  </si>
+  <si>
+    <t>patient,role</t>
+  </si>
+  <si>
+    <t>support searching for all current care team member roles for a patient. DOES THIS DO ANYTHING?</t>
+  </si>
+  <si>
+    <t>GET [base]/CareTeam?patient=1137192&amp;role=http://snomed.info/sct\|17561000</t>
+  </si>
+  <si>
+    <t>Fetches a bundle of all CareTeam resources for the specified patient and participant role</t>
+  </si>
+  <si>
+    <t>support searching for all reports for a patient for a given status (for example completed reports )</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=1137192&amp;status=completed</t>
+  </si>
+  <si>
+    <t>support searching for all reports by category codes specified in US Core DiagnosticReport Category Codes</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=f201&amp;category=http://loinc.org\|LG41762-2</t>
+  </si>
+  <si>
+    <t>support searching for all  reports by code</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=1032702&amp;code=http://snomed.info/sct\|35637008</t>
+  </si>
+  <si>
+    <t>patient,category,authored</t>
+  </si>
+  <si>
+    <t>support searching for all  reports by category codes specified in US Core DiagnosticReport Category Codes and date</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=f201&amp;category=http://loinc.org\|LG41762-2&amp;date=ge2010-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>patient,code,authored</t>
+  </si>
+  <si>
+    <t>support searching for reports by code and date DOES THIS DO ANYTHING!!!!</t>
+  </si>
+  <si>
+    <t>GET [base]/ServiceRequest?patient=f201&amp;code=http://snomed.info/sct\|35637008&amp;date=ge2019-01-14T00:00:00Z</t>
+  </si>
+  <si>
+    <t>patient,description</t>
+  </si>
+  <si>
+    <t>support searching for all goals for a patient by date DOES THIS DO ANYTHING!!!</t>
+  </si>
+  <si>
+    <t>GET [base]/Goal?patient=1137192&amp;description=http://snomed.info/sct\|1078229009</t>
+  </si>
+  <si>
+    <t>combo description field ...DOES THIS DO ANYTHING?</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse?patient=1137192&amp;status=completed</t>
+  </si>
+  <si>
+    <t>patient,_tag</t>
+  </si>
+  <si>
+    <t>_tag=sdoh</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse?patient=1137192&amp;_tag=sdoh</t>
+  </si>
+  <si>
+    <t>patient,authored</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse?patient=113192&amp;date=ge2021</t>
+  </si>
+  <si>
+    <t>patient,_tag,authored</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse?patient=113192&amp;date=ge2021&amp;_tag=sdoh</t>
+  </si>
+  <si>
+    <t>patient,questionnaire</t>
+  </si>
+  <si>
+    <t>GET [base]/QuestionnaireResponse?patient=113192&amp;questionnaire=http://hl7.org/fhir/us/sdoh-clinicalcare/Questionnaire/SDOHCC-QuestionnaireHungerVitalSign</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on their dispensed status</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationDispense?patient=1137192&amp;status=completed~GET [base]/MedicationDispense?patient=1137192&amp;status=completed&amp;_include=MedicationDispense:medication</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on their dispensed status and dispense type.</t>
+  </si>
+  <si>
+    <t>GET [base]/MedicationDispense?patient=1137192&amp;status=&amp;type=~GET [base]/MedicationDispense?patient=1137192&amp;status=&amp;type=FFP&amp;_include=MedicationDispense:medication</t>
+  </si>
+  <si>
+    <t>patient,whenhandedover</t>
+  </si>
+  <si>
+    <t>support searching for prescriptions for a patient based on when it was dispensed to the patient.</t>
+  </si>
+  <si>
+    <t>foo</t>
+  </si>
+  <si>
+    <t>patient,name</t>
+  </si>
+  <si>
+    <t>reference,string</t>
+  </si>
+  <si>
+    <t>GET [base]/RelatedPerson?patient=1137192&amp;name=van%20Putten</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1777,6 +2638,24 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFA31515"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF005C00"/>
+      <name val="Monaco"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1830,7 +2709,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1867,6 +2746,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -1874,7 +2757,17 @@
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2233,6 +3126,23 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C1" dT="2021-11-10T17:47:31.83" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{3D6593B2-8A1E-A24A-80BE-57CB27553CF1}">
+    <text>add column for include file</text>
+  </threadedComment>
+  <threadedComment ref="C1" dT="2021-11-10T17:48:52.85" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{207C0DF5-3227-F342-A86E-CEBD1F88C9BE}" parentId="{3D6593B2-8A1E-A24A-80BE-57CB27553CF1}">
+    <text>make this a comma separate list of profiles</text>
+  </threadedComment>
+  <threadedComment ref="I1" dT="2021-11-08T19:54:50.37" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{D8B0DCD9-3CF9-B14D-BBD2-ED0D75EDCEE7}">
+    <text>does this do anything if not delete row</text>
+  </threadedComment>
+  <threadedComment ref="I42" dT="2021-11-06T02:44:23.26" personId="{01DB13A2-9E02-7A4D-96F1-9E53507C2507}" id="{28AD8D2E-6B3A-D044-9128-B122FA094994}">
+    <text>is column being used???</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A508ECBD-F3E5-4662-8D7C-0F31D75EC9A2}">
   <dimension ref="A1:B9"/>
@@ -2327,7 +3237,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9F73F9-34B4-C04F-A2E4-99114F8B7BF7}">
   <dimension ref="A1:AB132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B44" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -9411,13 +10321,3078 @@
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1832F48A-473A-3546-820D-6A8E9142FE06}">
+  <dimension ref="A1:K101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.1640625" customWidth="1"/>
+    <col min="3" max="3" width="96.5" customWidth="1"/>
+    <col min="4" max="4" width="33" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5" customWidth="1"/>
+    <col min="8" max="8" width="121.6640625" customWidth="1"/>
+    <col min="9" max="9" width="88.83203125" customWidth="1"/>
+    <col min="10" max="10" width="255.83203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="83.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>481</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>484</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>485</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="16" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>486</v>
+      </c>
+      <c r="C2" t="str">
+        <f t="shared" ref="C2:C49" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D2" t="s">
+        <v>487</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>488</v>
+      </c>
+      <c r="K2" s="4" t="str">
+        <f t="shared" ref="K2:K17" si="1">"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
+        <v>Fetches a bundle of all !Encounter resources matching the specified class and date</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D3" t="s">
+        <v>489</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>490</v>
+      </c>
+      <c r="K3" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>486</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D4" t="s">
+        <v>491</v>
+      </c>
+      <c r="F4" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" t="s">
+        <v>490</v>
+      </c>
+      <c r="K4" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified class and date and patient and type</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>486</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D5" t="s">
+        <v>492</v>
+      </c>
+      <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" t="s">
+        <v>488</v>
+      </c>
+      <c r="K5" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified class and date and type</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
+      </c>
+      <c r="D6" t="s">
+        <v>493</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>494</v>
+      </c>
+      <c r="I6" t="s">
+        <v>495</v>
+      </c>
+      <c r="J6" t="s">
+        <v>496</v>
+      </c>
+      <c r="K6" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all Encounter resources matching the specified class and patient</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>486</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D7" t="s">
+        <v>497</v>
+      </c>
+      <c r="F7" t="s">
+        <v>69</v>
+      </c>
+      <c r="G7" t="s">
+        <v>494</v>
+      </c>
+      <c r="K7" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>486</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D8" t="s">
+        <v>498</v>
+      </c>
+      <c r="F8" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" t="s">
+        <v>494</v>
+      </c>
+      <c r="K8" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and status and type</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>486</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D9" t="s">
+        <v>499</v>
+      </c>
+      <c r="F9" t="s">
+        <v>69</v>
+      </c>
+      <c r="G9" t="s">
+        <v>494</v>
+      </c>
+      <c r="J9" s="4"/>
+      <c r="K9" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified class and patient and type</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>486</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D10" t="s">
+        <v>500</v>
+      </c>
+      <c r="F10" t="s">
+        <v>69</v>
+      </c>
+      <c r="G10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified class and status</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>486</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D11" t="s">
+        <v>501</v>
+      </c>
+      <c r="F11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="K11" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified class and status and type</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>486</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D12" t="s">
+        <v>502</v>
+      </c>
+      <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified class and type</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
+      </c>
+      <c r="D13" t="s">
+        <v>503</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>504</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>505</v>
+      </c>
+      <c r="J13" t="s">
+        <v>506</v>
+      </c>
+      <c r="K13" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all Encounter resources matching the specified date and patient</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>486</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D14" t="s">
+        <v>507</v>
+      </c>
+      <c r="F14" t="s">
+        <v>69</v>
+      </c>
+      <c r="G14" t="s">
+        <v>490</v>
+      </c>
+      <c r="K14" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified date and patient and type</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>486</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D15" t="s">
+        <v>508</v>
+      </c>
+      <c r="F15" t="s">
+        <v>69</v>
+      </c>
+      <c r="G15" t="s">
+        <v>488</v>
+      </c>
+      <c r="K15" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified date and type</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
+      </c>
+      <c r="D16" t="s">
+        <v>509</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>494</v>
+      </c>
+      <c r="I16" t="s">
+        <v>510</v>
+      </c>
+      <c r="J16" t="s">
+        <v>511</v>
+      </c>
+      <c r="K16" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all Encounter resources matching the specified patient and type</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
+      </c>
+      <c r="D17" t="s">
+        <v>512</v>
+      </c>
+      <c r="F17" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" t="s">
+        <v>89</v>
+      </c>
+      <c r="I17" t="s">
+        <v>510</v>
+      </c>
+      <c r="J17" t="s">
+        <v>513</v>
+      </c>
+      <c r="K17" s="4" t="str">
+        <f t="shared" si="1"/>
+        <v>Fetches a bundle of all Encounter resources matching the specified patient and location</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
+      </c>
+      <c r="D18" t="s">
+        <v>514</v>
+      </c>
+      <c r="F18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" t="s">
+        <v>515</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="24" t="s">
+        <v>516</v>
+      </c>
+      <c r="K18" s="25" t="str">
+        <f>"Fetches a bundle of all "&amp;B18&amp;" resources for the specified "&amp;SUBSTITUTE(D18,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
+        <v>Fetches a bundle of all Encounter resources for the specified patient and _lastUpdated. See the US Core General Guidance page for [Searching Using lastUpdated].</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>486</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D19" t="s">
+        <v>517</v>
+      </c>
+      <c r="F19" t="s">
+        <v>69</v>
+      </c>
+      <c r="G19" t="s">
+        <v>494</v>
+      </c>
+      <c r="J19" s="4"/>
+      <c r="K19" s="4" t="str">
+        <f t="shared" ref="K19:K36" si="2">"Fetches a bundle of all "&amp;B19&amp;" resources matching the specified "&amp;SUBSTITUTE(D19,","," and ")</f>
+        <v>Fetches a bundle of all !Encounter resources matching the specified patient and status and type</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
+      </c>
+      <c r="D20" t="s">
+        <v>518</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" t="s">
+        <v>494</v>
+      </c>
+      <c r="I20" t="s">
+        <v>519</v>
+      </c>
+      <c r="J20" t="s">
+        <v>520</v>
+      </c>
+      <c r="K20" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all Encounter resources matching the specified patient and status</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
+      </c>
+      <c r="D21" t="s">
+        <v>521</v>
+      </c>
+      <c r="F21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" t="s">
+        <v>494</v>
+      </c>
+      <c r="I21" t="s">
+        <v>519</v>
+      </c>
+      <c r="J21" t="s">
+        <v>522</v>
+      </c>
+      <c r="K21" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all Encounter resources matching the specified patient and discharge-disposition</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>486</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
+      </c>
+      <c r="D22" t="s">
+        <v>523</v>
+      </c>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" t="s">
+        <v>57</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all !Encounter resources matching the specified status and type</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>524</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
+      </c>
+      <c r="D23" t="s">
+        <v>525</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
+        <v>526</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>524</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
+      </c>
+      <c r="D24" t="s">
+        <v>527</v>
+      </c>
+      <c r="F24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" t="s">
+        <v>528</v>
+      </c>
+      <c r="K24" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and publisher and status</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>524</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
+      </c>
+      <c r="D25" t="s">
+        <v>529</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" t="s">
+        <v>530</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="K25" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all !Questionnaire resources matching the specified context-type-value and status</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>524</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
+      </c>
+      <c r="D26" t="s">
+        <v>531</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
+        <v>532</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>524</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
+      </c>
+      <c r="D27" t="s">
+        <v>533</v>
+      </c>
+      <c r="F27" t="s">
+        <v>69</v>
+      </c>
+      <c r="G27" t="s">
+        <v>532</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and status and version</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>524</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
+      </c>
+      <c r="D28" t="s">
+        <v>534</v>
+      </c>
+      <c r="F28" t="s">
+        <v>69</v>
+      </c>
+      <c r="G28" t="s">
+        <v>532</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all !Questionnaire resources matching the specified publisher and version</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>524</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
+      </c>
+      <c r="D29" t="s">
+        <v>535</v>
+      </c>
+      <c r="F29" t="s">
+        <v>69</v>
+      </c>
+      <c r="G29" t="s">
+        <v>532</v>
+      </c>
+      <c r="K29" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all !Questionnaire resources matching the specified status and title and version</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>524</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
+      </c>
+      <c r="D30" t="s">
+        <v>536</v>
+      </c>
+      <c r="F30" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" t="s">
+        <v>57</v>
+      </c>
+      <c r="K30" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all !Questionnaire resources matching the specified status and version</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>524</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
+      </c>
+      <c r="D31" t="s">
+        <v>537</v>
+      </c>
+      <c r="F31" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" t="s">
+        <v>532</v>
+      </c>
+      <c r="K31" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all !Questionnaire resources matching the specified title and version</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>21</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
+      </c>
+      <c r="D32" t="s">
+        <v>538</v>
+      </c>
+      <c r="F32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" t="s">
+        <v>539</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>540</v>
+      </c>
+      <c r="J32" s="4" t="s">
+        <v>541</v>
+      </c>
+      <c r="K32" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all Patient resources matching the specified birthdate and family</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
+      </c>
+      <c r="D33" t="s">
+        <v>542</v>
+      </c>
+      <c r="F33" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" t="s">
+        <v>539</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="J33" s="4" t="s">
+        <v>544</v>
+      </c>
+      <c r="K33" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all Patient resources matching the specified death-date and family</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
+      </c>
+      <c r="D34" t="s">
+        <v>545</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>539</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>547</v>
+      </c>
+      <c r="K34" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all Patient resources matching the specified birthdate and name</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
+      </c>
+      <c r="D35" t="s">
+        <v>548</v>
+      </c>
+      <c r="F35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" t="s">
+        <v>532</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>549</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>550</v>
+      </c>
+      <c r="K35" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all Patient resources matching the specified family and gender</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
+      </c>
+      <c r="D36" t="s">
+        <v>551</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>532</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>552</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="K36" s="4" t="str">
+        <f t="shared" si="2"/>
+        <v>Fetches a bundle of all Patient resources matching the specified gender and name</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
+      </c>
+      <c r="D37" t="s">
+        <v>554</v>
+      </c>
+      <c r="F37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" t="s">
+        <v>494</v>
+      </c>
+      <c r="H37" t="s">
+        <v>555</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="J37" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="K37" s="4" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>93</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
+      </c>
+      <c r="D38" t="s">
+        <v>559</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>494</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="K38" s="4" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>93</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
+      </c>
+      <c r="D39" t="s">
+        <v>563</v>
+      </c>
+      <c r="F39" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" t="s">
+        <v>494</v>
+      </c>
+      <c r="H39" t="s">
+        <v>555</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>565</v>
+      </c>
+      <c r="K39" s="4" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
+      </c>
+      <c r="D40" t="s">
+        <v>567</v>
+      </c>
+      <c r="F40" t="s">
+        <v>69</v>
+      </c>
+      <c r="G40" t="s">
+        <v>494</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>560</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="K40" s="4" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>93</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
+      </c>
+      <c r="D41" t="s">
+        <v>570</v>
+      </c>
+      <c r="F41" t="s">
+        <v>69</v>
+      </c>
+      <c r="G41" t="s">
+        <v>494</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="K41" s="4" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
+      </c>
+      <c r="D42" t="s">
+        <v>574</v>
+      </c>
+      <c r="F42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G42" t="s">
+        <v>515</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="K42" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>93</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
+      </c>
+      <c r="D43" t="s">
+        <v>578</v>
+      </c>
+      <c r="F43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" t="s">
+        <v>515</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="J43" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="K43" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>93</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
+      </c>
+      <c r="D44" t="s">
+        <v>580</v>
+      </c>
+      <c r="F44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" t="s">
+        <v>515</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="J44" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
+      </c>
+      <c r="D45" t="s">
+        <v>582</v>
+      </c>
+      <c r="F45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45" t="s">
+        <v>515</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>575</v>
+      </c>
+      <c r="J45" s="4" t="s">
+        <v>583</v>
+      </c>
+      <c r="K45" s="4" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>40</v>
+      </c>
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
+      </c>
+      <c r="D46" t="s">
+        <v>514</v>
+      </c>
+      <c r="F46" t="s">
+        <v>69</v>
+      </c>
+      <c r="G46" t="s">
+        <v>515</v>
+      </c>
+      <c r="I46" s="4"/>
+      <c r="J46" s="25" t="s">
+        <v>584</v>
+      </c>
+      <c r="K46" s="25" t="str">
+        <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
+        <v>Fetches a bundle of all Condition resources for the specified patient and _lastUpdated. See the US Core General Guidance page for [Searching Using lastUpdated].</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
+      </c>
+      <c r="D47" t="s">
+        <v>554</v>
+      </c>
+      <c r="F47" t="s">
+        <v>69</v>
+      </c>
+      <c r="G47" t="s">
+        <v>494</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>586</v>
+      </c>
+      <c r="K47" s="4" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>101</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
+      </c>
+      <c r="D48" t="s">
+        <v>588</v>
+      </c>
+      <c r="F48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G48" t="s">
+        <v>504</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>589</v>
+      </c>
+      <c r="J48" s="4" t="s">
+        <v>590</v>
+      </c>
+      <c r="K48" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified "&amp;SUBSTITUTE(D48,","," and ")</f>
+        <v>Fetches a bundle of all Immunization resources for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" si="0"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
+      </c>
+      <c r="D49" t="s">
+        <v>518</v>
+      </c>
+      <c r="F49" t="s">
+        <v>69</v>
+      </c>
+      <c r="G49" t="s">
+        <v>515</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>591</v>
+      </c>
+      <c r="J49" s="4" t="s">
+        <v>592</v>
+      </c>
+      <c r="K49" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified "&amp;SUBSTITUTE(D49,","," and ")</f>
+        <v>Fetches a bundle of all Immunization resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>107</v>
+      </c>
+      <c r="C50" t="s">
+        <v>593</v>
+      </c>
+      <c r="D50" t="s">
+        <v>518</v>
+      </c>
+      <c r="F50" t="s">
+        <v>69</v>
+      </c>
+      <c r="G50" t="s">
+        <v>494</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="J50" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="K50" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified "&amp;SUBSTITUTE(D50,","," and ")</f>
+        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" t="s">
+        <v>593</v>
+      </c>
+      <c r="D51" t="s">
+        <v>559</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" t="s">
+        <v>494</v>
+      </c>
+      <c r="H51" t="s">
+        <v>596</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>597</v>
+      </c>
+      <c r="J51" s="26" t="s">
+        <v>598</v>
+      </c>
+      <c r="K51" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B51&amp;" resources for the specified patient and  a category code = `LAB`"</f>
+        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  a category code = `LAB`</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" t="s">
+        <v>593</v>
+      </c>
+      <c r="D52" t="s">
+        <v>570</v>
+      </c>
+      <c r="F52" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" t="s">
+        <v>494</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>599</v>
+      </c>
+      <c r="J52" s="26" t="s">
+        <v>600</v>
+      </c>
+      <c r="K52" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B52&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>107</v>
+      </c>
+      <c r="C53" t="s">
+        <v>593</v>
+      </c>
+      <c r="D53" t="s">
+        <v>601</v>
+      </c>
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s">
+        <v>602</v>
+      </c>
+      <c r="H53" t="s">
+        <v>596</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>603</v>
+      </c>
+      <c r="J53" s="26" t="s">
+        <v>604</v>
+      </c>
+      <c r="K53" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B53&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
+        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and a category code = `LAB`</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" t="str">
+        <f>"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B54)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
+      </c>
+      <c r="D54" t="s">
+        <v>605</v>
+      </c>
+      <c r="F54" t="s">
+        <v>69</v>
+      </c>
+      <c r="G54" t="s">
+        <v>602</v>
+      </c>
+      <c r="I54" s="4"/>
+      <c r="J54" s="24" t="s">
+        <v>606</v>
+      </c>
+      <c r="K54" s="25" t="str">
+        <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified "&amp;SUBSTITUTE(D54,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
+        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and category and _lastUpdated. See the US Core General Guidance page for [Searching Using lastUpdated].</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>107</v>
+      </c>
+      <c r="C55" t="s">
+        <v>593</v>
+      </c>
+      <c r="D55" t="s">
+        <v>607</v>
+      </c>
+      <c r="F55" t="s">
+        <v>69</v>
+      </c>
+      <c r="G55" t="s">
+        <v>602</v>
+      </c>
+      <c r="I55" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="J55" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="K55" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B55&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all DiagnosticReport resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" ref="C56:C66" si="3">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B56)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
+      </c>
+      <c r="D56" t="s">
+        <v>610</v>
+      </c>
+      <c r="F56" t="s">
+        <v>69</v>
+      </c>
+      <c r="G56" t="s">
+        <v>494</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="J56" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="K56" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B56&amp;" resources for the specified "&amp;SUBSTITUTE(D56,","," and ")</f>
+        <v>Fetches a bundle of all Goal resources for the specified patient and lifecycle-status</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>108</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
+      </c>
+      <c r="D57" t="s">
+        <v>613</v>
+      </c>
+      <c r="F57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G57" t="s">
+        <v>515</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="J57" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="K57" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B57&amp;" resources for the specified "&amp;SUBSTITUTE(D57,","," and ")</f>
+        <v>Fetches a bundle of all Goal resources for the specified patient and target-date</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>109</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
+      </c>
+      <c r="D58" t="s">
+        <v>616</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" t="s">
+        <v>494</v>
+      </c>
+      <c r="H58" t="s">
+        <v>617</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="J58" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="K58" s="4" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
+      </c>
+      <c r="D59" t="s">
+        <v>621</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>494</v>
+      </c>
+      <c r="H59" t="s">
+        <v>617</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="K59" s="4" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
+      </c>
+      <c r="D60" t="s">
+        <v>625</v>
+      </c>
+      <c r="F60" t="s">
+        <v>69</v>
+      </c>
+      <c r="G60" t="s">
+        <v>494</v>
+      </c>
+      <c r="H60" t="s">
+        <v>617</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>622</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="K60" s="4" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>109</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
+      </c>
+      <c r="D61" t="s">
+        <v>628</v>
+      </c>
+      <c r="F61" t="s">
+        <v>69</v>
+      </c>
+      <c r="G61" t="s">
+        <v>602</v>
+      </c>
+      <c r="H61" t="s">
+        <v>617</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>630</v>
+      </c>
+      <c r="K61" s="4" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
+        <v>250</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
+      </c>
+      <c r="D62" t="s">
+        <v>518</v>
+      </c>
+      <c r="F62" t="s">
+        <v>69</v>
+      </c>
+      <c r="G62" t="s">
+        <v>494</v>
+      </c>
+      <c r="I62" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="J62" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="K62" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified "&amp;SUBSTITUTE(D62,","," and ")</f>
+        <v>Fetches a bundle of all !MedicationStatement resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
+        <v>250</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
+      </c>
+      <c r="D63" t="s">
+        <v>634</v>
+      </c>
+      <c r="F63" t="s">
+        <v>69</v>
+      </c>
+      <c r="G63" t="s">
+        <v>515</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>635</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="K63" s="4" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
+        <v>110</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
+      </c>
+      <c r="D64" t="s">
+        <v>518</v>
+      </c>
+      <c r="F64" t="s">
+        <v>69</v>
+      </c>
+      <c r="G64" t="s">
+        <v>494</v>
+      </c>
+      <c r="I64" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="K64" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified "&amp;SUBSTITUTE(D64,","," and ")</f>
+        <v>Fetches a bundle of all Procedure resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
+        <v>110</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
+      </c>
+      <c r="D65" t="s">
+        <v>588</v>
+      </c>
+      <c r="F65" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" t="s">
+        <v>494</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="J65" s="4" t="s">
+        <v>641</v>
+      </c>
+      <c r="K65" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified "&amp;SUBSTITUTE(D65,","," and ")</f>
+        <v>Fetches a bundle of all Procedure resources for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A66">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" si="3"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
+      </c>
+      <c r="D66" t="s">
+        <v>607</v>
+      </c>
+      <c r="F66" t="s">
+        <v>69</v>
+      </c>
+      <c r="G66" t="s">
+        <v>602</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>642</v>
+      </c>
+      <c r="J66" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="K66" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
+        <v>Fetches a bundle of all Procedure resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes.</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A67">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
+        <v>111</v>
+      </c>
+      <c r="C67" t="s">
+        <v>644</v>
+      </c>
+      <c r="D67" t="s">
+        <v>645</v>
+      </c>
+      <c r="F67" t="s">
+        <v>69</v>
+      </c>
+      <c r="G67" t="s">
+        <v>494</v>
+      </c>
+      <c r="H67" t="s">
+        <v>646</v>
+      </c>
+      <c r="I67" s="4" t="s">
+        <v>647</v>
+      </c>
+      <c r="J67" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="K67" s="4" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A68">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
+        <v>111</v>
+      </c>
+      <c r="C68" t="s">
+        <v>644</v>
+      </c>
+      <c r="D68" t="s">
+        <v>559</v>
+      </c>
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" t="s">
+        <v>494</v>
+      </c>
+      <c r="H68" t="s">
+        <v>646</v>
+      </c>
+      <c r="I68" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="J68" s="4" t="s">
+        <v>651</v>
+      </c>
+      <c r="K68" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and a category code = `laboratory`</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" ht="31" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
+        <v>111</v>
+      </c>
+      <c r="C69" t="s">
+        <v>644</v>
+      </c>
+      <c r="D69" t="s">
+        <v>570</v>
+      </c>
+      <c r="F69" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" t="s">
+        <v>494</v>
+      </c>
+      <c r="I69" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="J69" s="8" t="s">
+        <v>653</v>
+      </c>
+      <c r="K69" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only.</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
+        <v>111</v>
+      </c>
+      <c r="C70" t="s">
+        <v>644</v>
+      </c>
+      <c r="D70" t="s">
+        <v>601</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s">
+        <v>602</v>
+      </c>
+      <c r="H70" t="s">
+        <v>646</v>
+      </c>
+      <c r="I70" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="J70" s="4" t="s">
+        <v>655</v>
+      </c>
+      <c r="K70" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and date and a category code = `laboratory`</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
+        <v>111</v>
+      </c>
+      <c r="C71" t="s">
+        <v>644</v>
+      </c>
+      <c r="D71" t="s">
+        <v>605</v>
+      </c>
+      <c r="F71" t="s">
+        <v>69</v>
+      </c>
+      <c r="G71" t="s">
+        <v>602</v>
+      </c>
+      <c r="I71" s="4"/>
+      <c r="J71" s="24" t="s">
+        <v>656</v>
+      </c>
+      <c r="K71" s="25" t="str">
+        <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and category and _lastUpdated. See the US Core General Guidance page for [Searching Using lastUpdated].</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A72">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
+        <v>111</v>
+      </c>
+      <c r="C72" t="s">
+        <v>644</v>
+      </c>
+      <c r="D72" t="s">
+        <v>607</v>
+      </c>
+      <c r="F72" t="s">
+        <v>69</v>
+      </c>
+      <c r="G72" t="s">
+        <v>602</v>
+      </c>
+      <c r="I72" s="4" t="s">
+        <v>657</v>
+      </c>
+      <c r="J72" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="K72" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all Observation resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A73">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
+        <v>126</v>
+      </c>
+      <c r="C73" t="s">
+        <v>128</v>
+      </c>
+      <c r="D73" t="s">
+        <v>559</v>
+      </c>
+      <c r="F73" t="s">
+        <v>12</v>
+      </c>
+      <c r="G73" t="s">
+        <v>494</v>
+      </c>
+      <c r="H73" t="s">
+        <v>659</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>660</v>
+      </c>
+      <c r="J73" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="K73" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified "&amp;SUBSTITUTE(D73,","," and ")&amp;"=`assess-plan`"</f>
+        <v>Fetches a bundle of all CarePlan resources for the specified patient and category=`assess-plan`</v>
+      </c>
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74" t="s">
+        <v>128</v>
+      </c>
+      <c r="D74" t="s">
+        <v>601</v>
+      </c>
+      <c r="F74" t="s">
+        <v>69</v>
+      </c>
+      <c r="G74" t="s">
+        <v>602</v>
+      </c>
+      <c r="H74" t="s">
+        <v>659</v>
+      </c>
+      <c r="I74" s="4" t="s">
+        <v>662</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>663</v>
+      </c>
+      <c r="K74" s="4" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A75">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
+        <v>126</v>
+      </c>
+      <c r="C75" t="s">
+        <v>128</v>
+      </c>
+      <c r="D75" t="s">
+        <v>645</v>
+      </c>
+      <c r="F75" t="s">
+        <v>69</v>
+      </c>
+      <c r="G75" t="s">
+        <v>494</v>
+      </c>
+      <c r="H75" t="s">
+        <v>659</v>
+      </c>
+      <c r="I75" s="4" t="s">
+        <v>665</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="K75" s="4" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A76">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
+        <v>126</v>
+      </c>
+      <c r="C76" t="s">
+        <v>128</v>
+      </c>
+      <c r="D76" t="s">
+        <v>668</v>
+      </c>
+      <c r="F76" t="s">
+        <v>69</v>
+      </c>
+      <c r="G76" t="s">
+        <v>602</v>
+      </c>
+      <c r="H76" t="s">
+        <v>659</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>669</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="K76" s="4" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" ht="136" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
+        <v>129</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" ref="C77:C83" si="4">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B77)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
+      </c>
+      <c r="D77" t="s">
+        <v>518</v>
+      </c>
+      <c r="F77" t="s">
+        <v>12</v>
+      </c>
+      <c r="G77" t="s">
+        <v>494</v>
+      </c>
+      <c r="H77" t="s">
+        <v>672</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>673</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>674</v>
+      </c>
+      <c r="K77" s="8" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A78">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
+        <v>106</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" si="4"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
+      </c>
+      <c r="D78" t="s">
+        <v>518</v>
+      </c>
+      <c r="F78" t="s">
+        <v>69</v>
+      </c>
+      <c r="G78" t="s">
+        <v>494</v>
+      </c>
+      <c r="I78" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="J78" s="4" t="s">
+        <v>677</v>
+      </c>
+      <c r="K78" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B78&amp;" resources for the specified "&amp;SUBSTITUTE(D78,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
+        <v>Fetches a bundle of all DocumentReference resources for the specified patient and status. See the implementation notes above for how to access the actual document.</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
+        <v>678</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" si="4"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
+      </c>
+      <c r="D79" t="s">
+        <v>679</v>
+      </c>
+      <c r="F79" t="s">
+        <v>69</v>
+      </c>
+      <c r="G79" t="s">
+        <v>515</v>
+      </c>
+      <c r="I79" s="4" t="s">
+        <v>676</v>
+      </c>
+      <c r="J79" s="4"/>
+      <c r="K79" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B79&amp;" resources for the specified "&amp;SUBSTITUTE(D79,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
+        <v>Fetches a bundle of all !DocumentReference resources for the specified patient and period. See the implementation notes above for how to access the actual document.</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
+        <v>106</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" si="4"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
+      </c>
+      <c r="D80" t="s">
+        <v>559</v>
+      </c>
+      <c r="F80" t="s">
+        <v>12</v>
+      </c>
+      <c r="G80" t="s">
+        <v>494</v>
+      </c>
+      <c r="H80" t="s">
+        <v>680</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>681</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>682</v>
+      </c>
+      <c r="K80" s="4" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="81" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
+        <v>106</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="4"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
+      </c>
+      <c r="D81" t="s">
+        <v>601</v>
+      </c>
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s">
+        <v>602</v>
+      </c>
+      <c r="H81" t="s">
+        <v>680</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>684</v>
+      </c>
+      <c r="J81" s="26" t="s">
+        <v>685</v>
+      </c>
+      <c r="K81" s="4" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
+        <v>106</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="4"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
+      </c>
+      <c r="D82" t="s">
+        <v>509</v>
+      </c>
+      <c r="F82" t="s">
+        <v>12</v>
+      </c>
+      <c r="G82" t="s">
+        <v>494</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>687</v>
+      </c>
+      <c r="J82" s="4" t="s">
+        <v>688</v>
+      </c>
+      <c r="K82" s="4" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
+        <v>106</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="4"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
+      </c>
+      <c r="D83" t="s">
+        <v>690</v>
+      </c>
+      <c r="F83" t="s">
+        <v>69</v>
+      </c>
+      <c r="G83" t="s">
+        <v>602</v>
+      </c>
+      <c r="I83" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="J83" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="K83" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
+        <v>Fetches a bundle of all DocumentReference resources for the specified patient and type and period. See the implementation notes above for how to access the actual document.</v>
+      </c>
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A84">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
+        <v>130</v>
+      </c>
+      <c r="C84" t="s">
+        <v>693</v>
+      </c>
+      <c r="D84" t="s">
+        <v>509</v>
+      </c>
+      <c r="F84" t="s">
+        <v>69</v>
+      </c>
+      <c r="G84" t="s">
+        <v>494</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>694</v>
+      </c>
+      <c r="J84" s="4" t="s">
+        <v>695</v>
+      </c>
+      <c r="K84" s="4" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A85">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
+        <v>130</v>
+      </c>
+      <c r="C85" t="s">
+        <v>693</v>
+      </c>
+      <c r="D85" t="s">
+        <v>518</v>
+      </c>
+      <c r="F85" t="s">
+        <v>69</v>
+      </c>
+      <c r="G85" t="s">
+        <v>494</v>
+      </c>
+      <c r="I85" s="4" t="s">
+        <v>697</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="K85" s="4" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A86">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
+        <v>129</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" ref="C86:C100" si="5">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B86)</f>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
+      </c>
+      <c r="D86" t="s">
+        <v>700</v>
+      </c>
+      <c r="F86" t="s">
+        <v>69</v>
+      </c>
+      <c r="G86" t="s">
+        <v>494</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>701</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="K86" s="4" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
+        <v>340</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="D87" t="s">
+        <v>518</v>
+      </c>
+      <c r="F87" t="s">
+        <v>69</v>
+      </c>
+      <c r="G87" t="s">
+        <v>494</v>
+      </c>
+      <c r="I87" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="J87" s="4" t="s">
+        <v>705</v>
+      </c>
+      <c r="K87" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified "&amp;SUBSTITUTE(D87,","," and ")</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
+        <v>340</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="D88" t="s">
+        <v>559</v>
+      </c>
+      <c r="F88" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88" t="s">
+        <v>494</v>
+      </c>
+      <c r="I88" s="4" t="s">
+        <v>706</v>
+      </c>
+      <c r="J88" s="4" t="s">
+        <v>707</v>
+      </c>
+      <c r="K88" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified patient and  a category code"</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  a category code</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
+        <v>340</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="D89" t="s">
+        <v>570</v>
+      </c>
+      <c r="F89" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" t="s">
+        <v>494</v>
+      </c>
+      <c r="I89" s="4" t="s">
+        <v>708</v>
+      </c>
+      <c r="J89" s="4" t="s">
+        <v>709</v>
+      </c>
+      <c r="K89" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
+        <v>340</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="D90" t="s">
+        <v>710</v>
+      </c>
+      <c r="F90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" t="s">
+        <v>602</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>711</v>
+      </c>
+      <c r="J90" s="4" t="s">
+        <v>712</v>
+      </c>
+      <c r="K90" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified patient and date and a category code"</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and a category code</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
+        <v>340</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
+      </c>
+      <c r="D91" t="s">
+        <v>713</v>
+      </c>
+      <c r="F91" t="s">
+        <v>69</v>
+      </c>
+      <c r="G91" t="s">
+        <v>602</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>714</v>
+      </c>
+      <c r="J91" s="4" t="s">
+        <v>715</v>
+      </c>
+      <c r="K91" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
+        <v>Fetches a bundle of all ServiceRequest resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes.</v>
+      </c>
+    </row>
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A92">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
+        <v>108</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
+      </c>
+      <c r="D92" t="s">
+        <v>716</v>
+      </c>
+      <c r="F92" t="s">
+        <v>69</v>
+      </c>
+      <c r="G92" t="s">
+        <v>494</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>717</v>
+      </c>
+      <c r="J92" s="4" t="s">
+        <v>718</v>
+      </c>
+      <c r="K92" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
+        <v>Fetches a bundle of all Goal resources for the specified patient and description</v>
+      </c>
+    </row>
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A93">
+        <v>92</v>
+      </c>
+      <c r="B93" t="s">
+        <v>368</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+      </c>
+      <c r="D93" t="s">
+        <v>518</v>
+      </c>
+      <c r="F93" t="s">
+        <v>69</v>
+      </c>
+      <c r="G93" t="s">
+        <v>494</v>
+      </c>
+      <c r="I93" t="s">
+        <v>719</v>
+      </c>
+      <c r="J93" s="4" t="s">
+        <v>720</v>
+      </c>
+      <c r="K93" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and status</v>
+      </c>
+    </row>
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A94">
+        <v>93</v>
+      </c>
+      <c r="B94" t="s">
+        <v>442</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+      </c>
+      <c r="D94" t="s">
+        <v>721</v>
+      </c>
+      <c r="F94" t="s">
+        <v>69</v>
+      </c>
+      <c r="G94" t="s">
+        <v>494</v>
+      </c>
+      <c r="H94" t="s">
+        <v>722</v>
+      </c>
+      <c r="I94" t="s">
+        <v>719</v>
+      </c>
+      <c r="J94" s="4" t="s">
+        <v>723</v>
+      </c>
+      <c r="K94" t="str">
+        <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified "&amp;SUBSTITUTE(D94,","," and  ") &amp; "= 'sdoh'"</f>
+        <v>Fetches a bundle of all !QuestionnaireResponse resources for the specified patient and  _tag= 'sdoh'</v>
+      </c>
+    </row>
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A95">
+        <v>94</v>
+      </c>
+      <c r="B95" t="s">
+        <v>368</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+      </c>
+      <c r="D95" t="s">
+        <v>724</v>
+      </c>
+      <c r="F95" t="s">
+        <v>69</v>
+      </c>
+      <c r="G95" t="s">
+        <v>515</v>
+      </c>
+      <c r="I95" t="s">
+        <v>719</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>725</v>
+      </c>
+      <c r="K95" s="4" t="str">
+        <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date"</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>95</v>
+      </c>
+      <c r="B96" t="s">
+        <v>442</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
+      </c>
+      <c r="D96" s="16" t="s">
+        <v>726</v>
+      </c>
+      <c r="F96" t="s">
+        <v>69</v>
+      </c>
+      <c r="G96" t="s">
+        <v>602</v>
+      </c>
+      <c r="H96" t="s">
+        <v>722</v>
+      </c>
+      <c r="I96" t="s">
+        <v>719</v>
+      </c>
+      <c r="J96" s="4" t="s">
+        <v>727</v>
+      </c>
+      <c r="K96" t="str">
+        <f>"Fetches a bundle of all "&amp;B96&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
+        <v>Fetches a bundle of all !QuestionnaireResponse resources tagged as 'sdoh' for the specified patient and date</v>
+      </c>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>368</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
+      </c>
+      <c r="D97" s="16" t="s">
+        <v>728</v>
+      </c>
+      <c r="F97" t="s">
+        <v>69</v>
+      </c>
+      <c r="G97" t="s">
+        <v>89</v>
+      </c>
+      <c r="I97" t="s">
+        <v>719</v>
+      </c>
+      <c r="J97" s="4" t="s">
+        <v>729</v>
+      </c>
+      <c r="K97" t="str">
+        <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient that have been completed against a specified form."</f>
+        <v>Fetches a bundle of all QuestionnaireResponse resources for the specified patient that have been completed against a specified form.</v>
+      </c>
+    </row>
+    <row r="98" spans="1:11" ht="151" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+      </c>
+      <c r="D98" s="16" t="s">
+        <v>518</v>
+      </c>
+      <c r="E98" s="16"/>
+      <c r="F98" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G98" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="H98" s="16"/>
+      <c r="I98" s="4" t="s">
+        <v>730</v>
+      </c>
+      <c r="J98" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="K98" t="str">
+        <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed)).</v>
+      </c>
+    </row>
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
+      </c>
+      <c r="D99" s="16" t="s">
+        <v>517</v>
+      </c>
+      <c r="E99" s="16"/>
+      <c r="F99" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G99" s="16" t="s">
+        <v>494</v>
+      </c>
+      <c r="H99" s="16"/>
+      <c r="I99" s="4" t="s">
+        <v>732</v>
+      </c>
+      <c r="J99" s="4" t="s">
+        <v>733</v>
+      </c>
+      <c r="K99" t="str">
+        <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed).</v>
+      </c>
+    </row>
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" s="16" t="s">
+        <v>405</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" si="5"/>
+        <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
+      </c>
+      <c r="D100" s="16" t="s">
+        <v>734</v>
+      </c>
+      <c r="E100" s="16"/>
+      <c r="F100" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G100" s="16" t="s">
+        <v>515</v>
+      </c>
+      <c r="H100" s="16"/>
+      <c r="I100" s="4" t="s">
+        <v>735</v>
+      </c>
+      <c r="J100" s="4" t="s">
+        <v>736</v>
+      </c>
+      <c r="K100" t="str">
+        <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient for a given dispense and date or range"</f>
+        <v>Fetches a bundle of all MedicationDispense resources for the specified patient for a given dispense and date or range</v>
+      </c>
+    </row>
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" s="16" t="s">
+        <v>349</v>
+      </c>
+      <c r="C101" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="D101" s="16" t="s">
+        <v>737</v>
+      </c>
+      <c r="E101" s="16"/>
+      <c r="F101" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G101" s="16" t="s">
+        <v>738</v>
+      </c>
+      <c r="H101" s="16"/>
+      <c r="I101" s="4"/>
+      <c r="J101" s="4" t="s">
+        <v>739</v>
+      </c>
+      <c r="K101" t="str">
+        <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
+        <v>Fetches a bundle of all RelatedPerson resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:K101" xr:uid="{331E0B16-168F-459B-8951-3DF614BF0371}"/>
+  <conditionalFormatting sqref="B1:B100 B102:B1048576">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="!">
+      <formula>NOT(ISERROR(SEARCH("!",B1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="C101" r:id="rId1" xr:uid="{E5D9E9A5-D437-E344-976B-BF6F06BE5521}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -10552,7 +14527,7 @@
     <sortCondition ref="B2:B46"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11365,7 +15340,7 @@
     <sortCondition ref="A2:A26"/>
   </sortState>
   <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="!">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="!">
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
FHIR-48443	Add USCDI v5 Data Elements to US Core Medications, Orders update version
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354E736D-0A82-CC4E-A54D-35F6E3F6D31C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148F263E-9157-704F-A063-2EF60F27DBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34100" yWindow="500" windowWidth="34140" windowHeight="28300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19640" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1568,12 +1568,6 @@
 </t>
   </si>
   <si>
-    <t>7.0.0</t>
-  </si>
-  <si>
-    <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ONC 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and the ONC [U.S. Core Data for Interoperability (USCDI) Version 4 July 2023](https://www.healthit.gov/sites/isa/files/2023-07/Final-USCDI-Version-4-July-2023-Final.pdf).</t>
-  </si>
-  <si>
     <t>_lastUpdated</t>
   </si>
   <si>
@@ -1653,13 +1647,6 @@
   </si>
   <si>
     <t>* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `RelatedPerson.address.line` and  `RelatedPerson.address.city`.</t>
-  </si>
-  <si>
-    <t>* Servers and Clients **SHALL** support both US Core ServiceRequest and US Core Procedure Profiles for communicating the reason or justification for a referral as Additional USCDI Requirements. Typically, the reason or justification for a referral or consultation is communicated through `Procedure.basedOn` linking the Procedure to the US Core ServiceRequest Profile that includes either `ServiceRequest.reasonCode` or `ServiceRequest.reasonReference`. When the Procedure does not have an associated ServiceRequest, it is communicated through the US Core Procedure Profile's `Procedure.reasonCode` or `Procedure.reasonReference`.  Depending on the procedure being documented, a server will select the appropriate Profile to use.
-   * `ServiceRequest.reasonCode` and `ServiceRequest.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
-      * when using  `ServiceRequest.reasonReference`:
-         * Servers **SHALL** support *at least one* target resource in `ServiceRequest.reasonReference`. Clients **SHALL** support all target resources.
-         * The referenced resources **SHOULD** be a US Core Profile.</t>
   </si>
   <si>
     <t>* Although both `Specimen.identifier` and `Specimen.accessionIdentifier` are marked as Must Support, the server system is not required to support both, but **SHALL** support at least one of these elements. The client application **SHALL** support both.</t>
@@ -2529,12 +2516,38 @@
   <si>
     <t>GET [base]/RelatedPerson?patient=1137192&amp;name=van%20Putten</t>
   </si>
+  <si>
+    <t>- The Must Support `ServiceRequest.category` is bound, *at a minimum*, to the [US Core ServiceRequest Category Codes], and other category codes can be used. API consumers can query by category when accessing patient information. For the USCDI *Laboratory Order*, *Imaging Order*, *Clinical Test Order*, and *Procedure Order* Data Elements, implementers **SHOULD** use the corresponding category codes listed in the table below. For example, laboratory orders would have the category code "108252007" (Laboratory procedure).
+  |USCDI Order Data Element|Category Codes|
+  |---|---|
+  |Laboratory Order| 108252007 Laboratory procedure (procedure)|
+  |Imaging Order|363679005 Imaging (procedure)|
+  |Clinical Test Order|386053000 Evaluation procedure (procedure), 410606002 Social service procedure (procedure), or 387713003 Surgical procedure (procedure)|
+  |Procedure Order|386053000 Evaluation procedure (procedure), 410606002 Social service procedure (procedure), or 387713003 Surgical procedure (procedure)| 
+- The `ServiceRequest.code` value set is broad to accommodate a wide variety of use cases and **SHOULD** be constrained to a subset for a particular use case or domain.  These value sets contain concepts that span many use cases and are not bound to any USCDI Data Element. However, the table below identifies *additional* value set bindings for the USCDI *Laboratory Order, Imaging Order and Clinical Test Order* Data Elements. Implementers **SHOULD** conform to the binding strengths listed for each USCDI Order context. For example, laboratory orders are extensibly bound to the LOINC Common Laboratory Orders Value Set. Note that the USCDI Class *Procedure Order* Data Element has no additional binding.
+  |USCDI Order Data Element|Additional Binding|Binding Strength|Comments|
+  |---|---|---|---|
+  |Laboratory Order|LOINC Common Laboratory Orders Value Set|extensible|The LOINC Common Laboratory Orders Value Set is a "starter set" for mapping commonly used laboratory orders. It does not attempt to include all possible laboratory order codes. For additional information on LOINC Common Laboratory Orders Value Set, refer to www.loinc.org/usage/orders.|
+  |Imaging Order|LOINC Radiology Codes|preferred|The LOINC Radiology Codes include all imaging codes minus concepts that are deprecated or discouraged.|
+  |Clinical Test Order|LOINC Clinical Test Codes|example|LOINC Clinical Test Codes include all non-laboratory and non-imaging clinical test codes|
+- *Servers and Clients **SHALL** support both US Core ServiceRequest and US Core Procedure Profiles for communicating the reason or justification for a referral as Additional USCDI Requirements. Typically, the reason or justification for a referral or consultation is communicated through `Procedure.basedOn` linking the Procedure to the US Core ServiceRequest Profile that includes either `ServiceRequest.reasonCode` or `ServiceRequest.reasonReference`. When the Procedure does not have an associated ServiceRequest, it is communicated through the US Core Procedure Profile's `Procedure.reasonCode` or `Procedure.reasonReference`. Depending on the procedure being documented, a server will select the appropriate Profile to use.
+   - Although both `ServiceRequest.reasonCode` and `ServiceRequest.reasonReference` are marked as Additional USCDI Requirements, the certifying server system is not required to support both, but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
+     - when using  `ServiceRequest.reasonReference`:
+       - Servers **SHALL** support *at least one* target resource in `ServiceRequest.reasonReference`. Clients **SHALL** support all target resources.
+       - The referenced resources **SHOULD** be a US Core Profile as documented in [Referencing US Core Profiles].</t>
+  </si>
+  <si>
+    <t>8.0.0-ballot</t>
+  </si>
+  <si>
+    <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ONC 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and the ONC [U.S. Core Data for Interoperability (USCDI) Version 5 July 2024](https://www.healthit.gov/isp/sites/isp/files/2024-07/USCDI-Version-5-July-2024-Final.pdf).</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2648,12 +2661,6 @@
       <sz val="12"/>
       <color rgb="FF005C00"/>
       <name val="Monaco"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -3148,7 +3155,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5546,7 +5553,7 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D44" t="s">
         <v>30</v>
@@ -5555,7 +5562,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" ref="G44" si="5">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B44)</f>
@@ -5975,7 +5982,7 @@
         <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D52" t="s">
         <v>30</v>
@@ -5984,7 +5991,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="4"/>
@@ -6672,7 +6679,7 @@
         <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D65" t="s">
         <v>30</v>
@@ -6681,7 +6688,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="4"/>
@@ -8279,7 +8286,7 @@
         <v>111</v>
       </c>
       <c r="C95" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="D95" t="s">
         <v>30</v>
@@ -8288,7 +8295,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" ref="G95" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B95)</f>
@@ -10335,7 +10342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1832F48A-473A-3546-820D-6A8E9142FE06}">
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -10358,7 +10365,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>37</v>
@@ -10367,19 +10374,19 @@
         <v>39</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>333</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
@@ -10396,20 +10403,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C49" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D2" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="F2" t="s">
         <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="K2" s="4" t="str">
         <f t="shared" ref="K2:K17" si="1">"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
@@ -10421,20 +10428,20 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D3" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="F3" t="s">
         <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="K3" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10446,20 +10453,20 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D4" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="F4" t="s">
         <v>69</v>
       </c>
       <c r="G4" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="K4" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10471,20 +10478,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D5" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F5" t="s">
         <v>69</v>
       </c>
       <c r="G5" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="K5" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10503,19 +10510,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D6" t="s">
+        <v>490</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
+        <v>491</v>
+      </c>
+      <c r="I6" t="s">
+        <v>492</v>
+      </c>
+      <c r="J6" t="s">
         <v>493</v>
-      </c>
-      <c r="F6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" t="s">
-        <v>494</v>
-      </c>
-      <c r="I6" t="s">
-        <v>495</v>
-      </c>
-      <c r="J6" t="s">
-        <v>496</v>
       </c>
       <c r="K6" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10527,20 +10534,20 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D7" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="F7" t="s">
         <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="K7" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10552,20 +10559,20 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D8" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="F8" t="s">
         <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="K8" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10577,20 +10584,20 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D9" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="str">
@@ -10603,14 +10610,14 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D10" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F10" t="s">
         <v>69</v>
@@ -10630,14 +10637,14 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D11" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="F11" t="s">
         <v>69</v>
@@ -10656,14 +10663,14 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D12" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="F12" t="s">
         <v>69</v>
@@ -10688,19 +10695,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D13" t="s">
+        <v>500</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>501</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>502</v>
+      </c>
+      <c r="J13" t="s">
         <v>503</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>504</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>505</v>
-      </c>
-      <c r="J13" t="s">
-        <v>506</v>
       </c>
       <c r="K13" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10712,20 +10719,20 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D14" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="F14" t="s">
         <v>69</v>
       </c>
       <c r="G14" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="K14" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10737,20 +10744,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D15" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="F15" t="s">
         <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
       <c r="K15" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10769,19 +10776,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D16" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F16" t="s">
         <v>69</v>
       </c>
       <c r="G16" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I16" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="J16" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="K16" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10800,7 +10807,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="F17" t="s">
         <v>69</v>
@@ -10809,10 +10816,10 @@
         <v>89</v>
       </c>
       <c r="I17" t="s">
+        <v>507</v>
+      </c>
+      <c r="J17" t="s">
         <v>510</v>
-      </c>
-      <c r="J17" t="s">
-        <v>513</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10831,17 +10838,17 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="F18" t="s">
         <v>69</v>
       </c>
       <c r="G18" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="24" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
       <c r="K18" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B18&amp;" resources for the specified "&amp;SUBSTITUTE(D18,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -10853,20 +10860,20 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D19" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="F19" t="s">
         <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="str">
@@ -10886,19 +10893,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F20" t="s">
         <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I20" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="J20" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="2"/>
@@ -10917,19 +10924,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D21" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="F21" t="s">
         <v>69</v>
       </c>
       <c r="G21" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I21" t="s">
+        <v>516</v>
+      </c>
+      <c r="J21" t="s">
         <v>519</v>
-      </c>
-      <c r="J21" t="s">
-        <v>522</v>
       </c>
       <c r="K21" s="4" t="str">
         <f t="shared" si="2"/>
@@ -10941,14 +10948,14 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D22" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F22" t="s">
         <v>69</v>
@@ -10968,20 +10975,20 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D23" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="F23" t="s">
         <v>69</v>
       </c>
       <c r="G23" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="str">
@@ -10994,20 +11001,20 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D24" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="F24" t="s">
         <v>69</v>
       </c>
       <c r="G24" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="K24" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11019,20 +11026,20 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D25" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="F25" t="s">
         <v>69</v>
       </c>
       <c r="G25" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I25" s="4"/>
       <c r="K25" s="4" t="str">
@@ -11045,20 +11052,20 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D26" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="F26" t="s">
         <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -11072,20 +11079,20 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D27" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="F27" t="s">
         <v>69</v>
       </c>
       <c r="G27" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -11099,20 +11106,20 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D28" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="F28" t="s">
         <v>69</v>
       </c>
       <c r="G28" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -11126,20 +11133,20 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D29" t="s">
-        <v>535</v>
+        <v>532</v>
       </c>
       <c r="F29" t="s">
         <v>69</v>
       </c>
       <c r="G29" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="K29" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11151,14 +11158,14 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D30" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="F30" t="s">
         <v>69</v>
@@ -11176,20 +11183,20 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D31" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="F31" t="s">
         <v>69</v>
       </c>
       <c r="G31" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="K31" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11208,19 +11215,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
+        <v>535</v>
+      </c>
+      <c r="F32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" t="s">
+        <v>536</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>537</v>
+      </c>
+      <c r="J32" s="4" t="s">
         <v>538</v>
-      </c>
-      <c r="F32" t="s">
-        <v>69</v>
-      </c>
-      <c r="G32" t="s">
-        <v>539</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>540</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11239,19 +11246,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D33" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="F33" t="s">
         <v>69</v>
       </c>
       <c r="G33" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="I33" s="4" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="J33" s="4" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="K33" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11270,19 +11277,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D34" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
       <c r="F34" t="s">
         <v>12</v>
       </c>
       <c r="G34" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="J34" s="4" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="K34" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11301,19 +11308,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D35" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="F35" t="s">
         <v>69</v>
       </c>
       <c r="G35" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="I35" s="4" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="J35" s="4" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="K35" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11332,19 +11339,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D36" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="F36" t="s">
         <v>12</v>
       </c>
       <c r="G36" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="I36" s="4" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="J36" s="4" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="K36" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11363,25 +11370,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" t="s">
+        <v>551</v>
+      </c>
+      <c r="F37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" t="s">
+        <v>491</v>
+      </c>
+      <c r="H37" t="s">
+        <v>552</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>553</v>
+      </c>
+      <c r="J37" s="4" t="s">
         <v>554</v>
       </c>
-      <c r="F37" t="s">
-        <v>69</v>
-      </c>
-      <c r="G37" t="s">
-        <v>494</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="K37" s="4" t="s">
         <v>555</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>556</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>557</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>558</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -11396,22 +11403,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
+        <v>556</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>491</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>557</v>
+      </c>
+      <c r="J38" s="4" t="s">
+        <v>558</v>
+      </c>
+      <c r="K38" s="4" t="s">
         <v>559</v>
-      </c>
-      <c r="F38" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" t="s">
-        <v>494</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>560</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>561</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -11426,25 +11433,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
+        <v>560</v>
+      </c>
+      <c r="F39" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" t="s">
+        <v>491</v>
+      </c>
+      <c r="H39" t="s">
+        <v>552</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="J39" s="25" t="s">
+        <v>562</v>
+      </c>
+      <c r="K39" s="4" t="s">
         <v>563</v>
-      </c>
-      <c r="F39" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" t="s">
-        <v>494</v>
-      </c>
-      <c r="H39" t="s">
-        <v>555</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>564</v>
-      </c>
-      <c r="J39" s="25" t="s">
-        <v>565</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -11459,22 +11466,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="F40" t="s">
         <v>69</v>
       </c>
       <c r="G40" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -11489,22 +11496,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
+        <v>567</v>
+      </c>
+      <c r="F41" t="s">
+        <v>69</v>
+      </c>
+      <c r="G41" t="s">
+        <v>491</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>568</v>
+      </c>
+      <c r="J41" s="4" t="s">
+        <v>569</v>
+      </c>
+      <c r="K41" s="4" t="s">
         <v>570</v>
-      </c>
-      <c r="F41" t="s">
-        <v>69</v>
-      </c>
-      <c r="G41" t="s">
-        <v>494</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="J41" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>573</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -11519,22 +11526,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
+        <v>571</v>
+      </c>
+      <c r="F42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G42" t="s">
+        <v>512</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="J42" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="K42" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="F42" t="s">
-        <v>69</v>
-      </c>
-      <c r="G42" t="s">
-        <v>515</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="J42" s="4" t="s">
-        <v>576</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -11549,22 +11556,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="F43" t="s">
         <v>69</v>
       </c>
       <c r="G43" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="J43" s="4" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -11579,22 +11586,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="F44" t="s">
         <v>69</v>
       </c>
       <c r="G44" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="J44" s="4" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -11609,22 +11616,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D45" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="F45" t="s">
         <v>69</v>
       </c>
       <c r="G45" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="J45" s="4" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -11639,17 +11646,17 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D46" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="F46" t="s">
         <v>69</v>
       </c>
       <c r="G46" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="25" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="K46" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11668,22 +11675,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D47" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="F47" t="s">
         <v>69</v>
       </c>
       <c r="G47" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I47" s="4" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="J47" s="4" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="K47" s="4" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -11698,19 +11705,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D48" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="F48" t="s">
         <v>69</v>
       </c>
       <c r="G48" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="I48" s="4" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="J48" s="4" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="K48" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified "&amp;SUBSTITUTE(D48,","," and ")</f>
@@ -11729,19 +11736,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D49" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F49" t="s">
         <v>69</v>
       </c>
       <c r="G49" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="K49" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified "&amp;SUBSTITUTE(D49,","," and ")</f>
@@ -11756,22 +11763,22 @@
         <v>107</v>
       </c>
       <c r="C50" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D50" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F50" t="s">
         <v>69</v>
       </c>
       <c r="G50" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="J50" s="4" t="s">
-        <v>595</v>
+        <v>592</v>
       </c>
       <c r="K50" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified "&amp;SUBSTITUTE(D50,","," and ")</f>
@@ -11786,25 +11793,25 @@
         <v>107</v>
       </c>
       <c r="C51" t="s">
+        <v>590</v>
+      </c>
+      <c r="D51" t="s">
+        <v>556</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" t="s">
+        <v>491</v>
+      </c>
+      <c r="H51" t="s">
         <v>593</v>
       </c>
-      <c r="D51" t="s">
-        <v>559</v>
-      </c>
-      <c r="F51" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" t="s">
-        <v>494</v>
-      </c>
-      <c r="H51" t="s">
-        <v>596</v>
-      </c>
       <c r="I51" s="4" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="J51" s="26" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
       <c r="K51" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B51&amp;" resources for the specified patient and  a category code = `LAB`"</f>
@@ -11819,22 +11826,22 @@
         <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D52" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F52" t="s">
         <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="J52" s="26" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="K52" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B52&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11849,25 +11856,25 @@
         <v>107</v>
       </c>
       <c r="C53" t="s">
+        <v>590</v>
+      </c>
+      <c r="D53" t="s">
+        <v>598</v>
+      </c>
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s">
+        <v>599</v>
+      </c>
+      <c r="H53" t="s">
         <v>593</v>
       </c>
-      <c r="D53" t="s">
+      <c r="I53" s="4" t="s">
+        <v>600</v>
+      </c>
+      <c r="J53" s="26" t="s">
         <v>601</v>
-      </c>
-      <c r="F53" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" t="s">
-        <v>602</v>
-      </c>
-      <c r="H53" t="s">
-        <v>596</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>603</v>
-      </c>
-      <c r="J53" s="26" t="s">
-        <v>604</v>
       </c>
       <c r="K53" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B53&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -11886,17 +11893,17 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="D54" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="F54" t="s">
         <v>69</v>
       </c>
       <c r="G54" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="24" t="s">
-        <v>606</v>
+        <v>603</v>
       </c>
       <c r="K54" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified "&amp;SUBSTITUTE(D54,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11911,22 +11918,22 @@
         <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="D55" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="F55" t="s">
         <v>69</v>
       </c>
       <c r="G55" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="J55" s="4" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="K55" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B55&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11945,19 +11952,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D56" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="F56" t="s">
         <v>69</v>
       </c>
       <c r="G56" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I56" s="4" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="K56" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp;" resources for the specified "&amp;SUBSTITUTE(D56,","," and ")</f>
@@ -11976,19 +11983,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D57" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="F57" t="s">
         <v>69</v>
       </c>
       <c r="G57" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I57" s="4" t="s">
-        <v>614</v>
+        <v>611</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>615</v>
+        <v>612</v>
       </c>
       <c r="K57" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B57&amp;" resources for the specified "&amp;SUBSTITUTE(D57,","," and ")</f>
@@ -12007,25 +12014,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" t="s">
+        <v>613</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" t="s">
+        <v>491</v>
+      </c>
+      <c r="H58" t="s">
+        <v>614</v>
+      </c>
+      <c r="I58" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="J58" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="F58" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" t="s">
-        <v>494</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="K58" s="4" t="s">
         <v>617</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>618</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>619</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>620</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -12040,25 +12047,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D59" t="s">
+        <v>618</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>491</v>
+      </c>
+      <c r="H59" t="s">
+        <v>614</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>620</v>
+      </c>
+      <c r="K59" s="4" t="s">
         <v>621</v>
-      </c>
-      <c r="F59" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" t="s">
-        <v>494</v>
-      </c>
-      <c r="H59" t="s">
-        <v>617</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>622</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>623</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -12073,25 +12080,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D60" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="F60" t="s">
         <v>69</v>
       </c>
       <c r="G60" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H60" t="s">
-        <v>617</v>
+        <v>614</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="J60" s="4" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="K60" s="4" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -12106,25 +12113,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D61" t="s">
+        <v>625</v>
+      </c>
+      <c r="F61" t="s">
+        <v>69</v>
+      </c>
+      <c r="G61" t="s">
+        <v>599</v>
+      </c>
+      <c r="H61" t="s">
+        <v>614</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>626</v>
+      </c>
+      <c r="J61" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="K61" s="4" t="s">
         <v>628</v>
-      </c>
-      <c r="F61" t="s">
-        <v>69</v>
-      </c>
-      <c r="G61" t="s">
-        <v>602</v>
-      </c>
-      <c r="H61" t="s">
-        <v>617</v>
-      </c>
-      <c r="I61" s="4" t="s">
-        <v>629</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>630</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>631</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -12139,19 +12146,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D62" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F62" t="s">
         <v>69</v>
       </c>
       <c r="G62" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>633</v>
+        <v>630</v>
       </c>
       <c r="K62" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified "&amp;SUBSTITUTE(D62,","," and ")</f>
@@ -12170,22 +12177,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D63" t="s">
+        <v>631</v>
+      </c>
+      <c r="F63" t="s">
+        <v>69</v>
+      </c>
+      <c r="G63" t="s">
+        <v>512</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>632</v>
+      </c>
+      <c r="J63" s="4" t="s">
+        <v>633</v>
+      </c>
+      <c r="K63" s="4" t="s">
         <v>634</v>
-      </c>
-      <c r="F63" t="s">
-        <v>69</v>
-      </c>
-      <c r="G63" t="s">
-        <v>515</v>
-      </c>
-      <c r="I63" s="4" t="s">
-        <v>635</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>636</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>637</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -12200,19 +12207,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D64" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F64" t="s">
         <v>69</v>
       </c>
       <c r="G64" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>638</v>
+        <v>635</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>639</v>
+        <v>636</v>
       </c>
       <c r="K64" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified "&amp;SUBSTITUTE(D64,","," and ")</f>
@@ -12231,19 +12238,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D65" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="K65" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified "&amp;SUBSTITUTE(D65,","," and ")</f>
@@ -12262,19 +12269,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D66" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="F66" t="s">
         <v>69</v>
       </c>
       <c r="G66" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="K66" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -12289,28 +12296,28 @@
         <v>111</v>
       </c>
       <c r="C67" t="s">
+        <v>641</v>
+      </c>
+      <c r="D67" t="s">
+        <v>642</v>
+      </c>
+      <c r="F67" t="s">
+        <v>69</v>
+      </c>
+      <c r="G67" t="s">
+        <v>491</v>
+      </c>
+      <c r="H67" t="s">
+        <v>643</v>
+      </c>
+      <c r="I67" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="D67" t="s">
+      <c r="J67" s="4" t="s">
         <v>645</v>
       </c>
-      <c r="F67" t="s">
-        <v>69</v>
-      </c>
-      <c r="G67" t="s">
-        <v>494</v>
-      </c>
-      <c r="H67" t="s">
+      <c r="K67" s="4" t="s">
         <v>646</v>
-      </c>
-      <c r="I67" s="4" t="s">
-        <v>647</v>
-      </c>
-      <c r="J67" s="4" t="s">
-        <v>648</v>
-      </c>
-      <c r="K67" s="4" t="s">
-        <v>649</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -12321,25 +12328,25 @@
         <v>111</v>
       </c>
       <c r="C68" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D68" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="F68" t="s">
         <v>12</v>
       </c>
       <c r="G68" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H68" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="I68" s="4" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="K68" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -12354,22 +12361,22 @@
         <v>111</v>
       </c>
       <c r="C69" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D69" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F69" t="s">
         <v>12</v>
       </c>
       <c r="G69" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="J69" s="8" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="K69" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -12384,25 +12391,25 @@
         <v>111</v>
       </c>
       <c r="C70" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D70" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F70" t="s">
         <v>12</v>
       </c>
       <c r="G70" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H70" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="I70" s="4" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="K70" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -12417,20 +12424,20 @@
         <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D71" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="F71" t="s">
         <v>69</v>
       </c>
       <c r="G71" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="24" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K71" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -12445,22 +12452,22 @@
         <v>111</v>
       </c>
       <c r="C72" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="D72" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="F72" t="s">
         <v>69</v>
       </c>
       <c r="G72" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12478,22 +12485,22 @@
         <v>128</v>
       </c>
       <c r="D73" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="F73" t="s">
         <v>12</v>
       </c>
       <c r="G73" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H73" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="I73" s="4" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="J73" s="4" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="K73" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified "&amp;SUBSTITUTE(D73,","," and ")&amp;"=`assess-plan`"</f>
@@ -12511,25 +12518,25 @@
         <v>128</v>
       </c>
       <c r="D74" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F74" t="s">
         <v>69</v>
       </c>
       <c r="G74" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H74" t="s">
+        <v>656</v>
+      </c>
+      <c r="I74" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="I74" s="4" t="s">
-        <v>662</v>
-      </c>
       <c r="J74" s="4" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="K74" s="4" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -12543,25 +12550,25 @@
         <v>128</v>
       </c>
       <c r="D75" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="F75" t="s">
         <v>69</v>
       </c>
       <c r="G75" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H75" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="I75" s="4" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="J75" s="4" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="K75" s="4" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -12575,25 +12582,25 @@
         <v>128</v>
       </c>
       <c r="D76" t="s">
+        <v>665</v>
+      </c>
+      <c r="F76" t="s">
+        <v>69</v>
+      </c>
+      <c r="G76" t="s">
+        <v>599</v>
+      </c>
+      <c r="H76" t="s">
+        <v>656</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>666</v>
+      </c>
+      <c r="J76" s="4" t="s">
+        <v>667</v>
+      </c>
+      <c r="K76" s="4" t="s">
         <v>668</v>
-      </c>
-      <c r="F76" t="s">
-        <v>69</v>
-      </c>
-      <c r="G76" t="s">
-        <v>602</v>
-      </c>
-      <c r="H76" t="s">
-        <v>659</v>
-      </c>
-      <c r="I76" s="4" t="s">
-        <v>669</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>670</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>671</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="136" x14ac:dyDescent="0.2">
@@ -12608,25 +12615,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D77" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F77" t="s">
         <v>12</v>
       </c>
       <c r="G77" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H77" t="s">
+        <v>669</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>670</v>
+      </c>
+      <c r="J77" s="4" t="s">
+        <v>671</v>
+      </c>
+      <c r="K77" s="8" t="s">
         <v>672</v>
-      </c>
-      <c r="I77" s="4" t="s">
-        <v>673</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>674</v>
-      </c>
-      <c r="K77" s="8" t="s">
-        <v>675</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -12641,19 +12648,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D78" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F78" t="s">
         <v>69</v>
       </c>
       <c r="G78" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="J78" s="4" t="s">
-        <v>677</v>
+        <v>674</v>
       </c>
       <c r="K78" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B78&amp;" resources for the specified "&amp;SUBSTITUTE(D78,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -12665,23 +12672,23 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>678</v>
+        <v>675</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D79" t="s">
-        <v>679</v>
+        <v>676</v>
       </c>
       <c r="F79" t="s">
         <v>69</v>
       </c>
       <c r="G79" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>676</v>
+        <v>673</v>
       </c>
       <c r="J79" s="4"/>
       <c r="K79" s="4" t="str">
@@ -12701,25 +12708,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D80" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="F80" t="s">
         <v>12</v>
       </c>
       <c r="G80" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H80" t="s">
+        <v>677</v>
+      </c>
+      <c r="I80" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="J80" s="4" t="s">
+        <v>679</v>
+      </c>
+      <c r="K80" s="4" t="s">
         <v>680</v>
-      </c>
-      <c r="I80" s="4" t="s">
-        <v>681</v>
-      </c>
-      <c r="J80" s="4" t="s">
-        <v>682</v>
-      </c>
-      <c r="K80" s="4" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12734,25 +12741,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="F81" t="s">
         <v>12</v>
       </c>
       <c r="G81" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H81" t="s">
-        <v>680</v>
+        <v>677</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>684</v>
+        <v>681</v>
       </c>
       <c r="J81" s="26" t="s">
-        <v>685</v>
+        <v>682</v>
       </c>
       <c r="K81" s="4" t="s">
-        <v>686</v>
+        <v>683</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -12767,22 +12774,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D82" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="F82" t="s">
         <v>12</v>
       </c>
       <c r="G82" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>687</v>
+        <v>684</v>
       </c>
       <c r="J82" s="4" t="s">
-        <v>688</v>
+        <v>685</v>
       </c>
       <c r="K82" s="4" t="s">
-        <v>689</v>
+        <v>686</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12797,19 +12804,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D83" t="s">
-        <v>690</v>
+        <v>687</v>
       </c>
       <c r="F83" t="s">
         <v>69</v>
       </c>
       <c r="G83" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>691</v>
+        <v>688</v>
       </c>
       <c r="J83" s="4" t="s">
-        <v>692</v>
+        <v>689</v>
       </c>
       <c r="K83" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -12824,25 +12831,25 @@
         <v>130</v>
       </c>
       <c r="C84" t="s">
+        <v>690</v>
+      </c>
+      <c r="D84" t="s">
+        <v>506</v>
+      </c>
+      <c r="F84" t="s">
+        <v>69</v>
+      </c>
+      <c r="G84" t="s">
+        <v>491</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>691</v>
+      </c>
+      <c r="J84" s="4" t="s">
+        <v>692</v>
+      </c>
+      <c r="K84" s="4" t="s">
         <v>693</v>
-      </c>
-      <c r="D84" t="s">
-        <v>509</v>
-      </c>
-      <c r="F84" t="s">
-        <v>69</v>
-      </c>
-      <c r="G84" t="s">
-        <v>494</v>
-      </c>
-      <c r="I84" s="4" t="s">
-        <v>694</v>
-      </c>
-      <c r="J84" s="4" t="s">
-        <v>695</v>
-      </c>
-      <c r="K84" s="4" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -12853,25 +12860,25 @@
         <v>130</v>
       </c>
       <c r="C85" t="s">
-        <v>693</v>
+        <v>690</v>
       </c>
       <c r="D85" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F85" t="s">
         <v>69</v>
       </c>
       <c r="G85" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I85" s="4" t="s">
-        <v>697</v>
+        <v>694</v>
       </c>
       <c r="J85" s="4" t="s">
-        <v>698</v>
+        <v>695</v>
       </c>
       <c r="K85" s="4" t="s">
-        <v>699</v>
+        <v>696</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -12886,22 +12893,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D86" t="s">
+        <v>697</v>
+      </c>
+      <c r="F86" t="s">
+        <v>69</v>
+      </c>
+      <c r="G86" t="s">
+        <v>491</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>698</v>
+      </c>
+      <c r="J86" s="4" t="s">
+        <v>699</v>
+      </c>
+      <c r="K86" s="4" t="s">
         <v>700</v>
-      </c>
-      <c r="F86" t="s">
-        <v>69</v>
-      </c>
-      <c r="G86" t="s">
-        <v>494</v>
-      </c>
-      <c r="I86" s="4" t="s">
-        <v>701</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>702</v>
-      </c>
-      <c r="K86" s="4" t="s">
-        <v>703</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -12916,19 +12923,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F87" t="s">
         <v>69</v>
       </c>
       <c r="G87" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>704</v>
+        <v>701</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>705</v>
+        <v>702</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified "&amp;SUBSTITUTE(D87,","," and ")</f>
@@ -12947,19 +12954,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D88" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="F88" t="s">
         <v>12</v>
       </c>
       <c r="G88" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>706</v>
+        <v>703</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified patient and  a category code"</f>
@@ -12978,19 +12985,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D89" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="F89" t="s">
         <v>12</v>
       </c>
       <c r="G89" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -13009,19 +13016,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D90" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="F90" t="s">
         <v>12</v>
       </c>
       <c r="G90" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="I90" s="4" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="J90" s="4" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="K90" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified patient and date and a category code"</f>
@@ -13040,19 +13047,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D91" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="F91" t="s">
         <v>69</v>
       </c>
       <c r="G91" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="I91" s="4" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="J91" s="4" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -13071,19 +13078,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D92" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="F92" t="s">
         <v>69</v>
       </c>
       <c r="G92" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I92" s="4" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="J92" s="4" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="K92" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -13102,19 +13109,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D93" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F93" t="s">
         <v>69</v>
       </c>
       <c r="G93" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="I93" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="K93" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
@@ -13133,22 +13140,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D94" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="F94" t="s">
         <v>69</v>
       </c>
       <c r="G94" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H94" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="I94" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="J94" s="4" t="s">
-        <v>723</v>
+        <v>720</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified "&amp;SUBSTITUTE(D94,","," and  ") &amp; "= 'sdoh'"</f>
@@ -13167,19 +13174,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D95" t="s">
-        <v>724</v>
+        <v>721</v>
       </c>
       <c r="F95" t="s">
         <v>69</v>
       </c>
       <c r="G95" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="I95" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>725</v>
+        <v>722</v>
       </c>
       <c r="K95" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date"</f>
@@ -13198,22 +13205,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>726</v>
+        <v>723</v>
       </c>
       <c r="F96" t="s">
         <v>69</v>
       </c>
       <c r="G96" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="H96" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="I96" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>727</v>
+        <v>724</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -13232,7 +13239,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>728</v>
+        <v>725</v>
       </c>
       <c r="F97" t="s">
         <v>69</v>
@@ -13241,10 +13248,10 @@
         <v>89</v>
       </c>
       <c r="I97" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>729</v>
+        <v>726</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -13263,21 +13270,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="E98" s="16"/>
       <c r="F98" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G98" s="16" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4" t="s">
-        <v>730</v>
+        <v>727</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>731</v>
+        <v>728</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -13296,21 +13303,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="E99" s="16"/>
       <c r="F99" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G99" s="16" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H99" s="16"/>
       <c r="I99" s="4" t="s">
-        <v>732</v>
+        <v>729</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>733</v>
+        <v>730</v>
       </c>
       <c r="K99" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -13329,21 +13336,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>734</v>
+        <v>731</v>
       </c>
       <c r="E100" s="16"/>
       <c r="F100" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G100" s="16" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="H100" s="16"/>
       <c r="I100" s="4" t="s">
-        <v>735</v>
+        <v>732</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>736</v>
+        <v>733</v>
       </c>
       <c r="K100" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -13361,19 +13368,19 @@
         <v>348</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>737</v>
+        <v>734</v>
       </c>
       <c r="E101" s="16"/>
       <c r="F101" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G101" s="16" t="s">
-        <v>738</v>
+        <v>735</v>
       </c>
       <c r="H101" s="16"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4" t="s">
-        <v>739</v>
+        <v>736</v>
       </c>
       <c r="K101" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13400,7 +13407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -13431,7 +13438,7 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>461</v>
+        <v>738</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13447,7 +13454,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>462</v>
+        <v>739</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -14540,8 +14547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y69"/>
   <sheetViews>
-    <sheetView topLeftCell="T19" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="W25" sqref="W25"/>
+    <sheetView topLeftCell="A31" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -14691,7 +14698,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="T4" t="s">
         <v>19</v>
@@ -14786,7 +14793,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>464</v>
+        <v>462</v>
       </c>
       <c r="T8" t="s">
         <v>19</v>
@@ -14809,7 +14816,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14832,7 +14839,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>466</v>
+        <v>464</v>
       </c>
       <c r="T10" t="s">
         <v>19</v>
@@ -14939,7 +14946,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="T15" t="s">
         <v>19</v>
@@ -14996,7 +15003,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="T18" t="s">
         <v>19</v>
@@ -15025,7 +15032,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="T19" t="s">
         <v>19</v>
@@ -15083,7 +15090,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>467</v>
+        <v>465</v>
       </c>
       <c r="T21" t="s">
         <v>19</v>
@@ -15106,7 +15113,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="T22" t="s">
         <v>19</v>
@@ -15125,7 +15132,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="T23" t="s">
         <v>19</v>
@@ -15148,7 +15155,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="T24" t="s">
         <v>19</v>
@@ -15192,7 +15199,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="T26" t="s">
         <v>19</v>
@@ -15232,7 +15239,7 @@
         <v>69</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -15245,7 +15252,7 @@
         <v>69</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>262</v>
@@ -15262,7 +15269,7 @@
         <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="T30" t="s">
         <v>19</v>
@@ -15277,15 +15284,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:25" ht="225" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:25" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>340</v>
       </c>
       <c r="B31" t="s">
         <v>12</v>
       </c>
-      <c r="C31" s="1" t="s">
-        <v>474</v>
+      <c r="C31" s="2" t="s">
+        <v>737</v>
       </c>
       <c r="T31" t="s">
         <v>19</v>
@@ -15308,7 +15315,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="T32" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
pre-apply FHIR-48442 Update Must Support Resource References section in general and for Observation.performer targets
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{148F263E-9157-704F-A063-2EF60F27DBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55E2116-3F0A-7B4C-A3FF-8C8E481CB8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19640" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19640" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -2716,7 +2716,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2757,6 +2757,7 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -3155,7 +3156,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13407,7 +13408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -13644,8 +13645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14235,7 +14236,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="28" t="s">
         <v>288</v>
       </c>
       <c r="B42" t="s">

</xml_diff>

<commit_message>
Make Must Support Reference Table more visible FHIR-44977 add MS=False flag to QuestionnaireResponse.authored target FHIR-48847 add MS=False flags to Procedure.basedOn targets FHIR-48848 Update Condition.code ICD9 value set link and add STU Note FHIR-45136 Update Change log
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55E2116-3F0A-7B4C-A3FF-8C8E481CB8E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3812D082-1B4D-1F4B-AAD0-4EC24EE75A6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19640" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53720" yWindow="500" windowWidth="26440" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1550,24 +1550,6 @@
     <t>* Due to implementer feedback, some US Core Profiles reference the PractitionerRole resource instead of the US Core PractitionerRole Profile. However the US Core PractitionerRole Profile **SHOULD** be used as the default profile if referenced by another US Core profile.</t>
   </si>
   <si>
-    <t xml:space="preserve">The US Core Server **SHALL**:
-1. Support the US Core Patient resource profile AND at least one additional resource profile from the list of US Core Profiles AND and all Must Support US Core Profiles and resources it references.
-     - The [Table below](#ms-ref-table) summarizes the Must Support references to other US Core Profiles and FHIR resources for each US Core Profile:
-1. Implement the RESTful behavior according to the FHIR specification.
-1. Follow the requirements documented in the [General Requirements](general-requirements.html) and [Must Support](must-support.html) pages
-1. Return the following response classes:
-   - (Status 400): invalid parameter
-   - (Status 401/4xx): unauthorized request
-   - (Status 403): insufficient scopes
-   - (Status 404): unknown resource
-1. Support JSON source formats for all US Core interactions.
-The US Core Server **SHOULD**:
-1. Follow the guidance documented in the [General Guidance](general-guidance.html) page
-1. Support XML source formats for all US Core interactions.
-1. Identify the US Core profiles supported as part of the FHIR `meta.profile` attribute for each instance.
-</t>
-  </si>
-  <si>
     <t>_lastUpdated</t>
   </si>
   <si>
@@ -2541,6 +2523,23 @@
   </si>
   <si>
     <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ONC 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and the ONC [U.S. Core Data for Interoperability (USCDI) Version 5 July 2024](https://www.healthit.gov/isp/sites/isp/files/2024-07/USCDI-Version-5-July-2024-Final.pdf).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The US Core Server **SHALL**:
+1. Support the US Core Patient resource profile AND at least one additional resource profile from the list of US Core Profiles AND and all *Must Support* US Core Profiles and resources it references.
+     -  A summary table listing all the *Must Support* references to other US Core Profiles and FHIR resources for each US Core Profile is located in the [Must Support - Resource References](must-support.html#must-support---resource-references) section of the guide.
+1. Follow the requirements documented in the [General Requirements](general-requirements.html) and [Must Support](must-support.html) pages
+1. Return the following response classes:
+   - (Status 400): invalid parameter
+   - (Status 401/4xx): unauthorized request
+   - (Status 403): insufficient scopes
+   - (Status 404): unknown resource
+1. Support JSON source formats for all US Core interactions.
+The US Core Server **SHOULD**:
+1. Follow the guidance documented in the [General Guidance](general-guidance.html) page
+1. Support XML source formats for all US Core interactions.
+1. Identify the US Core profiles supported as part of the FHIR `meta.profile` attribute for each instance.
+</t>
   </si>
 </sst>
 </file>
@@ -2716,7 +2715,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2757,7 +2756,6 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -5554,7 +5552,7 @@
         <v>93</v>
       </c>
       <c r="C44" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D44" t="s">
         <v>30</v>
@@ -5563,7 +5561,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" ref="G44" si="5">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B44)</f>
@@ -5983,7 +5981,7 @@
         <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D52" t="s">
         <v>30</v>
@@ -5992,7 +5990,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="4"/>
@@ -6680,7 +6678,7 @@
         <v>22</v>
       </c>
       <c r="C65" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D65" t="s">
         <v>30</v>
@@ -6689,7 +6687,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="4"/>
@@ -8287,7 +8285,7 @@
         <v>111</v>
       </c>
       <c r="C95" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="D95" t="s">
         <v>30</v>
@@ -8296,7 +8294,7 @@
         <v>0</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="G95" t="str">
         <f t="shared" ref="G95" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B95)</f>
@@ -10366,7 +10364,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>37</v>
@@ -10375,19 +10373,19 @@
         <v>39</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>333</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>479</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>480</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>481</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>482</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
@@ -10404,20 +10402,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C49" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D2" t="s">
+        <v>483</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
         <v>484</v>
-      </c>
-      <c r="F2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" t="s">
-        <v>485</v>
       </c>
       <c r="K2" s="4" t="str">
         <f t="shared" ref="K2:K17" si="1">"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
@@ -10429,20 +10427,20 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D3" t="s">
+        <v>485</v>
+      </c>
+      <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
         <v>486</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" t="s">
-        <v>487</v>
       </c>
       <c r="K3" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10454,20 +10452,20 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D4" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F4" t="s">
         <v>69</v>
       </c>
       <c r="G4" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K4" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10479,20 +10477,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="F5" t="s">
         <v>69</v>
       </c>
       <c r="G5" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K5" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10511,19 +10509,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D6" t="s">
+        <v>489</v>
+      </c>
+      <c r="F6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G6" t="s">
         <v>490</v>
       </c>
-      <c r="F6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>491</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>492</v>
-      </c>
-      <c r="J6" t="s">
-        <v>493</v>
       </c>
       <c r="K6" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10535,20 +10533,20 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D7" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F7" t="s">
         <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K7" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10560,20 +10558,20 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D8" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="F8" t="s">
         <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="K8" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10585,20 +10583,20 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D9" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="F9" t="s">
         <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="str">
@@ -10611,14 +10609,14 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D10" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="F10" t="s">
         <v>69</v>
@@ -10638,14 +10636,14 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D11" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="F11" t="s">
         <v>69</v>
@@ -10664,14 +10662,14 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D12" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F12" t="s">
         <v>69</v>
@@ -10696,19 +10694,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D13" t="s">
+        <v>499</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
         <v>500</v>
       </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="I13" s="4" t="s">
         <v>501</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" t="s">
         <v>502</v>
-      </c>
-      <c r="J13" t="s">
-        <v>503</v>
       </c>
       <c r="K13" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10720,20 +10718,20 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D14" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="F14" t="s">
         <v>69</v>
       </c>
       <c r="G14" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="K14" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10745,20 +10743,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D15" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F15" t="s">
         <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="K15" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10777,19 +10775,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D16" t="s">
+        <v>505</v>
+      </c>
+      <c r="F16" t="s">
+        <v>69</v>
+      </c>
+      <c r="G16" t="s">
+        <v>490</v>
+      </c>
+      <c r="I16" t="s">
         <v>506</v>
       </c>
-      <c r="F16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" t="s">
-        <v>491</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>507</v>
-      </c>
-      <c r="J16" t="s">
-        <v>508</v>
       </c>
       <c r="K16" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10808,7 +10806,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F17" t="s">
         <v>69</v>
@@ -10817,10 +10815,10 @@
         <v>89</v>
       </c>
       <c r="I17" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="J17" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -10839,17 +10837,17 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" t="s">
+        <v>510</v>
+      </c>
+      <c r="F18" t="s">
+        <v>69</v>
+      </c>
+      <c r="G18" t="s">
         <v>511</v>
-      </c>
-      <c r="F18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" t="s">
-        <v>512</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="24" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="K18" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B18&amp;" resources for the specified "&amp;SUBSTITUTE(D18,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -10861,20 +10859,20 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D19" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="F19" t="s">
         <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="str">
@@ -10894,19 +10892,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
+        <v>514</v>
+      </c>
+      <c r="F20" t="s">
+        <v>69</v>
+      </c>
+      <c r="G20" t="s">
+        <v>490</v>
+      </c>
+      <c r="I20" t="s">
         <v>515</v>
       </c>
-      <c r="F20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" t="s">
-        <v>491</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>516</v>
-      </c>
-      <c r="J20" t="s">
-        <v>517</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="2"/>
@@ -10925,19 +10923,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D21" t="s">
+        <v>517</v>
+      </c>
+      <c r="F21" t="s">
+        <v>69</v>
+      </c>
+      <c r="G21" t="s">
+        <v>490</v>
+      </c>
+      <c r="I21" t="s">
+        <v>515</v>
+      </c>
+      <c r="J21" t="s">
         <v>518</v>
-      </c>
-      <c r="F21" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" t="s">
-        <v>491</v>
-      </c>
-      <c r="I21" t="s">
-        <v>516</v>
-      </c>
-      <c r="J21" t="s">
-        <v>519</v>
       </c>
       <c r="K21" s="4" t="str">
         <f t="shared" si="2"/>
@@ -10949,14 +10947,14 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D22" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F22" t="s">
         <v>69</v>
@@ -10976,20 +10974,20 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D23" t="s">
+        <v>521</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+      <c r="G23" t="s">
         <v>522</v>
-      </c>
-      <c r="F23" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" t="s">
-        <v>523</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="str">
@@ -11002,20 +11000,20 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D24" t="s">
+        <v>523</v>
+      </c>
+      <c r="F24" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" t="s">
         <v>524</v>
-      </c>
-      <c r="F24" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" t="s">
-        <v>525</v>
       </c>
       <c r="K24" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11027,20 +11025,20 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D25" t="s">
+        <v>525</v>
+      </c>
+      <c r="F25" t="s">
+        <v>69</v>
+      </c>
+      <c r="G25" t="s">
         <v>526</v>
-      </c>
-      <c r="F25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" t="s">
-        <v>527</v>
       </c>
       <c r="I25" s="4"/>
       <c r="K25" s="4" t="str">
@@ -11053,20 +11051,20 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D26" t="s">
+        <v>527</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
         <v>528</v>
-      </c>
-      <c r="F26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" t="s">
-        <v>529</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -11080,20 +11078,20 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D27" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F27" t="s">
         <v>69</v>
       </c>
       <c r="G27" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -11107,20 +11105,20 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D28" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="F28" t="s">
         <v>69</v>
       </c>
       <c r="G28" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -11134,20 +11132,20 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D29" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="F29" t="s">
         <v>69</v>
       </c>
       <c r="G29" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K29" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11159,14 +11157,14 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D30" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="F30" t="s">
         <v>69</v>
@@ -11184,20 +11182,20 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D31" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F31" t="s">
         <v>69</v>
       </c>
       <c r="G31" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="K31" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11216,19 +11214,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
+        <v>534</v>
+      </c>
+      <c r="F32" t="s">
+        <v>69</v>
+      </c>
+      <c r="G32" t="s">
         <v>535</v>
       </c>
-      <c r="F32" t="s">
-        <v>69</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="I32" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="J32" s="4" t="s">
         <v>537</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>538</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11247,19 +11245,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D33" t="s">
+        <v>538</v>
+      </c>
+      <c r="F33" t="s">
+        <v>69</v>
+      </c>
+      <c r="G33" t="s">
+        <v>535</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="F33" t="s">
-        <v>69</v>
-      </c>
-      <c r="G33" t="s">
-        <v>536</v>
-      </c>
-      <c r="I33" s="4" t="s">
+      <c r="J33" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>541</v>
       </c>
       <c r="K33" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11278,19 +11276,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D34" t="s">
+        <v>541</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>535</v>
+      </c>
+      <c r="I34" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="F34" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" t="s">
-        <v>536</v>
-      </c>
-      <c r="I34" s="4" t="s">
+      <c r="J34" s="4" t="s">
         <v>543</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>544</v>
       </c>
       <c r="K34" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11309,19 +11307,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D35" t="s">
+        <v>544</v>
+      </c>
+      <c r="F35" t="s">
+        <v>69</v>
+      </c>
+      <c r="G35" t="s">
+        <v>528</v>
+      </c>
+      <c r="I35" s="4" t="s">
         <v>545</v>
       </c>
-      <c r="F35" t="s">
-        <v>69</v>
-      </c>
-      <c r="G35" t="s">
-        <v>529</v>
-      </c>
-      <c r="I35" s="4" t="s">
+      <c r="J35" s="4" t="s">
         <v>546</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>547</v>
       </c>
       <c r="K35" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11340,19 +11338,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D36" t="s">
+        <v>547</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>528</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>548</v>
       </c>
-      <c r="F36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" t="s">
-        <v>529</v>
-      </c>
-      <c r="I36" s="4" t="s">
+      <c r="J36" s="4" t="s">
         <v>549</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>550</v>
       </c>
       <c r="K36" s="4" t="str">
         <f t="shared" si="2"/>
@@ -11371,25 +11369,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" t="s">
+        <v>550</v>
+      </c>
+      <c r="F37" t="s">
+        <v>69</v>
+      </c>
+      <c r="G37" t="s">
+        <v>490</v>
+      </c>
+      <c r="H37" t="s">
         <v>551</v>
       </c>
-      <c r="F37" t="s">
-        <v>69</v>
-      </c>
-      <c r="G37" t="s">
-        <v>491</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="I37" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="J37" s="4" t="s">
         <v>553</v>
       </c>
-      <c r="J37" s="4" t="s">
+      <c r="K37" s="4" t="s">
         <v>554</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
@@ -11404,22 +11402,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
+        <v>555</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>490</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="F38" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" t="s">
-        <v>491</v>
-      </c>
-      <c r="I38" s="4" t="s">
+      <c r="J38" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="J38" s="4" t="s">
+      <c r="K38" s="4" t="s">
         <v>558</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>559</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -11434,25 +11432,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
+        <v>559</v>
+      </c>
+      <c r="F39" t="s">
+        <v>69</v>
+      </c>
+      <c r="G39" t="s">
+        <v>490</v>
+      </c>
+      <c r="H39" t="s">
+        <v>551</v>
+      </c>
+      <c r="I39" s="4" t="s">
         <v>560</v>
       </c>
-      <c r="F39" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" t="s">
-        <v>491</v>
-      </c>
-      <c r="H39" t="s">
-        <v>552</v>
-      </c>
-      <c r="I39" s="4" t="s">
+      <c r="J39" s="25" t="s">
         <v>561</v>
       </c>
-      <c r="J39" s="25" t="s">
+      <c r="K39" s="4" t="s">
         <v>562</v>
-      </c>
-      <c r="K39" s="4" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
@@ -11467,22 +11465,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" t="s">
+        <v>563</v>
+      </c>
+      <c r="F40" t="s">
+        <v>69</v>
+      </c>
+      <c r="G40" t="s">
+        <v>490</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>556</v>
+      </c>
+      <c r="J40" s="4" t="s">
         <v>564</v>
       </c>
-      <c r="F40" t="s">
-        <v>69</v>
-      </c>
-      <c r="G40" t="s">
-        <v>491</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>557</v>
-      </c>
-      <c r="J40" s="4" t="s">
+      <c r="K40" s="4" t="s">
         <v>565</v>
-      </c>
-      <c r="K40" s="4" t="s">
-        <v>566</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
@@ -11497,22 +11495,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
+        <v>566</v>
+      </c>
+      <c r="F41" t="s">
+        <v>69</v>
+      </c>
+      <c r="G41" t="s">
+        <v>490</v>
+      </c>
+      <c r="I41" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="F41" t="s">
-        <v>69</v>
-      </c>
-      <c r="G41" t="s">
-        <v>491</v>
-      </c>
-      <c r="I41" s="4" t="s">
+      <c r="J41" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="J41" s="4" t="s">
+      <c r="K41" s="4" t="s">
         <v>569</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>570</v>
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
@@ -11527,22 +11525,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
+        <v>570</v>
+      </c>
+      <c r="F42" t="s">
+        <v>69</v>
+      </c>
+      <c r="G42" t="s">
+        <v>511</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>571</v>
       </c>
-      <c r="F42" t="s">
-        <v>69</v>
-      </c>
-      <c r="G42" t="s">
-        <v>512</v>
-      </c>
-      <c r="I42" s="4" t="s">
+      <c r="J42" s="4" t="s">
         <v>572</v>
       </c>
-      <c r="J42" s="4" t="s">
+      <c r="K42" s="4" t="s">
         <v>573</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
@@ -11557,22 +11555,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
+        <v>574</v>
+      </c>
+      <c r="F43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G43" t="s">
+        <v>511</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="J43" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="F43" t="s">
-        <v>69</v>
-      </c>
-      <c r="G43" t="s">
-        <v>512</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="J43" s="4" t="s">
-        <v>576</v>
-      </c>
       <c r="K43" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
@@ -11587,22 +11585,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
+        <v>576</v>
+      </c>
+      <c r="F44" t="s">
+        <v>69</v>
+      </c>
+      <c r="G44" t="s">
+        <v>511</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="J44" s="4" t="s">
         <v>577</v>
       </c>
-      <c r="F44" t="s">
-        <v>69</v>
-      </c>
-      <c r="G44" t="s">
-        <v>512</v>
-      </c>
-      <c r="I44" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="J44" s="4" t="s">
-        <v>578</v>
-      </c>
       <c r="K44" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
@@ -11617,22 +11615,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D45" t="s">
+        <v>578</v>
+      </c>
+      <c r="F45" t="s">
+        <v>69</v>
+      </c>
+      <c r="G45" t="s">
+        <v>511</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>571</v>
+      </c>
+      <c r="J45" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="F45" t="s">
-        <v>69</v>
-      </c>
-      <c r="G45" t="s">
-        <v>512</v>
-      </c>
-      <c r="I45" s="4" t="s">
-        <v>572</v>
-      </c>
-      <c r="J45" s="4" t="s">
-        <v>580</v>
-      </c>
       <c r="K45" s="4" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -11647,17 +11645,17 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D46" t="s">
+        <v>510</v>
+      </c>
+      <c r="F46" t="s">
+        <v>69</v>
+      </c>
+      <c r="G46" t="s">
         <v>511</v>
-      </c>
-      <c r="F46" t="s">
-        <v>69</v>
-      </c>
-      <c r="G46" t="s">
-        <v>512</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="25" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="K46" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11676,22 +11674,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D47" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="F47" t="s">
         <v>69</v>
       </c>
       <c r="G47" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I47" s="4" t="s">
+        <v>581</v>
+      </c>
+      <c r="J47" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="K47" s="4" t="s">
         <v>583</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -11706,19 +11704,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D48" t="s">
+        <v>584</v>
+      </c>
+      <c r="F48" t="s">
+        <v>69</v>
+      </c>
+      <c r="G48" t="s">
+        <v>500</v>
+      </c>
+      <c r="I48" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="F48" t="s">
-        <v>69</v>
-      </c>
-      <c r="G48" t="s">
-        <v>501</v>
-      </c>
-      <c r="I48" s="4" t="s">
+      <c r="J48" s="4" t="s">
         <v>586</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>587</v>
       </c>
       <c r="K48" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified "&amp;SUBSTITUTE(D48,","," and ")</f>
@@ -11737,19 +11735,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D49" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F49" t="s">
         <v>69</v>
       </c>
       <c r="G49" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I49" s="4" t="s">
+        <v>587</v>
+      </c>
+      <c r="J49" s="4" t="s">
         <v>588</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>589</v>
       </c>
       <c r="K49" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified "&amp;SUBSTITUTE(D49,","," and ")</f>
@@ -11764,22 +11762,22 @@
         <v>107</v>
       </c>
       <c r="C50" t="s">
+        <v>589</v>
+      </c>
+      <c r="D50" t="s">
+        <v>514</v>
+      </c>
+      <c r="F50" t="s">
+        <v>69</v>
+      </c>
+      <c r="G50" t="s">
+        <v>490</v>
+      </c>
+      <c r="I50" s="4" t="s">
         <v>590</v>
       </c>
-      <c r="D50" t="s">
-        <v>515</v>
-      </c>
-      <c r="F50" t="s">
-        <v>69</v>
-      </c>
-      <c r="G50" t="s">
-        <v>491</v>
-      </c>
-      <c r="I50" s="4" t="s">
+      <c r="J50" s="4" t="s">
         <v>591</v>
-      </c>
-      <c r="J50" s="4" t="s">
-        <v>592</v>
       </c>
       <c r="K50" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B50&amp;" resources for the specified "&amp;SUBSTITUTE(D50,","," and ")</f>
@@ -11794,25 +11792,25 @@
         <v>107</v>
       </c>
       <c r="C51" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D51" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F51" t="s">
         <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H51" t="s">
+        <v>592</v>
+      </c>
+      <c r="I51" s="4" t="s">
         <v>593</v>
       </c>
-      <c r="I51" s="4" t="s">
+      <c r="J51" s="26" t="s">
         <v>594</v>
-      </c>
-      <c r="J51" s="26" t="s">
-        <v>595</v>
       </c>
       <c r="K51" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B51&amp;" resources for the specified patient and  a category code = `LAB`"</f>
@@ -11827,22 +11825,22 @@
         <v>107</v>
       </c>
       <c r="C52" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D52" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F52" t="s">
         <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I52" s="4" t="s">
+        <v>595</v>
+      </c>
+      <c r="J52" s="26" t="s">
         <v>596</v>
-      </c>
-      <c r="J52" s="26" t="s">
-        <v>597</v>
       </c>
       <c r="K52" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B52&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11857,25 +11855,25 @@
         <v>107</v>
       </c>
       <c r="C53" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D53" t="s">
+        <v>597</v>
+      </c>
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s">
         <v>598</v>
       </c>
-      <c r="F53" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
+        <v>592</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>599</v>
       </c>
-      <c r="H53" t="s">
-        <v>593</v>
-      </c>
-      <c r="I53" s="4" t="s">
+      <c r="J53" s="26" t="s">
         <v>600</v>
-      </c>
-      <c r="J53" s="26" t="s">
-        <v>601</v>
       </c>
       <c r="K53" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B53&amp;" resources for the specified patient and date and a category code = `LAB`"</f>
@@ -11894,17 +11892,17 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="D54" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F54" t="s">
         <v>69</v>
       </c>
       <c r="G54" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="24" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="K54" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B54&amp;" resources for the specified "&amp;SUBSTITUTE(D54,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -11919,22 +11917,22 @@
         <v>107</v>
       </c>
       <c r="C55" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
       <c r="D55" t="s">
+        <v>603</v>
+      </c>
+      <c r="F55" t="s">
+        <v>69</v>
+      </c>
+      <c r="G55" t="s">
+        <v>598</v>
+      </c>
+      <c r="I55" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="F55" t="s">
-        <v>69</v>
-      </c>
-      <c r="G55" t="s">
-        <v>599</v>
-      </c>
-      <c r="I55" s="4" t="s">
+      <c r="J55" s="4" t="s">
         <v>605</v>
-      </c>
-      <c r="J55" s="4" t="s">
-        <v>606</v>
       </c>
       <c r="K55" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B55&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -11953,19 +11951,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D56" t="s">
+        <v>606</v>
+      </c>
+      <c r="F56" t="s">
+        <v>69</v>
+      </c>
+      <c r="G56" t="s">
+        <v>490</v>
+      </c>
+      <c r="I56" s="4" t="s">
         <v>607</v>
       </c>
-      <c r="F56" t="s">
-        <v>69</v>
-      </c>
-      <c r="G56" t="s">
-        <v>491</v>
-      </c>
-      <c r="I56" s="4" t="s">
+      <c r="J56" s="4" t="s">
         <v>608</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>609</v>
       </c>
       <c r="K56" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp;" resources for the specified "&amp;SUBSTITUTE(D56,","," and ")</f>
@@ -11984,19 +11982,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D57" t="s">
+        <v>609</v>
+      </c>
+      <c r="F57" t="s">
+        <v>69</v>
+      </c>
+      <c r="G57" t="s">
+        <v>511</v>
+      </c>
+      <c r="I57" s="4" t="s">
         <v>610</v>
       </c>
-      <c r="F57" t="s">
-        <v>69</v>
-      </c>
-      <c r="G57" t="s">
-        <v>512</v>
-      </c>
-      <c r="I57" s="4" t="s">
+      <c r="J57" s="4" t="s">
         <v>611</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>612</v>
       </c>
       <c r="K57" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B57&amp;" resources for the specified "&amp;SUBSTITUTE(D57,","," and ")</f>
@@ -12015,25 +12013,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" t="s">
+        <v>612</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" t="s">
+        <v>490</v>
+      </c>
+      <c r="H58" t="s">
         <v>613</v>
       </c>
-      <c r="F58" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" t="s">
-        <v>491</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="I58" s="4" t="s">
         <v>614</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="J58" s="4" t="s">
         <v>615</v>
       </c>
-      <c r="J58" s="4" t="s">
+      <c r="K58" s="4" t="s">
         <v>616</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -12048,25 +12046,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D59" t="s">
+        <v>617</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>490</v>
+      </c>
+      <c r="H59" t="s">
+        <v>613</v>
+      </c>
+      <c r="I59" s="4" t="s">
         <v>618</v>
       </c>
-      <c r="F59" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" t="s">
-        <v>491</v>
-      </c>
-      <c r="H59" t="s">
-        <v>614</v>
-      </c>
-      <c r="I59" s="4" t="s">
+      <c r="J59" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="J59" s="4" t="s">
+      <c r="K59" s="4" t="s">
         <v>620</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -12081,25 +12079,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D60" t="s">
+        <v>621</v>
+      </c>
+      <c r="F60" t="s">
+        <v>69</v>
+      </c>
+      <c r="G60" t="s">
+        <v>490</v>
+      </c>
+      <c r="H60" t="s">
+        <v>613</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="J60" s="4" t="s">
         <v>622</v>
       </c>
-      <c r="F60" t="s">
-        <v>69</v>
-      </c>
-      <c r="G60" t="s">
-        <v>491</v>
-      </c>
-      <c r="H60" t="s">
-        <v>614</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>619</v>
-      </c>
-      <c r="J60" s="4" t="s">
+      <c r="K60" s="4" t="s">
         <v>623</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -12114,25 +12112,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D61" t="s">
+        <v>624</v>
+      </c>
+      <c r="F61" t="s">
+        <v>69</v>
+      </c>
+      <c r="G61" t="s">
+        <v>598</v>
+      </c>
+      <c r="H61" t="s">
+        <v>613</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>625</v>
       </c>
-      <c r="F61" t="s">
-        <v>69</v>
-      </c>
-      <c r="G61" t="s">
-        <v>599</v>
-      </c>
-      <c r="H61" t="s">
-        <v>614</v>
-      </c>
-      <c r="I61" s="4" t="s">
+      <c r="J61" s="4" t="s">
         <v>626</v>
       </c>
-      <c r="J61" s="4" t="s">
+      <c r="K61" s="4" t="s">
         <v>627</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -12147,19 +12145,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D62" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F62" t="s">
         <v>69</v>
       </c>
       <c r="G62" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I62" s="4" t="s">
+        <v>628</v>
+      </c>
+      <c r="J62" s="4" t="s">
         <v>629</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>630</v>
       </c>
       <c r="K62" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified "&amp;SUBSTITUTE(D62,","," and ")</f>
@@ -12178,22 +12176,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D63" t="s">
+        <v>630</v>
+      </c>
+      <c r="F63" t="s">
+        <v>69</v>
+      </c>
+      <c r="G63" t="s">
+        <v>511</v>
+      </c>
+      <c r="I63" s="4" t="s">
         <v>631</v>
       </c>
-      <c r="F63" t="s">
-        <v>69</v>
-      </c>
-      <c r="G63" t="s">
-        <v>512</v>
-      </c>
-      <c r="I63" s="4" t="s">
+      <c r="J63" s="4" t="s">
         <v>632</v>
       </c>
-      <c r="J63" s="4" t="s">
+      <c r="K63" s="4" t="s">
         <v>633</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>634</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -12208,19 +12206,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D64" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F64" t="s">
         <v>69</v>
       </c>
       <c r="G64" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I64" s="4" t="s">
+        <v>634</v>
+      </c>
+      <c r="J64" s="4" t="s">
         <v>635</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>636</v>
       </c>
       <c r="K64" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified "&amp;SUBSTITUTE(D64,","," and ")</f>
@@ -12239,19 +12237,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D65" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I65" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="J65" s="4" t="s">
         <v>637</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>638</v>
       </c>
       <c r="K65" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified "&amp;SUBSTITUTE(D65,","," and ")</f>
@@ -12270,19 +12268,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D66" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F66" t="s">
         <v>69</v>
       </c>
       <c r="G66" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I66" s="4" t="s">
+        <v>638</v>
+      </c>
+      <c r="J66" s="4" t="s">
         <v>639</v>
-      </c>
-      <c r="J66" s="4" t="s">
-        <v>640</v>
       </c>
       <c r="K66" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -12297,28 +12295,28 @@
         <v>111</v>
       </c>
       <c r="C67" t="s">
+        <v>640</v>
+      </c>
+      <c r="D67" t="s">
         <v>641</v>
       </c>
-      <c r="D67" t="s">
+      <c r="F67" t="s">
+        <v>69</v>
+      </c>
+      <c r="G67" t="s">
+        <v>490</v>
+      </c>
+      <c r="H67" t="s">
         <v>642</v>
       </c>
-      <c r="F67" t="s">
-        <v>69</v>
-      </c>
-      <c r="G67" t="s">
-        <v>491</v>
-      </c>
-      <c r="H67" t="s">
+      <c r="I67" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="I67" s="4" t="s">
+      <c r="J67" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="J67" s="4" t="s">
+      <c r="K67" s="4" t="s">
         <v>645</v>
-      </c>
-      <c r="K67" s="4" t="s">
-        <v>646</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -12329,25 +12327,25 @@
         <v>111</v>
       </c>
       <c r="C68" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D68" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F68" t="s">
         <v>12</v>
       </c>
       <c r="G68" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H68" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I68" s="4" t="s">
+        <v>646</v>
+      </c>
+      <c r="J68" s="4" t="s">
         <v>647</v>
-      </c>
-      <c r="J68" s="4" t="s">
-        <v>648</v>
       </c>
       <c r="K68" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -12362,22 +12360,22 @@
         <v>111</v>
       </c>
       <c r="C69" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D69" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F69" t="s">
         <v>12</v>
       </c>
       <c r="G69" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I69" s="4" t="s">
+        <v>648</v>
+      </c>
+      <c r="J69" s="8" t="s">
         <v>649</v>
-      </c>
-      <c r="J69" s="8" t="s">
-        <v>650</v>
       </c>
       <c r="K69" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -12392,25 +12390,25 @@
         <v>111</v>
       </c>
       <c r="C70" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D70" t="s">
+        <v>597</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s">
         <v>598</v>
       </c>
-      <c r="F70" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" t="s">
-        <v>599</v>
-      </c>
       <c r="H70" t="s">
-        <v>643</v>
+        <v>642</v>
       </c>
       <c r="I70" s="4" t="s">
+        <v>650</v>
+      </c>
+      <c r="J70" s="4" t="s">
         <v>651</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>652</v>
       </c>
       <c r="K70" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -12425,20 +12423,20 @@
         <v>111</v>
       </c>
       <c r="C71" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D71" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F71" t="s">
         <v>69</v>
       </c>
       <c r="G71" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="24" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="K71" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -12453,22 +12451,22 @@
         <v>111</v>
       </c>
       <c r="C72" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="D72" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="F72" t="s">
         <v>69</v>
       </c>
       <c r="G72" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="I72" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="J72" s="4" t="s">
         <v>654</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>655</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -12486,22 +12484,22 @@
         <v>128</v>
       </c>
       <c r="D73" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F73" t="s">
         <v>12</v>
       </c>
       <c r="G73" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H73" t="s">
+        <v>655</v>
+      </c>
+      <c r="I73" s="4" t="s">
         <v>656</v>
       </c>
-      <c r="I73" s="4" t="s">
+      <c r="J73" s="4" t="s">
         <v>657</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>658</v>
       </c>
       <c r="K73" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified "&amp;SUBSTITUTE(D73,","," and ")&amp;"=`assess-plan`"</f>
@@ -12519,25 +12517,25 @@
         <v>128</v>
       </c>
       <c r="D74" t="s">
+        <v>597</v>
+      </c>
+      <c r="F74" t="s">
+        <v>69</v>
+      </c>
+      <c r="G74" t="s">
         <v>598</v>
       </c>
-      <c r="F74" t="s">
-        <v>69</v>
-      </c>
-      <c r="G74" t="s">
-        <v>599</v>
-      </c>
       <c r="H74" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I74" s="4" t="s">
+        <v>658</v>
+      </c>
+      <c r="J74" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="J74" s="4" t="s">
+      <c r="K74" s="4" t="s">
         <v>660</v>
-      </c>
-      <c r="K74" s="4" t="s">
-        <v>661</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -12551,25 +12549,25 @@
         <v>128</v>
       </c>
       <c r="D75" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="F75" t="s">
         <v>69</v>
       </c>
       <c r="G75" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H75" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="I75" s="4" t="s">
+        <v>661</v>
+      </c>
+      <c r="J75" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="J75" s="4" t="s">
+      <c r="K75" s="4" t="s">
         <v>663</v>
-      </c>
-      <c r="K75" s="4" t="s">
-        <v>664</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -12583,25 +12581,25 @@
         <v>128</v>
       </c>
       <c r="D76" t="s">
+        <v>664</v>
+      </c>
+      <c r="F76" t="s">
+        <v>69</v>
+      </c>
+      <c r="G76" t="s">
+        <v>598</v>
+      </c>
+      <c r="H76" t="s">
+        <v>655</v>
+      </c>
+      <c r="I76" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="F76" t="s">
-        <v>69</v>
-      </c>
-      <c r="G76" t="s">
-        <v>599</v>
-      </c>
-      <c r="H76" t="s">
-        <v>656</v>
-      </c>
-      <c r="I76" s="4" t="s">
+      <c r="J76" s="4" t="s">
         <v>666</v>
       </c>
-      <c r="J76" s="4" t="s">
+      <c r="K76" s="4" t="s">
         <v>667</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>668</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="136" x14ac:dyDescent="0.2">
@@ -12616,25 +12614,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D77" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F77" t="s">
         <v>12</v>
       </c>
       <c r="G77" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H77" t="s">
+        <v>668</v>
+      </c>
+      <c r="I77" s="4" t="s">
         <v>669</v>
       </c>
-      <c r="I77" s="4" t="s">
+      <c r="J77" s="4" t="s">
         <v>670</v>
       </c>
-      <c r="J77" s="4" t="s">
+      <c r="K77" s="8" t="s">
         <v>671</v>
-      </c>
-      <c r="K77" s="8" t="s">
-        <v>672</v>
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.2">
@@ -12649,19 +12647,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D78" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F78" t="s">
         <v>69</v>
       </c>
       <c r="G78" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I78" s="4" t="s">
+        <v>672</v>
+      </c>
+      <c r="J78" s="4" t="s">
         <v>673</v>
-      </c>
-      <c r="J78" s="4" t="s">
-        <v>674</v>
       </c>
       <c r="K78" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B78&amp;" resources for the specified "&amp;SUBSTITUTE(D78,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -12673,23 +12671,23 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D79" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="F79" t="s">
         <v>69</v>
       </c>
       <c r="G79" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="J79" s="4"/>
       <c r="K79" s="4" t="str">
@@ -12709,25 +12707,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D80" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F80" t="s">
         <v>12</v>
       </c>
       <c r="G80" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H80" t="s">
+        <v>676</v>
+      </c>
+      <c r="I80" s="4" t="s">
         <v>677</v>
       </c>
-      <c r="I80" s="4" t="s">
+      <c r="J80" s="4" t="s">
         <v>678</v>
       </c>
-      <c r="J80" s="4" t="s">
+      <c r="K80" s="4" t="s">
         <v>679</v>
-      </c>
-      <c r="K80" s="4" t="s">
-        <v>680</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12742,25 +12740,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" t="s">
+        <v>597</v>
+      </c>
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s">
         <v>598</v>
       </c>
-      <c r="F81" t="s">
-        <v>12</v>
-      </c>
-      <c r="G81" t="s">
-        <v>599</v>
-      </c>
       <c r="H81" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="I81" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="J81" s="26" t="s">
         <v>681</v>
       </c>
-      <c r="J81" s="26" t="s">
+      <c r="K81" s="4" t="s">
         <v>682</v>
-      </c>
-      <c r="K81" s="4" t="s">
-        <v>683</v>
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.2">
@@ -12775,22 +12773,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D82" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F82" t="s">
         <v>12</v>
       </c>
       <c r="G82" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="J82" s="4" t="s">
         <v>684</v>
       </c>
-      <c r="J82" s="4" t="s">
+      <c r="K82" s="4" t="s">
         <v>685</v>
-      </c>
-      <c r="K82" s="4" t="s">
-        <v>686</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -12805,19 +12803,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D83" t="s">
+        <v>686</v>
+      </c>
+      <c r="F83" t="s">
+        <v>69</v>
+      </c>
+      <c r="G83" t="s">
+        <v>598</v>
+      </c>
+      <c r="I83" s="4" t="s">
         <v>687</v>
       </c>
-      <c r="F83" t="s">
-        <v>69</v>
-      </c>
-      <c r="G83" t="s">
-        <v>599</v>
-      </c>
-      <c r="I83" s="4" t="s">
+      <c r="J83" s="4" t="s">
         <v>688</v>
-      </c>
-      <c r="J83" s="4" t="s">
-        <v>689</v>
       </c>
       <c r="K83" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B83&amp;" resources for the specified "&amp;SUBSTITUTE(D83,","," and ") &amp;". See the implementation notes above for how to access the actual document."</f>
@@ -12832,25 +12830,25 @@
         <v>130</v>
       </c>
       <c r="C84" t="s">
+        <v>689</v>
+      </c>
+      <c r="D84" t="s">
+        <v>505</v>
+      </c>
+      <c r="F84" t="s">
+        <v>69</v>
+      </c>
+      <c r="G84" t="s">
+        <v>490</v>
+      </c>
+      <c r="I84" s="4" t="s">
         <v>690</v>
       </c>
-      <c r="D84" t="s">
-        <v>506</v>
-      </c>
-      <c r="F84" t="s">
-        <v>69</v>
-      </c>
-      <c r="G84" t="s">
-        <v>491</v>
-      </c>
-      <c r="I84" s="4" t="s">
+      <c r="J84" s="4" t="s">
         <v>691</v>
       </c>
-      <c r="J84" s="4" t="s">
+      <c r="K84" s="4" t="s">
         <v>692</v>
-      </c>
-      <c r="K84" s="4" t="s">
-        <v>693</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -12861,25 +12859,25 @@
         <v>130</v>
       </c>
       <c r="C85" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="D85" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F85" t="s">
         <v>69</v>
       </c>
       <c r="G85" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I85" s="4" t="s">
+        <v>693</v>
+      </c>
+      <c r="J85" s="4" t="s">
         <v>694</v>
       </c>
-      <c r="J85" s="4" t="s">
+      <c r="K85" s="4" t="s">
         <v>695</v>
-      </c>
-      <c r="K85" s="4" t="s">
-        <v>696</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -12894,22 +12892,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D86" t="s">
+        <v>696</v>
+      </c>
+      <c r="F86" t="s">
+        <v>69</v>
+      </c>
+      <c r="G86" t="s">
+        <v>490</v>
+      </c>
+      <c r="I86" s="4" t="s">
         <v>697</v>
       </c>
-      <c r="F86" t="s">
-        <v>69</v>
-      </c>
-      <c r="G86" t="s">
-        <v>491</v>
-      </c>
-      <c r="I86" s="4" t="s">
+      <c r="J86" s="4" t="s">
         <v>698</v>
       </c>
-      <c r="J86" s="4" t="s">
+      <c r="K86" s="4" t="s">
         <v>699</v>
-      </c>
-      <c r="K86" s="4" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -12924,19 +12922,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F87" t="s">
         <v>69</v>
       </c>
       <c r="G87" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I87" s="4" t="s">
+        <v>700</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>701</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>702</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified "&amp;SUBSTITUTE(D87,","," and ")</f>
@@ -12955,19 +12953,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D88" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F88" t="s">
         <v>12</v>
       </c>
       <c r="G88" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I88" s="4" t="s">
+        <v>702</v>
+      </c>
+      <c r="J88" s="4" t="s">
         <v>703</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>704</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified patient and  a category code"</f>
@@ -12986,19 +12984,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D89" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="F89" t="s">
         <v>12</v>
       </c>
       <c r="G89" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I89" s="4" t="s">
+        <v>704</v>
+      </c>
+      <c r="J89" s="4" t="s">
         <v>705</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>706</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -13017,19 +13015,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D90" t="s">
+        <v>706</v>
+      </c>
+      <c r="F90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" t="s">
+        <v>598</v>
+      </c>
+      <c r="I90" s="4" t="s">
         <v>707</v>
       </c>
-      <c r="F90" t="s">
-        <v>12</v>
-      </c>
-      <c r="G90" t="s">
-        <v>599</v>
-      </c>
-      <c r="I90" s="4" t="s">
+      <c r="J90" s="4" t="s">
         <v>708</v>
-      </c>
-      <c r="J90" s="4" t="s">
-        <v>709</v>
       </c>
       <c r="K90" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified patient and date and a category code"</f>
@@ -13048,19 +13046,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D91" t="s">
+        <v>709</v>
+      </c>
+      <c r="F91" t="s">
+        <v>69</v>
+      </c>
+      <c r="G91" t="s">
+        <v>598</v>
+      </c>
+      <c r="I91" s="4" t="s">
         <v>710</v>
       </c>
-      <c r="F91" t="s">
-        <v>69</v>
-      </c>
-      <c r="G91" t="s">
-        <v>599</v>
-      </c>
-      <c r="I91" s="4" t="s">
+      <c r="J91" s="4" t="s">
         <v>711</v>
-      </c>
-      <c r="J91" s="4" t="s">
-        <v>712</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -13079,19 +13077,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D92" t="s">
+        <v>712</v>
+      </c>
+      <c r="F92" t="s">
+        <v>69</v>
+      </c>
+      <c r="G92" t="s">
+        <v>490</v>
+      </c>
+      <c r="I92" s="4" t="s">
         <v>713</v>
       </c>
-      <c r="F92" t="s">
-        <v>69</v>
-      </c>
-      <c r="G92" t="s">
-        <v>491</v>
-      </c>
-      <c r="I92" s="4" t="s">
+      <c r="J92" s="4" t="s">
         <v>714</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>715</v>
       </c>
       <c r="K92" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -13110,19 +13108,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D93" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F93" t="s">
         <v>69</v>
       </c>
       <c r="G93" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I93" t="s">
+        <v>715</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>716</v>
-      </c>
-      <c r="J93" s="4" t="s">
-        <v>717</v>
       </c>
       <c r="K93" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
@@ -13141,22 +13139,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D94" t="s">
+        <v>717</v>
+      </c>
+      <c r="F94" t="s">
+        <v>69</v>
+      </c>
+      <c r="G94" t="s">
+        <v>490</v>
+      </c>
+      <c r="H94" t="s">
         <v>718</v>
       </c>
-      <c r="F94" t="s">
-        <v>69</v>
-      </c>
-      <c r="G94" t="s">
-        <v>491</v>
-      </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
+        <v>715</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>719</v>
-      </c>
-      <c r="I94" t="s">
-        <v>716</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>720</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified "&amp;SUBSTITUTE(D94,","," and  ") &amp; "= 'sdoh'"</f>
@@ -13175,19 +13173,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D95" t="s">
+        <v>720</v>
+      </c>
+      <c r="F95" t="s">
+        <v>69</v>
+      </c>
+      <c r="G95" t="s">
+        <v>511</v>
+      </c>
+      <c r="I95" t="s">
+        <v>715</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>721</v>
-      </c>
-      <c r="F95" t="s">
-        <v>69</v>
-      </c>
-      <c r="G95" t="s">
-        <v>512</v>
-      </c>
-      <c r="I95" t="s">
-        <v>716</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>722</v>
       </c>
       <c r="K95" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date"</f>
@@ -13206,22 +13204,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D96" s="16" t="s">
+        <v>722</v>
+      </c>
+      <c r="F96" t="s">
+        <v>69</v>
+      </c>
+      <c r="G96" t="s">
+        <v>598</v>
+      </c>
+      <c r="H96" t="s">
+        <v>718</v>
+      </c>
+      <c r="I96" t="s">
+        <v>715</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>723</v>
-      </c>
-      <c r="F96" t="s">
-        <v>69</v>
-      </c>
-      <c r="G96" t="s">
-        <v>599</v>
-      </c>
-      <c r="H96" t="s">
-        <v>719</v>
-      </c>
-      <c r="I96" t="s">
-        <v>716</v>
-      </c>
-      <c r="J96" s="4" t="s">
-        <v>724</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -13240,7 +13238,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="F97" t="s">
         <v>69</v>
@@ -13249,10 +13247,10 @@
         <v>89</v>
       </c>
       <c r="I97" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -13271,21 +13269,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="E98" s="16"/>
       <c r="F98" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G98" s="16" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4" t="s">
+        <v>726</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>727</v>
-      </c>
-      <c r="J98" s="4" t="s">
-        <v>728</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -13304,21 +13302,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E99" s="16"/>
       <c r="F99" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G99" s="16" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H99" s="16"/>
       <c r="I99" s="4" t="s">
+        <v>728</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>729</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>730</v>
       </c>
       <c r="K99" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -13337,21 +13335,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="E100" s="16"/>
       <c r="F100" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G100" s="16" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="H100" s="16"/>
       <c r="I100" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="J100" s="4" t="s">
         <v>732</v>
-      </c>
-      <c r="J100" s="4" t="s">
-        <v>733</v>
       </c>
       <c r="K100" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -13369,19 +13367,19 @@
         <v>348</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="E101" s="16"/>
       <c r="F101" s="16" t="s">
         <v>69</v>
       </c>
       <c r="G101" s="16" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="H101" s="16"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="K101" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -13408,8 +13406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13439,7 +13437,7 @@
         <v>66</v>
       </c>
       <c r="B3" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -13455,7 +13453,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -13471,7 +13469,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>460</v>
+        <v>739</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -13645,7 +13643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
@@ -14236,7 +14234,7 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="28" t="s">
+      <c r="A42" t="s">
         <v>288</v>
       </c>
       <c r="B42" t="s">
@@ -14699,7 +14697,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="T4" t="s">
         <v>19</v>
@@ -14794,7 +14792,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="T8" t="s">
         <v>19</v>
@@ -14817,7 +14815,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="T9" t="s">
         <v>19</v>
@@ -14840,7 +14838,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="T10" t="s">
         <v>19</v>
@@ -14947,7 +14945,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="T15" t="s">
         <v>19</v>
@@ -15004,7 +15002,7 @@
         <v>12</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="T18" t="s">
         <v>19</v>
@@ -15033,7 +15031,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="T19" t="s">
         <v>19</v>
@@ -15091,7 +15089,7 @@
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="T21" t="s">
         <v>19</v>
@@ -15114,7 +15112,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="T22" t="s">
         <v>19</v>
@@ -15133,7 +15131,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="T23" t="s">
         <v>19</v>
@@ -15156,7 +15154,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="T24" t="s">
         <v>19</v>
@@ -15200,7 +15198,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="T26" t="s">
         <v>19</v>
@@ -15240,7 +15238,7 @@
         <v>69</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="X28" s="13"/>
       <c r="Y28" s="13"/>
@@ -15253,7 +15251,7 @@
         <v>69</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="X29" s="13" t="s">
         <v>262</v>
@@ -15270,7 +15268,7 @@
         <v>12</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="T30" t="s">
         <v>19</v>
@@ -15293,7 +15291,7 @@
         <v>12</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="T31" t="s">
         <v>19</v>
@@ -15316,7 +15314,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="T32" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Add USCDI v6 Data Elements to US Core FHIR-52965: FamilyMemberHistory SearchParameters
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DFBFF7-405F-7844-A8D4-268B86695822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB4815B-3B53-5A49-BCBA-8301E8707E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="500" windowWidth="38500" windowHeight="28300" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5780" yWindow="500" windowWidth="38500" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -121,7 +121,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2824" uniqueCount="759">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2825" uniqueCount="759">
   <si>
     <t>Element</t>
   </si>
@@ -1432,30 +1432,6 @@
   </si>
   <si>
     <t>conf_Questionnaire</t>
-  </si>
-  <si>
-    <t>* The US Core Provenance resource **SHALL** be supported for these US Core resources:
-    * AllergyIntolerance
-    * CarePlan
-    * CareTeam
-    * Condition
-    * Coverage
-    * Device
-    * DiagnosticReport
-    * DocumentReference
-    * Encounter
-    * Goal
-    * Immunization
-    * MedicationDispense
-    * MedicationRequest
-    * Observation
-    * Patient
-    * Procedure
-    * QuestionnaireResponse
-    * RelatedPerson
-    * ServiceRequest
-* If a system receives a provider in `Provenance.agent.who` as free text they must capture who sent them the information as the organization. On request they **SHALL** provide this organization as the source and **MAY** include the free text provider.
-* Systems that need to know the activity has occurred **SHOULD** populate the activity.</t>
   </si>
   <si>
     <t>* Although both `Goal.startDate` and `Goal.target.dueDate` are marked as must support, the server system is not required to support both, but **SHALL** support at least one of these elements. The client application **SHALL** support both elements.</t>
@@ -5477,9 +5453,6 @@
     <t>support searching for all family member’s relevant health history</t>
   </si>
   <si>
-    <t>GET [base]/FamilyMemberHistory?patient=1032702&amp;code={{include.code | default: '[code]'}}</t>
-  </si>
-  <si>
     <t>support searching for family member’s condition for a patient (e.g., all family members with breast cancer)</t>
   </si>
   <si>
@@ -5492,10 +5465,38 @@
     <t>9.0.0-ballot</t>
   </si>
   <si>
-    <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ASTP 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and the ASTP [U.S. Core Data for Interoperability (USCDI) Version 6 July 2026](https://www.healthit.gov/isp/sites/isp/files/2025-07/USCDI-Version-6-July-2025.pdf).</t>
-  </si>
-  <si>
     <t>conf_FamilyMemberHistory</t>
+  </si>
+  <si>
+    <t>* The US Core Provenance resource **SHALL** be supported for these US Core resources:
+    * AllergyIntolerance
+    * CarePlan
+    * CareTeam
+    * Condition
+    * Coverage
+    * Device
+    * DiagnosticReport
+    * DocumentReference
+    * Encounter
+    * FamilyMemberHistory
+    * Goal
+    * Immunization
+    * MedicationDispense
+    * MedicationRequest
+    * Observation
+    * Patient
+    * Procedure
+    * QuestionnaireResponse
+    * RelatedPerson
+    * ServiceRequest
+* If a system receives a provider in `Provenance.agent.who` as free text they must capture who sent them the information as the organization. On request they **SHALL** provide this organization as the source and **MAY** include the free text provider.
+* Systems that need to know the activity has occurred **SHOULD** populate the activity.</t>
+  </si>
+  <si>
+    <t>This Section describes the expected capabilities of the US Core Server actor which is responsible for providing responses to the queries submitted by the US Core Requestors. The complete list of FHIR profiles, RESTful operations, and search parameters supported by US Core Servers are defined. Systems implementing this capability statement should meet the ASTP 2015 Common Clinical Data Set (CCDS) access requirement for Patient Selection 170.315(g)(7) and Application Access - Data Category Request 170.315(g)(8) and the ASTP [U.S. Core Data for Interoperability (USCDI) Version 6 July 2025](https://www.healthit.gov/isp/sites/isp/files/2025-07/USCDI-Version-6-July-2025.pdf).</t>
+  </si>
+  <si>
+    <t>GET [base]/FamilyMemberHistory?patient=1032702&amp;code=http://snomed.info/sct\|709044004</t>
   </si>
 </sst>
 </file>
@@ -5684,7 +5685,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5724,6 +5725,7 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -6143,7 +6145,7 @@
         <v>269</v>
       </c>
       <c r="B2" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -6211,11 +6213,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A9F73F9-34B4-C04F-A2E4-99114F8B7BF7}">
   <dimension ref="A1:AB135"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C65" sqref="C65"/>
+      <selection pane="bottomRight" activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="19" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7492,7 +7494,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C25" t="s">
         <v>373</v>
@@ -8520,7 +8522,7 @@
         <v>92</v>
       </c>
       <c r="C44" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D44" t="s">
         <v>29</v>
@@ -8529,7 +8531,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" ref="G44" si="5">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B44)</f>
@@ -8949,7 +8951,7 @@
         <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D52" t="s">
         <v>29</v>
@@ -8958,7 +8960,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="4"/>
@@ -9646,7 +9648,7 @@
         <v>21</v>
       </c>
       <c r="C65" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D65" t="s">
         <v>29</v>
@@ -9655,7 +9657,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="4"/>
@@ -10020,7 +10022,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C72" t="s">
         <v>87</v>
@@ -10061,7 +10063,7 @@
         <v>55</v>
       </c>
       <c r="Y72" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="Z72" s="4" t="str">
         <f>"GET [base]/"&amp;B72&amp;"?patient=1137192"</f>
@@ -10081,7 +10083,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C73" t="s">
         <v>25</v>
@@ -10112,7 +10114,7 @@
         <v>56</v>
       </c>
       <c r="L73" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="M73" t="s">
         <v>55</v>
@@ -10133,7 +10135,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="C74" t="s">
         <v>60</v>
@@ -11414,7 +11416,7 @@
         <v>110</v>
       </c>
       <c r="C98" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="D98" t="s">
         <v>29</v>
@@ -11423,7 +11425,7 @@
         <v>0</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="G98" t="str">
         <f t="shared" ref="G98" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B98)</f>
@@ -13471,10 +13473,10 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="G91" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G102" sqref="G102"/>
+      <selection pane="bottomRight" activeCell="J105" sqref="J105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -13493,7 +13495,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>36</v>
@@ -13502,19 +13504,19 @@
         <v>38</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>330</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>460</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>461</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
@@ -13531,20 +13533,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C49" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D2" t="s">
+        <v>462</v>
+      </c>
+      <c r="F2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G2" t="s">
         <v>463</v>
-      </c>
-      <c r="F2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G2" t="s">
-        <v>464</v>
       </c>
       <c r="K2" s="4" t="str">
         <f t="shared" ref="K2:K17" si="1">"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
@@ -13556,20 +13558,20 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D3" t="s">
+        <v>464</v>
+      </c>
+      <c r="F3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" t="s">
         <v>465</v>
-      </c>
-      <c r="F3" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" t="s">
-        <v>466</v>
       </c>
       <c r="K3" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13581,20 +13583,20 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D4" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F4" t="s">
         <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K4" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13606,20 +13608,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D5" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="F5" t="s">
         <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K5" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13638,19 +13640,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D6" t="s">
+        <v>468</v>
+      </c>
+      <c r="F6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
         <v>469</v>
       </c>
-      <c r="F6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>470</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>471</v>
-      </c>
-      <c r="J6" t="s">
-        <v>472</v>
       </c>
       <c r="K6" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13662,20 +13664,20 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D7" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F7" t="s">
         <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K7" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13687,20 +13689,20 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D8" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="F8" t="s">
         <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="K8" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13712,20 +13714,20 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D9" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="F9" t="s">
         <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="str">
@@ -13738,14 +13740,14 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D10" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="F10" t="s">
         <v>68</v>
@@ -13765,14 +13767,14 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D11" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F11" t="s">
         <v>68</v>
@@ -13791,14 +13793,14 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D12" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="F12" t="s">
         <v>68</v>
@@ -13823,19 +13825,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D13" t="s">
+        <v>478</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
         <v>479</v>
       </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="I13" s="4" t="s">
         <v>480</v>
       </c>
-      <c r="I13" s="4" t="s">
+      <c r="J13" t="s">
         <v>481</v>
-      </c>
-      <c r="J13" t="s">
-        <v>482</v>
       </c>
       <c r="K13" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13847,20 +13849,20 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D14" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="F14" t="s">
         <v>68</v>
       </c>
       <c r="G14" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="K14" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13872,20 +13874,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D15" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="F15" t="s">
         <v>68</v>
       </c>
       <c r="G15" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="K15" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13904,19 +13906,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D16" t="s">
+        <v>484</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" t="s">
+        <v>469</v>
+      </c>
+      <c r="I16" t="s">
         <v>485</v>
       </c>
-      <c r="F16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" t="s">
-        <v>470</v>
-      </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>486</v>
-      </c>
-      <c r="J16" t="s">
-        <v>487</v>
       </c>
       <c r="K16" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13935,7 +13937,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F17" t="s">
         <v>68</v>
@@ -13944,10 +13946,10 @@
         <v>88</v>
       </c>
       <c r="I17" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="J17" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13966,17 +13968,17 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" t="s">
+        <v>489</v>
+      </c>
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" t="s">
         <v>490</v>
-      </c>
-      <c r="F18" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" t="s">
-        <v>491</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="24" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="K18" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B18&amp;" resources for the specified "&amp;SUBSTITUTE(D18,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -13988,20 +13990,20 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D19" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F19" t="s">
         <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="str">
@@ -14021,19 +14023,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
+        <v>493</v>
+      </c>
+      <c r="F20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
+        <v>469</v>
+      </c>
+      <c r="I20" t="s">
         <v>494</v>
       </c>
-      <c r="F20" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" t="s">
-        <v>470</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>495</v>
-      </c>
-      <c r="J20" t="s">
-        <v>496</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14052,19 +14054,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D21" t="s">
+        <v>496</v>
+      </c>
+      <c r="F21" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" t="s">
+        <v>469</v>
+      </c>
+      <c r="I21" t="s">
+        <v>494</v>
+      </c>
+      <c r="J21" t="s">
         <v>497</v>
-      </c>
-      <c r="F21" t="s">
-        <v>68</v>
-      </c>
-      <c r="G21" t="s">
-        <v>470</v>
-      </c>
-      <c r="I21" t="s">
-        <v>495</v>
-      </c>
-      <c r="J21" t="s">
-        <v>498</v>
       </c>
       <c r="K21" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14076,14 +14078,14 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D22" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="F22" t="s">
         <v>68</v>
@@ -14103,20 +14105,20 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D23" t="s">
+        <v>500</v>
+      </c>
+      <c r="F23" t="s">
+        <v>68</v>
+      </c>
+      <c r="G23" t="s">
         <v>501</v>
-      </c>
-      <c r="F23" t="s">
-        <v>68</v>
-      </c>
-      <c r="G23" t="s">
-        <v>502</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="str">
@@ -14129,20 +14131,20 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D24" t="s">
+        <v>502</v>
+      </c>
+      <c r="F24" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" t="s">
         <v>503</v>
-      </c>
-      <c r="F24" t="s">
-        <v>68</v>
-      </c>
-      <c r="G24" t="s">
-        <v>504</v>
       </c>
       <c r="K24" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14154,20 +14156,20 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D25" t="s">
+        <v>504</v>
+      </c>
+      <c r="F25" t="s">
+        <v>68</v>
+      </c>
+      <c r="G25" t="s">
         <v>505</v>
-      </c>
-      <c r="F25" t="s">
-        <v>68</v>
-      </c>
-      <c r="G25" t="s">
-        <v>506</v>
       </c>
       <c r="I25" s="4"/>
       <c r="K25" s="4" t="str">
@@ -14180,20 +14182,20 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D26" t="s">
+        <v>506</v>
+      </c>
+      <c r="F26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" t="s">
         <v>507</v>
-      </c>
-      <c r="F26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" t="s">
-        <v>508</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -14207,20 +14209,20 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D27" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="F27" t="s">
         <v>68</v>
       </c>
       <c r="G27" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -14234,20 +14236,20 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D28" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F28" t="s">
         <v>68</v>
       </c>
       <c r="G28" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -14261,20 +14263,20 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D29" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F29" t="s">
         <v>68</v>
       </c>
       <c r="G29" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K29" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14286,14 +14288,14 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D30" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F30" t="s">
         <v>68</v>
@@ -14311,20 +14313,20 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D31" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F31" t="s">
         <v>68</v>
       </c>
       <c r="G31" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="K31" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14343,19 +14345,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
+        <v>513</v>
+      </c>
+      <c r="F32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" t="s">
         <v>514</v>
       </c>
-      <c r="F32" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="I32" s="4" t="s">
         <v>515</v>
       </c>
-      <c r="I32" s="4" t="s">
+      <c r="J32" s="4" t="s">
         <v>516</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>517</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14374,19 +14376,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D33" t="s">
+        <v>517</v>
+      </c>
+      <c r="F33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" t="s">
+        <v>514</v>
+      </c>
+      <c r="I33" s="4" t="s">
         <v>518</v>
       </c>
-      <c r="F33" t="s">
-        <v>68</v>
-      </c>
-      <c r="G33" t="s">
-        <v>515</v>
-      </c>
-      <c r="I33" s="4" t="s">
+      <c r="J33" s="4" t="s">
         <v>519</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>520</v>
       </c>
       <c r="K33" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14405,19 +14407,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D34" t="s">
+        <v>520</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>514</v>
+      </c>
+      <c r="I34" s="4" t="s">
         <v>521</v>
       </c>
-      <c r="F34" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" t="s">
-        <v>515</v>
-      </c>
-      <c r="I34" s="4" t="s">
+      <c r="J34" s="4" t="s">
         <v>522</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>523</v>
       </c>
       <c r="K34" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14436,19 +14438,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="D35" t="s">
+        <v>523</v>
+      </c>
+      <c r="F35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" t="s">
+        <v>507</v>
+      </c>
+      <c r="I35" s="4" t="s">
         <v>524</v>
       </c>
-      <c r="F35" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" t="s">
-        <v>508</v>
-      </c>
-      <c r="I35" s="4" t="s">
+      <c r="J35" s="4" t="s">
         <v>525</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>526</v>
       </c>
       <c r="K35" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14467,19 +14469,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="D36" t="s">
+        <v>526</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>507</v>
+      </c>
+      <c r="I36" s="4" t="s">
         <v>527</v>
       </c>
-      <c r="F36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" t="s">
-        <v>508</v>
-      </c>
-      <c r="I36" s="4" t="s">
+      <c r="J36" s="4" t="s">
         <v>528</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>529</v>
       </c>
       <c r="K36" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14498,25 +14500,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" t="s">
+        <v>529</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" t="s">
+        <v>469</v>
+      </c>
+      <c r="H37" t="s">
         <v>530</v>
       </c>
-      <c r="F37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G37" t="s">
-        <v>470</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="I37" s="4" t="s">
         <v>531</v>
       </c>
-      <c r="I37" s="4" t="s">
+      <c r="J37" s="25" t="s">
         <v>532</v>
       </c>
-      <c r="J37" s="25" t="s">
-        <v>533</v>
-      </c>
       <c r="K37" s="4" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14531,22 +14533,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
+        <v>533</v>
+      </c>
+      <c r="F38" t="s">
+        <v>12</v>
+      </c>
+      <c r="G38" t="s">
+        <v>469</v>
+      </c>
+      <c r="I38" s="4" t="s">
         <v>534</v>
       </c>
-      <c r="F38" t="s">
-        <v>12</v>
-      </c>
-      <c r="G38" t="s">
-        <v>470</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>535</v>
-      </c>
       <c r="J38" s="25" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14561,25 +14563,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
+        <v>535</v>
+      </c>
+      <c r="F39" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" t="s">
+        <v>469</v>
+      </c>
+      <c r="H39" t="s">
+        <v>530</v>
+      </c>
+      <c r="I39" s="4" t="s">
         <v>536</v>
       </c>
-      <c r="F39" t="s">
-        <v>68</v>
-      </c>
-      <c r="G39" t="s">
-        <v>470</v>
-      </c>
-      <c r="H39" t="s">
-        <v>531</v>
-      </c>
-      <c r="I39" s="4" t="s">
-        <v>537</v>
-      </c>
       <c r="J39" s="25" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="K39" s="25" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14594,22 +14596,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="F40" t="s">
         <v>68</v>
       </c>
       <c r="G40" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="J40" s="25" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="K40" s="25" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14624,22 +14626,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
+        <v>538</v>
+      </c>
+      <c r="F41" t="s">
+        <v>68</v>
+      </c>
+      <c r="G41" t="s">
+        <v>469</v>
+      </c>
+      <c r="I41" s="4" t="s">
         <v>539</v>
       </c>
-      <c r="F41" t="s">
-        <v>68</v>
-      </c>
-      <c r="G41" t="s">
-        <v>470</v>
-      </c>
-      <c r="I41" s="4" t="s">
+      <c r="J41" s="25" t="s">
+        <v>716</v>
+      </c>
+      <c r="K41" s="4" t="s">
         <v>540</v>
-      </c>
-      <c r="J41" s="25" t="s">
-        <v>717</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>541</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14654,22 +14656,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
+        <v>541</v>
+      </c>
+      <c r="F42" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" t="s">
+        <v>490</v>
+      </c>
+      <c r="I42" s="4" t="s">
         <v>542</v>
       </c>
-      <c r="F42" t="s">
-        <v>68</v>
-      </c>
-      <c r="G42" t="s">
-        <v>491</v>
-      </c>
-      <c r="I42" s="4" t="s">
+      <c r="J42" s="25" t="s">
+        <v>717</v>
+      </c>
+      <c r="K42" s="4" t="s">
         <v>543</v>
-      </c>
-      <c r="J42" s="25" t="s">
-        <v>718</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14684,22 +14686,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="F43" t="s">
         <v>68</v>
       </c>
       <c r="G43" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I43" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="J43" s="25" t="s">
+        <v>718</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>543</v>
-      </c>
-      <c r="J43" s="25" t="s">
-        <v>719</v>
-      </c>
-      <c r="K43" s="4" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14714,22 +14716,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="F44" t="s">
         <v>68</v>
       </c>
       <c r="G44" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I44" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="J44" s="25" t="s">
+        <v>719</v>
+      </c>
+      <c r="K44" s="4" t="s">
         <v>543</v>
-      </c>
-      <c r="J44" s="25" t="s">
-        <v>720</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14744,22 +14746,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D45" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="F45" t="s">
         <v>68</v>
       </c>
       <c r="G45" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I45" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="J45" s="25" t="s">
+        <v>720</v>
+      </c>
+      <c r="K45" s="4" t="s">
         <v>543</v>
-      </c>
-      <c r="J45" s="25" t="s">
-        <v>721</v>
-      </c>
-      <c r="K45" s="4" t="s">
-        <v>544</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14774,17 +14776,17 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D46" t="s">
+        <v>489</v>
+      </c>
+      <c r="F46" t="s">
+        <v>68</v>
+      </c>
+      <c r="G46" t="s">
         <v>490</v>
-      </c>
-      <c r="F46" t="s">
-        <v>68</v>
-      </c>
-      <c r="G46" t="s">
-        <v>491</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="25" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="K46" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -14803,22 +14805,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D47" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F47" t="s">
         <v>68</v>
       </c>
       <c r="G47" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I47" s="4" t="s">
+        <v>548</v>
+      </c>
+      <c r="J47" s="4" t="s">
         <v>549</v>
       </c>
-      <c r="J47" s="4" t="s">
+      <c r="K47" s="4" t="s">
         <v>550</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>551</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -14833,19 +14835,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D48" t="s">
+        <v>551</v>
+      </c>
+      <c r="F48" t="s">
+        <v>68</v>
+      </c>
+      <c r="G48" t="s">
+        <v>479</v>
+      </c>
+      <c r="I48" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="F48" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" t="s">
-        <v>480</v>
-      </c>
-      <c r="I48" s="4" t="s">
+      <c r="J48" s="4" t="s">
         <v>553</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>554</v>
       </c>
       <c r="K48" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified "&amp;SUBSTITUTE(D48,","," and ")</f>
@@ -14864,19 +14866,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D49" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F49" t="s">
         <v>68</v>
       </c>
       <c r="G49" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I49" s="4" t="s">
+        <v>554</v>
+      </c>
+      <c r="J49" s="4" t="s">
         <v>555</v>
-      </c>
-      <c r="J49" s="4" t="s">
-        <v>556</v>
       </c>
       <c r="K49" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified "&amp;SUBSTITUTE(D49,","," and ")</f>
@@ -14891,25 +14893,25 @@
         <v>106</v>
       </c>
       <c r="C50" t="s">
+        <v>556</v>
+      </c>
+      <c r="D50" t="s">
+        <v>493</v>
+      </c>
+      <c r="F50" t="s">
+        <v>68</v>
+      </c>
+      <c r="G50" t="s">
+        <v>469</v>
+      </c>
+      <c r="I50" s="4" t="s">
         <v>557</v>
       </c>
-      <c r="D50" t="s">
-        <v>494</v>
-      </c>
-      <c r="F50" t="s">
-        <v>68</v>
-      </c>
-      <c r="G50" t="s">
-        <v>470</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>558</v>
-      </c>
       <c r="J50" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="K50" s="25" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14920,25 +14922,25 @@
         <v>106</v>
       </c>
       <c r="C51" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D51" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F51" t="s">
         <v>12</v>
       </c>
       <c r="G51" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I51" s="4" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="J51" s="25" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="K51" s="25" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14949,25 +14951,25 @@
         <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D52" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F52" t="s">
         <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="J52" s="25" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="K52" s="25" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14978,25 +14980,25 @@
         <v>106</v>
       </c>
       <c r="C53" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D53" t="s">
+        <v>560</v>
+      </c>
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s">
         <v>561</v>
       </c>
-      <c r="F53" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" t="s">
+      <c r="I53" s="4" t="s">
         <v>562</v>
       </c>
-      <c r="I53" s="4" t="s">
-        <v>563</v>
-      </c>
       <c r="J53" s="25" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="K53" s="25" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15011,20 +15013,20 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="D54" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F54" t="s">
         <v>68</v>
       </c>
       <c r="G54" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="25" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="K54" s="25" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15035,25 +15037,25 @@
         <v>106</v>
       </c>
       <c r="C55" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="D55" t="s">
+        <v>564</v>
+      </c>
+      <c r="F55" t="s">
+        <v>68</v>
+      </c>
+      <c r="G55" t="s">
+        <v>561</v>
+      </c>
+      <c r="I55" s="4" t="s">
         <v>565</v>
       </c>
-      <c r="F55" t="s">
-        <v>68</v>
-      </c>
-      <c r="G55" t="s">
-        <v>562</v>
-      </c>
-      <c r="I55" s="4" t="s">
-        <v>566</v>
-      </c>
       <c r="J55" s="25" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="K55" s="25" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -15068,19 +15070,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D56" t="s">
+        <v>566</v>
+      </c>
+      <c r="F56" t="s">
+        <v>68</v>
+      </c>
+      <c r="G56" t="s">
+        <v>469</v>
+      </c>
+      <c r="I56" s="4" t="s">
         <v>567</v>
       </c>
-      <c r="F56" t="s">
-        <v>68</v>
-      </c>
-      <c r="G56" t="s">
-        <v>470</v>
-      </c>
-      <c r="I56" s="4" t="s">
+      <c r="J56" s="4" t="s">
         <v>568</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>569</v>
       </c>
       <c r="K56" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp;" resources for the specified "&amp;SUBSTITUTE(D56,","," and ")</f>
@@ -15099,19 +15101,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D57" t="s">
+        <v>569</v>
+      </c>
+      <c r="F57" t="s">
+        <v>68</v>
+      </c>
+      <c r="G57" t="s">
+        <v>490</v>
+      </c>
+      <c r="I57" s="4" t="s">
         <v>570</v>
       </c>
-      <c r="F57" t="s">
-        <v>68</v>
-      </c>
-      <c r="G57" t="s">
-        <v>491</v>
-      </c>
-      <c r="I57" s="4" t="s">
+      <c r="J57" s="4" t="s">
         <v>571</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>572</v>
       </c>
       <c r="K57" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B57&amp;" resources for the specified "&amp;SUBSTITUTE(D57,","," and ")</f>
@@ -15130,25 +15132,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" t="s">
+        <v>572</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" t="s">
+        <v>469</v>
+      </c>
+      <c r="H58" t="s">
         <v>573</v>
       </c>
-      <c r="F58" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" t="s">
-        <v>470</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="I58" s="4" t="s">
         <v>574</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="J58" s="4" t="s">
         <v>575</v>
       </c>
-      <c r="J58" s="4" t="s">
+      <c r="K58" s="4" t="s">
         <v>576</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>577</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -15163,25 +15165,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D59" t="s">
+        <v>577</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>469</v>
+      </c>
+      <c r="H59" t="s">
+        <v>573</v>
+      </c>
+      <c r="I59" s="4" t="s">
         <v>578</v>
       </c>
-      <c r="F59" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" t="s">
-        <v>470</v>
-      </c>
-      <c r="H59" t="s">
-        <v>574</v>
-      </c>
-      <c r="I59" s="4" t="s">
+      <c r="J59" s="4" t="s">
         <v>579</v>
       </c>
-      <c r="J59" s="4" t="s">
+      <c r="K59" s="4" t="s">
         <v>580</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -15196,25 +15198,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D60" t="s">
+        <v>581</v>
+      </c>
+      <c r="F60" t="s">
+        <v>68</v>
+      </c>
+      <c r="G60" t="s">
+        <v>469</v>
+      </c>
+      <c r="H60" t="s">
+        <v>573</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>578</v>
+      </c>
+      <c r="J60" s="4" t="s">
         <v>582</v>
       </c>
-      <c r="F60" t="s">
-        <v>68</v>
-      </c>
-      <c r="G60" t="s">
-        <v>470</v>
-      </c>
-      <c r="H60" t="s">
-        <v>574</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>579</v>
-      </c>
-      <c r="J60" s="4" t="s">
+      <c r="K60" s="4" t="s">
         <v>583</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>584</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -15229,25 +15231,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D61" t="s">
+        <v>584</v>
+      </c>
+      <c r="F61" t="s">
+        <v>68</v>
+      </c>
+      <c r="G61" t="s">
+        <v>561</v>
+      </c>
+      <c r="H61" t="s">
+        <v>573</v>
+      </c>
+      <c r="I61" s="4" t="s">
         <v>585</v>
       </c>
-      <c r="F61" t="s">
-        <v>68</v>
-      </c>
-      <c r="G61" t="s">
-        <v>562</v>
-      </c>
-      <c r="H61" t="s">
-        <v>574</v>
-      </c>
-      <c r="I61" s="4" t="s">
+      <c r="J61" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="J61" s="4" t="s">
+      <c r="K61" s="4" t="s">
         <v>587</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>588</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -15262,19 +15264,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D62" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F62" t="s">
         <v>68</v>
       </c>
       <c r="G62" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I62" s="4" t="s">
+        <v>588</v>
+      </c>
+      <c r="J62" s="4" t="s">
         <v>589</v>
-      </c>
-      <c r="J62" s="4" t="s">
-        <v>590</v>
       </c>
       <c r="K62" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified "&amp;SUBSTITUTE(D62,","," and ")</f>
@@ -15293,22 +15295,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D63" t="s">
+        <v>590</v>
+      </c>
+      <c r="F63" t="s">
+        <v>68</v>
+      </c>
+      <c r="G63" t="s">
+        <v>490</v>
+      </c>
+      <c r="I63" s="4" t="s">
         <v>591</v>
       </c>
-      <c r="F63" t="s">
-        <v>68</v>
-      </c>
-      <c r="G63" t="s">
-        <v>491</v>
-      </c>
-      <c r="I63" s="4" t="s">
+      <c r="J63" s="4" t="s">
         <v>592</v>
       </c>
-      <c r="J63" s="4" t="s">
+      <c r="K63" s="4" t="s">
         <v>593</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>594</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -15323,19 +15325,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D64" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F64" t="s">
         <v>68</v>
       </c>
       <c r="G64" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I64" s="4" t="s">
+        <v>594</v>
+      </c>
+      <c r="J64" s="4" t="s">
         <v>595</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>596</v>
       </c>
       <c r="K64" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified "&amp;SUBSTITUTE(D64,","," and ")</f>
@@ -15354,19 +15356,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D65" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I65" s="4" t="s">
+        <v>596</v>
+      </c>
+      <c r="J65" s="4" t="s">
         <v>597</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>598</v>
       </c>
       <c r="K65" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified "&amp;SUBSTITUTE(D65,","," and ")</f>
@@ -15385,19 +15387,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D66" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F66" t="s">
         <v>68</v>
       </c>
       <c r="G66" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I66" s="4" t="s">
+        <v>598</v>
+      </c>
+      <c r="J66" s="4" t="s">
         <v>599</v>
-      </c>
-      <c r="J66" s="4" t="s">
-        <v>600</v>
       </c>
       <c r="K66" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -15412,28 +15414,28 @@
         <v>110</v>
       </c>
       <c r="C67" t="s">
+        <v>600</v>
+      </c>
+      <c r="D67" t="s">
         <v>601</v>
       </c>
-      <c r="D67" t="s">
+      <c r="F67" t="s">
+        <v>68</v>
+      </c>
+      <c r="G67" t="s">
+        <v>469</v>
+      </c>
+      <c r="H67" t="s">
         <v>602</v>
       </c>
-      <c r="F67" t="s">
-        <v>68</v>
-      </c>
-      <c r="G67" t="s">
-        <v>470</v>
-      </c>
-      <c r="H67" t="s">
+      <c r="I67" s="4" t="s">
         <v>603</v>
       </c>
-      <c r="I67" s="4" t="s">
+      <c r="J67" s="4" t="s">
         <v>604</v>
       </c>
-      <c r="J67" s="4" t="s">
+      <c r="K67" s="4" t="s">
         <v>605</v>
-      </c>
-      <c r="K67" s="4" t="s">
-        <v>606</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -15444,25 +15446,25 @@
         <v>110</v>
       </c>
       <c r="C68" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D68" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F68" t="s">
         <v>12</v>
       </c>
       <c r="G68" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H68" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I68" s="4" t="s">
+        <v>606</v>
+      </c>
+      <c r="J68" s="4" t="s">
         <v>607</v>
-      </c>
-      <c r="J68" s="4" t="s">
-        <v>608</v>
       </c>
       <c r="K68" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -15477,22 +15479,22 @@
         <v>110</v>
       </c>
       <c r="C69" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D69" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F69" t="s">
         <v>12</v>
       </c>
       <c r="G69" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I69" s="4" t="s">
+        <v>608</v>
+      </c>
+      <c r="J69" s="8" t="s">
         <v>609</v>
-      </c>
-      <c r="J69" s="8" t="s">
-        <v>610</v>
       </c>
       <c r="K69" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -15507,25 +15509,25 @@
         <v>110</v>
       </c>
       <c r="C70" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D70" t="s">
+        <v>560</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s">
         <v>561</v>
       </c>
-      <c r="F70" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" t="s">
-        <v>562</v>
-      </c>
       <c r="H70" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
       <c r="I70" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="J70" s="4" t="s">
         <v>611</v>
-      </c>
-      <c r="J70" s="4" t="s">
-        <v>612</v>
       </c>
       <c r="K70" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -15540,20 +15542,20 @@
         <v>110</v>
       </c>
       <c r="C71" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D71" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F71" t="s">
         <v>68</v>
       </c>
       <c r="G71" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="24" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="K71" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -15568,22 +15570,22 @@
         <v>110</v>
       </c>
       <c r="C72" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D72" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="F72" t="s">
         <v>68</v>
       </c>
       <c r="G72" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I72" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="J72" s="4" t="s">
         <v>614</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>615</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -15601,22 +15603,22 @@
         <v>127</v>
       </c>
       <c r="D73" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F73" t="s">
         <v>12</v>
       </c>
       <c r="G73" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H73" t="s">
+        <v>615</v>
+      </c>
+      <c r="I73" s="4" t="s">
         <v>616</v>
       </c>
-      <c r="I73" s="4" t="s">
+      <c r="J73" s="4" t="s">
         <v>617</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>618</v>
       </c>
       <c r="K73" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified "&amp;SUBSTITUTE(D73,","," and ")&amp;"=`assess-plan`"</f>
@@ -15634,25 +15636,25 @@
         <v>127</v>
       </c>
       <c r="D74" t="s">
+        <v>560</v>
+      </c>
+      <c r="F74" t="s">
+        <v>68</v>
+      </c>
+      <c r="G74" t="s">
         <v>561</v>
       </c>
-      <c r="F74" t="s">
-        <v>68</v>
-      </c>
-      <c r="G74" t="s">
-        <v>562</v>
-      </c>
       <c r="H74" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I74" s="4" t="s">
+        <v>618</v>
+      </c>
+      <c r="J74" s="4" t="s">
         <v>619</v>
       </c>
-      <c r="J74" s="4" t="s">
+      <c r="K74" s="4" t="s">
         <v>620</v>
-      </c>
-      <c r="K74" s="4" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -15666,25 +15668,25 @@
         <v>127</v>
       </c>
       <c r="D75" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="F75" t="s">
         <v>68</v>
       </c>
       <c r="G75" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H75" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="I75" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="J75" s="4" t="s">
         <v>622</v>
       </c>
-      <c r="J75" s="4" t="s">
+      <c r="K75" s="4" t="s">
         <v>623</v>
-      </c>
-      <c r="K75" s="4" t="s">
-        <v>624</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -15698,25 +15700,25 @@
         <v>127</v>
       </c>
       <c r="D76" t="s">
+        <v>624</v>
+      </c>
+      <c r="F76" t="s">
+        <v>68</v>
+      </c>
+      <c r="G76" t="s">
+        <v>561</v>
+      </c>
+      <c r="H76" t="s">
+        <v>615</v>
+      </c>
+      <c r="I76" s="4" t="s">
         <v>625</v>
       </c>
-      <c r="F76" t="s">
-        <v>68</v>
-      </c>
-      <c r="G76" t="s">
-        <v>562</v>
-      </c>
-      <c r="H76" t="s">
-        <v>616</v>
-      </c>
-      <c r="I76" s="4" t="s">
+      <c r="J76" s="4" t="s">
         <v>626</v>
       </c>
-      <c r="J76" s="4" t="s">
+      <c r="K76" s="4" t="s">
         <v>627</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>628</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="136" x14ac:dyDescent="0.2">
@@ -15731,25 +15733,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D77" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F77" t="s">
         <v>12</v>
       </c>
       <c r="G77" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H77" t="s">
+        <v>628</v>
+      </c>
+      <c r="I77" s="4" t="s">
         <v>629</v>
       </c>
-      <c r="I77" s="4" t="s">
+      <c r="J77" s="4" t="s">
         <v>630</v>
       </c>
-      <c r="J77" s="4" t="s">
+      <c r="K77" s="8" t="s">
         <v>631</v>
-      </c>
-      <c r="K77" s="8" t="s">
-        <v>632</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15764,22 +15766,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D78" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F78" t="s">
         <v>68</v>
       </c>
       <c r="G78" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="J78" s="25" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15787,26 +15789,26 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D79" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="F79" t="s">
         <v>68</v>
       </c>
       <c r="G79" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15821,22 +15823,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D80" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F80" t="s">
         <v>12</v>
       </c>
       <c r="G80" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
       <c r="J80" s="25" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="K80" s="25" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15851,22 +15853,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" t="s">
+        <v>560</v>
+      </c>
+      <c r="F81" t="s">
+        <v>12</v>
+      </c>
+      <c r="G81" t="s">
         <v>561</v>
       </c>
-      <c r="F81" t="s">
-        <v>12</v>
-      </c>
-      <c r="G81" t="s">
-        <v>562</v>
-      </c>
       <c r="I81" s="4" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
       <c r="J81" s="25" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="K81" s="25" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15881,22 +15883,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D82" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F82" t="s">
         <v>12</v>
       </c>
       <c r="G82" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I82" s="4" t="s">
+        <v>637</v>
+      </c>
+      <c r="J82" s="25" t="s">
+        <v>708</v>
+      </c>
+      <c r="K82" s="25" t="s">
         <v>638</v>
-      </c>
-      <c r="J82" s="25" t="s">
-        <v>709</v>
-      </c>
-      <c r="K82" s="25" t="s">
-        <v>639</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15911,22 +15913,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D83" t="s">
+        <v>639</v>
+      </c>
+      <c r="F83" t="s">
+        <v>68</v>
+      </c>
+      <c r="G83" t="s">
+        <v>561</v>
+      </c>
+      <c r="I83" s="4" t="s">
         <v>640</v>
       </c>
-      <c r="F83" t="s">
-        <v>68</v>
-      </c>
-      <c r="G83" t="s">
-        <v>562</v>
-      </c>
-      <c r="I83" s="4" t="s">
-        <v>641</v>
-      </c>
       <c r="J83" s="25" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="K83" s="25" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -15937,25 +15939,25 @@
         <v>129</v>
       </c>
       <c r="C84" t="s">
+        <v>641</v>
+      </c>
+      <c r="D84" t="s">
+        <v>484</v>
+      </c>
+      <c r="F84" t="s">
+        <v>68</v>
+      </c>
+      <c r="G84" t="s">
+        <v>469</v>
+      </c>
+      <c r="I84" s="4" t="s">
         <v>642</v>
       </c>
-      <c r="D84" t="s">
-        <v>485</v>
-      </c>
-      <c r="F84" t="s">
-        <v>68</v>
-      </c>
-      <c r="G84" t="s">
-        <v>470</v>
-      </c>
-      <c r="I84" s="4" t="s">
+      <c r="J84" s="4" t="s">
         <v>643</v>
       </c>
-      <c r="J84" s="4" t="s">
+      <c r="K84" s="4" t="s">
         <v>644</v>
-      </c>
-      <c r="K84" s="4" t="s">
-        <v>645</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -15966,25 +15968,25 @@
         <v>129</v>
       </c>
       <c r="C85" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
       <c r="D85" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F85" t="s">
         <v>68</v>
       </c>
       <c r="G85" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I85" s="4" t="s">
+        <v>645</v>
+      </c>
+      <c r="J85" s="4" t="s">
         <v>646</v>
       </c>
-      <c r="J85" s="4" t="s">
+      <c r="K85" s="4" t="s">
         <v>647</v>
-      </c>
-      <c r="K85" s="4" t="s">
-        <v>648</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -15999,22 +16001,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D86" t="s">
+        <v>648</v>
+      </c>
+      <c r="F86" t="s">
+        <v>68</v>
+      </c>
+      <c r="G86" t="s">
+        <v>469</v>
+      </c>
+      <c r="I86" s="4" t="s">
         <v>649</v>
       </c>
-      <c r="F86" t="s">
-        <v>68</v>
-      </c>
-      <c r="G86" t="s">
-        <v>470</v>
-      </c>
-      <c r="I86" s="4" t="s">
+      <c r="J86" s="4" t="s">
         <v>650</v>
       </c>
-      <c r="J86" s="4" t="s">
+      <c r="K86" s="4" t="s">
         <v>651</v>
-      </c>
-      <c r="K86" s="4" t="s">
-        <v>652</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -16029,19 +16031,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F87" t="s">
         <v>68</v>
       </c>
       <c r="G87" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I87" s="4" t="s">
+        <v>652</v>
+      </c>
+      <c r="J87" s="4" t="s">
         <v>653</v>
-      </c>
-      <c r="J87" s="4" t="s">
-        <v>654</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified "&amp;SUBSTITUTE(D87,","," and ")</f>
@@ -16060,19 +16062,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D88" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="F88" t="s">
         <v>12</v>
       </c>
       <c r="G88" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I88" s="4" t="s">
+        <v>654</v>
+      </c>
+      <c r="J88" s="4" t="s">
         <v>655</v>
-      </c>
-      <c r="J88" s="4" t="s">
-        <v>656</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified patient and  a category code"</f>
@@ -16091,19 +16093,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D89" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="F89" t="s">
         <v>12</v>
       </c>
       <c r="G89" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I89" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="J89" s="4" t="s">
         <v>657</v>
-      </c>
-      <c r="J89" s="4" t="s">
-        <v>658</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -16122,19 +16124,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D90" t="s">
+        <v>658</v>
+      </c>
+      <c r="F90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" t="s">
+        <v>561</v>
+      </c>
+      <c r="I90" s="4" t="s">
         <v>659</v>
       </c>
-      <c r="F90" t="s">
-        <v>12</v>
-      </c>
-      <c r="G90" t="s">
-        <v>562</v>
-      </c>
-      <c r="I90" s="4" t="s">
+      <c r="J90" s="4" t="s">
         <v>660</v>
-      </c>
-      <c r="J90" s="4" t="s">
-        <v>661</v>
       </c>
       <c r="K90" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified patient and date and a category code"</f>
@@ -16153,19 +16155,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D91" t="s">
+        <v>661</v>
+      </c>
+      <c r="F91" t="s">
+        <v>68</v>
+      </c>
+      <c r="G91" t="s">
+        <v>561</v>
+      </c>
+      <c r="I91" s="4" t="s">
         <v>662</v>
       </c>
-      <c r="F91" t="s">
-        <v>68</v>
-      </c>
-      <c r="G91" t="s">
-        <v>562</v>
-      </c>
-      <c r="I91" s="4" t="s">
+      <c r="J91" s="4" t="s">
         <v>663</v>
-      </c>
-      <c r="J91" s="4" t="s">
-        <v>664</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -16184,19 +16186,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D92" t="s">
+        <v>664</v>
+      </c>
+      <c r="F92" t="s">
+        <v>68</v>
+      </c>
+      <c r="G92" t="s">
+        <v>469</v>
+      </c>
+      <c r="I92" s="4" t="s">
         <v>665</v>
       </c>
-      <c r="F92" t="s">
-        <v>68</v>
-      </c>
-      <c r="G92" t="s">
-        <v>470</v>
-      </c>
-      <c r="I92" s="4" t="s">
+      <c r="J92" s="4" t="s">
         <v>666</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>667</v>
       </c>
       <c r="K92" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -16215,19 +16217,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D93" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="F93" t="s">
         <v>68</v>
       </c>
       <c r="G93" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I93" t="s">
+        <v>667</v>
+      </c>
+      <c r="J93" s="4" t="s">
         <v>668</v>
-      </c>
-      <c r="J93" s="4" t="s">
-        <v>669</v>
       </c>
       <c r="K93" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
@@ -16239,29 +16241,29 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C94" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D94" t="s">
+        <v>669</v>
+      </c>
+      <c r="F94" t="s">
+        <v>68</v>
+      </c>
+      <c r="G94" t="s">
+        <v>469</v>
+      </c>
+      <c r="H94" t="s">
         <v>670</v>
       </c>
-      <c r="F94" t="s">
-        <v>68</v>
-      </c>
-      <c r="G94" t="s">
-        <v>470</v>
-      </c>
-      <c r="H94" t="s">
+      <c r="I94" t="s">
+        <v>667</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>671</v>
-      </c>
-      <c r="I94" t="s">
-        <v>668</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>672</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified "&amp;SUBSTITUTE(D94,","," and  ") &amp; "= 'sdoh'"</f>
@@ -16280,19 +16282,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D95" t="s">
+        <v>672</v>
+      </c>
+      <c r="F95" t="s">
+        <v>68</v>
+      </c>
+      <c r="G95" t="s">
+        <v>490</v>
+      </c>
+      <c r="I95" t="s">
+        <v>667</v>
+      </c>
+      <c r="J95" s="4" t="s">
         <v>673</v>
-      </c>
-      <c r="F95" t="s">
-        <v>68</v>
-      </c>
-      <c r="G95" t="s">
-        <v>491</v>
-      </c>
-      <c r="I95" t="s">
-        <v>668</v>
-      </c>
-      <c r="J95" s="4" t="s">
-        <v>674</v>
       </c>
       <c r="K95" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date"</f>
@@ -16304,29 +16306,29 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C96" t="str">
         <f t="shared" si="5"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D96" s="16" t="s">
+        <v>674</v>
+      </c>
+      <c r="F96" t="s">
+        <v>68</v>
+      </c>
+      <c r="G96" t="s">
+        <v>561</v>
+      </c>
+      <c r="H96" t="s">
+        <v>670</v>
+      </c>
+      <c r="I96" t="s">
+        <v>667</v>
+      </c>
+      <c r="J96" s="4" t="s">
         <v>675</v>
-      </c>
-      <c r="F96" t="s">
-        <v>68</v>
-      </c>
-      <c r="G96" t="s">
-        <v>562</v>
-      </c>
-      <c r="H96" t="s">
-        <v>671</v>
-      </c>
-      <c r="I96" t="s">
-        <v>668</v>
-      </c>
-      <c r="J96" s="4" t="s">
-        <v>676</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -16345,7 +16347,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="F97" t="s">
         <v>68</v>
@@ -16354,10 +16356,10 @@
         <v>88</v>
       </c>
       <c r="I97" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -16376,21 +16378,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E98" s="16"/>
       <c r="F98" s="16" t="s">
         <v>68</v>
       </c>
       <c r="G98" s="16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4" t="s">
+        <v>678</v>
+      </c>
+      <c r="J98" s="4" t="s">
         <v>679</v>
-      </c>
-      <c r="J98" s="4" t="s">
-        <v>680</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -16409,21 +16411,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="E99" s="16"/>
       <c r="F99" s="16" t="s">
         <v>68</v>
       </c>
       <c r="G99" s="16" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="H99" s="16"/>
       <c r="I99" s="4" t="s">
+        <v>680</v>
+      </c>
+      <c r="J99" s="4" t="s">
         <v>681</v>
-      </c>
-      <c r="J99" s="4" t="s">
-        <v>682</v>
       </c>
       <c r="K99" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -16442,21 +16444,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E100" s="16"/>
       <c r="F100" s="16" t="s">
         <v>68</v>
       </c>
       <c r="G100" s="16" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="H100" s="16"/>
       <c r="I100" s="4" t="s">
+        <v>683</v>
+      </c>
+      <c r="J100" s="4" t="s">
         <v>684</v>
-      </c>
-      <c r="J100" s="4" t="s">
-        <v>685</v>
       </c>
       <c r="K100" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -16474,19 +16476,19 @@
         <v>344</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E101" s="16"/>
       <c r="F101" s="16" t="s">
         <v>68</v>
       </c>
       <c r="G101" s="16" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="H101" s="16"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="K101" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -16498,29 +16500,32 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" ref="C102" si="6">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B102)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-familymemberhistory</v>
       </c>
       <c r="D102" t="s">
-        <v>539</v>
+        <v>538</v>
+      </c>
+      <c r="E102" t="s">
+        <v>55</v>
       </c>
       <c r="F102" t="s">
         <v>68</v>
       </c>
       <c r="G102" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="I102" s="4" t="s">
+        <v>751</v>
+      </c>
+      <c r="J102" s="25" t="s">
+        <v>758</v>
+      </c>
+      <c r="K102" s="4" t="s">
         <v>753</v>
-      </c>
-      <c r="J102" s="25" t="s">
-        <v>752</v>
-      </c>
-      <c r="K102" s="4" t="s">
-        <v>755</v>
       </c>
     </row>
   </sheetData>
@@ -16543,8 +16548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16574,7 +16579,7 @@
         <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -16606,7 +16611,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -16685,13 +16690,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>731</v>
+      </c>
+      <c r="B2" s="26" t="s">
         <v>732</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="C2" s="21" t="s">
         <v>733</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>734</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
@@ -16781,8 +16786,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16953,10 +16958,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
+        <v>726</v>
+      </c>
+      <c r="B12" t="s">
         <v>727</v>
-      </c>
-      <c r="B12" t="s">
-        <v>728</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -17064,17 +17069,17 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="A20" s="27" t="s">
+        <v>745</v>
+      </c>
+      <c r="B20" t="s">
         <v>746</v>
       </c>
-      <c r="B20" t="s">
+      <c r="D20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" t="s">
         <v>747</v>
-      </c>
-      <c r="D20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -17163,10 +17168,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
+        <v>728</v>
+      </c>
+      <c r="B27" t="s">
         <v>729</v>
-      </c>
-      <c r="B27" t="s">
-        <v>730</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -17275,10 +17280,10 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
+        <v>443</v>
+      </c>
+      <c r="B35" t="s">
         <v>444</v>
-      </c>
-      <c r="B35" t="s">
-        <v>445</v>
       </c>
       <c r="D35" t="s">
         <v>12</v>
@@ -17289,10 +17294,10 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
+        <v>445</v>
+      </c>
+      <c r="B36" t="s">
         <v>446</v>
-      </c>
-      <c r="B36" t="s">
-        <v>447</v>
       </c>
       <c r="D36" t="s">
         <v>12</v>
@@ -17443,10 +17448,10 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>441</v>
+      </c>
+      <c r="B47" t="s">
         <v>442</v>
-      </c>
-      <c r="B47" t="s">
-        <v>443</v>
       </c>
       <c r="D47" t="s">
         <v>12</v>
@@ -17727,10 +17732,10 @@
   <dimension ref="A1:Y70"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17851,7 +17856,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>261</v>
@@ -17868,7 +17873,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="V4" t="s">
         <v>346</v>
@@ -17891,7 +17896,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>261</v>
@@ -17939,7 +17944,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>261</v>
@@ -17956,7 +17961,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>261</v>
@@ -17973,7 +17978,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="X10" s="13" t="s">
         <v>261</v>
@@ -17984,20 +17989,20 @@
     </row>
     <row r="11" spans="1:25" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
     </row>
     <row r="12" spans="1:25" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -18017,7 +18022,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="X13" s="13" t="s">
         <v>261</v>
@@ -18028,13 +18033,13 @@
     </row>
     <row r="14" spans="1:25" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B14" t="s">
         <v>29</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
@@ -18047,7 +18052,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="X15" s="13" t="s">
         <v>261</v>
@@ -18064,20 +18069,20 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
     </row>
     <row r="17" spans="1:25" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B17" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -18103,7 +18108,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="V19" t="s">
         <v>68</v>
@@ -18126,7 +18131,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="V20" t="s">
         <v>68</v>
@@ -18172,7 +18177,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="X22" s="13" t="s">
         <v>261</v>
@@ -18189,7 +18194,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
@@ -18202,7 +18207,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="X24" s="13" t="s">
         <v>261</v>
@@ -18219,7 +18224,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
@@ -18232,7 +18237,7 @@
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="V26" t="s">
         <v>314</v>
@@ -18251,7 +18256,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="X27" s="13" t="s">
         <v>261</v>
@@ -18268,7 +18273,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>432</v>
+        <v>756</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="29" customHeight="1" x14ac:dyDescent="0.25">
@@ -18279,7 +18284,7 @@
         <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X29" s="13"/>
       <c r="Y29" s="13"/>
@@ -18292,7 +18297,7 @@
         <v>68</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="X30" s="13" t="s">
         <v>261</v>
@@ -18309,7 +18314,7 @@
         <v>12</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="X31" s="13" t="s">
         <v>261</v>
@@ -18326,7 +18331,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="X32" s="13" t="s">
         <v>261</v>
@@ -18343,7 +18348,7 @@
         <v>12</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
@@ -18442,7 +18447,7 @@
         <v>68</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -18526,16 +18531,16 @@
         <v>208</v>
       </c>
       <c r="L1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="M1" t="s">
-        <v>758</v>
+        <v>755</v>
       </c>
       <c r="N1" t="s">
         <v>209</v>
       </c>
       <c r="O1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="P1" t="s">
         <v>210</v>
@@ -18544,7 +18549,7 @@
         <v>211</v>
       </c>
       <c r="R1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="S1" t="s">
         <v>212</v>

</xml_diff>

<commit_message>
Add USCDI v6 Data Elements to US Core FHIR-52965
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EB4815B-3B53-5A49-BCBA-8301E8707E50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA119B5B-143F-6549-B848-61BF3BD29D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5780" yWindow="500" windowWidth="38500" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="500" windowWidth="38500" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -17167,7 +17167,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="A27" s="26" t="s">
         <v>728</v>
       </c>
       <c r="B27" t="s">
@@ -17722,8 +17722,11 @@
       <formula>NOT(ISERROR(SEARCH("!",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="A27" r:id="rId1" xr:uid="{7528BB40-97A4-574B-BF30-0F07FC3C77A1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
QA technical issues following update to new ig publisher
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEFE349-C5A8-7849-B3D4-1E1C019A7115}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67501AC2-1F7D-5242-BEAB-E4981A24826F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="500" windowWidth="55280" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47220" yWindow="500" windowWidth="55280" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -5478,17 +5478,18 @@
     <t>US Core Device Profile</t>
   </si>
   <si>
-    <t>* Implantable medical devices that have UDI information **SHALL** represent the UDI code in `Device.udiCarrier.carrierHRF`.
-   - All of the five UDI-PI elements that are present in the UDI code **SHALL** be represented in the corresponding US Core Device Profile element.
-   UDI may not be present in all scenarios such as historical implantable devices, patient reported implant information, payer reported devices, or improperly documented implants. If UDI is not present and the manufacturer and/or model number information is available, they **SHOULD** be included to support historical reports of implantable medical devices as follows:
-   manufacturer -&gt; `Device.manufacturer`  
-   model -&gt; `Device.model`  
-* Servers **SHOULD** support query by Device.type to allow clients to request the patient's devices by a specific type. Note: The Device.type is too granular to differentiate implantable vs. non-implantable devices.</t>
+    <t>* Medical devices with UDI information **SHALL** represent the UDI code in `Device.udiCarrier.carrierHRF`. All five UDI-PI elements defined in the UDI code may not always be present in every UDI instance. However, those UDI-PI elements present **SHALL** be represented in the corresponding *US Core Device Profile elements.
+   UDI may not be present in all scenarios, such as historical medical devices, patient-reported implant information, payer-reported devices, or improperly documented implants. If UDI is not present and the manufacturer or model number information is available, they **SHOULD** be included to support historical reports of medical devices as follows:
+   |data element|*US Core Device Profile element|
+   |---|---|
+   |manufacturer|`Device.manufacturer`|
+   |model|`Device.model`|
+   {:.grid}</t>
   </si>
   <si>
     <t>* Procedure codes can be taken from SNOMED-CT, CPT, HCPCS II, ICD-10-PCS, CDT. LOINC.
   * Only LOINC concepts that reflect actual procedures **SHOULD** be used
-* A procedure including an implantable device **SHOULD** use `Procedure.focalDevice` with a reference to the *US Core Device Profile*.
+* A procedure including a medical device **SHOULD** use `Procedure.focalDevice` with a reference to the *US Core Device Profile*.
 * Servers and Clients **SHALL** support both US Core ServiceRequest and US Core Procedure Profiles for communicating the reason or justification for a referral as Additional USCDI Requirements. Typically, the reason or justification for a referral or consultation is communicated through `Procedure.basedOn` linking the Procedure to the US Core ServiceRequest Profile that includes either `ServiceRequest.reasonCode` or `ServiceRequest.reasonReference`. When the Procedure does not have an associated ServiceRequest, it is communicated through the US Core Procedure Profile's `Procedure.reasonCode` or `Procedure.reasonReference`.  Depending on the procedure being documented, a server will select the appropriate Profile to use.
    * Although both `Procedure.reasonCode` and `Procedure.reasonReference` are marked as Additional USCDI Requirements. The certifying server system is not required to support both but **SHALL** support at least one of these elements. The certifying client application **SHALL** support both elements.
       * when using  `Procedure.reasonReference`:
@@ -5682,7 +5683,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -5722,7 +5723,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -13470,10 +13470,10 @@
   <dimension ref="A1:K102"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J81" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I81" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J105" sqref="J105"/>
+      <selection pane="bottomRight" activeCell="I84" sqref="I84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16898,7 +16898,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
+      <c r="A8" t="s">
         <v>637</v>
       </c>
       <c r="B8" t="s">
@@ -17732,10 +17732,10 @@
   <dimension ref="A1:Y70"/>
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E14" sqref="E14"/>
+      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17926,7 +17926,7 @@
       <c r="B7" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="2" t="s">
         <v>756</v>
       </c>
       <c r="X7" s="13" t="s">

</xml_diff>

<commit_message>
FHIR-52994 : Update context for Sex Extension FHIR-51159: Non-substantive (Enhancement) Relax US@ address requirements (Pre-Applied) FHIR-53113 - Update US Core Race and Ethnicity Extension descriptions
</commit_message>
<xml_diff>
--- a/input/resources_spreadsheets/uscore-server.xlsx
+++ b/input/resources_spreadsheets/uscore-server.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ehaas/Documents/FHIR/US-Core/input/resources_spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67501AC2-1F7D-5242-BEAB-E4981A24826F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD31F6BC-75D5-E546-9493-63E2E5A45244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="47220" yWindow="500" windowWidth="55280" windowHeight="28300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="47120" yWindow="500" windowWidth="55280" windowHeight="28300" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="12" r:id="rId1"/>
@@ -1471,12 +1471,6 @@
     <t>_lastUpdated</t>
   </si>
   <si>
-    <t>* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Location.address.line` and  `Location.address.city`.</t>
-  </si>
-  <si>
-    <t>* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `RelatedPerson.address.line` and  `RelatedPerson.address.city`.</t>
-  </si>
-  <si>
     <t>* Although both `Specimen.identifier` and `Specimen.accessionIdentifier` are marked as Must Support, the server system is not required to support both, but **SHALL** support at least one of these elements. The client application **SHALL** support both.</t>
   </si>
   <si>
@@ -5341,22 +5335,6 @@
  * There are multiple Observation profiles.  Refer to the specific profile page for profile specific conformance rules and guidance </t>
   </si>
   <si>
-    <t>* The Patient's Social Security Numbers **SHOULD NOT** be used as a patient identifier in `Patient.identifier.value`.
-*  The Complex Extensions for Race and Ethnicity allow for one or more codes of which: Must Support at least one category code from the OMB Race and Ethnicity Category Value Sets that draw from the Race &amp; Ethnicity - CDC (CDCREC] code system.
-    - **MAY** include additional codes from the detailed ethnicity and detailed race value sets drawn from the Race &amp; Ethnicity - CDC (CDCREC) code system
-    - **SHALL** include a text description
-* Although Patient.deceased[x] is marked as 𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜, certifying systems are not required to support both choices, but **SHALL** support at least `Patient.deceasedDateTime`.
-*  Servers can use the US Core Interpreter Needed Extension on this profile or the US Core Encounter Profile to communicate whether a patient needs an interpreter. Although the extension is marked as an *Additional USCDI Requirement* on both US Core Patient and US Core Encounter Profiles, the certifying Server system is not required to support the extension on both profiles but **SHALL** support the extension on at least one. The certifying Client application **SHALL** support the extension on both profiles.
-     - Systems **SHOULD** designate the patient's preferred language in the `Patient.communication.preferred` element.
-* Certifying systems **SHALL** and non-certifying systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Patient.address.line` and  `Patient.address.city` for new and updated records.</t>
-  </si>
-  <si>
-    <t>* Servers that support only US Core Practitioner Profile and do not support the US Core PractitionerRole Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.
-   * Although Practitioner.address is marked as Must Support, the server system is not required to support it if they support the US Core PractitionerRole Profile, but **SHALL** support it if they do not support the US Core PractitionerRole Profile. The client application **SHALL** support both.
-* To balance the privacy of healthcare workers with the patient's right to access information. Only professional/work contact information about the practitioner **SHOULD** be available to the patient (such as a work address or office telephone number).
-* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Practitioner.address.line` and  `Practitioner.address.city`.</t>
-  </si>
-  <si>
     <t>* This Profile can represent a medication using a code or reference a Medication resource.
   * The Server systems are not required to support both a code and a reference, but **SHALL** support at least one of these methods.
   * The Client application **SHALL** support all methods.
@@ -5378,10 +5356,6 @@
   * when using MedicationRequest.reasonReference:
       * Servers **SHALL** support at least one target resource in `MedicationRequest.reasonReference`. Clients **SHALL** support all target resources.
       * The referenced resources **SHOULD** be a US Core Profile as documented in Referencing US Core Profiles.</t>
-  </si>
-  <si>
-    <t>* Systems **SHALL** support National Provider Identifier (NPI) for organizations and **SHOULD** support Clinical Laboratory Improvement Amendments (CLIA) and the National Association of Insurance Commissioners NAIC Company code (sometimes called "NAIC Number" or "cocode")  for `Organization.Identifier`.
-* Systems **SHOULD** follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Organization.address.line` and  `Organization.address.city`.</t>
   </si>
   <si>
     <t>* For laboratory result reports use the *US Core DiagnosticReport Profile for Laboratory Results Reporting Profile*.
@@ -5495,6 +5469,32 @@
       * when using  `Procedure.reasonReference`:
          * Servers **SHALL** support *at least one* target resource in `Procedure.reasonReference`. Clients **SHALL** support all target resources .
          * The referenced resources **SHOULD** be a US Core Profile.</t>
+  </si>
+  <si>
+    <t>* Systems **SHOULD** enable the user who enters the address to follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Location.address.line` and  `Location.address.city`.</t>
+  </si>
+  <si>
+    <t>* Systems **SHALL** support National Provider Identifier (NPI) for organizations and **SHOULD** support Clinical Laboratory Improvement Amendments (CLIA) and the National Association of Insurance Commissioners NAIC Company code (sometimes called "NAIC Number" or "cocode")  for `Organization.Identifier`.
+* Systems **SHOULD** enable the user who enters the address to follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Organization.address.line` and  `Organization.address.city`.</t>
+  </si>
+  <si>
+    <t>* The Patient's Social Security Numbers **SHOULD NOT** be used as a patient identifier in `Patient.identifier.value`.
+*  The Complex Extensions for Race and Ethnicity allow for one or more codes of which: Must Support at least one category code from the OMB Race and Ethnicity Category Value Sets that draw from the Race &amp; Ethnicity - CDC (CDCREC] code system.
+    - **MAY** include additional codes from the detailed ethnicity and detailed race value sets drawn from the Race &amp; Ethnicity - CDC (CDCREC) code system
+    - **SHALL** include a text description
+* Although Patient.deceased[x] is marked as 𝗔𝗗𝗗𝗜𝗧𝗜𝗢𝗡𝗔𝗟 𝗨𝗦𝗖𝗗𝗜, certifying systems are not required to support both choices, but **SHALL** support at least `Patient.deceasedDateTime`.
+*  Servers can use the US Core Interpreter Needed Extension on this profile or the US Core Encounter Profile to communicate whether a patient needs an interpreter. Although the extension is marked as an *Additional USCDI Requirement* on both US Core Patient and US Core Encounter Profiles, the certifying Server system is not required to support the extension on both profiles but **SHALL** support the extension on at least one. The certifying Client application **SHALL** support the extension on both profiles.
+     - Systems **SHOULD** designate the patient's preferred language in the `Patient.communication.preferred` element.
+* Certifying systems **SHALL** and non-certifying systems **SHOULD** enable the user who enters the address to follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Patient.address.line` and  `Patient.address.city` for new and updated records.</t>
+  </si>
+  <si>
+    <t>* Servers that support only US Core Practitioner Profile and do not support the US Core PractitionerRole Profile **SHALL** provide implementation specific guidance how to access a provider’s location and contact information using only the Practitioner resource.
+   * Although Practitioner.address is marked as Must Support, the server system is not required to support it if they support the US Core PractitionerRole Profile, but **SHALL** support it if they do not support the US Core PractitionerRole Profile. The client application **SHALL** support both.
+* To balance the privacy of healthcare workers with the patient's right to access information. Only professional/work contact information about the practitioner **SHOULD** be available to the patient (such as a work address or office telephone number).
+* Systems **SHOULD** enable the user who enters the address to follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `Practitioner.address.line` and  `Practitioner.address.city`.</t>
+  </si>
+  <si>
+    <t>* Systems **SHOULD** enable the user who enters the address to follow the Project US@ Technical Specification for Patient Addresses Final Version 1.0 as the standard style guide for `RelatedPerson.address.line` and  `RelatedPerson.address.city`.</t>
   </si>
 </sst>
 </file>
@@ -6142,7 +6142,7 @@
         <v>267</v>
       </c>
       <c r="B2" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -8528,7 +8528,7 @@
         <v>0</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G44" t="str">
         <f t="shared" ref="G44" si="5">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B44)</f>
@@ -8957,7 +8957,7 @@
         <v>0</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G52" t="str">
         <f t="shared" si="4"/>
@@ -9654,7 +9654,7 @@
         <v>0</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G65" t="str">
         <f t="shared" si="4"/>
@@ -10019,7 +10019,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="C72" t="s">
         <v>87</v>
@@ -10060,7 +10060,7 @@
         <v>55</v>
       </c>
       <c r="Y72" t="s">
-        <v>746</v>
+        <v>741</v>
       </c>
       <c r="Z72" s="4" t="str">
         <f>"GET [base]/"&amp;B72&amp;"?patient=1137192"</f>
@@ -10080,7 +10080,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="C73" t="s">
         <v>25</v>
@@ -10111,7 +10111,7 @@
         <v>56</v>
       </c>
       <c r="L73" t="s">
-        <v>745</v>
+        <v>740</v>
       </c>
       <c r="M73" t="s">
         <v>55</v>
@@ -10132,7 +10132,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>748</v>
+        <v>743</v>
       </c>
       <c r="C74" t="s">
         <v>60</v>
@@ -11422,7 +11422,7 @@
         <v>0</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>451</v>
+        <v>449</v>
       </c>
       <c r="G98" t="str">
         <f t="shared" ref="G98" si="11">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B98)</f>
@@ -13492,7 +13492,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>452</v>
+        <v>450</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>36</v>
@@ -13501,19 +13501,19 @@
         <v>38</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>453</v>
+        <v>451</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>328</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>454</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>455</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>456</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>3</v>
@@ -13530,20 +13530,20 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C2" t="str">
         <f t="shared" ref="C2:C49" si="0">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B2)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D2" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="F2" t="s">
         <v>68</v>
       </c>
       <c r="G2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="K2" s="4" t="str">
         <f t="shared" ref="K2:K17" si="1">"Fetches a bundle of all "&amp;B2&amp;" resources matching the specified "&amp;SUBSTITUTE(D2,","," and ")</f>
@@ -13555,20 +13555,20 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D3" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="F3" t="s">
         <v>68</v>
       </c>
       <c r="G3" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="K3" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13580,20 +13580,20 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D4" t="s">
-        <v>462</v>
+        <v>460</v>
       </c>
       <c r="F4" t="s">
         <v>68</v>
       </c>
       <c r="G4" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="K4" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13605,20 +13605,20 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D5" t="s">
-        <v>463</v>
+        <v>461</v>
       </c>
       <c r="F5" t="s">
         <v>68</v>
       </c>
       <c r="G5" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="K5" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13637,19 +13637,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D6" t="s">
+        <v>462</v>
+      </c>
+      <c r="F6" t="s">
+        <v>68</v>
+      </c>
+      <c r="G6" t="s">
+        <v>463</v>
+      </c>
+      <c r="I6" t="s">
         <v>464</v>
       </c>
-      <c r="F6" t="s">
-        <v>68</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="J6" t="s">
         <v>465</v>
-      </c>
-      <c r="I6" t="s">
-        <v>466</v>
-      </c>
-      <c r="J6" t="s">
-        <v>467</v>
       </c>
       <c r="K6" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13661,20 +13661,20 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D7" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="F7" t="s">
         <v>68</v>
       </c>
       <c r="G7" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K7" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13686,20 +13686,20 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D8" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="F8" t="s">
         <v>68</v>
       </c>
       <c r="G8" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="K8" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13711,20 +13711,20 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D9" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="F9" t="s">
         <v>68</v>
       </c>
       <c r="G9" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4" t="str">
@@ -13737,14 +13737,14 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D10" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="F10" t="s">
         <v>68</v>
@@ -13764,14 +13764,14 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D11" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="F11" t="s">
         <v>68</v>
@@ -13790,14 +13790,14 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D12" t="s">
-        <v>473</v>
+        <v>471</v>
       </c>
       <c r="F12" t="s">
         <v>68</v>
@@ -13822,19 +13822,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D13" t="s">
+        <v>472</v>
+      </c>
+      <c r="F13" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>473</v>
+      </c>
+      <c r="I13" s="4" t="s">
         <v>474</v>
       </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
+      <c r="J13" t="s">
         <v>475</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>476</v>
-      </c>
-      <c r="J13" t="s">
-        <v>477</v>
       </c>
       <c r="K13" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13846,20 +13846,20 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D14" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="F14" t="s">
         <v>68</v>
       </c>
       <c r="G14" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="K14" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13871,20 +13871,20 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D15" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="F15" t="s">
         <v>68</v>
       </c>
       <c r="G15" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="K15" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13903,19 +13903,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D16" t="s">
+        <v>478</v>
+      </c>
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" t="s">
+        <v>463</v>
+      </c>
+      <c r="I16" t="s">
+        <v>479</v>
+      </c>
+      <c r="J16" t="s">
         <v>480</v>
-      </c>
-      <c r="F16" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" t="s">
-        <v>465</v>
-      </c>
-      <c r="I16" t="s">
-        <v>481</v>
-      </c>
-      <c r="J16" t="s">
-        <v>482</v>
       </c>
       <c r="K16" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13934,7 +13934,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D17" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="F17" t="s">
         <v>68</v>
@@ -13943,10 +13943,10 @@
         <v>88</v>
       </c>
       <c r="I17" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="J17" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="K17" s="4" t="str">
         <f t="shared" si="1"/>
@@ -13965,17 +13965,17 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D18" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F18" t="s">
         <v>68</v>
       </c>
       <c r="G18" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I18" s="4"/>
       <c r="J18" s="24" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="K18" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B18&amp;" resources for the specified "&amp;SUBSTITUTE(D18,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -13987,20 +13987,20 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D19" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="F19" t="s">
         <v>68</v>
       </c>
       <c r="G19" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="J19" s="4"/>
       <c r="K19" s="4" t="str">
@@ -14020,19 +14020,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D20" t="s">
+        <v>487</v>
+      </c>
+      <c r="F20" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" t="s">
+        <v>463</v>
+      </c>
+      <c r="I20" t="s">
+        <v>488</v>
+      </c>
+      <c r="J20" t="s">
         <v>489</v>
-      </c>
-      <c r="F20" t="s">
-        <v>68</v>
-      </c>
-      <c r="G20" t="s">
-        <v>465</v>
-      </c>
-      <c r="I20" t="s">
-        <v>490</v>
-      </c>
-      <c r="J20" t="s">
-        <v>491</v>
       </c>
       <c r="K20" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14051,19 +14051,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-encounter</v>
       </c>
       <c r="D21" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="F21" t="s">
         <v>68</v>
       </c>
       <c r="G21" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I21" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="J21" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="K21" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14075,14 +14075,14 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>457</v>
+        <v>455</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!encounter</v>
       </c>
       <c r="D22" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="F22" t="s">
         <v>68</v>
@@ -14102,20 +14102,20 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D23" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="F23" t="s">
         <v>68</v>
       </c>
       <c r="G23" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="4" t="str">
@@ -14128,20 +14128,20 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D24" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="F24" t="s">
         <v>68</v>
       </c>
       <c r="G24" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
       <c r="K24" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14153,20 +14153,20 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D25" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
       <c r="F25" t="s">
         <v>68</v>
       </c>
       <c r="G25" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
       <c r="I25" s="4"/>
       <c r="K25" s="4" t="str">
@@ -14179,20 +14179,20 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C26" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D26" t="s">
-        <v>502</v>
+        <v>500</v>
       </c>
       <c r="F26" t="s">
         <v>12</v>
       </c>
       <c r="G26" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
@@ -14206,20 +14206,20 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C27" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D27" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
       <c r="F27" t="s">
         <v>68</v>
       </c>
       <c r="G27" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
@@ -14233,20 +14233,20 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C28" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D28" t="s">
-        <v>505</v>
+        <v>503</v>
       </c>
       <c r="F28" t="s">
         <v>68</v>
       </c>
       <c r="G28" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
@@ -14260,20 +14260,20 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C29" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D29" t="s">
-        <v>506</v>
+        <v>504</v>
       </c>
       <c r="F29" t="s">
         <v>68</v>
       </c>
       <c r="G29" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="K29" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14285,14 +14285,14 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C30" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D30" t="s">
-        <v>507</v>
+        <v>505</v>
       </c>
       <c r="F30" t="s">
         <v>68</v>
@@ -14310,20 +14310,20 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C31" t="str">
         <f t="shared" si="0"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaire</v>
       </c>
       <c r="D31" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="F31" t="s">
         <v>68</v>
       </c>
       <c r="G31" t="s">
-        <v>503</v>
+        <v>501</v>
       </c>
       <c r="K31" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14342,19 +14342,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D32" t="s">
+        <v>507</v>
+      </c>
+      <c r="F32" t="s">
+        <v>68</v>
+      </c>
+      <c r="G32" t="s">
+        <v>508</v>
+      </c>
+      <c r="I32" s="4" t="s">
         <v>509</v>
       </c>
-      <c r="F32" t="s">
-        <v>68</v>
-      </c>
-      <c r="G32" t="s">
+      <c r="J32" s="4" t="s">
         <v>510</v>
-      </c>
-      <c r="I32" s="4" t="s">
-        <v>511</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>512</v>
       </c>
       <c r="K32" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14373,19 +14373,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D33" t="s">
+        <v>511</v>
+      </c>
+      <c r="F33" t="s">
+        <v>68</v>
+      </c>
+      <c r="G33" t="s">
+        <v>508</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>512</v>
+      </c>
+      <c r="J33" s="4" t="s">
         <v>513</v>
-      </c>
-      <c r="F33" t="s">
-        <v>68</v>
-      </c>
-      <c r="G33" t="s">
-        <v>510</v>
-      </c>
-      <c r="I33" s="4" t="s">
-        <v>514</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>515</v>
       </c>
       <c r="K33" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14404,19 +14404,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-patient</v>
       </c>
       <c r="D34" t="s">
+        <v>514</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" t="s">
+        <v>508</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>515</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>516</v>
-      </c>
-      <c r="F34" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" t="s">
-        <v>510</v>
-      </c>
-      <c r="I34" s="4" t="s">
-        <v>517</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>518</v>
       </c>
       <c r="K34" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14435,19 +14435,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="D35" t="s">
+        <v>517</v>
+      </c>
+      <c r="F35" t="s">
+        <v>68</v>
+      </c>
+      <c r="G35" t="s">
+        <v>501</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>518</v>
+      </c>
+      <c r="J35" s="4" t="s">
         <v>519</v>
-      </c>
-      <c r="F35" t="s">
-        <v>68</v>
-      </c>
-      <c r="G35" t="s">
-        <v>503</v>
-      </c>
-      <c r="I35" s="4" t="s">
-        <v>520</v>
-      </c>
-      <c r="J35" s="4" t="s">
-        <v>521</v>
       </c>
       <c r="K35" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14466,19 +14466,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!patient</v>
       </c>
       <c r="D36" t="s">
+        <v>520</v>
+      </c>
+      <c r="F36" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" t="s">
+        <v>501</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>521</v>
+      </c>
+      <c r="J36" s="4" t="s">
         <v>522</v>
-      </c>
-      <c r="F36" t="s">
-        <v>12</v>
-      </c>
-      <c r="G36" t="s">
-        <v>503</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>523</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>524</v>
       </c>
       <c r="K36" s="4" t="str">
         <f t="shared" si="2"/>
@@ -14497,25 +14497,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D37" t="s">
+        <v>523</v>
+      </c>
+      <c r="F37" t="s">
+        <v>68</v>
+      </c>
+      <c r="G37" t="s">
+        <v>463</v>
+      </c>
+      <c r="H37" t="s">
+        <v>524</v>
+      </c>
+      <c r="I37" s="4" t="s">
         <v>525</v>
       </c>
-      <c r="F37" t="s">
-        <v>68</v>
-      </c>
-      <c r="G37" t="s">
-        <v>465</v>
-      </c>
-      <c r="H37" t="s">
+      <c r="J37" s="25" t="s">
         <v>526</v>
       </c>
-      <c r="I37" s="4" t="s">
-        <v>527</v>
-      </c>
-      <c r="J37" s="25" t="s">
-        <v>528</v>
-      </c>
       <c r="K37" s="4" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
     </row>
     <row r="38" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14530,22 +14530,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D38" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F38" t="s">
         <v>12</v>
       </c>
       <c r="G38" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I38" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="J38" s="25" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="K38" s="25" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14560,25 +14560,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D39" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="F39" t="s">
         <v>68</v>
       </c>
       <c r="G39" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H39" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="I39" s="4" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="J39" s="25" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="K39" s="25" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
     </row>
     <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14593,22 +14593,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D40" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="F40" t="s">
         <v>68</v>
       </c>
       <c r="G40" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="J40" s="25" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="K40" s="25" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
     </row>
     <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14623,22 +14623,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D41" t="s">
+        <v>532</v>
+      </c>
+      <c r="F41" t="s">
+        <v>68</v>
+      </c>
+      <c r="G41" t="s">
+        <v>463</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>533</v>
+      </c>
+      <c r="J41" s="25" t="s">
+        <v>710</v>
+      </c>
+      <c r="K41" s="4" t="s">
         <v>534</v>
-      </c>
-      <c r="F41" t="s">
-        <v>68</v>
-      </c>
-      <c r="G41" t="s">
-        <v>465</v>
-      </c>
-      <c r="I41" s="4" t="s">
-        <v>535</v>
-      </c>
-      <c r="J41" s="25" t="s">
-        <v>712</v>
-      </c>
-      <c r="K41" s="4" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14653,22 +14653,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D42" t="s">
+        <v>535</v>
+      </c>
+      <c r="F42" t="s">
+        <v>68</v>
+      </c>
+      <c r="G42" t="s">
+        <v>484</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>536</v>
+      </c>
+      <c r="J42" s="25" t="s">
+        <v>711</v>
+      </c>
+      <c r="K42" s="4" t="s">
         <v>537</v>
-      </c>
-      <c r="F42" t="s">
-        <v>68</v>
-      </c>
-      <c r="G42" t="s">
-        <v>486</v>
-      </c>
-      <c r="I42" s="4" t="s">
-        <v>538</v>
-      </c>
-      <c r="J42" s="25" t="s">
-        <v>713</v>
-      </c>
-      <c r="K42" s="4" t="s">
-        <v>539</v>
       </c>
     </row>
     <row r="43" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14683,22 +14683,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D43" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="F43" t="s">
         <v>68</v>
       </c>
       <c r="G43" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I43" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J43" s="25" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="K43" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="44" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14713,22 +14713,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D44" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="F44" t="s">
         <v>68</v>
       </c>
       <c r="G44" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J44" s="25" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14743,22 +14743,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D45" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="F45" t="s">
         <v>68</v>
       </c>
       <c r="G45" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I45" s="4" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="J45" s="25" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="K45" s="4" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14773,17 +14773,17 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-condition</v>
       </c>
       <c r="D46" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="F46" t="s">
         <v>68</v>
       </c>
       <c r="G46" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I46" s="4"/>
       <c r="J46" s="25" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="K46" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B46&amp;" resources for the specified "&amp;SUBSTITUTE(D46,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -14802,22 +14802,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-allergyintolerance</v>
       </c>
       <c r="D47" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="F47" t="s">
         <v>68</v>
       </c>
       <c r="G47" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I47" s="4" t="s">
+        <v>542</v>
+      </c>
+      <c r="J47" s="4" t="s">
+        <v>543</v>
+      </c>
+      <c r="K47" s="4" t="s">
         <v>544</v>
-      </c>
-      <c r="J47" s="4" t="s">
-        <v>545</v>
-      </c>
-      <c r="K47" s="4" t="s">
-        <v>546</v>
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
@@ -14832,19 +14832,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D48" t="s">
+        <v>545</v>
+      </c>
+      <c r="F48" t="s">
+        <v>68</v>
+      </c>
+      <c r="G48" t="s">
+        <v>473</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>546</v>
+      </c>
+      <c r="J48" s="4" t="s">
         <v>547</v>
-      </c>
-      <c r="F48" t="s">
-        <v>68</v>
-      </c>
-      <c r="G48" t="s">
-        <v>475</v>
-      </c>
-      <c r="I48" s="4" t="s">
-        <v>548</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>549</v>
       </c>
       <c r="K48" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B48&amp;" resources for the specified "&amp;SUBSTITUTE(D48,","," and ")</f>
@@ -14863,19 +14863,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-immunization</v>
       </c>
       <c r="D49" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F49" t="s">
         <v>68</v>
       </c>
       <c r="G49" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I49" s="4" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="J49" s="4" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="K49" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B49&amp;" resources for the specified "&amp;SUBSTITUTE(D49,","," and ")</f>
@@ -14890,25 +14890,25 @@
         <v>106</v>
       </c>
       <c r="C50" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D50" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F50" t="s">
         <v>68</v>
       </c>
       <c r="G50" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I50" s="4" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="J50" s="25" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="K50" s="25" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14919,25 +14919,25 @@
         <v>106</v>
       </c>
       <c r="C51" t="s">
+        <v>550</v>
+      </c>
+      <c r="D51" t="s">
+        <v>527</v>
+      </c>
+      <c r="F51" t="s">
+        <v>12</v>
+      </c>
+      <c r="G51" t="s">
+        <v>463</v>
+      </c>
+      <c r="I51" s="4" t="s">
         <v>552</v>
       </c>
-      <c r="D51" t="s">
-        <v>529</v>
-      </c>
-      <c r="F51" t="s">
-        <v>12</v>
-      </c>
-      <c r="G51" t="s">
-        <v>465</v>
-      </c>
-      <c r="I51" s="4" t="s">
-        <v>554</v>
-      </c>
       <c r="J51" s="25" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="K51" s="25" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
     </row>
     <row r="52" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14948,25 +14948,25 @@
         <v>106</v>
       </c>
       <c r="C52" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D52" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F52" t="s">
         <v>12</v>
       </c>
       <c r="G52" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I52" s="4" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="J52" s="25" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="K52" s="25" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
     </row>
     <row r="53" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -14977,25 +14977,25 @@
         <v>106</v>
       </c>
       <c r="C53" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D53" t="s">
+        <v>554</v>
+      </c>
+      <c r="F53" t="s">
+        <v>12</v>
+      </c>
+      <c r="G53" t="s">
+        <v>555</v>
+      </c>
+      <c r="I53" s="4" t="s">
         <v>556</v>
       </c>
-      <c r="F53" t="s">
-        <v>12</v>
-      </c>
-      <c r="G53" t="s">
-        <v>557</v>
-      </c>
-      <c r="I53" s="4" t="s">
-        <v>558</v>
-      </c>
       <c r="J53" s="25" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="K53" s="25" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15010,20 +15010,20 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-diagnosticreport</v>
       </c>
       <c r="D54" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F54" t="s">
         <v>68</v>
       </c>
       <c r="G54" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I54" s="4"/>
       <c r="J54" s="25" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="K54" s="25" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15034,25 +15034,25 @@
         <v>106</v>
       </c>
       <c r="C55" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="D55" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F55" t="s">
         <v>68</v>
       </c>
       <c r="G55" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="J55" s="25" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="K55" s="25" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
@@ -15067,19 +15067,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D56" t="s">
+        <v>560</v>
+      </c>
+      <c r="F56" t="s">
+        <v>68</v>
+      </c>
+      <c r="G56" t="s">
+        <v>463</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>561</v>
+      </c>
+      <c r="J56" s="4" t="s">
         <v>562</v>
-      </c>
-      <c r="F56" t="s">
-        <v>68</v>
-      </c>
-      <c r="G56" t="s">
-        <v>465</v>
-      </c>
-      <c r="I56" s="4" t="s">
-        <v>563</v>
-      </c>
-      <c r="J56" s="4" t="s">
-        <v>564</v>
       </c>
       <c r="K56" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B56&amp;" resources for the specified "&amp;SUBSTITUTE(D56,","," and ")</f>
@@ -15098,19 +15098,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D57" t="s">
+        <v>563</v>
+      </c>
+      <c r="F57" t="s">
+        <v>68</v>
+      </c>
+      <c r="G57" t="s">
+        <v>484</v>
+      </c>
+      <c r="I57" s="4" t="s">
+        <v>564</v>
+      </c>
+      <c r="J57" s="4" t="s">
         <v>565</v>
-      </c>
-      <c r="F57" t="s">
-        <v>68</v>
-      </c>
-      <c r="G57" t="s">
-        <v>486</v>
-      </c>
-      <c r="I57" s="4" t="s">
-        <v>566</v>
-      </c>
-      <c r="J57" s="4" t="s">
-        <v>567</v>
       </c>
       <c r="K57" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B57&amp;" resources for the specified "&amp;SUBSTITUTE(D57,","," and ")</f>
@@ -15129,25 +15129,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D58" t="s">
+        <v>566</v>
+      </c>
+      <c r="F58" t="s">
+        <v>12</v>
+      </c>
+      <c r="G58" t="s">
+        <v>463</v>
+      </c>
+      <c r="H58" t="s">
+        <v>567</v>
+      </c>
+      <c r="I58" s="4" t="s">
         <v>568</v>
       </c>
-      <c r="F58" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" t="s">
-        <v>465</v>
-      </c>
-      <c r="H58" t="s">
+      <c r="J58" s="4" t="s">
         <v>569</v>
       </c>
-      <c r="I58" s="4" t="s">
+      <c r="K58" s="4" t="s">
         <v>570</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>571</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>572</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
@@ -15162,25 +15162,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D59" t="s">
+        <v>571</v>
+      </c>
+      <c r="F59" t="s">
+        <v>12</v>
+      </c>
+      <c r="G59" t="s">
+        <v>463</v>
+      </c>
+      <c r="H59" t="s">
+        <v>567</v>
+      </c>
+      <c r="I59" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="J59" s="4" t="s">
         <v>573</v>
       </c>
-      <c r="F59" t="s">
-        <v>12</v>
-      </c>
-      <c r="G59" t="s">
-        <v>465</v>
-      </c>
-      <c r="H59" t="s">
-        <v>569</v>
-      </c>
-      <c r="I59" s="4" t="s">
+      <c r="K59" s="4" t="s">
         <v>574</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>575</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>576</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
@@ -15195,25 +15195,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D60" t="s">
+        <v>575</v>
+      </c>
+      <c r="F60" t="s">
+        <v>68</v>
+      </c>
+      <c r="G60" t="s">
+        <v>463</v>
+      </c>
+      <c r="H60" t="s">
+        <v>567</v>
+      </c>
+      <c r="I60" s="4" t="s">
+        <v>572</v>
+      </c>
+      <c r="J60" s="4" t="s">
+        <v>576</v>
+      </c>
+      <c r="K60" s="4" t="s">
         <v>577</v>
-      </c>
-      <c r="F60" t="s">
-        <v>68</v>
-      </c>
-      <c r="G60" t="s">
-        <v>465</v>
-      </c>
-      <c r="H60" t="s">
-        <v>569</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>574</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>578</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
@@ -15228,25 +15228,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationrequest</v>
       </c>
       <c r="D61" t="s">
+        <v>578</v>
+      </c>
+      <c r="F61" t="s">
+        <v>68</v>
+      </c>
+      <c r="G61" t="s">
+        <v>555</v>
+      </c>
+      <c r="H61" t="s">
+        <v>567</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>579</v>
+      </c>
+      <c r="J61" s="4" t="s">
         <v>580</v>
       </c>
-      <c r="F61" t="s">
-        <v>68</v>
-      </c>
-      <c r="G61" t="s">
-        <v>557</v>
-      </c>
-      <c r="H61" t="s">
-        <v>569</v>
-      </c>
-      <c r="I61" s="4" t="s">
+      <c r="K61" s="4" t="s">
         <v>581</v>
-      </c>
-      <c r="J61" s="4" t="s">
-        <v>582</v>
-      </c>
-      <c r="K61" s="4" t="s">
-        <v>583</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
@@ -15261,19 +15261,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D62" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F62" t="s">
         <v>68</v>
       </c>
       <c r="G62" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I62" s="4" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="K62" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B62&amp;" resources for the specified "&amp;SUBSTITUTE(D62,","," and ")</f>
@@ -15292,22 +15292,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationstatement</v>
       </c>
       <c r="D63" t="s">
+        <v>584</v>
+      </c>
+      <c r="F63" t="s">
+        <v>68</v>
+      </c>
+      <c r="G63" t="s">
+        <v>484</v>
+      </c>
+      <c r="I63" s="4" t="s">
+        <v>585</v>
+      </c>
+      <c r="J63" s="4" t="s">
         <v>586</v>
       </c>
-      <c r="F63" t="s">
-        <v>68</v>
-      </c>
-      <c r="G63" t="s">
-        <v>486</v>
-      </c>
-      <c r="I63" s="4" t="s">
+      <c r="K63" s="4" t="s">
         <v>587</v>
-      </c>
-      <c r="J63" s="4" t="s">
-        <v>588</v>
-      </c>
-      <c r="K63" s="4" t="s">
-        <v>589</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.2">
@@ -15322,19 +15322,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D64" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F64" t="s">
         <v>68</v>
       </c>
       <c r="G64" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="K64" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B64&amp;" resources for the specified "&amp;SUBSTITUTE(D64,","," and ")</f>
@@ -15353,19 +15353,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D65" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="F65" t="s">
         <v>12</v>
       </c>
       <c r="G65" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I65" s="4" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="K65" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B65&amp;" resources for the specified "&amp;SUBSTITUTE(D65,","," and ")</f>
@@ -15384,19 +15384,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-procedure</v>
       </c>
       <c r="D66" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F66" t="s">
         <v>68</v>
       </c>
       <c r="G66" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I66" s="4" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="J66" s="4" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="K66" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B66&amp;" resources for the specified patient and date and procedure code(s).  SHOULD support search by multiple codes."</f>
@@ -15411,28 +15411,28 @@
         <v>110</v>
       </c>
       <c r="C67" t="s">
+        <v>594</v>
+      </c>
+      <c r="D67" t="s">
+        <v>595</v>
+      </c>
+      <c r="F67" t="s">
+        <v>68</v>
+      </c>
+      <c r="G67" t="s">
+        <v>463</v>
+      </c>
+      <c r="H67" t="s">
         <v>596</v>
       </c>
-      <c r="D67" t="s">
+      <c r="I67" s="4" t="s">
         <v>597</v>
       </c>
-      <c r="F67" t="s">
-        <v>68</v>
-      </c>
-      <c r="G67" t="s">
-        <v>465</v>
-      </c>
-      <c r="H67" t="s">
+      <c r="J67" s="4" t="s">
         <v>598</v>
       </c>
-      <c r="I67" s="4" t="s">
+      <c r="K67" s="4" t="s">
         <v>599</v>
-      </c>
-      <c r="J67" s="4" t="s">
-        <v>600</v>
-      </c>
-      <c r="K67" s="4" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.2">
@@ -15443,25 +15443,25 @@
         <v>110</v>
       </c>
       <c r="C68" t="s">
+        <v>594</v>
+      </c>
+      <c r="D68" t="s">
+        <v>527</v>
+      </c>
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68" t="s">
+        <v>463</v>
+      </c>
+      <c r="H68" t="s">
         <v>596</v>
       </c>
-      <c r="D68" t="s">
-        <v>529</v>
-      </c>
-      <c r="F68" t="s">
-        <v>12</v>
-      </c>
-      <c r="G68" t="s">
-        <v>465</v>
-      </c>
-      <c r="H68" t="s">
-        <v>598</v>
-      </c>
       <c r="I68" s="4" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="J68" s="4" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
       <c r="K68" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B68&amp;" resources for the specified patient and a category code = `laboratory`"</f>
@@ -15476,22 +15476,22 @@
         <v>110</v>
       </c>
       <c r="C69" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D69" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F69" t="s">
         <v>12</v>
       </c>
       <c r="G69" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I69" s="4" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="J69" s="8" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
       <c r="K69" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B69&amp;" resources for the specified patient and observation code(s).  SHOULD support search by multiple report codes. The Observation `code` parameter searches `Observation.code only."</f>
@@ -15506,25 +15506,25 @@
         <v>110</v>
       </c>
       <c r="C70" t="s">
+        <v>594</v>
+      </c>
+      <c r="D70" t="s">
+        <v>554</v>
+      </c>
+      <c r="F70" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" t="s">
+        <v>555</v>
+      </c>
+      <c r="H70" t="s">
         <v>596</v>
       </c>
-      <c r="D70" t="s">
-        <v>556</v>
-      </c>
-      <c r="F70" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" t="s">
-        <v>557</v>
-      </c>
-      <c r="H70" t="s">
-        <v>598</v>
-      </c>
       <c r="I70" s="4" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="J70" s="4" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
       <c r="K70" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B70&amp;" resources for the specified patient and date and a category code = `laboratory`"</f>
@@ -15539,20 +15539,20 @@
         <v>110</v>
       </c>
       <c r="C71" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D71" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="F71" t="s">
         <v>68</v>
       </c>
       <c r="G71" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I71" s="4"/>
       <c r="J71" s="24" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="K71" s="25" t="str">
         <f>"Fetches a bundle of all "&amp;B71&amp;" resources for the specified "&amp;SUBSTITUTE(D71,","," and ") &amp; ". See the US Core General Guidance page for [Searching Using lastUpdated]."</f>
@@ -15567,22 +15567,22 @@
         <v>110</v>
       </c>
       <c r="C72" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
       <c r="D72" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F72" t="s">
         <v>68</v>
       </c>
       <c r="G72" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I72" s="4" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
       <c r="J72" s="4" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="K72" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B72&amp;" resources for the specified patient and date and report code(s).  SHOULD support search by multiple report codes."</f>
@@ -15600,22 +15600,22 @@
         <v>127</v>
       </c>
       <c r="D73" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F73" t="s">
         <v>12</v>
       </c>
       <c r="G73" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H73" t="s">
+        <v>609</v>
+      </c>
+      <c r="I73" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="J73" s="4" t="s">
         <v>611</v>
-      </c>
-      <c r="I73" s="4" t="s">
-        <v>612</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>613</v>
       </c>
       <c r="K73" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B73&amp;" resources for the specified "&amp;SUBSTITUTE(D73,","," and ")&amp;"=`assess-plan`"</f>
@@ -15633,25 +15633,25 @@
         <v>127</v>
       </c>
       <c r="D74" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F74" t="s">
         <v>68</v>
       </c>
       <c r="G74" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H74" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="I74" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="J74" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="K74" s="4" t="s">
         <v>614</v>
-      </c>
-      <c r="J74" s="4" t="s">
-        <v>615</v>
-      </c>
-      <c r="K74" s="4" t="s">
-        <v>616</v>
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.2">
@@ -15665,25 +15665,25 @@
         <v>127</v>
       </c>
       <c r="D75" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="F75" t="s">
         <v>68</v>
       </c>
       <c r="G75" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H75" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
       <c r="I75" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="J75" s="4" t="s">
+        <v>616</v>
+      </c>
+      <c r="K75" s="4" t="s">
         <v>617</v>
-      </c>
-      <c r="J75" s="4" t="s">
-        <v>618</v>
-      </c>
-      <c r="K75" s="4" t="s">
-        <v>619</v>
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.2">
@@ -15697,25 +15697,25 @@
         <v>127</v>
       </c>
       <c r="D76" t="s">
+        <v>618</v>
+      </c>
+      <c r="F76" t="s">
+        <v>68</v>
+      </c>
+      <c r="G76" t="s">
+        <v>555</v>
+      </c>
+      <c r="H76" t="s">
+        <v>609</v>
+      </c>
+      <c r="I76" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="J76" s="4" t="s">
         <v>620</v>
       </c>
-      <c r="F76" t="s">
-        <v>68</v>
-      </c>
-      <c r="G76" t="s">
-        <v>557</v>
-      </c>
-      <c r="H76" t="s">
-        <v>611</v>
-      </c>
-      <c r="I76" s="4" t="s">
+      <c r="K76" s="4" t="s">
         <v>621</v>
-      </c>
-      <c r="J76" s="4" t="s">
-        <v>622</v>
-      </c>
-      <c r="K76" s="4" t="s">
-        <v>623</v>
       </c>
     </row>
     <row r="77" spans="1:11" ht="136" x14ac:dyDescent="0.2">
@@ -15730,25 +15730,25 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D77" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F77" t="s">
         <v>12</v>
       </c>
       <c r="G77" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H77" t="s">
+        <v>622</v>
+      </c>
+      <c r="I77" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="J77" s="4" t="s">
         <v>624</v>
       </c>
-      <c r="I77" s="4" t="s">
+      <c r="K77" s="8" t="s">
         <v>625</v>
-      </c>
-      <c r="J77" s="4" t="s">
-        <v>626</v>
-      </c>
-      <c r="K77" s="8" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="78" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15763,22 +15763,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D78" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F78" t="s">
         <v>68</v>
       </c>
       <c r="G78" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I78" s="4" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="J78" s="25" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
     </row>
     <row r="79" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15786,26 +15786,26 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C79" t="str">
         <f t="shared" si="4"/>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!documentreference</v>
       </c>
       <c r="D79" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="F79" t="s">
         <v>68</v>
       </c>
       <c r="G79" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I79" s="4" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="K79" s="25" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
     </row>
     <row r="80" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15820,22 +15820,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D80" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F80" t="s">
         <v>12</v>
       </c>
       <c r="G80" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I80" s="4" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="J80" s="25" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="K80" s="25" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
     </row>
     <row r="81" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15850,22 +15850,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D81" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="F81" t="s">
         <v>12</v>
       </c>
       <c r="G81" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I81" s="4" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="J81" s="25" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="K81" s="25" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
     </row>
     <row r="82" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -15880,22 +15880,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D82" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="F82" t="s">
         <v>12</v>
       </c>
       <c r="G82" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I82" s="4" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
       <c r="J82" s="25" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="K82" s="25" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="83" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -15910,22 +15910,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-documentreference</v>
       </c>
       <c r="D83" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="F83" t="s">
         <v>68</v>
       </c>
       <c r="G83" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="I83" s="4" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
       <c r="J83" s="25" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="K83" s="25" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.2">
@@ -15936,25 +15936,25 @@
         <v>129</v>
       </c>
       <c r="C84" t="s">
+        <v>635</v>
+      </c>
+      <c r="D84" t="s">
+        <v>478</v>
+      </c>
+      <c r="F84" t="s">
+        <v>68</v>
+      </c>
+      <c r="G84" t="s">
+        <v>463</v>
+      </c>
+      <c r="I84" s="4" t="s">
+        <v>636</v>
+      </c>
+      <c r="J84" s="4" t="s">
         <v>637</v>
       </c>
-      <c r="D84" t="s">
-        <v>480</v>
-      </c>
-      <c r="F84" t="s">
-        <v>68</v>
-      </c>
-      <c r="G84" t="s">
-        <v>465</v>
-      </c>
-      <c r="I84" s="4" t="s">
+      <c r="K84" s="4" t="s">
         <v>638</v>
-      </c>
-      <c r="J84" s="4" t="s">
-        <v>639</v>
-      </c>
-      <c r="K84" s="4" t="s">
-        <v>640</v>
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.2">
@@ -15965,25 +15965,25 @@
         <v>129</v>
       </c>
       <c r="C85" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="D85" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F85" t="s">
         <v>68</v>
       </c>
       <c r="G85" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I85" s="4" t="s">
+        <v>639</v>
+      </c>
+      <c r="J85" s="4" t="s">
+        <v>640</v>
+      </c>
+      <c r="K85" s="4" t="s">
         <v>641</v>
-      </c>
-      <c r="J85" s="4" t="s">
-        <v>642</v>
-      </c>
-      <c r="K85" s="4" t="s">
-        <v>643</v>
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.2">
@@ -15998,22 +15998,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-careteam</v>
       </c>
       <c r="D86" t="s">
+        <v>642</v>
+      </c>
+      <c r="F86" t="s">
+        <v>68</v>
+      </c>
+      <c r="G86" t="s">
+        <v>463</v>
+      </c>
+      <c r="I86" s="4" t="s">
+        <v>643</v>
+      </c>
+      <c r="J86" s="4" t="s">
         <v>644</v>
       </c>
-      <c r="F86" t="s">
-        <v>68</v>
-      </c>
-      <c r="G86" t="s">
-        <v>465</v>
-      </c>
-      <c r="I86" s="4" t="s">
+      <c r="K86" s="4" t="s">
         <v>645</v>
-      </c>
-      <c r="J86" s="4" t="s">
-        <v>646</v>
-      </c>
-      <c r="K86" s="4" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.2">
@@ -16028,19 +16028,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D87" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F87" t="s">
         <v>68</v>
       </c>
       <c r="G87" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I87" s="4" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="J87" s="4" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="K87" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B87&amp;" resources for the specified "&amp;SUBSTITUTE(D87,","," and ")</f>
@@ -16059,19 +16059,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D88" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="F88" t="s">
         <v>12</v>
       </c>
       <c r="G88" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I88" s="4" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="K88" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B88&amp;" resources for the specified patient and  a category code"</f>
@@ -16090,19 +16090,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D89" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="F89" t="s">
         <v>12</v>
       </c>
       <c r="G89" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I89" s="4" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="J89" s="4" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K89" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B89&amp;" resources for the specified patient and  report code(s).  SHOULD support search by multiple report codes."</f>
@@ -16121,19 +16121,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D90" t="s">
+        <v>652</v>
+      </c>
+      <c r="F90" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" t="s">
+        <v>555</v>
+      </c>
+      <c r="I90" s="4" t="s">
+        <v>653</v>
+      </c>
+      <c r="J90" s="4" t="s">
         <v>654</v>
-      </c>
-      <c r="F90" t="s">
-        <v>12</v>
-      </c>
-      <c r="G90" t="s">
-        <v>557</v>
-      </c>
-      <c r="I90" s="4" t="s">
-        <v>655</v>
-      </c>
-      <c r="J90" s="4" t="s">
-        <v>656</v>
       </c>
       <c r="K90" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B90&amp;" resources for the specified patient and date and a category code"</f>
@@ -16152,19 +16152,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-servicerequest</v>
       </c>
       <c r="D91" t="s">
+        <v>655</v>
+      </c>
+      <c r="F91" t="s">
+        <v>68</v>
+      </c>
+      <c r="G91" t="s">
+        <v>555</v>
+      </c>
+      <c r="I91" s="4" t="s">
+        <v>656</v>
+      </c>
+      <c r="J91" s="4" t="s">
         <v>657</v>
-      </c>
-      <c r="F91" t="s">
-        <v>68</v>
-      </c>
-      <c r="G91" t="s">
-        <v>557</v>
-      </c>
-      <c r="I91" s="4" t="s">
-        <v>658</v>
-      </c>
-      <c r="J91" s="4" t="s">
-        <v>659</v>
       </c>
       <c r="K91" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B91&amp;" resources for the specified patient and date and service code(s).  SHOULD support search by multiple report codes."</f>
@@ -16183,19 +16183,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-goal</v>
       </c>
       <c r="D92" t="s">
+        <v>658</v>
+      </c>
+      <c r="F92" t="s">
+        <v>68</v>
+      </c>
+      <c r="G92" t="s">
+        <v>463</v>
+      </c>
+      <c r="I92" s="4" t="s">
+        <v>659</v>
+      </c>
+      <c r="J92" s="4" t="s">
         <v>660</v>
-      </c>
-      <c r="F92" t="s">
-        <v>68</v>
-      </c>
-      <c r="G92" t="s">
-        <v>465</v>
-      </c>
-      <c r="I92" s="4" t="s">
-        <v>661</v>
-      </c>
-      <c r="J92" s="4" t="s">
-        <v>662</v>
       </c>
       <c r="K92" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B92&amp;" resources for the specified "&amp;SUBSTITUTE(D92,","," and ")</f>
@@ -16214,19 +16214,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D93" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="F93" t="s">
         <v>68</v>
       </c>
       <c r="G93" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I93" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J93" s="4" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="K93" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B93&amp;" resources for the specified "&amp;SUBSTITUTE(D93,","," and ")</f>
@@ -16245,22 +16245,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D94" t="s">
+        <v>663</v>
+      </c>
+      <c r="F94" t="s">
+        <v>68</v>
+      </c>
+      <c r="G94" t="s">
+        <v>463</v>
+      </c>
+      <c r="H94" t="s">
+        <v>664</v>
+      </c>
+      <c r="I94" t="s">
+        <v>661</v>
+      </c>
+      <c r="J94" s="4" t="s">
         <v>665</v>
-      </c>
-      <c r="F94" t="s">
-        <v>68</v>
-      </c>
-      <c r="G94" t="s">
-        <v>465</v>
-      </c>
-      <c r="H94" t="s">
-        <v>666</v>
-      </c>
-      <c r="I94" t="s">
-        <v>663</v>
-      </c>
-      <c r="J94" s="4" t="s">
-        <v>667</v>
       </c>
       <c r="K94" t="str">
         <f>"Fetches a bundle of all "&amp;B94&amp;" resources for the specified "&amp;SUBSTITUTE(D94,","," and  ") &amp; "= 'sdoh'"</f>
@@ -16279,19 +16279,19 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D95" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="F95" t="s">
         <v>68</v>
       </c>
       <c r="G95" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="I95" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J95" s="4" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="K95" s="4" t="str">
         <f>"Fetches a bundle of all "&amp;B95&amp;" resources for the specified patient and date"</f>
@@ -16310,22 +16310,22 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!questionnaireresponse</v>
       </c>
       <c r="D96" s="16" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="F96" t="s">
         <v>68</v>
       </c>
       <c r="G96" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="H96" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="I96" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J96" s="4" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="K96" t="str">
         <f>"Fetches a bundle of all "&amp;B96&amp;" resources tagged as 'sdoh' for the specified patient and date"</f>
@@ -16344,7 +16344,7 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-questionnaireresponse</v>
       </c>
       <c r="D97" s="16" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="F97" t="s">
         <v>68</v>
@@ -16353,10 +16353,10 @@
         <v>88</v>
       </c>
       <c r="I97" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="J97" s="4" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="K97" t="str">
         <f>"Fetches a bundle of all "&amp;B97&amp;" resources for the specified patient that have been completed against a specified form."</f>
@@ -16375,21 +16375,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D98" s="16" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="E98" s="16"/>
       <c r="F98" s="16" t="s">
         <v>68</v>
       </c>
       <c r="G98" s="16" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H98" s="16"/>
       <c r="I98" s="4" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="J98" s="4" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="K98" t="str">
         <f>"Fetches a bundle of all "&amp;B98&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed))."</f>
@@ -16408,21 +16408,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-medicationdispense</v>
       </c>
       <c r="D99" s="16" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="E99" s="16"/>
       <c r="F99" s="16" t="s">
         <v>68</v>
       </c>
       <c r="G99" s="16" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="H99" s="16"/>
       <c r="I99" s="4" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="J99" s="4" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="K99" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient that have a given dispense status (e.g., dispensed, not dispensed) and type of dispense (e.g., partially dispensed)."</f>
@@ -16441,21 +16441,21 @@
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-!medicationdispense</v>
       </c>
       <c r="D100" s="16" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="E100" s="16"/>
       <c r="F100" s="16" t="s">
         <v>68</v>
       </c>
       <c r="G100" s="16" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="H100" s="16"/>
       <c r="I100" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="K100" t="str">
         <f>"Fetches a bundle of all "&amp;B99&amp;" resources for the specified patient for a given dispense and date or range"</f>
@@ -16473,19 +16473,19 @@
         <v>342</v>
       </c>
       <c r="D101" s="16" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="E101" s="16"/>
       <c r="F101" s="16" t="s">
         <v>68</v>
       </c>
       <c r="G101" s="16" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="H101" s="16"/>
       <c r="I101" s="4"/>
       <c r="J101" s="4" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="K101" t="str">
         <f>"Fetches a bundle of all "&amp;B101&amp;" resources for the specified patient that may match any of the string fields in the name element (including family, give, prefix, suffix, suffix, and/or text)"</f>
@@ -16497,14 +16497,14 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="C102" t="str">
         <f t="shared" ref="C102" si="6">"http://hl7.org/fhir/us/core/StructureDefinition/us-core-"&amp;LOWER(B102)</f>
         <v>http://hl7.org/fhir/us/core/StructureDefinition/us-core-familymemberhistory</v>
       </c>
       <c r="D102" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E102" t="s">
         <v>55</v>
@@ -16513,16 +16513,16 @@
         <v>68</v>
       </c>
       <c r="G102" t="s">
-        <v>465</v>
+        <v>463</v>
       </c>
       <c r="I102" s="4" t="s">
-        <v>747</v>
+        <v>742</v>
       </c>
       <c r="J102" s="25" t="s">
-        <v>754</v>
+        <v>749</v>
       </c>
       <c r="K102" s="4" t="s">
-        <v>749</v>
+        <v>744</v>
       </c>
     </row>
   </sheetData>
@@ -16546,7 +16546,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView topLeftCell="A5" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16576,7 +16576,7 @@
         <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>750</v>
+        <v>745</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -16592,7 +16592,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>753</v>
+        <v>748</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -16608,7 +16608,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -16687,13 +16687,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>725</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>726</v>
+      </c>
+      <c r="C2" s="21" t="s">
         <v>727</v>
-      </c>
-      <c r="B2" s="26" t="s">
-        <v>728</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>729</v>
       </c>
       <c r="D2" t="s">
         <v>68</v>
@@ -16783,7 +16783,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E65"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -16899,10 +16899,10 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
       <c r="B8" t="s">
-        <v>755</v>
+        <v>750</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -16955,10 +16955,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="B12" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -17067,16 +17067,16 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>741</v>
+        <v>736</v>
       </c>
       <c r="B20" t="s">
-        <v>742</v>
+        <v>737</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
       </c>
       <c r="E20" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -17165,10 +17165,10 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="26" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="B27" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="D27" t="s">
         <v>12</v>
@@ -17731,11 +17731,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Y70"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="29" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17856,7 +17856,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="X3" s="13" t="s">
         <v>259</v>
@@ -17873,7 +17873,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>450</v>
+        <v>448</v>
       </c>
       <c r="V4" t="s">
         <v>344</v>
@@ -17896,7 +17896,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>744</v>
+        <v>739</v>
       </c>
       <c r="X5" s="13" t="s">
         <v>259</v>
@@ -17927,7 +17927,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>756</v>
+        <v>751</v>
       </c>
       <c r="X7" s="13" t="s">
         <v>259</v>
@@ -17944,7 +17944,7 @@
         <v>12</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>739</v>
+        <v>734</v>
       </c>
       <c r="X8" s="13" t="s">
         <v>259</v>
@@ -17961,7 +17961,7 @@
         <v>12</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="X9" s="13" t="s">
         <v>259</v>
@@ -17978,7 +17978,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="X10" s="13" t="s">
         <v>259</v>
@@ -17995,14 +17995,14 @@
         <v>12</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="X11" s="13"/>
       <c r="Y11" s="13"/>
     </row>
     <row r="12" spans="1:25" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>743</v>
+        <v>738</v>
       </c>
       <c r="B12" t="s">
         <v>12</v>
@@ -18039,7 +18039,7 @@
         <v>29</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="X14" s="13"/>
       <c r="Y14" s="13"/>
@@ -18052,7 +18052,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="X15" s="13" t="s">
         <v>259</v>
@@ -18069,7 +18069,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>446</v>
+        <v>753</v>
       </c>
       <c r="X16" s="13"/>
       <c r="Y16" s="13"/>
@@ -18082,7 +18082,7 @@
         <v>12</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="X17" s="13"/>
       <c r="Y17" s="13"/>
@@ -18108,7 +18108,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>737</v>
+        <v>733</v>
       </c>
       <c r="V19" t="s">
         <v>68</v>
@@ -18131,7 +18131,7 @@
         <v>12</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>736</v>
+        <v>732</v>
       </c>
       <c r="V20" t="s">
         <v>68</v>
@@ -18177,7 +18177,7 @@
         <v>12</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="X22" s="13" t="s">
         <v>259</v>
@@ -18194,7 +18194,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>738</v>
+        <v>754</v>
       </c>
       <c r="X23" s="13"/>
       <c r="Y23" s="13"/>
@@ -18207,7 +18207,7 @@
         <v>12</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>734</v>
+        <v>755</v>
       </c>
       <c r="X24" s="13" t="s">
         <v>259</v>
@@ -18224,7 +18224,7 @@
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>735</v>
+        <v>756</v>
       </c>
       <c r="X25" s="13"/>
       <c r="Y25" s="13"/>
@@ -18256,7 +18256,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>757</v>
+        <v>752</v>
       </c>
       <c r="X27" s="13" t="s">
         <v>259</v>
@@ -18273,7 +18273,7 @@
         <v>12</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>752</v>
+        <v>747</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="29" customHeight="1" x14ac:dyDescent="0.25">
@@ -18284,7 +18284,7 @@
         <v>68</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="X29" s="13"/>
       <c r="Y29" s="13"/>
@@ -18297,7 +18297,7 @@
         <v>68</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>449</v>
+        <v>447</v>
       </c>
       <c r="X30" s="13" t="s">
         <v>259</v>
@@ -18314,7 +18314,7 @@
         <v>12</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>447</v>
+        <v>757</v>
       </c>
       <c r="X31" s="13" t="s">
         <v>259</v>
@@ -18331,7 +18331,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>740</v>
+        <v>735</v>
       </c>
       <c r="X32" s="13" t="s">
         <v>259</v>
@@ -18348,7 +18348,7 @@
         <v>12</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>448</v>
+        <v>446</v>
       </c>
       <c r="X33" s="13"/>
       <c r="Y33" s="13"/>
@@ -18534,7 +18534,7 @@
         <v>437</v>
       </c>
       <c r="M1" t="s">
-        <v>751</v>
+        <v>746</v>
       </c>
       <c r="N1" t="s">
         <v>209</v>

</xml_diff>